<commit_message>
Connected with Git (Rapli)
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="184">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -566,6 +566,9 @@
   </si>
   <si>
     <t>No Rek GAS (Mandiri) : 137-00-1307107-7 a/n Irvan Nasher Alimi</t>
+  </si>
+  <si>
+    <t>Connected with Github</t>
   </si>
 </sst>
 </file>
@@ -1313,7 +1316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1563,6 +1566,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="17" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1577,14 +1594,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1600,15 +1612,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1633,39 +1664,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2420,126 +2426,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="125" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
-      <c r="O1" s="126"/>
-      <c r="P1" s="126"/>
-      <c r="Q1" s="126"/>
-      <c r="R1" s="126"/>
+      <c r="A1" s="131" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="132"/>
+      <c r="J1" s="132"/>
+      <c r="K1" s="132"/>
+      <c r="L1" s="132"/>
+      <c r="M1" s="132"/>
+      <c r="N1" s="132"/>
+      <c r="O1" s="132"/>
+      <c r="P1" s="132"/>
+      <c r="Q1" s="132"/>
+      <c r="R1" s="132"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="127"/>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="128"/>
-      <c r="M2" s="128"/>
-      <c r="N2" s="128"/>
-      <c r="O2" s="128"/>
-      <c r="P2" s="128"/>
-      <c r="Q2" s="128"/>
-      <c r="R2" s="128"/>
+      <c r="A2" s="133"/>
+      <c r="B2" s="134"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="134"/>
+      <c r="O2" s="134"/>
+      <c r="P2" s="134"/>
+      <c r="Q2" s="134"/>
+      <c r="R2" s="134"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="127"/>
-      <c r="B3" s="128"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
-      <c r="N3" s="128"/>
-      <c r="O3" s="128"/>
-      <c r="P3" s="128"/>
-      <c r="Q3" s="128"/>
-      <c r="R3" s="128"/>
+      <c r="A3" s="133"/>
+      <c r="B3" s="134"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="134"/>
+      <c r="J3" s="134"/>
+      <c r="K3" s="134"/>
+      <c r="L3" s="134"/>
+      <c r="M3" s="134"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
+      <c r="R3" s="134"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="127"/>
-      <c r="B4" s="128"/>
-      <c r="C4" s="128"/>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
-      <c r="H4" s="128"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="128"/>
-      <c r="K4" s="128"/>
-      <c r="L4" s="128"/>
-      <c r="M4" s="128"/>
-      <c r="N4" s="128"/>
-      <c r="O4" s="128"/>
-      <c r="P4" s="128"/>
-      <c r="Q4" s="128"/>
-      <c r="R4" s="128"/>
+      <c r="A4" s="133"/>
+      <c r="B4" s="134"/>
+      <c r="C4" s="134"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="134"/>
+      <c r="F4" s="134"/>
+      <c r="G4" s="134"/>
+      <c r="H4" s="134"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="134"/>
+      <c r="L4" s="134"/>
+      <c r="M4" s="134"/>
+      <c r="N4" s="134"/>
+      <c r="O4" s="134"/>
+      <c r="P4" s="134"/>
+      <c r="Q4" s="134"/>
+      <c r="R4" s="134"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="127"/>
-      <c r="B5" s="128"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="128"/>
-      <c r="I5" s="128"/>
-      <c r="J5" s="128"/>
-      <c r="K5" s="128"/>
-      <c r="L5" s="128"/>
-      <c r="M5" s="128"/>
-      <c r="N5" s="128"/>
-      <c r="O5" s="128"/>
-      <c r="P5" s="128"/>
-      <c r="Q5" s="128"/>
-      <c r="R5" s="128"/>
+      <c r="A5" s="133"/>
+      <c r="B5" s="134"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="134"/>
+      <c r="L5" s="134"/>
+      <c r="M5" s="134"/>
+      <c r="N5" s="134"/>
+      <c r="O5" s="134"/>
+      <c r="P5" s="134"/>
+      <c r="Q5" s="134"/>
+      <c r="R5" s="134"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="127"/>
-      <c r="B6" s="128"/>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="128"/>
-      <c r="K6" s="128"/>
-      <c r="L6" s="128"/>
-      <c r="M6" s="128"/>
-      <c r="N6" s="128"/>
-      <c r="O6" s="128"/>
-      <c r="P6" s="128"/>
-      <c r="Q6" s="128"/>
-      <c r="R6" s="128"/>
+      <c r="A6" s="133"/>
+      <c r="B6" s="134"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="134"/>
+      <c r="L6" s="134"/>
+      <c r="M6" s="134"/>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -2610,10 +2616,10 @@
       <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="121" t="s">
+      <c r="C10" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="121" t="s">
+      <c r="D10" s="127" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="1">
@@ -2625,7 +2631,7 @@
       <c r="G10" s="1">
         <v>20</v>
       </c>
-      <c r="H10" s="124" t="s">
+      <c r="H10" s="130" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="1">
@@ -2673,8 +2679,8 @@
       <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="122"/>
-      <c r="D11" s="122"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
       <c r="E11" s="1">
         <v>20</v>
       </c>
@@ -2684,7 +2690,7 @@
       <c r="G11" s="1">
         <v>20</v>
       </c>
-      <c r="H11" s="122"/>
+      <c r="H11" s="128"/>
       <c r="I11" s="1">
         <v>20</v>
       </c>
@@ -2730,8 +2736,8 @@
       <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="122"/>
-      <c r="D12" s="122"/>
+      <c r="C12" s="128"/>
+      <c r="D12" s="128"/>
       <c r="E12" s="1">
         <v>10</v>
       </c>
@@ -2741,7 +2747,7 @@
       <c r="G12" s="1">
         <v>10</v>
       </c>
-      <c r="H12" s="122"/>
+      <c r="H12" s="128"/>
       <c r="I12" s="1">
         <v>20</v>
       </c>
@@ -2781,8 +2787,8 @@
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="122"/>
-      <c r="D13" s="122"/>
+      <c r="C13" s="128"/>
+      <c r="D13" s="128"/>
       <c r="E13" s="1">
         <v>20</v>
       </c>
@@ -2792,7 +2798,7 @@
       <c r="G13" s="1">
         <v>20</v>
       </c>
-      <c r="H13" s="122"/>
+      <c r="H13" s="128"/>
       <c r="I13" s="1">
         <v>20</v>
       </c>
@@ -2832,14 +2838,14 @@
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="122"/>
-      <c r="D14" s="122"/>
+      <c r="C14" s="128"/>
+      <c r="D14" s="128"/>
       <c r="E14" s="1">
         <v>20</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="122"/>
+      <c r="H14" s="128"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -2875,8 +2881,8 @@
       <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="122"/>
-      <c r="D15" s="122"/>
+      <c r="C15" s="128"/>
+      <c r="D15" s="128"/>
       <c r="E15" s="1">
         <v>20</v>
       </c>
@@ -2886,7 +2892,7 @@
       <c r="G15" s="1">
         <v>20</v>
       </c>
-      <c r="H15" s="122"/>
+      <c r="H15" s="128"/>
       <c r="I15" s="1">
         <v>20</v>
       </c>
@@ -2934,8 +2940,8 @@
       <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="122"/>
-      <c r="D16" s="122"/>
+      <c r="C16" s="128"/>
+      <c r="D16" s="128"/>
       <c r="E16" s="1">
         <v>20</v>
       </c>
@@ -2943,7 +2949,7 @@
         <v>10</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="122"/>
+      <c r="H16" s="128"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2979,8 +2985,8 @@
       <c r="B17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="122"/>
-      <c r="D17" s="122"/>
+      <c r="C17" s="128"/>
+      <c r="D17" s="128"/>
       <c r="E17" s="1">
         <v>20</v>
       </c>
@@ -2988,7 +2994,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="122"/>
+      <c r="H17" s="128"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -3024,12 +3030,12 @@
       <c r="B18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="122"/>
-      <c r="D18" s="122"/>
+      <c r="C18" s="128"/>
+      <c r="D18" s="128"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="122"/>
+      <c r="H18" s="128"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -3065,8 +3071,8 @@
       <c r="B19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
+      <c r="C19" s="128"/>
+      <c r="D19" s="128"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1">
         <v>20</v>
@@ -3074,7 +3080,7 @@
       <c r="G19" s="1">
         <v>20</v>
       </c>
-      <c r="H19" s="122"/>
+      <c r="H19" s="128"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -3112,8 +3118,8 @@
       <c r="B20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="122"/>
-      <c r="D20" s="122"/>
+      <c r="C20" s="128"/>
+      <c r="D20" s="128"/>
       <c r="E20" s="1">
         <v>20</v>
       </c>
@@ -3121,7 +3127,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="122"/>
+      <c r="H20" s="128"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -3157,8 +3163,8 @@
       <c r="B21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="122"/>
-      <c r="D21" s="122"/>
+      <c r="C21" s="128"/>
+      <c r="D21" s="128"/>
       <c r="E21" s="1">
         <v>20</v>
       </c>
@@ -3168,7 +3174,7 @@
       <c r="G21" s="1">
         <v>20</v>
       </c>
-      <c r="H21" s="122"/>
+      <c r="H21" s="128"/>
       <c r="I21" s="1">
         <v>20</v>
       </c>
@@ -3208,8 +3214,8 @@
       <c r="B22" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="122"/>
-      <c r="D22" s="122"/>
+      <c r="C22" s="128"/>
+      <c r="D22" s="128"/>
       <c r="E22" s="1">
         <v>20</v>
       </c>
@@ -3219,7 +3225,7 @@
       <c r="G22" s="1">
         <v>15</v>
       </c>
-      <c r="H22" s="122"/>
+      <c r="H22" s="128"/>
       <c r="I22" s="1">
         <v>10</v>
       </c>
@@ -3257,14 +3263,14 @@
       <c r="B23" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="122"/>
-      <c r="D23" s="122"/>
+      <c r="C23" s="128"/>
+      <c r="D23" s="128"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1">
         <v>20</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="122"/>
+      <c r="H23" s="128"/>
       <c r="I23" s="1"/>
       <c r="J23" s="9">
         <v>-40</v>
@@ -3304,8 +3310,8 @@
       <c r="B24" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="122"/>
-      <c r="D24" s="122"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
       <c r="E24" s="1">
         <v>20</v>
       </c>
@@ -3313,7 +3319,7 @@
       <c r="G24" s="1">
         <v>20</v>
       </c>
-      <c r="H24" s="122"/>
+      <c r="H24" s="128"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -3349,12 +3355,12 @@
       <c r="B25" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="122"/>
-      <c r="D25" s="122"/>
+      <c r="C25" s="128"/>
+      <c r="D25" s="128"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
-      <c r="H25" s="122"/>
+      <c r="H25" s="128"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -3390,8 +3396,8 @@
       <c r="B26" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="122"/>
-      <c r="D26" s="122"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
       <c r="E26" s="1">
         <v>20</v>
       </c>
@@ -3401,7 +3407,7 @@
       <c r="G26" s="1">
         <v>20</v>
       </c>
-      <c r="H26" s="122"/>
+      <c r="H26" s="128"/>
       <c r="I26" s="1">
         <v>20</v>
       </c>
@@ -3441,14 +3447,14 @@
       <c r="B27" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="122"/>
-      <c r="D27" s="122"/>
+      <c r="C27" s="128"/>
+      <c r="D27" s="128"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1">
         <v>20</v>
       </c>
-      <c r="H27" s="122"/>
+      <c r="H27" s="128"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -3484,8 +3490,8 @@
       <c r="B28" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="122"/>
-      <c r="D28" s="122"/>
+      <c r="C28" s="128"/>
+      <c r="D28" s="128"/>
       <c r="E28" s="1">
         <v>20</v>
       </c>
@@ -3493,7 +3499,7 @@
         <v>20</v>
       </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="122"/>
+      <c r="H28" s="128"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -3529,14 +3535,14 @@
       <c r="B29" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="122"/>
-      <c r="D29" s="122"/>
+      <c r="C29" s="128"/>
+      <c r="D29" s="128"/>
       <c r="E29" s="1">
         <v>20</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="122"/>
+      <c r="H29" s="128"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -3572,8 +3578,8 @@
       <c r="B30" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="122"/>
-      <c r="D30" s="122"/>
+      <c r="C30" s="128"/>
+      <c r="D30" s="128"/>
       <c r="E30" s="1">
         <v>20</v>
       </c>
@@ -3583,7 +3589,7 @@
       <c r="G30" s="1">
         <v>20</v>
       </c>
-      <c r="H30" s="122"/>
+      <c r="H30" s="128"/>
       <c r="I30" s="1">
         <v>20</v>
       </c>
@@ -3629,14 +3635,14 @@
       <c r="B31" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="122"/>
-      <c r="D31" s="122"/>
+      <c r="C31" s="128"/>
+      <c r="D31" s="128"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1">
         <v>20</v>
       </c>
       <c r="G31" s="1"/>
-      <c r="H31" s="122"/>
+      <c r="H31" s="128"/>
       <c r="I31" s="1">
         <v>20</v>
       </c>
@@ -3676,8 +3682,8 @@
       <c r="B32" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="122"/>
-      <c r="D32" s="122"/>
+      <c r="C32" s="128"/>
+      <c r="D32" s="128"/>
       <c r="E32" s="1">
         <v>20</v>
       </c>
@@ -3687,7 +3693,7 @@
       <c r="G32" s="1">
         <v>20</v>
       </c>
-      <c r="H32" s="122"/>
+      <c r="H32" s="128"/>
       <c r="I32" s="1">
         <v>20</v>
       </c>
@@ -3733,8 +3739,8 @@
       <c r="B33" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="122"/>
-      <c r="D33" s="122"/>
+      <c r="C33" s="128"/>
+      <c r="D33" s="128"/>
       <c r="E33" s="1">
         <v>20</v>
       </c>
@@ -3742,7 +3748,7 @@
         <v>15</v>
       </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="122"/>
+      <c r="H33" s="128"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -3778,14 +3784,14 @@
       <c r="B34" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="122"/>
-      <c r="D34" s="122"/>
+      <c r="C34" s="128"/>
+      <c r="D34" s="128"/>
       <c r="E34" s="1">
         <v>20</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="122"/>
+      <c r="H34" s="128"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -3821,8 +3827,8 @@
       <c r="B35" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="122"/>
-      <c r="D35" s="122"/>
+      <c r="C35" s="128"/>
+      <c r="D35" s="128"/>
       <c r="E35" s="1">
         <v>20</v>
       </c>
@@ -3830,7 +3836,7 @@
         <v>20</v>
       </c>
       <c r="G35" s="1"/>
-      <c r="H35" s="122"/>
+      <c r="H35" s="128"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -3866,8 +3872,8 @@
       <c r="B36" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="122"/>
-      <c r="D36" s="122"/>
+      <c r="C36" s="128"/>
+      <c r="D36" s="128"/>
       <c r="E36" s="1">
         <v>20</v>
       </c>
@@ -3877,7 +3883,7 @@
       <c r="G36" s="1">
         <v>20</v>
       </c>
-      <c r="H36" s="122"/>
+      <c r="H36" s="128"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1">
         <v>20</v>
@@ -3915,8 +3921,8 @@
       <c r="B37" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="122"/>
-      <c r="D37" s="122"/>
+      <c r="C37" s="128"/>
+      <c r="D37" s="128"/>
       <c r="E37" s="1">
         <v>20</v>
       </c>
@@ -3926,7 +3932,7 @@
       <c r="G37" s="1">
         <v>20</v>
       </c>
-      <c r="H37" s="122"/>
+      <c r="H37" s="128"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1">
         <v>20</v>
@@ -3970,8 +3976,8 @@
       <c r="B38" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="122"/>
-      <c r="D38" s="122"/>
+      <c r="C38" s="128"/>
+      <c r="D38" s="128"/>
       <c r="E38" s="1">
         <v>20</v>
       </c>
@@ -3981,7 +3987,7 @@
       <c r="G38" s="1">
         <v>20</v>
       </c>
-      <c r="H38" s="122"/>
+      <c r="H38" s="128"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1">
         <v>20</v>
@@ -4019,8 +4025,8 @@
       <c r="B39" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="122"/>
-      <c r="D39" s="122"/>
+      <c r="C39" s="128"/>
+      <c r="D39" s="128"/>
       <c r="E39" s="1">
         <v>20</v>
       </c>
@@ -4028,7 +4034,7 @@
         <v>20</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="122"/>
+      <c r="H39" s="128"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -4064,8 +4070,8 @@
       <c r="B40" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="122"/>
-      <c r="D40" s="122"/>
+      <c r="C40" s="128"/>
+      <c r="D40" s="128"/>
       <c r="E40" s="1">
         <v>20</v>
       </c>
@@ -4075,7 +4081,7 @@
       <c r="G40" s="1">
         <v>20</v>
       </c>
-      <c r="H40" s="122"/>
+      <c r="H40" s="128"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1">
         <v>20</v>
@@ -4119,8 +4125,8 @@
       <c r="B41" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="122"/>
-      <c r="D41" s="122"/>
+      <c r="C41" s="128"/>
+      <c r="D41" s="128"/>
       <c r="E41" s="1">
         <v>20</v>
       </c>
@@ -4128,7 +4134,7 @@
         <v>20</v>
       </c>
       <c r="G41" s="1"/>
-      <c r="H41" s="122"/>
+      <c r="H41" s="128"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -4164,14 +4170,14 @@
       <c r="B42" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="122"/>
-      <c r="D42" s="122"/>
+      <c r="C42" s="128"/>
+      <c r="D42" s="128"/>
       <c r="E42" s="1">
         <v>20</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="122"/>
+      <c r="H42" s="128"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -4207,8 +4213,8 @@
       <c r="B43" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="122"/>
-      <c r="D43" s="122"/>
+      <c r="C43" s="128"/>
+      <c r="D43" s="128"/>
       <c r="E43" s="1">
         <v>20</v>
       </c>
@@ -4218,7 +4224,7 @@
       <c r="G43" s="1">
         <v>20</v>
       </c>
-      <c r="H43" s="122"/>
+      <c r="H43" s="128"/>
       <c r="I43" s="1">
         <v>20</v>
       </c>
@@ -4266,8 +4272,8 @@
       <c r="B44" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="122"/>
-      <c r="D44" s="122"/>
+      <c r="C44" s="128"/>
+      <c r="D44" s="128"/>
       <c r="E44" s="1">
         <v>20</v>
       </c>
@@ -4277,7 +4283,7 @@
       <c r="G44" s="1">
         <v>20</v>
       </c>
-      <c r="H44" s="122"/>
+      <c r="H44" s="128"/>
       <c r="I44" s="1">
         <v>20</v>
       </c>
@@ -4321,8 +4327,8 @@
       <c r="B45" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="122"/>
-      <c r="D45" s="122"/>
+      <c r="C45" s="128"/>
+      <c r="D45" s="128"/>
       <c r="E45" s="1">
         <v>20</v>
       </c>
@@ -4332,7 +4338,7 @@
       <c r="G45" s="1">
         <v>20</v>
       </c>
-      <c r="H45" s="122"/>
+      <c r="H45" s="128"/>
       <c r="I45" s="1">
         <v>15</v>
       </c>
@@ -4370,8 +4376,8 @@
       <c r="B46" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="122"/>
-      <c r="D46" s="122"/>
+      <c r="C46" s="128"/>
+      <c r="D46" s="128"/>
       <c r="E46" s="1">
         <v>20</v>
       </c>
@@ -4381,7 +4387,7 @@
       <c r="G46" s="1">
         <v>20</v>
       </c>
-      <c r="H46" s="122"/>
+      <c r="H46" s="128"/>
       <c r="I46" s="1">
         <v>20</v>
       </c>
@@ -4419,8 +4425,8 @@
       <c r="B47" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="122"/>
-      <c r="D47" s="122"/>
+      <c r="C47" s="128"/>
+      <c r="D47" s="128"/>
       <c r="E47" s="1">
         <v>20</v>
       </c>
@@ -4430,7 +4436,7 @@
       <c r="G47" s="1">
         <v>20</v>
       </c>
-      <c r="H47" s="122"/>
+      <c r="H47" s="128"/>
       <c r="I47" s="1">
         <v>20</v>
       </c>
@@ -4474,8 +4480,8 @@
       <c r="B48" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="122"/>
-      <c r="D48" s="122"/>
+      <c r="C48" s="128"/>
+      <c r="D48" s="128"/>
       <c r="E48" s="1">
         <v>20</v>
       </c>
@@ -4483,7 +4489,7 @@
         <v>20</v>
       </c>
       <c r="G48" s="1"/>
-      <c r="H48" s="122"/>
+      <c r="H48" s="128"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
@@ -4519,8 +4525,8 @@
       <c r="B49" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="122"/>
-      <c r="D49" s="122"/>
+      <c r="C49" s="128"/>
+      <c r="D49" s="128"/>
       <c r="E49" s="1">
         <v>20</v>
       </c>
@@ -4530,7 +4536,7 @@
       <c r="G49" s="1">
         <v>20</v>
       </c>
-      <c r="H49" s="122"/>
+      <c r="H49" s="128"/>
       <c r="I49" s="1">
         <v>20</v>
       </c>
@@ -4570,12 +4576,12 @@
       <c r="B50" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C50" s="122"/>
-      <c r="D50" s="122"/>
+      <c r="C50" s="128"/>
+      <c r="D50" s="128"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
-      <c r="H50" s="122"/>
+      <c r="H50" s="128"/>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
@@ -4611,12 +4617,12 @@
       <c r="B51" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="122"/>
-      <c r="D51" s="122"/>
+      <c r="C51" s="128"/>
+      <c r="D51" s="128"/>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
-      <c r="H51" s="122"/>
+      <c r="H51" s="128"/>
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
@@ -4652,12 +4658,12 @@
       <c r="B52" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="123"/>
-      <c r="D52" s="123"/>
+      <c r="C52" s="129"/>
+      <c r="D52" s="129"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="123"/>
+      <c r="H52" s="129"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -4694,58 +4700,58 @@
     <row r="56" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I58" s="133" t="s">
+      <c r="I58" s="136" t="s">
         <v>68</v>
       </c>
-      <c r="J58" s="134"/>
-      <c r="K58" s="134"/>
-      <c r="L58" s="134"/>
-      <c r="M58" s="135"/>
-      <c r="O58" s="141" t="s">
+      <c r="J58" s="137"/>
+      <c r="K58" s="137"/>
+      <c r="L58" s="137"/>
+      <c r="M58" s="138"/>
+      <c r="O58" s="144" t="s">
         <v>69</v>
       </c>
-      <c r="P58" s="134"/>
-      <c r="Q58" s="134"/>
-      <c r="R58" s="135"/>
+      <c r="P58" s="137"/>
+      <c r="Q58" s="137"/>
+      <c r="R58" s="138"/>
     </row>
     <row r="59" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I59" s="136" t="s">
+      <c r="I59" s="139" t="s">
         <v>70</v>
       </c>
-      <c r="J59" s="128"/>
-      <c r="K59" s="128"/>
-      <c r="L59" s="128"/>
-      <c r="M59" s="137"/>
-      <c r="O59" s="136" t="s">
+      <c r="J59" s="134"/>
+      <c r="K59" s="134"/>
+      <c r="L59" s="134"/>
+      <c r="M59" s="140"/>
+      <c r="O59" s="139" t="s">
         <v>71</v>
       </c>
-      <c r="P59" s="128"/>
-      <c r="Q59" s="128"/>
-      <c r="R59" s="137"/>
+      <c r="P59" s="134"/>
+      <c r="Q59" s="134"/>
+      <c r="R59" s="140"/>
     </row>
     <row r="60" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I60" s="138"/>
-      <c r="J60" s="139"/>
-      <c r="K60" s="139"/>
-      <c r="L60" s="139"/>
-      <c r="M60" s="140"/>
-      <c r="O60" s="138"/>
-      <c r="P60" s="139"/>
-      <c r="Q60" s="139"/>
-      <c r="R60" s="140"/>
+      <c r="I60" s="141"/>
+      <c r="J60" s="142"/>
+      <c r="K60" s="142"/>
+      <c r="L60" s="142"/>
+      <c r="M60" s="143"/>
+      <c r="O60" s="141"/>
+      <c r="P60" s="142"/>
+      <c r="Q60" s="142"/>
+      <c r="R60" s="143"/>
     </row>
     <row r="61" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I61" s="131" t="s">
-        <v>20</v>
-      </c>
-      <c r="J61" s="132"/>
-      <c r="K61" s="130"/>
-      <c r="L61" s="131" t="s">
+      <c r="I61" s="135" t="s">
+        <v>20</v>
+      </c>
+      <c r="J61" s="122"/>
+      <c r="K61" s="123"/>
+      <c r="L61" s="135" t="s">
         <v>72</v>
       </c>
-      <c r="M61" s="130"/>
-      <c r="O61" s="131"/>
-      <c r="P61" s="130"/>
+      <c r="M61" s="123"/>
+      <c r="O61" s="135"/>
+      <c r="P61" s="123"/>
       <c r="Q61" s="11" t="s">
         <v>20</v>
       </c>
@@ -4754,38 +4760,38 @@
       </c>
     </row>
     <row r="62" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I62" s="142" t="s">
+      <c r="I62" s="121" t="s">
         <v>73</v>
       </c>
-      <c r="J62" s="132"/>
-      <c r="K62" s="130"/>
-      <c r="L62" s="143">
+      <c r="J62" s="122"/>
+      <c r="K62" s="123"/>
+      <c r="L62" s="124">
         <v>7350000</v>
       </c>
-      <c r="M62" s="130"/>
-      <c r="O62" s="129" t="s">
+      <c r="M62" s="123"/>
+      <c r="O62" s="125" t="s">
         <v>74</v>
       </c>
-      <c r="P62" s="130"/>
+      <c r="P62" s="123"/>
       <c r="Q62" s="12"/>
       <c r="R62" s="13">
         <v>40000</v>
       </c>
     </row>
     <row r="63" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I63" s="142" t="s">
+      <c r="I63" s="121" t="s">
         <v>75</v>
       </c>
-      <c r="J63" s="132"/>
-      <c r="K63" s="130"/>
-      <c r="L63" s="144">
+      <c r="J63" s="122"/>
+      <c r="K63" s="123"/>
+      <c r="L63" s="126">
         <v>1100000</v>
       </c>
-      <c r="M63" s="130"/>
-      <c r="O63" s="129" t="s">
+      <c r="M63" s="123"/>
+      <c r="O63" s="125" t="s">
         <v>76</v>
       </c>
-      <c r="P63" s="130"/>
+      <c r="P63" s="123"/>
       <c r="Q63" s="14" t="s">
         <v>77</v>
       </c>
@@ -4794,39 +4800,39 @@
       </c>
     </row>
     <row r="64" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I64" s="142" t="s">
+      <c r="I64" s="121" t="s">
         <v>78</v>
       </c>
-      <c r="J64" s="132"/>
-      <c r="K64" s="130"/>
-      <c r="L64" s="143">
+      <c r="J64" s="122"/>
+      <c r="K64" s="123"/>
+      <c r="L64" s="124">
         <f>L62+L63</f>
         <v>8450000</v>
       </c>
-      <c r="M64" s="130"/>
-      <c r="O64" s="129" t="s">
+      <c r="M64" s="123"/>
+      <c r="O64" s="125" t="s">
         <v>79</v>
       </c>
-      <c r="P64" s="130"/>
+      <c r="P64" s="123"/>
       <c r="Q64" s="12"/>
       <c r="R64" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="9:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I65" s="142" t="s">
+      <c r="I65" s="121" t="s">
         <v>80</v>
       </c>
-      <c r="J65" s="132"/>
-      <c r="K65" s="130"/>
-      <c r="L65" s="143">
+      <c r="J65" s="122"/>
+      <c r="K65" s="123"/>
+      <c r="L65" s="124">
         <v>8411850</v>
       </c>
-      <c r="M65" s="130"/>
-      <c r="O65" s="129" t="s">
+      <c r="M65" s="123"/>
+      <c r="O65" s="125" t="s">
         <v>81</v>
       </c>
-      <c r="P65" s="130"/>
+      <c r="P65" s="123"/>
       <c r="Q65" s="12"/>
       <c r="R65" s="13">
         <f>R62-R63+R64</f>
@@ -4834,20 +4840,20 @@
       </c>
     </row>
     <row r="66" spans="9:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I66" s="142" t="s">
+      <c r="I66" s="121" t="s">
         <v>82</v>
       </c>
-      <c r="J66" s="132"/>
-      <c r="K66" s="130"/>
-      <c r="L66" s="143">
+      <c r="J66" s="122"/>
+      <c r="K66" s="123"/>
+      <c r="L66" s="124">
         <f>L64-L65</f>
         <v>38150</v>
       </c>
-      <c r="M66" s="130"/>
-      <c r="O66" s="129" t="s">
+      <c r="M66" s="123"/>
+      <c r="O66" s="125" t="s">
         <v>83</v>
       </c>
-      <c r="P66" s="130"/>
+      <c r="P66" s="123"/>
       <c r="Q66" s="12"/>
       <c r="R66" s="13">
         <f>L66+R65</f>
@@ -5056,17 +5062,6 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="I66:K66"/>
-    <mergeCell ref="L65:M65"/>
-    <mergeCell ref="I65:K65"/>
-    <mergeCell ref="L66:M66"/>
-    <mergeCell ref="O66:P66"/>
-    <mergeCell ref="O65:P65"/>
-    <mergeCell ref="I64:K64"/>
-    <mergeCell ref="L64:M64"/>
-    <mergeCell ref="O64:P64"/>
-    <mergeCell ref="I63:K63"/>
-    <mergeCell ref="L63:M63"/>
     <mergeCell ref="C10:C52"/>
     <mergeCell ref="D10:D52"/>
     <mergeCell ref="H10:H52"/>
@@ -5082,6 +5077,17 @@
     <mergeCell ref="O62:P62"/>
     <mergeCell ref="O61:P61"/>
     <mergeCell ref="O59:R60"/>
+    <mergeCell ref="I64:K64"/>
+    <mergeCell ref="L64:M64"/>
+    <mergeCell ref="O64:P64"/>
+    <mergeCell ref="I63:K63"/>
+    <mergeCell ref="L63:M63"/>
+    <mergeCell ref="I66:K66"/>
+    <mergeCell ref="L65:M65"/>
+    <mergeCell ref="I65:K65"/>
+    <mergeCell ref="L66:M66"/>
+    <mergeCell ref="O66:P66"/>
+    <mergeCell ref="O65:P65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -5093,7 +5099,7 @@
   <dimension ref="A2:AM263"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I69" sqref="I69"/>
+      <selection activeCell="I66" sqref="I66:M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5133,42 +5139,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C2" s="153" t="s">
+      <c r="C2" s="151" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="126"/>
-      <c r="O2" s="126"/>
-      <c r="P2" s="127"/>
-      <c r="Q2" s="126"/>
-      <c r="R2" s="126"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="132"/>
+      <c r="L2" s="132"/>
+      <c r="M2" s="132"/>
+      <c r="N2" s="132"/>
+      <c r="O2" s="132"/>
+      <c r="P2" s="133"/>
+      <c r="Q2" s="132"/>
+      <c r="R2" s="132"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C3" s="127"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
-      <c r="N3" s="128"/>
-      <c r="O3" s="128"/>
-      <c r="P3" s="128"/>
-      <c r="Q3" s="128"/>
-      <c r="R3" s="128"/>
+      <c r="C3" s="133"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="134"/>
+      <c r="J3" s="134"/>
+      <c r="K3" s="134"/>
+      <c r="L3" s="134"/>
+      <c r="M3" s="134"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
+      <c r="R3" s="134"/>
       <c r="W3" s="15"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
@@ -5242,25 +5248,25 @@
       <c r="T5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V5" s="145" t="s">
+      <c r="V5" s="155" t="s">
         <v>87</v>
       </c>
-      <c r="W5" s="132"/>
-      <c r="X5" s="132"/>
-      <c r="Y5" s="132"/>
-      <c r="Z5" s="132"/>
-      <c r="AA5" s="132"/>
-      <c r="AB5" s="132"/>
-      <c r="AC5" s="132"/>
-      <c r="AD5" s="132"/>
-      <c r="AE5" s="132"/>
-      <c r="AF5" s="132"/>
-      <c r="AG5" s="132"/>
-      <c r="AH5" s="132"/>
-      <c r="AI5" s="132"/>
-      <c r="AJ5" s="132"/>
-      <c r="AK5" s="132"/>
-      <c r="AL5" s="130"/>
+      <c r="W5" s="122"/>
+      <c r="X5" s="122"/>
+      <c r="Y5" s="122"/>
+      <c r="Z5" s="122"/>
+      <c r="AA5" s="122"/>
+      <c r="AB5" s="122"/>
+      <c r="AC5" s="122"/>
+      <c r="AD5" s="122"/>
+      <c r="AE5" s="122"/>
+      <c r="AF5" s="122"/>
+      <c r="AG5" s="122"/>
+      <c r="AH5" s="122"/>
+      <c r="AI5" s="122"/>
+      <c r="AJ5" s="122"/>
+      <c r="AK5" s="122"/>
+      <c r="AL5" s="123"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
@@ -5308,29 +5314,29 @@
         <v>NO</v>
       </c>
       <c r="T6" s="23"/>
-      <c r="V6" s="154" t="s">
+      <c r="V6" s="152" t="s">
         <v>1</v>
       </c>
-      <c r="W6" s="154" t="s">
+      <c r="W6" s="152" t="s">
         <v>88</v>
       </c>
-      <c r="X6" s="145" t="s">
+      <c r="X6" s="155" t="s">
         <v>89</v>
       </c>
-      <c r="Y6" s="132"/>
-      <c r="Z6" s="132"/>
-      <c r="AA6" s="132"/>
-      <c r="AB6" s="132"/>
-      <c r="AC6" s="132"/>
-      <c r="AD6" s="132"/>
-      <c r="AE6" s="132"/>
-      <c r="AF6" s="132"/>
-      <c r="AG6" s="132"/>
-      <c r="AH6" s="132"/>
-      <c r="AI6" s="132"/>
-      <c r="AJ6" s="132"/>
-      <c r="AK6" s="132"/>
-      <c r="AL6" s="130"/>
+      <c r="Y6" s="122"/>
+      <c r="Z6" s="122"/>
+      <c r="AA6" s="122"/>
+      <c r="AB6" s="122"/>
+      <c r="AC6" s="122"/>
+      <c r="AD6" s="122"/>
+      <c r="AE6" s="122"/>
+      <c r="AF6" s="122"/>
+      <c r="AG6" s="122"/>
+      <c r="AH6" s="122"/>
+      <c r="AI6" s="122"/>
+      <c r="AJ6" s="122"/>
+      <c r="AK6" s="122"/>
+      <c r="AL6" s="123"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
@@ -5376,27 +5382,27 @@
         <v>NO</v>
       </c>
       <c r="T7" s="23"/>
-      <c r="V7" s="122"/>
-      <c r="W7" s="122"/>
-      <c r="X7" s="145" t="s">
+      <c r="V7" s="128"/>
+      <c r="W7" s="128"/>
+      <c r="X7" s="155" t="s">
         <v>90</v>
       </c>
-      <c r="Y7" s="132"/>
-      <c r="Z7" s="132"/>
-      <c r="AA7" s="130"/>
-      <c r="AB7" s="145" t="s">
+      <c r="Y7" s="122"/>
+      <c r="Z7" s="122"/>
+      <c r="AA7" s="123"/>
+      <c r="AB7" s="155" t="s">
         <v>91</v>
       </c>
-      <c r="AC7" s="132"/>
-      <c r="AD7" s="132"/>
-      <c r="AE7" s="132"/>
-      <c r="AF7" s="132"/>
-      <c r="AG7" s="132"/>
-      <c r="AH7" s="132"/>
-      <c r="AI7" s="132"/>
-      <c r="AJ7" s="132"/>
-      <c r="AK7" s="132"/>
-      <c r="AL7" s="130"/>
+      <c r="AC7" s="122"/>
+      <c r="AD7" s="122"/>
+      <c r="AE7" s="122"/>
+      <c r="AF7" s="122"/>
+      <c r="AG7" s="122"/>
+      <c r="AH7" s="122"/>
+      <c r="AI7" s="122"/>
+      <c r="AJ7" s="122"/>
+      <c r="AK7" s="122"/>
+      <c r="AL7" s="123"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
@@ -5438,8 +5444,8 @@
         <v>NO</v>
       </c>
       <c r="T8" s="23"/>
-      <c r="V8" s="123"/>
-      <c r="W8" s="123"/>
+      <c r="V8" s="129"/>
+      <c r="W8" s="129"/>
       <c r="X8" s="10" t="s">
         <v>20</v>
       </c>
@@ -9012,10 +9018,10 @@
       <c r="V49" s="68"/>
       <c r="W49" s="68"/>
       <c r="X49" s="68"/>
-      <c r="Y49" s="155" t="s">
+      <c r="Y49" s="153" t="s">
         <v>145</v>
       </c>
-      <c r="Z49" s="156"/>
+      <c r="Z49" s="154"/>
       <c r="AA49" s="41">
         <f>SUM(AA9:AA21)</f>
         <v>20000</v>
@@ -9079,12 +9085,12 @@
         <v>NO</v>
       </c>
       <c r="T50" s="3"/>
-      <c r="AG50" s="146" t="s">
+      <c r="AG50" s="156" t="s">
         <v>172</v>
       </c>
-      <c r="AH50" s="146"/>
-      <c r="AI50" s="146"/>
-      <c r="AJ50" s="146"/>
+      <c r="AH50" s="156"/>
+      <c r="AI50" s="156"/>
+      <c r="AJ50" s="156"/>
       <c r="AK50" s="93">
         <v>3087000</v>
       </c>
@@ -9141,12 +9147,12 @@
       <c r="AC51" s="48"/>
       <c r="AD51" s="48"/>
       <c r="AE51" s="48"/>
-      <c r="AG51" s="150" t="s">
+      <c r="AG51" s="160" t="s">
         <v>174</v>
       </c>
-      <c r="AH51" s="151"/>
-      <c r="AI51" s="151"/>
-      <c r="AJ51" s="152"/>
+      <c r="AH51" s="161"/>
+      <c r="AI51" s="161"/>
+      <c r="AJ51" s="162"/>
       <c r="AK51" s="105">
         <v>3077000</v>
       </c>
@@ -9202,12 +9208,12 @@
       <c r="AD52" s="48"/>
       <c r="AE52" s="48"/>
       <c r="AF52" s="48"/>
-      <c r="AG52" s="147" t="s">
+      <c r="AG52" s="157" t="s">
         <v>181</v>
       </c>
-      <c r="AH52" s="148"/>
-      <c r="AI52" s="148"/>
-      <c r="AJ52" s="149"/>
+      <c r="AH52" s="158"/>
+      <c r="AI52" s="158"/>
+      <c r="AJ52" s="159"/>
       <c r="AK52" s="109">
         <v>2550000</v>
       </c>
@@ -9417,12 +9423,12 @@
         <v>NO</v>
       </c>
       <c r="T56" s="3"/>
-      <c r="AG56" s="150" t="s">
+      <c r="AG56" s="160" t="s">
         <v>179</v>
       </c>
-      <c r="AH56" s="151"/>
-      <c r="AI56" s="151"/>
-      <c r="AJ56" s="152"/>
+      <c r="AH56" s="161"/>
+      <c r="AI56" s="161"/>
+      <c r="AJ56" s="162"/>
       <c r="AK56" s="94">
         <f>AK55</f>
         <v>2627000</v>
@@ -9463,12 +9469,12 @@
         <v>NO</v>
       </c>
       <c r="T57" s="3"/>
-      <c r="AG57" s="146" t="s">
+      <c r="AG57" s="156" t="s">
         <v>171</v>
       </c>
-      <c r="AH57" s="146"/>
-      <c r="AI57" s="146"/>
-      <c r="AJ57" s="146"/>
+      <c r="AH57" s="156"/>
+      <c r="AI57" s="156"/>
+      <c r="AJ57" s="156"/>
       <c r="AK57" s="120">
         <f>AK51-AK56</f>
         <v>450000</v>
@@ -9686,36 +9692,48 @@
       <c r="T63" s="3"/>
     </row>
     <row r="64" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="159" t="s">
+    <row r="65" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="145" t="s">
         <v>182</v>
       </c>
-      <c r="D66" s="160"/>
-      <c r="E66" s="160"/>
-      <c r="F66" s="160"/>
-      <c r="G66" s="161"/>
-    </row>
-    <row r="67" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="162"/>
-      <c r="D67" s="163"/>
-      <c r="E67" s="163"/>
-      <c r="F67" s="163"/>
-      <c r="G67" s="164"/>
-    </row>
-    <row r="68" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D66" s="146"/>
+      <c r="E66" s="146"/>
+      <c r="F66" s="146"/>
+      <c r="G66" s="147"/>
+      <c r="I66" s="165" t="s">
+        <v>183</v>
+      </c>
+      <c r="J66" s="165"/>
+      <c r="K66" s="165"/>
+      <c r="L66" s="165"/>
+      <c r="M66" s="165"/>
+    </row>
+    <row r="67" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="148"/>
+      <c r="D67" s="149"/>
+      <c r="E67" s="149"/>
+      <c r="F67" s="149"/>
+      <c r="G67" s="150"/>
+      <c r="I67" s="165"/>
+      <c r="J67" s="165"/>
+      <c r="K67" s="165"/>
+      <c r="L67" s="165"/>
+      <c r="M67" s="165"/>
+    </row>
+    <row r="68" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9900,13 +9918,7 @@
     <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="C66:G67"/>
-    <mergeCell ref="C2:R3"/>
-    <mergeCell ref="W6:W8"/>
-    <mergeCell ref="V6:V8"/>
-    <mergeCell ref="Y49:Z49"/>
-    <mergeCell ref="X7:AA7"/>
+  <mergeCells count="15">
     <mergeCell ref="AB7:AL7"/>
     <mergeCell ref="V5:AL5"/>
     <mergeCell ref="X6:AL6"/>
@@ -9915,6 +9927,13 @@
     <mergeCell ref="AG51:AJ51"/>
     <mergeCell ref="AG50:AJ50"/>
     <mergeCell ref="AG56:AJ56"/>
+    <mergeCell ref="C66:G67"/>
+    <mergeCell ref="C2:R3"/>
+    <mergeCell ref="W6:W8"/>
+    <mergeCell ref="V6:V8"/>
+    <mergeCell ref="Y49:Z49"/>
+    <mergeCell ref="X7:AA7"/>
+    <mergeCell ref="I66:M67"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:T63">
     <cfRule type="expression" dxfId="6" priority="2">
@@ -9972,17 +9991,17 @@
     <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="77"/>
-      <c r="C4" s="157" t="s">
+      <c r="C4" s="163" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="158"/>
+      <c r="D4" s="164"/>
       <c r="E4" s="78"/>
       <c r="F4" s="84"/>
       <c r="G4" s="85"/>
-      <c r="H4" s="157" t="s">
+      <c r="H4" s="163" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="158"/>
+      <c r="I4" s="164"/>
       <c r="J4" s="86"/>
       <c r="K4" s="78"/>
     </row>
@@ -10109,17 +10128,17 @@
     <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="77"/>
-      <c r="C17" s="157" t="s">
+      <c r="C17" s="163" t="s">
         <v>147</v>
       </c>
-      <c r="D17" s="158"/>
+      <c r="D17" s="164"/>
       <c r="E17" s="78"/>
       <c r="F17" s="77"/>
       <c r="G17" s="86"/>
-      <c r="H17" s="157" t="s">
+      <c r="H17" s="163" t="s">
         <v>149</v>
       </c>
-      <c r="I17" s="158"/>
+      <c r="I17" s="164"/>
       <c r="J17" s="86"/>
       <c r="K17" s="78"/>
     </row>

</xml_diff>

<commit_message>
Ace KAS (2019 LUNAS)
Nyumbang 250.000 untuk Gelex
=========================
KAS thn 2019 lunas
========================
Sumbangan Gelex = 250.000
Tagihan Kas 2019  = 235.000
--------------------------------- -
                                  15.000
*****************************************
*Sisa 45 rb simpanan
*****************************************
Kembalian Wanabaya = 30.000
Sisa sumbang gelex =    15.000
------------------------------------+
                                         45.000
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="186">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -571,7 +571,10 @@
     <t>Connected with Github</t>
   </si>
   <si>
-    <t>abi</t>
+    <t>ace</t>
+  </si>
+  <si>
+    <t>sisa 15</t>
   </si>
 </sst>
 </file>
@@ -1570,6 +1573,20 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1584,14 +1601,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1605,39 +1617,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1668,8 +1647,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1681,7 +1684,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2452,126 +2469,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="125"/>
-      <c r="R1" s="125"/>
+      <c r="A1" s="130" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
+      <c r="O1" s="131"/>
+      <c r="P1" s="131"/>
+      <c r="Q1" s="131"/>
+      <c r="R1" s="131"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="126"/>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="127"/>
-      <c r="K2" s="127"/>
-      <c r="L2" s="127"/>
-      <c r="M2" s="127"/>
-      <c r="N2" s="127"/>
-      <c r="O2" s="127"/>
-      <c r="P2" s="127"/>
-      <c r="Q2" s="127"/>
-      <c r="R2" s="127"/>
+      <c r="A2" s="132"/>
+      <c r="B2" s="133"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="133"/>
+      <c r="H2" s="133"/>
+      <c r="I2" s="133"/>
+      <c r="J2" s="133"/>
+      <c r="K2" s="133"/>
+      <c r="L2" s="133"/>
+      <c r="M2" s="133"/>
+      <c r="N2" s="133"/>
+      <c r="O2" s="133"/>
+      <c r="P2" s="133"/>
+      <c r="Q2" s="133"/>
+      <c r="R2" s="133"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="126"/>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="127"/>
-      <c r="K3" s="127"/>
-      <c r="L3" s="127"/>
-      <c r="M3" s="127"/>
-      <c r="N3" s="127"/>
-      <c r="O3" s="127"/>
-      <c r="P3" s="127"/>
-      <c r="Q3" s="127"/>
-      <c r="R3" s="127"/>
+      <c r="A3" s="132"/>
+      <c r="B3" s="133"/>
+      <c r="C3" s="133"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="133"/>
+      <c r="K3" s="133"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="133"/>
+      <c r="N3" s="133"/>
+      <c r="O3" s="133"/>
+      <c r="P3" s="133"/>
+      <c r="Q3" s="133"/>
+      <c r="R3" s="133"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="126"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="127"/>
-      <c r="E4" s="127"/>
-      <c r="F4" s="127"/>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="127"/>
-      <c r="K4" s="127"/>
-      <c r="L4" s="127"/>
-      <c r="M4" s="127"/>
-      <c r="N4" s="127"/>
-      <c r="O4" s="127"/>
-      <c r="P4" s="127"/>
-      <c r="Q4" s="127"/>
-      <c r="R4" s="127"/>
+      <c r="A4" s="132"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="133"/>
+      <c r="D4" s="133"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
+      <c r="H4" s="133"/>
+      <c r="I4" s="133"/>
+      <c r="J4" s="133"/>
+      <c r="K4" s="133"/>
+      <c r="L4" s="133"/>
+      <c r="M4" s="133"/>
+      <c r="N4" s="133"/>
+      <c r="O4" s="133"/>
+      <c r="P4" s="133"/>
+      <c r="Q4" s="133"/>
+      <c r="R4" s="133"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="126"/>
-      <c r="B5" s="127"/>
-      <c r="C5" s="127"/>
-      <c r="D5" s="127"/>
-      <c r="E5" s="127"/>
-      <c r="F5" s="127"/>
-      <c r="G5" s="127"/>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="127"/>
-      <c r="K5" s="127"/>
-      <c r="L5" s="127"/>
-      <c r="M5" s="127"/>
-      <c r="N5" s="127"/>
-      <c r="O5" s="127"/>
-      <c r="P5" s="127"/>
-      <c r="Q5" s="127"/>
-      <c r="R5" s="127"/>
+      <c r="A5" s="132"/>
+      <c r="B5" s="133"/>
+      <c r="C5" s="133"/>
+      <c r="D5" s="133"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="133"/>
+      <c r="H5" s="133"/>
+      <c r="I5" s="133"/>
+      <c r="J5" s="133"/>
+      <c r="K5" s="133"/>
+      <c r="L5" s="133"/>
+      <c r="M5" s="133"/>
+      <c r="N5" s="133"/>
+      <c r="O5" s="133"/>
+      <c r="P5" s="133"/>
+      <c r="Q5" s="133"/>
+      <c r="R5" s="133"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="126"/>
-      <c r="B6" s="127"/>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="127"/>
-      <c r="M6" s="127"/>
-      <c r="N6" s="127"/>
-      <c r="O6" s="127"/>
-      <c r="P6" s="127"/>
-      <c r="Q6" s="127"/>
-      <c r="R6" s="127"/>
+      <c r="A6" s="132"/>
+      <c r="B6" s="133"/>
+      <c r="C6" s="133"/>
+      <c r="D6" s="133"/>
+      <c r="E6" s="133"/>
+      <c r="F6" s="133"/>
+      <c r="G6" s="133"/>
+      <c r="H6" s="133"/>
+      <c r="I6" s="133"/>
+      <c r="J6" s="133"/>
+      <c r="K6" s="133"/>
+      <c r="L6" s="133"/>
+      <c r="M6" s="133"/>
+      <c r="N6" s="133"/>
+      <c r="O6" s="133"/>
+      <c r="P6" s="133"/>
+      <c r="Q6" s="133"/>
+      <c r="R6" s="133"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -2642,10 +2659,10 @@
       <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="120" t="s">
+      <c r="C10" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="120" t="s">
+      <c r="D10" s="126" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="1">
@@ -2657,7 +2674,7 @@
       <c r="G10" s="1">
         <v>20</v>
       </c>
-      <c r="H10" s="123" t="s">
+      <c r="H10" s="129" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="1">
@@ -2705,8 +2722,8 @@
       <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="121"/>
-      <c r="D11" s="121"/>
+      <c r="C11" s="127"/>
+      <c r="D11" s="127"/>
       <c r="E11" s="1">
         <v>20</v>
       </c>
@@ -2716,7 +2733,7 @@
       <c r="G11" s="1">
         <v>20</v>
       </c>
-      <c r="H11" s="121"/>
+      <c r="H11" s="127"/>
       <c r="I11" s="1">
         <v>20</v>
       </c>
@@ -2762,8 +2779,8 @@
       <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="121"/>
-      <c r="D12" s="121"/>
+      <c r="C12" s="127"/>
+      <c r="D12" s="127"/>
       <c r="E12" s="1">
         <v>10</v>
       </c>
@@ -2773,7 +2790,7 @@
       <c r="G12" s="1">
         <v>10</v>
       </c>
-      <c r="H12" s="121"/>
+      <c r="H12" s="127"/>
       <c r="I12" s="1">
         <v>20</v>
       </c>
@@ -2813,8 +2830,8 @@
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="121"/>
-      <c r="D13" s="121"/>
+      <c r="C13" s="127"/>
+      <c r="D13" s="127"/>
       <c r="E13" s="1">
         <v>20</v>
       </c>
@@ -2824,7 +2841,7 @@
       <c r="G13" s="1">
         <v>20</v>
       </c>
-      <c r="H13" s="121"/>
+      <c r="H13" s="127"/>
       <c r="I13" s="1">
         <v>20</v>
       </c>
@@ -2864,14 +2881,14 @@
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="121"/>
-      <c r="D14" s="121"/>
+      <c r="C14" s="127"/>
+      <c r="D14" s="127"/>
       <c r="E14" s="1">
         <v>20</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="121"/>
+      <c r="H14" s="127"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -2907,8 +2924,8 @@
       <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="121"/>
-      <c r="D15" s="121"/>
+      <c r="C15" s="127"/>
+      <c r="D15" s="127"/>
       <c r="E15" s="1">
         <v>20</v>
       </c>
@@ -2918,7 +2935,7 @@
       <c r="G15" s="1">
         <v>20</v>
       </c>
-      <c r="H15" s="121"/>
+      <c r="H15" s="127"/>
       <c r="I15" s="1">
         <v>20</v>
       </c>
@@ -2966,8 +2983,8 @@
       <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="121"/>
-      <c r="D16" s="121"/>
+      <c r="C16" s="127"/>
+      <c r="D16" s="127"/>
       <c r="E16" s="1">
         <v>20</v>
       </c>
@@ -2975,7 +2992,7 @@
         <v>10</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="121"/>
+      <c r="H16" s="127"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -3011,8 +3028,8 @@
       <c r="B17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="121"/>
-      <c r="D17" s="121"/>
+      <c r="C17" s="127"/>
+      <c r="D17" s="127"/>
       <c r="E17" s="1">
         <v>20</v>
       </c>
@@ -3020,7 +3037,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="121"/>
+      <c r="H17" s="127"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -3056,12 +3073,12 @@
       <c r="B18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="121"/>
-      <c r="D18" s="121"/>
+      <c r="C18" s="127"/>
+      <c r="D18" s="127"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="121"/>
+      <c r="H18" s="127"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -3097,8 +3114,8 @@
       <c r="B19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="121"/>
-      <c r="D19" s="121"/>
+      <c r="C19" s="127"/>
+      <c r="D19" s="127"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1">
         <v>20</v>
@@ -3106,7 +3123,7 @@
       <c r="G19" s="1">
         <v>20</v>
       </c>
-      <c r="H19" s="121"/>
+      <c r="H19" s="127"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -3144,8 +3161,8 @@
       <c r="B20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="121"/>
-      <c r="D20" s="121"/>
+      <c r="C20" s="127"/>
+      <c r="D20" s="127"/>
       <c r="E20" s="1">
         <v>20</v>
       </c>
@@ -3153,7 +3170,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="121"/>
+      <c r="H20" s="127"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -3189,8 +3206,8 @@
       <c r="B21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="121"/>
-      <c r="D21" s="121"/>
+      <c r="C21" s="127"/>
+      <c r="D21" s="127"/>
       <c r="E21" s="1">
         <v>20</v>
       </c>
@@ -3200,7 +3217,7 @@
       <c r="G21" s="1">
         <v>20</v>
       </c>
-      <c r="H21" s="121"/>
+      <c r="H21" s="127"/>
       <c r="I21" s="1">
         <v>20</v>
       </c>
@@ -3242,8 +3259,8 @@
       <c r="B22" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="121"/>
-      <c r="D22" s="121"/>
+      <c r="C22" s="127"/>
+      <c r="D22" s="127"/>
       <c r="E22" s="1">
         <v>20</v>
       </c>
@@ -3253,7 +3270,7 @@
       <c r="G22" s="1">
         <v>15</v>
       </c>
-      <c r="H22" s="121"/>
+      <c r="H22" s="127"/>
       <c r="I22" s="1">
         <v>10</v>
       </c>
@@ -3291,14 +3308,14 @@
       <c r="B23" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="121"/>
-      <c r="D23" s="121"/>
+      <c r="C23" s="127"/>
+      <c r="D23" s="127"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1">
         <v>20</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="121"/>
+      <c r="H23" s="127"/>
       <c r="I23" s="1"/>
       <c r="J23" s="9">
         <v>-40</v>
@@ -3338,8 +3355,8 @@
       <c r="B24" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="121"/>
-      <c r="D24" s="121"/>
+      <c r="C24" s="127"/>
+      <c r="D24" s="127"/>
       <c r="E24" s="1">
         <v>20</v>
       </c>
@@ -3347,7 +3364,7 @@
       <c r="G24" s="1">
         <v>20</v>
       </c>
-      <c r="H24" s="121"/>
+      <c r="H24" s="127"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -3383,12 +3400,12 @@
       <c r="B25" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="121"/>
-      <c r="D25" s="121"/>
+      <c r="C25" s="127"/>
+      <c r="D25" s="127"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
-      <c r="H25" s="121"/>
+      <c r="H25" s="127"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -3424,8 +3441,8 @@
       <c r="B26" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="121"/>
-      <c r="D26" s="121"/>
+      <c r="C26" s="127"/>
+      <c r="D26" s="127"/>
       <c r="E26" s="1">
         <v>20</v>
       </c>
@@ -3435,7 +3452,7 @@
       <c r="G26" s="1">
         <v>20</v>
       </c>
-      <c r="H26" s="121"/>
+      <c r="H26" s="127"/>
       <c r="I26" s="1">
         <v>20</v>
       </c>
@@ -3475,14 +3492,14 @@
       <c r="B27" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="121"/>
-      <c r="D27" s="121"/>
+      <c r="C27" s="127"/>
+      <c r="D27" s="127"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1">
         <v>20</v>
       </c>
-      <c r="H27" s="121"/>
+      <c r="H27" s="127"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -3518,8 +3535,8 @@
       <c r="B28" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="121"/>
-      <c r="D28" s="121"/>
+      <c r="C28" s="127"/>
+      <c r="D28" s="127"/>
       <c r="E28" s="1">
         <v>20</v>
       </c>
@@ -3527,7 +3544,7 @@
         <v>20</v>
       </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="121"/>
+      <c r="H28" s="127"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -3563,14 +3580,14 @@
       <c r="B29" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="121"/>
-      <c r="D29" s="121"/>
+      <c r="C29" s="127"/>
+      <c r="D29" s="127"/>
       <c r="E29" s="1">
         <v>20</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="121"/>
+      <c r="H29" s="127"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -3606,8 +3623,8 @@
       <c r="B30" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="121"/>
-      <c r="D30" s="121"/>
+      <c r="C30" s="127"/>
+      <c r="D30" s="127"/>
       <c r="E30" s="1">
         <v>20</v>
       </c>
@@ -3617,7 +3634,7 @@
       <c r="G30" s="1">
         <v>20</v>
       </c>
-      <c r="H30" s="121"/>
+      <c r="H30" s="127"/>
       <c r="I30" s="1">
         <v>20</v>
       </c>
@@ -3663,14 +3680,14 @@
       <c r="B31" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="121"/>
-      <c r="D31" s="121"/>
+      <c r="C31" s="127"/>
+      <c r="D31" s="127"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1">
         <v>20</v>
       </c>
       <c r="G31" s="1"/>
-      <c r="H31" s="121"/>
+      <c r="H31" s="127"/>
       <c r="I31" s="1">
         <v>20</v>
       </c>
@@ -3710,8 +3727,8 @@
       <c r="B32" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="121"/>
-      <c r="D32" s="121"/>
+      <c r="C32" s="127"/>
+      <c r="D32" s="127"/>
       <c r="E32" s="1">
         <v>20</v>
       </c>
@@ -3721,7 +3738,7 @@
       <c r="G32" s="1">
         <v>20</v>
       </c>
-      <c r="H32" s="121"/>
+      <c r="H32" s="127"/>
       <c r="I32" s="1">
         <v>20</v>
       </c>
@@ -3767,8 +3784,8 @@
       <c r="B33" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="121"/>
-      <c r="D33" s="121"/>
+      <c r="C33" s="127"/>
+      <c r="D33" s="127"/>
       <c r="E33" s="1">
         <v>20</v>
       </c>
@@ -3776,7 +3793,7 @@
         <v>15</v>
       </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="121"/>
+      <c r="H33" s="127"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -3812,14 +3829,14 @@
       <c r="B34" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="121"/>
-      <c r="D34" s="121"/>
+      <c r="C34" s="127"/>
+      <c r="D34" s="127"/>
       <c r="E34" s="1">
         <v>20</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="121"/>
+      <c r="H34" s="127"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -3855,8 +3872,8 @@
       <c r="B35" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="121"/>
-      <c r="D35" s="121"/>
+      <c r="C35" s="127"/>
+      <c r="D35" s="127"/>
       <c r="E35" s="1">
         <v>20</v>
       </c>
@@ -3864,7 +3881,7 @@
         <v>20</v>
       </c>
       <c r="G35" s="1"/>
-      <c r="H35" s="121"/>
+      <c r="H35" s="127"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -3900,8 +3917,8 @@
       <c r="B36" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="121"/>
-      <c r="D36" s="121"/>
+      <c r="C36" s="127"/>
+      <c r="D36" s="127"/>
       <c r="E36" s="1">
         <v>20</v>
       </c>
@@ -3911,7 +3928,7 @@
       <c r="G36" s="1">
         <v>20</v>
       </c>
-      <c r="H36" s="121"/>
+      <c r="H36" s="127"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1">
         <v>20</v>
@@ -3949,8 +3966,8 @@
       <c r="B37" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="121"/>
-      <c r="D37" s="121"/>
+      <c r="C37" s="127"/>
+      <c r="D37" s="127"/>
       <c r="E37" s="1">
         <v>20</v>
       </c>
@@ -3960,7 +3977,7 @@
       <c r="G37" s="1">
         <v>20</v>
       </c>
-      <c r="H37" s="121"/>
+      <c r="H37" s="127"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1">
         <v>20</v>
@@ -4004,8 +4021,8 @@
       <c r="B38" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="121"/>
-      <c r="D38" s="121"/>
+      <c r="C38" s="127"/>
+      <c r="D38" s="127"/>
       <c r="E38" s="1">
         <v>20</v>
       </c>
@@ -4015,7 +4032,7 @@
       <c r="G38" s="1">
         <v>20</v>
       </c>
-      <c r="H38" s="121"/>
+      <c r="H38" s="127"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1">
         <v>20</v>
@@ -4053,8 +4070,8 @@
       <c r="B39" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="121"/>
-      <c r="D39" s="121"/>
+      <c r="C39" s="127"/>
+      <c r="D39" s="127"/>
       <c r="E39" s="1">
         <v>20</v>
       </c>
@@ -4062,7 +4079,7 @@
         <v>20</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="121"/>
+      <c r="H39" s="127"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -4098,8 +4115,8 @@
       <c r="B40" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="121"/>
-      <c r="D40" s="121"/>
+      <c r="C40" s="127"/>
+      <c r="D40" s="127"/>
       <c r="E40" s="1">
         <v>20</v>
       </c>
@@ -4109,7 +4126,7 @@
       <c r="G40" s="1">
         <v>20</v>
       </c>
-      <c r="H40" s="121"/>
+      <c r="H40" s="127"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1">
         <v>20</v>
@@ -4153,8 +4170,8 @@
       <c r="B41" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="121"/>
-      <c r="D41" s="121"/>
+      <c r="C41" s="127"/>
+      <c r="D41" s="127"/>
       <c r="E41" s="1">
         <v>20</v>
       </c>
@@ -4162,7 +4179,7 @@
         <v>20</v>
       </c>
       <c r="G41" s="1"/>
-      <c r="H41" s="121"/>
+      <c r="H41" s="127"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -4198,14 +4215,14 @@
       <c r="B42" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="121"/>
-      <c r="D42" s="121"/>
+      <c r="C42" s="127"/>
+      <c r="D42" s="127"/>
       <c r="E42" s="1">
         <v>20</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="121"/>
+      <c r="H42" s="127"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -4241,8 +4258,8 @@
       <c r="B43" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="121"/>
-      <c r="D43" s="121"/>
+      <c r="C43" s="127"/>
+      <c r="D43" s="127"/>
       <c r="E43" s="1">
         <v>20</v>
       </c>
@@ -4252,7 +4269,7 @@
       <c r="G43" s="1">
         <v>20</v>
       </c>
-      <c r="H43" s="121"/>
+      <c r="H43" s="127"/>
       <c r="I43" s="1">
         <v>20</v>
       </c>
@@ -4300,8 +4317,8 @@
       <c r="B44" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="121"/>
-      <c r="D44" s="121"/>
+      <c r="C44" s="127"/>
+      <c r="D44" s="127"/>
       <c r="E44" s="1">
         <v>20</v>
       </c>
@@ -4311,7 +4328,7 @@
       <c r="G44" s="1">
         <v>20</v>
       </c>
-      <c r="H44" s="121"/>
+      <c r="H44" s="127"/>
       <c r="I44" s="1">
         <v>20</v>
       </c>
@@ -4355,8 +4372,8 @@
       <c r="B45" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="121"/>
-      <c r="D45" s="121"/>
+      <c r="C45" s="127"/>
+      <c r="D45" s="127"/>
       <c r="E45" s="1">
         <v>20</v>
       </c>
@@ -4366,7 +4383,7 @@
       <c r="G45" s="1">
         <v>20</v>
       </c>
-      <c r="H45" s="121"/>
+      <c r="H45" s="127"/>
       <c r="I45" s="1">
         <v>15</v>
       </c>
@@ -4404,8 +4421,8 @@
       <c r="B46" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="121"/>
-      <c r="D46" s="121"/>
+      <c r="C46" s="127"/>
+      <c r="D46" s="127"/>
       <c r="E46" s="1">
         <v>20</v>
       </c>
@@ -4415,7 +4432,7 @@
       <c r="G46" s="1">
         <v>20</v>
       </c>
-      <c r="H46" s="121"/>
+      <c r="H46" s="127"/>
       <c r="I46" s="1">
         <v>20</v>
       </c>
@@ -4453,8 +4470,8 @@
       <c r="B47" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="121"/>
-      <c r="D47" s="121"/>
+      <c r="C47" s="127"/>
+      <c r="D47" s="127"/>
       <c r="E47" s="1">
         <v>20</v>
       </c>
@@ -4464,7 +4481,7 @@
       <c r="G47" s="1">
         <v>20</v>
       </c>
-      <c r="H47" s="121"/>
+      <c r="H47" s="127"/>
       <c r="I47" s="1">
         <v>20</v>
       </c>
@@ -4508,8 +4525,8 @@
       <c r="B48" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="121"/>
-      <c r="D48" s="121"/>
+      <c r="C48" s="127"/>
+      <c r="D48" s="127"/>
       <c r="E48" s="1">
         <v>20</v>
       </c>
@@ -4517,7 +4534,7 @@
         <v>20</v>
       </c>
       <c r="G48" s="1"/>
-      <c r="H48" s="121"/>
+      <c r="H48" s="127"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
@@ -4553,8 +4570,8 @@
       <c r="B49" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="121"/>
-      <c r="D49" s="121"/>
+      <c r="C49" s="127"/>
+      <c r="D49" s="127"/>
       <c r="E49" s="1">
         <v>20</v>
       </c>
@@ -4564,7 +4581,7 @@
       <c r="G49" s="1">
         <v>20</v>
       </c>
-      <c r="H49" s="121"/>
+      <c r="H49" s="127"/>
       <c r="I49" s="1">
         <v>20</v>
       </c>
@@ -4604,12 +4621,12 @@
       <c r="B50" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C50" s="121"/>
-      <c r="D50" s="121"/>
+      <c r="C50" s="127"/>
+      <c r="D50" s="127"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
-      <c r="H50" s="121"/>
+      <c r="H50" s="127"/>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
@@ -4645,12 +4662,12 @@
       <c r="B51" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="121"/>
-      <c r="D51" s="121"/>
+      <c r="C51" s="127"/>
+      <c r="D51" s="127"/>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
-      <c r="H51" s="121"/>
+      <c r="H51" s="127"/>
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
@@ -4686,12 +4703,12 @@
       <c r="B52" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="122"/>
-      <c r="D52" s="122"/>
+      <c r="C52" s="128"/>
+      <c r="D52" s="128"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="122"/>
+      <c r="H52" s="128"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -4728,58 +4745,58 @@
     <row r="56" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I58" s="132" t="s">
+      <c r="I58" s="135" t="s">
         <v>68</v>
       </c>
-      <c r="J58" s="133"/>
-      <c r="K58" s="133"/>
-      <c r="L58" s="133"/>
-      <c r="M58" s="134"/>
-      <c r="O58" s="140" t="s">
+      <c r="J58" s="136"/>
+      <c r="K58" s="136"/>
+      <c r="L58" s="136"/>
+      <c r="M58" s="137"/>
+      <c r="O58" s="143" t="s">
         <v>69</v>
       </c>
-      <c r="P58" s="133"/>
-      <c r="Q58" s="133"/>
-      <c r="R58" s="134"/>
+      <c r="P58" s="136"/>
+      <c r="Q58" s="136"/>
+      <c r="R58" s="137"/>
     </row>
     <row r="59" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I59" s="135" t="s">
+      <c r="I59" s="138" t="s">
         <v>70</v>
       </c>
-      <c r="J59" s="127"/>
-      <c r="K59" s="127"/>
-      <c r="L59" s="127"/>
-      <c r="M59" s="136"/>
-      <c r="O59" s="135" t="s">
+      <c r="J59" s="133"/>
+      <c r="K59" s="133"/>
+      <c r="L59" s="133"/>
+      <c r="M59" s="139"/>
+      <c r="O59" s="138" t="s">
         <v>71</v>
       </c>
-      <c r="P59" s="127"/>
-      <c r="Q59" s="127"/>
-      <c r="R59" s="136"/>
+      <c r="P59" s="133"/>
+      <c r="Q59" s="133"/>
+      <c r="R59" s="139"/>
     </row>
     <row r="60" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I60" s="137"/>
-      <c r="J60" s="138"/>
-      <c r="K60" s="138"/>
-      <c r="L60" s="138"/>
-      <c r="M60" s="139"/>
-      <c r="O60" s="137"/>
-      <c r="P60" s="138"/>
-      <c r="Q60" s="138"/>
-      <c r="R60" s="139"/>
+      <c r="I60" s="140"/>
+      <c r="J60" s="141"/>
+      <c r="K60" s="141"/>
+      <c r="L60" s="141"/>
+      <c r="M60" s="142"/>
+      <c r="O60" s="140"/>
+      <c r="P60" s="141"/>
+      <c r="Q60" s="141"/>
+      <c r="R60" s="142"/>
     </row>
     <row r="61" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I61" s="130" t="s">
-        <v>20</v>
-      </c>
-      <c r="J61" s="131"/>
-      <c r="K61" s="129"/>
-      <c r="L61" s="130" t="s">
+      <c r="I61" s="134" t="s">
+        <v>20</v>
+      </c>
+      <c r="J61" s="121"/>
+      <c r="K61" s="122"/>
+      <c r="L61" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="M61" s="129"/>
-      <c r="O61" s="130"/>
-      <c r="P61" s="129"/>
+      <c r="M61" s="122"/>
+      <c r="O61" s="134"/>
+      <c r="P61" s="122"/>
       <c r="Q61" s="11" t="s">
         <v>20</v>
       </c>
@@ -4788,38 +4805,38 @@
       </c>
     </row>
     <row r="62" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I62" s="141" t="s">
+      <c r="I62" s="120" t="s">
         <v>73</v>
       </c>
-      <c r="J62" s="131"/>
-      <c r="K62" s="129"/>
-      <c r="L62" s="142">
+      <c r="J62" s="121"/>
+      <c r="K62" s="122"/>
+      <c r="L62" s="123">
         <v>7350000</v>
       </c>
-      <c r="M62" s="129"/>
-      <c r="O62" s="128" t="s">
+      <c r="M62" s="122"/>
+      <c r="O62" s="124" t="s">
         <v>74</v>
       </c>
-      <c r="P62" s="129"/>
+      <c r="P62" s="122"/>
       <c r="Q62" s="12"/>
       <c r="R62" s="13">
         <v>40000</v>
       </c>
     </row>
     <row r="63" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I63" s="141" t="s">
+      <c r="I63" s="120" t="s">
         <v>75</v>
       </c>
-      <c r="J63" s="131"/>
-      <c r="K63" s="129"/>
-      <c r="L63" s="143">
+      <c r="J63" s="121"/>
+      <c r="K63" s="122"/>
+      <c r="L63" s="125">
         <v>1100000</v>
       </c>
-      <c r="M63" s="129"/>
-      <c r="O63" s="128" t="s">
+      <c r="M63" s="122"/>
+      <c r="O63" s="124" t="s">
         <v>76</v>
       </c>
-      <c r="P63" s="129"/>
+      <c r="P63" s="122"/>
       <c r="Q63" s="14" t="s">
         <v>77</v>
       </c>
@@ -4828,39 +4845,39 @@
       </c>
     </row>
     <row r="64" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I64" s="141" t="s">
+      <c r="I64" s="120" t="s">
         <v>78</v>
       </c>
-      <c r="J64" s="131"/>
-      <c r="K64" s="129"/>
-      <c r="L64" s="142">
+      <c r="J64" s="121"/>
+      <c r="K64" s="122"/>
+      <c r="L64" s="123">
         <f>L62+L63</f>
         <v>8450000</v>
       </c>
-      <c r="M64" s="129"/>
-      <c r="O64" s="128" t="s">
+      <c r="M64" s="122"/>
+      <c r="O64" s="124" t="s">
         <v>79</v>
       </c>
-      <c r="P64" s="129"/>
+      <c r="P64" s="122"/>
       <c r="Q64" s="12"/>
       <c r="R64" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="9:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I65" s="141" t="s">
+      <c r="I65" s="120" t="s">
         <v>80</v>
       </c>
-      <c r="J65" s="131"/>
-      <c r="K65" s="129"/>
-      <c r="L65" s="142">
+      <c r="J65" s="121"/>
+      <c r="K65" s="122"/>
+      <c r="L65" s="123">
         <v>8411850</v>
       </c>
-      <c r="M65" s="129"/>
-      <c r="O65" s="128" t="s">
+      <c r="M65" s="122"/>
+      <c r="O65" s="124" t="s">
         <v>81</v>
       </c>
-      <c r="P65" s="129"/>
+      <c r="P65" s="122"/>
       <c r="Q65" s="12"/>
       <c r="R65" s="13">
         <f>R62-R63+R64</f>
@@ -4868,20 +4885,20 @@
       </c>
     </row>
     <row r="66" spans="9:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I66" s="141" t="s">
+      <c r="I66" s="120" t="s">
         <v>82</v>
       </c>
-      <c r="J66" s="131"/>
-      <c r="K66" s="129"/>
-      <c r="L66" s="142">
+      <c r="J66" s="121"/>
+      <c r="K66" s="122"/>
+      <c r="L66" s="123">
         <f>L64-L65</f>
         <v>38150</v>
       </c>
-      <c r="M66" s="129"/>
-      <c r="O66" s="128" t="s">
+      <c r="M66" s="122"/>
+      <c r="O66" s="124" t="s">
         <v>83</v>
       </c>
-      <c r="P66" s="129"/>
+      <c r="P66" s="122"/>
       <c r="Q66" s="12"/>
       <c r="R66" s="13">
         <f>L66+R65</f>
@@ -5090,17 +5107,6 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="I66:K66"/>
-    <mergeCell ref="L65:M65"/>
-    <mergeCell ref="I65:K65"/>
-    <mergeCell ref="L66:M66"/>
-    <mergeCell ref="O66:P66"/>
-    <mergeCell ref="O65:P65"/>
-    <mergeCell ref="I64:K64"/>
-    <mergeCell ref="L64:M64"/>
-    <mergeCell ref="O64:P64"/>
-    <mergeCell ref="I63:K63"/>
-    <mergeCell ref="L63:M63"/>
     <mergeCell ref="C10:C52"/>
     <mergeCell ref="D10:D52"/>
     <mergeCell ref="H10:H52"/>
@@ -5116,12 +5122,23 @@
     <mergeCell ref="O62:P62"/>
     <mergeCell ref="O61:P61"/>
     <mergeCell ref="O59:R60"/>
+    <mergeCell ref="I64:K64"/>
+    <mergeCell ref="L64:M64"/>
+    <mergeCell ref="O64:P64"/>
+    <mergeCell ref="I63:K63"/>
+    <mergeCell ref="L63:M63"/>
+    <mergeCell ref="I66:K66"/>
+    <mergeCell ref="L65:M65"/>
+    <mergeCell ref="I65:K65"/>
+    <mergeCell ref="L66:M66"/>
+    <mergeCell ref="O66:P66"/>
+    <mergeCell ref="O65:P65"/>
   </mergeCells>
   <conditionalFormatting sqref="R10:R52">
-    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",R10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",R10)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5134,8 +5151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AM263"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6:P63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5175,42 +5192,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C2" s="158" t="s">
+      <c r="C2" s="150" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="125"/>
-      <c r="O2" s="125"/>
-      <c r="P2" s="126"/>
-      <c r="Q2" s="125"/>
-      <c r="R2" s="125"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="131"/>
+      <c r="P2" s="132"/>
+      <c r="Q2" s="131"/>
+      <c r="R2" s="131"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C3" s="126"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="127"/>
-      <c r="K3" s="127"/>
-      <c r="L3" s="127"/>
-      <c r="M3" s="127"/>
-      <c r="N3" s="127"/>
-      <c r="O3" s="127"/>
-      <c r="P3" s="127"/>
-      <c r="Q3" s="127"/>
-      <c r="R3" s="127"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="133"/>
+      <c r="K3" s="133"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="133"/>
+      <c r="N3" s="133"/>
+      <c r="O3" s="133"/>
+      <c r="P3" s="133"/>
+      <c r="Q3" s="133"/>
+      <c r="R3" s="133"/>
       <c r="W3" s="15"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
@@ -5286,25 +5303,25 @@
       <c r="T5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V5" s="144" t="s">
+      <c r="V5" s="154" t="s">
         <v>87</v>
       </c>
-      <c r="W5" s="131"/>
-      <c r="X5" s="131"/>
-      <c r="Y5" s="131"/>
-      <c r="Z5" s="131"/>
-      <c r="AA5" s="131"/>
-      <c r="AB5" s="131"/>
-      <c r="AC5" s="131"/>
-      <c r="AD5" s="131"/>
-      <c r="AE5" s="131"/>
-      <c r="AF5" s="131"/>
-      <c r="AG5" s="131"/>
-      <c r="AH5" s="131"/>
-      <c r="AI5" s="131"/>
-      <c r="AJ5" s="131"/>
-      <c r="AK5" s="131"/>
-      <c r="AL5" s="129"/>
+      <c r="W5" s="121"/>
+      <c r="X5" s="121"/>
+      <c r="Y5" s="121"/>
+      <c r="Z5" s="121"/>
+      <c r="AA5" s="121"/>
+      <c r="AB5" s="121"/>
+      <c r="AC5" s="121"/>
+      <c r="AD5" s="121"/>
+      <c r="AE5" s="121"/>
+      <c r="AF5" s="121"/>
+      <c r="AG5" s="121"/>
+      <c r="AH5" s="121"/>
+      <c r="AI5" s="121"/>
+      <c r="AJ5" s="121"/>
+      <c r="AK5" s="121"/>
+      <c r="AL5" s="122"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
@@ -5332,7 +5349,7 @@
       <c r="M6" s="22"/>
       <c r="N6" s="22"/>
       <c r="O6" s="22">
-        <f t="shared" ref="O6:O63" si="0">C6+D6+E6+F6+G6+I6+J6+K6+L6+M6+N6</f>
+        <f>SUM(C6:N6)</f>
         <v>30</v>
       </c>
       <c r="P6" s="104">
@@ -5344,37 +5361,37 @@
         <v>210</v>
       </c>
       <c r="R6" s="23">
-        <f t="shared" ref="R6:R63" si="1">Q6-60</f>
+        <f t="shared" ref="R6:R63" si="0">Q6-60</f>
         <v>150</v>
       </c>
       <c r="S6" s="24" t="str">
-        <f t="shared" ref="S6:S63" si="2">IF(R6&lt;=0,"OK","NO")</f>
+        <f t="shared" ref="S6:S63" si="1">IF(R6&lt;=0,"OK","NO")</f>
         <v>NO</v>
       </c>
       <c r="T6" s="22"/>
-      <c r="V6" s="159" t="s">
+      <c r="V6" s="151" t="s">
         <v>1</v>
       </c>
-      <c r="W6" s="159" t="s">
+      <c r="W6" s="151" t="s">
         <v>88</v>
       </c>
-      <c r="X6" s="144" t="s">
+      <c r="X6" s="154" t="s">
         <v>89</v>
       </c>
-      <c r="Y6" s="131"/>
-      <c r="Z6" s="131"/>
-      <c r="AA6" s="131"/>
-      <c r="AB6" s="131"/>
-      <c r="AC6" s="131"/>
-      <c r="AD6" s="131"/>
-      <c r="AE6" s="131"/>
-      <c r="AF6" s="131"/>
-      <c r="AG6" s="131"/>
-      <c r="AH6" s="131"/>
-      <c r="AI6" s="131"/>
-      <c r="AJ6" s="131"/>
-      <c r="AK6" s="131"/>
-      <c r="AL6" s="129"/>
+      <c r="Y6" s="121"/>
+      <c r="Z6" s="121"/>
+      <c r="AA6" s="121"/>
+      <c r="AB6" s="121"/>
+      <c r="AC6" s="121"/>
+      <c r="AD6" s="121"/>
+      <c r="AE6" s="121"/>
+      <c r="AF6" s="121"/>
+      <c r="AG6" s="121"/>
+      <c r="AH6" s="121"/>
+      <c r="AI6" s="121"/>
+      <c r="AJ6" s="121"/>
+      <c r="AK6" s="121"/>
+      <c r="AL6" s="122"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
@@ -5400,7 +5417,7 @@
       <c r="M7" s="22"/>
       <c r="N7" s="22"/>
       <c r="O7" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="O7:O63" si="2">SUM(C7:N7)</f>
         <v>10</v>
       </c>
       <c r="P7" s="104">
@@ -5412,35 +5429,35 @@
         <v>230</v>
       </c>
       <c r="R7" s="23">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+      <c r="S7" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>170</v>
-      </c>
-      <c r="S7" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T7" s="22"/>
-      <c r="V7" s="121"/>
-      <c r="W7" s="121"/>
-      <c r="X7" s="144" t="s">
+      <c r="V7" s="127"/>
+      <c r="W7" s="127"/>
+      <c r="X7" s="154" t="s">
         <v>90</v>
       </c>
-      <c r="Y7" s="131"/>
-      <c r="Z7" s="131"/>
-      <c r="AA7" s="129"/>
-      <c r="AB7" s="144" t="s">
+      <c r="Y7" s="121"/>
+      <c r="Z7" s="121"/>
+      <c r="AA7" s="122"/>
+      <c r="AB7" s="154" t="s">
         <v>91</v>
       </c>
-      <c r="AC7" s="131"/>
-      <c r="AD7" s="131"/>
-      <c r="AE7" s="131"/>
-      <c r="AF7" s="131"/>
-      <c r="AG7" s="131"/>
-      <c r="AH7" s="131"/>
-      <c r="AI7" s="131"/>
-      <c r="AJ7" s="131"/>
-      <c r="AK7" s="131"/>
-      <c r="AL7" s="129"/>
+      <c r="AC7" s="121"/>
+      <c r="AD7" s="121"/>
+      <c r="AE7" s="121"/>
+      <c r="AF7" s="121"/>
+      <c r="AG7" s="121"/>
+      <c r="AH7" s="121"/>
+      <c r="AI7" s="121"/>
+      <c r="AJ7" s="121"/>
+      <c r="AK7" s="121"/>
+      <c r="AL7" s="122"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
@@ -5462,7 +5479,7 @@
       <c r="M8" s="22"/>
       <c r="N8" s="22"/>
       <c r="O8" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P8" s="104">
@@ -5474,16 +5491,16 @@
         <v>240</v>
       </c>
       <c r="R8" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S8" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S8" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T8" s="22"/>
-      <c r="V8" s="122"/>
-      <c r="W8" s="122"/>
+      <c r="V8" s="128"/>
+      <c r="W8" s="128"/>
       <c r="X8" s="10" t="s">
         <v>20</v>
       </c>
@@ -5554,7 +5571,7 @@
       <c r="M9" s="22"/>
       <c r="N9" s="22"/>
       <c r="O9" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="P9" s="104">
@@ -5566,11 +5583,11 @@
         <v>230</v>
       </c>
       <c r="R9" s="23">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+      <c r="S9" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>170</v>
-      </c>
-      <c r="S9" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T9" s="22"/>
@@ -5635,7 +5652,7 @@
       <c r="M10" s="22"/>
       <c r="N10" s="22"/>
       <c r="O10" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P10" s="104">
@@ -5647,11 +5664,11 @@
         <v>240</v>
       </c>
       <c r="R10" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S10" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S10" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T10" s="22"/>
@@ -5728,7 +5745,7 @@
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
       <c r="O11" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P11" s="104">
@@ -5740,11 +5757,11 @@
         <v>240</v>
       </c>
       <c r="R11" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S11" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S11" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T11" s="22"/>
@@ -5815,7 +5832,7 @@
       <c r="M12" s="22"/>
       <c r="N12" s="22"/>
       <c r="O12" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P12" s="104">
@@ -5827,11 +5844,11 @@
         <v>240</v>
       </c>
       <c r="R12" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S12" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S12" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T12" s="22"/>
@@ -5902,7 +5919,7 @@
       <c r="M13" s="22"/>
       <c r="N13" s="22"/>
       <c r="O13" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P13" s="104">
@@ -5914,11 +5931,11 @@
         <v>240</v>
       </c>
       <c r="R13" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S13" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S13" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T13" s="22"/>
@@ -5989,7 +6006,7 @@
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>
       <c r="O14" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P14" s="104">
@@ -6001,11 +6018,11 @@
         <v>240</v>
       </c>
       <c r="R14" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S14" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S14" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T14" s="22"/>
@@ -6076,7 +6093,7 @@
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
       <c r="O15" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P15" s="104">
@@ -6088,11 +6105,11 @@
         <v>240</v>
       </c>
       <c r="R15" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S15" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S15" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T15" s="22"/>
@@ -6163,7 +6180,7 @@
       <c r="M16" s="22"/>
       <c r="N16" s="22"/>
       <c r="O16" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P16" s="104">
@@ -6175,11 +6192,11 @@
         <v>240</v>
       </c>
       <c r="R16" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S16" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S16" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T16" s="22"/>
@@ -6254,8 +6271,8 @@
       <c r="M17" s="22"/>
       <c r="N17" s="22"/>
       <c r="O17" s="22">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f t="shared" si="2"/>
+        <v>120</v>
       </c>
       <c r="P17" s="104">
         <f t="shared" si="3"/>
@@ -6263,14 +6280,14 @@
       </c>
       <c r="Q17" s="22">
         <f t="shared" si="4"/>
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="R17" s="23">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="S17" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="S17" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T17" s="22"/>
@@ -6335,7 +6352,7 @@
       <c r="M18" s="22"/>
       <c r="N18" s="22"/>
       <c r="O18" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="P18" s="104">
@@ -6347,11 +6364,11 @@
         <v>235</v>
       </c>
       <c r="R18" s="23">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="S18" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-      <c r="S18" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T18" s="22"/>
@@ -6424,7 +6441,7 @@
       <c r="M19" s="22"/>
       <c r="N19" s="22"/>
       <c r="O19" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P19" s="104">
@@ -6436,11 +6453,11 @@
         <v>240</v>
       </c>
       <c r="R19" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S19" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S19" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T19" s="22"/>
@@ -6515,7 +6532,7 @@
       <c r="M20" s="22"/>
       <c r="N20" s="22"/>
       <c r="O20" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="P20" s="104">
@@ -6527,11 +6544,11 @@
         <v>230</v>
       </c>
       <c r="R20" s="23">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+      <c r="S20" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>170</v>
-      </c>
-      <c r="S20" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T20" s="22"/>
@@ -6596,7 +6613,7 @@
       <c r="M21" s="22"/>
       <c r="N21" s="22"/>
       <c r="O21" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="P21" s="104">
@@ -6608,11 +6625,11 @@
         <v>235</v>
       </c>
       <c r="R21" s="23">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="S21" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-      <c r="S21" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T21" s="22"/>
@@ -6683,7 +6700,7 @@
       <c r="M22" s="22"/>
       <c r="N22" s="22"/>
       <c r="O22" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P22" s="104">
@@ -6695,11 +6712,11 @@
         <v>240</v>
       </c>
       <c r="R22" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S22" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S22" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T22" s="22"/>
@@ -6770,7 +6787,7 @@
       <c r="M23" s="22"/>
       <c r="N23" s="22"/>
       <c r="O23" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P23" s="104">
@@ -6782,11 +6799,11 @@
         <v>240</v>
       </c>
       <c r="R23" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S23" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S23" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T23" s="22"/>
@@ -6857,7 +6874,7 @@
       <c r="M24" s="22"/>
       <c r="N24" s="22"/>
       <c r="O24" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P24" s="104">
@@ -6869,11 +6886,11 @@
         <v>240</v>
       </c>
       <c r="R24" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S24" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S24" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T24" s="22"/>
@@ -6944,7 +6961,7 @@
       <c r="M25" s="22"/>
       <c r="N25" s="22"/>
       <c r="O25" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P25" s="104">
@@ -6956,11 +6973,11 @@
         <v>240</v>
       </c>
       <c r="R25" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S25" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S25" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T25" s="22"/>
@@ -7035,7 +7052,7 @@
       <c r="M26" s="22"/>
       <c r="N26" s="22"/>
       <c r="O26" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="P26" s="104">
@@ -7047,11 +7064,11 @@
         <v>230</v>
       </c>
       <c r="R26" s="23">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+      <c r="S26" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>170</v>
-      </c>
-      <c r="S26" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T26" s="22"/>
@@ -7128,7 +7145,7 @@
       <c r="M27" s="22"/>
       <c r="N27" s="22"/>
       <c r="O27" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="P27" s="104">
@@ -7140,11 +7157,11 @@
         <v>225</v>
       </c>
       <c r="R27" s="23">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="S27" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>165</v>
-      </c>
-      <c r="S27" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T27" s="22"/>
@@ -7221,7 +7238,7 @@
       <c r="M28" s="22"/>
       <c r="N28" s="22"/>
       <c r="O28" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>52.8</v>
       </c>
       <c r="P28" s="104">
@@ -7233,11 +7250,11 @@
         <v>187.2</v>
       </c>
       <c r="R28" s="23">
+        <f t="shared" si="0"/>
+        <v>127.19999999999999</v>
+      </c>
+      <c r="S28" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>127.19999999999999</v>
-      </c>
-      <c r="S28" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T28" s="22"/>
@@ -7308,7 +7325,7 @@
       <c r="M29" s="22"/>
       <c r="N29" s="22"/>
       <c r="O29" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P29" s="104">
@@ -7320,11 +7337,11 @@
         <v>240</v>
       </c>
       <c r="R29" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S29" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S29" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T29" s="22"/>
@@ -7395,7 +7412,7 @@
       <c r="M30" s="22"/>
       <c r="N30" s="22"/>
       <c r="O30" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P30" s="104">
@@ -7407,11 +7424,11 @@
         <v>240</v>
       </c>
       <c r="R30" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S30" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S30" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T30" s="22"/>
@@ -7482,7 +7499,7 @@
       <c r="M31" s="22"/>
       <c r="N31" s="22"/>
       <c r="O31" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P31" s="104">
@@ -7494,11 +7511,11 @@
         <v>240</v>
       </c>
       <c r="R31" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S31" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S31" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T31" s="22"/>
@@ -7569,7 +7586,7 @@
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
       <c r="O32" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P32" s="104">
@@ -7581,11 +7598,11 @@
         <v>240</v>
       </c>
       <c r="R32" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S32" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S32" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T32" s="22"/>
@@ -7656,7 +7673,7 @@
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
       <c r="O33" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P33" s="104">
@@ -7668,11 +7685,11 @@
         <v>240</v>
       </c>
       <c r="R33" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S33" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S33" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T33" s="22"/>
@@ -7745,7 +7762,7 @@
       <c r="M34" s="22"/>
       <c r="N34" s="22"/>
       <c r="O34" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="P34" s="104">
@@ -7757,11 +7774,11 @@
         <v>235</v>
       </c>
       <c r="R34" s="23">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="S34" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-      <c r="S34" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T34" s="22"/>
@@ -7834,7 +7851,7 @@
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
       <c r="O35" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="P35" s="104">
@@ -7846,11 +7863,11 @@
         <v>235</v>
       </c>
       <c r="R35" s="23">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="S35" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-      <c r="S35" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T35" s="22"/>
@@ -7931,7 +7948,7 @@
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
       <c r="O36" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="P36" s="104">
@@ -7943,11 +7960,11 @@
         <v>140</v>
       </c>
       <c r="R36" s="23">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="S36" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="S36" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T36" s="22"/>
@@ -8020,7 +8037,7 @@
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
       <c r="O37" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="P37" s="104">
@@ -8032,11 +8049,11 @@
         <v>235</v>
       </c>
       <c r="R37" s="23">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="S37" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-      <c r="S37" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T37" s="22"/>
@@ -8107,7 +8124,7 @@
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
       <c r="O38" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P38" s="104">
@@ -8119,11 +8136,11 @@
         <v>240</v>
       </c>
       <c r="R38" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S38" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S38" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T38" s="22"/>
@@ -8194,7 +8211,7 @@
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
       <c r="O39" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P39" s="104">
@@ -8206,11 +8223,11 @@
         <v>240</v>
       </c>
       <c r="R39" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S39" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S39" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T39" s="22"/>
@@ -8280,7 +8297,7 @@
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
       <c r="O40" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P40" s="104">
@@ -8292,11 +8309,11 @@
         <v>240</v>
       </c>
       <c r="R40" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S40" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S40" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T40" s="22"/>
@@ -8359,7 +8376,7 @@
       <c r="M41" s="22"/>
       <c r="N41" s="22"/>
       <c r="O41" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P41" s="104">
@@ -8371,11 +8388,11 @@
         <v>240</v>
       </c>
       <c r="R41" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S41" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S41" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T41" s="22"/>
@@ -8452,7 +8469,7 @@
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
       <c r="O42" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>37.4</v>
       </c>
       <c r="P42" s="104">
@@ -8464,11 +8481,11 @@
         <v>202.6</v>
       </c>
       <c r="R42" s="23">
+        <f t="shared" si="0"/>
+        <v>142.6</v>
+      </c>
+      <c r="S42" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>142.6</v>
-      </c>
-      <c r="S42" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T42" s="22"/>
@@ -8541,7 +8558,7 @@
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
       <c r="O43" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P43" s="104">
@@ -8553,11 +8570,11 @@
         <v>240</v>
       </c>
       <c r="R43" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S43" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S43" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T43" s="22"/>
@@ -8628,7 +8645,7 @@
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
       <c r="O44" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P44" s="104">
@@ -8640,11 +8657,11 @@
         <v>240</v>
       </c>
       <c r="R44" s="23">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S44" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S44" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T44" s="22"/>
@@ -8717,7 +8734,7 @@
       <c r="M45" s="22"/>
       <c r="N45" s="22"/>
       <c r="O45" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="P45" s="104">
@@ -8729,11 +8746,11 @@
         <v>235</v>
       </c>
       <c r="R45" s="23">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="S45" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-      <c r="S45" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T45" s="22"/>
@@ -8804,7 +8821,7 @@
       <c r="M46" s="22"/>
       <c r="N46" s="22"/>
       <c r="O46" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P46" s="104">
@@ -8816,11 +8833,11 @@
         <v>240</v>
       </c>
       <c r="R46" s="21">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S46" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S46" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T46" s="22"/>
@@ -8885,7 +8902,7 @@
       <c r="M47" s="22"/>
       <c r="N47" s="22"/>
       <c r="O47" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="P47" s="104">
@@ -8897,11 +8914,11 @@
         <v>235</v>
       </c>
       <c r="R47" s="21">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="S47" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-      <c r="S47" s="24" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T47" s="22"/>
@@ -8951,41 +8968,65 @@
       <c r="B48" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="119"/>
-      <c r="D48" s="119"/>
-      <c r="E48" s="42"/>
+      <c r="C48" s="119">
+        <v>20</v>
+      </c>
+      <c r="D48" s="119">
+        <v>20</v>
+      </c>
+      <c r="E48" s="42">
+        <v>20</v>
+      </c>
       <c r="F48" s="42">
-        <v>5</v>
-      </c>
-      <c r="G48" s="42"/>
-      <c r="H48" s="119"/>
-      <c r="I48" s="42"/>
-      <c r="J48" s="42"/>
-      <c r="K48" s="42"/>
-      <c r="L48" s="42"/>
-      <c r="M48" s="42"/>
-      <c r="N48" s="42"/>
+        <v>20</v>
+      </c>
+      <c r="G48" s="42">
+        <v>20</v>
+      </c>
+      <c r="H48" s="119">
+        <v>20</v>
+      </c>
+      <c r="I48" s="42">
+        <v>20</v>
+      </c>
+      <c r="J48" s="42">
+        <v>20</v>
+      </c>
+      <c r="K48" s="42">
+        <v>20</v>
+      </c>
+      <c r="L48" s="42">
+        <v>20</v>
+      </c>
+      <c r="M48" s="42">
+        <v>20</v>
+      </c>
+      <c r="N48" s="42">
+        <v>20</v>
+      </c>
       <c r="O48" s="22">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+      <c r="P48" s="104">
+        <f>120-SUM(C48:N48)</f>
+        <v>-120</v>
+      </c>
+      <c r="Q48" s="22">
+        <f>(240)-(O48)</f>
+        <v>0</v>
+      </c>
+      <c r="R48" s="41">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="P48" s="104">
-        <f t="shared" si="3"/>
-        <v>115</v>
-      </c>
-      <c r="Q48" s="22">
-        <f t="shared" si="4"/>
-        <v>235</v>
-      </c>
-      <c r="R48" s="41">
+        <v>-60</v>
+      </c>
+      <c r="S48" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-      <c r="S48" s="42" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-      <c r="T48" s="42"/>
+        <v>OK</v>
+      </c>
+      <c r="T48" s="42" t="s">
+        <v>185</v>
+      </c>
       <c r="V48" s="72"/>
       <c r="W48" s="72"/>
       <c r="X48" s="72"/>
@@ -9045,7 +9086,7 @@
       <c r="M49" s="10"/>
       <c r="N49" s="10"/>
       <c r="O49" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="P49" s="104">
@@ -9057,21 +9098,21 @@
         <v>180</v>
       </c>
       <c r="R49" s="21">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="S49" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="S49" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T49" s="3"/>
       <c r="V49" s="65"/>
       <c r="W49" s="65"/>
       <c r="X49" s="65"/>
-      <c r="Y49" s="160" t="s">
+      <c r="Y49" s="152" t="s">
         <v>145</v>
       </c>
-      <c r="Z49" s="161"/>
+      <c r="Z49" s="153"/>
       <c r="AA49" s="39">
         <f>SUM(AA9:AA21)</f>
         <v>20000</v>
@@ -9115,7 +9156,7 @@
       <c r="M50" s="10"/>
       <c r="N50" s="10"/>
       <c r="O50" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="P50" s="104">
@@ -9127,20 +9168,20 @@
         <v>245</v>
       </c>
       <c r="R50" s="21">
+        <f t="shared" si="0"/>
+        <v>185</v>
+      </c>
+      <c r="S50" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>185</v>
-      </c>
-      <c r="S50" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T50" s="3"/>
-      <c r="AG50" s="145" t="s">
+      <c r="AG50" s="156" t="s">
         <v>172</v>
       </c>
-      <c r="AH50" s="145"/>
-      <c r="AI50" s="145"/>
-      <c r="AJ50" s="145"/>
+      <c r="AH50" s="156"/>
+      <c r="AI50" s="156"/>
+      <c r="AJ50" s="156"/>
       <c r="AK50" s="90">
         <v>3087000</v>
       </c>
@@ -9170,7 +9211,7 @@
       <c r="M51" s="10"/>
       <c r="N51" s="10"/>
       <c r="O51" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="P51" s="104">
@@ -9182,11 +9223,11 @@
         <v>210</v>
       </c>
       <c r="R51" s="21">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="S51" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>150</v>
-      </c>
-      <c r="S51" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T51" s="3"/>
@@ -9197,12 +9238,12 @@
       <c r="AC51" s="45"/>
       <c r="AD51" s="45"/>
       <c r="AE51" s="45"/>
-      <c r="AG51" s="149" t="s">
+      <c r="AG51" s="160" t="s">
         <v>174</v>
       </c>
-      <c r="AH51" s="150"/>
-      <c r="AI51" s="150"/>
-      <c r="AJ51" s="151"/>
+      <c r="AH51" s="161"/>
+      <c r="AI51" s="161"/>
+      <c r="AJ51" s="162"/>
       <c r="AK51" s="102">
         <v>3077000</v>
       </c>
@@ -9230,7 +9271,7 @@
       <c r="M52" s="10"/>
       <c r="N52" s="10"/>
       <c r="O52" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="P52" s="104">
@@ -9242,11 +9283,11 @@
         <v>235</v>
       </c>
       <c r="R52" s="21">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="S52" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-      <c r="S52" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T52" s="3"/>
@@ -9258,12 +9299,12 @@
       <c r="AD52" s="45"/>
       <c r="AE52" s="45"/>
       <c r="AF52" s="45"/>
-      <c r="AG52" s="146" t="s">
+      <c r="AG52" s="157" t="s">
         <v>181</v>
       </c>
-      <c r="AH52" s="147"/>
-      <c r="AI52" s="147"/>
-      <c r="AJ52" s="148"/>
+      <c r="AH52" s="158"/>
+      <c r="AI52" s="158"/>
+      <c r="AJ52" s="159"/>
       <c r="AK52" s="106">
         <v>2550000</v>
       </c>
@@ -9301,8 +9342,8 @@
       <c r="M53" s="10"/>
       <c r="N53" s="10"/>
       <c r="O53" s="22">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f t="shared" si="2"/>
+        <v>120</v>
       </c>
       <c r="P53" s="104">
         <f t="shared" si="3"/>
@@ -9310,14 +9351,14 @@
       </c>
       <c r="Q53" s="22">
         <f t="shared" si="4"/>
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="R53" s="21">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="S53" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="S53" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T53" s="3"/>
@@ -9367,7 +9408,7 @@
       <c r="M54" s="10"/>
       <c r="N54" s="10"/>
       <c r="O54" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="P54" s="104">
@@ -9379,11 +9420,11 @@
         <v>235</v>
       </c>
       <c r="R54" s="21">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="S54" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-      <c r="S54" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T54" s="3"/>
@@ -9425,7 +9466,7 @@
       <c r="M55" s="10"/>
       <c r="N55" s="10"/>
       <c r="O55" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P55" s="104">
@@ -9437,11 +9478,11 @@
         <v>240</v>
       </c>
       <c r="R55" s="21">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S55" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S55" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T55" s="3"/>
@@ -9473,7 +9514,7 @@
       <c r="M56" s="10"/>
       <c r="N56" s="10"/>
       <c r="O56" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P56" s="104">
@@ -9485,20 +9526,20 @@
         <v>240</v>
       </c>
       <c r="R56" s="21">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S56" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S56" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T56" s="3"/>
-      <c r="AG56" s="149" t="s">
+      <c r="AG56" s="160" t="s">
         <v>179</v>
       </c>
-      <c r="AH56" s="150"/>
-      <c r="AI56" s="150"/>
-      <c r="AJ56" s="151"/>
+      <c r="AH56" s="161"/>
+      <c r="AI56" s="161"/>
+      <c r="AJ56" s="162"/>
       <c r="AK56" s="91">
         <f>AK55</f>
         <v>2627000</v>
@@ -9522,7 +9563,7 @@
       <c r="M57" s="10"/>
       <c r="N57" s="10"/>
       <c r="O57" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P57" s="104">
@@ -9534,20 +9575,20 @@
         <v>240</v>
       </c>
       <c r="R57" s="21">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S57" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S57" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T57" s="3"/>
-      <c r="AG57" s="145" t="s">
+      <c r="AG57" s="156" t="s">
         <v>171</v>
       </c>
-      <c r="AH57" s="145"/>
-      <c r="AI57" s="145"/>
-      <c r="AJ57" s="145"/>
+      <c r="AH57" s="156"/>
+      <c r="AI57" s="156"/>
+      <c r="AJ57" s="156"/>
       <c r="AK57" s="117">
         <f>AK51-AK56</f>
         <v>450000</v>
@@ -9571,7 +9612,7 @@
       <c r="M58" s="10"/>
       <c r="N58" s="10"/>
       <c r="O58" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P58" s="104">
@@ -9583,11 +9624,11 @@
         <v>240</v>
       </c>
       <c r="R58" s="21">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S58" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S58" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T58" s="3"/>
@@ -9610,7 +9651,7 @@
       <c r="M59" s="10"/>
       <c r="N59" s="10"/>
       <c r="O59" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P59" s="104">
@@ -9622,11 +9663,11 @@
         <v>240</v>
       </c>
       <c r="R59" s="21">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S59" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S59" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T59" s="3"/>
@@ -9649,7 +9690,7 @@
       <c r="M60" s="10"/>
       <c r="N60" s="10"/>
       <c r="O60" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P60" s="104">
@@ -9661,11 +9702,11 @@
         <v>240</v>
       </c>
       <c r="R60" s="21">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S60" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S60" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T60" s="3"/>
@@ -9687,7 +9728,7 @@
       <c r="M61" s="10"/>
       <c r="N61" s="10"/>
       <c r="O61" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P61" s="104">
@@ -9699,11 +9740,11 @@
         <v>240</v>
       </c>
       <c r="R61" s="21">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S61" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S61" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T61" s="3"/>
@@ -9724,7 +9765,7 @@
       <c r="M62" s="10"/>
       <c r="N62" s="10"/>
       <c r="O62" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P62" s="104">
@@ -9736,11 +9777,11 @@
         <v>240</v>
       </c>
       <c r="R62" s="21">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S62" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S62" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T62" s="3"/>
@@ -9761,7 +9802,7 @@
       <c r="M63" s="10"/>
       <c r="N63" s="10"/>
       <c r="O63" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P63" s="104">
@@ -9773,11 +9814,11 @@
         <v>240</v>
       </c>
       <c r="R63" s="21">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="S63" s="43" t="str">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="S63" s="43" t="str">
-        <f t="shared" si="2"/>
         <v>NO</v>
       </c>
       <c r="T63" s="3"/>
@@ -9785,32 +9826,32 @@
     <row r="64" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="152" t="s">
+      <c r="C66" s="144" t="s">
         <v>182</v>
       </c>
-      <c r="D66" s="153"/>
-      <c r="E66" s="153"/>
-      <c r="F66" s="153"/>
-      <c r="G66" s="154"/>
-      <c r="I66" s="162" t="s">
+      <c r="D66" s="145"/>
+      <c r="E66" s="145"/>
+      <c r="F66" s="145"/>
+      <c r="G66" s="146"/>
+      <c r="I66" s="155" t="s">
         <v>183</v>
       </c>
-      <c r="J66" s="162"/>
-      <c r="K66" s="162"/>
-      <c r="L66" s="162"/>
-      <c r="M66" s="162"/>
+      <c r="J66" s="155"/>
+      <c r="K66" s="155"/>
+      <c r="L66" s="155"/>
+      <c r="M66" s="155"/>
     </row>
     <row r="67" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="155"/>
-      <c r="D67" s="156"/>
-      <c r="E67" s="156"/>
-      <c r="F67" s="156"/>
-      <c r="G67" s="157"/>
-      <c r="I67" s="162"/>
-      <c r="J67" s="162"/>
-      <c r="K67" s="162"/>
-      <c r="L67" s="162"/>
-      <c r="M67" s="162"/>
+      <c r="C67" s="147"/>
+      <c r="D67" s="148"/>
+      <c r="E67" s="148"/>
+      <c r="F67" s="148"/>
+      <c r="G67" s="149"/>
+      <c r="I67" s="155"/>
+      <c r="J67" s="155"/>
+      <c r="K67" s="155"/>
+      <c r="L67" s="155"/>
+      <c r="M67" s="155"/>
     </row>
     <row r="68" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10010,13 +10051,6 @@
     <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C66:G67"/>
-    <mergeCell ref="C2:R3"/>
-    <mergeCell ref="W6:W8"/>
-    <mergeCell ref="V6:V8"/>
-    <mergeCell ref="Y49:Z49"/>
-    <mergeCell ref="X7:AA7"/>
-    <mergeCell ref="I66:M67"/>
     <mergeCell ref="AB7:AL7"/>
     <mergeCell ref="V5:AL5"/>
     <mergeCell ref="X6:AL6"/>
@@ -10025,44 +10059,59 @@
     <mergeCell ref="AG51:AJ51"/>
     <mergeCell ref="AG50:AJ50"/>
     <mergeCell ref="AG56:AJ56"/>
+    <mergeCell ref="C66:G67"/>
+    <mergeCell ref="C2:R3"/>
+    <mergeCell ref="W6:W8"/>
+    <mergeCell ref="V6:V8"/>
+    <mergeCell ref="Y49:Z49"/>
+    <mergeCell ref="X7:AA7"/>
+    <mergeCell ref="I66:M67"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:T63">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>IF(ISBLANK($B$4), 0, SEARCH($B$4,$B6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI9:AI48">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH(("YES"),(AI9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI9:AI48">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH(("NO"),(AI9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W9:AL9 W46:AA46 AB46:AJ48 AA47:AA48 W10:AJ45 AK10:AL48">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>IF(ISBLANK($X$4), 0, SEARCH($X$4,$W9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S6:S63">
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH(("NO"),(S6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S6:S63">
-    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH(("OK"),(S6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W10:W45">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>IF(AI10="YES",1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P6:P63">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="P48" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Ruman KAS (2019 LUNAS)
Tagihan KAS 2019
: 70k
Bayar : 70k
------------------------------- -
0k

Tagihan KAS 2019 LUNAS
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-2205" yWindow="555" windowWidth="19815" windowHeight="7365" tabRatio="533" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-2205" yWindow="555" windowWidth="19815" windowHeight="7365" tabRatio="533" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2018(NOT UPDATED)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="270">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -824,6 +824,12 @@
   </si>
   <si>
     <t>Ruman Bayar KAS 60k tunai</t>
+  </si>
+  <si>
+    <t>Ruman KAS 70k tunai</t>
+  </si>
+  <si>
+    <t>Dia KAS 200k tunai</t>
   </si>
 </sst>
 </file>
@@ -2400,29 +2406,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2438,37 +2435,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2476,28 +2475,185 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2512,33 +2668,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2557,133 +2692,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2695,47 +2719,29 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2778,15 +2784,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
@@ -3602,126 +3600,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="213" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="220"/>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="220"/>
-      <c r="K1" s="220"/>
-      <c r="L1" s="220"/>
-      <c r="M1" s="220"/>
-      <c r="N1" s="220"/>
-      <c r="O1" s="220"/>
-      <c r="P1" s="220"/>
-      <c r="Q1" s="220"/>
-      <c r="R1" s="220"/>
+      <c r="B1" s="214"/>
+      <c r="C1" s="214"/>
+      <c r="D1" s="214"/>
+      <c r="E1" s="214"/>
+      <c r="F1" s="214"/>
+      <c r="G1" s="214"/>
+      <c r="H1" s="214"/>
+      <c r="I1" s="214"/>
+      <c r="J1" s="214"/>
+      <c r="K1" s="214"/>
+      <c r="L1" s="214"/>
+      <c r="M1" s="214"/>
+      <c r="N1" s="214"/>
+      <c r="O1" s="214"/>
+      <c r="P1" s="214"/>
+      <c r="Q1" s="214"/>
+      <c r="R1" s="214"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="221"/>
-      <c r="B2" s="222"/>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="222"/>
-      <c r="H2" s="222"/>
-      <c r="I2" s="222"/>
-      <c r="J2" s="222"/>
-      <c r="K2" s="222"/>
-      <c r="L2" s="222"/>
-      <c r="M2" s="222"/>
-      <c r="N2" s="222"/>
-      <c r="O2" s="222"/>
-      <c r="P2" s="222"/>
-      <c r="Q2" s="222"/>
-      <c r="R2" s="222"/>
+      <c r="A2" s="215"/>
+      <c r="B2" s="216"/>
+      <c r="C2" s="216"/>
+      <c r="D2" s="216"/>
+      <c r="E2" s="216"/>
+      <c r="F2" s="216"/>
+      <c r="G2" s="216"/>
+      <c r="H2" s="216"/>
+      <c r="I2" s="216"/>
+      <c r="J2" s="216"/>
+      <c r="K2" s="216"/>
+      <c r="L2" s="216"/>
+      <c r="M2" s="216"/>
+      <c r="N2" s="216"/>
+      <c r="O2" s="216"/>
+      <c r="P2" s="216"/>
+      <c r="Q2" s="216"/>
+      <c r="R2" s="216"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="221"/>
-      <c r="B3" s="222"/>
-      <c r="C3" s="222"/>
-      <c r="D3" s="222"/>
-      <c r="E3" s="222"/>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="222"/>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="222"/>
-      <c r="M3" s="222"/>
-      <c r="N3" s="222"/>
-      <c r="O3" s="222"/>
-      <c r="P3" s="222"/>
-      <c r="Q3" s="222"/>
-      <c r="R3" s="222"/>
+      <c r="A3" s="215"/>
+      <c r="B3" s="216"/>
+      <c r="C3" s="216"/>
+      <c r="D3" s="216"/>
+      <c r="E3" s="216"/>
+      <c r="F3" s="216"/>
+      <c r="G3" s="216"/>
+      <c r="H3" s="216"/>
+      <c r="I3" s="216"/>
+      <c r="J3" s="216"/>
+      <c r="K3" s="216"/>
+      <c r="L3" s="216"/>
+      <c r="M3" s="216"/>
+      <c r="N3" s="216"/>
+      <c r="O3" s="216"/>
+      <c r="P3" s="216"/>
+      <c r="Q3" s="216"/>
+      <c r="R3" s="216"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="221"/>
-      <c r="B4" s="222"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="222"/>
-      <c r="H4" s="222"/>
-      <c r="I4" s="222"/>
-      <c r="J4" s="222"/>
-      <c r="K4" s="222"/>
-      <c r="L4" s="222"/>
-      <c r="M4" s="222"/>
-      <c r="N4" s="222"/>
-      <c r="O4" s="222"/>
-      <c r="P4" s="222"/>
-      <c r="Q4" s="222"/>
-      <c r="R4" s="222"/>
+      <c r="A4" s="215"/>
+      <c r="B4" s="216"/>
+      <c r="C4" s="216"/>
+      <c r="D4" s="216"/>
+      <c r="E4" s="216"/>
+      <c r="F4" s="216"/>
+      <c r="G4" s="216"/>
+      <c r="H4" s="216"/>
+      <c r="I4" s="216"/>
+      <c r="J4" s="216"/>
+      <c r="K4" s="216"/>
+      <c r="L4" s="216"/>
+      <c r="M4" s="216"/>
+      <c r="N4" s="216"/>
+      <c r="O4" s="216"/>
+      <c r="P4" s="216"/>
+      <c r="Q4" s="216"/>
+      <c r="R4" s="216"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="221"/>
-      <c r="B5" s="222"/>
-      <c r="C5" s="222"/>
-      <c r="D5" s="222"/>
-      <c r="E5" s="222"/>
-      <c r="F5" s="222"/>
-      <c r="G5" s="222"/>
-      <c r="H5" s="222"/>
-      <c r="I5" s="222"/>
-      <c r="J5" s="222"/>
-      <c r="K5" s="222"/>
-      <c r="L5" s="222"/>
-      <c r="M5" s="222"/>
-      <c r="N5" s="222"/>
-      <c r="O5" s="222"/>
-      <c r="P5" s="222"/>
-      <c r="Q5" s="222"/>
-      <c r="R5" s="222"/>
+      <c r="A5" s="215"/>
+      <c r="B5" s="216"/>
+      <c r="C5" s="216"/>
+      <c r="D5" s="216"/>
+      <c r="E5" s="216"/>
+      <c r="F5" s="216"/>
+      <c r="G5" s="216"/>
+      <c r="H5" s="216"/>
+      <c r="I5" s="216"/>
+      <c r="J5" s="216"/>
+      <c r="K5" s="216"/>
+      <c r="L5" s="216"/>
+      <c r="M5" s="216"/>
+      <c r="N5" s="216"/>
+      <c r="O5" s="216"/>
+      <c r="P5" s="216"/>
+      <c r="Q5" s="216"/>
+      <c r="R5" s="216"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="221"/>
-      <c r="B6" s="222"/>
-      <c r="C6" s="222"/>
-      <c r="D6" s="222"/>
-      <c r="E6" s="222"/>
-      <c r="F6" s="222"/>
-      <c r="G6" s="222"/>
-      <c r="H6" s="222"/>
-      <c r="I6" s="222"/>
-      <c r="J6" s="222"/>
-      <c r="K6" s="222"/>
-      <c r="L6" s="222"/>
-      <c r="M6" s="222"/>
-      <c r="N6" s="222"/>
-      <c r="O6" s="222"/>
-      <c r="P6" s="222"/>
-      <c r="Q6" s="222"/>
-      <c r="R6" s="222"/>
+      <c r="A6" s="215"/>
+      <c r="B6" s="216"/>
+      <c r="C6" s="216"/>
+      <c r="D6" s="216"/>
+      <c r="E6" s="216"/>
+      <c r="F6" s="216"/>
+      <c r="G6" s="216"/>
+      <c r="H6" s="216"/>
+      <c r="I6" s="216"/>
+      <c r="J6" s="216"/>
+      <c r="K6" s="216"/>
+      <c r="L6" s="216"/>
+      <c r="M6" s="216"/>
+      <c r="N6" s="216"/>
+      <c r="O6" s="216"/>
+      <c r="P6" s="216"/>
+      <c r="Q6" s="216"/>
+      <c r="R6" s="216"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -6666,58 +6664,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="224" t="s">
+      <c r="J79" s="221" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="225"/>
-      <c r="L79" s="225"/>
-      <c r="M79" s="225"/>
-      <c r="N79" s="226"/>
-      <c r="P79" s="232" t="s">
+      <c r="K79" s="222"/>
+      <c r="L79" s="222"/>
+      <c r="M79" s="222"/>
+      <c r="N79" s="223"/>
+      <c r="P79" s="229" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="225"/>
-      <c r="R79" s="225"/>
-      <c r="S79" s="226"/>
+      <c r="Q79" s="222"/>
+      <c r="R79" s="222"/>
+      <c r="S79" s="223"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="227" t="s">
+      <c r="J80" s="224" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="222"/>
-      <c r="L80" s="222"/>
-      <c r="M80" s="222"/>
-      <c r="N80" s="228"/>
-      <c r="P80" s="227" t="s">
+      <c r="K80" s="216"/>
+      <c r="L80" s="216"/>
+      <c r="M80" s="216"/>
+      <c r="N80" s="225"/>
+      <c r="P80" s="224" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="222"/>
-      <c r="R80" s="222"/>
-      <c r="S80" s="228"/>
+      <c r="Q80" s="216"/>
+      <c r="R80" s="216"/>
+      <c r="S80" s="225"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="229"/>
-      <c r="K81" s="230"/>
-      <c r="L81" s="230"/>
-      <c r="M81" s="230"/>
-      <c r="N81" s="231"/>
-      <c r="P81" s="229"/>
-      <c r="Q81" s="230"/>
-      <c r="R81" s="230"/>
-      <c r="S81" s="231"/>
+      <c r="J81" s="226"/>
+      <c r="K81" s="227"/>
+      <c r="L81" s="227"/>
+      <c r="M81" s="227"/>
+      <c r="N81" s="228"/>
+      <c r="P81" s="226"/>
+      <c r="Q81" s="227"/>
+      <c r="R81" s="227"/>
+      <c r="S81" s="228"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="223" t="s">
+      <c r="J82" s="219" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="214"/>
-      <c r="L82" s="215"/>
-      <c r="M82" s="223" t="s">
+      <c r="K82" s="220"/>
+      <c r="L82" s="218"/>
+      <c r="M82" s="219" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="215"/>
-      <c r="P82" s="223"/>
-      <c r="Q82" s="215"/>
+      <c r="N82" s="218"/>
+      <c r="P82" s="219"/>
+      <c r="Q82" s="218"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -6726,38 +6724,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="213" t="s">
+      <c r="J83" s="230" t="s">
         <v>70</v>
       </c>
-      <c r="K83" s="214"/>
-      <c r="L83" s="215"/>
-      <c r="M83" s="216">
+      <c r="K83" s="220"/>
+      <c r="L83" s="218"/>
+      <c r="M83" s="231">
         <v>7350000</v>
       </c>
-      <c r="N83" s="215"/>
+      <c r="N83" s="218"/>
       <c r="P83" s="217" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="215"/>
+      <c r="Q83" s="218"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="213" t="s">
+      <c r="J84" s="230" t="s">
         <v>72</v>
       </c>
-      <c r="K84" s="214"/>
-      <c r="L84" s="215"/>
-      <c r="M84" s="218">
+      <c r="K84" s="220"/>
+      <c r="L84" s="218"/>
+      <c r="M84" s="232">
         <v>1100000</v>
       </c>
-      <c r="N84" s="215"/>
+      <c r="N84" s="218"/>
       <c r="P84" s="217" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="215"/>
+      <c r="Q84" s="218"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -6766,39 +6764,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="213" t="s">
+      <c r="J85" s="230" t="s">
         <v>75</v>
       </c>
-      <c r="K85" s="214"/>
-      <c r="L85" s="215"/>
-      <c r="M85" s="216">
+      <c r="K85" s="220"/>
+      <c r="L85" s="218"/>
+      <c r="M85" s="231">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="215"/>
+      <c r="N85" s="218"/>
       <c r="P85" s="217" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="215"/>
+      <c r="Q85" s="218"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="213" t="s">
+      <c r="J86" s="230" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="214"/>
-      <c r="L86" s="215"/>
-      <c r="M86" s="216">
+      <c r="K86" s="220"/>
+      <c r="L86" s="218"/>
+      <c r="M86" s="231">
         <v>8411850</v>
       </c>
-      <c r="N86" s="215"/>
+      <c r="N86" s="218"/>
       <c r="P86" s="217" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="215"/>
+      <c r="Q86" s="218"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -6806,20 +6804,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="213" t="s">
+      <c r="J87" s="230" t="s">
         <v>79</v>
       </c>
-      <c r="K87" s="214"/>
-      <c r="L87" s="215"/>
-      <c r="M87" s="216">
+      <c r="K87" s="220"/>
+      <c r="L87" s="218"/>
+      <c r="M87" s="231">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="215"/>
+      <c r="N87" s="218"/>
       <c r="P87" s="217" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="215"/>
+      <c r="Q87" s="218"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -7008,6 +7006,17 @@
   </sheetData>
   <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="23">
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="P86:Q86"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="M84:N84"/>
     <mergeCell ref="A1:R6"/>
     <mergeCell ref="P84:Q84"/>
     <mergeCell ref="J82:L82"/>
@@ -7020,38 +7029,27 @@
     <mergeCell ref="P83:Q83"/>
     <mergeCell ref="P82:Q82"/>
     <mergeCell ref="P80:S81"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="P86:Q86"/>
   </mergeCells>
   <conditionalFormatting sqref="T10:T52">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S52">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S51">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>$S$12=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7064,7 +7062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BM260"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="L16" colorId="8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView defaultGridColor="0" topLeftCell="L16" colorId="8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
@@ -7107,46 +7105,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="241" t="s">
+      <c r="C2" s="253" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
-      <c r="H2" s="220"/>
-      <c r="I2" s="220"/>
-      <c r="J2" s="220"/>
-      <c r="K2" s="220"/>
-      <c r="L2" s="220"/>
-      <c r="M2" s="220"/>
-      <c r="N2" s="220"/>
-      <c r="O2" s="220"/>
-      <c r="P2" s="221"/>
-      <c r="Q2" s="221"/>
-      <c r="R2" s="221"/>
-      <c r="S2" s="220"/>
-      <c r="T2" s="220"/>
+      <c r="D2" s="214"/>
+      <c r="E2" s="214"/>
+      <c r="F2" s="214"/>
+      <c r="G2" s="214"/>
+      <c r="H2" s="214"/>
+      <c r="I2" s="214"/>
+      <c r="J2" s="214"/>
+      <c r="K2" s="214"/>
+      <c r="L2" s="214"/>
+      <c r="M2" s="214"/>
+      <c r="N2" s="214"/>
+      <c r="O2" s="214"/>
+      <c r="P2" s="215"/>
+      <c r="Q2" s="215"/>
+      <c r="R2" s="215"/>
+      <c r="S2" s="214"/>
+      <c r="T2" s="214"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="221"/>
-      <c r="D3" s="222"/>
-      <c r="E3" s="222"/>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="222"/>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="222"/>
-      <c r="M3" s="222"/>
-      <c r="N3" s="222"/>
-      <c r="O3" s="222"/>
-      <c r="P3" s="222"/>
-      <c r="Q3" s="222"/>
-      <c r="R3" s="222"/>
-      <c r="S3" s="222"/>
-      <c r="T3" s="222"/>
+      <c r="C3" s="215"/>
+      <c r="D3" s="216"/>
+      <c r="E3" s="216"/>
+      <c r="F3" s="216"/>
+      <c r="G3" s="216"/>
+      <c r="H3" s="216"/>
+      <c r="I3" s="216"/>
+      <c r="J3" s="216"/>
+      <c r="K3" s="216"/>
+      <c r="L3" s="216"/>
+      <c r="M3" s="216"/>
+      <c r="N3" s="216"/>
+      <c r="O3" s="216"/>
+      <c r="P3" s="216"/>
+      <c r="Q3" s="216"/>
+      <c r="R3" s="216"/>
+      <c r="S3" s="216"/>
+      <c r="T3" s="216"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7233,25 +7231,25 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="247" t="s">
+      <c r="X5" s="245" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="214"/>
-      <c r="Z5" s="214"/>
-      <c r="AA5" s="214"/>
-      <c r="AB5" s="214"/>
-      <c r="AC5" s="214"/>
-      <c r="AD5" s="214"/>
-      <c r="AE5" s="214"/>
-      <c r="AF5" s="214"/>
-      <c r="AG5" s="214"/>
-      <c r="AH5" s="214"/>
-      <c r="AI5" s="214"/>
-      <c r="AJ5" s="214"/>
-      <c r="AK5" s="214"/>
-      <c r="AL5" s="214"/>
-      <c r="AM5" s="214"/>
-      <c r="AN5" s="215"/>
+      <c r="Y5" s="220"/>
+      <c r="Z5" s="220"/>
+      <c r="AA5" s="220"/>
+      <c r="AB5" s="220"/>
+      <c r="AC5" s="220"/>
+      <c r="AD5" s="220"/>
+      <c r="AE5" s="220"/>
+      <c r="AF5" s="220"/>
+      <c r="AG5" s="220"/>
+      <c r="AH5" s="220"/>
+      <c r="AI5" s="220"/>
+      <c r="AJ5" s="220"/>
+      <c r="AK5" s="220"/>
+      <c r="AL5" s="220"/>
+      <c r="AM5" s="220"/>
+      <c r="AN5" s="218"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -7316,29 +7314,29 @@
         <v>NO</v>
       </c>
       <c r="V6" s="13"/>
-      <c r="X6" s="242" t="s">
+      <c r="X6" s="254" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="242" t="s">
+      <c r="Y6" s="254" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="246" t="s">
+      <c r="Z6" s="243" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="243"/>
-      <c r="AB6" s="243"/>
-      <c r="AC6" s="243"/>
-      <c r="AD6" s="243"/>
-      <c r="AE6" s="243"/>
-      <c r="AF6" s="243"/>
-      <c r="AG6" s="243"/>
-      <c r="AH6" s="243"/>
-      <c r="AI6" s="243"/>
-      <c r="AJ6" s="243"/>
-      <c r="AK6" s="243"/>
-      <c r="AL6" s="243"/>
-      <c r="AM6" s="243"/>
-      <c r="AN6" s="243"/>
+      <c r="AA6" s="244"/>
+      <c r="AB6" s="244"/>
+      <c r="AC6" s="244"/>
+      <c r="AD6" s="244"/>
+      <c r="AE6" s="244"/>
+      <c r="AF6" s="244"/>
+      <c r="AG6" s="244"/>
+      <c r="AH6" s="244"/>
+      <c r="AI6" s="244"/>
+      <c r="AJ6" s="244"/>
+      <c r="AK6" s="244"/>
+      <c r="AL6" s="244"/>
+      <c r="AM6" s="244"/>
+      <c r="AN6" s="244"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -7401,27 +7399,27 @@
         <v>NO</v>
       </c>
       <c r="V7" s="13"/>
-      <c r="X7" s="243"/>
-      <c r="Y7" s="243"/>
-      <c r="Z7" s="246" t="s">
+      <c r="X7" s="244"/>
+      <c r="Y7" s="244"/>
+      <c r="Z7" s="243" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="243"/>
-      <c r="AB7" s="243"/>
-      <c r="AC7" s="243"/>
-      <c r="AD7" s="246" t="s">
+      <c r="AA7" s="244"/>
+      <c r="AB7" s="244"/>
+      <c r="AC7" s="244"/>
+      <c r="AD7" s="243" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="243"/>
-      <c r="AF7" s="243"/>
-      <c r="AG7" s="243"/>
-      <c r="AH7" s="243"/>
-      <c r="AI7" s="243"/>
-      <c r="AJ7" s="243"/>
-      <c r="AK7" s="243"/>
-      <c r="AL7" s="243"/>
-      <c r="AM7" s="243"/>
-      <c r="AN7" s="243"/>
+      <c r="AE7" s="244"/>
+      <c r="AF7" s="244"/>
+      <c r="AG7" s="244"/>
+      <c r="AH7" s="244"/>
+      <c r="AI7" s="244"/>
+      <c r="AJ7" s="244"/>
+      <c r="AK7" s="244"/>
+      <c r="AL7" s="244"/>
+      <c r="AM7" s="244"/>
+      <c r="AN7" s="244"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -7471,8 +7469,8 @@
         <v>NO</v>
       </c>
       <c r="V8" s="13"/>
-      <c r="X8" s="243"/>
-      <c r="Y8" s="243"/>
+      <c r="X8" s="244"/>
+      <c r="Y8" s="244"/>
       <c r="Z8" s="172" t="s">
         <v>19</v>
       </c>
@@ -12017,10 +12015,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="244" t="s">
+      <c r="AA49" s="241" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="245"/>
+      <c r="AB49" s="242"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -12098,12 +12096,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="251" t="s">
+      <c r="AI50" s="237" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="252"/>
-      <c r="AK50" s="252"/>
-      <c r="AL50" s="253"/>
+      <c r="AJ50" s="238"/>
+      <c r="AK50" s="238"/>
+      <c r="AL50" s="239"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -12164,12 +12162,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="248" t="s">
+      <c r="AI51" s="234" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="249"/>
-      <c r="AK51" s="249"/>
-      <c r="AL51" s="250"/>
+      <c r="AJ51" s="235"/>
+      <c r="AK51" s="235"/>
+      <c r="AL51" s="236"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -12435,14 +12433,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="254"/>
-      <c r="AD55" s="254"/>
-      <c r="AI55" s="251" t="s">
+      <c r="AC55" s="240"/>
+      <c r="AD55" s="240"/>
+      <c r="AI55" s="237" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="252"/>
-      <c r="AK55" s="252"/>
-      <c r="AL55" s="253"/>
+      <c r="AJ55" s="238"/>
+      <c r="AK55" s="238"/>
+      <c r="AL55" s="239"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -12695,32 +12693,32 @@
     <row r="61" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="234" t="s">
+      <c r="C63" s="246" t="s">
         <v>177</v>
       </c>
-      <c r="D63" s="235"/>
-      <c r="E63" s="235"/>
-      <c r="F63" s="235"/>
-      <c r="G63" s="236"/>
-      <c r="I63" s="240" t="s">
+      <c r="D63" s="247"/>
+      <c r="E63" s="247"/>
+      <c r="F63" s="247"/>
+      <c r="G63" s="248"/>
+      <c r="I63" s="252" t="s">
         <v>178</v>
       </c>
-      <c r="J63" s="240"/>
-      <c r="K63" s="240"/>
-      <c r="L63" s="240"/>
-      <c r="M63" s="240"/>
+      <c r="J63" s="252"/>
+      <c r="K63" s="252"/>
+      <c r="L63" s="252"/>
+      <c r="M63" s="252"/>
     </row>
     <row r="64" spans="1:41" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="237"/>
-      <c r="D64" s="238"/>
-      <c r="E64" s="238"/>
-      <c r="F64" s="238"/>
-      <c r="G64" s="239"/>
-      <c r="I64" s="240"/>
-      <c r="J64" s="240"/>
-      <c r="K64" s="240"/>
-      <c r="L64" s="240"/>
-      <c r="M64" s="240"/>
+      <c r="C64" s="249"/>
+      <c r="D64" s="250"/>
+      <c r="E64" s="250"/>
+      <c r="F64" s="250"/>
+      <c r="G64" s="251"/>
+      <c r="I64" s="252"/>
+      <c r="J64" s="252"/>
+      <c r="K64" s="252"/>
+      <c r="L64" s="252"/>
+      <c r="M64" s="252"/>
     </row>
     <row r="65" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13210,74 +13208,75 @@
     <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="16">
-    <mergeCell ref="AI56:AL56"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AI50:AL50"/>
-    <mergeCell ref="AI55:AL55"/>
-    <mergeCell ref="AC55:AD55"/>
-    <mergeCell ref="AA49:AB49"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="AD7:AN7"/>
-    <mergeCell ref="X5:AN5"/>
-    <mergeCell ref="Z6:AN6"/>
     <mergeCell ref="P70:Q70"/>
     <mergeCell ref="C63:G64"/>
     <mergeCell ref="I63:M64"/>
     <mergeCell ref="C2:T3"/>
     <mergeCell ref="Y6:Y8"/>
     <mergeCell ref="X6:X8"/>
+    <mergeCell ref="AA49:AB49"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="AD7:AN7"/>
+    <mergeCell ref="X5:AN5"/>
+    <mergeCell ref="Z6:AN6"/>
+    <mergeCell ref="AI56:AL56"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AI50:AL50"/>
+    <mergeCell ref="AI55:AL55"/>
+    <mergeCell ref="AC55:AD55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:V60">
-    <cfRule type="expression" dxfId="11" priority="7">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>IF(ISBLANK($B$4), 0, SEARCH($B$4,$B6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK48">
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH(("YES"),(AK9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK48">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH(("NO"),(AK9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y9:AN9 Y46:AC46 AD46:AL48 AC47:AC48 Y10:AL45 AM10:AN48">
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="7" priority="10">
       <formula>IF(ISBLANK($Z$4), 0, SEARCH($Z$4,$Y9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6:U60">
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH(("NO"),(U6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6:U60">
-    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="5" priority="12" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH(("OK"),(U6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y10:Y45">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>IF(AK10="YES",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q6:R60">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6:P60">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y9:AN48">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>IF(ISBLANK($AA$4), 0, SEARCH($AA$4,$Y9))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13290,8 +13289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21:S21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13312,17 +13311,17 @@
       <c r="A2" s="199"/>
       <c r="B2" s="200"/>
       <c r="C2" s="200"/>
-      <c r="D2" s="316" t="s">
+      <c r="D2" s="263" t="s">
         <v>247</v>
       </c>
-      <c r="E2" s="316"/>
-      <c r="F2" s="316"/>
-      <c r="G2" s="316"/>
-      <c r="H2" s="316"/>
-      <c r="I2" s="316"/>
-      <c r="J2" s="316"/>
-      <c r="K2" s="316"/>
-      <c r="L2" s="316"/>
+      <c r="E2" s="263"/>
+      <c r="F2" s="263"/>
+      <c r="G2" s="263"/>
+      <c r="H2" s="263"/>
+      <c r="I2" s="263"/>
+      <c r="J2" s="263"/>
+      <c r="K2" s="263"/>
+      <c r="L2" s="263"/>
       <c r="M2" s="201"/>
       <c r="N2" s="24"/>
     </row>
@@ -13340,205 +13339,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="203"/>
-      <c r="U3" s="255" t="s">
+      <c r="U3" s="305" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="256"/>
-      <c r="W3" s="257" t="s">
+      <c r="V3" s="306"/>
+      <c r="W3" s="307" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="256"/>
-      <c r="Y3" s="256"/>
-      <c r="Z3" s="256"/>
-      <c r="AA3" s="256"/>
-      <c r="AB3" s="256"/>
-      <c r="AC3" s="256"/>
-      <c r="AD3" s="258"/>
+      <c r="X3" s="306"/>
+      <c r="Y3" s="306"/>
+      <c r="Z3" s="306"/>
+      <c r="AA3" s="306"/>
+      <c r="AB3" s="306"/>
+      <c r="AC3" s="306"/>
+      <c r="AD3" s="308"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="202"/>
-      <c r="B4" s="311" t="s">
+      <c r="B4" s="264" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="312"/>
-      <c r="D4" s="312"/>
-      <c r="E4" s="312"/>
-      <c r="F4" s="312"/>
+      <c r="C4" s="265"/>
+      <c r="D4" s="265"/>
+      <c r="E4" s="265"/>
+      <c r="F4" s="265"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="264" t="s">
+      <c r="I4" s="266" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="246"/>
-      <c r="K4" s="246"/>
-      <c r="L4" s="246"/>
+      <c r="J4" s="243"/>
+      <c r="K4" s="243"/>
+      <c r="L4" s="243"/>
       <c r="M4" s="203"/>
-      <c r="U4" s="276" t="s">
+      <c r="U4" s="280" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="246"/>
-      <c r="W4" s="264" t="s">
+      <c r="V4" s="243"/>
+      <c r="W4" s="266" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="246"/>
-      <c r="Y4" s="246"/>
-      <c r="Z4" s="246"/>
-      <c r="AA4" s="246"/>
-      <c r="AB4" s="246"/>
-      <c r="AC4" s="246"/>
-      <c r="AD4" s="259"/>
+      <c r="X4" s="243"/>
+      <c r="Y4" s="243"/>
+      <c r="Z4" s="243"/>
+      <c r="AA4" s="243"/>
+      <c r="AB4" s="243"/>
+      <c r="AC4" s="243"/>
+      <c r="AD4" s="279"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="202"/>
-      <c r="B5" s="281" t="s">
+      <c r="B5" s="273" t="s">
         <v>237</v>
       </c>
-      <c r="C5" s="246"/>
-      <c r="D5" s="246"/>
-      <c r="E5" s="246"/>
-      <c r="F5" s="246"/>
+      <c r="C5" s="243"/>
+      <c r="D5" s="243"/>
+      <c r="E5" s="243"/>
+      <c r="F5" s="243"/>
       <c r="G5" s="173">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="283" t="s">
+      <c r="I5" s="261" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="300"/>
-      <c r="K5" s="302">
+      <c r="J5" s="262"/>
+      <c r="K5" s="269">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="303"/>
+      <c r="L5" s="270"/>
       <c r="M5" s="203"/>
-      <c r="U5" s="277" t="s">
+      <c r="U5" s="301" t="s">
         <v>233</v>
       </c>
-      <c r="V5" s="278"/>
-      <c r="W5" s="283" t="s">
+      <c r="V5" s="302"/>
+      <c r="W5" s="261" t="s">
         <v>234</v>
       </c>
-      <c r="X5" s="284"/>
-      <c r="Y5" s="284"/>
-      <c r="Z5" s="284"/>
-      <c r="AA5" s="284"/>
-      <c r="AB5" s="284"/>
-      <c r="AC5" s="284"/>
-      <c r="AD5" s="285"/>
+      <c r="X5" s="291"/>
+      <c r="Y5" s="291"/>
+      <c r="Z5" s="291"/>
+      <c r="AA5" s="291"/>
+      <c r="AB5" s="291"/>
+      <c r="AC5" s="291"/>
+      <c r="AD5" s="292"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="202"/>
-      <c r="B6" s="274" t="s">
+      <c r="B6" s="255" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="275"/>
-      <c r="D6" s="275"/>
-      <c r="E6" s="275"/>
-      <c r="F6" s="275"/>
+      <c r="C6" s="256"/>
+      <c r="D6" s="256"/>
+      <c r="E6" s="256"/>
+      <c r="F6" s="256"/>
       <c r="G6" s="173">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="301" t="s">
+      <c r="I6" s="259" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="293"/>
-      <c r="K6" s="306">
+      <c r="J6" s="260"/>
+      <c r="K6" s="271">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="307"/>
+      <c r="L6" s="272"/>
       <c r="M6" s="203"/>
-      <c r="U6" s="279"/>
-      <c r="V6" s="280"/>
-      <c r="W6" s="265" t="s">
+      <c r="U6" s="303"/>
+      <c r="V6" s="304"/>
+      <c r="W6" s="293" t="s">
         <v>235</v>
       </c>
-      <c r="X6" s="266"/>
-      <c r="Y6" s="266"/>
-      <c r="Z6" s="266"/>
-      <c r="AA6" s="266"/>
-      <c r="AB6" s="266"/>
-      <c r="AC6" s="266"/>
-      <c r="AD6" s="267"/>
+      <c r="X6" s="294"/>
+      <c r="Y6" s="294"/>
+      <c r="Z6" s="294"/>
+      <c r="AA6" s="294"/>
+      <c r="AB6" s="294"/>
+      <c r="AC6" s="294"/>
+      <c r="AD6" s="295"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="202"/>
-      <c r="B7" s="291" t="s">
+      <c r="B7" s="276" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="292"/>
-      <c r="D7" s="292"/>
-      <c r="E7" s="292"/>
-      <c r="F7" s="293"/>
+      <c r="C7" s="277"/>
+      <c r="D7" s="277"/>
+      <c r="E7" s="277"/>
+      <c r="F7" s="260"/>
       <c r="G7" s="173">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="301" t="s">
+      <c r="I7" s="259" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="293"/>
-      <c r="K7" s="304">
+      <c r="J7" s="260"/>
+      <c r="K7" s="267">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="305"/>
+      <c r="L7" s="268"/>
       <c r="M7" s="203"/>
-      <c r="U7" s="262"/>
-      <c r="V7" s="263"/>
-      <c r="W7" s="264" t="s">
+      <c r="U7" s="309"/>
+      <c r="V7" s="310"/>
+      <c r="W7" s="266" t="s">
         <v>236</v>
       </c>
-      <c r="X7" s="246"/>
-      <c r="Y7" s="246"/>
-      <c r="Z7" s="246"/>
-      <c r="AA7" s="246"/>
-      <c r="AB7" s="246"/>
-      <c r="AC7" s="246"/>
-      <c r="AD7" s="259"/>
+      <c r="X7" s="243"/>
+      <c r="Y7" s="243"/>
+      <c r="Z7" s="243"/>
+      <c r="AA7" s="243"/>
+      <c r="AB7" s="243"/>
+      <c r="AC7" s="243"/>
+      <c r="AD7" s="279"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="202"/>
-      <c r="B8" s="313" t="s">
+      <c r="B8" s="274" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="314"/>
-      <c r="D8" s="314"/>
-      <c r="E8" s="314"/>
-      <c r="F8" s="314"/>
+      <c r="C8" s="275"/>
+      <c r="D8" s="275"/>
+      <c r="E8" s="275"/>
+      <c r="F8" s="275"/>
       <c r="G8" s="174">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="283" t="s">
+      <c r="I8" s="261" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="300"/>
-      <c r="K8" s="308">
+      <c r="J8" s="262"/>
+      <c r="K8" s="257">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="309"/>
+      <c r="L8" s="258"/>
       <c r="M8" s="203"/>
-      <c r="U8" s="270" t="s">
+      <c r="U8" s="313" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="271"/>
-      <c r="W8" s="265" t="s">
+      <c r="V8" s="314"/>
+      <c r="W8" s="293" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="266"/>
-      <c r="Y8" s="266"/>
-      <c r="Z8" s="266"/>
-      <c r="AA8" s="266"/>
-      <c r="AB8" s="266"/>
-      <c r="AC8" s="266"/>
-      <c r="AD8" s="267"/>
+      <c r="X8" s="294"/>
+      <c r="Y8" s="294"/>
+      <c r="Z8" s="294"/>
+      <c r="AA8" s="294"/>
+      <c r="AB8" s="294"/>
+      <c r="AC8" s="294"/>
+      <c r="AD8" s="295"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="202"/>
@@ -13554,28 +13553,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="203"/>
-      <c r="U9" s="272"/>
-      <c r="V9" s="273"/>
-      <c r="W9" s="265" t="s">
+      <c r="U9" s="315"/>
+      <c r="V9" s="316"/>
+      <c r="W9" s="293" t="s">
         <v>239</v>
       </c>
-      <c r="X9" s="266"/>
-      <c r="Y9" s="266"/>
-      <c r="Z9" s="266"/>
-      <c r="AA9" s="266"/>
-      <c r="AB9" s="266"/>
-      <c r="AC9" s="266"/>
-      <c r="AD9" s="267"/>
+      <c r="X9" s="294"/>
+      <c r="Y9" s="294"/>
+      <c r="Z9" s="294"/>
+      <c r="AA9" s="294"/>
+      <c r="AB9" s="294"/>
+      <c r="AC9" s="294"/>
+      <c r="AD9" s="295"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="202"/>
-      <c r="B10" s="246" t="s">
+      <c r="B10" s="243" t="s">
         <v>258</v>
       </c>
-      <c r="C10" s="246"/>
-      <c r="D10" s="246"/>
-      <c r="E10" s="246"/>
-      <c r="F10" s="246"/>
+      <c r="C10" s="243"/>
+      <c r="D10" s="243"/>
+      <c r="E10" s="243"/>
+      <c r="F10" s="243"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -13586,30 +13585,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="203"/>
-      <c r="U10" s="274" t="s">
+      <c r="U10" s="255" t="s">
         <v>246</v>
       </c>
-      <c r="V10" s="275"/>
-      <c r="W10" s="246" t="s">
+      <c r="V10" s="256"/>
+      <c r="W10" s="243" t="s">
         <v>263</v>
       </c>
-      <c r="X10" s="246"/>
-      <c r="Y10" s="246"/>
-      <c r="Z10" s="246"/>
-      <c r="AA10" s="246"/>
-      <c r="AB10" s="246"/>
-      <c r="AC10" s="246"/>
-      <c r="AD10" s="259"/>
+      <c r="X10" s="243"/>
+      <c r="Y10" s="243"/>
+      <c r="Z10" s="243"/>
+      <c r="AA10" s="243"/>
+      <c r="AB10" s="243"/>
+      <c r="AC10" s="243"/>
+      <c r="AD10" s="279"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="202"/>
-      <c r="B11" s="246" t="s">
+      <c r="B11" s="243" t="s">
         <v>259</v>
       </c>
-      <c r="C11" s="246"/>
-      <c r="D11" s="246"/>
-      <c r="E11" s="246"/>
-      <c r="F11" s="246"/>
+      <c r="C11" s="243"/>
+      <c r="D11" s="243"/>
+      <c r="E11" s="243"/>
+      <c r="F11" s="243"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -13619,30 +13618,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="203"/>
-      <c r="U11" s="274" t="s">
+      <c r="U11" s="255" t="s">
         <v>262</v>
       </c>
-      <c r="V11" s="275"/>
-      <c r="W11" s="268" t="s">
+      <c r="V11" s="256"/>
+      <c r="W11" s="311" t="s">
         <v>264</v>
       </c>
-      <c r="X11" s="268"/>
-      <c r="Y11" s="268"/>
-      <c r="Z11" s="268"/>
-      <c r="AA11" s="268"/>
-      <c r="AB11" s="268"/>
-      <c r="AC11" s="268"/>
-      <c r="AD11" s="269"/>
+      <c r="X11" s="311"/>
+      <c r="Y11" s="311"/>
+      <c r="Z11" s="311"/>
+      <c r="AA11" s="311"/>
+      <c r="AB11" s="311"/>
+      <c r="AC11" s="311"/>
+      <c r="AD11" s="312"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="202"/>
-      <c r="B12" s="315" t="s">
+      <c r="B12" s="278" t="s">
         <v>260</v>
       </c>
-      <c r="C12" s="315"/>
-      <c r="D12" s="315"/>
-      <c r="E12" s="315"/>
-      <c r="F12" s="315"/>
+      <c r="C12" s="278"/>
+      <c r="D12" s="278"/>
+      <c r="E12" s="278"/>
+      <c r="F12" s="278"/>
       <c r="G12" s="207">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -13653,16 +13652,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="203"/>
-      <c r="U12" s="274"/>
-      <c r="V12" s="275"/>
-      <c r="W12" s="246"/>
-      <c r="X12" s="246"/>
-      <c r="Y12" s="246"/>
-      <c r="Z12" s="246"/>
-      <c r="AA12" s="246"/>
-      <c r="AB12" s="246"/>
-      <c r="AC12" s="246"/>
-      <c r="AD12" s="259"/>
+      <c r="U12" s="255"/>
+      <c r="V12" s="256"/>
+      <c r="W12" s="243"/>
+      <c r="X12" s="243"/>
+      <c r="Y12" s="243"/>
+      <c r="Z12" s="243"/>
+      <c r="AA12" s="243"/>
+      <c r="AB12" s="243"/>
+      <c r="AC12" s="243"/>
+      <c r="AD12" s="279"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="204"/>
@@ -13678,221 +13677,223 @@
       <c r="K13" s="205"/>
       <c r="L13" s="205"/>
       <c r="M13" s="206"/>
-      <c r="U13" s="274"/>
-      <c r="V13" s="275"/>
-      <c r="W13" s="246"/>
-      <c r="X13" s="246"/>
-      <c r="Y13" s="246"/>
-      <c r="Z13" s="246"/>
-      <c r="AA13" s="246"/>
-      <c r="AB13" s="246"/>
-      <c r="AC13" s="246"/>
-      <c r="AD13" s="259"/>
+      <c r="U13" s="255"/>
+      <c r="V13" s="256"/>
+      <c r="W13" s="243"/>
+      <c r="X13" s="243"/>
+      <c r="Y13" s="243"/>
+      <c r="Z13" s="243"/>
+      <c r="AA13" s="243"/>
+      <c r="AB13" s="243"/>
+      <c r="AC13" s="243"/>
+      <c r="AD13" s="279"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="286"/>
-      <c r="V14" s="287"/>
-      <c r="W14" s="260"/>
-      <c r="X14" s="260"/>
-      <c r="Y14" s="260"/>
-      <c r="Z14" s="260"/>
-      <c r="AA14" s="260"/>
-      <c r="AB14" s="260"/>
-      <c r="AC14" s="260"/>
-      <c r="AD14" s="261"/>
+      <c r="U14" s="296"/>
+      <c r="V14" s="297"/>
+      <c r="W14" s="289"/>
+      <c r="X14" s="289"/>
+      <c r="Y14" s="289"/>
+      <c r="Z14" s="289"/>
+      <c r="AA14" s="289"/>
+      <c r="AB14" s="289"/>
+      <c r="AC14" s="289"/>
+      <c r="AD14" s="290"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="199"/>
       <c r="B18" s="200"/>
       <c r="C18" s="200"/>
-      <c r="D18" s="316" t="s">
+      <c r="D18" s="263" t="s">
         <v>252</v>
       </c>
-      <c r="E18" s="316"/>
-      <c r="F18" s="316"/>
-      <c r="G18" s="316"/>
-      <c r="H18" s="316"/>
-      <c r="I18" s="316"/>
-      <c r="J18" s="316"/>
-      <c r="K18" s="316"/>
-      <c r="L18" s="316"/>
+      <c r="E18" s="263"/>
+      <c r="F18" s="263"/>
+      <c r="G18" s="263"/>
+      <c r="H18" s="263"/>
+      <c r="I18" s="263"/>
+      <c r="J18" s="263"/>
+      <c r="K18" s="263"/>
+      <c r="L18" s="263"/>
       <c r="M18" s="201"/>
-      <c r="O18" s="288" t="s">
+      <c r="O18" s="298" t="s">
         <v>253</v>
       </c>
-      <c r="P18" s="289"/>
-      <c r="Q18" s="289"/>
-      <c r="R18" s="289"/>
-      <c r="S18" s="290"/>
+      <c r="P18" s="299"/>
+      <c r="Q18" s="299"/>
+      <c r="R18" s="299"/>
+      <c r="S18" s="300"/>
     </row>
     <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="202"/>
       <c r="M19" s="203"/>
-      <c r="O19" s="281" t="s">
+      <c r="O19" s="273" t="s">
         <v>254</v>
       </c>
-      <c r="P19" s="246"/>
-      <c r="Q19" s="246"/>
-      <c r="R19" s="246"/>
-      <c r="S19" s="259"/>
+      <c r="P19" s="243"/>
+      <c r="Q19" s="243"/>
+      <c r="R19" s="243"/>
+      <c r="S19" s="279"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="202"/>
-      <c r="B20" s="311" t="s">
+      <c r="B20" s="264" t="s">
         <v>257</v>
       </c>
-      <c r="C20" s="312"/>
-      <c r="D20" s="312"/>
-      <c r="E20" s="312"/>
-      <c r="F20" s="312"/>
+      <c r="C20" s="265"/>
+      <c r="D20" s="265"/>
+      <c r="E20" s="265"/>
+      <c r="F20" s="265"/>
       <c r="G20" s="70">
-        <v>160000</v>
+        <v>430000</v>
       </c>
       <c r="H20" s="24"/>
-      <c r="I20" s="264" t="s">
+      <c r="I20" s="266" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="246"/>
-      <c r="K20" s="246"/>
-      <c r="L20" s="246"/>
+      <c r="J20" s="243"/>
+      <c r="K20" s="243"/>
+      <c r="L20" s="243"/>
       <c r="M20" s="203"/>
-      <c r="O20" s="281" t="s">
+      <c r="O20" s="273" t="s">
         <v>255</v>
       </c>
-      <c r="P20" s="246"/>
-      <c r="Q20" s="246"/>
-      <c r="R20" s="246"/>
-      <c r="S20" s="259"/>
+      <c r="P20" s="243"/>
+      <c r="Q20" s="243"/>
+      <c r="R20" s="243"/>
+      <c r="S20" s="279"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="202"/>
-      <c r="B21" s="291" t="s">
+      <c r="B21" s="276" t="s">
         <v>237</v>
       </c>
-      <c r="C21" s="292"/>
-      <c r="D21" s="292"/>
-      <c r="E21" s="292"/>
-      <c r="F21" s="293"/>
+      <c r="C21" s="277"/>
+      <c r="D21" s="277"/>
+      <c r="E21" s="277"/>
+      <c r="F21" s="260"/>
       <c r="G21" s="173">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="283" t="s">
+      <c r="I21" s="261" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="300"/>
-      <c r="K21" s="302">
+      <c r="J21" s="262"/>
+      <c r="K21" s="269">
         <f>G23</f>
-        <v>2017729.1800000002</v>
-      </c>
-      <c r="L21" s="303"/>
+        <v>2287729.1800000002</v>
+      </c>
+      <c r="L21" s="270"/>
       <c r="M21" s="203"/>
       <c r="N21" s="197"/>
-      <c r="O21" s="281" t="s">
+      <c r="O21" s="273" t="s">
         <v>261</v>
       </c>
-      <c r="P21" s="246"/>
-      <c r="Q21" s="246"/>
-      <c r="R21" s="246"/>
-      <c r="S21" s="259"/>
+      <c r="P21" s="243"/>
+      <c r="Q21" s="243"/>
+      <c r="R21" s="243"/>
+      <c r="S21" s="279"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="202"/>
-      <c r="B22" s="294" t="s">
+      <c r="B22" s="282" t="s">
         <v>256</v>
       </c>
-      <c r="C22" s="295"/>
-      <c r="D22" s="295"/>
-      <c r="E22" s="295"/>
-      <c r="F22" s="296"/>
+      <c r="C22" s="283"/>
+      <c r="D22" s="283"/>
+      <c r="E22" s="283"/>
+      <c r="F22" s="284"/>
       <c r="G22" s="173">
         <v>200000</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="301" t="s">
+      <c r="I22" s="259" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="293"/>
-      <c r="K22" s="306">
+      <c r="J22" s="260"/>
+      <c r="K22" s="271">
         <f>Pengeluaran!L30</f>
         <v>46000</v>
       </c>
-      <c r="L22" s="307"/>
+      <c r="L22" s="272"/>
       <c r="M22" s="203"/>
       <c r="N22" s="197"/>
-      <c r="O22" s="276" t="s">
+      <c r="O22" s="280" t="s">
         <v>265</v>
       </c>
-      <c r="P22" s="264"/>
-      <c r="Q22" s="264"/>
-      <c r="R22" s="264"/>
-      <c r="S22" s="310"/>
+      <c r="P22" s="266"/>
+      <c r="Q22" s="266"/>
+      <c r="R22" s="266"/>
+      <c r="S22" s="281"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="202"/>
-      <c r="B23" s="291" t="s">
+      <c r="B23" s="276" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="292"/>
-      <c r="D23" s="292"/>
-      <c r="E23" s="292"/>
-      <c r="F23" s="293"/>
+      <c r="C23" s="277"/>
+      <c r="D23" s="277"/>
+      <c r="E23" s="277"/>
+      <c r="F23" s="260"/>
       <c r="G23" s="173">
         <f>SUM(G20:G22)</f>
-        <v>2017729.1800000002</v>
+        <v>2287729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="301" t="s">
+      <c r="I23" s="259" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="293"/>
-      <c r="K23" s="304">
+      <c r="J23" s="260"/>
+      <c r="K23" s="267">
         <f>Pemasukkan!F42</f>
         <v>0</v>
       </c>
-      <c r="L23" s="305"/>
+      <c r="L23" s="268"/>
       <c r="M23" s="203"/>
       <c r="N23" s="197"/>
-      <c r="O23" s="281" t="s">
+      <c r="O23" s="273" t="s">
         <v>267</v>
       </c>
-      <c r="P23" s="246"/>
-      <c r="Q23" s="246"/>
-      <c r="R23" s="246"/>
-      <c r="S23" s="259"/>
+      <c r="P23" s="243"/>
+      <c r="Q23" s="243"/>
+      <c r="R23" s="243"/>
+      <c r="S23" s="279"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="202"/>
-      <c r="B24" s="297" t="s">
+      <c r="B24" s="285" t="s">
         <v>192</v>
       </c>
-      <c r="C24" s="298"/>
-      <c r="D24" s="298"/>
-      <c r="E24" s="298"/>
-      <c r="F24" s="299"/>
+      <c r="C24" s="286"/>
+      <c r="D24" s="286"/>
+      <c r="E24" s="286"/>
+      <c r="F24" s="287"/>
       <c r="G24" s="174">
         <f>K24</f>
-        <v>1971729.1800000002</v>
+        <v>2241729.1800000002</v>
       </c>
       <c r="H24" s="24"/>
-      <c r="I24" s="283" t="s">
+      <c r="I24" s="261" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="300"/>
-      <c r="K24" s="308">
+      <c r="J24" s="262"/>
+      <c r="K24" s="257">
         <f>(K21-K22)+K23</f>
-        <v>1971729.1800000002</v>
-      </c>
-      <c r="L24" s="309"/>
+        <v>2241729.1800000002</v>
+      </c>
+      <c r="L24" s="258"/>
       <c r="M24" s="203"/>
       <c r="N24" s="197"/>
-      <c r="O24" s="281"/>
-      <c r="P24" s="246"/>
-      <c r="Q24" s="246"/>
-      <c r="R24" s="246"/>
-      <c r="S24" s="259"/>
+      <c r="O24" s="273" t="s">
+        <v>268</v>
+      </c>
+      <c r="P24" s="243"/>
+      <c r="Q24" s="243"/>
+      <c r="R24" s="243"/>
+      <c r="S24" s="279"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="202"/>
@@ -13909,11 +13910,13 @@
       <c r="L25" s="24"/>
       <c r="M25" s="203"/>
       <c r="N25" s="197"/>
-      <c r="O25" s="281"/>
-      <c r="P25" s="246"/>
-      <c r="Q25" s="246"/>
-      <c r="R25" s="246"/>
-      <c r="S25" s="259"/>
+      <c r="O25" s="273" t="s">
+        <v>269</v>
+      </c>
+      <c r="P25" s="243"/>
+      <c r="Q25" s="243"/>
+      <c r="R25" s="243"/>
+      <c r="S25" s="279"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="202"/>
@@ -13930,11 +13933,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="203"/>
       <c r="N26" s="197"/>
-      <c r="O26" s="281"/>
-      <c r="P26" s="246"/>
-      <c r="Q26" s="246"/>
-      <c r="R26" s="246"/>
-      <c r="S26" s="259"/>
+      <c r="O26" s="273"/>
+      <c r="P26" s="243"/>
+      <c r="Q26" s="243"/>
+      <c r="R26" s="243"/>
+      <c r="S26" s="279"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="204"/>
@@ -13951,11 +13954,11 @@
       <c r="L27" s="205"/>
       <c r="M27" s="206"/>
       <c r="N27" s="197"/>
-      <c r="O27" s="282"/>
-      <c r="P27" s="260"/>
-      <c r="Q27" s="260"/>
-      <c r="R27" s="260"/>
-      <c r="S27" s="261"/>
+      <c r="O27" s="288"/>
+      <c r="P27" s="289"/>
+      <c r="Q27" s="289"/>
+      <c r="R27" s="289"/>
+      <c r="S27" s="290"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="197"/>
@@ -13979,12 +13982,53 @@
       <c r="S28" s="197"/>
     </row>
   </sheetData>
+  <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="66">
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:AD3"/>
+    <mergeCell ref="W12:AD12"/>
+    <mergeCell ref="W13:AD13"/>
+    <mergeCell ref="W14:AD14"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:AD7"/>
+    <mergeCell ref="W9:AD9"/>
+    <mergeCell ref="W10:AD10"/>
+    <mergeCell ref="W11:AD11"/>
+    <mergeCell ref="U8:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:AD4"/>
+    <mergeCell ref="W8:AD8"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="O23:S23"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="O27:S27"/>
+    <mergeCell ref="W5:AD5"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="O25:S25"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="O18:S18"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O22:S22"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="I20:L20"/>
     <mergeCell ref="K7:L7"/>
@@ -14001,51 +14045,11 @@
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="D18:L18"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="O24:S24"/>
-    <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="O27:S27"/>
-    <mergeCell ref="W5:AD5"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="O25:S25"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="O18:S18"/>
-    <mergeCell ref="W4:AD4"/>
-    <mergeCell ref="W8:AD8"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="O23:S23"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:AD3"/>
-    <mergeCell ref="W12:AD12"/>
-    <mergeCell ref="W13:AD13"/>
-    <mergeCell ref="W14:AD14"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="W7:AD7"/>
-    <mergeCell ref="W9:AD9"/>
-    <mergeCell ref="W10:AD10"/>
-    <mergeCell ref="W11:AD11"/>
-    <mergeCell ref="U8:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="D2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -14078,44 +14082,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="326" t="s">
+      <c r="C2" s="317" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="327"/>
-      <c r="E2" s="327"/>
-      <c r="F2" s="327"/>
-      <c r="G2" s="327"/>
-      <c r="H2" s="327"/>
-      <c r="I2" s="327"/>
-      <c r="J2" s="327"/>
-      <c r="K2" s="327"/>
+      <c r="D2" s="318"/>
+      <c r="E2" s="318"/>
+      <c r="F2" s="318"/>
+      <c r="G2" s="318"/>
+      <c r="H2" s="318"/>
+      <c r="I2" s="318"/>
+      <c r="J2" s="318"/>
+      <c r="K2" s="318"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="327"/>
-      <c r="D3" s="327"/>
-      <c r="E3" s="327"/>
-      <c r="F3" s="327"/>
-      <c r="G3" s="327"/>
-      <c r="H3" s="327"/>
-      <c r="I3" s="327"/>
-      <c r="J3" s="327"/>
-      <c r="K3" s="327"/>
+      <c r="C3" s="318"/>
+      <c r="D3" s="318"/>
+      <c r="E3" s="318"/>
+      <c r="F3" s="318"/>
+      <c r="G3" s="318"/>
+      <c r="H3" s="318"/>
+      <c r="I3" s="318"/>
+      <c r="J3" s="318"/>
+      <c r="K3" s="318"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="319" t="s">
+      <c r="C5" s="325" t="s">
         <v>250</v>
       </c>
-      <c r="D5" s="319"/>
-      <c r="E5" s="319"/>
-      <c r="F5" s="319"/>
-      <c r="G5" s="319"/>
-      <c r="I5" s="319" t="s">
+      <c r="D5" s="325"/>
+      <c r="E5" s="325"/>
+      <c r="F5" s="325"/>
+      <c r="G5" s="325"/>
+      <c r="I5" s="325" t="s">
         <v>251</v>
       </c>
-      <c r="J5" s="319"/>
-      <c r="K5" s="319"/>
-      <c r="L5" s="319"/>
-      <c r="M5" s="319"/>
+      <c r="J5" s="325"/>
+      <c r="K5" s="325"/>
+      <c r="L5" s="325"/>
+      <c r="M5" s="325"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -14515,88 +14519,88 @@
       <c r="M28" s="197"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="311" t="s">
+      <c r="D29" s="264" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="312"/>
-      <c r="F29" s="320">
+      <c r="E29" s="265"/>
+      <c r="F29" s="319">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="321"/>
+      <c r="G29" s="320"/>
       <c r="I29" s="197"/>
-      <c r="J29" s="311" t="s">
+      <c r="J29" s="264" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="312"/>
-      <c r="L29" s="320">
+      <c r="K29" s="265"/>
+      <c r="L29" s="319">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
-        <v>2017729.1800000002</v>
-      </c>
-      <c r="M29" s="321"/>
+        <v>2287729.1800000002</v>
+      </c>
+      <c r="M29" s="320"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="276" t="s">
+      <c r="D30" s="280" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="246"/>
-      <c r="F30" s="322">
+      <c r="E30" s="243"/>
+      <c r="F30" s="321">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="323"/>
+      <c r="G30" s="322"/>
       <c r="I30" s="197"/>
-      <c r="J30" s="276" t="s">
+      <c r="J30" s="280" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="246"/>
-      <c r="L30" s="322">
+      <c r="K30" s="243"/>
+      <c r="L30" s="321">
         <f>Pengeluaran!L30</f>
         <v>46000</v>
       </c>
-      <c r="M30" s="323"/>
+      <c r="M30" s="322"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="281" t="s">
+      <c r="D31" s="273" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="246"/>
-      <c r="F31" s="324">
+      <c r="E31" s="243"/>
+      <c r="F31" s="326">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="325"/>
+      <c r="G31" s="327"/>
       <c r="I31" s="197"/>
-      <c r="J31" s="281" t="s">
+      <c r="J31" s="273" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="246"/>
-      <c r="L31" s="324">
+      <c r="K31" s="243"/>
+      <c r="L31" s="326">
         <f>L27</f>
         <v>0</v>
       </c>
-      <c r="M31" s="325"/>
+      <c r="M31" s="327"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="313" t="s">
+      <c r="D32" s="274" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="314"/>
-      <c r="F32" s="317">
+      <c r="E32" s="275"/>
+      <c r="F32" s="323">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="318"/>
+      <c r="G32" s="324"/>
       <c r="I32" s="197"/>
-      <c r="J32" s="313" t="s">
+      <c r="J32" s="274" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="314"/>
-      <c r="L32" s="317">
+      <c r="K32" s="275"/>
+      <c r="L32" s="323">
         <f>'Hitung Pemasukan Pengeluaran'!G24</f>
-        <v>1971729.1800000002</v>
-      </c>
-      <c r="M32" s="318"/>
+        <v>2241729.1800000002</v>
+      </c>
+      <c r="M32" s="324"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14789,12 +14793,6 @@
   </sheetData>
   <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="19">
-    <mergeCell ref="C2:K3"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J29:K29"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="I5:M5"/>
@@ -14808,6 +14806,12 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J32:K32"/>
+    <mergeCell ref="C2:K3"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -14839,44 +14843,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="332" t="s">
+      <c r="C2" s="328" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="333"/>
-      <c r="E2" s="333"/>
-      <c r="F2" s="333"/>
-      <c r="G2" s="333"/>
-      <c r="H2" s="333"/>
-      <c r="I2" s="333"/>
-      <c r="J2" s="333"/>
-      <c r="K2" s="333"/>
+      <c r="D2" s="329"/>
+      <c r="E2" s="329"/>
+      <c r="F2" s="329"/>
+      <c r="G2" s="329"/>
+      <c r="H2" s="329"/>
+      <c r="I2" s="329"/>
+      <c r="J2" s="329"/>
+      <c r="K2" s="329"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="333"/>
-      <c r="D3" s="333"/>
-      <c r="E3" s="333"/>
-      <c r="F3" s="333"/>
-      <c r="G3" s="333"/>
-      <c r="H3" s="333"/>
-      <c r="I3" s="333"/>
-      <c r="J3" s="333"/>
-      <c r="K3" s="333"/>
+      <c r="C3" s="329"/>
+      <c r="D3" s="329"/>
+      <c r="E3" s="329"/>
+      <c r="F3" s="329"/>
+      <c r="G3" s="329"/>
+      <c r="H3" s="329"/>
+      <c r="I3" s="329"/>
+      <c r="J3" s="329"/>
+      <c r="K3" s="329"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="319" t="s">
+      <c r="C5" s="325" t="s">
         <v>248</v>
       </c>
-      <c r="D5" s="319"/>
-      <c r="E5" s="319"/>
-      <c r="F5" s="319"/>
-      <c r="G5" s="319"/>
-      <c r="I5" s="319" t="s">
+      <c r="D5" s="325"/>
+      <c r="E5" s="325"/>
+      <c r="F5" s="325"/>
+      <c r="G5" s="325"/>
+      <c r="I5" s="325" t="s">
         <v>249</v>
       </c>
-      <c r="J5" s="319"/>
-      <c r="K5" s="319"/>
-      <c r="L5" s="319"/>
-      <c r="M5" s="319"/>
+      <c r="J5" s="325"/>
+      <c r="K5" s="325"/>
+      <c r="L5" s="325"/>
+      <c r="M5" s="325"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -15302,88 +15306,88 @@
       <c r="M28" s="197"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="255" t="s">
+      <c r="D29" s="305" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="257"/>
+      <c r="E29" s="307"/>
       <c r="F29" s="330">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
       <c r="G29" s="331"/>
       <c r="I29" s="197"/>
-      <c r="J29" s="255" t="s">
+      <c r="J29" s="305" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="257"/>
+      <c r="K29" s="307"/>
       <c r="L29" s="330">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
-        <v>2017729.1800000002</v>
+        <v>2287729.1800000002</v>
       </c>
       <c r="M29" s="331"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="281" t="s">
+      <c r="D30" s="273" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="246"/>
-      <c r="F30" s="322">
+      <c r="E30" s="243"/>
+      <c r="F30" s="321">
         <f>F27</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="323"/>
+      <c r="G30" s="322"/>
       <c r="I30" s="197"/>
-      <c r="J30" s="281" t="s">
+      <c r="J30" s="273" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="246"/>
-      <c r="L30" s="322">
+      <c r="K30" s="243"/>
+      <c r="L30" s="321">
         <f>L27</f>
         <v>46000</v>
       </c>
-      <c r="M30" s="323"/>
+      <c r="M30" s="322"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="281" t="s">
+      <c r="D31" s="273" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="246"/>
-      <c r="F31" s="324">
+      <c r="E31" s="243"/>
+      <c r="F31" s="326">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="325"/>
+      <c r="G31" s="327"/>
       <c r="I31" s="197"/>
-      <c r="J31" s="281" t="s">
+      <c r="J31" s="273" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="246"/>
-      <c r="L31" s="324">
+      <c r="K31" s="243"/>
+      <c r="L31" s="326">
         <f>Pemasukkan!L27</f>
         <v>0</v>
       </c>
-      <c r="M31" s="325"/>
+      <c r="M31" s="327"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="313" t="s">
+      <c r="D32" s="274" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="314"/>
-      <c r="F32" s="328">
+      <c r="E32" s="275"/>
+      <c r="F32" s="332">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="329"/>
+      <c r="G32" s="333"/>
       <c r="I32" s="197"/>
-      <c r="J32" s="313" t="s">
+      <c r="J32" s="274" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="314"/>
-      <c r="L32" s="328">
+      <c r="K32" s="275"/>
+      <c r="L32" s="332">
         <f>'Hitung Pemasukan Pengeluaran'!M8</f>
         <v>0</v>
       </c>
-      <c r="M32" s="329"/>
+      <c r="M32" s="333"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15576,6 +15580,14 @@
   </sheetData>
   <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="19">
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
     <mergeCell ref="C2:K3"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
@@ -15587,14 +15599,6 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Updated Format & Patch OH
Kas Tunai/Total KAS (*A) pada perhitungan pemasukan dan pengeluaran dimasukkan ke sheet pemasukkan

Dana KAS dikurangi sebanyak 320k untuk PATCH OH 2019
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-2205" yWindow="555" windowWidth="19815" windowHeight="7365" tabRatio="533" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-630" yWindow="570" windowWidth="19815" windowHeight="7365" tabRatio="533" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2018(NOT UPDATED)" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="Pengeluaran" sheetId="4" r:id="rId5"/>
     <sheet name="Inventaris" sheetId="7" r:id="rId6"/>
     <sheet name="Lampiran Polo" sheetId="3" r:id="rId7"/>
+    <sheet name="Patch OH" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="292">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -790,12 +791,6 @@
     <t>Josh Bayar KAS 130k Transfer</t>
   </si>
   <si>
-    <t xml:space="preserve"> Total KAS Dibayarkan (*T)</t>
-  </si>
-  <si>
-    <t>Total Uang KAS GAS (*A)</t>
-  </si>
-  <si>
     <t>Uang Rekening</t>
   </si>
   <si>
@@ -857,13 +852,58 @@
   </si>
   <si>
     <t>Simpanan 205k</t>
+  </si>
+  <si>
+    <t>Pendaftaran OH3</t>
+  </si>
+  <si>
+    <t>Risang,Arif,Adin,Duta,Tisang,Arkan,Don,Zelda,Puan(15k)</t>
+  </si>
+  <si>
+    <t>Patch OH</t>
+  </si>
+  <si>
+    <t>Harga /pcs</t>
+  </si>
+  <si>
+    <t>Pendaftaran OH</t>
+  </si>
+  <si>
+    <t>Total Harga patch</t>
+  </si>
+  <si>
+    <t>Patch OH 2019</t>
+  </si>
+  <si>
+    <t>Total Harga</t>
+  </si>
+  <si>
+    <t>Ambil dari KAS</t>
+  </si>
+  <si>
+    <t>18 September 2019</t>
+  </si>
+  <si>
+    <t>KAS Dibayarkan Transfer</t>
+  </si>
+  <si>
+    <t>Tas Plastik &amp; Amplop</t>
+  </si>
+  <si>
+    <t>Ambil tunai</t>
+  </si>
+  <si>
+    <t>Tombok untuk PATCH Tunai</t>
+  </si>
+  <si>
+    <t>KAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="13">
+  <numFmts count="14">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-[$Rp-421]* #,##0.00_-;\-[$Rp-421]* #,##0.00_-;_-[$Rp-421]* &quot;-&quot;??_-;_-@"/>
@@ -877,6 +917,7 @@
     <numFmt numFmtId="173" formatCode="[$IDR]\ #,##0.00_);\([$IDR]\ #,##0.00\)"/>
     <numFmt numFmtId="174" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="175" formatCode="0_);\(0\)"/>
+    <numFmt numFmtId="176" formatCode="[$IDR]\ #,##0_);\([$IDR]\ #,##0\)"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -924,6 +965,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1116,7 +1158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="75">
+  <borders count="78">
     <border>
       <left/>
       <right/>
@@ -1994,13 +2036,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="353">
+  <cellXfs count="371">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2443,14 +2522,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="4" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2458,14 +2578,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2481,39 +2596,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2521,36 +2634,209 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2558,187 +2844,43 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2747,31 +2889,16 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2780,18 +2907,6 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2826,6 +2941,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3650,126 +3783,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="234" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="220"/>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="220"/>
-      <c r="K1" s="220"/>
-      <c r="L1" s="220"/>
-      <c r="M1" s="220"/>
-      <c r="N1" s="220"/>
-      <c r="O1" s="220"/>
-      <c r="P1" s="220"/>
-      <c r="Q1" s="220"/>
-      <c r="R1" s="220"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="235"/>
+      <c r="K1" s="235"/>
+      <c r="L1" s="235"/>
+      <c r="M1" s="235"/>
+      <c r="N1" s="235"/>
+      <c r="O1" s="235"/>
+      <c r="P1" s="235"/>
+      <c r="Q1" s="235"/>
+      <c r="R1" s="235"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="221"/>
-      <c r="B2" s="222"/>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="222"/>
-      <c r="H2" s="222"/>
-      <c r="I2" s="222"/>
-      <c r="J2" s="222"/>
-      <c r="K2" s="222"/>
-      <c r="L2" s="222"/>
-      <c r="M2" s="222"/>
-      <c r="N2" s="222"/>
-      <c r="O2" s="222"/>
-      <c r="P2" s="222"/>
-      <c r="Q2" s="222"/>
-      <c r="R2" s="222"/>
+      <c r="A2" s="236"/>
+      <c r="B2" s="237"/>
+      <c r="C2" s="237"/>
+      <c r="D2" s="237"/>
+      <c r="E2" s="237"/>
+      <c r="F2" s="237"/>
+      <c r="G2" s="237"/>
+      <c r="H2" s="237"/>
+      <c r="I2" s="237"/>
+      <c r="J2" s="237"/>
+      <c r="K2" s="237"/>
+      <c r="L2" s="237"/>
+      <c r="M2" s="237"/>
+      <c r="N2" s="237"/>
+      <c r="O2" s="237"/>
+      <c r="P2" s="237"/>
+      <c r="Q2" s="237"/>
+      <c r="R2" s="237"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="221"/>
-      <c r="B3" s="222"/>
-      <c r="C3" s="222"/>
-      <c r="D3" s="222"/>
-      <c r="E3" s="222"/>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="222"/>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="222"/>
-      <c r="M3" s="222"/>
-      <c r="N3" s="222"/>
-      <c r="O3" s="222"/>
-      <c r="P3" s="222"/>
-      <c r="Q3" s="222"/>
-      <c r="R3" s="222"/>
+      <c r="A3" s="236"/>
+      <c r="B3" s="237"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
+      <c r="H3" s="237"/>
+      <c r="I3" s="237"/>
+      <c r="J3" s="237"/>
+      <c r="K3" s="237"/>
+      <c r="L3" s="237"/>
+      <c r="M3" s="237"/>
+      <c r="N3" s="237"/>
+      <c r="O3" s="237"/>
+      <c r="P3" s="237"/>
+      <c r="Q3" s="237"/>
+      <c r="R3" s="237"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="221"/>
-      <c r="B4" s="222"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="222"/>
-      <c r="H4" s="222"/>
-      <c r="I4" s="222"/>
-      <c r="J4" s="222"/>
-      <c r="K4" s="222"/>
-      <c r="L4" s="222"/>
-      <c r="M4" s="222"/>
-      <c r="N4" s="222"/>
-      <c r="O4" s="222"/>
-      <c r="P4" s="222"/>
-      <c r="Q4" s="222"/>
-      <c r="R4" s="222"/>
+      <c r="A4" s="236"/>
+      <c r="B4" s="237"/>
+      <c r="C4" s="237"/>
+      <c r="D4" s="237"/>
+      <c r="E4" s="237"/>
+      <c r="F4" s="237"/>
+      <c r="G4" s="237"/>
+      <c r="H4" s="237"/>
+      <c r="I4" s="237"/>
+      <c r="J4" s="237"/>
+      <c r="K4" s="237"/>
+      <c r="L4" s="237"/>
+      <c r="M4" s="237"/>
+      <c r="N4" s="237"/>
+      <c r="O4" s="237"/>
+      <c r="P4" s="237"/>
+      <c r="Q4" s="237"/>
+      <c r="R4" s="237"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="221"/>
-      <c r="B5" s="222"/>
-      <c r="C5" s="222"/>
-      <c r="D5" s="222"/>
-      <c r="E5" s="222"/>
-      <c r="F5" s="222"/>
-      <c r="G5" s="222"/>
-      <c r="H5" s="222"/>
-      <c r="I5" s="222"/>
-      <c r="J5" s="222"/>
-      <c r="K5" s="222"/>
-      <c r="L5" s="222"/>
-      <c r="M5" s="222"/>
-      <c r="N5" s="222"/>
-      <c r="O5" s="222"/>
-      <c r="P5" s="222"/>
-      <c r="Q5" s="222"/>
-      <c r="R5" s="222"/>
+      <c r="A5" s="236"/>
+      <c r="B5" s="237"/>
+      <c r="C5" s="237"/>
+      <c r="D5" s="237"/>
+      <c r="E5" s="237"/>
+      <c r="F5" s="237"/>
+      <c r="G5" s="237"/>
+      <c r="H5" s="237"/>
+      <c r="I5" s="237"/>
+      <c r="J5" s="237"/>
+      <c r="K5" s="237"/>
+      <c r="L5" s="237"/>
+      <c r="M5" s="237"/>
+      <c r="N5" s="237"/>
+      <c r="O5" s="237"/>
+      <c r="P5" s="237"/>
+      <c r="Q5" s="237"/>
+      <c r="R5" s="237"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="221"/>
-      <c r="B6" s="222"/>
-      <c r="C6" s="222"/>
-      <c r="D6" s="222"/>
-      <c r="E6" s="222"/>
-      <c r="F6" s="222"/>
-      <c r="G6" s="222"/>
-      <c r="H6" s="222"/>
-      <c r="I6" s="222"/>
-      <c r="J6" s="222"/>
-      <c r="K6" s="222"/>
-      <c r="L6" s="222"/>
-      <c r="M6" s="222"/>
-      <c r="N6" s="222"/>
-      <c r="O6" s="222"/>
-      <c r="P6" s="222"/>
-      <c r="Q6" s="222"/>
-      <c r="R6" s="222"/>
+      <c r="A6" s="236"/>
+      <c r="B6" s="237"/>
+      <c r="C6" s="237"/>
+      <c r="D6" s="237"/>
+      <c r="E6" s="237"/>
+      <c r="F6" s="237"/>
+      <c r="G6" s="237"/>
+      <c r="H6" s="237"/>
+      <c r="I6" s="237"/>
+      <c r="J6" s="237"/>
+      <c r="K6" s="237"/>
+      <c r="L6" s="237"/>
+      <c r="M6" s="237"/>
+      <c r="N6" s="237"/>
+      <c r="O6" s="237"/>
+      <c r="P6" s="237"/>
+      <c r="Q6" s="237"/>
+      <c r="R6" s="237"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -6714,58 +6847,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="227" t="s">
+      <c r="J79" s="239" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="228"/>
-      <c r="L79" s="228"/>
-      <c r="M79" s="228"/>
-      <c r="N79" s="229"/>
-      <c r="P79" s="235" t="s">
+      <c r="K79" s="240"/>
+      <c r="L79" s="240"/>
+      <c r="M79" s="240"/>
+      <c r="N79" s="241"/>
+      <c r="P79" s="247" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="228"/>
-      <c r="R79" s="228"/>
-      <c r="S79" s="229"/>
+      <c r="Q79" s="240"/>
+      <c r="R79" s="240"/>
+      <c r="S79" s="241"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="230" t="s">
+      <c r="J80" s="242" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="222"/>
-      <c r="L80" s="222"/>
-      <c r="M80" s="222"/>
-      <c r="N80" s="231"/>
-      <c r="P80" s="230" t="s">
+      <c r="K80" s="237"/>
+      <c r="L80" s="237"/>
+      <c r="M80" s="237"/>
+      <c r="N80" s="243"/>
+      <c r="P80" s="242" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="222"/>
-      <c r="R80" s="222"/>
-      <c r="S80" s="231"/>
+      <c r="Q80" s="237"/>
+      <c r="R80" s="237"/>
+      <c r="S80" s="243"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="232"/>
-      <c r="K81" s="233"/>
-      <c r="L81" s="233"/>
-      <c r="M81" s="233"/>
-      <c r="N81" s="234"/>
-      <c r="P81" s="232"/>
-      <c r="Q81" s="233"/>
-      <c r="R81" s="233"/>
-      <c r="S81" s="234"/>
+      <c r="J81" s="244"/>
+      <c r="K81" s="245"/>
+      <c r="L81" s="245"/>
+      <c r="M81" s="245"/>
+      <c r="N81" s="246"/>
+      <c r="P81" s="244"/>
+      <c r="Q81" s="245"/>
+      <c r="R81" s="245"/>
+      <c r="S81" s="246"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="225" t="s">
+      <c r="J82" s="238" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="226"/>
-      <c r="L82" s="224"/>
-      <c r="M82" s="225" t="s">
+      <c r="K82" s="229"/>
+      <c r="L82" s="230"/>
+      <c r="M82" s="238" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="224"/>
-      <c r="P82" s="225"/>
-      <c r="Q82" s="224"/>
+      <c r="N82" s="230"/>
+      <c r="P82" s="238"/>
+      <c r="Q82" s="230"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -6774,38 +6907,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="236" t="s">
+      <c r="J83" s="228" t="s">
         <v>70</v>
       </c>
-      <c r="K83" s="226"/>
-      <c r="L83" s="224"/>
-      <c r="M83" s="237">
+      <c r="K83" s="229"/>
+      <c r="L83" s="230"/>
+      <c r="M83" s="231">
         <v>7350000</v>
       </c>
-      <c r="N83" s="224"/>
-      <c r="P83" s="223" t="s">
+      <c r="N83" s="230"/>
+      <c r="P83" s="232" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="224"/>
+      <c r="Q83" s="230"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="236" t="s">
+      <c r="J84" s="228" t="s">
         <v>72</v>
       </c>
-      <c r="K84" s="226"/>
-      <c r="L84" s="224"/>
-      <c r="M84" s="238">
+      <c r="K84" s="229"/>
+      <c r="L84" s="230"/>
+      <c r="M84" s="233">
         <v>1100000</v>
       </c>
-      <c r="N84" s="224"/>
-      <c r="P84" s="223" t="s">
+      <c r="N84" s="230"/>
+      <c r="P84" s="232" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="224"/>
+      <c r="Q84" s="230"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -6814,39 +6947,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="236" t="s">
+      <c r="J85" s="228" t="s">
         <v>75</v>
       </c>
-      <c r="K85" s="226"/>
-      <c r="L85" s="224"/>
-      <c r="M85" s="237">
+      <c r="K85" s="229"/>
+      <c r="L85" s="230"/>
+      <c r="M85" s="231">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="224"/>
-      <c r="P85" s="223" t="s">
+      <c r="N85" s="230"/>
+      <c r="P85" s="232" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="224"/>
+      <c r="Q85" s="230"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="236" t="s">
+      <c r="J86" s="228" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="226"/>
-      <c r="L86" s="224"/>
-      <c r="M86" s="237">
+      <c r="K86" s="229"/>
+      <c r="L86" s="230"/>
+      <c r="M86" s="231">
         <v>8411850</v>
       </c>
-      <c r="N86" s="224"/>
-      <c r="P86" s="223" t="s">
+      <c r="N86" s="230"/>
+      <c r="P86" s="232" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="224"/>
+      <c r="Q86" s="230"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -6854,20 +6987,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="236" t="s">
+      <c r="J87" s="228" t="s">
         <v>79</v>
       </c>
-      <c r="K87" s="226"/>
-      <c r="L87" s="224"/>
-      <c r="M87" s="237">
+      <c r="K87" s="229"/>
+      <c r="L87" s="230"/>
+      <c r="M87" s="231">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="224"/>
-      <c r="P87" s="223" t="s">
+      <c r="N87" s="230"/>
+      <c r="P87" s="232" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="224"/>
+      <c r="Q87" s="230"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -7056,17 +7189,6 @@
   </sheetData>
   <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="23">
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="P86:Q86"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="M84:N84"/>
     <mergeCell ref="A1:R6"/>
     <mergeCell ref="P84:Q84"/>
     <mergeCell ref="J82:L82"/>
@@ -7079,6 +7201,17 @@
     <mergeCell ref="P83:Q83"/>
     <mergeCell ref="P82:Q82"/>
     <mergeCell ref="P80:S81"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="P86:Q86"/>
   </mergeCells>
   <conditionalFormatting sqref="T10:T52">
     <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
@@ -7112,7 +7245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BM260"/>
   <sheetViews>
-    <sheetView defaultGridColor="0" topLeftCell="N28" colorId="8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView defaultGridColor="0" topLeftCell="V28" colorId="8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="V49" sqref="V49"/>
     </sheetView>
   </sheetViews>
@@ -7155,46 +7288,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="259" t="s">
+      <c r="C2" s="256" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
-      <c r="H2" s="220"/>
-      <c r="I2" s="220"/>
-      <c r="J2" s="220"/>
-      <c r="K2" s="220"/>
-      <c r="L2" s="220"/>
-      <c r="M2" s="220"/>
-      <c r="N2" s="220"/>
-      <c r="O2" s="220"/>
-      <c r="P2" s="221"/>
-      <c r="Q2" s="221"/>
-      <c r="R2" s="221"/>
-      <c r="S2" s="220"/>
-      <c r="T2" s="220"/>
+      <c r="D2" s="235"/>
+      <c r="E2" s="235"/>
+      <c r="F2" s="235"/>
+      <c r="G2" s="235"/>
+      <c r="H2" s="235"/>
+      <c r="I2" s="235"/>
+      <c r="J2" s="235"/>
+      <c r="K2" s="235"/>
+      <c r="L2" s="235"/>
+      <c r="M2" s="235"/>
+      <c r="N2" s="235"/>
+      <c r="O2" s="235"/>
+      <c r="P2" s="236"/>
+      <c r="Q2" s="236"/>
+      <c r="R2" s="236"/>
+      <c r="S2" s="235"/>
+      <c r="T2" s="235"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="221"/>
-      <c r="D3" s="222"/>
-      <c r="E3" s="222"/>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="222"/>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="222"/>
-      <c r="M3" s="222"/>
-      <c r="N3" s="222"/>
-      <c r="O3" s="222"/>
-      <c r="P3" s="222"/>
-      <c r="Q3" s="222"/>
-      <c r="R3" s="222"/>
-      <c r="S3" s="222"/>
-      <c r="T3" s="222"/>
+      <c r="C3" s="236"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
+      <c r="H3" s="237"/>
+      <c r="I3" s="237"/>
+      <c r="J3" s="237"/>
+      <c r="K3" s="237"/>
+      <c r="L3" s="237"/>
+      <c r="M3" s="237"/>
+      <c r="N3" s="237"/>
+      <c r="O3" s="237"/>
+      <c r="P3" s="237"/>
+      <c r="Q3" s="237"/>
+      <c r="R3" s="237"/>
+      <c r="S3" s="237"/>
+      <c r="T3" s="237"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7281,25 +7414,25 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="251" t="s">
+      <c r="X5" s="262" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="226"/>
-      <c r="Z5" s="226"/>
-      <c r="AA5" s="226"/>
-      <c r="AB5" s="226"/>
-      <c r="AC5" s="226"/>
-      <c r="AD5" s="226"/>
-      <c r="AE5" s="226"/>
-      <c r="AF5" s="226"/>
-      <c r="AG5" s="226"/>
-      <c r="AH5" s="226"/>
-      <c r="AI5" s="226"/>
-      <c r="AJ5" s="226"/>
-      <c r="AK5" s="226"/>
-      <c r="AL5" s="226"/>
-      <c r="AM5" s="226"/>
-      <c r="AN5" s="224"/>
+      <c r="Y5" s="229"/>
+      <c r="Z5" s="229"/>
+      <c r="AA5" s="229"/>
+      <c r="AB5" s="229"/>
+      <c r="AC5" s="229"/>
+      <c r="AD5" s="229"/>
+      <c r="AE5" s="229"/>
+      <c r="AF5" s="229"/>
+      <c r="AG5" s="229"/>
+      <c r="AH5" s="229"/>
+      <c r="AI5" s="229"/>
+      <c r="AJ5" s="229"/>
+      <c r="AK5" s="229"/>
+      <c r="AL5" s="229"/>
+      <c r="AM5" s="229"/>
+      <c r="AN5" s="230"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -7364,29 +7497,29 @@
         <v>NO</v>
       </c>
       <c r="V6" s="13"/>
-      <c r="X6" s="260" t="s">
+      <c r="X6" s="257" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="260" t="s">
+      <c r="Y6" s="257" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="249" t="s">
+      <c r="Z6" s="261" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="250"/>
-      <c r="AB6" s="250"/>
-      <c r="AC6" s="250"/>
-      <c r="AD6" s="250"/>
-      <c r="AE6" s="250"/>
-      <c r="AF6" s="250"/>
-      <c r="AG6" s="250"/>
-      <c r="AH6" s="250"/>
-      <c r="AI6" s="250"/>
-      <c r="AJ6" s="250"/>
-      <c r="AK6" s="250"/>
-      <c r="AL6" s="250"/>
-      <c r="AM6" s="250"/>
-      <c r="AN6" s="250"/>
+      <c r="AA6" s="258"/>
+      <c r="AB6" s="258"/>
+      <c r="AC6" s="258"/>
+      <c r="AD6" s="258"/>
+      <c r="AE6" s="258"/>
+      <c r="AF6" s="258"/>
+      <c r="AG6" s="258"/>
+      <c r="AH6" s="258"/>
+      <c r="AI6" s="258"/>
+      <c r="AJ6" s="258"/>
+      <c r="AK6" s="258"/>
+      <c r="AL6" s="258"/>
+      <c r="AM6" s="258"/>
+      <c r="AN6" s="258"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -7449,27 +7582,27 @@
         <v>NO</v>
       </c>
       <c r="V7" s="13"/>
-      <c r="X7" s="250"/>
-      <c r="Y7" s="250"/>
-      <c r="Z7" s="249" t="s">
+      <c r="X7" s="258"/>
+      <c r="Y7" s="258"/>
+      <c r="Z7" s="261" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="250"/>
-      <c r="AB7" s="250"/>
-      <c r="AC7" s="250"/>
-      <c r="AD7" s="249" t="s">
+      <c r="AA7" s="258"/>
+      <c r="AB7" s="258"/>
+      <c r="AC7" s="258"/>
+      <c r="AD7" s="261" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="250"/>
-      <c r="AF7" s="250"/>
-      <c r="AG7" s="250"/>
-      <c r="AH7" s="250"/>
-      <c r="AI7" s="250"/>
-      <c r="AJ7" s="250"/>
-      <c r="AK7" s="250"/>
-      <c r="AL7" s="250"/>
-      <c r="AM7" s="250"/>
-      <c r="AN7" s="250"/>
+      <c r="AE7" s="258"/>
+      <c r="AF7" s="258"/>
+      <c r="AG7" s="258"/>
+      <c r="AH7" s="258"/>
+      <c r="AI7" s="258"/>
+      <c r="AJ7" s="258"/>
+      <c r="AK7" s="258"/>
+      <c r="AL7" s="258"/>
+      <c r="AM7" s="258"/>
+      <c r="AN7" s="258"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -7519,8 +7652,8 @@
         <v>NO</v>
       </c>
       <c r="V8" s="13"/>
-      <c r="X8" s="250"/>
-      <c r="Y8" s="250"/>
+      <c r="X8" s="258"/>
+      <c r="Y8" s="258"/>
       <c r="Z8" s="172" t="s">
         <v>19</v>
       </c>
@@ -11978,7 +12111,7 @@
         <v>OK</v>
       </c>
       <c r="V48" s="74" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="X48" s="57"/>
       <c r="Y48" s="59"/>
@@ -12067,10 +12200,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="247" t="s">
+      <c r="AA49" s="259" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="248"/>
+      <c r="AB49" s="260"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -12148,12 +12281,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="243" t="s">
+      <c r="AI50" s="266" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="244"/>
-      <c r="AK50" s="244"/>
-      <c r="AL50" s="245"/>
+      <c r="AJ50" s="267"/>
+      <c r="AK50" s="267"/>
+      <c r="AL50" s="268"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -12214,12 +12347,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="240" t="s">
+      <c r="AI51" s="263" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="241"/>
-      <c r="AK51" s="241"/>
-      <c r="AL51" s="242"/>
+      <c r="AJ51" s="264"/>
+      <c r="AK51" s="264"/>
+      <c r="AL51" s="265"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -12485,14 +12618,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="246"/>
-      <c r="AD55" s="246"/>
-      <c r="AI55" s="243" t="s">
+      <c r="AC55" s="269"/>
+      <c r="AD55" s="269"/>
+      <c r="AI55" s="266" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="244"/>
-      <c r="AK55" s="244"/>
-      <c r="AL55" s="245"/>
+      <c r="AJ55" s="267"/>
+      <c r="AK55" s="267"/>
+      <c r="AL55" s="268"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -12545,12 +12678,12 @@
         <v>NO</v>
       </c>
       <c r="V56" s="2"/>
-      <c r="AI56" s="239" t="s">
+      <c r="AI56" s="248" t="s">
         <v>168</v>
       </c>
-      <c r="AJ56" s="239"/>
-      <c r="AK56" s="239"/>
-      <c r="AL56" s="239"/>
+      <c r="AJ56" s="248"/>
+      <c r="AK56" s="248"/>
+      <c r="AL56" s="248"/>
       <c r="AM56" s="52">
         <f>AM50-AM55</f>
         <v>450000</v>
@@ -12745,32 +12878,32 @@
     <row r="61" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="252" t="s">
+      <c r="C63" s="249" t="s">
         <v>177</v>
       </c>
-      <c r="D63" s="253"/>
-      <c r="E63" s="253"/>
-      <c r="F63" s="253"/>
-      <c r="G63" s="254"/>
-      <c r="I63" s="258" t="s">
+      <c r="D63" s="250"/>
+      <c r="E63" s="250"/>
+      <c r="F63" s="250"/>
+      <c r="G63" s="251"/>
+      <c r="I63" s="255" t="s">
         <v>178</v>
       </c>
-      <c r="J63" s="258"/>
-      <c r="K63" s="258"/>
-      <c r="L63" s="258"/>
-      <c r="M63" s="258"/>
+      <c r="J63" s="255"/>
+      <c r="K63" s="255"/>
+      <c r="L63" s="255"/>
+      <c r="M63" s="255"/>
     </row>
     <row r="64" spans="1:41" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="255"/>
-      <c r="D64" s="256"/>
-      <c r="E64" s="256"/>
-      <c r="F64" s="256"/>
-      <c r="G64" s="257"/>
-      <c r="I64" s="258"/>
-      <c r="J64" s="258"/>
-      <c r="K64" s="258"/>
-      <c r="L64" s="258"/>
-      <c r="M64" s="258"/>
+      <c r="C64" s="252"/>
+      <c r="D64" s="253"/>
+      <c r="E64" s="253"/>
+      <c r="F64" s="253"/>
+      <c r="G64" s="254"/>
+      <c r="I64" s="255"/>
+      <c r="J64" s="255"/>
+      <c r="K64" s="255"/>
+      <c r="L64" s="255"/>
+      <c r="M64" s="255"/>
     </row>
     <row r="65" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12791,10 +12924,10 @@
       <c r="M70" s="55"/>
       <c r="N70" s="55"/>
       <c r="O70" s="55"/>
-      <c r="P70" s="239" t="s">
+      <c r="P70" s="248" t="s">
         <v>214</v>
       </c>
-      <c r="Q70" s="239"/>
+      <c r="Q70" s="248"/>
       <c r="R70" s="55"/>
       <c r="S70" s="55"/>
     </row>
@@ -13262,22 +13395,22 @@
   </sheetData>
   <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="16">
+    <mergeCell ref="AI56:AL56"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AI50:AL50"/>
+    <mergeCell ref="AI55:AL55"/>
+    <mergeCell ref="AC55:AD55"/>
+    <mergeCell ref="AA49:AB49"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="AD7:AN7"/>
+    <mergeCell ref="X5:AN5"/>
+    <mergeCell ref="Z6:AN6"/>
     <mergeCell ref="P70:Q70"/>
     <mergeCell ref="C63:G64"/>
     <mergeCell ref="I63:M64"/>
     <mergeCell ref="C2:T3"/>
     <mergeCell ref="Y6:Y8"/>
     <mergeCell ref="X6:X8"/>
-    <mergeCell ref="AA49:AB49"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="AD7:AN7"/>
-    <mergeCell ref="X5:AN5"/>
-    <mergeCell ref="Z6:AN6"/>
-    <mergeCell ref="AI56:AL56"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AI50:AL50"/>
-    <mergeCell ref="AI55:AL55"/>
-    <mergeCell ref="AC55:AD55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:V60">
     <cfRule type="expression" dxfId="10" priority="7">
@@ -13341,7 +13474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -13363,17 +13496,17 @@
       <c r="A2" s="199"/>
       <c r="B2" s="200"/>
       <c r="C2" s="200"/>
-      <c r="D2" s="261" t="s">
+      <c r="D2" s="330" t="s">
         <v>247</v>
       </c>
-      <c r="E2" s="261"/>
-      <c r="F2" s="261"/>
-      <c r="G2" s="261"/>
-      <c r="H2" s="261"/>
-      <c r="I2" s="261"/>
-      <c r="J2" s="261"/>
-      <c r="K2" s="261"/>
-      <c r="L2" s="261"/>
+      <c r="E2" s="330"/>
+      <c r="F2" s="330"/>
+      <c r="G2" s="330"/>
+      <c r="H2" s="330"/>
+      <c r="I2" s="330"/>
+      <c r="J2" s="330"/>
+      <c r="K2" s="330"/>
+      <c r="L2" s="330"/>
       <c r="M2" s="201"/>
       <c r="N2" s="24"/>
     </row>
@@ -13391,205 +13524,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="203"/>
-      <c r="U3" s="311" t="s">
+      <c r="U3" s="270" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="312"/>
-      <c r="W3" s="313" t="s">
+      <c r="V3" s="271"/>
+      <c r="W3" s="272" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="312"/>
-      <c r="Y3" s="312"/>
-      <c r="Z3" s="312"/>
-      <c r="AA3" s="312"/>
-      <c r="AB3" s="312"/>
-      <c r="AC3" s="312"/>
-      <c r="AD3" s="314"/>
+      <c r="X3" s="271"/>
+      <c r="Y3" s="271"/>
+      <c r="Z3" s="271"/>
+      <c r="AA3" s="271"/>
+      <c r="AB3" s="271"/>
+      <c r="AC3" s="271"/>
+      <c r="AD3" s="273"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="202"/>
-      <c r="B4" s="276" t="s">
+      <c r="B4" s="334" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="277"/>
-      <c r="D4" s="277"/>
-      <c r="E4" s="277"/>
-      <c r="F4" s="277"/>
+      <c r="C4" s="335"/>
+      <c r="D4" s="335"/>
+      <c r="E4" s="335"/>
+      <c r="F4" s="335"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="280" t="s">
+      <c r="I4" s="279" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="249"/>
-      <c r="K4" s="249"/>
-      <c r="L4" s="249"/>
+      <c r="J4" s="261"/>
+      <c r="K4" s="261"/>
+      <c r="L4" s="261"/>
       <c r="M4" s="203"/>
-      <c r="U4" s="323" t="s">
+      <c r="U4" s="291" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="249"/>
-      <c r="W4" s="280" t="s">
+      <c r="V4" s="261"/>
+      <c r="W4" s="279" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="249"/>
-      <c r="Y4" s="249"/>
-      <c r="Z4" s="249"/>
-      <c r="AA4" s="249"/>
-      <c r="AB4" s="249"/>
-      <c r="AC4" s="249"/>
-      <c r="AD4" s="300"/>
+      <c r="X4" s="261"/>
+      <c r="Y4" s="261"/>
+      <c r="Z4" s="261"/>
+      <c r="AA4" s="261"/>
+      <c r="AB4" s="261"/>
+      <c r="AC4" s="261"/>
+      <c r="AD4" s="274"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="202"/>
-      <c r="B5" s="271" t="s">
+      <c r="B5" s="296" t="s">
         <v>237</v>
       </c>
-      <c r="C5" s="249"/>
-      <c r="D5" s="249"/>
-      <c r="E5" s="249"/>
-      <c r="F5" s="249"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
       <c r="G5" s="173">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="269" t="s">
+      <c r="I5" s="298" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="270"/>
-      <c r="K5" s="281">
+      <c r="J5" s="322"/>
+      <c r="K5" s="324">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="282"/>
+      <c r="L5" s="325"/>
       <c r="M5" s="203"/>
-      <c r="U5" s="307" t="s">
+      <c r="U5" s="292" t="s">
         <v>233</v>
       </c>
-      <c r="V5" s="308"/>
-      <c r="W5" s="269" t="s">
+      <c r="V5" s="293"/>
+      <c r="W5" s="298" t="s">
         <v>234</v>
       </c>
-      <c r="X5" s="294"/>
-      <c r="Y5" s="294"/>
-      <c r="Z5" s="294"/>
-      <c r="AA5" s="294"/>
-      <c r="AB5" s="294"/>
-      <c r="AC5" s="294"/>
-      <c r="AD5" s="295"/>
+      <c r="X5" s="299"/>
+      <c r="Y5" s="299"/>
+      <c r="Z5" s="299"/>
+      <c r="AA5" s="299"/>
+      <c r="AB5" s="299"/>
+      <c r="AC5" s="299"/>
+      <c r="AD5" s="300"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="202"/>
-      <c r="B6" s="263" t="s">
+      <c r="B6" s="289" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="264"/>
-      <c r="D6" s="264"/>
-      <c r="E6" s="264"/>
-      <c r="F6" s="264"/>
+      <c r="C6" s="290"/>
+      <c r="D6" s="290"/>
+      <c r="E6" s="290"/>
+      <c r="F6" s="290"/>
       <c r="G6" s="173">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="267" t="s">
+      <c r="I6" s="323" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="268"/>
-      <c r="K6" s="283">
+      <c r="J6" s="318"/>
+      <c r="K6" s="326">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="284"/>
+      <c r="L6" s="327"/>
       <c r="M6" s="203"/>
-      <c r="U6" s="309"/>
-      <c r="V6" s="310"/>
-      <c r="W6" s="296" t="s">
+      <c r="U6" s="294"/>
+      <c r="V6" s="295"/>
+      <c r="W6" s="280" t="s">
         <v>235</v>
       </c>
-      <c r="X6" s="297"/>
-      <c r="Y6" s="297"/>
-      <c r="Z6" s="297"/>
-      <c r="AA6" s="297"/>
-      <c r="AB6" s="297"/>
-      <c r="AC6" s="297"/>
-      <c r="AD6" s="298"/>
+      <c r="X6" s="281"/>
+      <c r="Y6" s="281"/>
+      <c r="Z6" s="281"/>
+      <c r="AA6" s="281"/>
+      <c r="AB6" s="281"/>
+      <c r="AC6" s="281"/>
+      <c r="AD6" s="282"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="202"/>
-      <c r="B7" s="274" t="s">
+      <c r="B7" s="301" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="275"/>
-      <c r="D7" s="275"/>
-      <c r="E7" s="275"/>
-      <c r="F7" s="268"/>
+      <c r="C7" s="302"/>
+      <c r="D7" s="302"/>
+      <c r="E7" s="302"/>
+      <c r="F7" s="318"/>
       <c r="G7" s="173">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="267" t="s">
+      <c r="I7" s="323" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="268"/>
-      <c r="K7" s="278">
+      <c r="J7" s="318"/>
+      <c r="K7" s="328">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="279"/>
+      <c r="L7" s="329"/>
       <c r="M7" s="203"/>
-      <c r="U7" s="315"/>
-      <c r="V7" s="316"/>
-      <c r="W7" s="280" t="s">
+      <c r="U7" s="277"/>
+      <c r="V7" s="278"/>
+      <c r="W7" s="279" t="s">
         <v>236</v>
       </c>
-      <c r="X7" s="249"/>
-      <c r="Y7" s="249"/>
-      <c r="Z7" s="249"/>
-      <c r="AA7" s="249"/>
-      <c r="AB7" s="249"/>
-      <c r="AC7" s="249"/>
-      <c r="AD7" s="300"/>
+      <c r="X7" s="261"/>
+      <c r="Y7" s="261"/>
+      <c r="Z7" s="261"/>
+      <c r="AA7" s="261"/>
+      <c r="AB7" s="261"/>
+      <c r="AC7" s="261"/>
+      <c r="AD7" s="274"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="202"/>
-      <c r="B8" s="272" t="s">
+      <c r="B8" s="332" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="273"/>
-      <c r="D8" s="273"/>
-      <c r="E8" s="273"/>
-      <c r="F8" s="273"/>
+      <c r="C8" s="333"/>
+      <c r="D8" s="333"/>
+      <c r="E8" s="333"/>
+      <c r="F8" s="333"/>
       <c r="G8" s="174">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="269" t="s">
+      <c r="I8" s="298" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="270"/>
-      <c r="K8" s="265">
+      <c r="J8" s="322"/>
+      <c r="K8" s="310">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="266"/>
+      <c r="L8" s="311"/>
       <c r="M8" s="203"/>
-      <c r="U8" s="319" t="s">
+      <c r="U8" s="285" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="320"/>
-      <c r="W8" s="296" t="s">
+      <c r="V8" s="286"/>
+      <c r="W8" s="280" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="297"/>
-      <c r="Y8" s="297"/>
-      <c r="Z8" s="297"/>
-      <c r="AA8" s="297"/>
-      <c r="AB8" s="297"/>
-      <c r="AC8" s="297"/>
-      <c r="AD8" s="298"/>
+      <c r="X8" s="281"/>
+      <c r="Y8" s="281"/>
+      <c r="Z8" s="281"/>
+      <c r="AA8" s="281"/>
+      <c r="AB8" s="281"/>
+      <c r="AC8" s="281"/>
+      <c r="AD8" s="282"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="202"/>
@@ -13605,28 +13738,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="203"/>
-      <c r="U9" s="321"/>
-      <c r="V9" s="322"/>
-      <c r="W9" s="296" t="s">
+      <c r="U9" s="287"/>
+      <c r="V9" s="288"/>
+      <c r="W9" s="280" t="s">
         <v>239</v>
       </c>
-      <c r="X9" s="297"/>
-      <c r="Y9" s="297"/>
-      <c r="Z9" s="297"/>
-      <c r="AA9" s="297"/>
-      <c r="AB9" s="297"/>
-      <c r="AC9" s="297"/>
-      <c r="AD9" s="298"/>
+      <c r="X9" s="281"/>
+      <c r="Y9" s="281"/>
+      <c r="Z9" s="281"/>
+      <c r="AA9" s="281"/>
+      <c r="AB9" s="281"/>
+      <c r="AC9" s="281"/>
+      <c r="AD9" s="282"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="202"/>
-      <c r="B10" s="249" t="s">
-        <v>258</v>
-      </c>
-      <c r="C10" s="249"/>
-      <c r="D10" s="249"/>
-      <c r="E10" s="249"/>
-      <c r="F10" s="249"/>
+      <c r="B10" s="261" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" s="261"/>
+      <c r="D10" s="261"/>
+      <c r="E10" s="261"/>
+      <c r="F10" s="261"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -13637,30 +13770,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="203"/>
-      <c r="U10" s="263" t="s">
+      <c r="U10" s="289" t="s">
         <v>246</v>
       </c>
-      <c r="V10" s="264"/>
-      <c r="W10" s="249" t="s">
-        <v>262</v>
-      </c>
-      <c r="X10" s="249"/>
-      <c r="Y10" s="249"/>
-      <c r="Z10" s="249"/>
-      <c r="AA10" s="249"/>
-      <c r="AB10" s="249"/>
-      <c r="AC10" s="249"/>
-      <c r="AD10" s="300"/>
+      <c r="V10" s="290"/>
+      <c r="W10" s="261" t="s">
+        <v>260</v>
+      </c>
+      <c r="X10" s="261"/>
+      <c r="Y10" s="261"/>
+      <c r="Z10" s="261"/>
+      <c r="AA10" s="261"/>
+      <c r="AB10" s="261"/>
+      <c r="AC10" s="261"/>
+      <c r="AD10" s="274"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="202"/>
-      <c r="B11" s="249" t="s">
-        <v>259</v>
-      </c>
-      <c r="C11" s="249"/>
-      <c r="D11" s="249"/>
-      <c r="E11" s="249"/>
-      <c r="F11" s="249"/>
+      <c r="B11" s="261" t="s">
+        <v>257</v>
+      </c>
+      <c r="C11" s="261"/>
+      <c r="D11" s="261"/>
+      <c r="E11" s="261"/>
+      <c r="F11" s="261"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -13670,30 +13803,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="203"/>
-      <c r="U11" s="263" t="s">
+      <c r="U11" s="289" t="s">
+        <v>259</v>
+      </c>
+      <c r="V11" s="290"/>
+      <c r="W11" s="283" t="s">
         <v>261</v>
       </c>
-      <c r="V11" s="264"/>
-      <c r="W11" s="317" t="s">
-        <v>263</v>
-      </c>
-      <c r="X11" s="317"/>
-      <c r="Y11" s="317"/>
-      <c r="Z11" s="317"/>
-      <c r="AA11" s="317"/>
-      <c r="AB11" s="317"/>
-      <c r="AC11" s="317"/>
-      <c r="AD11" s="318"/>
+      <c r="X11" s="283"/>
+      <c r="Y11" s="283"/>
+      <c r="Z11" s="283"/>
+      <c r="AA11" s="283"/>
+      <c r="AB11" s="283"/>
+      <c r="AC11" s="283"/>
+      <c r="AD11" s="284"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="202"/>
-      <c r="B12" s="262" t="s">
-        <v>260</v>
-      </c>
-      <c r="C12" s="262"/>
-      <c r="D12" s="262"/>
-      <c r="E12" s="262"/>
-      <c r="F12" s="262"/>
+      <c r="B12" s="331" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" s="331"/>
+      <c r="D12" s="331"/>
+      <c r="E12" s="331"/>
+      <c r="F12" s="331"/>
       <c r="G12" s="207">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -13704,16 +13837,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="203"/>
-      <c r="U12" s="263"/>
-      <c r="V12" s="264"/>
-      <c r="W12" s="249"/>
-      <c r="X12" s="249"/>
-      <c r="Y12" s="249"/>
-      <c r="Z12" s="249"/>
-      <c r="AA12" s="249"/>
-      <c r="AB12" s="249"/>
-      <c r="AC12" s="249"/>
-      <c r="AD12" s="300"/>
+      <c r="U12" s="289"/>
+      <c r="V12" s="290"/>
+      <c r="W12" s="261"/>
+      <c r="X12" s="261"/>
+      <c r="Y12" s="261"/>
+      <c r="Z12" s="261"/>
+      <c r="AA12" s="261"/>
+      <c r="AB12" s="261"/>
+      <c r="AC12" s="261"/>
+      <c r="AD12" s="274"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="204"/>
@@ -13729,223 +13862,219 @@
       <c r="K13" s="205"/>
       <c r="L13" s="205"/>
       <c r="M13" s="206"/>
-      <c r="U13" s="263"/>
-      <c r="V13" s="264"/>
-      <c r="W13" s="249"/>
-      <c r="X13" s="249"/>
-      <c r="Y13" s="249"/>
-      <c r="Z13" s="249"/>
-      <c r="AA13" s="249"/>
-      <c r="AB13" s="249"/>
-      <c r="AC13" s="249"/>
-      <c r="AD13" s="300"/>
+      <c r="U13" s="289"/>
+      <c r="V13" s="290"/>
+      <c r="W13" s="261"/>
+      <c r="X13" s="261"/>
+      <c r="Y13" s="261"/>
+      <c r="Z13" s="261"/>
+      <c r="AA13" s="261"/>
+      <c r="AB13" s="261"/>
+      <c r="AC13" s="261"/>
+      <c r="AD13" s="274"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="301"/>
-      <c r="V14" s="302"/>
-      <c r="W14" s="292"/>
-      <c r="X14" s="292"/>
-      <c r="Y14" s="292"/>
-      <c r="Z14" s="292"/>
-      <c r="AA14" s="292"/>
-      <c r="AB14" s="292"/>
-      <c r="AC14" s="292"/>
-      <c r="AD14" s="293"/>
+      <c r="U14" s="304"/>
+      <c r="V14" s="305"/>
+      <c r="W14" s="275"/>
+      <c r="X14" s="275"/>
+      <c r="Y14" s="275"/>
+      <c r="Z14" s="275"/>
+      <c r="AA14" s="275"/>
+      <c r="AB14" s="275"/>
+      <c r="AC14" s="275"/>
+      <c r="AD14" s="276"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="199"/>
       <c r="B18" s="200"/>
       <c r="C18" s="200"/>
-      <c r="D18" s="261" t="s">
+      <c r="D18" s="330" t="s">
         <v>252</v>
       </c>
-      <c r="E18" s="261"/>
-      <c r="F18" s="261"/>
-      <c r="G18" s="261"/>
-      <c r="H18" s="261"/>
-      <c r="I18" s="261"/>
-      <c r="J18" s="261"/>
-      <c r="K18" s="261"/>
-      <c r="L18" s="261"/>
+      <c r="E18" s="330"/>
+      <c r="F18" s="330"/>
+      <c r="G18" s="330"/>
+      <c r="H18" s="330"/>
+      <c r="I18" s="330"/>
+      <c r="J18" s="330"/>
+      <c r="K18" s="330"/>
+      <c r="L18" s="330"/>
       <c r="M18" s="201"/>
-      <c r="O18" s="303" t="s">
+      <c r="O18" s="306" t="s">
         <v>253</v>
       </c>
-      <c r="P18" s="304"/>
-      <c r="Q18" s="304"/>
-      <c r="R18" s="304"/>
-      <c r="S18" s="305"/>
-    </row>
-    <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P18" s="307"/>
+      <c r="Q18" s="307"/>
+      <c r="R18" s="307"/>
+      <c r="S18" s="308"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="202"/>
       <c r="M19" s="203"/>
-      <c r="O19" s="271" t="s">
+      <c r="O19" s="296" t="s">
         <v>254</v>
       </c>
-      <c r="P19" s="249"/>
-      <c r="Q19" s="249"/>
-      <c r="R19" s="249"/>
-      <c r="S19" s="300"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P19" s="261"/>
+      <c r="Q19" s="261"/>
+      <c r="R19" s="261"/>
+      <c r="S19" s="274"/>
+    </row>
+    <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="202"/>
-      <c r="B20" s="276" t="s">
-        <v>257</v>
-      </c>
-      <c r="C20" s="277"/>
-      <c r="D20" s="277"/>
-      <c r="E20" s="277"/>
-      <c r="F20" s="277"/>
-      <c r="G20" s="70">
-        <v>440000</v>
-      </c>
+      <c r="B20" s="227"/>
+      <c r="C20" s="227"/>
+      <c r="D20" s="227"/>
+      <c r="E20" s="227"/>
+      <c r="F20" s="227"/>
+      <c r="G20" s="68"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="280" t="s">
+      <c r="I20" s="279" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="249"/>
-      <c r="K20" s="249"/>
-      <c r="L20" s="249"/>
+      <c r="J20" s="261"/>
+      <c r="K20" s="261"/>
+      <c r="L20" s="261"/>
       <c r="M20" s="203"/>
-      <c r="O20" s="271" t="s">
+      <c r="O20" s="296" t="s">
         <v>255</v>
       </c>
-      <c r="P20" s="249"/>
-      <c r="Q20" s="249"/>
-      <c r="R20" s="249"/>
-      <c r="S20" s="300"/>
+      <c r="P20" s="261"/>
+      <c r="Q20" s="261"/>
+      <c r="R20" s="261"/>
+      <c r="S20" s="274"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="202"/>
-      <c r="B21" s="274" t="s">
+      <c r="B21" s="312" t="s">
         <v>237</v>
       </c>
-      <c r="C21" s="275"/>
-      <c r="D21" s="275"/>
-      <c r="E21" s="275"/>
-      <c r="F21" s="268"/>
-      <c r="G21" s="173">
+      <c r="C21" s="313"/>
+      <c r="D21" s="313"/>
+      <c r="E21" s="313"/>
+      <c r="F21" s="314"/>
+      <c r="G21" s="70">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="269" t="s">
+      <c r="I21" s="298" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="270"/>
-      <c r="K21" s="281">
+      <c r="J21" s="322"/>
+      <c r="K21" s="324">
         <f>G23</f>
-        <v>2297729.1800000002</v>
-      </c>
-      <c r="L21" s="282"/>
+        <v>1857729.1800000002</v>
+      </c>
+      <c r="L21" s="325"/>
       <c r="M21" s="203"/>
       <c r="N21" s="197"/>
-      <c r="O21" s="306" t="s">
-        <v>264</v>
-      </c>
-      <c r="P21" s="294"/>
-      <c r="Q21" s="294"/>
-      <c r="R21" s="294"/>
-      <c r="S21" s="295"/>
+      <c r="O21" s="309" t="s">
+        <v>262</v>
+      </c>
+      <c r="P21" s="299"/>
+      <c r="Q21" s="299"/>
+      <c r="R21" s="299"/>
+      <c r="S21" s="300"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="202"/>
-      <c r="B22" s="285" t="s">
-        <v>256</v>
-      </c>
-      <c r="C22" s="286"/>
-      <c r="D22" s="286"/>
-      <c r="E22" s="286"/>
-      <c r="F22" s="287"/>
+      <c r="B22" s="315" t="s">
+        <v>287</v>
+      </c>
+      <c r="C22" s="316"/>
+      <c r="D22" s="316"/>
+      <c r="E22" s="316"/>
+      <c r="F22" s="317"/>
       <c r="G22" s="173">
         <v>200000</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="267" t="s">
+      <c r="I22" s="323" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="268"/>
-      <c r="K22" s="283">
+      <c r="J22" s="318"/>
+      <c r="K22" s="326">
         <f>Pengeluaran!L30</f>
-        <v>146000</v>
-      </c>
-      <c r="L22" s="284"/>
+        <v>474000</v>
+      </c>
+      <c r="L22" s="327"/>
       <c r="M22" s="203"/>
       <c r="N22" s="197"/>
-      <c r="O22" s="274" t="s">
-        <v>265</v>
-      </c>
-      <c r="P22" s="275"/>
-      <c r="Q22" s="275"/>
-      <c r="R22" s="275"/>
-      <c r="S22" s="299"/>
+      <c r="O22" s="301" t="s">
+        <v>263</v>
+      </c>
+      <c r="P22" s="302"/>
+      <c r="Q22" s="302"/>
+      <c r="R22" s="302"/>
+      <c r="S22" s="303"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="202"/>
-      <c r="B23" s="274" t="s">
+      <c r="B23" s="301" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="275"/>
-      <c r="D23" s="275"/>
-      <c r="E23" s="275"/>
-      <c r="F23" s="268"/>
+      <c r="C23" s="302"/>
+      <c r="D23" s="302"/>
+      <c r="E23" s="302"/>
+      <c r="F23" s="318"/>
       <c r="G23" s="173">
         <f>SUM(G20:G22)</f>
-        <v>2297729.1800000002</v>
+        <v>1857729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="267" t="s">
+      <c r="I23" s="323" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="268"/>
-      <c r="K23" s="278">
+      <c r="J23" s="318"/>
+      <c r="K23" s="328">
         <f>Pemasukkan!L31</f>
-        <v>130000</v>
-      </c>
-      <c r="L23" s="279"/>
+        <v>650000</v>
+      </c>
+      <c r="L23" s="329"/>
       <c r="M23" s="203"/>
       <c r="N23" s="197"/>
-      <c r="O23" s="274" t="s">
-        <v>266</v>
-      </c>
-      <c r="P23" s="275"/>
-      <c r="Q23" s="275"/>
-      <c r="R23" s="275"/>
-      <c r="S23" s="299"/>
+      <c r="O23" s="301" t="s">
+        <v>264</v>
+      </c>
+      <c r="P23" s="302"/>
+      <c r="Q23" s="302"/>
+      <c r="R23" s="302"/>
+      <c r="S23" s="303"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="202"/>
-      <c r="B24" s="288" t="s">
+      <c r="B24" s="319" t="s">
         <v>192</v>
       </c>
-      <c r="C24" s="289"/>
-      <c r="D24" s="289"/>
-      <c r="E24" s="289"/>
-      <c r="F24" s="290"/>
+      <c r="C24" s="320"/>
+      <c r="D24" s="320"/>
+      <c r="E24" s="320"/>
+      <c r="F24" s="321"/>
       <c r="G24" s="174">
         <f>K24</f>
-        <v>2281729.1800000002</v>
+        <v>2033729.1800000002</v>
       </c>
       <c r="H24" s="24"/>
-      <c r="I24" s="269" t="s">
+      <c r="I24" s="298" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="270"/>
-      <c r="K24" s="265">
+      <c r="J24" s="322"/>
+      <c r="K24" s="310">
         <f>(K21-K22)+K23</f>
-        <v>2281729.1800000002</v>
-      </c>
-      <c r="L24" s="266"/>
+        <v>2033729.1800000002</v>
+      </c>
+      <c r="L24" s="311"/>
       <c r="M24" s="203"/>
       <c r="N24" s="197"/>
-      <c r="O24" s="274" t="s">
-        <v>267</v>
-      </c>
-      <c r="P24" s="275"/>
-      <c r="Q24" s="275"/>
-      <c r="R24" s="275"/>
-      <c r="S24" s="299"/>
+      <c r="O24" s="301" t="s">
+        <v>265</v>
+      </c>
+      <c r="P24" s="302"/>
+      <c r="Q24" s="302"/>
+      <c r="R24" s="302"/>
+      <c r="S24" s="303"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="202"/>
@@ -13962,13 +14091,13 @@
       <c r="L25" s="24"/>
       <c r="M25" s="203"/>
       <c r="N25" s="197"/>
-      <c r="O25" s="271" t="s">
-        <v>272</v>
-      </c>
-      <c r="P25" s="249"/>
-      <c r="Q25" s="249"/>
-      <c r="R25" s="249"/>
-      <c r="S25" s="300"/>
+      <c r="O25" s="296" t="s">
+        <v>270</v>
+      </c>
+      <c r="P25" s="261"/>
+      <c r="Q25" s="261"/>
+      <c r="R25" s="261"/>
+      <c r="S25" s="274"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="202"/>
@@ -13985,11 +14114,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="203"/>
       <c r="N26" s="197"/>
-      <c r="O26" s="291"/>
-      <c r="P26" s="292"/>
-      <c r="Q26" s="292"/>
-      <c r="R26" s="292"/>
-      <c r="S26" s="293"/>
+      <c r="O26" s="297"/>
+      <c r="P26" s="275"/>
+      <c r="Q26" s="275"/>
+      <c r="R26" s="275"/>
+      <c r="S26" s="276"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="204"/>
@@ -14029,8 +14158,55 @@
       <c r="S28" s="197"/>
     </row>
   </sheetData>
-  <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="65">
+  <mergeCells count="64">
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="D18:L18"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="W5:AD5"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="O18:S18"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O23:S23"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="W4:AD4"/>
+    <mergeCell ref="W8:AD8"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="O25:S25"/>
     <mergeCell ref="U3:V3"/>
     <mergeCell ref="W3:AD3"/>
     <mergeCell ref="W12:AD12"/>
@@ -14047,55 +14223,6 @@
     <mergeCell ref="U12:V12"/>
     <mergeCell ref="U13:V13"/>
     <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:AD4"/>
-    <mergeCell ref="W8:AD8"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="O25:S25"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="W5:AD5"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="O24:S24"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="O18:S18"/>
-    <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O23:S23"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="D18:L18"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -14106,8 +14233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:M220"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14128,44 +14255,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="324" t="s">
+      <c r="C2" s="345" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="325"/>
-      <c r="E2" s="325"/>
-      <c r="F2" s="325"/>
-      <c r="G2" s="325"/>
-      <c r="H2" s="325"/>
-      <c r="I2" s="325"/>
-      <c r="J2" s="325"/>
-      <c r="K2" s="325"/>
+      <c r="D2" s="346"/>
+      <c r="E2" s="346"/>
+      <c r="F2" s="346"/>
+      <c r="G2" s="346"/>
+      <c r="H2" s="346"/>
+      <c r="I2" s="346"/>
+      <c r="J2" s="346"/>
+      <c r="K2" s="346"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="325"/>
-      <c r="D3" s="325"/>
-      <c r="E3" s="325"/>
-      <c r="F3" s="325"/>
-      <c r="G3" s="325"/>
-      <c r="H3" s="325"/>
-      <c r="I3" s="325"/>
-      <c r="J3" s="325"/>
-      <c r="K3" s="325"/>
+      <c r="C3" s="346"/>
+      <c r="D3" s="346"/>
+      <c r="E3" s="346"/>
+      <c r="F3" s="346"/>
+      <c r="G3" s="346"/>
+      <c r="H3" s="346"/>
+      <c r="I3" s="346"/>
+      <c r="J3" s="346"/>
+      <c r="K3" s="346"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="332" t="s">
+      <c r="C5" s="338" t="s">
         <v>250</v>
       </c>
-      <c r="D5" s="332"/>
-      <c r="E5" s="332"/>
-      <c r="F5" s="332"/>
-      <c r="G5" s="332"/>
-      <c r="I5" s="332" t="s">
+      <c r="D5" s="338"/>
+      <c r="E5" s="338"/>
+      <c r="F5" s="338"/>
+      <c r="G5" s="338"/>
+      <c r="I5" s="338" t="s">
         <v>251</v>
       </c>
-      <c r="J5" s="332"/>
-      <c r="K5" s="332"/>
-      <c r="L5" s="332"/>
-      <c r="M5" s="332"/>
+      <c r="J5" s="338"/>
+      <c r="K5" s="338"/>
+      <c r="L5" s="338"/>
+      <c r="M5" s="338"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -14218,8 +14345,8 @@
       <c r="I7" s="1">
         <v>1</v>
       </c>
-      <c r="J7" s="198" t="s">
-        <v>268</v>
+      <c r="J7" s="219" t="s">
+        <v>266</v>
       </c>
       <c r="K7" s="60">
         <v>43709</v>
@@ -14228,7 +14355,7 @@
         <v>64000</v>
       </c>
       <c r="M7" s="66" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="3:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14251,16 +14378,16 @@
         <v>2</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K8" s="60">
         <v>43716</v>
       </c>
       <c r="L8" s="64">
-        <v>66000</v>
+        <v>64000</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14274,10 +14401,18 @@
       <c r="I9" s="1">
         <v>3</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="1"/>
+      <c r="J9" s="135" t="s">
+        <v>291</v>
+      </c>
+      <c r="K9" s="226" t="s">
+        <v>272</v>
+      </c>
+      <c r="L9" s="64">
+        <v>443000</v>
+      </c>
+      <c r="M9" s="219" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="10" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
@@ -14290,10 +14425,18 @@
       <c r="I10" s="1">
         <v>4</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="K10" s="60">
+        <v>43726</v>
+      </c>
+      <c r="L10" s="64">
+        <v>79000</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="11" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
@@ -14569,7 +14712,7 @@
       </c>
       <c r="L27" s="63">
         <f>SUM(L7:L26)</f>
-        <v>130000</v>
+        <v>650000</v>
       </c>
       <c r="M27" s="24"/>
     </row>
@@ -14581,88 +14724,88 @@
       <c r="M28" s="197"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="276" t="s">
+      <c r="D29" s="334" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="277"/>
-      <c r="F29" s="326">
+      <c r="E29" s="335"/>
+      <c r="F29" s="339">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="327"/>
+      <c r="G29" s="340"/>
       <c r="I29" s="197"/>
-      <c r="J29" s="276" t="s">
+      <c r="J29" s="334" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="277"/>
-      <c r="L29" s="326">
+      <c r="K29" s="335"/>
+      <c r="L29" s="339">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
-        <v>2297729.1800000002</v>
-      </c>
-      <c r="M29" s="327"/>
+        <v>1857729.1800000002</v>
+      </c>
+      <c r="M29" s="340"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="323" t="s">
+      <c r="D30" s="291" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="249"/>
-      <c r="F30" s="328">
+      <c r="E30" s="261"/>
+      <c r="F30" s="341">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="329"/>
+      <c r="G30" s="342"/>
       <c r="I30" s="197"/>
-      <c r="J30" s="323" t="s">
+      <c r="J30" s="291" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="249"/>
-      <c r="L30" s="328">
+      <c r="K30" s="261"/>
+      <c r="L30" s="341">
         <f>Pengeluaran!L30</f>
-        <v>146000</v>
-      </c>
-      <c r="M30" s="329"/>
+        <v>474000</v>
+      </c>
+      <c r="M30" s="342"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="271" t="s">
+      <c r="D31" s="296" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="249"/>
-      <c r="F31" s="333">
+      <c r="E31" s="261"/>
+      <c r="F31" s="343">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="334"/>
+      <c r="G31" s="344"/>
       <c r="I31" s="197"/>
-      <c r="J31" s="271" t="s">
+      <c r="J31" s="296" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="249"/>
-      <c r="L31" s="333">
+      <c r="K31" s="261"/>
+      <c r="L31" s="343">
         <f>L27</f>
-        <v>130000</v>
-      </c>
-      <c r="M31" s="334"/>
+        <v>650000</v>
+      </c>
+      <c r="M31" s="344"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="272" t="s">
+      <c r="D32" s="332" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="273"/>
-      <c r="F32" s="330">
+      <c r="E32" s="333"/>
+      <c r="F32" s="336">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="331"/>
+      <c r="G32" s="337"/>
       <c r="I32" s="197"/>
-      <c r="J32" s="272" t="s">
+      <c r="J32" s="332" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="273"/>
-      <c r="L32" s="330">
+      <c r="K32" s="333"/>
+      <c r="L32" s="336">
         <f>'Hitung Pemasukan Pengeluaran'!G24</f>
-        <v>2281729.1800000002</v>
-      </c>
-      <c r="M32" s="331"/>
+        <v>2033729.1800000002</v>
+      </c>
+      <c r="M32" s="337"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14853,8 +14996,13 @@
     <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="19">
+    <mergeCell ref="C2:K3"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J29:K29"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="I5:M5"/>
@@ -14868,12 +15016,6 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J32:K32"/>
-    <mergeCell ref="C2:K3"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -14884,8 +15026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:M220"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14905,44 +15047,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="335" t="s">
+      <c r="C2" s="351" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="336"/>
-      <c r="E2" s="336"/>
-      <c r="F2" s="336"/>
-      <c r="G2" s="336"/>
-      <c r="H2" s="336"/>
-      <c r="I2" s="336"/>
-      <c r="J2" s="336"/>
-      <c r="K2" s="336"/>
+      <c r="D2" s="352"/>
+      <c r="E2" s="352"/>
+      <c r="F2" s="352"/>
+      <c r="G2" s="352"/>
+      <c r="H2" s="352"/>
+      <c r="I2" s="352"/>
+      <c r="J2" s="352"/>
+      <c r="K2" s="352"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="336"/>
-      <c r="D3" s="336"/>
-      <c r="E3" s="336"/>
-      <c r="F3" s="336"/>
-      <c r="G3" s="336"/>
-      <c r="H3" s="336"/>
-      <c r="I3" s="336"/>
-      <c r="J3" s="336"/>
-      <c r="K3" s="336"/>
+      <c r="C3" s="352"/>
+      <c r="D3" s="352"/>
+      <c r="E3" s="352"/>
+      <c r="F3" s="352"/>
+      <c r="G3" s="352"/>
+      <c r="H3" s="352"/>
+      <c r="I3" s="352"/>
+      <c r="J3" s="352"/>
+      <c r="K3" s="352"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="332" t="s">
+      <c r="C5" s="338" t="s">
         <v>248</v>
       </c>
-      <c r="D5" s="332"/>
-      <c r="E5" s="332"/>
-      <c r="F5" s="332"/>
-      <c r="G5" s="332"/>
-      <c r="I5" s="332" t="s">
+      <c r="D5" s="338"/>
+      <c r="E5" s="338"/>
+      <c r="F5" s="338"/>
+      <c r="G5" s="338"/>
+      <c r="I5" s="338" t="s">
         <v>249</v>
       </c>
-      <c r="J5" s="332"/>
-      <c r="K5" s="332"/>
-      <c r="L5" s="332"/>
-      <c r="M5" s="332"/>
+      <c r="J5" s="338"/>
+      <c r="K5" s="338"/>
+      <c r="L5" s="338"/>
+      <c r="M5" s="338"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -15052,16 +15194,16 @@
         <v>3</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="K9" s="217" t="s">
-        <v>274</v>
+        <v>271</v>
+      </c>
+      <c r="K9" s="216" t="s">
+        <v>272</v>
       </c>
       <c r="L9" s="64">
         <v>100000</v>
       </c>
       <c r="M9" s="57" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15081,10 +15223,18 @@
       <c r="I10" s="9">
         <v>4</v>
       </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="216"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="1"/>
+      <c r="J10" s="224" t="s">
+        <v>283</v>
+      </c>
+      <c r="K10" s="225" t="s">
+        <v>286</v>
+      </c>
+      <c r="L10" s="64">
+        <v>320000</v>
+      </c>
+      <c r="M10" s="218" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="11" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="57">
@@ -15103,10 +15253,18 @@
       <c r="I11" s="214">
         <v>5</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="1"/>
+      <c r="J11" s="218" t="s">
+        <v>288</v>
+      </c>
+      <c r="K11" s="225" t="s">
+        <v>286</v>
+      </c>
+      <c r="L11" s="64">
+        <v>8000</v>
+      </c>
+      <c r="M11" s="219" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="12" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="57">
@@ -15368,7 +15526,7 @@
       </c>
       <c r="L27" s="56">
         <f>SUM(L7:L26)</f>
-        <v>146000</v>
+        <v>474000</v>
       </c>
       <c r="M27" s="57"/>
     </row>
@@ -15380,88 +15538,88 @@
       <c r="M28" s="197"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="311" t="s">
+      <c r="D29" s="270" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="313"/>
-      <c r="F29" s="337">
+      <c r="E29" s="272"/>
+      <c r="F29" s="349">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="338"/>
+      <c r="G29" s="350"/>
       <c r="I29" s="197"/>
-      <c r="J29" s="311" t="s">
+      <c r="J29" s="270" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="313"/>
-      <c r="L29" s="337">
+      <c r="K29" s="272"/>
+      <c r="L29" s="349">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
-        <v>2297729.1800000002</v>
-      </c>
-      <c r="M29" s="338"/>
+        <v>1857729.1800000002</v>
+      </c>
+      <c r="M29" s="350"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="271" t="s">
+      <c r="D30" s="296" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="249"/>
-      <c r="F30" s="328">
+      <c r="E30" s="261"/>
+      <c r="F30" s="341">
         <f>F27</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="329"/>
+      <c r="G30" s="342"/>
       <c r="I30" s="197"/>
-      <c r="J30" s="271" t="s">
+      <c r="J30" s="296" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="249"/>
-      <c r="L30" s="328">
+      <c r="K30" s="261"/>
+      <c r="L30" s="341">
         <f>L27</f>
-        <v>146000</v>
-      </c>
-      <c r="M30" s="329"/>
+        <v>474000</v>
+      </c>
+      <c r="M30" s="342"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="271" t="s">
+      <c r="D31" s="296" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="249"/>
-      <c r="F31" s="333">
+      <c r="E31" s="261"/>
+      <c r="F31" s="343">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="334"/>
+      <c r="G31" s="344"/>
       <c r="I31" s="197"/>
-      <c r="J31" s="271" t="s">
+      <c r="J31" s="296" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="249"/>
-      <c r="L31" s="333">
+      <c r="K31" s="261"/>
+      <c r="L31" s="343">
         <f>Pemasukkan!L27</f>
-        <v>130000</v>
-      </c>
-      <c r="M31" s="334"/>
+        <v>650000</v>
+      </c>
+      <c r="M31" s="344"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="272" t="s">
+      <c r="D32" s="332" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="273"/>
-      <c r="F32" s="339">
+      <c r="E32" s="333"/>
+      <c r="F32" s="347">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="340"/>
+      <c r="G32" s="348"/>
       <c r="I32" s="197"/>
-      <c r="J32" s="272" t="s">
+      <c r="J32" s="332" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="273"/>
-      <c r="L32" s="339">
+      <c r="K32" s="333"/>
+      <c r="L32" s="347">
         <f>'Hitung Pemasukan Pengeluaran'!G24</f>
-        <v>2281729.1800000002</v>
-      </c>
-      <c r="M32" s="340"/>
+        <v>2033729.1800000002</v>
+      </c>
+      <c r="M32" s="348"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15652,16 +15810,7 @@
     <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="19">
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
     <mergeCell ref="C2:K3"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
@@ -15673,6 +15822,14 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -15683,8 +15840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15697,28 +15854,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="343" t="s">
+      <c r="C2" s="355" t="s">
         <v>232</v>
       </c>
-      <c r="D2" s="344"/>
-      <c r="E2" s="344"/>
-      <c r="F2" s="344"/>
-      <c r="G2" s="344"/>
-      <c r="H2" s="344"/>
-      <c r="I2" s="344"/>
-      <c r="J2" s="344"/>
-      <c r="K2" s="344"/>
+      <c r="D2" s="356"/>
+      <c r="E2" s="356"/>
+      <c r="F2" s="356"/>
+      <c r="G2" s="356"/>
+      <c r="H2" s="356"/>
+      <c r="I2" s="356"/>
+      <c r="J2" s="356"/>
+      <c r="K2" s="356"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="344"/>
-      <c r="D3" s="344"/>
-      <c r="E3" s="344"/>
-      <c r="F3" s="344"/>
-      <c r="G3" s="344"/>
-      <c r="H3" s="344"/>
-      <c r="I3" s="344"/>
-      <c r="J3" s="344"/>
-      <c r="K3" s="344"/>
+      <c r="C3" s="356"/>
+      <c r="D3" s="356"/>
+      <c r="E3" s="356"/>
+      <c r="F3" s="356"/>
+      <c r="G3" s="356"/>
+      <c r="H3" s="356"/>
+      <c r="I3" s="356"/>
+      <c r="J3" s="356"/>
+      <c r="K3" s="356"/>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="156"/>
@@ -15789,16 +15946,16 @@
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E8" s="218" t="s">
         <v>274</v>
+      </c>
+      <c r="E8" s="217" t="s">
+        <v>272</v>
       </c>
       <c r="F8" s="64">
         <v>160000</v>
       </c>
       <c r="G8" s="164" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="H8" s="156"/>
       <c r="I8" s="156"/>
@@ -16068,10 +16225,10 @@
     </row>
     <row r="29" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="156"/>
-      <c r="D29" s="345"/>
-      <c r="E29" s="345"/>
-      <c r="F29" s="346"/>
-      <c r="G29" s="346"/>
+      <c r="D29" s="357"/>
+      <c r="E29" s="357"/>
+      <c r="F29" s="358"/>
+      <c r="G29" s="358"/>
       <c r="H29" s="156"/>
       <c r="I29" s="156"/>
       <c r="J29" s="156"/>
@@ -16079,15 +16236,15 @@
     </row>
     <row r="30" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="24"/>
-      <c r="D30" s="347" t="s">
+      <c r="D30" s="359" t="s">
         <v>231</v>
       </c>
-      <c r="E30" s="348"/>
-      <c r="F30" s="349">
+      <c r="E30" s="360"/>
+      <c r="F30" s="361">
         <f>F27</f>
         <v>220000</v>
       </c>
-      <c r="G30" s="350"/>
+      <c r="G30" s="362"/>
       <c r="H30" s="156"/>
       <c r="I30" s="156"/>
       <c r="J30" s="156"/>
@@ -16102,10 +16259,10 @@
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="156"/>
-      <c r="D32" s="341"/>
-      <c r="E32" s="341"/>
-      <c r="F32" s="342"/>
-      <c r="G32" s="341"/>
+      <c r="D32" s="353"/>
+      <c r="E32" s="353"/>
+      <c r="F32" s="354"/>
+      <c r="G32" s="353"/>
       <c r="H32" s="156"/>
       <c r="I32" s="156"/>
       <c r="J32" s="156"/>
@@ -16143,17 +16300,17 @@
     <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="351" t="s">
+      <c r="C4" s="363" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="352"/>
+      <c r="D4" s="364"/>
       <c r="E4" s="27"/>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
-      <c r="H4" s="351" t="s">
+      <c r="H4" s="363" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="352"/>
+      <c r="I4" s="364"/>
       <c r="J4" s="35"/>
       <c r="K4" s="27"/>
     </row>
@@ -16280,17 +16437,17 @@
     <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26"/>
-      <c r="C17" s="351" t="s">
+      <c r="C17" s="363" t="s">
         <v>144</v>
       </c>
-      <c r="D17" s="352"/>
+      <c r="D17" s="364"/>
       <c r="E17" s="27"/>
       <c r="F17" s="26"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="351" t="s">
+      <c r="H17" s="363" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="352"/>
+      <c r="I17" s="364"/>
       <c r="J17" s="35"/>
       <c r="K17" s="27"/>
     </row>
@@ -16425,4 +16582,220 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="366" t="s">
+        <v>279</v>
+      </c>
+      <c r="C2" s="367"/>
+      <c r="D2" s="367"/>
+      <c r="E2" s="367"/>
+      <c r="F2" s="367"/>
+      <c r="G2" s="367"/>
+      <c r="H2" s="367"/>
+      <c r="I2" s="367"/>
+      <c r="J2" s="367"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="367"/>
+      <c r="C3" s="367"/>
+      <c r="D3" s="367"/>
+      <c r="E3" s="367"/>
+      <c r="F3" s="367"/>
+      <c r="G3" s="367"/>
+      <c r="H3" s="367"/>
+      <c r="I3" s="367"/>
+      <c r="J3" s="367"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H6" s="279" t="s">
+        <v>284</v>
+      </c>
+      <c r="I6" s="261"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D7" s="1">
+        <v>35</v>
+      </c>
+      <c r="E7" s="220">
+        <v>15000</v>
+      </c>
+      <c r="F7" s="220">
+        <f>D7*E7</f>
+        <v>525000</v>
+      </c>
+      <c r="G7" s="220">
+        <v>205000</v>
+      </c>
+      <c r="H7" s="368">
+        <f>F7-G7</f>
+        <v>320000</v>
+      </c>
+      <c r="I7" s="261"/>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="221"/>
+      <c r="C8" s="221"/>
+      <c r="D8" s="221"/>
+      <c r="E8" s="222"/>
+      <c r="F8" s="222"/>
+      <c r="G8" s="222"/>
+      <c r="H8" s="365"/>
+      <c r="I8" s="365"/>
+    </row>
+    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="221"/>
+      <c r="C9" s="221"/>
+      <c r="D9" s="221"/>
+      <c r="E9" s="222"/>
+      <c r="F9" s="222"/>
+      <c r="G9" s="223" t="s">
+        <v>285</v>
+      </c>
+      <c r="H9" s="369">
+        <f>H7</f>
+        <v>320000</v>
+      </c>
+      <c r="I9" s="370"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="221"/>
+      <c r="C10" s="221"/>
+      <c r="D10" s="221"/>
+      <c r="E10" s="222"/>
+      <c r="F10" s="222"/>
+      <c r="G10" s="222"/>
+      <c r="H10" s="365"/>
+      <c r="I10" s="365"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="221"/>
+      <c r="C11" s="221"/>
+      <c r="D11" s="221"/>
+      <c r="E11" s="222"/>
+      <c r="F11" s="222"/>
+      <c r="G11" s="222"/>
+      <c r="H11" s="365"/>
+      <c r="I11" s="365"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="221"/>
+      <c r="C12" s="221"/>
+      <c r="D12" s="221"/>
+      <c r="E12" s="222"/>
+      <c r="F12" s="222"/>
+      <c r="G12" s="222"/>
+      <c r="H12" s="365"/>
+      <c r="I12" s="365"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="221"/>
+      <c r="C13" s="221"/>
+      <c r="D13" s="221"/>
+      <c r="E13" s="222"/>
+      <c r="F13" s="222"/>
+      <c r="G13" s="222"/>
+      <c r="H13" s="365"/>
+      <c r="I13" s="365"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="221"/>
+      <c r="C14" s="221"/>
+      <c r="D14" s="221"/>
+      <c r="E14" s="222"/>
+      <c r="F14" s="222"/>
+      <c r="G14" s="222"/>
+      <c r="H14" s="365"/>
+      <c r="I14" s="365"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="221"/>
+      <c r="C15" s="221"/>
+      <c r="D15" s="221"/>
+      <c r="E15" s="222"/>
+      <c r="F15" s="222"/>
+      <c r="G15" s="222"/>
+      <c r="H15" s="365"/>
+      <c r="I15" s="365"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="221"/>
+      <c r="C16" s="221"/>
+      <c r="D16" s="221"/>
+      <c r="E16" s="222"/>
+      <c r="F16" s="222"/>
+      <c r="G16" s="222"/>
+      <c r="H16" s="365"/>
+      <c r="I16" s="365"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="221"/>
+      <c r="C17" s="221"/>
+      <c r="D17" s="221"/>
+      <c r="E17" s="222"/>
+      <c r="F17" s="222"/>
+      <c r="G17" s="222"/>
+      <c r="H17" s="365"/>
+      <c r="I17" s="365"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B2:J3"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revisi format pengeluaran & Pemasukkan
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -4,24 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-630" yWindow="570" windowWidth="19815" windowHeight="7365" tabRatio="533" activeTab="1"/>
+    <workbookView xWindow="-630" yWindow="570" windowWidth="19815" windowHeight="7365" tabRatio="761" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2018(NOT UPDATED)" sheetId="1" r:id="rId1"/>
     <sheet name="2019" sheetId="2" r:id="rId2"/>
-    <sheet name="Hitung Pemasukan Pengeluaran" sheetId="8" r:id="rId3"/>
-    <sheet name="Pemasukkan" sheetId="6" r:id="rId4"/>
-    <sheet name="Pengeluaran" sheetId="4" r:id="rId5"/>
-    <sheet name="Inventaris" sheetId="7" r:id="rId6"/>
-    <sheet name="Lampiran Polo" sheetId="3" r:id="rId7"/>
-    <sheet name="Patch OH" sheetId="9" r:id="rId8"/>
+    <sheet name="Sirkulasi" sheetId="10" r:id="rId3"/>
+    <sheet name="Hitung Pemasukan Pengeluaran" sheetId="8" r:id="rId4"/>
+    <sheet name="Pemasukkan" sheetId="6" r:id="rId5"/>
+    <sheet name="Pengeluaran" sheetId="4" r:id="rId6"/>
+    <sheet name="Inventaris" sheetId="7" r:id="rId7"/>
+    <sheet name="Lampiran Polo" sheetId="3" r:id="rId8"/>
+    <sheet name="Patch OH" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="318">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -902,9 +903,6 @@
     <t>Ambil ATM</t>
   </si>
   <si>
-    <t>Puan</t>
-  </si>
-  <si>
     <t>Rapli utang</t>
   </si>
   <si>
@@ -936,13 +934,55 @@
   </si>
   <si>
     <t>Biaya Tak Terduga</t>
+  </si>
+  <si>
+    <t>Sirkulasi Keuangan</t>
+  </si>
+  <si>
+    <t>Tanggal</t>
+  </si>
+  <si>
+    <t>16 Agustus 2019</t>
+  </si>
+  <si>
+    <t>Sirkulasi Mulai dari 15 Agustus - September</t>
+  </si>
+  <si>
+    <t>08 Agustus 2019</t>
+  </si>
+  <si>
+    <t>KAS Juli</t>
+  </si>
+  <si>
+    <t>Trofi Reward OH</t>
+  </si>
+  <si>
+    <t>Kembalian Puan</t>
+  </si>
+  <si>
+    <t>Rapli Utang</t>
+  </si>
+  <si>
+    <t>Patch OH 2019 Tambahan 4pcs</t>
+  </si>
+  <si>
+    <t>GELEX</t>
+  </si>
+  <si>
+    <t>DP Stempel</t>
+  </si>
+  <si>
+    <t>KAS Akhir Januari</t>
+  </si>
+  <si>
+    <t>Total KAS September</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="14">
+  <numFmts count="15">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-[$Rp-421]* #,##0.00_-;\-[$Rp-421]* #,##0.00_-;_-[$Rp-421]* &quot;-&quot;??_-;_-@"/>
@@ -957,6 +997,7 @@
     <numFmt numFmtId="174" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="175" formatCode="0_);\(0\)"/>
     <numFmt numFmtId="176" formatCode="[$IDR]\ #,##0_);\([$IDR]\ #,##0\)"/>
+    <numFmt numFmtId="177" formatCode="dd\ mmmm\ yyyy"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -1039,7 +1080,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1193,6 +1234,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2118,7 +2165,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="369">
+  <cellXfs count="403">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2600,29 +2647,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="174" fontId="4" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="20" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="13" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="20" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2638,37 +2737,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2676,28 +2777,185 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2712,33 +2970,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2758,136 +2995,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2898,29 +3024,23 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2928,16 +3048,37 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="0" fillId="17" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="27" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="27" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="27" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="27" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="27" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="27" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3201,6 +3342,285 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>67235</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>448235</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="672353" y="134471"/>
+          <a:ext cx="11631706" cy="5109882"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>163606</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1205752</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>129989</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="2065243" y="1773892"/>
+          <a:ext cx="8657665" cy="5109882"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1088570</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>565095</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>139594</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Connector 1"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="11316178" y="1773892"/>
+          <a:ext cx="8657665" cy="5109882"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4354285</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>3589884</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11035392" y="1115786"/>
+          <a:ext cx="11631706" cy="5109882"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609920</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>5603</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Connector 1"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9429750" y="134471"/>
+          <a:ext cx="11631706" cy="5109882"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1615568</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>751914</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>153201</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="10822640" y="1773892"/>
+          <a:ext cx="8657665" cy="5109882"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3816,126 +4236,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="252" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="236"/>
-      <c r="I1" s="236"/>
-      <c r="J1" s="236"/>
-      <c r="K1" s="236"/>
-      <c r="L1" s="236"/>
-      <c r="M1" s="236"/>
-      <c r="N1" s="236"/>
-      <c r="O1" s="236"/>
-      <c r="P1" s="236"/>
-      <c r="Q1" s="236"/>
-      <c r="R1" s="236"/>
+      <c r="B1" s="253"/>
+      <c r="C1" s="253"/>
+      <c r="D1" s="253"/>
+      <c r="E1" s="253"/>
+      <c r="F1" s="253"/>
+      <c r="G1" s="253"/>
+      <c r="H1" s="253"/>
+      <c r="I1" s="253"/>
+      <c r="J1" s="253"/>
+      <c r="K1" s="253"/>
+      <c r="L1" s="253"/>
+      <c r="M1" s="253"/>
+      <c r="N1" s="253"/>
+      <c r="O1" s="253"/>
+      <c r="P1" s="253"/>
+      <c r="Q1" s="253"/>
+      <c r="R1" s="253"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="237"/>
-      <c r="B2" s="238"/>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
-      <c r="G2" s="238"/>
-      <c r="H2" s="238"/>
-      <c r="I2" s="238"/>
-      <c r="J2" s="238"/>
-      <c r="K2" s="238"/>
-      <c r="L2" s="238"/>
-      <c r="M2" s="238"/>
-      <c r="N2" s="238"/>
-      <c r="O2" s="238"/>
-      <c r="P2" s="238"/>
-      <c r="Q2" s="238"/>
-      <c r="R2" s="238"/>
+      <c r="A2" s="254"/>
+      <c r="B2" s="255"/>
+      <c r="C2" s="255"/>
+      <c r="D2" s="255"/>
+      <c r="E2" s="255"/>
+      <c r="F2" s="255"/>
+      <c r="G2" s="255"/>
+      <c r="H2" s="255"/>
+      <c r="I2" s="255"/>
+      <c r="J2" s="255"/>
+      <c r="K2" s="255"/>
+      <c r="L2" s="255"/>
+      <c r="M2" s="255"/>
+      <c r="N2" s="255"/>
+      <c r="O2" s="255"/>
+      <c r="P2" s="255"/>
+      <c r="Q2" s="255"/>
+      <c r="R2" s="255"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="237"/>
-      <c r="B3" s="238"/>
-      <c r="C3" s="238"/>
-      <c r="D3" s="238"/>
-      <c r="E3" s="238"/>
-      <c r="F3" s="238"/>
-      <c r="G3" s="238"/>
-      <c r="H3" s="238"/>
-      <c r="I3" s="238"/>
-      <c r="J3" s="238"/>
-      <c r="K3" s="238"/>
-      <c r="L3" s="238"/>
-      <c r="M3" s="238"/>
-      <c r="N3" s="238"/>
-      <c r="O3" s="238"/>
-      <c r="P3" s="238"/>
-      <c r="Q3" s="238"/>
-      <c r="R3" s="238"/>
+      <c r="A3" s="254"/>
+      <c r="B3" s="255"/>
+      <c r="C3" s="255"/>
+      <c r="D3" s="255"/>
+      <c r="E3" s="255"/>
+      <c r="F3" s="255"/>
+      <c r="G3" s="255"/>
+      <c r="H3" s="255"/>
+      <c r="I3" s="255"/>
+      <c r="J3" s="255"/>
+      <c r="K3" s="255"/>
+      <c r="L3" s="255"/>
+      <c r="M3" s="255"/>
+      <c r="N3" s="255"/>
+      <c r="O3" s="255"/>
+      <c r="P3" s="255"/>
+      <c r="Q3" s="255"/>
+      <c r="R3" s="255"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="237"/>
-      <c r="B4" s="238"/>
-      <c r="C4" s="238"/>
-      <c r="D4" s="238"/>
-      <c r="E4" s="238"/>
-      <c r="F4" s="238"/>
-      <c r="G4" s="238"/>
-      <c r="H4" s="238"/>
-      <c r="I4" s="238"/>
-      <c r="J4" s="238"/>
-      <c r="K4" s="238"/>
-      <c r="L4" s="238"/>
-      <c r="M4" s="238"/>
-      <c r="N4" s="238"/>
-      <c r="O4" s="238"/>
-      <c r="P4" s="238"/>
-      <c r="Q4" s="238"/>
-      <c r="R4" s="238"/>
+      <c r="A4" s="254"/>
+      <c r="B4" s="255"/>
+      <c r="C4" s="255"/>
+      <c r="D4" s="255"/>
+      <c r="E4" s="255"/>
+      <c r="F4" s="255"/>
+      <c r="G4" s="255"/>
+      <c r="H4" s="255"/>
+      <c r="I4" s="255"/>
+      <c r="J4" s="255"/>
+      <c r="K4" s="255"/>
+      <c r="L4" s="255"/>
+      <c r="M4" s="255"/>
+      <c r="N4" s="255"/>
+      <c r="O4" s="255"/>
+      <c r="P4" s="255"/>
+      <c r="Q4" s="255"/>
+      <c r="R4" s="255"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="237"/>
-      <c r="B5" s="238"/>
-      <c r="C5" s="238"/>
-      <c r="D5" s="238"/>
-      <c r="E5" s="238"/>
-      <c r="F5" s="238"/>
-      <c r="G5" s="238"/>
-      <c r="H5" s="238"/>
-      <c r="I5" s="238"/>
-      <c r="J5" s="238"/>
-      <c r="K5" s="238"/>
-      <c r="L5" s="238"/>
-      <c r="M5" s="238"/>
-      <c r="N5" s="238"/>
-      <c r="O5" s="238"/>
-      <c r="P5" s="238"/>
-      <c r="Q5" s="238"/>
-      <c r="R5" s="238"/>
+      <c r="A5" s="254"/>
+      <c r="B5" s="255"/>
+      <c r="C5" s="255"/>
+      <c r="D5" s="255"/>
+      <c r="E5" s="255"/>
+      <c r="F5" s="255"/>
+      <c r="G5" s="255"/>
+      <c r="H5" s="255"/>
+      <c r="I5" s="255"/>
+      <c r="J5" s="255"/>
+      <c r="K5" s="255"/>
+      <c r="L5" s="255"/>
+      <c r="M5" s="255"/>
+      <c r="N5" s="255"/>
+      <c r="O5" s="255"/>
+      <c r="P5" s="255"/>
+      <c r="Q5" s="255"/>
+      <c r="R5" s="255"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="237"/>
-      <c r="B6" s="238"/>
-      <c r="C6" s="238"/>
-      <c r="D6" s="238"/>
-      <c r="E6" s="238"/>
-      <c r="F6" s="238"/>
-      <c r="G6" s="238"/>
-      <c r="H6" s="238"/>
-      <c r="I6" s="238"/>
-      <c r="J6" s="238"/>
-      <c r="K6" s="238"/>
-      <c r="L6" s="238"/>
-      <c r="M6" s="238"/>
-      <c r="N6" s="238"/>
-      <c r="O6" s="238"/>
-      <c r="P6" s="238"/>
-      <c r="Q6" s="238"/>
-      <c r="R6" s="238"/>
+      <c r="A6" s="254"/>
+      <c r="B6" s="255"/>
+      <c r="C6" s="255"/>
+      <c r="D6" s="255"/>
+      <c r="E6" s="255"/>
+      <c r="F6" s="255"/>
+      <c r="G6" s="255"/>
+      <c r="H6" s="255"/>
+      <c r="I6" s="255"/>
+      <c r="J6" s="255"/>
+      <c r="K6" s="255"/>
+      <c r="L6" s="255"/>
+      <c r="M6" s="255"/>
+      <c r="N6" s="255"/>
+      <c r="O6" s="255"/>
+      <c r="P6" s="255"/>
+      <c r="Q6" s="255"/>
+      <c r="R6" s="255"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -6880,58 +7300,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="240" t="s">
+      <c r="J79" s="260" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="241"/>
-      <c r="L79" s="241"/>
-      <c r="M79" s="241"/>
-      <c r="N79" s="242"/>
-      <c r="P79" s="248" t="s">
+      <c r="K79" s="261"/>
+      <c r="L79" s="261"/>
+      <c r="M79" s="261"/>
+      <c r="N79" s="262"/>
+      <c r="P79" s="268" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="241"/>
-      <c r="R79" s="241"/>
-      <c r="S79" s="242"/>
+      <c r="Q79" s="261"/>
+      <c r="R79" s="261"/>
+      <c r="S79" s="262"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="243" t="s">
+      <c r="J80" s="263" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="238"/>
-      <c r="L80" s="238"/>
-      <c r="M80" s="238"/>
-      <c r="N80" s="244"/>
-      <c r="P80" s="243" t="s">
+      <c r="K80" s="255"/>
+      <c r="L80" s="255"/>
+      <c r="M80" s="255"/>
+      <c r="N80" s="264"/>
+      <c r="P80" s="263" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="238"/>
-      <c r="R80" s="238"/>
-      <c r="S80" s="244"/>
+      <c r="Q80" s="255"/>
+      <c r="R80" s="255"/>
+      <c r="S80" s="264"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="245"/>
-      <c r="K81" s="246"/>
-      <c r="L81" s="246"/>
-      <c r="M81" s="246"/>
-      <c r="N81" s="247"/>
-      <c r="P81" s="245"/>
-      <c r="Q81" s="246"/>
-      <c r="R81" s="246"/>
-      <c r="S81" s="247"/>
+      <c r="J81" s="265"/>
+      <c r="K81" s="266"/>
+      <c r="L81" s="266"/>
+      <c r="M81" s="266"/>
+      <c r="N81" s="267"/>
+      <c r="P81" s="265"/>
+      <c r="Q81" s="266"/>
+      <c r="R81" s="266"/>
+      <c r="S81" s="267"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="239" t="s">
+      <c r="J82" s="258" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="230"/>
-      <c r="L82" s="231"/>
-      <c r="M82" s="239" t="s">
+      <c r="K82" s="259"/>
+      <c r="L82" s="257"/>
+      <c r="M82" s="258" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="231"/>
-      <c r="P82" s="239"/>
-      <c r="Q82" s="231"/>
+      <c r="N82" s="257"/>
+      <c r="P82" s="258"/>
+      <c r="Q82" s="257"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -6940,38 +7360,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="229" t="s">
+      <c r="J83" s="269" t="s">
         <v>70</v>
       </c>
-      <c r="K83" s="230"/>
-      <c r="L83" s="231"/>
-      <c r="M83" s="232">
+      <c r="K83" s="259"/>
+      <c r="L83" s="257"/>
+      <c r="M83" s="270">
         <v>7350000</v>
       </c>
-      <c r="N83" s="231"/>
-      <c r="P83" s="233" t="s">
+      <c r="N83" s="257"/>
+      <c r="P83" s="256" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="231"/>
+      <c r="Q83" s="257"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="229" t="s">
+      <c r="J84" s="269" t="s">
         <v>72</v>
       </c>
-      <c r="K84" s="230"/>
-      <c r="L84" s="231"/>
-      <c r="M84" s="234">
+      <c r="K84" s="259"/>
+      <c r="L84" s="257"/>
+      <c r="M84" s="271">
         <v>1100000</v>
       </c>
-      <c r="N84" s="231"/>
-      <c r="P84" s="233" t="s">
+      <c r="N84" s="257"/>
+      <c r="P84" s="256" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="231"/>
+      <c r="Q84" s="257"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -6980,39 +7400,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="229" t="s">
+      <c r="J85" s="269" t="s">
         <v>75</v>
       </c>
-      <c r="K85" s="230"/>
-      <c r="L85" s="231"/>
-      <c r="M85" s="232">
+      <c r="K85" s="259"/>
+      <c r="L85" s="257"/>
+      <c r="M85" s="270">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="231"/>
-      <c r="P85" s="233" t="s">
+      <c r="N85" s="257"/>
+      <c r="P85" s="256" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="231"/>
+      <c r="Q85" s="257"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="229" t="s">
+      <c r="J86" s="269" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="230"/>
-      <c r="L86" s="231"/>
-      <c r="M86" s="232">
+      <c r="K86" s="259"/>
+      <c r="L86" s="257"/>
+      <c r="M86" s="270">
         <v>8411850</v>
       </c>
-      <c r="N86" s="231"/>
-      <c r="P86" s="233" t="s">
+      <c r="N86" s="257"/>
+      <c r="P86" s="256" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="231"/>
+      <c r="Q86" s="257"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -7020,20 +7440,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="229" t="s">
+      <c r="J87" s="269" t="s">
         <v>79</v>
       </c>
-      <c r="K87" s="230"/>
-      <c r="L87" s="231"/>
-      <c r="M87" s="232">
+      <c r="K87" s="259"/>
+      <c r="L87" s="257"/>
+      <c r="M87" s="270">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="231"/>
-      <c r="P87" s="233" t="s">
+      <c r="N87" s="257"/>
+      <c r="P87" s="256" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="231"/>
+      <c r="Q87" s="257"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -7222,6 +7642,17 @@
   </sheetData>
   <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="23">
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="P86:Q86"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="M84:N84"/>
     <mergeCell ref="A1:R6"/>
     <mergeCell ref="P84:Q84"/>
     <mergeCell ref="J82:L82"/>
@@ -7234,17 +7665,6 @@
     <mergeCell ref="P83:Q83"/>
     <mergeCell ref="P82:Q82"/>
     <mergeCell ref="P80:S81"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="P86:Q86"/>
   </mergeCells>
   <conditionalFormatting sqref="T10:T52">
     <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
@@ -7278,7 +7698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BM260"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A28" colorId="8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView defaultGridColor="0" topLeftCell="A28" colorId="8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -7321,46 +7741,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="257" t="s">
+      <c r="C2" s="292" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="236"/>
-      <c r="E2" s="236"/>
-      <c r="F2" s="236"/>
-      <c r="G2" s="236"/>
-      <c r="H2" s="236"/>
-      <c r="I2" s="236"/>
-      <c r="J2" s="236"/>
-      <c r="K2" s="236"/>
-      <c r="L2" s="236"/>
-      <c r="M2" s="236"/>
-      <c r="N2" s="236"/>
-      <c r="O2" s="236"/>
-      <c r="P2" s="237"/>
-      <c r="Q2" s="237"/>
-      <c r="R2" s="237"/>
-      <c r="S2" s="236"/>
-      <c r="T2" s="236"/>
+      <c r="D2" s="253"/>
+      <c r="E2" s="253"/>
+      <c r="F2" s="253"/>
+      <c r="G2" s="253"/>
+      <c r="H2" s="253"/>
+      <c r="I2" s="253"/>
+      <c r="J2" s="253"/>
+      <c r="K2" s="253"/>
+      <c r="L2" s="253"/>
+      <c r="M2" s="253"/>
+      <c r="N2" s="253"/>
+      <c r="O2" s="253"/>
+      <c r="P2" s="254"/>
+      <c r="Q2" s="254"/>
+      <c r="R2" s="254"/>
+      <c r="S2" s="253"/>
+      <c r="T2" s="253"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="237"/>
-      <c r="D3" s="238"/>
-      <c r="E3" s="238"/>
-      <c r="F3" s="238"/>
-      <c r="G3" s="238"/>
-      <c r="H3" s="238"/>
-      <c r="I3" s="238"/>
-      <c r="J3" s="238"/>
-      <c r="K3" s="238"/>
-      <c r="L3" s="238"/>
-      <c r="M3" s="238"/>
-      <c r="N3" s="238"/>
-      <c r="O3" s="238"/>
-      <c r="P3" s="238"/>
-      <c r="Q3" s="238"/>
-      <c r="R3" s="238"/>
-      <c r="S3" s="238"/>
-      <c r="T3" s="238"/>
+      <c r="C3" s="254"/>
+      <c r="D3" s="255"/>
+      <c r="E3" s="255"/>
+      <c r="F3" s="255"/>
+      <c r="G3" s="255"/>
+      <c r="H3" s="255"/>
+      <c r="I3" s="255"/>
+      <c r="J3" s="255"/>
+      <c r="K3" s="255"/>
+      <c r="L3" s="255"/>
+      <c r="M3" s="255"/>
+      <c r="N3" s="255"/>
+      <c r="O3" s="255"/>
+      <c r="P3" s="255"/>
+      <c r="Q3" s="255"/>
+      <c r="R3" s="255"/>
+      <c r="S3" s="255"/>
+      <c r="T3" s="255"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7447,25 +7867,25 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="263" t="s">
+      <c r="X5" s="284" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="230"/>
-      <c r="Z5" s="230"/>
-      <c r="AA5" s="230"/>
-      <c r="AB5" s="230"/>
-      <c r="AC5" s="230"/>
-      <c r="AD5" s="230"/>
-      <c r="AE5" s="230"/>
-      <c r="AF5" s="230"/>
-      <c r="AG5" s="230"/>
-      <c r="AH5" s="230"/>
-      <c r="AI5" s="230"/>
-      <c r="AJ5" s="230"/>
-      <c r="AK5" s="230"/>
-      <c r="AL5" s="230"/>
-      <c r="AM5" s="230"/>
-      <c r="AN5" s="231"/>
+      <c r="Y5" s="259"/>
+      <c r="Z5" s="259"/>
+      <c r="AA5" s="259"/>
+      <c r="AB5" s="259"/>
+      <c r="AC5" s="259"/>
+      <c r="AD5" s="259"/>
+      <c r="AE5" s="259"/>
+      <c r="AF5" s="259"/>
+      <c r="AG5" s="259"/>
+      <c r="AH5" s="259"/>
+      <c r="AI5" s="259"/>
+      <c r="AJ5" s="259"/>
+      <c r="AK5" s="259"/>
+      <c r="AL5" s="259"/>
+      <c r="AM5" s="259"/>
+      <c r="AN5" s="257"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -7530,29 +7950,29 @@
         <v>NO</v>
       </c>
       <c r="V6" s="13"/>
-      <c r="X6" s="258" t="s">
+      <c r="X6" s="293" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="258" t="s">
+      <c r="Y6" s="293" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="262" t="s">
+      <c r="Z6" s="282" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="259"/>
-      <c r="AB6" s="259"/>
-      <c r="AC6" s="259"/>
-      <c r="AD6" s="259"/>
-      <c r="AE6" s="259"/>
-      <c r="AF6" s="259"/>
-      <c r="AG6" s="259"/>
-      <c r="AH6" s="259"/>
-      <c r="AI6" s="259"/>
-      <c r="AJ6" s="259"/>
-      <c r="AK6" s="259"/>
-      <c r="AL6" s="259"/>
-      <c r="AM6" s="259"/>
-      <c r="AN6" s="259"/>
+      <c r="AA6" s="283"/>
+      <c r="AB6" s="283"/>
+      <c r="AC6" s="283"/>
+      <c r="AD6" s="283"/>
+      <c r="AE6" s="283"/>
+      <c r="AF6" s="283"/>
+      <c r="AG6" s="283"/>
+      <c r="AH6" s="283"/>
+      <c r="AI6" s="283"/>
+      <c r="AJ6" s="283"/>
+      <c r="AK6" s="283"/>
+      <c r="AL6" s="283"/>
+      <c r="AM6" s="283"/>
+      <c r="AN6" s="283"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -7615,27 +8035,27 @@
         <v>NO</v>
       </c>
       <c r="V7" s="13"/>
-      <c r="X7" s="259"/>
-      <c r="Y7" s="259"/>
-      <c r="Z7" s="262" t="s">
+      <c r="X7" s="283"/>
+      <c r="Y7" s="283"/>
+      <c r="Z7" s="282" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="259"/>
-      <c r="AB7" s="259"/>
-      <c r="AC7" s="259"/>
-      <c r="AD7" s="262" t="s">
+      <c r="AA7" s="283"/>
+      <c r="AB7" s="283"/>
+      <c r="AC7" s="283"/>
+      <c r="AD7" s="282" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="259"/>
-      <c r="AF7" s="259"/>
-      <c r="AG7" s="259"/>
-      <c r="AH7" s="259"/>
-      <c r="AI7" s="259"/>
-      <c r="AJ7" s="259"/>
-      <c r="AK7" s="259"/>
-      <c r="AL7" s="259"/>
-      <c r="AM7" s="259"/>
-      <c r="AN7" s="259"/>
+      <c r="AE7" s="283"/>
+      <c r="AF7" s="283"/>
+      <c r="AG7" s="283"/>
+      <c r="AH7" s="283"/>
+      <c r="AI7" s="283"/>
+      <c r="AJ7" s="283"/>
+      <c r="AK7" s="283"/>
+      <c r="AL7" s="283"/>
+      <c r="AM7" s="283"/>
+      <c r="AN7" s="283"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -7685,8 +8105,8 @@
         <v>NO</v>
       </c>
       <c r="V8" s="13"/>
-      <c r="X8" s="259"/>
-      <c r="Y8" s="259"/>
+      <c r="X8" s="283"/>
+      <c r="Y8" s="283"/>
       <c r="Z8" s="172" t="s">
         <v>19</v>
       </c>
@@ -12233,10 +12653,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="260" t="s">
+      <c r="AA49" s="280" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="261"/>
+      <c r="AB49" s="281"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -12314,12 +12734,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="267" t="s">
+      <c r="AI50" s="276" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="268"/>
-      <c r="AK50" s="268"/>
-      <c r="AL50" s="269"/>
+      <c r="AJ50" s="277"/>
+      <c r="AK50" s="277"/>
+      <c r="AL50" s="278"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -12380,12 +12800,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="264" t="s">
+      <c r="AI51" s="273" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="265"/>
-      <c r="AK51" s="265"/>
-      <c r="AL51" s="266"/>
+      <c r="AJ51" s="274"/>
+      <c r="AK51" s="274"/>
+      <c r="AL51" s="275"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -12651,14 +13071,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="270"/>
-      <c r="AD55" s="270"/>
-      <c r="AI55" s="267" t="s">
+      <c r="AC55" s="279"/>
+      <c r="AD55" s="279"/>
+      <c r="AI55" s="276" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="268"/>
-      <c r="AK55" s="268"/>
-      <c r="AL55" s="269"/>
+      <c r="AJ55" s="277"/>
+      <c r="AK55" s="277"/>
+      <c r="AL55" s="278"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -12711,12 +13131,12 @@
         <v>NO</v>
       </c>
       <c r="V56" s="2"/>
-      <c r="AI56" s="249" t="s">
+      <c r="AI56" s="272" t="s">
         <v>168</v>
       </c>
-      <c r="AJ56" s="249"/>
-      <c r="AK56" s="249"/>
-      <c r="AL56" s="249"/>
+      <c r="AJ56" s="272"/>
+      <c r="AK56" s="272"/>
+      <c r="AL56" s="272"/>
       <c r="AM56" s="52">
         <f>AM50-AM55</f>
         <v>450000</v>
@@ -12911,32 +13331,32 @@
     <row r="61" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="250" t="s">
+      <c r="C63" s="285" t="s">
         <v>177</v>
       </c>
-      <c r="D63" s="251"/>
-      <c r="E63" s="251"/>
-      <c r="F63" s="251"/>
-      <c r="G63" s="252"/>
-      <c r="I63" s="256" t="s">
+      <c r="D63" s="286"/>
+      <c r="E63" s="286"/>
+      <c r="F63" s="286"/>
+      <c r="G63" s="287"/>
+      <c r="I63" s="291" t="s">
         <v>178</v>
       </c>
-      <c r="J63" s="256"/>
-      <c r="K63" s="256"/>
-      <c r="L63" s="256"/>
-      <c r="M63" s="256"/>
+      <c r="J63" s="291"/>
+      <c r="K63" s="291"/>
+      <c r="L63" s="291"/>
+      <c r="M63" s="291"/>
     </row>
     <row r="64" spans="1:41" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="253"/>
-      <c r="D64" s="254"/>
-      <c r="E64" s="254"/>
-      <c r="F64" s="254"/>
-      <c r="G64" s="255"/>
-      <c r="I64" s="256"/>
-      <c r="J64" s="256"/>
-      <c r="K64" s="256"/>
-      <c r="L64" s="256"/>
-      <c r="M64" s="256"/>
+      <c r="C64" s="288"/>
+      <c r="D64" s="289"/>
+      <c r="E64" s="289"/>
+      <c r="F64" s="289"/>
+      <c r="G64" s="290"/>
+      <c r="I64" s="291"/>
+      <c r="J64" s="291"/>
+      <c r="K64" s="291"/>
+      <c r="L64" s="291"/>
+      <c r="M64" s="291"/>
     </row>
     <row r="65" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12957,10 +13377,10 @@
       <c r="M70" s="55"/>
       <c r="N70" s="55"/>
       <c r="O70" s="55"/>
-      <c r="P70" s="249" t="s">
+      <c r="P70" s="272" t="s">
         <v>214</v>
       </c>
-      <c r="Q70" s="249"/>
+      <c r="Q70" s="272"/>
       <c r="R70" s="55"/>
       <c r="S70" s="55"/>
     </row>
@@ -13428,22 +13848,22 @@
   </sheetData>
   <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="16">
-    <mergeCell ref="AI56:AL56"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AI50:AL50"/>
-    <mergeCell ref="AI55:AL55"/>
-    <mergeCell ref="AC55:AD55"/>
-    <mergeCell ref="AA49:AB49"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="AD7:AN7"/>
-    <mergeCell ref="X5:AN5"/>
-    <mergeCell ref="Z6:AN6"/>
     <mergeCell ref="P70:Q70"/>
     <mergeCell ref="C63:G64"/>
     <mergeCell ref="I63:M64"/>
     <mergeCell ref="C2:T3"/>
     <mergeCell ref="Y6:Y8"/>
     <mergeCell ref="X6:X8"/>
+    <mergeCell ref="AA49:AB49"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="AD7:AN7"/>
+    <mergeCell ref="X5:AN5"/>
+    <mergeCell ref="Z6:AN6"/>
+    <mergeCell ref="AI56:AL56"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AI50:AL50"/>
+    <mergeCell ref="AI55:AL55"/>
+    <mergeCell ref="AC55:AD55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:V60">
     <cfRule type="expression" dxfId="10" priority="7">
@@ -13505,14 +13925,523 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD28"/>
+  <dimension ref="A2:L36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="230" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="241" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" style="230" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28" style="242" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="374" t="s">
+        <v>304</v>
+      </c>
+      <c r="B2" s="374"/>
+      <c r="C2" s="374"/>
+      <c r="D2" s="374"/>
+      <c r="E2" s="374"/>
+      <c r="F2" s="374"/>
+      <c r="G2" s="374"/>
+      <c r="H2" s="374"/>
+      <c r="I2" s="374"/>
+      <c r="J2" s="374"/>
+      <c r="K2" s="374"/>
+      <c r="L2" s="374"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="374"/>
+      <c r="B3" s="374"/>
+      <c r="C3" s="374"/>
+      <c r="D3" s="374"/>
+      <c r="E3" s="374"/>
+      <c r="F3" s="374"/>
+      <c r="G3" s="374"/>
+      <c r="H3" s="374"/>
+      <c r="I3" s="374"/>
+      <c r="J3" s="374"/>
+      <c r="K3" s="374"/>
+      <c r="L3" s="374"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="291" t="s">
+        <v>307</v>
+      </c>
+      <c r="B5" s="291"/>
+      <c r="C5" s="291"/>
+      <c r="D5" s="291"/>
+      <c r="E5" s="291"/>
+      <c r="F5" s="291"/>
+      <c r="G5" s="291"/>
+      <c r="H5" s="291"/>
+      <c r="I5" s="291"/>
+      <c r="J5" s="291"/>
+      <c r="K5" s="291"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="291"/>
+      <c r="B6" s="291"/>
+      <c r="C6" s="291"/>
+      <c r="D6" s="291"/>
+      <c r="E6" s="291"/>
+      <c r="F6" s="291"/>
+      <c r="G6" s="291"/>
+      <c r="H6" s="291"/>
+      <c r="I6" s="291"/>
+      <c r="J6" s="291"/>
+      <c r="K6" s="291"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="243" t="s">
+        <v>305</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="244" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="245" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="243" t="s">
+        <v>308</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E9" s="246">
+        <v>1657729.18</v>
+      </c>
+      <c r="F9" s="238" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="243" t="s">
+        <v>243</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E10" s="247" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="237">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="243" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E11" s="247" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" s="237">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
+      <c r="C12" s="236" t="s">
+        <v>306</v>
+      </c>
+      <c r="D12" s="229" t="s">
+        <v>314</v>
+      </c>
+      <c r="E12" s="237">
+        <v>1214000</v>
+      </c>
+      <c r="F12" s="238" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>5</v>
+      </c>
+      <c r="C13" s="236">
+        <v>43709</v>
+      </c>
+      <c r="D13" s="229" t="s">
+        <v>266</v>
+      </c>
+      <c r="E13" s="237">
+        <v>64000</v>
+      </c>
+      <c r="F13" s="238" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>6</v>
+      </c>
+      <c r="C14" s="236">
+        <v>43716</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E14" s="237">
+        <v>64000</v>
+      </c>
+      <c r="F14" s="238" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>7</v>
+      </c>
+      <c r="C15" s="243">
+        <v>43718</v>
+      </c>
+      <c r="D15" s="229" t="s">
+        <v>290</v>
+      </c>
+      <c r="E15" s="237">
+        <v>443000</v>
+      </c>
+      <c r="F15" s="238" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>8</v>
+      </c>
+      <c r="C16" s="243">
+        <v>43719</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E16" s="238" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" s="237">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>9</v>
+      </c>
+      <c r="C17" s="243">
+        <v>43726</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E17" s="237">
+        <v>79000</v>
+      </c>
+      <c r="F17" s="238" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>10</v>
+      </c>
+      <c r="C18" s="243">
+        <v>43726</v>
+      </c>
+      <c r="D18" s="229" t="s">
+        <v>283</v>
+      </c>
+      <c r="E18" s="238" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" s="237">
+        <v>320000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>11</v>
+      </c>
+      <c r="C19" s="243">
+        <v>43726</v>
+      </c>
+      <c r="D19" s="229" t="s">
+        <v>287</v>
+      </c>
+      <c r="E19" s="238" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" s="238">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>12</v>
+      </c>
+      <c r="C20" s="243">
+        <v>43728</v>
+      </c>
+      <c r="D20" s="229" t="s">
+        <v>310</v>
+      </c>
+      <c r="E20" s="237" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="238">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>13</v>
+      </c>
+      <c r="C21" s="243">
+        <v>43728</v>
+      </c>
+      <c r="D21" s="229" t="s">
+        <v>311</v>
+      </c>
+      <c r="E21" s="238" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="237">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>14</v>
+      </c>
+      <c r="C22" s="243">
+        <v>43729</v>
+      </c>
+      <c r="D22" s="229" t="s">
+        <v>312</v>
+      </c>
+      <c r="E22" s="238" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" s="238">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>15</v>
+      </c>
+      <c r="C23" s="243">
+        <v>43729</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E23" s="237">
+        <v>40000</v>
+      </c>
+      <c r="F23" s="238" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>16</v>
+      </c>
+      <c r="C24" s="243">
+        <v>43729</v>
+      </c>
+      <c r="D24" s="229" t="s">
+        <v>313</v>
+      </c>
+      <c r="E24" s="238" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" s="237">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>17</v>
+      </c>
+      <c r="C25" s="243">
+        <v>43737</v>
+      </c>
+      <c r="D25" s="229" t="s">
+        <v>315</v>
+      </c>
+      <c r="E25" s="237" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" s="237">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>18</v>
+      </c>
+      <c r="C26" s="243"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="237"/>
+      <c r="F26" s="237"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>19</v>
+      </c>
+      <c r="C27" s="243"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="237"/>
+      <c r="F27" s="237"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>20</v>
+      </c>
+      <c r="C28" s="243"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="237"/>
+      <c r="F28" s="237"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>21</v>
+      </c>
+      <c r="C29" s="243"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="237"/>
+      <c r="F29" s="237"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>22</v>
+      </c>
+      <c r="C30" s="243"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="237"/>
+      <c r="F30" s="237"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>23</v>
+      </c>
+      <c r="C31" s="243"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="237"/>
+      <c r="F31" s="237"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>24</v>
+      </c>
+      <c r="C32" s="243"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="56"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>25</v>
+      </c>
+      <c r="C33" s="243">
+        <v>43738</v>
+      </c>
+      <c r="D33" s="229" t="s">
+        <v>303</v>
+      </c>
+      <c r="E33" s="57"/>
+      <c r="F33" s="56">
+        <v>41858</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="221"/>
+      <c r="C34" s="248">
+        <v>43738</v>
+      </c>
+      <c r="D34" s="249" t="s">
+        <v>316</v>
+      </c>
+      <c r="E34" s="250">
+        <f>SUM(E9:E33)</f>
+        <v>3561729.1799999997</v>
+      </c>
+      <c r="F34" s="251">
+        <f>SUM(F9:F33)</f>
+        <v>910858</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="379" t="s">
+        <v>317</v>
+      </c>
+      <c r="C35" s="380"/>
+      <c r="D35" s="381"/>
+      <c r="E35" s="375">
+        <f>E34-F34</f>
+        <v>2650871.1799999997</v>
+      </c>
+      <c r="F35" s="376"/>
+    </row>
+    <row r="36" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="382"/>
+      <c r="C36" s="383"/>
+      <c r="D36" s="384"/>
+      <c r="E36" s="377"/>
+      <c r="F36" s="378"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:L3"/>
+    <mergeCell ref="A5:K6"/>
+    <mergeCell ref="E35:F36"/>
+    <mergeCell ref="B35:D36"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD28"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R3" sqref="O3:R5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" customWidth="1"/>
     <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="12" max="12" width="25.42578125" customWidth="1"/>
@@ -13529,17 +14458,17 @@
       <c r="A2" s="199"/>
       <c r="B2" s="200"/>
       <c r="C2" s="200"/>
-      <c r="D2" s="328" t="s">
+      <c r="D2" s="294" t="s">
         <v>247</v>
       </c>
-      <c r="E2" s="328"/>
-      <c r="F2" s="328"/>
-      <c r="G2" s="328"/>
-      <c r="H2" s="328"/>
-      <c r="I2" s="328"/>
-      <c r="J2" s="328"/>
-      <c r="K2" s="328"/>
-      <c r="L2" s="328"/>
+      <c r="E2" s="294"/>
+      <c r="F2" s="294"/>
+      <c r="G2" s="294"/>
+      <c r="H2" s="294"/>
+      <c r="I2" s="294"/>
+      <c r="J2" s="294"/>
+      <c r="K2" s="294"/>
+      <c r="L2" s="294"/>
       <c r="M2" s="201"/>
       <c r="N2" s="24"/>
     </row>
@@ -13557,205 +14486,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="203"/>
-      <c r="U3" s="271" t="s">
+      <c r="U3" s="344" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="272"/>
-      <c r="W3" s="273" t="s">
+      <c r="V3" s="345"/>
+      <c r="W3" s="346" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="272"/>
-      <c r="Y3" s="272"/>
-      <c r="Z3" s="272"/>
-      <c r="AA3" s="272"/>
-      <c r="AB3" s="272"/>
-      <c r="AC3" s="272"/>
-      <c r="AD3" s="274"/>
+      <c r="X3" s="345"/>
+      <c r="Y3" s="345"/>
+      <c r="Z3" s="345"/>
+      <c r="AA3" s="345"/>
+      <c r="AB3" s="345"/>
+      <c r="AC3" s="345"/>
+      <c r="AD3" s="347"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="202"/>
-      <c r="B4" s="332" t="s">
+      <c r="B4" s="309" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="333"/>
-      <c r="D4" s="333"/>
-      <c r="E4" s="333"/>
-      <c r="F4" s="333"/>
+      <c r="C4" s="310"/>
+      <c r="D4" s="310"/>
+      <c r="E4" s="310"/>
+      <c r="F4" s="310"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="280" t="s">
+      <c r="I4" s="313" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="262"/>
-      <c r="K4" s="262"/>
-      <c r="L4" s="262"/>
+      <c r="J4" s="282"/>
+      <c r="K4" s="282"/>
+      <c r="L4" s="282"/>
       <c r="M4" s="203"/>
-      <c r="U4" s="292" t="s">
+      <c r="U4" s="356" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="262"/>
-      <c r="W4" s="280" t="s">
+      <c r="V4" s="282"/>
+      <c r="W4" s="313" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="262"/>
-      <c r="Y4" s="262"/>
-      <c r="Z4" s="262"/>
-      <c r="AA4" s="262"/>
-      <c r="AB4" s="262"/>
-      <c r="AC4" s="262"/>
-      <c r="AD4" s="275"/>
+      <c r="X4" s="282"/>
+      <c r="Y4" s="282"/>
+      <c r="Z4" s="282"/>
+      <c r="AA4" s="282"/>
+      <c r="AB4" s="282"/>
+      <c r="AC4" s="282"/>
+      <c r="AD4" s="333"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="202"/>
-      <c r="B5" s="297" t="s">
+      <c r="B5" s="304" t="s">
         <v>237</v>
       </c>
-      <c r="C5" s="262"/>
-      <c r="D5" s="262"/>
-      <c r="E5" s="262"/>
-      <c r="F5" s="262"/>
+      <c r="C5" s="282"/>
+      <c r="D5" s="282"/>
+      <c r="E5" s="282"/>
+      <c r="F5" s="282"/>
       <c r="G5" s="173">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="299" t="s">
+      <c r="I5" s="302" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="320"/>
-      <c r="K5" s="322">
+      <c r="J5" s="303"/>
+      <c r="K5" s="314">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="323"/>
+      <c r="L5" s="315"/>
       <c r="M5" s="203"/>
-      <c r="U5" s="293" t="s">
+      <c r="U5" s="340" t="s">
         <v>233</v>
       </c>
-      <c r="V5" s="294"/>
-      <c r="W5" s="299" t="s">
+      <c r="V5" s="341"/>
+      <c r="W5" s="302" t="s">
         <v>234</v>
       </c>
-      <c r="X5" s="300"/>
-      <c r="Y5" s="300"/>
-      <c r="Z5" s="300"/>
-      <c r="AA5" s="300"/>
-      <c r="AB5" s="300"/>
-      <c r="AC5" s="300"/>
-      <c r="AD5" s="301"/>
+      <c r="X5" s="327"/>
+      <c r="Y5" s="327"/>
+      <c r="Z5" s="327"/>
+      <c r="AA5" s="327"/>
+      <c r="AB5" s="327"/>
+      <c r="AC5" s="327"/>
+      <c r="AD5" s="328"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="202"/>
-      <c r="B6" s="290" t="s">
+      <c r="B6" s="296" t="s">
         <v>238</v>
       </c>
-      <c r="C6" s="291"/>
-      <c r="D6" s="291"/>
-      <c r="E6" s="291"/>
-      <c r="F6" s="291"/>
+      <c r="C6" s="297"/>
+      <c r="D6" s="297"/>
+      <c r="E6" s="297"/>
+      <c r="F6" s="297"/>
       <c r="G6" s="173">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="321" t="s">
+      <c r="I6" s="300" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="316"/>
-      <c r="K6" s="324">
+      <c r="J6" s="301"/>
+      <c r="K6" s="316">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="325"/>
+      <c r="L6" s="317"/>
       <c r="M6" s="203"/>
-      <c r="U6" s="295"/>
-      <c r="V6" s="296"/>
-      <c r="W6" s="281" t="s">
+      <c r="U6" s="342"/>
+      <c r="V6" s="343"/>
+      <c r="W6" s="329" t="s">
         <v>235</v>
       </c>
-      <c r="X6" s="282"/>
-      <c r="Y6" s="282"/>
-      <c r="Z6" s="282"/>
-      <c r="AA6" s="282"/>
-      <c r="AB6" s="282"/>
-      <c r="AC6" s="282"/>
-      <c r="AD6" s="283"/>
+      <c r="X6" s="330"/>
+      <c r="Y6" s="330"/>
+      <c r="Z6" s="330"/>
+      <c r="AA6" s="330"/>
+      <c r="AB6" s="330"/>
+      <c r="AC6" s="330"/>
+      <c r="AD6" s="331"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="202"/>
-      <c r="B7" s="302" t="s">
+      <c r="B7" s="307" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="303"/>
-      <c r="D7" s="303"/>
-      <c r="E7" s="303"/>
-      <c r="F7" s="316"/>
+      <c r="C7" s="308"/>
+      <c r="D7" s="308"/>
+      <c r="E7" s="308"/>
+      <c r="F7" s="301"/>
       <c r="G7" s="173">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="321" t="s">
+      <c r="I7" s="300" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="316"/>
-      <c r="K7" s="326">
+      <c r="J7" s="301"/>
+      <c r="K7" s="311">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="327"/>
+      <c r="L7" s="312"/>
       <c r="M7" s="203"/>
-      <c r="U7" s="278"/>
-      <c r="V7" s="279"/>
-      <c r="W7" s="280" t="s">
+      <c r="U7" s="348"/>
+      <c r="V7" s="349"/>
+      <c r="W7" s="313" t="s">
         <v>236</v>
       </c>
-      <c r="X7" s="262"/>
-      <c r="Y7" s="262"/>
-      <c r="Z7" s="262"/>
-      <c r="AA7" s="262"/>
-      <c r="AB7" s="262"/>
-      <c r="AC7" s="262"/>
-      <c r="AD7" s="275"/>
+      <c r="X7" s="282"/>
+      <c r="Y7" s="282"/>
+      <c r="Z7" s="282"/>
+      <c r="AA7" s="282"/>
+      <c r="AB7" s="282"/>
+      <c r="AC7" s="282"/>
+      <c r="AD7" s="333"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="202"/>
-      <c r="B8" s="330" t="s">
+      <c r="B8" s="305" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="331"/>
-      <c r="D8" s="331"/>
-      <c r="E8" s="331"/>
-      <c r="F8" s="331"/>
+      <c r="C8" s="306"/>
+      <c r="D8" s="306"/>
+      <c r="E8" s="306"/>
+      <c r="F8" s="306"/>
       <c r="G8" s="174">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="299" t="s">
+      <c r="I8" s="302" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="320"/>
-      <c r="K8" s="311">
+      <c r="J8" s="303"/>
+      <c r="K8" s="298">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="312"/>
+      <c r="L8" s="299"/>
       <c r="M8" s="203"/>
-      <c r="U8" s="286" t="s">
+      <c r="U8" s="352" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="287"/>
-      <c r="W8" s="281" t="s">
+      <c r="V8" s="353"/>
+      <c r="W8" s="329" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="282"/>
-      <c r="Y8" s="282"/>
-      <c r="Z8" s="282"/>
-      <c r="AA8" s="282"/>
-      <c r="AB8" s="282"/>
-      <c r="AC8" s="282"/>
-      <c r="AD8" s="283"/>
+      <c r="X8" s="330"/>
+      <c r="Y8" s="330"/>
+      <c r="Z8" s="330"/>
+      <c r="AA8" s="330"/>
+      <c r="AB8" s="330"/>
+      <c r="AC8" s="330"/>
+      <c r="AD8" s="331"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="202"/>
@@ -13771,28 +14700,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="203"/>
-      <c r="U9" s="288"/>
-      <c r="V9" s="289"/>
-      <c r="W9" s="281" t="s">
+      <c r="U9" s="354"/>
+      <c r="V9" s="355"/>
+      <c r="W9" s="329" t="s">
         <v>239</v>
       </c>
-      <c r="X9" s="282"/>
-      <c r="Y9" s="282"/>
-      <c r="Z9" s="282"/>
-      <c r="AA9" s="282"/>
-      <c r="AB9" s="282"/>
-      <c r="AC9" s="282"/>
-      <c r="AD9" s="283"/>
+      <c r="X9" s="330"/>
+      <c r="Y9" s="330"/>
+      <c r="Z9" s="330"/>
+      <c r="AA9" s="330"/>
+      <c r="AB9" s="330"/>
+      <c r="AC9" s="330"/>
+      <c r="AD9" s="331"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="202"/>
-      <c r="B10" s="262" t="s">
+      <c r="B10" s="282" t="s">
         <v>256</v>
       </c>
-      <c r="C10" s="262"/>
-      <c r="D10" s="262"/>
-      <c r="E10" s="262"/>
-      <c r="F10" s="262"/>
+      <c r="C10" s="282"/>
+      <c r="D10" s="282"/>
+      <c r="E10" s="282"/>
+      <c r="F10" s="282"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -13803,30 +14732,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="203"/>
-      <c r="U10" s="290" t="s">
+      <c r="U10" s="296" t="s">
         <v>246</v>
       </c>
-      <c r="V10" s="291"/>
-      <c r="W10" s="262" t="s">
+      <c r="V10" s="297"/>
+      <c r="W10" s="282" t="s">
         <v>260</v>
       </c>
-      <c r="X10" s="262"/>
-      <c r="Y10" s="262"/>
-      <c r="Z10" s="262"/>
-      <c r="AA10" s="262"/>
-      <c r="AB10" s="262"/>
-      <c r="AC10" s="262"/>
-      <c r="AD10" s="275"/>
+      <c r="X10" s="282"/>
+      <c r="Y10" s="282"/>
+      <c r="Z10" s="282"/>
+      <c r="AA10" s="282"/>
+      <c r="AB10" s="282"/>
+      <c r="AC10" s="282"/>
+      <c r="AD10" s="333"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="202"/>
-      <c r="B11" s="262" t="s">
+      <c r="B11" s="282" t="s">
         <v>257</v>
       </c>
-      <c r="C11" s="262"/>
-      <c r="D11" s="262"/>
-      <c r="E11" s="262"/>
-      <c r="F11" s="262"/>
+      <c r="C11" s="282"/>
+      <c r="D11" s="282"/>
+      <c r="E11" s="282"/>
+      <c r="F11" s="282"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -13836,30 +14765,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="203"/>
-      <c r="U11" s="290" t="s">
+      <c r="U11" s="296" t="s">
         <v>259</v>
       </c>
-      <c r="V11" s="291"/>
-      <c r="W11" s="284" t="s">
+      <c r="V11" s="297"/>
+      <c r="W11" s="350" t="s">
         <v>261</v>
       </c>
-      <c r="X11" s="284"/>
-      <c r="Y11" s="284"/>
-      <c r="Z11" s="284"/>
-      <c r="AA11" s="284"/>
-      <c r="AB11" s="284"/>
-      <c r="AC11" s="284"/>
-      <c r="AD11" s="285"/>
+      <c r="X11" s="350"/>
+      <c r="Y11" s="350"/>
+      <c r="Z11" s="350"/>
+      <c r="AA11" s="350"/>
+      <c r="AB11" s="350"/>
+      <c r="AC11" s="350"/>
+      <c r="AD11" s="351"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="202"/>
-      <c r="B12" s="329" t="s">
+      <c r="B12" s="295" t="s">
         <v>258</v>
       </c>
-      <c r="C12" s="329"/>
-      <c r="D12" s="329"/>
-      <c r="E12" s="329"/>
-      <c r="F12" s="329"/>
+      <c r="C12" s="295"/>
+      <c r="D12" s="295"/>
+      <c r="E12" s="295"/>
+      <c r="F12" s="295"/>
       <c r="G12" s="207">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -13870,16 +14799,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="203"/>
-      <c r="U12" s="290"/>
-      <c r="V12" s="291"/>
-      <c r="W12" s="262"/>
-      <c r="X12" s="262"/>
-      <c r="Y12" s="262"/>
-      <c r="Z12" s="262"/>
-      <c r="AA12" s="262"/>
-      <c r="AB12" s="262"/>
-      <c r="AC12" s="262"/>
-      <c r="AD12" s="275"/>
+      <c r="U12" s="296"/>
+      <c r="V12" s="297"/>
+      <c r="W12" s="282"/>
+      <c r="X12" s="282"/>
+      <c r="Y12" s="282"/>
+      <c r="Z12" s="282"/>
+      <c r="AA12" s="282"/>
+      <c r="AB12" s="282"/>
+      <c r="AC12" s="282"/>
+      <c r="AD12" s="333"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="204"/>
@@ -13895,64 +14824,64 @@
       <c r="K13" s="205"/>
       <c r="L13" s="205"/>
       <c r="M13" s="206"/>
-      <c r="U13" s="290"/>
-      <c r="V13" s="291"/>
-      <c r="W13" s="262"/>
-      <c r="X13" s="262"/>
-      <c r="Y13" s="262"/>
-      <c r="Z13" s="262"/>
-      <c r="AA13" s="262"/>
-      <c r="AB13" s="262"/>
-      <c r="AC13" s="262"/>
-      <c r="AD13" s="275"/>
+      <c r="U13" s="296"/>
+      <c r="V13" s="297"/>
+      <c r="W13" s="282"/>
+      <c r="X13" s="282"/>
+      <c r="Y13" s="282"/>
+      <c r="Z13" s="282"/>
+      <c r="AA13" s="282"/>
+      <c r="AB13" s="282"/>
+      <c r="AC13" s="282"/>
+      <c r="AD13" s="333"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="305"/>
-      <c r="V14" s="306"/>
-      <c r="W14" s="276"/>
-      <c r="X14" s="276"/>
-      <c r="Y14" s="276"/>
-      <c r="Z14" s="276"/>
-      <c r="AA14" s="276"/>
-      <c r="AB14" s="276"/>
-      <c r="AC14" s="276"/>
-      <c r="AD14" s="277"/>
+      <c r="U14" s="334"/>
+      <c r="V14" s="335"/>
+      <c r="W14" s="325"/>
+      <c r="X14" s="325"/>
+      <c r="Y14" s="325"/>
+      <c r="Z14" s="325"/>
+      <c r="AA14" s="325"/>
+      <c r="AB14" s="325"/>
+      <c r="AC14" s="325"/>
+      <c r="AD14" s="326"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="199"/>
       <c r="B18" s="200"/>
       <c r="C18" s="200"/>
-      <c r="D18" s="328" t="s">
+      <c r="D18" s="294" t="s">
         <v>252</v>
       </c>
-      <c r="E18" s="328"/>
-      <c r="F18" s="328"/>
-      <c r="G18" s="328"/>
-      <c r="H18" s="328"/>
-      <c r="I18" s="328"/>
-      <c r="J18" s="328"/>
-      <c r="K18" s="328"/>
-      <c r="L18" s="328"/>
+      <c r="E18" s="294"/>
+      <c r="F18" s="294"/>
+      <c r="G18" s="294"/>
+      <c r="H18" s="294"/>
+      <c r="I18" s="294"/>
+      <c r="J18" s="294"/>
+      <c r="K18" s="294"/>
+      <c r="L18" s="294"/>
       <c r="M18" s="201"/>
-      <c r="O18" s="307" t="s">
+      <c r="O18" s="336" t="s">
         <v>253</v>
       </c>
-      <c r="P18" s="308"/>
-      <c r="Q18" s="308"/>
-      <c r="R18" s="308"/>
-      <c r="S18" s="309"/>
+      <c r="P18" s="337"/>
+      <c r="Q18" s="337"/>
+      <c r="R18" s="337"/>
+      <c r="S18" s="338"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="202"/>
       <c r="M19" s="203"/>
-      <c r="O19" s="297" t="s">
+      <c r="O19" s="304" t="s">
         <v>254</v>
       </c>
-      <c r="P19" s="262"/>
-      <c r="Q19" s="262"/>
-      <c r="R19" s="262"/>
-      <c r="S19" s="275"/>
+      <c r="P19" s="282"/>
+      <c r="Q19" s="282"/>
+      <c r="R19" s="282"/>
+      <c r="S19" s="333"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="202"/>
@@ -13963,119 +14892,119 @@
       <c r="F20" s="227"/>
       <c r="G20" s="68"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="280" t="s">
+      <c r="I20" s="313" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="262"/>
-      <c r="K20" s="262"/>
-      <c r="L20" s="262"/>
+      <c r="J20" s="282"/>
+      <c r="K20" s="282"/>
+      <c r="L20" s="282"/>
       <c r="M20" s="203"/>
-      <c r="O20" s="297" t="s">
+      <c r="O20" s="304" t="s">
         <v>255</v>
       </c>
-      <c r="P20" s="262"/>
-      <c r="Q20" s="262"/>
-      <c r="R20" s="262"/>
-      <c r="S20" s="275"/>
+      <c r="P20" s="282"/>
+      <c r="Q20" s="282"/>
+      <c r="R20" s="282"/>
+      <c r="S20" s="333"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="202"/>
-      <c r="B21" s="313" t="s">
-        <v>301</v>
-      </c>
-      <c r="C21" s="314"/>
-      <c r="D21" s="314"/>
-      <c r="E21" s="314"/>
-      <c r="F21" s="315"/>
+      <c r="B21" s="318" t="s">
+        <v>300</v>
+      </c>
+      <c r="C21" s="319"/>
+      <c r="D21" s="319"/>
+      <c r="E21" s="319"/>
+      <c r="F21" s="320"/>
       <c r="G21" s="70">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="299" t="s">
+      <c r="I21" s="302" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="320"/>
-      <c r="K21" s="322">
+      <c r="J21" s="303"/>
+      <c r="K21" s="314">
         <f>G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="L21" s="323"/>
+      <c r="L21" s="315"/>
       <c r="M21" s="203"/>
       <c r="N21" s="197"/>
-      <c r="O21" s="310" t="s">
+      <c r="O21" s="339" t="s">
         <v>262</v>
       </c>
-      <c r="P21" s="300"/>
-      <c r="Q21" s="300"/>
-      <c r="R21" s="300"/>
-      <c r="S21" s="301"/>
+      <c r="P21" s="327"/>
+      <c r="Q21" s="327"/>
+      <c r="R21" s="327"/>
+      <c r="S21" s="328"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="202"/>
-      <c r="B22" s="302" t="s">
+      <c r="B22" s="307" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="303"/>
-      <c r="D22" s="303"/>
-      <c r="E22" s="303"/>
-      <c r="F22" s="316"/>
+      <c r="C22" s="308"/>
+      <c r="D22" s="308"/>
+      <c r="E22" s="308"/>
+      <c r="F22" s="301"/>
       <c r="G22" s="173">
         <f>G21</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="321" t="s">
+      <c r="I22" s="300" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="316"/>
-      <c r="K22" s="324">
+      <c r="J22" s="301"/>
+      <c r="K22" s="316">
         <f>Pengeluaran!L30</f>
-        <v>836358</v>
-      </c>
-      <c r="L22" s="325"/>
+        <v>779000</v>
+      </c>
+      <c r="L22" s="317"/>
       <c r="M22" s="203"/>
       <c r="N22" s="197"/>
-      <c r="O22" s="302" t="s">
+      <c r="O22" s="307" t="s">
         <v>263</v>
       </c>
-      <c r="P22" s="303"/>
-      <c r="Q22" s="303"/>
-      <c r="R22" s="303"/>
-      <c r="S22" s="304"/>
+      <c r="P22" s="308"/>
+      <c r="Q22" s="308"/>
+      <c r="R22" s="308"/>
+      <c r="S22" s="332"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="202"/>
-      <c r="B23" s="317" t="s">
+      <c r="B23" s="321" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="318"/>
-      <c r="D23" s="318"/>
-      <c r="E23" s="318"/>
-      <c r="F23" s="319"/>
+      <c r="C23" s="322"/>
+      <c r="D23" s="322"/>
+      <c r="E23" s="322"/>
+      <c r="F23" s="323"/>
       <c r="G23" s="174">
         <f>K24</f>
-        <v>1511371.1800000002</v>
+        <v>1568729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="321" t="s">
+      <c r="I23" s="300" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="316"/>
-      <c r="K23" s="326">
+      <c r="J23" s="301"/>
+      <c r="K23" s="311">
         <f>Pemasukkan!L31</f>
         <v>690000</v>
       </c>
-      <c r="L23" s="327"/>
+      <c r="L23" s="312"/>
       <c r="M23" s="203"/>
       <c r="N23" s="197"/>
-      <c r="O23" s="302" t="s">
+      <c r="O23" s="307" t="s">
         <v>264</v>
       </c>
-      <c r="P23" s="303"/>
-      <c r="Q23" s="303"/>
-      <c r="R23" s="303"/>
-      <c r="S23" s="304"/>
+      <c r="P23" s="308"/>
+      <c r="Q23" s="308"/>
+      <c r="R23" s="308"/>
+      <c r="S23" s="332"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="202"/>
@@ -14086,24 +15015,24 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="299" t="s">
+      <c r="I24" s="302" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="320"/>
-      <c r="K24" s="311">
+      <c r="J24" s="303"/>
+      <c r="K24" s="298">
         <f>(K21-K22)+K23</f>
-        <v>1511371.1800000002</v>
-      </c>
-      <c r="L24" s="312"/>
+        <v>1568729.1800000002</v>
+      </c>
+      <c r="L24" s="299"/>
       <c r="M24" s="203"/>
       <c r="N24" s="197"/>
-      <c r="O24" s="302" t="s">
+      <c r="O24" s="307" t="s">
         <v>265</v>
       </c>
-      <c r="P24" s="303"/>
-      <c r="Q24" s="303"/>
-      <c r="R24" s="303"/>
-      <c r="S24" s="304"/>
+      <c r="P24" s="308"/>
+      <c r="Q24" s="308"/>
+      <c r="R24" s="308"/>
+      <c r="S24" s="332"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="202"/>
@@ -14120,13 +15049,13 @@
       <c r="L25" s="24"/>
       <c r="M25" s="203"/>
       <c r="N25" s="197"/>
-      <c r="O25" s="297" t="s">
+      <c r="O25" s="304" t="s">
         <v>270</v>
       </c>
-      <c r="P25" s="262"/>
-      <c r="Q25" s="262"/>
-      <c r="R25" s="262"/>
-      <c r="S25" s="275"/>
+      <c r="P25" s="282"/>
+      <c r="Q25" s="282"/>
+      <c r="R25" s="282"/>
+      <c r="S25" s="333"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="202"/>
@@ -14143,11 +15072,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="203"/>
       <c r="N26" s="197"/>
-      <c r="O26" s="298"/>
-      <c r="P26" s="276"/>
-      <c r="Q26" s="276"/>
-      <c r="R26" s="276"/>
-      <c r="S26" s="277"/>
+      <c r="O26" s="324"/>
+      <c r="P26" s="325"/>
+      <c r="Q26" s="325"/>
+      <c r="R26" s="325"/>
+      <c r="S26" s="326"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="204"/>
@@ -14182,6 +15111,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:AD3"/>
+    <mergeCell ref="W12:AD12"/>
+    <mergeCell ref="W13:AD13"/>
+    <mergeCell ref="W14:AD14"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:AD7"/>
+    <mergeCell ref="W9:AD9"/>
+    <mergeCell ref="W10:AD10"/>
+    <mergeCell ref="W11:AD11"/>
+    <mergeCell ref="U8:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:AD4"/>
+    <mergeCell ref="W8:AD8"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="O25:S25"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="W5:AD5"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="O18:S18"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O23:S23"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
     <mergeCell ref="D2:L2"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
@@ -14198,65 +15174,19 @@
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="W5:AD5"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="O24:S24"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="O18:S18"/>
-    <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O23:S23"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="W4:AD4"/>
-    <mergeCell ref="W8:AD8"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="O25:S25"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:AD3"/>
-    <mergeCell ref="W12:AD12"/>
-    <mergeCell ref="W13:AD13"/>
-    <mergeCell ref="W14:AD14"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="W7:AD7"/>
-    <mergeCell ref="W9:AD9"/>
-    <mergeCell ref="W10:AD10"/>
-    <mergeCell ref="W11:AD11"/>
-    <mergeCell ref="U8:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U4:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:M220"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29:K29"/>
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14277,44 +15207,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="343" t="s">
+      <c r="C2" s="357" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="344"/>
-      <c r="E2" s="344"/>
-      <c r="F2" s="344"/>
-      <c r="G2" s="344"/>
-      <c r="H2" s="344"/>
-      <c r="I2" s="344"/>
-      <c r="J2" s="344"/>
-      <c r="K2" s="344"/>
+      <c r="D2" s="358"/>
+      <c r="E2" s="358"/>
+      <c r="F2" s="358"/>
+      <c r="G2" s="358"/>
+      <c r="H2" s="358"/>
+      <c r="I2" s="358"/>
+      <c r="J2" s="358"/>
+      <c r="K2" s="358"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="344"/>
-      <c r="D3" s="344"/>
-      <c r="E3" s="344"/>
-      <c r="F3" s="344"/>
-      <c r="G3" s="344"/>
-      <c r="H3" s="344"/>
-      <c r="I3" s="344"/>
-      <c r="J3" s="344"/>
-      <c r="K3" s="344"/>
+      <c r="C3" s="358"/>
+      <c r="D3" s="358"/>
+      <c r="E3" s="358"/>
+      <c r="F3" s="358"/>
+      <c r="G3" s="358"/>
+      <c r="H3" s="358"/>
+      <c r="I3" s="358"/>
+      <c r="J3" s="358"/>
+      <c r="K3" s="358"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="336" t="s">
+      <c r="C5" s="365" t="s">
         <v>250</v>
       </c>
-      <c r="D5" s="336"/>
-      <c r="E5" s="336"/>
-      <c r="F5" s="336"/>
-      <c r="G5" s="336"/>
-      <c r="I5" s="336" t="s">
+      <c r="D5" s="365"/>
+      <c r="E5" s="365"/>
+      <c r="F5" s="365"/>
+      <c r="G5" s="365"/>
+      <c r="I5" s="365" t="s">
         <v>251</v>
       </c>
-      <c r="J5" s="336"/>
-      <c r="K5" s="336"/>
-      <c r="L5" s="336"/>
-      <c r="M5" s="336"/>
+      <c r="J5" s="365"/>
+      <c r="K5" s="365"/>
+      <c r="L5" s="365"/>
+      <c r="M5" s="365"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -14427,7 +15357,7 @@
         <v>290</v>
       </c>
       <c r="K9" s="226" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L9" s="64">
         <v>443000</v>
@@ -14471,17 +15401,17 @@
       <c r="I11" s="1">
         <v>5</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="23" t="s">
+        <v>297</v>
+      </c>
+      <c r="K11" s="239" t="s">
         <v>298</v>
       </c>
-      <c r="K11" s="226" t="s">
+      <c r="L11" s="67">
+        <v>40000</v>
+      </c>
+      <c r="M11" s="23" t="s">
         <v>299</v>
-      </c>
-      <c r="L11" s="64">
-        <v>40000</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="12" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14492,13 +15422,13 @@
       <c r="E12" s="1"/>
       <c r="F12" s="64"/>
       <c r="G12" s="1"/>
-      <c r="I12" s="1">
+      <c r="I12" s="214">
         <v>6</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="1"/>
+      <c r="J12" s="231"/>
+      <c r="K12" s="231"/>
+      <c r="L12" s="231"/>
+      <c r="M12" s="231"/>
     </row>
     <row r="13" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
@@ -14511,10 +15441,10 @@
       <c r="I13" s="1">
         <v>7</v>
       </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="1"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="240"/>
+      <c r="L13" s="233"/>
+      <c r="M13" s="10"/>
     </row>
     <row r="14" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
@@ -14754,88 +15684,88 @@
       <c r="M28" s="197"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="332" t="s">
+      <c r="D29" s="309" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="333"/>
-      <c r="F29" s="337">
+      <c r="E29" s="310"/>
+      <c r="F29" s="359">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="338"/>
+      <c r="G29" s="360"/>
       <c r="I29" s="197"/>
-      <c r="J29" s="332" t="s">
+      <c r="J29" s="309" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="333"/>
-      <c r="L29" s="337">
+      <c r="K29" s="310"/>
+      <c r="L29" s="359">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="338"/>
+      <c r="M29" s="360"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="292" t="s">
+      <c r="D30" s="356" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="262"/>
-      <c r="F30" s="339">
+      <c r="E30" s="282"/>
+      <c r="F30" s="361">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="340"/>
+      <c r="G30" s="362"/>
       <c r="I30" s="197"/>
-      <c r="J30" s="292" t="s">
+      <c r="J30" s="356" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="262"/>
-      <c r="L30" s="339">
+      <c r="K30" s="282"/>
+      <c r="L30" s="361">
         <f>Pengeluaran!L30</f>
-        <v>836358</v>
-      </c>
-      <c r="M30" s="340"/>
+        <v>779000</v>
+      </c>
+      <c r="M30" s="362"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="297" t="s">
+      <c r="D31" s="304" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="262"/>
-      <c r="F31" s="341">
+      <c r="E31" s="282"/>
+      <c r="F31" s="366">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="342"/>
+      <c r="G31" s="367"/>
       <c r="I31" s="197"/>
-      <c r="J31" s="297" t="s">
+      <c r="J31" s="304" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="262"/>
-      <c r="L31" s="341">
+      <c r="K31" s="282"/>
+      <c r="L31" s="366">
         <f>L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="342"/>
+      <c r="M31" s="367"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="330" t="s">
+      <c r="D32" s="305" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="331"/>
-      <c r="F32" s="334">
+      <c r="E32" s="306"/>
+      <c r="F32" s="363">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="335"/>
+      <c r="G32" s="364"/>
       <c r="I32" s="197"/>
-      <c r="J32" s="330" t="s">
+      <c r="J32" s="305" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="331"/>
-      <c r="L32" s="334">
+      <c r="K32" s="306"/>
+      <c r="L32" s="363">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
-        <v>1511371.1800000002</v>
-      </c>
-      <c r="M32" s="335"/>
+        <v>1568729.1800000002</v>
+      </c>
+      <c r="M32" s="364"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15027,12 +15957,6 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C2:K3"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J29:K29"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="I5:M5"/>
@@ -15046,18 +15970,25 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J32:K32"/>
+    <mergeCell ref="C2:K3"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:M220"/>
   <sheetViews>
-    <sheetView topLeftCell="H4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15077,44 +16008,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="349" t="s">
+      <c r="C2" s="368" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="350"/>
-      <c r="E2" s="350"/>
-      <c r="F2" s="350"/>
-      <c r="G2" s="350"/>
-      <c r="H2" s="350"/>
-      <c r="I2" s="350"/>
-      <c r="J2" s="350"/>
-      <c r="K2" s="350"/>
+      <c r="D2" s="369"/>
+      <c r="E2" s="369"/>
+      <c r="F2" s="369"/>
+      <c r="G2" s="369"/>
+      <c r="H2" s="369"/>
+      <c r="I2" s="369"/>
+      <c r="J2" s="369"/>
+      <c r="K2" s="369"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="350"/>
-      <c r="D3" s="350"/>
-      <c r="E3" s="350"/>
-      <c r="F3" s="350"/>
-      <c r="G3" s="350"/>
-      <c r="H3" s="350"/>
-      <c r="I3" s="350"/>
-      <c r="J3" s="350"/>
-      <c r="K3" s="350"/>
+      <c r="C3" s="369"/>
+      <c r="D3" s="369"/>
+      <c r="E3" s="369"/>
+      <c r="F3" s="369"/>
+      <c r="G3" s="369"/>
+      <c r="H3" s="369"/>
+      <c r="I3" s="369"/>
+      <c r="J3" s="369"/>
+      <c r="K3" s="369"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="336" t="s">
+      <c r="C5" s="365" t="s">
         <v>248</v>
       </c>
-      <c r="D5" s="336"/>
-      <c r="E5" s="336"/>
-      <c r="F5" s="336"/>
-      <c r="G5" s="336"/>
-      <c r="I5" s="336" t="s">
+      <c r="D5" s="365"/>
+      <c r="E5" s="365"/>
+      <c r="F5" s="365"/>
+      <c r="G5" s="365"/>
+      <c r="I5" s="365" t="s">
         <v>249</v>
       </c>
-      <c r="J5" s="336"/>
-      <c r="K5" s="336"/>
-      <c r="L5" s="336"/>
-      <c r="M5" s="336"/>
+      <c r="J5" s="365"/>
+      <c r="K5" s="365"/>
+      <c r="L5" s="365"/>
+      <c r="M5" s="365"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -15314,7 +16245,7 @@
         <v>6</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K12" s="217" t="s">
         <v>291</v>
@@ -15335,14 +16266,14 @@
       <c r="I13" s="1">
         <v>7</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>293</v>
+      <c r="J13" s="229" t="s">
+        <v>311</v>
       </c>
       <c r="K13" s="228" t="s">
         <v>291</v>
       </c>
       <c r="L13" s="64">
-        <v>25000</v>
+        <v>10000</v>
       </c>
       <c r="M13" s="1"/>
     </row>
@@ -15355,16 +16286,16 @@
       <c r="I14" s="1">
         <v>8</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="23" t="s">
+        <v>293</v>
+      </c>
+      <c r="K14" s="232" t="s">
         <v>294</v>
       </c>
-      <c r="K14" s="217" t="s">
-        <v>295</v>
-      </c>
-      <c r="L14" s="64">
+      <c r="L14" s="67">
         <v>25000</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="M14" s="23" t="s">
         <v>292</v>
       </c>
     </row>
@@ -15376,20 +16307,20 @@
       <c r="E15" s="1"/>
       <c r="F15" s="56"/>
       <c r="G15" s="57"/>
-      <c r="I15" s="1">
+      <c r="I15" s="214">
         <v>9</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>296</v>
+      <c r="J15" s="229" t="s">
+        <v>295</v>
       </c>
       <c r="K15" s="228" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L15" s="64">
         <v>20000</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15400,19 +16331,13 @@
       <c r="E16" s="1"/>
       <c r="F16" s="56"/>
       <c r="G16" s="57"/>
-      <c r="I16" s="1">
+      <c r="I16" s="214">
         <v>10</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="K16" s="228" t="s">
-        <v>295</v>
-      </c>
-      <c r="L16" s="64">
-        <v>42358</v>
-      </c>
-      <c r="M16" s="1"/>
+      <c r="J16" s="163"/>
+      <c r="K16" s="234"/>
+      <c r="L16" s="235"/>
+      <c r="M16" s="163"/>
     </row>
     <row r="17" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="57">
@@ -15425,10 +16350,10 @@
       <c r="I17" s="1">
         <v>11</v>
       </c>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="1"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="233"/>
+      <c r="M17" s="10"/>
     </row>
     <row r="18" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="57">
@@ -15592,7 +16517,7 @@
       </c>
       <c r="L27" s="56">
         <f>SUM(L7:L26)</f>
-        <v>836358</v>
+        <v>779000</v>
       </c>
       <c r="M27" s="57"/>
     </row>
@@ -15604,88 +16529,88 @@
       <c r="M28" s="197"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="271" t="s">
+      <c r="D29" s="344" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="273"/>
-      <c r="F29" s="347">
+      <c r="E29" s="346"/>
+      <c r="F29" s="370">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="348"/>
+      <c r="G29" s="371"/>
       <c r="I29" s="197"/>
-      <c r="J29" s="271" t="s">
+      <c r="J29" s="344" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="273"/>
-      <c r="L29" s="347">
+      <c r="K29" s="346"/>
+      <c r="L29" s="370">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="348"/>
+      <c r="M29" s="371"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="297" t="s">
+      <c r="D30" s="304" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="262"/>
-      <c r="F30" s="339">
+      <c r="E30" s="282"/>
+      <c r="F30" s="361">
         <f>F27</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="340"/>
+      <c r="G30" s="362"/>
       <c r="I30" s="197"/>
-      <c r="J30" s="297" t="s">
+      <c r="J30" s="304" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="262"/>
-      <c r="L30" s="339">
+      <c r="K30" s="282"/>
+      <c r="L30" s="361">
         <f>L27</f>
-        <v>836358</v>
-      </c>
-      <c r="M30" s="340"/>
+        <v>779000</v>
+      </c>
+      <c r="M30" s="362"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="297" t="s">
+      <c r="D31" s="304" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="262"/>
-      <c r="F31" s="341">
+      <c r="E31" s="282"/>
+      <c r="F31" s="366">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="342"/>
+      <c r="G31" s="367"/>
       <c r="I31" s="197"/>
-      <c r="J31" s="297" t="s">
+      <c r="J31" s="304" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="262"/>
-      <c r="L31" s="341">
+      <c r="K31" s="282"/>
+      <c r="L31" s="366">
         <f>Pemasukkan!L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="342"/>
+      <c r="M31" s="367"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="330" t="s">
+      <c r="D32" s="305" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="331"/>
-      <c r="F32" s="345">
+      <c r="E32" s="306"/>
+      <c r="F32" s="372">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="346"/>
+      <c r="G32" s="373"/>
       <c r="I32" s="197"/>
-      <c r="J32" s="330" t="s">
+      <c r="J32" s="305" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="331"/>
-      <c r="L32" s="345">
+      <c r="K32" s="306"/>
+      <c r="L32" s="372">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
-        <v>1511371.1800000002</v>
-      </c>
-      <c r="M32" s="346"/>
+        <v>1568729.1800000002</v>
+      </c>
+      <c r="M32" s="373"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15877,6 +16802,14 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
     <mergeCell ref="C2:K3"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
@@ -15888,21 +16821,14 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:K32"/>
   <sheetViews>
@@ -15920,28 +16846,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="353" t="s">
+      <c r="C2" s="387" t="s">
         <v>232</v>
       </c>
-      <c r="D2" s="354"/>
-      <c r="E2" s="354"/>
-      <c r="F2" s="354"/>
-      <c r="G2" s="354"/>
-      <c r="H2" s="354"/>
-      <c r="I2" s="354"/>
-      <c r="J2" s="354"/>
-      <c r="K2" s="354"/>
+      <c r="D2" s="388"/>
+      <c r="E2" s="388"/>
+      <c r="F2" s="388"/>
+      <c r="G2" s="388"/>
+      <c r="H2" s="388"/>
+      <c r="I2" s="388"/>
+      <c r="J2" s="388"/>
+      <c r="K2" s="388"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="354"/>
-      <c r="D3" s="354"/>
-      <c r="E3" s="354"/>
-      <c r="F3" s="354"/>
-      <c r="G3" s="354"/>
-      <c r="H3" s="354"/>
-      <c r="I3" s="354"/>
-      <c r="J3" s="354"/>
-      <c r="K3" s="354"/>
+      <c r="C3" s="388"/>
+      <c r="D3" s="388"/>
+      <c r="E3" s="388"/>
+      <c r="F3" s="388"/>
+      <c r="G3" s="388"/>
+      <c r="H3" s="388"/>
+      <c r="I3" s="388"/>
+      <c r="J3" s="388"/>
+      <c r="K3" s="388"/>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="156"/>
@@ -16291,10 +17217,10 @@
     </row>
     <row r="29" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="156"/>
-      <c r="D29" s="355"/>
-      <c r="E29" s="355"/>
-      <c r="F29" s="356"/>
-      <c r="G29" s="356"/>
+      <c r="D29" s="389"/>
+      <c r="E29" s="389"/>
+      <c r="F29" s="390"/>
+      <c r="G29" s="390"/>
       <c r="H29" s="156"/>
       <c r="I29" s="156"/>
       <c r="J29" s="156"/>
@@ -16302,15 +17228,15 @@
     </row>
     <row r="30" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="24"/>
-      <c r="D30" s="357" t="s">
+      <c r="D30" s="391" t="s">
         <v>231</v>
       </c>
-      <c r="E30" s="358"/>
-      <c r="F30" s="359">
+      <c r="E30" s="392"/>
+      <c r="F30" s="393">
         <f>F27</f>
         <v>220000</v>
       </c>
-      <c r="G30" s="360"/>
+      <c r="G30" s="394"/>
       <c r="H30" s="156"/>
       <c r="I30" s="156"/>
       <c r="J30" s="156"/>
@@ -16325,10 +17251,10 @@
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="156"/>
-      <c r="D32" s="351"/>
-      <c r="E32" s="351"/>
-      <c r="F32" s="352"/>
-      <c r="G32" s="351"/>
+      <c r="D32" s="385"/>
+      <c r="E32" s="385"/>
+      <c r="F32" s="386"/>
+      <c r="G32" s="385"/>
       <c r="H32" s="156"/>
       <c r="I32" s="156"/>
       <c r="J32" s="156"/>
@@ -16350,7 +17276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -16366,17 +17292,17 @@
     <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="361" t="s">
+      <c r="C4" s="395" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="362"/>
+      <c r="D4" s="396"/>
       <c r="E4" s="27"/>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
-      <c r="H4" s="361" t="s">
+      <c r="H4" s="395" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="362"/>
+      <c r="I4" s="396"/>
       <c r="J4" s="35"/>
       <c r="K4" s="27"/>
     </row>
@@ -16503,17 +17429,17 @@
     <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26"/>
-      <c r="C17" s="361" t="s">
+      <c r="C17" s="395" t="s">
         <v>144</v>
       </c>
-      <c r="D17" s="362"/>
+      <c r="D17" s="396"/>
       <c r="E17" s="27"/>
       <c r="F17" s="26"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="361" t="s">
+      <c r="H17" s="395" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="362"/>
+      <c r="I17" s="396"/>
       <c r="J17" s="35"/>
       <c r="K17" s="27"/>
     </row>
@@ -16650,12 +17576,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16667,28 +17593,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="364" t="s">
+      <c r="B2" s="398" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="365"/>
-      <c r="D2" s="365"/>
-      <c r="E2" s="365"/>
-      <c r="F2" s="365"/>
-      <c r="G2" s="365"/>
-      <c r="H2" s="365"/>
-      <c r="I2" s="365"/>
-      <c r="J2" s="365"/>
+      <c r="C2" s="399"/>
+      <c r="D2" s="399"/>
+      <c r="E2" s="399"/>
+      <c r="F2" s="399"/>
+      <c r="G2" s="399"/>
+      <c r="H2" s="399"/>
+      <c r="I2" s="399"/>
+      <c r="J2" s="399"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="365"/>
-      <c r="C3" s="365"/>
-      <c r="D3" s="365"/>
-      <c r="E3" s="365"/>
-      <c r="F3" s="365"/>
-      <c r="G3" s="365"/>
-      <c r="H3" s="365"/>
-      <c r="I3" s="365"/>
-      <c r="J3" s="365"/>
+      <c r="B3" s="399"/>
+      <c r="C3" s="399"/>
+      <c r="D3" s="399"/>
+      <c r="E3" s="399"/>
+      <c r="F3" s="399"/>
+      <c r="G3" s="399"/>
+      <c r="H3" s="399"/>
+      <c r="I3" s="399"/>
+      <c r="J3" s="399"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -16709,10 +17635,10 @@
       <c r="G6" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="H6" s="280" t="s">
+      <c r="H6" s="313" t="s">
         <v>284</v>
       </c>
-      <c r="I6" s="262"/>
+      <c r="I6" s="282"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -16734,11 +17660,11 @@
       <c r="G7" s="220">
         <v>205000</v>
       </c>
-      <c r="H7" s="366">
+      <c r="H7" s="400">
         <f>F7-G7</f>
         <v>380000</v>
       </c>
-      <c r="I7" s="262"/>
+      <c r="I7" s="282"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="221"/>
@@ -16747,8 +17673,8 @@
       <c r="E8" s="222"/>
       <c r="F8" s="222"/>
       <c r="G8" s="222"/>
-      <c r="H8" s="363"/>
-      <c r="I8" s="363"/>
+      <c r="H8" s="397"/>
+      <c r="I8" s="397"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="221"/>
@@ -16759,11 +17685,11 @@
       <c r="G9" s="223" t="s">
         <v>285</v>
       </c>
-      <c r="H9" s="367">
+      <c r="H9" s="401">
         <f>H7</f>
         <v>380000</v>
       </c>
-      <c r="I9" s="368"/>
+      <c r="I9" s="402"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="221"/>
@@ -16772,8 +17698,8 @@
       <c r="E10" s="222"/>
       <c r="F10" s="222"/>
       <c r="G10" s="222"/>
-      <c r="H10" s="363"/>
-      <c r="I10" s="363"/>
+      <c r="H10" s="397"/>
+      <c r="I10" s="397"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="221"/>
@@ -16782,8 +17708,8 @@
       <c r="E11" s="222"/>
       <c r="F11" s="222"/>
       <c r="G11" s="222"/>
-      <c r="H11" s="363"/>
-      <c r="I11" s="363"/>
+      <c r="H11" s="397"/>
+      <c r="I11" s="397"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="221"/>
@@ -16792,8 +17718,8 @@
       <c r="E12" s="222"/>
       <c r="F12" s="222"/>
       <c r="G12" s="222"/>
-      <c r="H12" s="363"/>
-      <c r="I12" s="363"/>
+      <c r="H12" s="397"/>
+      <c r="I12" s="397"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="221"/>
@@ -16802,8 +17728,8 @@
       <c r="E13" s="222"/>
       <c r="F13" s="222"/>
       <c r="G13" s="222"/>
-      <c r="H13" s="363"/>
-      <c r="I13" s="363"/>
+      <c r="H13" s="397"/>
+      <c r="I13" s="397"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="221"/>
@@ -16812,8 +17738,8 @@
       <c r="E14" s="222"/>
       <c r="F14" s="222"/>
       <c r="G14" s="222"/>
-      <c r="H14" s="363"/>
-      <c r="I14" s="363"/>
+      <c r="H14" s="397"/>
+      <c r="I14" s="397"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="221"/>
@@ -16822,8 +17748,8 @@
       <c r="E15" s="222"/>
       <c r="F15" s="222"/>
       <c r="G15" s="222"/>
-      <c r="H15" s="363"/>
-      <c r="I15" s="363"/>
+      <c r="H15" s="397"/>
+      <c r="I15" s="397"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="221"/>
@@ -16832,8 +17758,8 @@
       <c r="E16" s="222"/>
       <c r="F16" s="222"/>
       <c r="G16" s="222"/>
-      <c r="H16" s="363"/>
-      <c r="I16" s="363"/>
+      <c r="H16" s="397"/>
+      <c r="I16" s="397"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="221"/>
@@ -16842,16 +17768,11 @@
       <c r="E17" s="222"/>
       <c r="F17" s="222"/>
       <c r="G17" s="222"/>
-      <c r="H17" s="363"/>
-      <c r="I17" s="363"/>
+      <c r="H17" s="397"/>
+      <c r="I17" s="397"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="H6:I6"/>
@@ -16860,6 +17781,11 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Irvan KAS, Fadly KAS, Mada KAS, Joshua KAS, Daniel KAS, Fatah KAS,Alfi KAS
KAS Mada:
180.000 (tagihan kas)
5.000 (Kas yang dibayarkan)
------------- -
175.000 (sisa tagihan kas)

KAS Joshua:
100.000 (tagihan kas)
5.000 (Kas yang dibayarkan)
------------- -
95.000 (sisa tagihan kas)

KAS Daniel :

240.000 (tagihan kas)
5.000 (Kas yang dibayarkan)
------------- -
235.000 (sisa tagihan kas)

KAS Alfi:

255.000 (tagihan kas)
20.000 (Kas yang dibayarkan)
------------- -
235.000 (sisa tagihan kas)

KAS Fadly :

100.000 (tagihan kas)
100.000 (Kas yang dibayarkan)
------------- -
0 (sisa tagihan kas)

KAS Irvan :

80.000 (tagihan kas)
80.000 (Kas yang dibayarkan)
------------- -
0 (sisa tagihan kas)

KAS Fatah :

290.000 (tagihan kas)
290.000 (Kas yang dibayarkan)
------------- -
0 (sisa tagihan kas)
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="346">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -1021,6 +1021,45 @@
   </si>
   <si>
     <t>Kekurangan 2018 + 2019-Desember</t>
+  </si>
+  <si>
+    <t>16 Desember 2019</t>
+  </si>
+  <si>
+    <t>Irvan KAS (trf)</t>
+  </si>
+  <si>
+    <t>Fadly KAS (trf)</t>
+  </si>
+  <si>
+    <t>Fatah KAS (tunai)</t>
+  </si>
+  <si>
+    <t>Alfi KAS (tunai)</t>
+  </si>
+  <si>
+    <t>simpanan 5k</t>
+  </si>
+  <si>
+    <t>Irvan KAS (simpanan)</t>
+  </si>
+  <si>
+    <t>Fadly KAS (simpanan)</t>
+  </si>
+  <si>
+    <t>Mada  KAS(tunai)</t>
+  </si>
+  <si>
+    <t>Joshua KAS(tunai)</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Daniel KAS (tunai)</t>
+  </si>
+  <si>
+    <t>josh</t>
   </si>
 </sst>
 </file>
@@ -2228,7 +2267,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="410">
+  <cellXfs count="427">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2781,14 +2820,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3217,16 +3257,216 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="14" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="14" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B050"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B050"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B050"/>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -4363,126 +4603,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="265" t="s">
+      <c r="A1" s="266" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="266"/>
-      <c r="C1" s="266"/>
-      <c r="D1" s="266"/>
-      <c r="E1" s="266"/>
-      <c r="F1" s="266"/>
-      <c r="G1" s="266"/>
-      <c r="H1" s="266"/>
-      <c r="I1" s="266"/>
-      <c r="J1" s="266"/>
-      <c r="K1" s="266"/>
-      <c r="L1" s="266"/>
-      <c r="M1" s="266"/>
-      <c r="N1" s="266"/>
-      <c r="O1" s="266"/>
-      <c r="P1" s="266"/>
-      <c r="Q1" s="266"/>
-      <c r="R1" s="266"/>
+      <c r="B1" s="267"/>
+      <c r="C1" s="267"/>
+      <c r="D1" s="267"/>
+      <c r="E1" s="267"/>
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="267"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="267"/>
+      <c r="O1" s="267"/>
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="267"/>
-      <c r="B2" s="268"/>
-      <c r="C2" s="268"/>
-      <c r="D2" s="268"/>
-      <c r="E2" s="268"/>
-      <c r="F2" s="268"/>
-      <c r="G2" s="268"/>
-      <c r="H2" s="268"/>
-      <c r="I2" s="268"/>
-      <c r="J2" s="268"/>
-      <c r="K2" s="268"/>
-      <c r="L2" s="268"/>
-      <c r="M2" s="268"/>
-      <c r="N2" s="268"/>
-      <c r="O2" s="268"/>
-      <c r="P2" s="268"/>
-      <c r="Q2" s="268"/>
-      <c r="R2" s="268"/>
+      <c r="A2" s="268"/>
+      <c r="B2" s="269"/>
+      <c r="C2" s="269"/>
+      <c r="D2" s="269"/>
+      <c r="E2" s="269"/>
+      <c r="F2" s="269"/>
+      <c r="G2" s="269"/>
+      <c r="H2" s="269"/>
+      <c r="I2" s="269"/>
+      <c r="J2" s="269"/>
+      <c r="K2" s="269"/>
+      <c r="L2" s="269"/>
+      <c r="M2" s="269"/>
+      <c r="N2" s="269"/>
+      <c r="O2" s="269"/>
+      <c r="P2" s="269"/>
+      <c r="Q2" s="269"/>
+      <c r="R2" s="269"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="267"/>
-      <c r="B3" s="268"/>
-      <c r="C3" s="268"/>
-      <c r="D3" s="268"/>
-      <c r="E3" s="268"/>
-      <c r="F3" s="268"/>
-      <c r="G3" s="268"/>
-      <c r="H3" s="268"/>
-      <c r="I3" s="268"/>
-      <c r="J3" s="268"/>
-      <c r="K3" s="268"/>
-      <c r="L3" s="268"/>
-      <c r="M3" s="268"/>
-      <c r="N3" s="268"/>
-      <c r="O3" s="268"/>
-      <c r="P3" s="268"/>
-      <c r="Q3" s="268"/>
-      <c r="R3" s="268"/>
+      <c r="A3" s="268"/>
+      <c r="B3" s="269"/>
+      <c r="C3" s="269"/>
+      <c r="D3" s="269"/>
+      <c r="E3" s="269"/>
+      <c r="F3" s="269"/>
+      <c r="G3" s="269"/>
+      <c r="H3" s="269"/>
+      <c r="I3" s="269"/>
+      <c r="J3" s="269"/>
+      <c r="K3" s="269"/>
+      <c r="L3" s="269"/>
+      <c r="M3" s="269"/>
+      <c r="N3" s="269"/>
+      <c r="O3" s="269"/>
+      <c r="P3" s="269"/>
+      <c r="Q3" s="269"/>
+      <c r="R3" s="269"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="267"/>
-      <c r="B4" s="268"/>
-      <c r="C4" s="268"/>
-      <c r="D4" s="268"/>
-      <c r="E4" s="268"/>
-      <c r="F4" s="268"/>
-      <c r="G4" s="268"/>
-      <c r="H4" s="268"/>
-      <c r="I4" s="268"/>
-      <c r="J4" s="268"/>
-      <c r="K4" s="268"/>
-      <c r="L4" s="268"/>
-      <c r="M4" s="268"/>
-      <c r="N4" s="268"/>
-      <c r="O4" s="268"/>
-      <c r="P4" s="268"/>
-      <c r="Q4" s="268"/>
-      <c r="R4" s="268"/>
+      <c r="A4" s="268"/>
+      <c r="B4" s="269"/>
+      <c r="C4" s="269"/>
+      <c r="D4" s="269"/>
+      <c r="E4" s="269"/>
+      <c r="F4" s="269"/>
+      <c r="G4" s="269"/>
+      <c r="H4" s="269"/>
+      <c r="I4" s="269"/>
+      <c r="J4" s="269"/>
+      <c r="K4" s="269"/>
+      <c r="L4" s="269"/>
+      <c r="M4" s="269"/>
+      <c r="N4" s="269"/>
+      <c r="O4" s="269"/>
+      <c r="P4" s="269"/>
+      <c r="Q4" s="269"/>
+      <c r="R4" s="269"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="267"/>
-      <c r="B5" s="268"/>
-      <c r="C5" s="268"/>
-      <c r="D5" s="268"/>
-      <c r="E5" s="268"/>
-      <c r="F5" s="268"/>
-      <c r="G5" s="268"/>
-      <c r="H5" s="268"/>
-      <c r="I5" s="268"/>
-      <c r="J5" s="268"/>
-      <c r="K5" s="268"/>
-      <c r="L5" s="268"/>
-      <c r="M5" s="268"/>
-      <c r="N5" s="268"/>
-      <c r="O5" s="268"/>
-      <c r="P5" s="268"/>
-      <c r="Q5" s="268"/>
-      <c r="R5" s="268"/>
+      <c r="A5" s="268"/>
+      <c r="B5" s="269"/>
+      <c r="C5" s="269"/>
+      <c r="D5" s="269"/>
+      <c r="E5" s="269"/>
+      <c r="F5" s="269"/>
+      <c r="G5" s="269"/>
+      <c r="H5" s="269"/>
+      <c r="I5" s="269"/>
+      <c r="J5" s="269"/>
+      <c r="K5" s="269"/>
+      <c r="L5" s="269"/>
+      <c r="M5" s="269"/>
+      <c r="N5" s="269"/>
+      <c r="O5" s="269"/>
+      <c r="P5" s="269"/>
+      <c r="Q5" s="269"/>
+      <c r="R5" s="269"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="267"/>
-      <c r="B6" s="268"/>
-      <c r="C6" s="268"/>
-      <c r="D6" s="268"/>
-      <c r="E6" s="268"/>
-      <c r="F6" s="268"/>
-      <c r="G6" s="268"/>
-      <c r="H6" s="268"/>
-      <c r="I6" s="268"/>
-      <c r="J6" s="268"/>
-      <c r="K6" s="268"/>
-      <c r="L6" s="268"/>
-      <c r="M6" s="268"/>
-      <c r="N6" s="268"/>
-      <c r="O6" s="268"/>
-      <c r="P6" s="268"/>
-      <c r="Q6" s="268"/>
-      <c r="R6" s="268"/>
+      <c r="A6" s="268"/>
+      <c r="B6" s="269"/>
+      <c r="C6" s="269"/>
+      <c r="D6" s="269"/>
+      <c r="E6" s="269"/>
+      <c r="F6" s="269"/>
+      <c r="G6" s="269"/>
+      <c r="H6" s="269"/>
+      <c r="I6" s="269"/>
+      <c r="J6" s="269"/>
+      <c r="K6" s="269"/>
+      <c r="L6" s="269"/>
+      <c r="M6" s="269"/>
+      <c r="N6" s="269"/>
+      <c r="O6" s="269"/>
+      <c r="P6" s="269"/>
+      <c r="Q6" s="269"/>
+      <c r="R6" s="269"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -7427,58 +7667,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="270" t="s">
+      <c r="J79" s="271" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="271"/>
-      <c r="L79" s="271"/>
-      <c r="M79" s="271"/>
-      <c r="N79" s="272"/>
-      <c r="P79" s="278" t="s">
+      <c r="K79" s="272"/>
+      <c r="L79" s="272"/>
+      <c r="M79" s="272"/>
+      <c r="N79" s="273"/>
+      <c r="P79" s="279" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="271"/>
-      <c r="R79" s="271"/>
-      <c r="S79" s="272"/>
+      <c r="Q79" s="272"/>
+      <c r="R79" s="272"/>
+      <c r="S79" s="273"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="273" t="s">
+      <c r="J80" s="274" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="268"/>
-      <c r="L80" s="268"/>
-      <c r="M80" s="268"/>
-      <c r="N80" s="274"/>
-      <c r="P80" s="273" t="s">
+      <c r="K80" s="269"/>
+      <c r="L80" s="269"/>
+      <c r="M80" s="269"/>
+      <c r="N80" s="275"/>
+      <c r="P80" s="274" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="268"/>
-      <c r="R80" s="268"/>
-      <c r="S80" s="274"/>
+      <c r="Q80" s="269"/>
+      <c r="R80" s="269"/>
+      <c r="S80" s="275"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="275"/>
-      <c r="K81" s="276"/>
-      <c r="L81" s="276"/>
-      <c r="M81" s="276"/>
-      <c r="N81" s="277"/>
-      <c r="P81" s="275"/>
-      <c r="Q81" s="276"/>
-      <c r="R81" s="276"/>
-      <c r="S81" s="277"/>
+      <c r="J81" s="276"/>
+      <c r="K81" s="277"/>
+      <c r="L81" s="277"/>
+      <c r="M81" s="277"/>
+      <c r="N81" s="278"/>
+      <c r="P81" s="276"/>
+      <c r="Q81" s="277"/>
+      <c r="R81" s="277"/>
+      <c r="S81" s="278"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="269" t="s">
+      <c r="J82" s="270" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="260"/>
-      <c r="L82" s="261"/>
-      <c r="M82" s="269" t="s">
+      <c r="K82" s="261"/>
+      <c r="L82" s="262"/>
+      <c r="M82" s="270" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="261"/>
-      <c r="P82" s="269"/>
-      <c r="Q82" s="261"/>
+      <c r="N82" s="262"/>
+      <c r="P82" s="270"/>
+      <c r="Q82" s="262"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -7487,38 +7727,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="259" t="s">
+      <c r="J83" s="260" t="s">
         <v>70</v>
       </c>
-      <c r="K83" s="260"/>
-      <c r="L83" s="261"/>
-      <c r="M83" s="262">
+      <c r="K83" s="261"/>
+      <c r="L83" s="262"/>
+      <c r="M83" s="263">
         <v>7350000</v>
       </c>
-      <c r="N83" s="261"/>
-      <c r="P83" s="263" t="s">
+      <c r="N83" s="262"/>
+      <c r="P83" s="264" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="261"/>
+      <c r="Q83" s="262"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="259" t="s">
+      <c r="J84" s="260" t="s">
         <v>72</v>
       </c>
-      <c r="K84" s="260"/>
-      <c r="L84" s="261"/>
-      <c r="M84" s="264">
+      <c r="K84" s="261"/>
+      <c r="L84" s="262"/>
+      <c r="M84" s="265">
         <v>1100000</v>
       </c>
-      <c r="N84" s="261"/>
-      <c r="P84" s="263" t="s">
+      <c r="N84" s="262"/>
+      <c r="P84" s="264" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="261"/>
+      <c r="Q84" s="262"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -7527,39 +7767,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="259" t="s">
+      <c r="J85" s="260" t="s">
         <v>75</v>
       </c>
-      <c r="K85" s="260"/>
-      <c r="L85" s="261"/>
-      <c r="M85" s="262">
+      <c r="K85" s="261"/>
+      <c r="L85" s="262"/>
+      <c r="M85" s="263">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="261"/>
-      <c r="P85" s="263" t="s">
+      <c r="N85" s="262"/>
+      <c r="P85" s="264" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="261"/>
+      <c r="Q85" s="262"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="259" t="s">
+      <c r="J86" s="260" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="260"/>
-      <c r="L86" s="261"/>
-      <c r="M86" s="262">
+      <c r="K86" s="261"/>
+      <c r="L86" s="262"/>
+      <c r="M86" s="263">
         <v>8411850</v>
       </c>
-      <c r="N86" s="261"/>
-      <c r="P86" s="263" t="s">
+      <c r="N86" s="262"/>
+      <c r="P86" s="264" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="261"/>
+      <c r="Q86" s="262"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -7567,20 +7807,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="259" t="s">
+      <c r="J87" s="260" t="s">
         <v>79</v>
       </c>
-      <c r="K87" s="260"/>
-      <c r="L87" s="261"/>
-      <c r="M87" s="262">
+      <c r="K87" s="261"/>
+      <c r="L87" s="262"/>
+      <c r="M87" s="263">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="261"/>
-      <c r="P87" s="263" t="s">
+      <c r="N87" s="262"/>
+      <c r="P87" s="264" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="261"/>
+      <c r="Q87" s="262"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -7794,25 +8034,25 @@
     <mergeCell ref="P86:Q86"/>
   </mergeCells>
   <conditionalFormatting sqref="T10:T52">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S52">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S51">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
       <formula>$S$12=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7823,10 +8063,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BM260"/>
+  <dimension ref="A2:BM266"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="A29" colorId="8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" defaultGridColor="0" colorId="8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7868,53 +8108,55 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="287" t="s">
+      <c r="C2" s="288" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="266"/>
-      <c r="E2" s="266"/>
-      <c r="F2" s="266"/>
-      <c r="G2" s="266"/>
-      <c r="H2" s="266"/>
-      <c r="I2" s="266"/>
-      <c r="J2" s="266"/>
-      <c r="K2" s="266"/>
-      <c r="L2" s="266"/>
-      <c r="M2" s="266"/>
-      <c r="N2" s="266"/>
-      <c r="O2" s="266"/>
-      <c r="P2" s="267"/>
-      <c r="Q2" s="267"/>
-      <c r="R2" s="267"/>
-      <c r="S2" s="266"/>
-      <c r="T2" s="266"/>
+      <c r="D2" s="267"/>
+      <c r="E2" s="267"/>
+      <c r="F2" s="267"/>
+      <c r="G2" s="267"/>
+      <c r="H2" s="267"/>
+      <c r="I2" s="267"/>
+      <c r="J2" s="267"/>
+      <c r="K2" s="267"/>
+      <c r="L2" s="267"/>
+      <c r="M2" s="267"/>
+      <c r="N2" s="267"/>
+      <c r="O2" s="267"/>
+      <c r="P2" s="268"/>
+      <c r="Q2" s="268"/>
+      <c r="R2" s="268"/>
+      <c r="S2" s="267"/>
+      <c r="T2" s="267"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="267"/>
-      <c r="D3" s="268"/>
-      <c r="E3" s="268"/>
-      <c r="F3" s="268"/>
-      <c r="G3" s="268"/>
-      <c r="H3" s="268"/>
-      <c r="I3" s="268"/>
-      <c r="J3" s="268"/>
-      <c r="K3" s="268"/>
-      <c r="L3" s="268"/>
-      <c r="M3" s="268"/>
-      <c r="N3" s="268"/>
-      <c r="O3" s="268"/>
-      <c r="P3" s="268"/>
-      <c r="Q3" s="268"/>
-      <c r="R3" s="268"/>
-      <c r="S3" s="268"/>
-      <c r="T3" s="268"/>
+      <c r="C3" s="268"/>
+      <c r="D3" s="269"/>
+      <c r="E3" s="269"/>
+      <c r="F3" s="269"/>
+      <c r="G3" s="269"/>
+      <c r="H3" s="269"/>
+      <c r="I3" s="269"/>
+      <c r="J3" s="269"/>
+      <c r="K3" s="269"/>
+      <c r="L3" s="269"/>
+      <c r="M3" s="269"/>
+      <c r="N3" s="269"/>
+      <c r="O3" s="269"/>
+      <c r="P3" s="269"/>
+      <c r="Q3" s="269"/>
+      <c r="R3" s="269"/>
+      <c r="S3" s="269"/>
+      <c r="T3" s="269"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="71"/>
+      <c r="B4" s="71" t="s">
+        <v>345</v>
+      </c>
       <c r="Q4" s="133"/>
       <c r="R4" s="133"/>
       <c r="Y4" s="8" t="s">
@@ -7992,25 +8234,25 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="293" t="s">
+      <c r="X5" s="294" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="260"/>
-      <c r="Z5" s="260"/>
-      <c r="AA5" s="260"/>
-      <c r="AB5" s="260"/>
-      <c r="AC5" s="260"/>
-      <c r="AD5" s="260"/>
-      <c r="AE5" s="260"/>
-      <c r="AF5" s="260"/>
-      <c r="AG5" s="260"/>
-      <c r="AH5" s="260"/>
-      <c r="AI5" s="260"/>
-      <c r="AJ5" s="260"/>
-      <c r="AK5" s="260"/>
-      <c r="AL5" s="260"/>
-      <c r="AM5" s="260"/>
-      <c r="AN5" s="261"/>
+      <c r="Y5" s="261"/>
+      <c r="Z5" s="261"/>
+      <c r="AA5" s="261"/>
+      <c r="AB5" s="261"/>
+      <c r="AC5" s="261"/>
+      <c r="AD5" s="261"/>
+      <c r="AE5" s="261"/>
+      <c r="AF5" s="261"/>
+      <c r="AG5" s="261"/>
+      <c r="AH5" s="261"/>
+      <c r="AI5" s="261"/>
+      <c r="AJ5" s="261"/>
+      <c r="AK5" s="261"/>
+      <c r="AL5" s="261"/>
+      <c r="AM5" s="261"/>
+      <c r="AN5" s="262"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -8043,61 +8285,71 @@
       <c r="J6" s="72">
         <v>20</v>
       </c>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="72"/>
+      <c r="K6" s="72">
+        <v>20</v>
+      </c>
+      <c r="L6" s="72">
+        <v>20</v>
+      </c>
+      <c r="M6" s="72">
+        <v>20</v>
+      </c>
+      <c r="N6" s="72">
+        <v>20</v>
+      </c>
       <c r="O6" s="13">
         <f t="shared" ref="O6:O37" si="0">SUM(C6:N6)</f>
-        <v>160</v>
+        <v>240</v>
       </c>
       <c r="P6" s="130">
         <v>0</v>
       </c>
       <c r="Q6" s="131">
         <f>(240-SUM(C6:N6))</f>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="R6" s="132">
         <f>Q6+P6</f>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="S6" s="13">
         <f t="shared" ref="S6:S37" si="1">(240)-(O6)</f>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="T6" s="14">
-        <f t="shared" ref="T6:T60" si="2">S6-60</f>
-        <v>20</v>
+        <f t="shared" ref="T6:T61" si="2">S6-60</f>
+        <v>-60</v>
       </c>
       <c r="U6" s="15" t="str">
-        <f t="shared" ref="U6:U60" si="3">IF(T6&lt;=0,"OK","NO")</f>
-        <v>NO</v>
-      </c>
-      <c r="V6" s="13"/>
-      <c r="X6" s="288" t="s">
+        <f t="shared" ref="U6:U61" si="3">IF(T6&lt;=0,"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="V6" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="X6" s="289" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="288" t="s">
+      <c r="Y6" s="289" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="292" t="s">
+      <c r="Z6" s="293" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="289"/>
-      <c r="AB6" s="289"/>
-      <c r="AC6" s="289"/>
-      <c r="AD6" s="289"/>
-      <c r="AE6" s="289"/>
-      <c r="AF6" s="289"/>
-      <c r="AG6" s="289"/>
-      <c r="AH6" s="289"/>
-      <c r="AI6" s="289"/>
-      <c r="AJ6" s="289"/>
-      <c r="AK6" s="289"/>
-      <c r="AL6" s="289"/>
-      <c r="AM6" s="289"/>
-      <c r="AN6" s="289"/>
+      <c r="AA6" s="290"/>
+      <c r="AB6" s="290"/>
+      <c r="AC6" s="290"/>
+      <c r="AD6" s="290"/>
+      <c r="AE6" s="290"/>
+      <c r="AF6" s="290"/>
+      <c r="AG6" s="290"/>
+      <c r="AH6" s="290"/>
+      <c r="AI6" s="290"/>
+      <c r="AJ6" s="290"/>
+      <c r="AK6" s="290"/>
+      <c r="AL6" s="290"/>
+      <c r="AM6" s="290"/>
+      <c r="AN6" s="290"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -8127,60 +8379,72 @@
       <c r="I7" s="73">
         <v>20</v>
       </c>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="72"/>
+      <c r="J7" s="72">
+        <v>20</v>
+      </c>
+      <c r="K7" s="72">
+        <v>20</v>
+      </c>
+      <c r="L7" s="72">
+        <v>20</v>
+      </c>
+      <c r="M7" s="72">
+        <v>20</v>
+      </c>
+      <c r="N7" s="72">
+        <v>20</v>
+      </c>
       <c r="O7" s="13">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>240</v>
       </c>
       <c r="P7" s="130">
         <v>0</v>
       </c>
       <c r="Q7" s="131">
-        <f t="shared" ref="Q7:Q60" si="4">(240-SUM(C7:N7))</f>
-        <v>100</v>
+        <f t="shared" ref="Q7:Q61" si="4">(240-SUM(C7:N7))</f>
+        <v>0</v>
       </c>
       <c r="R7" s="132">
-        <f t="shared" ref="R7:R60" si="5">Q7+P7</f>
-        <v>100</v>
+        <f t="shared" ref="R7:R61" si="5">Q7+P7</f>
+        <v>0</v>
       </c>
       <c r="S7" s="13">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="T7" s="14">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>-60</v>
       </c>
       <c r="U7" s="15" t="str">
         <f t="shared" si="3"/>
-        <v>NO</v>
-      </c>
-      <c r="V7" s="13"/>
-      <c r="X7" s="289"/>
-      <c r="Y7" s="289"/>
-      <c r="Z7" s="292" t="s">
+        <v>OK</v>
+      </c>
+      <c r="V7" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="X7" s="290"/>
+      <c r="Y7" s="290"/>
+      <c r="Z7" s="293" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="289"/>
-      <c r="AB7" s="289"/>
-      <c r="AC7" s="289"/>
-      <c r="AD7" s="292" t="s">
+      <c r="AA7" s="290"/>
+      <c r="AB7" s="290"/>
+      <c r="AC7" s="290"/>
+      <c r="AD7" s="293" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="289"/>
-      <c r="AF7" s="289"/>
-      <c r="AG7" s="289"/>
-      <c r="AH7" s="289"/>
-      <c r="AI7" s="289"/>
-      <c r="AJ7" s="289"/>
-      <c r="AK7" s="289"/>
-      <c r="AL7" s="289"/>
-      <c r="AM7" s="289"/>
-      <c r="AN7" s="289"/>
+      <c r="AE7" s="290"/>
+      <c r="AF7" s="290"/>
+      <c r="AG7" s="290"/>
+      <c r="AH7" s="290"/>
+      <c r="AI7" s="290"/>
+      <c r="AJ7" s="290"/>
+      <c r="AK7" s="290"/>
+      <c r="AL7" s="290"/>
+      <c r="AM7" s="290"/>
+      <c r="AN7" s="290"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -8230,8 +8494,8 @@
         <v>NO</v>
       </c>
       <c r="V8" s="13"/>
-      <c r="X8" s="289"/>
-      <c r="Y8" s="289"/>
+      <c r="X8" s="290"/>
+      <c r="Y8" s="290"/>
       <c r="Z8" s="153" t="s">
         <v>19</v>
       </c>
@@ -8306,14 +8570,16 @@
       <c r="I9" s="73">
         <v>20</v>
       </c>
-      <c r="J9" s="72"/>
+      <c r="J9" s="72">
+        <v>5</v>
+      </c>
       <c r="K9" s="72"/>
       <c r="L9" s="72"/>
       <c r="M9" s="72"/>
       <c r="N9" s="72"/>
       <c r="O9" s="13">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="P9" s="130">
         <f>'2018(NOT UPDATED)'!S13</f>
@@ -8321,19 +8587,19 @@
       </c>
       <c r="Q9" s="131">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R9" s="132">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S9" s="13">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="T9" s="14">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="U9" s="15" t="str">
         <f t="shared" si="3"/>
@@ -8895,21 +9161,45 @@
       <c r="B15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="72"/>
-      <c r="N15" s="72"/>
+      <c r="C15" s="73">
+        <v>20</v>
+      </c>
+      <c r="D15" s="73">
+        <v>20</v>
+      </c>
+      <c r="E15" s="73">
+        <v>20</v>
+      </c>
+      <c r="F15" s="73">
+        <v>20</v>
+      </c>
+      <c r="G15" s="73">
+        <v>20</v>
+      </c>
+      <c r="H15" s="73">
+        <v>20</v>
+      </c>
+      <c r="I15" s="73">
+        <v>20</v>
+      </c>
+      <c r="J15" s="73">
+        <v>20</v>
+      </c>
+      <c r="K15" s="73">
+        <v>20</v>
+      </c>
+      <c r="L15" s="73">
+        <v>20</v>
+      </c>
+      <c r="M15" s="73">
+        <v>20</v>
+      </c>
+      <c r="N15" s="73">
+        <v>20</v>
+      </c>
       <c r="O15" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="P15" s="130">
         <f>'2018(NOT UPDATED)'!S19</f>
@@ -8917,23 +9207,23 @@
       </c>
       <c r="Q15" s="131">
         <f t="shared" si="4"/>
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="R15" s="132">
         <f t="shared" si="5"/>
-        <v>290</v>
+        <v>50</v>
       </c>
       <c r="S15" s="13">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="T15" s="14">
         <f t="shared" si="2"/>
-        <v>180</v>
+        <v>-60</v>
       </c>
       <c r="U15" s="15" t="str">
         <f t="shared" si="3"/>
-        <v>NO</v>
+        <v>OK</v>
       </c>
       <c r="V15" s="13"/>
       <c r="W15" s="134"/>
@@ -9231,7 +9521,9 @@
       <c r="C18" s="73">
         <v>20</v>
       </c>
-      <c r="D18" s="73"/>
+      <c r="D18" s="73">
+        <v>20</v>
+      </c>
       <c r="E18" s="72"/>
       <c r="F18" s="72">
         <v>5</v>
@@ -9246,7 +9538,7 @@
       <c r="N18" s="72"/>
       <c r="O18" s="13">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="P18" s="130">
         <f>'2018(NOT UPDATED)'!S22</f>
@@ -9254,19 +9546,19 @@
       </c>
       <c r="Q18" s="131">
         <f t="shared" si="4"/>
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="R18" s="132">
         <f t="shared" si="5"/>
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="S18" s="13">
         <f t="shared" si="1"/>
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="T18" s="14">
         <f t="shared" si="2"/>
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="U18" s="15" t="str">
         <f t="shared" si="3"/>
@@ -11511,7 +11803,7 @@
       <c r="M38" s="231"/>
       <c r="N38" s="231"/>
       <c r="O38" s="232">
-        <f t="shared" ref="O38:O60" si="9">SUM(C38:N38)</f>
+        <f t="shared" ref="O38:O61" si="9">SUM(C38:N38)</f>
         <v>0</v>
       </c>
       <c r="P38" s="233">
@@ -11527,7 +11819,7 @@
         <v>340</v>
       </c>
       <c r="S38" s="232">
-        <f t="shared" ref="S38:S60" si="10">(240)-(O38)</f>
+        <f t="shared" ref="S38:S61" si="10">(240)-(O38)</f>
         <v>240</v>
       </c>
       <c r="T38" s="235">
@@ -12755,7 +13047,9 @@
       <c r="F49" s="65">
         <v>5</v>
       </c>
-      <c r="G49" s="65"/>
+      <c r="G49" s="65">
+        <v>5</v>
+      </c>
       <c r="H49" s="65"/>
       <c r="I49" s="65"/>
       <c r="J49" s="65"/>
@@ -12765,24 +13059,24 @@
       <c r="N49" s="65"/>
       <c r="O49" s="13">
         <f t="shared" si="9"/>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="P49" s="130"/>
       <c r="Q49" s="131">
         <f t="shared" si="4"/>
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="R49" s="132">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="S49" s="13">
         <f t="shared" si="10"/>
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="T49" s="12">
         <f t="shared" si="2"/>
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="U49" s="20" t="str">
         <f t="shared" si="3"/>
@@ -12792,10 +13086,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="290" t="s">
+      <c r="AA49" s="291" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="291"/>
+      <c r="AB49" s="292"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -12873,12 +13167,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="297" t="s">
+      <c r="AI50" s="298" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="298"/>
-      <c r="AK50" s="298"/>
-      <c r="AL50" s="299"/>
+      <c r="AJ50" s="299"/>
+      <c r="AK50" s="299"/>
+      <c r="AL50" s="300"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -12949,12 +13243,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="294" t="s">
+      <c r="AI51" s="295" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="295"/>
-      <c r="AK51" s="295"/>
-      <c r="AL51" s="296"/>
+      <c r="AJ51" s="296"/>
+      <c r="AK51" s="296"/>
+      <c r="AL51" s="297"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -13220,14 +13514,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="300"/>
-      <c r="AD55" s="300"/>
-      <c r="AI55" s="297" t="s">
+      <c r="AC55" s="301"/>
+      <c r="AD55" s="301"/>
+      <c r="AI55" s="298" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="298"/>
-      <c r="AK55" s="298"/>
-      <c r="AL55" s="299"/>
+      <c r="AJ55" s="299"/>
+      <c r="AK55" s="299"/>
+      <c r="AL55" s="300"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -13288,12 +13582,12 @@
         <v>NO</v>
       </c>
       <c r="V56" s="2"/>
-      <c r="AI56" s="279" t="s">
+      <c r="AI56" s="280" t="s">
         <v>168</v>
       </c>
-      <c r="AJ56" s="279"/>
-      <c r="AK56" s="279"/>
-      <c r="AL56" s="279"/>
+      <c r="AJ56" s="280"/>
+      <c r="AK56" s="280"/>
+      <c r="AL56" s="280"/>
       <c r="AM56" s="52">
         <f>AM50-AM55</f>
         <v>450000</v>
@@ -13396,333 +13690,279 @@
       <c r="V58" s="2"/>
     </row>
     <row r="59" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+      <c r="A59" s="23">
         <v>57</v>
       </c>
-      <c r="B59" s="89" t="s">
+      <c r="B59" s="411" t="s">
         <v>205</v>
       </c>
-      <c r="C59" s="65"/>
-      <c r="D59" s="65"/>
-      <c r="E59" s="65"/>
-      <c r="F59" s="65"/>
-      <c r="G59" s="65"/>
-      <c r="H59" s="65"/>
-      <c r="I59" s="65"/>
-      <c r="J59" s="65"/>
-      <c r="K59" s="65"/>
-      <c r="L59" s="65"/>
-      <c r="M59" s="65"/>
-      <c r="N59" s="65"/>
-      <c r="O59" s="13">
+      <c r="C59" s="412"/>
+      <c r="D59" s="412"/>
+      <c r="E59" s="412"/>
+      <c r="F59" s="412"/>
+      <c r="G59" s="412"/>
+      <c r="H59" s="412"/>
+      <c r="I59" s="412"/>
+      <c r="J59" s="412"/>
+      <c r="K59" s="412"/>
+      <c r="L59" s="412"/>
+      <c r="M59" s="412"/>
+      <c r="N59" s="412"/>
+      <c r="O59" s="413">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="P59" s="130"/>
-      <c r="Q59" s="131">
+      <c r="P59" s="414"/>
+      <c r="Q59" s="415">
         <f t="shared" si="4"/>
         <v>240</v>
       </c>
-      <c r="R59" s="132">
+      <c r="R59" s="416">
         <f t="shared" si="5"/>
         <v>240</v>
       </c>
-      <c r="S59" s="13">
+      <c r="S59" s="413">
         <f t="shared" si="10"/>
         <v>240</v>
       </c>
-      <c r="T59" s="12">
+      <c r="T59" s="18">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="U59" s="20" t="str">
+      <c r="U59" s="417" t="str">
         <f t="shared" si="3"/>
         <v>NO</v>
       </c>
-      <c r="V59" s="2"/>
+      <c r="V59" s="418"/>
     </row>
     <row r="60" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+      <c r="A60" s="148">
         <v>58</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="419" t="s">
         <v>326</v>
       </c>
-      <c r="C60" s="256">
+      <c r="C60" s="420">
         <v>6</v>
       </c>
-      <c r="D60" s="65"/>
-      <c r="E60" s="65"/>
-      <c r="F60" s="65"/>
-      <c r="G60" s="65"/>
-      <c r="H60" s="65"/>
-      <c r="I60" s="65"/>
-      <c r="J60" s="65"/>
-      <c r="K60" s="65"/>
-      <c r="L60" s="65"/>
-      <c r="M60" s="65"/>
-      <c r="N60" s="65"/>
-      <c r="O60" s="13">
+      <c r="D60" s="259"/>
+      <c r="E60" s="259"/>
+      <c r="F60" s="259"/>
+      <c r="G60" s="259"/>
+      <c r="H60" s="259"/>
+      <c r="I60" s="259"/>
+      <c r="J60" s="259"/>
+      <c r="K60" s="259"/>
+      <c r="L60" s="259"/>
+      <c r="M60" s="259"/>
+      <c r="N60" s="259"/>
+      <c r="O60" s="421">
         <f t="shared" si="9"/>
         <v>6</v>
       </c>
-      <c r="P60" s="130"/>
-      <c r="Q60" s="131">
+      <c r="P60" s="422"/>
+      <c r="Q60" s="423">
         <f t="shared" si="4"/>
         <v>234</v>
       </c>
-      <c r="R60" s="132">
+      <c r="R60" s="424">
         <f t="shared" si="5"/>
         <v>234</v>
       </c>
-      <c r="S60" s="13">
+      <c r="S60" s="421">
         <f t="shared" si="10"/>
         <v>234</v>
       </c>
-      <c r="T60" s="12">
+      <c r="T60" s="425">
         <f t="shared" si="2"/>
         <v>174</v>
       </c>
-      <c r="U60" s="20" t="str">
+      <c r="U60" s="426" t="str">
         <f t="shared" si="3"/>
         <v>NO</v>
       </c>
-      <c r="V60" s="2"/>
-    </row>
-    <row r="61" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="280" t="s">
+      <c r="V60" s="419"/>
+    </row>
+    <row r="61" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="148">
+        <v>59</v>
+      </c>
+      <c r="B61" s="206" t="s">
+        <v>343</v>
+      </c>
+      <c r="C61" s="206">
+        <v>5</v>
+      </c>
+      <c r="D61" s="206"/>
+      <c r="E61" s="206"/>
+      <c r="F61" s="206"/>
+      <c r="G61" s="206"/>
+      <c r="H61" s="206"/>
+      <c r="I61" s="206"/>
+      <c r="J61" s="206"/>
+      <c r="K61" s="206"/>
+      <c r="L61" s="206"/>
+      <c r="M61" s="206"/>
+      <c r="N61" s="206"/>
+      <c r="O61" s="206"/>
+      <c r="P61" s="422"/>
+      <c r="Q61" s="423">
+        <f t="shared" si="4"/>
+        <v>235</v>
+      </c>
+      <c r="R61" s="424">
+        <f t="shared" si="5"/>
+        <v>235</v>
+      </c>
+      <c r="S61" s="421">
+        <f t="shared" si="10"/>
+        <v>240</v>
+      </c>
+      <c r="T61" s="425">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="U61" s="426" t="str">
+        <f t="shared" si="3"/>
+        <v>NO</v>
+      </c>
+      <c r="V61" s="206"/>
+    </row>
+    <row r="62" spans="1:41" s="258" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:41" s="258" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:41" s="258" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="3:19" s="258" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="3:19" s="258" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="3:19" s="258" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="281" t="s">
         <v>177</v>
       </c>
-      <c r="D63" s="281"/>
-      <c r="E63" s="281"/>
-      <c r="F63" s="281"/>
-      <c r="G63" s="282"/>
-      <c r="I63" s="286" t="s">
+      <c r="D69" s="282"/>
+      <c r="E69" s="282"/>
+      <c r="F69" s="282"/>
+      <c r="G69" s="283"/>
+      <c r="I69" s="287" t="s">
         <v>178</v>
       </c>
-      <c r="J63" s="286"/>
-      <c r="K63" s="286"/>
-      <c r="L63" s="286"/>
-      <c r="M63" s="286"/>
-    </row>
-    <row r="64" spans="1:41" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="283"/>
-      <c r="D64" s="284"/>
-      <c r="E64" s="284"/>
-      <c r="F64" s="284"/>
-      <c r="G64" s="285"/>
-      <c r="I64" s="286"/>
-      <c r="J64" s="286"/>
-      <c r="K64" s="286"/>
-      <c r="L64" s="286"/>
-      <c r="M64" s="286"/>
-    </row>
-    <row r="65" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K69" s="55"/>
-      <c r="L69" s="55"/>
-      <c r="M69" s="55"/>
-      <c r="N69" s="55"/>
-      <c r="O69" s="55"/>
-      <c r="R69" s="55"/>
-      <c r="S69" s="55"/>
-    </row>
-    <row r="70" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K70" s="55"/>
-      <c r="L70" s="55"/>
-      <c r="M70" s="55"/>
-      <c r="N70" s="55"/>
-      <c r="O70" s="55"/>
-      <c r="P70" s="279" t="s">
+      <c r="J69" s="287"/>
+      <c r="K69" s="287"/>
+      <c r="L69" s="287"/>
+      <c r="M69" s="287"/>
+    </row>
+    <row r="70" spans="3:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C70" s="284"/>
+      <c r="D70" s="285"/>
+      <c r="E70" s="285"/>
+      <c r="F70" s="285"/>
+      <c r="G70" s="286"/>
+      <c r="I70" s="287"/>
+      <c r="J70" s="287"/>
+      <c r="K70" s="287"/>
+      <c r="L70" s="287"/>
+      <c r="M70" s="287"/>
+    </row>
+    <row r="71" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K75" s="55"/>
+      <c r="L75" s="55"/>
+      <c r="M75" s="55"/>
+      <c r="N75" s="55"/>
+      <c r="O75" s="55"/>
+      <c r="R75" s="55"/>
+      <c r="S75" s="55"/>
+    </row>
+    <row r="76" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K76" s="55"/>
+      <c r="L76" s="55"/>
+      <c r="M76" s="55"/>
+      <c r="N76" s="55"/>
+      <c r="O76" s="55"/>
+      <c r="P76" s="280" t="s">
         <v>214</v>
       </c>
-      <c r="Q70" s="279"/>
-      <c r="R70" s="55"/>
-      <c r="S70" s="55"/>
-    </row>
-    <row r="71" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K71" s="54"/>
-      <c r="L71" s="54"/>
-      <c r="M71" s="54"/>
-      <c r="N71" s="54"/>
-      <c r="O71" s="54"/>
-      <c r="P71" s="139">
+      <c r="Q76" s="280"/>
+      <c r="R76" s="55"/>
+      <c r="S76" s="55"/>
+    </row>
+    <row r="77" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K77" s="54"/>
+      <c r="L77" s="54"/>
+      <c r="M77" s="54"/>
+      <c r="N77" s="54"/>
+      <c r="O77" s="54"/>
+      <c r="P77" s="139">
         <f>MAX(R6:R59)</f>
         <v>360</v>
       </c>
-      <c r="Q71" s="140"/>
-      <c r="R71" s="54"/>
-      <c r="S71" s="54"/>
-    </row>
-    <row r="72" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K72" s="49"/>
-      <c r="L72" s="49"/>
-      <c r="M72" s="49"/>
-      <c r="N72" s="49"/>
-      <c r="O72" s="49"/>
-      <c r="P72" s="49"/>
-      <c r="Q72" s="49"/>
-      <c r="R72" s="49"/>
-      <c r="S72" s="49"/>
-    </row>
-    <row r="73" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K73" s="49"/>
-      <c r="L73" s="49"/>
-      <c r="M73" s="49"/>
-      <c r="N73" s="49"/>
-      <c r="O73" s="49"/>
-      <c r="P73" s="49"/>
-      <c r="Q73" s="49"/>
-      <c r="R73" s="49"/>
-      <c r="S73" s="49"/>
-    </row>
-    <row r="74" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K74" s="49"/>
-      <c r="L74" s="49"/>
-      <c r="M74" s="49"/>
-      <c r="N74" s="49"/>
-      <c r="O74" s="49"/>
-      <c r="P74" s="49"/>
-      <c r="Q74" s="49"/>
-      <c r="R74" s="49"/>
-      <c r="S74" s="49"/>
-    </row>
-    <row r="75" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K75" s="49"/>
-      <c r="L75" s="49"/>
-      <c r="M75" s="49"/>
-      <c r="N75" s="49"/>
-    </row>
-    <row r="76" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K76" s="49"/>
-      <c r="L76" s="49"/>
-      <c r="M76" s="49"/>
-      <c r="N76" s="49"/>
-    </row>
-    <row r="77" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K77" s="49"/>
-      <c r="L77" s="49"/>
-      <c r="M77" s="49"/>
-      <c r="N77" s="49"/>
-    </row>
-    <row r="78" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q77" s="140"/>
+      <c r="R77" s="54"/>
+      <c r="S77" s="54"/>
+    </row>
+    <row r="78" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K78" s="49"/>
       <c r="L78" s="49"/>
       <c r="M78" s="49"/>
       <c r="N78" s="49"/>
-    </row>
-    <row r="79" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="172"/>
-      <c r="B79" s="172"/>
-      <c r="C79" s="49"/>
-      <c r="D79" s="49"/>
-      <c r="E79" s="49"/>
-      <c r="F79" s="49"/>
-      <c r="G79" s="49"/>
-      <c r="H79" s="49"/>
-      <c r="I79" s="49"/>
-      <c r="J79" s="49"/>
+      <c r="O78" s="49"/>
+      <c r="P78" s="49"/>
+      <c r="Q78" s="49"/>
+      <c r="R78" s="49"/>
+      <c r="S78" s="49"/>
+    </row>
+    <row r="79" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K79" s="49"/>
       <c r="L79" s="49"/>
       <c r="M79" s="49"/>
       <c r="N79" s="49"/>
-    </row>
-    <row r="80" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C80" s="49"/>
-      <c r="D80" s="49"/>
-      <c r="E80" s="49"/>
-      <c r="F80" s="49"/>
-      <c r="G80" s="49"/>
-      <c r="H80" s="49"/>
-      <c r="I80" s="49"/>
-      <c r="J80" s="49"/>
+      <c r="O79" s="49"/>
+      <c r="P79" s="49"/>
+      <c r="Q79" s="49"/>
+      <c r="R79" s="49"/>
+      <c r="S79" s="49"/>
+    </row>
+    <row r="80" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K80" s="49"/>
       <c r="L80" s="49"/>
       <c r="M80" s="49"/>
       <c r="N80" s="49"/>
-    </row>
-    <row r="81" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C81" s="49"/>
-      <c r="D81" s="49"/>
-      <c r="E81" s="49"/>
-      <c r="F81" s="49"/>
-      <c r="G81" s="49"/>
-      <c r="H81" s="49"/>
-      <c r="I81" s="49"/>
-      <c r="J81" s="49"/>
+      <c r="O80" s="49"/>
+      <c r="P80" s="49"/>
+      <c r="Q80" s="49"/>
+      <c r="R80" s="49"/>
+      <c r="S80" s="49"/>
+    </row>
+    <row r="81" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K81" s="49"/>
       <c r="L81" s="49"/>
       <c r="M81" s="49"/>
       <c r="N81" s="49"/>
-      <c r="O81" s="49"/>
-      <c r="P81" s="49"/>
-      <c r="Q81" s="49"/>
-      <c r="R81" s="49"/>
-      <c r="S81" s="49"/>
-    </row>
-    <row r="82" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C82" s="49"/>
-      <c r="D82" s="49"/>
-      <c r="E82" s="49"/>
-      <c r="F82" s="49"/>
-      <c r="G82" s="49"/>
-      <c r="H82" s="49"/>
-      <c r="I82" s="49"/>
-      <c r="J82" s="49"/>
+    </row>
+    <row r="82" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K82" s="49"/>
       <c r="L82" s="49"/>
       <c r="M82" s="49"/>
       <c r="N82" s="49"/>
-      <c r="O82" s="49"/>
-      <c r="P82" s="49"/>
-      <c r="Q82" s="49"/>
-      <c r="R82" s="49"/>
-      <c r="S82" s="49"/>
-    </row>
-    <row r="83" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C83" s="49"/>
-      <c r="D83" s="49"/>
-      <c r="E83" s="49"/>
-      <c r="F83" s="49"/>
-      <c r="G83" s="49"/>
-      <c r="H83" s="49"/>
-      <c r="I83" s="49"/>
-      <c r="J83" s="49"/>
+    </row>
+    <row r="83" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K83" s="49"/>
       <c r="L83" s="49"/>
       <c r="M83" s="49"/>
       <c r="N83" s="49"/>
-      <c r="O83" s="49"/>
-      <c r="P83" s="49"/>
-      <c r="Q83" s="49"/>
-      <c r="R83" s="49"/>
-      <c r="S83" s="49"/>
-    </row>
-    <row r="84" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C84" s="49"/>
-      <c r="D84" s="49"/>
-      <c r="E84" s="49"/>
-      <c r="F84" s="49"/>
-      <c r="G84" s="49"/>
-      <c r="H84" s="49"/>
-      <c r="I84" s="49"/>
-      <c r="J84" s="49"/>
+    </row>
+    <row r="84" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K84" s="49"/>
       <c r="L84" s="49"/>
       <c r="M84" s="49"/>
       <c r="N84" s="49"/>
-      <c r="O84" s="49"/>
-      <c r="P84" s="49"/>
-      <c r="Q84" s="49"/>
-      <c r="R84" s="49"/>
-      <c r="S84" s="49"/>
-    </row>
-    <row r="85" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="172"/>
+      <c r="B85" s="172"/>
       <c r="C85" s="49"/>
       <c r="D85" s="49"/>
       <c r="E85" s="49"/>
@@ -13735,13 +13975,8 @@
       <c r="L85" s="49"/>
       <c r="M85" s="49"/>
       <c r="N85" s="49"/>
-      <c r="O85" s="49"/>
-      <c r="P85" s="49"/>
-      <c r="Q85" s="49"/>
-      <c r="R85" s="49"/>
-      <c r="S85" s="49"/>
-    </row>
-    <row r="86" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C86" s="49"/>
       <c r="D86" s="49"/>
       <c r="E86" s="49"/>
@@ -13754,13 +13989,8 @@
       <c r="L86" s="49"/>
       <c r="M86" s="49"/>
       <c r="N86" s="49"/>
-      <c r="O86" s="49"/>
-      <c r="P86" s="49"/>
-      <c r="Q86" s="49"/>
-      <c r="R86" s="49"/>
-      <c r="S86" s="49"/>
-    </row>
-    <row r="87" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C87" s="49"/>
       <c r="D87" s="49"/>
       <c r="E87" s="49"/>
@@ -13779,7 +14009,7 @@
       <c r="R87" s="49"/>
       <c r="S87" s="49"/>
     </row>
-    <row r="88" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C88" s="49"/>
       <c r="D88" s="49"/>
       <c r="E88" s="49"/>
@@ -13798,7 +14028,7 @@
       <c r="R88" s="49"/>
       <c r="S88" s="49"/>
     </row>
-    <row r="89" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C89" s="49"/>
       <c r="D89" s="49"/>
       <c r="E89" s="49"/>
@@ -13817,7 +14047,7 @@
       <c r="R89" s="49"/>
       <c r="S89" s="49"/>
     </row>
-    <row r="90" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C90" s="49"/>
       <c r="D90" s="49"/>
       <c r="E90" s="49"/>
@@ -13836,12 +14066,120 @@
       <c r="R90" s="49"/>
       <c r="S90" s="49"/>
     </row>
-    <row r="91" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C91" s="49"/>
+      <c r="D91" s="49"/>
+      <c r="E91" s="49"/>
+      <c r="F91" s="49"/>
+      <c r="G91" s="49"/>
+      <c r="H91" s="49"/>
+      <c r="I91" s="49"/>
+      <c r="J91" s="49"/>
+      <c r="K91" s="49"/>
+      <c r="L91" s="49"/>
+      <c r="M91" s="49"/>
+      <c r="N91" s="49"/>
+      <c r="O91" s="49"/>
+      <c r="P91" s="49"/>
+      <c r="Q91" s="49"/>
+      <c r="R91" s="49"/>
+      <c r="S91" s="49"/>
+    </row>
+    <row r="92" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C92" s="49"/>
+      <c r="D92" s="49"/>
+      <c r="E92" s="49"/>
+      <c r="F92" s="49"/>
+      <c r="G92" s="49"/>
+      <c r="H92" s="49"/>
+      <c r="I92" s="49"/>
+      <c r="J92" s="49"/>
+      <c r="K92" s="49"/>
+      <c r="L92" s="49"/>
+      <c r="M92" s="49"/>
+      <c r="N92" s="49"/>
+      <c r="O92" s="49"/>
+      <c r="P92" s="49"/>
+      <c r="Q92" s="49"/>
+      <c r="R92" s="49"/>
+      <c r="S92" s="49"/>
+    </row>
+    <row r="93" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C93" s="49"/>
+      <c r="D93" s="49"/>
+      <c r="E93" s="49"/>
+      <c r="F93" s="49"/>
+      <c r="G93" s="49"/>
+      <c r="H93" s="49"/>
+      <c r="I93" s="49"/>
+      <c r="J93" s="49"/>
+      <c r="K93" s="49"/>
+      <c r="L93" s="49"/>
+      <c r="M93" s="49"/>
+      <c r="N93" s="49"/>
+      <c r="O93" s="49"/>
+      <c r="P93" s="49"/>
+      <c r="Q93" s="49"/>
+      <c r="R93" s="49"/>
+      <c r="S93" s="49"/>
+    </row>
+    <row r="94" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C94" s="49"/>
+      <c r="D94" s="49"/>
+      <c r="E94" s="49"/>
+      <c r="F94" s="49"/>
+      <c r="G94" s="49"/>
+      <c r="H94" s="49"/>
+      <c r="I94" s="49"/>
+      <c r="J94" s="49"/>
+      <c r="K94" s="49"/>
+      <c r="L94" s="49"/>
+      <c r="M94" s="49"/>
+      <c r="N94" s="49"/>
+      <c r="O94" s="49"/>
+      <c r="P94" s="49"/>
+      <c r="Q94" s="49"/>
+      <c r="R94" s="49"/>
+      <c r="S94" s="49"/>
+    </row>
+    <row r="95" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C95" s="49"/>
+      <c r="D95" s="49"/>
+      <c r="E95" s="49"/>
+      <c r="F95" s="49"/>
+      <c r="G95" s="49"/>
+      <c r="H95" s="49"/>
+      <c r="I95" s="49"/>
+      <c r="J95" s="49"/>
+      <c r="K95" s="49"/>
+      <c r="L95" s="49"/>
+      <c r="M95" s="49"/>
+      <c r="N95" s="49"/>
+      <c r="O95" s="49"/>
+      <c r="P95" s="49"/>
+      <c r="Q95" s="49"/>
+      <c r="R95" s="49"/>
+      <c r="S95" s="49"/>
+    </row>
+    <row r="96" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C96" s="49"/>
+      <c r="D96" s="49"/>
+      <c r="E96" s="49"/>
+      <c r="F96" s="49"/>
+      <c r="G96" s="49"/>
+      <c r="H96" s="49"/>
+      <c r="I96" s="49"/>
+      <c r="J96" s="49"/>
+      <c r="K96" s="49"/>
+      <c r="L96" s="49"/>
+      <c r="M96" s="49"/>
+      <c r="N96" s="49"/>
+      <c r="O96" s="49"/>
+      <c r="P96" s="49"/>
+      <c r="Q96" s="49"/>
+      <c r="R96" s="49"/>
+      <c r="S96" s="49"/>
+    </row>
     <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14006,6 +14344,12 @@
     <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="AI56:AL56"/>
@@ -14018,63 +14362,63 @@
     <mergeCell ref="AD7:AN7"/>
     <mergeCell ref="X5:AN5"/>
     <mergeCell ref="Z6:AN6"/>
-    <mergeCell ref="P70:Q70"/>
-    <mergeCell ref="C63:G64"/>
-    <mergeCell ref="I63:M64"/>
+    <mergeCell ref="P76:Q76"/>
+    <mergeCell ref="C69:G70"/>
+    <mergeCell ref="I69:M70"/>
     <mergeCell ref="C2:T3"/>
     <mergeCell ref="Y6:Y8"/>
     <mergeCell ref="X6:X8"/>
   </mergeCells>
-  <conditionalFormatting sqref="B6:V60">
-    <cfRule type="expression" dxfId="12" priority="7">
+  <conditionalFormatting sqref="B6:V61">
+    <cfRule type="expression" dxfId="22" priority="7">
       <formula>IF(ISBLANK($B$4), 0, SEARCH($B$4,$B6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK48">
-    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="21" priority="8" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH(("YES"),(AK9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK48">
-    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="20" priority="9" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH(("NO"),(AK9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y9:AN9 Y46:AC46 AD46:AL48 AC47:AC48 Y10:AL45 AM10:AN48">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="19" priority="10">
       <formula>IF(ISBLANK($Z$4), 0, SEARCH($Z$4,$Y9))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U6:U60">
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="NO">
+  <conditionalFormatting sqref="U6:U61">
+    <cfRule type="containsText" dxfId="18" priority="11" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH(("NO"),(U6))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U6:U60">
-    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="OK">
+  <conditionalFormatting sqref="U6:U61">
+    <cfRule type="containsText" dxfId="17" priority="12" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH(("OK"),(U6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y10:Y45">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="16" priority="6">
       <formula>IF(AK10="YES",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q6:R60">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="Q6:R61">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P6:P60">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="P6:P61">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y9:AN48">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>IF(ISBLANK($AA$4), 0, SEARCH($AA$4,$Y9))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14087,8 +14431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W36"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView topLeftCell="L8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14108,86 +14452,86 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="301" t="s">
+      <c r="A2" s="302" t="s">
         <v>301</v>
       </c>
-      <c r="B2" s="301"/>
-      <c r="C2" s="301"/>
-      <c r="D2" s="301"/>
-      <c r="E2" s="301"/>
-      <c r="F2" s="301"/>
-      <c r="G2" s="301"/>
-      <c r="H2" s="301"/>
-      <c r="I2" s="301"/>
-      <c r="J2" s="301"/>
-      <c r="K2" s="301"/>
-      <c r="L2" s="301"/>
+      <c r="B2" s="302"/>
+      <c r="C2" s="302"/>
+      <c r="D2" s="302"/>
+      <c r="E2" s="302"/>
+      <c r="F2" s="302"/>
+      <c r="G2" s="302"/>
+      <c r="H2" s="302"/>
+      <c r="I2" s="302"/>
+      <c r="J2" s="302"/>
+      <c r="K2" s="302"/>
+      <c r="L2" s="302"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="301"/>
-      <c r="B3" s="301"/>
-      <c r="C3" s="301"/>
-      <c r="D3" s="301"/>
-      <c r="E3" s="301"/>
-      <c r="F3" s="301"/>
-      <c r="G3" s="301"/>
-      <c r="H3" s="301"/>
-      <c r="I3" s="301"/>
-      <c r="J3" s="301"/>
-      <c r="K3" s="301"/>
-      <c r="L3" s="301"/>
+      <c r="A3" s="302"/>
+      <c r="B3" s="302"/>
+      <c r="C3" s="302"/>
+      <c r="D3" s="302"/>
+      <c r="E3" s="302"/>
+      <c r="F3" s="302"/>
+      <c r="G3" s="302"/>
+      <c r="H3" s="302"/>
+      <c r="I3" s="302"/>
+      <c r="J3" s="302"/>
+      <c r="K3" s="302"/>
+      <c r="L3" s="302"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="286" t="s">
+      <c r="A5" s="287" t="s">
         <v>304</v>
       </c>
-      <c r="B5" s="286"/>
-      <c r="C5" s="286"/>
-      <c r="D5" s="286"/>
-      <c r="E5" s="286"/>
-      <c r="F5" s="286"/>
-      <c r="G5" s="286"/>
-      <c r="H5" s="286"/>
-      <c r="I5" s="286"/>
-      <c r="J5" s="286"/>
-      <c r="K5" s="286"/>
-      <c r="M5" s="286" t="s">
+      <c r="B5" s="287"/>
+      <c r="C5" s="287"/>
+      <c r="D5" s="287"/>
+      <c r="E5" s="287"/>
+      <c r="F5" s="287"/>
+      <c r="G5" s="287"/>
+      <c r="H5" s="287"/>
+      <c r="I5" s="287"/>
+      <c r="J5" s="287"/>
+      <c r="K5" s="287"/>
+      <c r="M5" s="287" t="s">
         <v>325</v>
       </c>
-      <c r="N5" s="286"/>
-      <c r="O5" s="286"/>
-      <c r="P5" s="286"/>
-      <c r="Q5" s="286"/>
-      <c r="R5" s="286"/>
-      <c r="S5" s="286"/>
-      <c r="T5" s="286"/>
-      <c r="U5" s="286"/>
-      <c r="V5" s="286"/>
-      <c r="W5" s="286"/>
+      <c r="N5" s="287"/>
+      <c r="O5" s="287"/>
+      <c r="P5" s="287"/>
+      <c r="Q5" s="287"/>
+      <c r="R5" s="287"/>
+      <c r="S5" s="287"/>
+      <c r="T5" s="287"/>
+      <c r="U5" s="287"/>
+      <c r="V5" s="287"/>
+      <c r="W5" s="287"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="286"/>
-      <c r="B6" s="286"/>
-      <c r="C6" s="286"/>
-      <c r="D6" s="286"/>
-      <c r="E6" s="286"/>
-      <c r="F6" s="286"/>
-      <c r="G6" s="286"/>
-      <c r="H6" s="286"/>
-      <c r="I6" s="286"/>
-      <c r="J6" s="286"/>
-      <c r="K6" s="286"/>
-      <c r="M6" s="286"/>
-      <c r="N6" s="286"/>
-      <c r="O6" s="286"/>
-      <c r="P6" s="286"/>
-      <c r="Q6" s="286"/>
-      <c r="R6" s="286"/>
-      <c r="S6" s="286"/>
-      <c r="T6" s="286"/>
-      <c r="U6" s="286"/>
-      <c r="V6" s="286"/>
-      <c r="W6" s="286"/>
+      <c r="A6" s="287"/>
+      <c r="B6" s="287"/>
+      <c r="C6" s="287"/>
+      <c r="D6" s="287"/>
+      <c r="E6" s="287"/>
+      <c r="F6" s="287"/>
+      <c r="G6" s="287"/>
+      <c r="H6" s="287"/>
+      <c r="I6" s="287"/>
+      <c r="J6" s="287"/>
+      <c r="K6" s="287"/>
+      <c r="M6" s="287"/>
+      <c r="N6" s="287"/>
+      <c r="O6" s="287"/>
+      <c r="P6" s="287"/>
+      <c r="Q6" s="287"/>
+      <c r="R6" s="287"/>
+      <c r="S6" s="287"/>
+      <c r="T6" s="287"/>
+      <c r="U6" s="287"/>
+      <c r="V6" s="287"/>
+      <c r="W6" s="287"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M7" s="251"/>
@@ -14476,9 +14820,15 @@
       <c r="N15" s="1">
         <v>7</v>
       </c>
-      <c r="O15" s="218"/>
-      <c r="P15" s="252"/>
-      <c r="Q15" s="212"/>
+      <c r="O15" s="218" t="s">
+        <v>333</v>
+      </c>
+      <c r="P15" s="252" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q15" s="212">
+        <v>80000</v>
+      </c>
       <c r="R15" s="213"/>
       <c r="S15" s="251"/>
       <c r="T15" s="251"/>
@@ -14506,9 +14856,15 @@
       <c r="N16" s="1">
         <v>8</v>
       </c>
-      <c r="O16" s="218"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="213"/>
+      <c r="O16" s="218" t="s">
+        <v>333</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q16" s="213">
+        <v>100000</v>
+      </c>
       <c r="R16" s="212"/>
       <c r="S16" s="251"/>
       <c r="T16" s="251"/>
@@ -14536,9 +14892,15 @@
       <c r="N17" s="1">
         <v>9</v>
       </c>
-      <c r="O17" s="218"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="212"/>
+      <c r="O17" s="218" t="s">
+        <v>333</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="Q17" s="212">
+        <v>290000</v>
+      </c>
       <c r="R17" s="213"/>
       <c r="S17" s="251"/>
       <c r="T17" s="251"/>
@@ -14566,9 +14928,15 @@
       <c r="N18" s="1">
         <v>10</v>
       </c>
-      <c r="O18" s="218"/>
-      <c r="P18" s="252"/>
-      <c r="Q18" s="213"/>
+      <c r="O18" s="218" t="s">
+        <v>333</v>
+      </c>
+      <c r="P18" s="252" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q18" s="213">
+        <v>20000</v>
+      </c>
       <c r="R18" s="212"/>
       <c r="S18" s="251"/>
       <c r="T18" s="251"/>
@@ -14596,9 +14964,15 @@
       <c r="N19" s="1">
         <v>11</v>
       </c>
-      <c r="O19" s="218"/>
-      <c r="P19" s="252"/>
-      <c r="Q19" s="213"/>
+      <c r="O19" s="218" t="s">
+        <v>333</v>
+      </c>
+      <c r="P19" s="252" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q19" s="213">
+        <v>5000</v>
+      </c>
       <c r="R19" s="213"/>
       <c r="S19" s="251"/>
       <c r="T19" s="251"/>
@@ -14626,9 +15000,15 @@
       <c r="N20" s="1">
         <v>12</v>
       </c>
-      <c r="O20" s="218"/>
-      <c r="P20" s="252"/>
-      <c r="Q20" s="212"/>
+      <c r="O20" s="218" t="s">
+        <v>333</v>
+      </c>
+      <c r="P20" s="252" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q20" s="212">
+        <v>5000</v>
+      </c>
       <c r="R20" s="213"/>
       <c r="S20" s="251"/>
       <c r="T20" s="251"/>
@@ -14656,9 +15036,15 @@
       <c r="N21" s="1">
         <v>13</v>
       </c>
-      <c r="O21" s="218"/>
-      <c r="P21" s="252"/>
-      <c r="Q21" s="213"/>
+      <c r="O21" s="218" t="s">
+        <v>333</v>
+      </c>
+      <c r="P21" s="252" t="s">
+        <v>341</v>
+      </c>
+      <c r="Q21" s="213">
+        <v>5000</v>
+      </c>
       <c r="R21" s="212"/>
       <c r="S21" s="251"/>
       <c r="T21" s="251"/>
@@ -14686,9 +15072,15 @@
       <c r="N22" s="1">
         <v>14</v>
       </c>
-      <c r="O22" s="218"/>
-      <c r="P22" s="252"/>
-      <c r="Q22" s="213"/>
+      <c r="O22" s="218" t="s">
+        <v>333</v>
+      </c>
+      <c r="P22" s="252" t="s">
+        <v>342</v>
+      </c>
+      <c r="Q22" s="213">
+        <v>5000</v>
+      </c>
       <c r="R22" s="213"/>
       <c r="S22" s="251"/>
       <c r="T22" s="251"/>
@@ -14716,9 +15108,15 @@
       <c r="N23" s="1">
         <v>15</v>
       </c>
-      <c r="O23" s="218"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="212"/>
+      <c r="O23" s="218" t="s">
+        <v>333</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q23" s="212">
+        <v>5000</v>
+      </c>
       <c r="R23" s="213"/>
       <c r="S23" s="251"/>
       <c r="T23" s="251"/>
@@ -15006,7 +15404,7 @@
       </c>
       <c r="Q34" s="225">
         <f>SUM(Q9:Q33)</f>
-        <v>2866144.27</v>
+        <v>3381144.27</v>
       </c>
       <c r="R34" s="226">
         <f>SUM(R9:R33)</f>
@@ -15019,27 +15417,27 @@
       <c r="W34" s="251"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B35" s="306" t="s">
+      <c r="B35" s="307" t="s">
         <v>313</v>
       </c>
-      <c r="C35" s="307"/>
-      <c r="D35" s="308"/>
-      <c r="E35" s="302">
+      <c r="C35" s="308"/>
+      <c r="D35" s="309"/>
+      <c r="E35" s="303">
         <f>E34-F34</f>
         <v>2610871.1799999997</v>
       </c>
-      <c r="F35" s="303"/>
+      <c r="F35" s="304"/>
       <c r="M35" s="251"/>
-      <c r="N35" s="306" t="s">
+      <c r="N35" s="307" t="s">
         <v>313</v>
       </c>
-      <c r="O35" s="307"/>
-      <c r="P35" s="308"/>
-      <c r="Q35" s="302">
+      <c r="O35" s="308"/>
+      <c r="P35" s="309"/>
+      <c r="Q35" s="303">
         <f>Q34-R34</f>
-        <v>2791144.27</v>
-      </c>
-      <c r="R35" s="303"/>
+        <v>3306144.27</v>
+      </c>
+      <c r="R35" s="304"/>
       <c r="S35" s="251"/>
       <c r="T35" s="251"/>
       <c r="U35" s="251"/>
@@ -15047,17 +15445,17 @@
       <c r="W35" s="251"/>
     </row>
     <row r="36" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="309"/>
-      <c r="C36" s="310"/>
-      <c r="D36" s="311"/>
-      <c r="E36" s="304"/>
-      <c r="F36" s="305"/>
+      <c r="B36" s="310"/>
+      <c r="C36" s="311"/>
+      <c r="D36" s="312"/>
+      <c r="E36" s="305"/>
+      <c r="F36" s="306"/>
       <c r="M36" s="251"/>
-      <c r="N36" s="309"/>
-      <c r="O36" s="310"/>
-      <c r="P36" s="311"/>
-      <c r="Q36" s="304"/>
-      <c r="R36" s="305"/>
+      <c r="N36" s="310"/>
+      <c r="O36" s="311"/>
+      <c r="P36" s="312"/>
+      <c r="Q36" s="305"/>
+      <c r="R36" s="306"/>
       <c r="S36" s="251"/>
       <c r="T36" s="251"/>
       <c r="U36" s="251"/>
@@ -15106,17 +15504,17 @@
       <c r="A2" s="174"/>
       <c r="B2" s="175"/>
       <c r="C2" s="175"/>
-      <c r="D2" s="369" t="s">
+      <c r="D2" s="370" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="369"/>
-      <c r="F2" s="369"/>
-      <c r="G2" s="369"/>
-      <c r="H2" s="369"/>
-      <c r="I2" s="369"/>
-      <c r="J2" s="369"/>
-      <c r="K2" s="369"/>
-      <c r="L2" s="369"/>
+      <c r="E2" s="370"/>
+      <c r="F2" s="370"/>
+      <c r="G2" s="370"/>
+      <c r="H2" s="370"/>
+      <c r="I2" s="370"/>
+      <c r="J2" s="370"/>
+      <c r="K2" s="370"/>
+      <c r="L2" s="370"/>
       <c r="M2" s="176"/>
       <c r="N2" s="24"/>
     </row>
@@ -15134,205 +15532,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="178"/>
-      <c r="U3" s="312" t="s">
+      <c r="U3" s="313" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="313"/>
-      <c r="W3" s="314" t="s">
+      <c r="V3" s="314"/>
+      <c r="W3" s="315" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="313"/>
-      <c r="Y3" s="313"/>
-      <c r="Z3" s="313"/>
-      <c r="AA3" s="313"/>
-      <c r="AB3" s="313"/>
-      <c r="AC3" s="313"/>
-      <c r="AD3" s="315"/>
+      <c r="X3" s="314"/>
+      <c r="Y3" s="314"/>
+      <c r="Z3" s="314"/>
+      <c r="AA3" s="314"/>
+      <c r="AB3" s="314"/>
+      <c r="AC3" s="314"/>
+      <c r="AD3" s="316"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="177"/>
-      <c r="B4" s="373" t="s">
+      <c r="B4" s="374" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="374"/>
-      <c r="D4" s="374"/>
-      <c r="E4" s="374"/>
-      <c r="F4" s="374"/>
+      <c r="C4" s="375"/>
+      <c r="D4" s="375"/>
+      <c r="E4" s="375"/>
+      <c r="F4" s="375"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="321" t="s">
+      <c r="I4" s="322" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="292"/>
-      <c r="K4" s="292"/>
-      <c r="L4" s="292"/>
+      <c r="J4" s="293"/>
+      <c r="K4" s="293"/>
+      <c r="L4" s="293"/>
       <c r="M4" s="178"/>
-      <c r="U4" s="333" t="s">
+      <c r="U4" s="334" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="292"/>
-      <c r="W4" s="321" t="s">
+      <c r="V4" s="293"/>
+      <c r="W4" s="322" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="292"/>
-      <c r="Y4" s="292"/>
-      <c r="Z4" s="292"/>
-      <c r="AA4" s="292"/>
-      <c r="AB4" s="292"/>
-      <c r="AC4" s="292"/>
-      <c r="AD4" s="316"/>
+      <c r="X4" s="293"/>
+      <c r="Y4" s="293"/>
+      <c r="Z4" s="293"/>
+      <c r="AA4" s="293"/>
+      <c r="AB4" s="293"/>
+      <c r="AC4" s="293"/>
+      <c r="AD4" s="317"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="177"/>
-      <c r="B5" s="338" t="s">
+      <c r="B5" s="339" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="292"/>
-      <c r="D5" s="292"/>
-      <c r="E5" s="292"/>
-      <c r="F5" s="292"/>
+      <c r="C5" s="293"/>
+      <c r="D5" s="293"/>
+      <c r="E5" s="293"/>
+      <c r="F5" s="293"/>
       <c r="G5" s="154">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="340" t="s">
+      <c r="I5" s="341" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="361"/>
-      <c r="K5" s="363">
+      <c r="J5" s="362"/>
+      <c r="K5" s="364">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="364"/>
+      <c r="L5" s="365"/>
       <c r="M5" s="178"/>
-      <c r="U5" s="334" t="s">
+      <c r="U5" s="335" t="s">
         <v>231</v>
       </c>
-      <c r="V5" s="335"/>
-      <c r="W5" s="340" t="s">
+      <c r="V5" s="336"/>
+      <c r="W5" s="341" t="s">
         <v>232</v>
       </c>
-      <c r="X5" s="341"/>
-      <c r="Y5" s="341"/>
-      <c r="Z5" s="341"/>
-      <c r="AA5" s="341"/>
-      <c r="AB5" s="341"/>
-      <c r="AC5" s="341"/>
-      <c r="AD5" s="342"/>
+      <c r="X5" s="342"/>
+      <c r="Y5" s="342"/>
+      <c r="Z5" s="342"/>
+      <c r="AA5" s="342"/>
+      <c r="AB5" s="342"/>
+      <c r="AC5" s="342"/>
+      <c r="AD5" s="343"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="177"/>
-      <c r="B6" s="331" t="s">
+      <c r="B6" s="332" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="332"/>
-      <c r="D6" s="332"/>
-      <c r="E6" s="332"/>
-      <c r="F6" s="332"/>
+      <c r="C6" s="333"/>
+      <c r="D6" s="333"/>
+      <c r="E6" s="333"/>
+      <c r="F6" s="333"/>
       <c r="G6" s="154">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="362" t="s">
+      <c r="I6" s="363" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="357"/>
-      <c r="K6" s="365">
+      <c r="J6" s="358"/>
+      <c r="K6" s="366">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="366"/>
+      <c r="L6" s="367"/>
       <c r="M6" s="178"/>
-      <c r="U6" s="336"/>
-      <c r="V6" s="337"/>
-      <c r="W6" s="322" t="s">
+      <c r="U6" s="337"/>
+      <c r="V6" s="338"/>
+      <c r="W6" s="323" t="s">
         <v>233</v>
       </c>
-      <c r="X6" s="323"/>
-      <c r="Y6" s="323"/>
-      <c r="Z6" s="323"/>
-      <c r="AA6" s="323"/>
-      <c r="AB6" s="323"/>
-      <c r="AC6" s="323"/>
-      <c r="AD6" s="324"/>
+      <c r="X6" s="324"/>
+      <c r="Y6" s="324"/>
+      <c r="Z6" s="324"/>
+      <c r="AA6" s="324"/>
+      <c r="AB6" s="324"/>
+      <c r="AC6" s="324"/>
+      <c r="AD6" s="325"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="177"/>
-      <c r="B7" s="343" t="s">
+      <c r="B7" s="344" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="344"/>
-      <c r="D7" s="344"/>
-      <c r="E7" s="344"/>
-      <c r="F7" s="357"/>
+      <c r="C7" s="345"/>
+      <c r="D7" s="345"/>
+      <c r="E7" s="345"/>
+      <c r="F7" s="358"/>
       <c r="G7" s="154">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="362" t="s">
+      <c r="I7" s="363" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="357"/>
-      <c r="K7" s="367">
+      <c r="J7" s="358"/>
+      <c r="K7" s="368">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="368"/>
+      <c r="L7" s="369"/>
       <c r="M7" s="178"/>
-      <c r="U7" s="319"/>
-      <c r="V7" s="320"/>
-      <c r="W7" s="321" t="s">
+      <c r="U7" s="320"/>
+      <c r="V7" s="321"/>
+      <c r="W7" s="322" t="s">
         <v>234</v>
       </c>
-      <c r="X7" s="292"/>
-      <c r="Y7" s="292"/>
-      <c r="Z7" s="292"/>
-      <c r="AA7" s="292"/>
-      <c r="AB7" s="292"/>
-      <c r="AC7" s="292"/>
-      <c r="AD7" s="316"/>
+      <c r="X7" s="293"/>
+      <c r="Y7" s="293"/>
+      <c r="Z7" s="293"/>
+      <c r="AA7" s="293"/>
+      <c r="AB7" s="293"/>
+      <c r="AC7" s="293"/>
+      <c r="AD7" s="317"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="177"/>
-      <c r="B8" s="371" t="s">
+      <c r="B8" s="372" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="372"/>
-      <c r="D8" s="372"/>
-      <c r="E8" s="372"/>
-      <c r="F8" s="372"/>
+      <c r="C8" s="373"/>
+      <c r="D8" s="373"/>
+      <c r="E8" s="373"/>
+      <c r="F8" s="373"/>
       <c r="G8" s="155">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="340" t="s">
+      <c r="I8" s="341" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="361"/>
-      <c r="K8" s="352">
+      <c r="J8" s="362"/>
+      <c r="K8" s="353">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="353"/>
+      <c r="L8" s="354"/>
       <c r="M8" s="178"/>
-      <c r="U8" s="327" t="s">
+      <c r="U8" s="328" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="328"/>
-      <c r="W8" s="322" t="s">
+      <c r="V8" s="329"/>
+      <c r="W8" s="323" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="323"/>
-      <c r="Y8" s="323"/>
-      <c r="Z8" s="323"/>
-      <c r="AA8" s="323"/>
-      <c r="AB8" s="323"/>
-      <c r="AC8" s="323"/>
-      <c r="AD8" s="324"/>
+      <c r="X8" s="324"/>
+      <c r="Y8" s="324"/>
+      <c r="Z8" s="324"/>
+      <c r="AA8" s="324"/>
+      <c r="AB8" s="324"/>
+      <c r="AC8" s="324"/>
+      <c r="AD8" s="325"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="177"/>
@@ -15348,28 +15746,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="178"/>
-      <c r="U9" s="329"/>
-      <c r="V9" s="330"/>
-      <c r="W9" s="322" t="s">
+      <c r="U9" s="330"/>
+      <c r="V9" s="331"/>
+      <c r="W9" s="323" t="s">
         <v>237</v>
       </c>
-      <c r="X9" s="323"/>
-      <c r="Y9" s="323"/>
-      <c r="Z9" s="323"/>
-      <c r="AA9" s="323"/>
-      <c r="AB9" s="323"/>
-      <c r="AC9" s="323"/>
-      <c r="AD9" s="324"/>
+      <c r="X9" s="324"/>
+      <c r="Y9" s="324"/>
+      <c r="Z9" s="324"/>
+      <c r="AA9" s="324"/>
+      <c r="AB9" s="324"/>
+      <c r="AC9" s="324"/>
+      <c r="AD9" s="325"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="177"/>
-      <c r="B10" s="292" t="s">
+      <c r="B10" s="293" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="292"/>
-      <c r="D10" s="292"/>
-      <c r="E10" s="292"/>
-      <c r="F10" s="292"/>
+      <c r="C10" s="293"/>
+      <c r="D10" s="293"/>
+      <c r="E10" s="293"/>
+      <c r="F10" s="293"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -15380,30 +15778,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="178"/>
-      <c r="U10" s="331" t="s">
+      <c r="U10" s="332" t="s">
         <v>243</v>
       </c>
-      <c r="V10" s="332"/>
-      <c r="W10" s="292" t="s">
+      <c r="V10" s="333"/>
+      <c r="W10" s="293" t="s">
         <v>257</v>
       </c>
-      <c r="X10" s="292"/>
-      <c r="Y10" s="292"/>
-      <c r="Z10" s="292"/>
-      <c r="AA10" s="292"/>
-      <c r="AB10" s="292"/>
-      <c r="AC10" s="292"/>
-      <c r="AD10" s="316"/>
+      <c r="X10" s="293"/>
+      <c r="Y10" s="293"/>
+      <c r="Z10" s="293"/>
+      <c r="AA10" s="293"/>
+      <c r="AB10" s="293"/>
+      <c r="AC10" s="293"/>
+      <c r="AD10" s="317"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="177"/>
-      <c r="B11" s="292" t="s">
+      <c r="B11" s="293" t="s">
         <v>254</v>
       </c>
-      <c r="C11" s="292"/>
-      <c r="D11" s="292"/>
-      <c r="E11" s="292"/>
-      <c r="F11" s="292"/>
+      <c r="C11" s="293"/>
+      <c r="D11" s="293"/>
+      <c r="E11" s="293"/>
+      <c r="F11" s="293"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -15413,30 +15811,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="178"/>
-      <c r="U11" s="331" t="s">
+      <c r="U11" s="332" t="s">
         <v>256</v>
       </c>
-      <c r="V11" s="332"/>
-      <c r="W11" s="325" t="s">
+      <c r="V11" s="333"/>
+      <c r="W11" s="326" t="s">
         <v>258</v>
       </c>
-      <c r="X11" s="325"/>
-      <c r="Y11" s="325"/>
-      <c r="Z11" s="325"/>
-      <c r="AA11" s="325"/>
-      <c r="AB11" s="325"/>
-      <c r="AC11" s="325"/>
-      <c r="AD11" s="326"/>
+      <c r="X11" s="326"/>
+      <c r="Y11" s="326"/>
+      <c r="Z11" s="326"/>
+      <c r="AA11" s="326"/>
+      <c r="AB11" s="326"/>
+      <c r="AC11" s="326"/>
+      <c r="AD11" s="327"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="177"/>
-      <c r="B12" s="370" t="s">
+      <c r="B12" s="371" t="s">
         <v>255</v>
       </c>
-      <c r="C12" s="370"/>
-      <c r="D12" s="370"/>
-      <c r="E12" s="370"/>
-      <c r="F12" s="370"/>
+      <c r="C12" s="371"/>
+      <c r="D12" s="371"/>
+      <c r="E12" s="371"/>
+      <c r="F12" s="371"/>
       <c r="G12" s="182">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -15447,16 +15845,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="178"/>
-      <c r="U12" s="331"/>
-      <c r="V12" s="332"/>
-      <c r="W12" s="292"/>
-      <c r="X12" s="292"/>
-      <c r="Y12" s="292"/>
-      <c r="Z12" s="292"/>
-      <c r="AA12" s="292"/>
-      <c r="AB12" s="292"/>
-      <c r="AC12" s="292"/>
-      <c r="AD12" s="316"/>
+      <c r="U12" s="332"/>
+      <c r="V12" s="333"/>
+      <c r="W12" s="293"/>
+      <c r="X12" s="293"/>
+      <c r="Y12" s="293"/>
+      <c r="Z12" s="293"/>
+      <c r="AA12" s="293"/>
+      <c r="AB12" s="293"/>
+      <c r="AC12" s="293"/>
+      <c r="AD12" s="317"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="179"/>
@@ -15472,64 +15870,64 @@
       <c r="K13" s="180"/>
       <c r="L13" s="180"/>
       <c r="M13" s="181"/>
-      <c r="U13" s="331"/>
-      <c r="V13" s="332"/>
-      <c r="W13" s="292"/>
-      <c r="X13" s="292"/>
-      <c r="Y13" s="292"/>
-      <c r="Z13" s="292"/>
-      <c r="AA13" s="292"/>
-      <c r="AB13" s="292"/>
-      <c r="AC13" s="292"/>
-      <c r="AD13" s="316"/>
+      <c r="U13" s="332"/>
+      <c r="V13" s="333"/>
+      <c r="W13" s="293"/>
+      <c r="X13" s="293"/>
+      <c r="Y13" s="293"/>
+      <c r="Z13" s="293"/>
+      <c r="AA13" s="293"/>
+      <c r="AB13" s="293"/>
+      <c r="AC13" s="293"/>
+      <c r="AD13" s="317"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="346"/>
-      <c r="V14" s="347"/>
-      <c r="W14" s="317"/>
-      <c r="X14" s="317"/>
-      <c r="Y14" s="317"/>
-      <c r="Z14" s="317"/>
-      <c r="AA14" s="317"/>
-      <c r="AB14" s="317"/>
-      <c r="AC14" s="317"/>
-      <c r="AD14" s="318"/>
+      <c r="U14" s="347"/>
+      <c r="V14" s="348"/>
+      <c r="W14" s="318"/>
+      <c r="X14" s="318"/>
+      <c r="Y14" s="318"/>
+      <c r="Z14" s="318"/>
+      <c r="AA14" s="318"/>
+      <c r="AB14" s="318"/>
+      <c r="AC14" s="318"/>
+      <c r="AD14" s="319"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="174"/>
       <c r="B18" s="175"/>
       <c r="C18" s="175"/>
-      <c r="D18" s="369" t="s">
+      <c r="D18" s="370" t="s">
         <v>249</v>
       </c>
-      <c r="E18" s="369"/>
-      <c r="F18" s="369"/>
-      <c r="G18" s="369"/>
-      <c r="H18" s="369"/>
-      <c r="I18" s="369"/>
-      <c r="J18" s="369"/>
-      <c r="K18" s="369"/>
-      <c r="L18" s="369"/>
+      <c r="E18" s="370"/>
+      <c r="F18" s="370"/>
+      <c r="G18" s="370"/>
+      <c r="H18" s="370"/>
+      <c r="I18" s="370"/>
+      <c r="J18" s="370"/>
+      <c r="K18" s="370"/>
+      <c r="L18" s="370"/>
       <c r="M18" s="176"/>
-      <c r="O18" s="348" t="s">
+      <c r="O18" s="349" t="s">
         <v>250</v>
       </c>
-      <c r="P18" s="349"/>
-      <c r="Q18" s="349"/>
-      <c r="R18" s="349"/>
-      <c r="S18" s="350"/>
+      <c r="P18" s="350"/>
+      <c r="Q18" s="350"/>
+      <c r="R18" s="350"/>
+      <c r="S18" s="351"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="177"/>
       <c r="M19" s="178"/>
-      <c r="O19" s="338" t="s">
+      <c r="O19" s="339" t="s">
         <v>251</v>
       </c>
-      <c r="P19" s="292"/>
-      <c r="Q19" s="292"/>
-      <c r="R19" s="292"/>
-      <c r="S19" s="316"/>
+      <c r="P19" s="293"/>
+      <c r="Q19" s="293"/>
+      <c r="R19" s="293"/>
+      <c r="S19" s="317"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="177"/>
@@ -15540,119 +15938,119 @@
       <c r="F20" s="202"/>
       <c r="G20" s="68"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="321" t="s">
+      <c r="I20" s="322" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="292"/>
-      <c r="K20" s="292"/>
-      <c r="L20" s="292"/>
+      <c r="J20" s="293"/>
+      <c r="K20" s="293"/>
+      <c r="L20" s="293"/>
       <c r="M20" s="178"/>
-      <c r="O20" s="338" t="s">
+      <c r="O20" s="339" t="s">
         <v>252</v>
       </c>
-      <c r="P20" s="292"/>
-      <c r="Q20" s="292"/>
-      <c r="R20" s="292"/>
-      <c r="S20" s="316"/>
+      <c r="P20" s="293"/>
+      <c r="Q20" s="293"/>
+      <c r="R20" s="293"/>
+      <c r="S20" s="317"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="177"/>
-      <c r="B21" s="354" t="s">
+      <c r="B21" s="355" t="s">
         <v>297</v>
       </c>
-      <c r="C21" s="355"/>
-      <c r="D21" s="355"/>
-      <c r="E21" s="355"/>
-      <c r="F21" s="356"/>
+      <c r="C21" s="356"/>
+      <c r="D21" s="356"/>
+      <c r="E21" s="356"/>
+      <c r="F21" s="357"/>
       <c r="G21" s="70">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="340" t="s">
+      <c r="I21" s="341" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="361"/>
-      <c r="K21" s="363">
+      <c r="J21" s="362"/>
+      <c r="K21" s="364">
         <f>G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="L21" s="364"/>
+      <c r="L21" s="365"/>
       <c r="M21" s="178"/>
       <c r="N21" s="172"/>
-      <c r="O21" s="351" t="s">
+      <c r="O21" s="352" t="s">
         <v>259</v>
       </c>
-      <c r="P21" s="341"/>
-      <c r="Q21" s="341"/>
-      <c r="R21" s="341"/>
-      <c r="S21" s="342"/>
+      <c r="P21" s="342"/>
+      <c r="Q21" s="342"/>
+      <c r="R21" s="342"/>
+      <c r="S21" s="343"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="177"/>
-      <c r="B22" s="343" t="s">
+      <c r="B22" s="344" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="344"/>
-      <c r="D22" s="344"/>
-      <c r="E22" s="344"/>
-      <c r="F22" s="357"/>
+      <c r="C22" s="345"/>
+      <c r="D22" s="345"/>
+      <c r="E22" s="345"/>
+      <c r="F22" s="358"/>
       <c r="G22" s="154">
         <f>G21</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="362" t="s">
+      <c r="I22" s="363" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="357"/>
-      <c r="K22" s="365">
+      <c r="J22" s="358"/>
+      <c r="K22" s="366">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="L22" s="366"/>
+      <c r="L22" s="367"/>
       <c r="M22" s="178"/>
       <c r="N22" s="172"/>
-      <c r="O22" s="343" t="s">
+      <c r="O22" s="344" t="s">
         <v>260</v>
       </c>
-      <c r="P22" s="344"/>
-      <c r="Q22" s="344"/>
-      <c r="R22" s="344"/>
-      <c r="S22" s="345"/>
+      <c r="P22" s="345"/>
+      <c r="Q22" s="345"/>
+      <c r="R22" s="345"/>
+      <c r="S22" s="346"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="177"/>
-      <c r="B23" s="358" t="s">
+      <c r="B23" s="359" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="359"/>
-      <c r="D23" s="359"/>
-      <c r="E23" s="359"/>
-      <c r="F23" s="360"/>
+      <c r="C23" s="360"/>
+      <c r="D23" s="360"/>
+      <c r="E23" s="360"/>
+      <c r="F23" s="361"/>
       <c r="G23" s="155">
         <f>K24</f>
         <v>1568729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="362" t="s">
+      <c r="I23" s="363" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="357"/>
-      <c r="K23" s="367">
+      <c r="J23" s="358"/>
+      <c r="K23" s="368">
         <f>Pemasukkan!L31</f>
         <v>690000</v>
       </c>
-      <c r="L23" s="368"/>
+      <c r="L23" s="369"/>
       <c r="M23" s="178"/>
       <c r="N23" s="172"/>
-      <c r="O23" s="343" t="s">
+      <c r="O23" s="344" t="s">
         <v>261</v>
       </c>
-      <c r="P23" s="344"/>
-      <c r="Q23" s="344"/>
-      <c r="R23" s="344"/>
-      <c r="S23" s="345"/>
+      <c r="P23" s="345"/>
+      <c r="Q23" s="345"/>
+      <c r="R23" s="345"/>
+      <c r="S23" s="346"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="177"/>
@@ -15663,24 +16061,24 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="340" t="s">
+      <c r="I24" s="341" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="361"/>
-      <c r="K24" s="352">
+      <c r="J24" s="362"/>
+      <c r="K24" s="353">
         <f>(K21-K22)+K23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="L24" s="353"/>
+      <c r="L24" s="354"/>
       <c r="M24" s="178"/>
       <c r="N24" s="172"/>
-      <c r="O24" s="343" t="s">
+      <c r="O24" s="344" t="s">
         <v>262</v>
       </c>
-      <c r="P24" s="344"/>
-      <c r="Q24" s="344"/>
-      <c r="R24" s="344"/>
-      <c r="S24" s="345"/>
+      <c r="P24" s="345"/>
+      <c r="Q24" s="345"/>
+      <c r="R24" s="345"/>
+      <c r="S24" s="346"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="177"/>
@@ -15697,13 +16095,13 @@
       <c r="L25" s="24"/>
       <c r="M25" s="178"/>
       <c r="N25" s="172"/>
-      <c r="O25" s="338" t="s">
+      <c r="O25" s="339" t="s">
         <v>267</v>
       </c>
-      <c r="P25" s="292"/>
-      <c r="Q25" s="292"/>
-      <c r="R25" s="292"/>
-      <c r="S25" s="316"/>
+      <c r="P25" s="293"/>
+      <c r="Q25" s="293"/>
+      <c r="R25" s="293"/>
+      <c r="S25" s="317"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="177"/>
@@ -15720,11 +16118,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="178"/>
       <c r="N26" s="172"/>
-      <c r="O26" s="339"/>
-      <c r="P26" s="317"/>
-      <c r="Q26" s="317"/>
-      <c r="R26" s="317"/>
-      <c r="S26" s="318"/>
+      <c r="O26" s="340"/>
+      <c r="P26" s="318"/>
+      <c r="Q26" s="318"/>
+      <c r="R26" s="318"/>
+      <c r="S26" s="319"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="179"/>
@@ -15855,44 +16253,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="384" t="s">
+      <c r="C2" s="385" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="385"/>
-      <c r="E2" s="385"/>
-      <c r="F2" s="385"/>
-      <c r="G2" s="385"/>
-      <c r="H2" s="385"/>
-      <c r="I2" s="385"/>
-      <c r="J2" s="385"/>
-      <c r="K2" s="385"/>
+      <c r="D2" s="386"/>
+      <c r="E2" s="386"/>
+      <c r="F2" s="386"/>
+      <c r="G2" s="386"/>
+      <c r="H2" s="386"/>
+      <c r="I2" s="386"/>
+      <c r="J2" s="386"/>
+      <c r="K2" s="386"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="385"/>
-      <c r="D3" s="385"/>
-      <c r="E3" s="385"/>
-      <c r="F3" s="385"/>
-      <c r="G3" s="385"/>
-      <c r="H3" s="385"/>
-      <c r="I3" s="385"/>
-      <c r="J3" s="385"/>
-      <c r="K3" s="385"/>
+      <c r="C3" s="386"/>
+      <c r="D3" s="386"/>
+      <c r="E3" s="386"/>
+      <c r="F3" s="386"/>
+      <c r="G3" s="386"/>
+      <c r="H3" s="386"/>
+      <c r="I3" s="386"/>
+      <c r="J3" s="386"/>
+      <c r="K3" s="386"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="377" t="s">
+      <c r="C5" s="378" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="377"/>
-      <c r="E5" s="377"/>
-      <c r="F5" s="377"/>
-      <c r="G5" s="377"/>
-      <c r="I5" s="377" t="s">
+      <c r="D5" s="378"/>
+      <c r="E5" s="378"/>
+      <c r="F5" s="378"/>
+      <c r="G5" s="378"/>
+      <c r="I5" s="378" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="377"/>
-      <c r="K5" s="377"/>
-      <c r="L5" s="377"/>
-      <c r="M5" s="377"/>
+      <c r="J5" s="378"/>
+      <c r="K5" s="378"/>
+      <c r="L5" s="378"/>
+      <c r="M5" s="378"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -16332,88 +16730,88 @@
       <c r="M28" s="172"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="373" t="s">
+      <c r="D29" s="374" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="374"/>
-      <c r="F29" s="378">
+      <c r="E29" s="375"/>
+      <c r="F29" s="379">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="379"/>
+      <c r="G29" s="380"/>
       <c r="I29" s="172"/>
-      <c r="J29" s="373" t="s">
+      <c r="J29" s="374" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="374"/>
-      <c r="L29" s="378">
+      <c r="K29" s="375"/>
+      <c r="L29" s="379">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="379"/>
+      <c r="M29" s="380"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="333" t="s">
+      <c r="D30" s="334" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="292"/>
-      <c r="F30" s="380">
+      <c r="E30" s="293"/>
+      <c r="F30" s="381">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="381"/>
+      <c r="G30" s="382"/>
       <c r="I30" s="172"/>
-      <c r="J30" s="333" t="s">
+      <c r="J30" s="334" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="292"/>
-      <c r="L30" s="380">
+      <c r="K30" s="293"/>
+      <c r="L30" s="381">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="381"/>
+      <c r="M30" s="382"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="338" t="s">
+      <c r="D31" s="339" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="292"/>
-      <c r="F31" s="382">
+      <c r="E31" s="293"/>
+      <c r="F31" s="383">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="383"/>
+      <c r="G31" s="384"/>
       <c r="I31" s="172"/>
-      <c r="J31" s="338" t="s">
+      <c r="J31" s="339" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="292"/>
-      <c r="L31" s="382">
+      <c r="K31" s="293"/>
+      <c r="L31" s="383">
         <f>L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="383"/>
+      <c r="M31" s="384"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="371" t="s">
+      <c r="D32" s="372" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="372"/>
-      <c r="F32" s="375">
+      <c r="E32" s="373"/>
+      <c r="F32" s="376">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="376"/>
+      <c r="G32" s="377"/>
       <c r="I32" s="172"/>
-      <c r="J32" s="371" t="s">
+      <c r="J32" s="372" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="372"/>
-      <c r="L32" s="375">
+      <c r="K32" s="373"/>
+      <c r="L32" s="376">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="376"/>
+      <c r="M32" s="377"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16656,44 +17054,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="390" t="s">
+      <c r="C2" s="391" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="391"/>
-      <c r="E2" s="391"/>
-      <c r="F2" s="391"/>
-      <c r="G2" s="391"/>
-      <c r="H2" s="391"/>
-      <c r="I2" s="391"/>
-      <c r="J2" s="391"/>
-      <c r="K2" s="391"/>
+      <c r="D2" s="392"/>
+      <c r="E2" s="392"/>
+      <c r="F2" s="392"/>
+      <c r="G2" s="392"/>
+      <c r="H2" s="392"/>
+      <c r="I2" s="392"/>
+      <c r="J2" s="392"/>
+      <c r="K2" s="392"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="391"/>
-      <c r="D3" s="391"/>
-      <c r="E3" s="391"/>
-      <c r="F3" s="391"/>
-      <c r="G3" s="391"/>
-      <c r="H3" s="391"/>
-      <c r="I3" s="391"/>
-      <c r="J3" s="391"/>
-      <c r="K3" s="391"/>
+      <c r="C3" s="392"/>
+      <c r="D3" s="392"/>
+      <c r="E3" s="392"/>
+      <c r="F3" s="392"/>
+      <c r="G3" s="392"/>
+      <c r="H3" s="392"/>
+      <c r="I3" s="392"/>
+      <c r="J3" s="392"/>
+      <c r="K3" s="392"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="377" t="s">
+      <c r="C5" s="378" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="377"/>
-      <c r="E5" s="377"/>
-      <c r="F5" s="377"/>
-      <c r="G5" s="377"/>
-      <c r="I5" s="377" t="s">
+      <c r="D5" s="378"/>
+      <c r="E5" s="378"/>
+      <c r="F5" s="378"/>
+      <c r="G5" s="378"/>
+      <c r="I5" s="378" t="s">
         <v>246</v>
       </c>
-      <c r="J5" s="377"/>
-      <c r="K5" s="377"/>
-      <c r="L5" s="377"/>
-      <c r="M5" s="377"/>
+      <c r="J5" s="378"/>
+      <c r="K5" s="378"/>
+      <c r="L5" s="378"/>
+      <c r="M5" s="378"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -17177,88 +17575,88 @@
       <c r="M28" s="172"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="312" t="s">
+      <c r="D29" s="313" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="314"/>
-      <c r="F29" s="388">
+      <c r="E29" s="315"/>
+      <c r="F29" s="389">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="389"/>
+      <c r="G29" s="390"/>
       <c r="I29" s="172"/>
-      <c r="J29" s="312" t="s">
+      <c r="J29" s="313" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="314"/>
-      <c r="L29" s="388">
+      <c r="K29" s="315"/>
+      <c r="L29" s="389">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="389"/>
+      <c r="M29" s="390"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="338" t="s">
+      <c r="D30" s="339" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="292"/>
-      <c r="F30" s="380">
+      <c r="E30" s="293"/>
+      <c r="F30" s="381">
         <f>F27</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="381"/>
+      <c r="G30" s="382"/>
       <c r="I30" s="172"/>
-      <c r="J30" s="338" t="s">
+      <c r="J30" s="339" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="292"/>
-      <c r="L30" s="380">
+      <c r="K30" s="293"/>
+      <c r="L30" s="381">
         <f>L27</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="381"/>
+      <c r="M30" s="382"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="338" t="s">
+      <c r="D31" s="339" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="292"/>
-      <c r="F31" s="382">
+      <c r="E31" s="293"/>
+      <c r="F31" s="383">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="383"/>
+      <c r="G31" s="384"/>
       <c r="I31" s="172"/>
-      <c r="J31" s="338" t="s">
+      <c r="J31" s="339" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="292"/>
-      <c r="L31" s="382">
+      <c r="K31" s="293"/>
+      <c r="L31" s="383">
         <f>Pemasukkan!L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="383"/>
+      <c r="M31" s="384"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="371" t="s">
+      <c r="D32" s="372" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="372"/>
-      <c r="F32" s="386">
+      <c r="E32" s="373"/>
+      <c r="F32" s="387">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="387"/>
+      <c r="G32" s="388"/>
       <c r="I32" s="172"/>
-      <c r="J32" s="371" t="s">
+      <c r="J32" s="372" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="372"/>
-      <c r="L32" s="386">
+      <c r="K32" s="373"/>
+      <c r="L32" s="387">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="387"/>
+      <c r="M32" s="388"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17494,28 +17892,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="394" t="s">
+      <c r="C2" s="395" t="s">
         <v>230</v>
       </c>
-      <c r="D2" s="395"/>
-      <c r="E2" s="395"/>
-      <c r="F2" s="395"/>
-      <c r="G2" s="395"/>
-      <c r="H2" s="395"/>
-      <c r="I2" s="395"/>
-      <c r="J2" s="395"/>
-      <c r="K2" s="395"/>
+      <c r="D2" s="396"/>
+      <c r="E2" s="396"/>
+      <c r="F2" s="396"/>
+      <c r="G2" s="396"/>
+      <c r="H2" s="396"/>
+      <c r="I2" s="396"/>
+      <c r="J2" s="396"/>
+      <c r="K2" s="396"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="395"/>
-      <c r="D3" s="395"/>
-      <c r="E3" s="395"/>
-      <c r="F3" s="395"/>
-      <c r="G3" s="395"/>
-      <c r="H3" s="395"/>
-      <c r="I3" s="395"/>
-      <c r="J3" s="395"/>
-      <c r="K3" s="395"/>
+      <c r="C3" s="396"/>
+      <c r="D3" s="396"/>
+      <c r="E3" s="396"/>
+      <c r="F3" s="396"/>
+      <c r="G3" s="396"/>
+      <c r="H3" s="396"/>
+      <c r="I3" s="396"/>
+      <c r="J3" s="396"/>
+      <c r="K3" s="396"/>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="141"/>
@@ -17609,13 +18007,13 @@
       <c r="D9" s="199" t="s">
         <v>327</v>
       </c>
-      <c r="E9" s="257" t="s">
+      <c r="E9" s="256" t="s">
         <v>328</v>
       </c>
       <c r="F9" s="151">
         <v>6000</v>
       </c>
-      <c r="G9" s="258" t="s">
+      <c r="G9" s="257" t="s">
         <v>329</v>
       </c>
       <c r="H9" s="141"/>
@@ -17873,10 +18271,10 @@
     </row>
     <row r="29" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="141"/>
-      <c r="D29" s="396"/>
-      <c r="E29" s="396"/>
-      <c r="F29" s="397"/>
-      <c r="G29" s="397"/>
+      <c r="D29" s="397"/>
+      <c r="E29" s="397"/>
+      <c r="F29" s="398"/>
+      <c r="G29" s="398"/>
       <c r="H29" s="141"/>
       <c r="I29" s="141"/>
       <c r="J29" s="141"/>
@@ -17884,15 +18282,15 @@
     </row>
     <row r="30" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="24"/>
-      <c r="D30" s="398" t="s">
+      <c r="D30" s="399" t="s">
         <v>229</v>
       </c>
-      <c r="E30" s="399"/>
-      <c r="F30" s="400">
+      <c r="E30" s="400"/>
+      <c r="F30" s="401">
         <f>F27</f>
         <v>226000</v>
       </c>
-      <c r="G30" s="401"/>
+      <c r="G30" s="402"/>
       <c r="H30" s="141"/>
       <c r="I30" s="141"/>
       <c r="J30" s="141"/>
@@ -17907,10 +18305,10 @@
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="141"/>
-      <c r="D32" s="392"/>
-      <c r="E32" s="392"/>
-      <c r="F32" s="393"/>
-      <c r="G32" s="392"/>
+      <c r="D32" s="393"/>
+      <c r="E32" s="393"/>
+      <c r="F32" s="394"/>
+      <c r="G32" s="393"/>
       <c r="H32" s="141"/>
       <c r="I32" s="141"/>
       <c r="J32" s="141"/>
@@ -17947,17 +18345,17 @@
     <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="402" t="s">
+      <c r="C4" s="403" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="403"/>
+      <c r="D4" s="404"/>
       <c r="E4" s="27"/>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
-      <c r="H4" s="402" t="s">
+      <c r="H4" s="403" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="403"/>
+      <c r="I4" s="404"/>
       <c r="J4" s="35"/>
       <c r="K4" s="27"/>
     </row>
@@ -18084,17 +18482,17 @@
     <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26"/>
-      <c r="C17" s="402" t="s">
+      <c r="C17" s="403" t="s">
         <v>144</v>
       </c>
-      <c r="D17" s="403"/>
+      <c r="D17" s="404"/>
       <c r="E17" s="27"/>
       <c r="F17" s="26"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="402" t="s">
+      <c r="H17" s="403" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="403"/>
+      <c r="I17" s="404"/>
       <c r="J17" s="35"/>
       <c r="K17" s="27"/>
     </row>
@@ -18248,28 +18646,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="405" t="s">
+      <c r="B2" s="406" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="406"/>
-      <c r="D2" s="406"/>
-      <c r="E2" s="406"/>
-      <c r="F2" s="406"/>
-      <c r="G2" s="406"/>
-      <c r="H2" s="406"/>
-      <c r="I2" s="406"/>
-      <c r="J2" s="406"/>
+      <c r="C2" s="407"/>
+      <c r="D2" s="407"/>
+      <c r="E2" s="407"/>
+      <c r="F2" s="407"/>
+      <c r="G2" s="407"/>
+      <c r="H2" s="407"/>
+      <c r="I2" s="407"/>
+      <c r="J2" s="407"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="406"/>
-      <c r="C3" s="406"/>
-      <c r="D3" s="406"/>
-      <c r="E3" s="406"/>
-      <c r="F3" s="406"/>
-      <c r="G3" s="406"/>
-      <c r="H3" s="406"/>
-      <c r="I3" s="406"/>
-      <c r="J3" s="406"/>
+      <c r="B3" s="407"/>
+      <c r="C3" s="407"/>
+      <c r="D3" s="407"/>
+      <c r="E3" s="407"/>
+      <c r="F3" s="407"/>
+      <c r="G3" s="407"/>
+      <c r="H3" s="407"/>
+      <c r="I3" s="407"/>
+      <c r="J3" s="407"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -18290,10 +18688,10 @@
       <c r="G6" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="H6" s="321" t="s">
+      <c r="H6" s="322" t="s">
         <v>281</v>
       </c>
-      <c r="I6" s="292"/>
+      <c r="I6" s="293"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -18315,11 +18713,11 @@
       <c r="G7" s="195">
         <v>205000</v>
       </c>
-      <c r="H7" s="407">
+      <c r="H7" s="408">
         <f>F7-G7</f>
         <v>380000</v>
       </c>
-      <c r="I7" s="292"/>
+      <c r="I7" s="293"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="196"/>
@@ -18328,8 +18726,8 @@
       <c r="E8" s="197"/>
       <c r="F8" s="197"/>
       <c r="G8" s="197"/>
-      <c r="H8" s="404"/>
-      <c r="I8" s="404"/>
+      <c r="H8" s="405"/>
+      <c r="I8" s="405"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="196"/>
@@ -18340,11 +18738,11 @@
       <c r="G9" s="198" t="s">
         <v>282</v>
       </c>
-      <c r="H9" s="408">
+      <c r="H9" s="409">
         <f>H7</f>
         <v>380000</v>
       </c>
-      <c r="I9" s="409"/>
+      <c r="I9" s="410"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="196"/>
@@ -18353,8 +18751,8 @@
       <c r="E10" s="197"/>
       <c r="F10" s="197"/>
       <c r="G10" s="197"/>
-      <c r="H10" s="404"/>
-      <c r="I10" s="404"/>
+      <c r="H10" s="405"/>
+      <c r="I10" s="405"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="196"/>
@@ -18363,8 +18761,8 @@
       <c r="E11" s="197"/>
       <c r="F11" s="197"/>
       <c r="G11" s="197"/>
-      <c r="H11" s="404"/>
-      <c r="I11" s="404"/>
+      <c r="H11" s="405"/>
+      <c r="I11" s="405"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="196"/>
@@ -18373,8 +18771,8 @@
       <c r="E12" s="197"/>
       <c r="F12" s="197"/>
       <c r="G12" s="197"/>
-      <c r="H12" s="404"/>
-      <c r="I12" s="404"/>
+      <c r="H12" s="405"/>
+      <c r="I12" s="405"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="196"/>
@@ -18383,8 +18781,8 @@
       <c r="E13" s="197"/>
       <c r="F13" s="197"/>
       <c r="G13" s="197"/>
-      <c r="H13" s="404"/>
-      <c r="I13" s="404"/>
+      <c r="H13" s="405"/>
+      <c r="I13" s="405"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="196"/>
@@ -18393,8 +18791,8 @@
       <c r="E14" s="197"/>
       <c r="F14" s="197"/>
       <c r="G14" s="197"/>
-      <c r="H14" s="404"/>
-      <c r="I14" s="404"/>
+      <c r="H14" s="405"/>
+      <c r="I14" s="405"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="196"/>
@@ -18403,8 +18801,8 @@
       <c r="E15" s="197"/>
       <c r="F15" s="197"/>
       <c r="G15" s="197"/>
-      <c r="H15" s="404"/>
-      <c r="I15" s="404"/>
+      <c r="H15" s="405"/>
+      <c r="I15" s="405"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="196"/>
@@ -18413,8 +18811,8 @@
       <c r="E16" s="197"/>
       <c r="F16" s="197"/>
       <c r="G16" s="197"/>
-      <c r="H16" s="404"/>
-      <c r="I16" s="404"/>
+      <c r="H16" s="405"/>
+      <c r="I16" s="405"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="196"/>
@@ -18423,8 +18821,8 @@
       <c r="E17" s="197"/>
       <c r="F17" s="197"/>
       <c r="G17" s="197"/>
-      <c r="H17" s="404"/>
-      <c r="I17" s="404"/>
+      <c r="H17" s="405"/>
+      <c r="I17" s="405"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>

<commit_message>
Joshua KAS, Rapli KAS, Revi KAS
KAS Josh :

95.000 (tagihan kas)
95.000 (Kas yang dibayarkan)
------------- -
0 (sisa tagihan kas)

KAS Revi :

100.000 (tagihan kas)
100.000 (Kas yang dibayarkan)
------------- -
0 (sisa tagihan kas)

KAS Rapli  :

263.000 (tagihan kas)
5.000 (Kas yang dibayarkan)
------------- -
258.000 (sisa tagihan kas)
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="349">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -1059,7 +1059,16 @@
     <t>Daniel KAS (tunai)</t>
   </si>
   <si>
-    <t>josh</t>
+    <t>21 Desember 2019</t>
+  </si>
+  <si>
+    <t>Rapli KAS(tunai)</t>
+  </si>
+  <si>
+    <t>Revi KAS(trf)</t>
+  </si>
+  <si>
+    <t>rapli</t>
   </si>
 </sst>
 </file>
@@ -2830,18 +2839,44 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="14" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="14" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2850,9 +2885,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2868,37 +2908,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2906,29 +2948,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2963,6 +3012,156 @@
     <xf numFmtId="177" fontId="4" fillId="26" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2975,33 +3174,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3021,136 +3199,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3161,29 +3228,23 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3191,18 +3252,6 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3255,46 +3304,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="14" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="14" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3303,171 +3312,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF92D050"/>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4603,126 +4453,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="266" t="s">
+      <c r="A1" s="276" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="267"/>
-      <c r="C1" s="267"/>
-      <c r="D1" s="267"/>
-      <c r="E1" s="267"/>
-      <c r="F1" s="267"/>
-      <c r="G1" s="267"/>
-      <c r="H1" s="267"/>
-      <c r="I1" s="267"/>
-      <c r="J1" s="267"/>
-      <c r="K1" s="267"/>
-      <c r="L1" s="267"/>
-      <c r="M1" s="267"/>
-      <c r="N1" s="267"/>
-      <c r="O1" s="267"/>
-      <c r="P1" s="267"/>
-      <c r="Q1" s="267"/>
-      <c r="R1" s="267"/>
+      <c r="B1" s="277"/>
+      <c r="C1" s="277"/>
+      <c r="D1" s="277"/>
+      <c r="E1" s="277"/>
+      <c r="F1" s="277"/>
+      <c r="G1" s="277"/>
+      <c r="H1" s="277"/>
+      <c r="I1" s="277"/>
+      <c r="J1" s="277"/>
+      <c r="K1" s="277"/>
+      <c r="L1" s="277"/>
+      <c r="M1" s="277"/>
+      <c r="N1" s="277"/>
+      <c r="O1" s="277"/>
+      <c r="P1" s="277"/>
+      <c r="Q1" s="277"/>
+      <c r="R1" s="277"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="268"/>
-      <c r="B2" s="269"/>
-      <c r="C2" s="269"/>
-      <c r="D2" s="269"/>
-      <c r="E2" s="269"/>
-      <c r="F2" s="269"/>
-      <c r="G2" s="269"/>
-      <c r="H2" s="269"/>
-      <c r="I2" s="269"/>
-      <c r="J2" s="269"/>
-      <c r="K2" s="269"/>
-      <c r="L2" s="269"/>
-      <c r="M2" s="269"/>
-      <c r="N2" s="269"/>
-      <c r="O2" s="269"/>
-      <c r="P2" s="269"/>
-      <c r="Q2" s="269"/>
-      <c r="R2" s="269"/>
+      <c r="A2" s="278"/>
+      <c r="B2" s="279"/>
+      <c r="C2" s="279"/>
+      <c r="D2" s="279"/>
+      <c r="E2" s="279"/>
+      <c r="F2" s="279"/>
+      <c r="G2" s="279"/>
+      <c r="H2" s="279"/>
+      <c r="I2" s="279"/>
+      <c r="J2" s="279"/>
+      <c r="K2" s="279"/>
+      <c r="L2" s="279"/>
+      <c r="M2" s="279"/>
+      <c r="N2" s="279"/>
+      <c r="O2" s="279"/>
+      <c r="P2" s="279"/>
+      <c r="Q2" s="279"/>
+      <c r="R2" s="279"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="268"/>
-      <c r="B3" s="269"/>
-      <c r="C3" s="269"/>
-      <c r="D3" s="269"/>
-      <c r="E3" s="269"/>
-      <c r="F3" s="269"/>
-      <c r="G3" s="269"/>
-      <c r="H3" s="269"/>
-      <c r="I3" s="269"/>
-      <c r="J3" s="269"/>
-      <c r="K3" s="269"/>
-      <c r="L3" s="269"/>
-      <c r="M3" s="269"/>
-      <c r="N3" s="269"/>
-      <c r="O3" s="269"/>
-      <c r="P3" s="269"/>
-      <c r="Q3" s="269"/>
-      <c r="R3" s="269"/>
+      <c r="A3" s="278"/>
+      <c r="B3" s="279"/>
+      <c r="C3" s="279"/>
+      <c r="D3" s="279"/>
+      <c r="E3" s="279"/>
+      <c r="F3" s="279"/>
+      <c r="G3" s="279"/>
+      <c r="H3" s="279"/>
+      <c r="I3" s="279"/>
+      <c r="J3" s="279"/>
+      <c r="K3" s="279"/>
+      <c r="L3" s="279"/>
+      <c r="M3" s="279"/>
+      <c r="N3" s="279"/>
+      <c r="O3" s="279"/>
+      <c r="P3" s="279"/>
+      <c r="Q3" s="279"/>
+      <c r="R3" s="279"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="268"/>
-      <c r="B4" s="269"/>
-      <c r="C4" s="269"/>
-      <c r="D4" s="269"/>
-      <c r="E4" s="269"/>
-      <c r="F4" s="269"/>
-      <c r="G4" s="269"/>
-      <c r="H4" s="269"/>
-      <c r="I4" s="269"/>
-      <c r="J4" s="269"/>
-      <c r="K4" s="269"/>
-      <c r="L4" s="269"/>
-      <c r="M4" s="269"/>
-      <c r="N4" s="269"/>
-      <c r="O4" s="269"/>
-      <c r="P4" s="269"/>
-      <c r="Q4" s="269"/>
-      <c r="R4" s="269"/>
+      <c r="A4" s="278"/>
+      <c r="B4" s="279"/>
+      <c r="C4" s="279"/>
+      <c r="D4" s="279"/>
+      <c r="E4" s="279"/>
+      <c r="F4" s="279"/>
+      <c r="G4" s="279"/>
+      <c r="H4" s="279"/>
+      <c r="I4" s="279"/>
+      <c r="J4" s="279"/>
+      <c r="K4" s="279"/>
+      <c r="L4" s="279"/>
+      <c r="M4" s="279"/>
+      <c r="N4" s="279"/>
+      <c r="O4" s="279"/>
+      <c r="P4" s="279"/>
+      <c r="Q4" s="279"/>
+      <c r="R4" s="279"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="268"/>
-      <c r="B5" s="269"/>
-      <c r="C5" s="269"/>
-      <c r="D5" s="269"/>
-      <c r="E5" s="269"/>
-      <c r="F5" s="269"/>
-      <c r="G5" s="269"/>
-      <c r="H5" s="269"/>
-      <c r="I5" s="269"/>
-      <c r="J5" s="269"/>
-      <c r="K5" s="269"/>
-      <c r="L5" s="269"/>
-      <c r="M5" s="269"/>
-      <c r="N5" s="269"/>
-      <c r="O5" s="269"/>
-      <c r="P5" s="269"/>
-      <c r="Q5" s="269"/>
-      <c r="R5" s="269"/>
+      <c r="A5" s="278"/>
+      <c r="B5" s="279"/>
+      <c r="C5" s="279"/>
+      <c r="D5" s="279"/>
+      <c r="E5" s="279"/>
+      <c r="F5" s="279"/>
+      <c r="G5" s="279"/>
+      <c r="H5" s="279"/>
+      <c r="I5" s="279"/>
+      <c r="J5" s="279"/>
+      <c r="K5" s="279"/>
+      <c r="L5" s="279"/>
+      <c r="M5" s="279"/>
+      <c r="N5" s="279"/>
+      <c r="O5" s="279"/>
+      <c r="P5" s="279"/>
+      <c r="Q5" s="279"/>
+      <c r="R5" s="279"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="268"/>
-      <c r="B6" s="269"/>
-      <c r="C6" s="269"/>
-      <c r="D6" s="269"/>
-      <c r="E6" s="269"/>
-      <c r="F6" s="269"/>
-      <c r="G6" s="269"/>
-      <c r="H6" s="269"/>
-      <c r="I6" s="269"/>
-      <c r="J6" s="269"/>
-      <c r="K6" s="269"/>
-      <c r="L6" s="269"/>
-      <c r="M6" s="269"/>
-      <c r="N6" s="269"/>
-      <c r="O6" s="269"/>
-      <c r="P6" s="269"/>
-      <c r="Q6" s="269"/>
-      <c r="R6" s="269"/>
+      <c r="A6" s="278"/>
+      <c r="B6" s="279"/>
+      <c r="C6" s="279"/>
+      <c r="D6" s="279"/>
+      <c r="E6" s="279"/>
+      <c r="F6" s="279"/>
+      <c r="G6" s="279"/>
+      <c r="H6" s="279"/>
+      <c r="I6" s="279"/>
+      <c r="J6" s="279"/>
+      <c r="K6" s="279"/>
+      <c r="L6" s="279"/>
+      <c r="M6" s="279"/>
+      <c r="N6" s="279"/>
+      <c r="O6" s="279"/>
+      <c r="P6" s="279"/>
+      <c r="Q6" s="279"/>
+      <c r="R6" s="279"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -7667,58 +7517,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="271" t="s">
+      <c r="J79" s="284" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="272"/>
-      <c r="L79" s="272"/>
-      <c r="M79" s="272"/>
-      <c r="N79" s="273"/>
-      <c r="P79" s="279" t="s">
+      <c r="K79" s="285"/>
+      <c r="L79" s="285"/>
+      <c r="M79" s="285"/>
+      <c r="N79" s="286"/>
+      <c r="P79" s="292" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="272"/>
-      <c r="R79" s="272"/>
-      <c r="S79" s="273"/>
+      <c r="Q79" s="285"/>
+      <c r="R79" s="285"/>
+      <c r="S79" s="286"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="274" t="s">
+      <c r="J80" s="287" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="269"/>
-      <c r="L80" s="269"/>
-      <c r="M80" s="269"/>
-      <c r="N80" s="275"/>
-      <c r="P80" s="274" t="s">
+      <c r="K80" s="279"/>
+      <c r="L80" s="279"/>
+      <c r="M80" s="279"/>
+      <c r="N80" s="288"/>
+      <c r="P80" s="287" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="269"/>
-      <c r="R80" s="269"/>
-      <c r="S80" s="275"/>
+      <c r="Q80" s="279"/>
+      <c r="R80" s="279"/>
+      <c r="S80" s="288"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="276"/>
-      <c r="K81" s="277"/>
-      <c r="L81" s="277"/>
-      <c r="M81" s="277"/>
-      <c r="N81" s="278"/>
-      <c r="P81" s="276"/>
-      <c r="Q81" s="277"/>
-      <c r="R81" s="277"/>
-      <c r="S81" s="278"/>
+      <c r="J81" s="289"/>
+      <c r="K81" s="290"/>
+      <c r="L81" s="290"/>
+      <c r="M81" s="290"/>
+      <c r="N81" s="291"/>
+      <c r="P81" s="289"/>
+      <c r="Q81" s="290"/>
+      <c r="R81" s="290"/>
+      <c r="S81" s="291"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="270" t="s">
+      <c r="J82" s="282" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="261"/>
-      <c r="L82" s="262"/>
-      <c r="M82" s="270" t="s">
+      <c r="K82" s="283"/>
+      <c r="L82" s="281"/>
+      <c r="M82" s="282" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="262"/>
-      <c r="P82" s="270"/>
-      <c r="Q82" s="262"/>
+      <c r="N82" s="281"/>
+      <c r="P82" s="282"/>
+      <c r="Q82" s="281"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -7727,38 +7577,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="260" t="s">
+      <c r="J83" s="293" t="s">
         <v>70</v>
       </c>
-      <c r="K83" s="261"/>
-      <c r="L83" s="262"/>
-      <c r="M83" s="263">
+      <c r="K83" s="283"/>
+      <c r="L83" s="281"/>
+      <c r="M83" s="294">
         <v>7350000</v>
       </c>
-      <c r="N83" s="262"/>
-      <c r="P83" s="264" t="s">
+      <c r="N83" s="281"/>
+      <c r="P83" s="280" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="262"/>
+      <c r="Q83" s="281"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="260" t="s">
+      <c r="J84" s="293" t="s">
         <v>72</v>
       </c>
-      <c r="K84" s="261"/>
-      <c r="L84" s="262"/>
-      <c r="M84" s="265">
+      <c r="K84" s="283"/>
+      <c r="L84" s="281"/>
+      <c r="M84" s="295">
         <v>1100000</v>
       </c>
-      <c r="N84" s="262"/>
-      <c r="P84" s="264" t="s">
+      <c r="N84" s="281"/>
+      <c r="P84" s="280" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="262"/>
+      <c r="Q84" s="281"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -7767,39 +7617,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="260" t="s">
+      <c r="J85" s="293" t="s">
         <v>75</v>
       </c>
-      <c r="K85" s="261"/>
-      <c r="L85" s="262"/>
-      <c r="M85" s="263">
+      <c r="K85" s="283"/>
+      <c r="L85" s="281"/>
+      <c r="M85" s="294">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="262"/>
-      <c r="P85" s="264" t="s">
+      <c r="N85" s="281"/>
+      <c r="P85" s="280" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="262"/>
+      <c r="Q85" s="281"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="260" t="s">
+      <c r="J86" s="293" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="261"/>
-      <c r="L86" s="262"/>
-      <c r="M86" s="263">
+      <c r="K86" s="283"/>
+      <c r="L86" s="281"/>
+      <c r="M86" s="294">
         <v>8411850</v>
       </c>
-      <c r="N86" s="262"/>
-      <c r="P86" s="264" t="s">
+      <c r="N86" s="281"/>
+      <c r="P86" s="280" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="262"/>
+      <c r="Q86" s="281"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -7807,20 +7657,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="260" t="s">
+      <c r="J87" s="293" t="s">
         <v>79</v>
       </c>
-      <c r="K87" s="261"/>
-      <c r="L87" s="262"/>
-      <c r="M87" s="263">
+      <c r="K87" s="283"/>
+      <c r="L87" s="281"/>
+      <c r="M87" s="294">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="262"/>
-      <c r="P87" s="264" t="s">
+      <c r="N87" s="281"/>
+      <c r="P87" s="280" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="262"/>
+      <c r="Q87" s="281"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -8009,6 +7859,17 @@
   </sheetData>
   <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="23">
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="P86:Q86"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="M84:N84"/>
     <mergeCell ref="A1:R6"/>
     <mergeCell ref="P84:Q84"/>
     <mergeCell ref="J82:L82"/>
@@ -8021,38 +7882,27 @@
     <mergeCell ref="P83:Q83"/>
     <mergeCell ref="P82:Q82"/>
     <mergeCell ref="P80:S81"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="P86:Q86"/>
   </mergeCells>
   <conditionalFormatting sqref="T10:T52">
-    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S52">
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S51">
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>$S$12=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8066,7 +7916,7 @@
   <dimension ref="A2:BM266"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" colorId="8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8108,46 +7958,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="288" t="s">
+      <c r="C2" s="316" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="267"/>
-      <c r="E2" s="267"/>
-      <c r="F2" s="267"/>
-      <c r="G2" s="267"/>
-      <c r="H2" s="267"/>
-      <c r="I2" s="267"/>
-      <c r="J2" s="267"/>
-      <c r="K2" s="267"/>
-      <c r="L2" s="267"/>
-      <c r="M2" s="267"/>
-      <c r="N2" s="267"/>
-      <c r="O2" s="267"/>
-      <c r="P2" s="268"/>
-      <c r="Q2" s="268"/>
-      <c r="R2" s="268"/>
-      <c r="S2" s="267"/>
-      <c r="T2" s="267"/>
+      <c r="D2" s="277"/>
+      <c r="E2" s="277"/>
+      <c r="F2" s="277"/>
+      <c r="G2" s="277"/>
+      <c r="H2" s="277"/>
+      <c r="I2" s="277"/>
+      <c r="J2" s="277"/>
+      <c r="K2" s="277"/>
+      <c r="L2" s="277"/>
+      <c r="M2" s="277"/>
+      <c r="N2" s="277"/>
+      <c r="O2" s="277"/>
+      <c r="P2" s="278"/>
+      <c r="Q2" s="278"/>
+      <c r="R2" s="278"/>
+      <c r="S2" s="277"/>
+      <c r="T2" s="277"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="268"/>
-      <c r="D3" s="269"/>
-      <c r="E3" s="269"/>
-      <c r="F3" s="269"/>
-      <c r="G3" s="269"/>
-      <c r="H3" s="269"/>
-      <c r="I3" s="269"/>
-      <c r="J3" s="269"/>
-      <c r="K3" s="269"/>
-      <c r="L3" s="269"/>
-      <c r="M3" s="269"/>
-      <c r="N3" s="269"/>
-      <c r="O3" s="269"/>
-      <c r="P3" s="269"/>
-      <c r="Q3" s="269"/>
-      <c r="R3" s="269"/>
-      <c r="S3" s="269"/>
-      <c r="T3" s="269"/>
+      <c r="C3" s="278"/>
+      <c r="D3" s="279"/>
+      <c r="E3" s="279"/>
+      <c r="F3" s="279"/>
+      <c r="G3" s="279"/>
+      <c r="H3" s="279"/>
+      <c r="I3" s="279"/>
+      <c r="J3" s="279"/>
+      <c r="K3" s="279"/>
+      <c r="L3" s="279"/>
+      <c r="M3" s="279"/>
+      <c r="N3" s="279"/>
+      <c r="O3" s="279"/>
+      <c r="P3" s="279"/>
+      <c r="Q3" s="279"/>
+      <c r="R3" s="279"/>
+      <c r="S3" s="279"/>
+      <c r="T3" s="279"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8155,7 +8005,7 @@
         <v>82</v>
       </c>
       <c r="B4" s="71" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="Q4" s="133"/>
       <c r="R4" s="133"/>
@@ -8234,25 +8084,25 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="294" t="s">
+      <c r="X5" s="308" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="261"/>
-      <c r="Z5" s="261"/>
-      <c r="AA5" s="261"/>
-      <c r="AB5" s="261"/>
-      <c r="AC5" s="261"/>
-      <c r="AD5" s="261"/>
-      <c r="AE5" s="261"/>
-      <c r="AF5" s="261"/>
-      <c r="AG5" s="261"/>
-      <c r="AH5" s="261"/>
-      <c r="AI5" s="261"/>
-      <c r="AJ5" s="261"/>
-      <c r="AK5" s="261"/>
-      <c r="AL5" s="261"/>
-      <c r="AM5" s="261"/>
-      <c r="AN5" s="262"/>
+      <c r="Y5" s="283"/>
+      <c r="Z5" s="283"/>
+      <c r="AA5" s="283"/>
+      <c r="AB5" s="283"/>
+      <c r="AC5" s="283"/>
+      <c r="AD5" s="283"/>
+      <c r="AE5" s="283"/>
+      <c r="AF5" s="283"/>
+      <c r="AG5" s="283"/>
+      <c r="AH5" s="283"/>
+      <c r="AI5" s="283"/>
+      <c r="AJ5" s="283"/>
+      <c r="AK5" s="283"/>
+      <c r="AL5" s="283"/>
+      <c r="AM5" s="283"/>
+      <c r="AN5" s="281"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -8327,29 +8177,29 @@
       <c r="V6" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="X6" s="289" t="s">
+      <c r="X6" s="317" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="289" t="s">
+      <c r="Y6" s="317" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="293" t="s">
+      <c r="Z6" s="306" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="290"/>
-      <c r="AB6" s="290"/>
-      <c r="AC6" s="290"/>
-      <c r="AD6" s="290"/>
-      <c r="AE6" s="290"/>
-      <c r="AF6" s="290"/>
-      <c r="AG6" s="290"/>
-      <c r="AH6" s="290"/>
-      <c r="AI6" s="290"/>
-      <c r="AJ6" s="290"/>
-      <c r="AK6" s="290"/>
-      <c r="AL6" s="290"/>
-      <c r="AM6" s="290"/>
-      <c r="AN6" s="290"/>
+      <c r="AA6" s="307"/>
+      <c r="AB6" s="307"/>
+      <c r="AC6" s="307"/>
+      <c r="AD6" s="307"/>
+      <c r="AE6" s="307"/>
+      <c r="AF6" s="307"/>
+      <c r="AG6" s="307"/>
+      <c r="AH6" s="307"/>
+      <c r="AI6" s="307"/>
+      <c r="AJ6" s="307"/>
+      <c r="AK6" s="307"/>
+      <c r="AL6" s="307"/>
+      <c r="AM6" s="307"/>
+      <c r="AN6" s="307"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -8424,27 +8274,27 @@
       <c r="V7" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="X7" s="290"/>
-      <c r="Y7" s="290"/>
-      <c r="Z7" s="293" t="s">
+      <c r="X7" s="307"/>
+      <c r="Y7" s="307"/>
+      <c r="Z7" s="306" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="290"/>
-      <c r="AB7" s="290"/>
-      <c r="AC7" s="290"/>
-      <c r="AD7" s="293" t="s">
+      <c r="AA7" s="307"/>
+      <c r="AB7" s="307"/>
+      <c r="AC7" s="307"/>
+      <c r="AD7" s="306" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="290"/>
-      <c r="AF7" s="290"/>
-      <c r="AG7" s="290"/>
-      <c r="AH7" s="290"/>
-      <c r="AI7" s="290"/>
-      <c r="AJ7" s="290"/>
-      <c r="AK7" s="290"/>
-      <c r="AL7" s="290"/>
-      <c r="AM7" s="290"/>
-      <c r="AN7" s="290"/>
+      <c r="AE7" s="307"/>
+      <c r="AF7" s="307"/>
+      <c r="AG7" s="307"/>
+      <c r="AH7" s="307"/>
+      <c r="AI7" s="307"/>
+      <c r="AJ7" s="307"/>
+      <c r="AK7" s="307"/>
+      <c r="AL7" s="307"/>
+      <c r="AM7" s="307"/>
+      <c r="AN7" s="307"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -8494,8 +8344,8 @@
         <v>NO</v>
       </c>
       <c r="V8" s="13"/>
-      <c r="X8" s="290"/>
-      <c r="Y8" s="290"/>
+      <c r="X8" s="307"/>
+      <c r="Y8" s="307"/>
       <c r="Z8" s="153" t="s">
         <v>19</v>
       </c>
@@ -8571,15 +8421,23 @@
         <v>20</v>
       </c>
       <c r="J9" s="72">
-        <v>5</v>
-      </c>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
-      <c r="N9" s="72"/>
+        <v>20</v>
+      </c>
+      <c r="K9" s="72">
+        <v>20</v>
+      </c>
+      <c r="L9" s="72">
+        <v>20</v>
+      </c>
+      <c r="M9" s="72">
+        <v>20</v>
+      </c>
+      <c r="N9" s="72">
+        <v>20</v>
+      </c>
       <c r="O9" s="13">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>240</v>
       </c>
       <c r="P9" s="130">
         <f>'2018(NOT UPDATED)'!S13</f>
@@ -8587,23 +8445,23 @@
       </c>
       <c r="Q9" s="131">
         <f t="shared" si="4"/>
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="R9" s="132">
         <f t="shared" si="5"/>
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="S9" s="13">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="T9" s="14">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>-60</v>
       </c>
       <c r="U9" s="15" t="str">
         <f t="shared" si="3"/>
-        <v>NO</v>
+        <v>OK</v>
       </c>
       <c r="V9" s="13"/>
       <c r="X9" s="1">
@@ -10522,7 +10380,9 @@
       <c r="D27" s="73">
         <v>5</v>
       </c>
-      <c r="E27" s="72"/>
+      <c r="E27" s="72">
+        <v>5</v>
+      </c>
       <c r="F27" s="72">
         <v>5</v>
       </c>
@@ -10538,7 +10398,7 @@
       <c r="N27" s="72"/>
       <c r="O27" s="13">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="P27" s="130">
         <f>'2018(NOT UPDATED)'!S31</f>
@@ -10546,19 +10406,19 @@
       </c>
       <c r="Q27" s="131">
         <f t="shared" si="4"/>
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="R27" s="132">
         <f t="shared" si="5"/>
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="S27" s="13">
         <f t="shared" si="1"/>
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="T27" s="14">
         <f t="shared" si="2"/>
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="U27" s="15" t="str">
         <f t="shared" si="3"/>
@@ -11198,37 +11058,47 @@
       <c r="I33" s="72">
         <v>20</v>
       </c>
-      <c r="J33" s="72"/>
-      <c r="K33" s="72"/>
-      <c r="L33" s="72"/>
-      <c r="M33" s="72"/>
-      <c r="N33" s="72"/>
+      <c r="J33" s="72">
+        <v>20</v>
+      </c>
+      <c r="K33" s="72">
+        <v>20</v>
+      </c>
+      <c r="L33" s="72">
+        <v>20</v>
+      </c>
+      <c r="M33" s="72">
+        <v>20</v>
+      </c>
+      <c r="N33" s="72">
+        <v>20</v>
+      </c>
       <c r="O33" s="13">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>240</v>
       </c>
       <c r="P33" s="130">
         <v>0</v>
       </c>
       <c r="Q33" s="131">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R33" s="132">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S33" s="13">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="T33" s="14">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>-60</v>
       </c>
       <c r="U33" s="15" t="str">
         <f t="shared" si="3"/>
-        <v>NO</v>
+        <v>OK</v>
       </c>
       <c r="V33" s="13"/>
       <c r="W33" s="134"/>
@@ -11803,7 +11673,7 @@
       <c r="M38" s="231"/>
       <c r="N38" s="231"/>
       <c r="O38" s="232">
-        <f t="shared" ref="O38:O61" si="9">SUM(C38:N38)</f>
+        <f t="shared" ref="O38:O60" si="9">SUM(C38:N38)</f>
         <v>0</v>
       </c>
       <c r="P38" s="233">
@@ -13086,10 +12956,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="291" t="s">
+      <c r="AA49" s="304" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="292"/>
+      <c r="AB49" s="305"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -13167,12 +13037,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="298" t="s">
+      <c r="AI50" s="300" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="299"/>
-      <c r="AK50" s="299"/>
-      <c r="AL50" s="300"/>
+      <c r="AJ50" s="301"/>
+      <c r="AK50" s="301"/>
+      <c r="AL50" s="302"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -13243,12 +13113,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="295" t="s">
+      <c r="AI51" s="297" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="296"/>
-      <c r="AK51" s="296"/>
-      <c r="AL51" s="297"/>
+      <c r="AJ51" s="298"/>
+      <c r="AK51" s="298"/>
+      <c r="AL51" s="299"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -13514,14 +13384,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="301"/>
-      <c r="AD55" s="301"/>
-      <c r="AI55" s="298" t="s">
+      <c r="AC55" s="303"/>
+      <c r="AD55" s="303"/>
+      <c r="AI55" s="300" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="299"/>
-      <c r="AK55" s="299"/>
-      <c r="AL55" s="300"/>
+      <c r="AJ55" s="301"/>
+      <c r="AK55" s="301"/>
+      <c r="AL55" s="302"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -13582,12 +13452,12 @@
         <v>NO</v>
       </c>
       <c r="V56" s="2"/>
-      <c r="AI56" s="280" t="s">
+      <c r="AI56" s="296" t="s">
         <v>168</v>
       </c>
-      <c r="AJ56" s="280"/>
-      <c r="AK56" s="280"/>
-      <c r="AL56" s="280"/>
+      <c r="AJ56" s="296"/>
+      <c r="AK56" s="296"/>
+      <c r="AL56" s="296"/>
       <c r="AM56" s="52">
         <f>AM50-AM55</f>
         <v>450000</v>
@@ -13693,35 +13563,35 @@
       <c r="A59" s="23">
         <v>57</v>
       </c>
-      <c r="B59" s="411" t="s">
+      <c r="B59" s="260" t="s">
         <v>205</v>
       </c>
-      <c r="C59" s="412"/>
-      <c r="D59" s="412"/>
-      <c r="E59" s="412"/>
-      <c r="F59" s="412"/>
-      <c r="G59" s="412"/>
-      <c r="H59" s="412"/>
-      <c r="I59" s="412"/>
-      <c r="J59" s="412"/>
-      <c r="K59" s="412"/>
-      <c r="L59" s="412"/>
-      <c r="M59" s="412"/>
-      <c r="N59" s="412"/>
-      <c r="O59" s="413">
+      <c r="C59" s="261"/>
+      <c r="D59" s="261"/>
+      <c r="E59" s="261"/>
+      <c r="F59" s="261"/>
+      <c r="G59" s="261"/>
+      <c r="H59" s="261"/>
+      <c r="I59" s="261"/>
+      <c r="J59" s="261"/>
+      <c r="K59" s="261"/>
+      <c r="L59" s="261"/>
+      <c r="M59" s="261"/>
+      <c r="N59" s="261"/>
+      <c r="O59" s="262">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="P59" s="414"/>
-      <c r="Q59" s="415">
+      <c r="P59" s="263"/>
+      <c r="Q59" s="264">
         <f t="shared" si="4"/>
         <v>240</v>
       </c>
-      <c r="R59" s="416">
+      <c r="R59" s="265">
         <f t="shared" si="5"/>
         <v>240</v>
       </c>
-      <c r="S59" s="413">
+      <c r="S59" s="262">
         <f t="shared" si="10"/>
         <v>240</v>
       </c>
@@ -13729,20 +13599,20 @@
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="U59" s="417" t="str">
+      <c r="U59" s="266" t="str">
         <f t="shared" si="3"/>
         <v>NO</v>
       </c>
-      <c r="V59" s="418"/>
+      <c r="V59" s="267"/>
     </row>
     <row r="60" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="148">
         <v>58</v>
       </c>
-      <c r="B60" s="419" t="s">
+      <c r="B60" s="268" t="s">
         <v>326</v>
       </c>
-      <c r="C60" s="420">
+      <c r="C60" s="269">
         <v>6</v>
       </c>
       <c r="D60" s="259"/>
@@ -13756,32 +13626,32 @@
       <c r="L60" s="259"/>
       <c r="M60" s="259"/>
       <c r="N60" s="259"/>
-      <c r="O60" s="421">
+      <c r="O60" s="270">
         <f t="shared" si="9"/>
         <v>6</v>
       </c>
-      <c r="P60" s="422"/>
-      <c r="Q60" s="423">
+      <c r="P60" s="271"/>
+      <c r="Q60" s="272">
         <f t="shared" si="4"/>
         <v>234</v>
       </c>
-      <c r="R60" s="424">
+      <c r="R60" s="273">
         <f t="shared" si="5"/>
         <v>234</v>
       </c>
-      <c r="S60" s="421">
+      <c r="S60" s="270">
         <f t="shared" si="10"/>
         <v>234</v>
       </c>
-      <c r="T60" s="425">
+      <c r="T60" s="274">
         <f t="shared" si="2"/>
         <v>174</v>
       </c>
-      <c r="U60" s="426" t="str">
+      <c r="U60" s="275" t="str">
         <f t="shared" si="3"/>
         <v>NO</v>
       </c>
-      <c r="V60" s="419"/>
+      <c r="V60" s="268"/>
     </row>
     <row r="61" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="148">
@@ -13805,24 +13675,24 @@
       <c r="M61" s="206"/>
       <c r="N61" s="206"/>
       <c r="O61" s="206"/>
-      <c r="P61" s="422"/>
-      <c r="Q61" s="423">
+      <c r="P61" s="271"/>
+      <c r="Q61" s="272">
         <f t="shared" si="4"/>
         <v>235</v>
       </c>
-      <c r="R61" s="424">
+      <c r="R61" s="273">
         <f t="shared" si="5"/>
         <v>235</v>
       </c>
-      <c r="S61" s="421">
+      <c r="S61" s="270">
         <f t="shared" si="10"/>
         <v>240</v>
       </c>
-      <c r="T61" s="425">
+      <c r="T61" s="274">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="U61" s="426" t="str">
+      <c r="U61" s="275" t="str">
         <f t="shared" si="3"/>
         <v>NO</v>
       </c>
@@ -13836,32 +13706,32 @@
     <row r="67" spans="3:19" s="258" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="281" t="s">
+      <c r="C69" s="309" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="282"/>
-      <c r="E69" s="282"/>
-      <c r="F69" s="282"/>
-      <c r="G69" s="283"/>
-      <c r="I69" s="287" t="s">
+      <c r="D69" s="310"/>
+      <c r="E69" s="310"/>
+      <c r="F69" s="310"/>
+      <c r="G69" s="311"/>
+      <c r="I69" s="315" t="s">
         <v>178</v>
       </c>
-      <c r="J69" s="287"/>
-      <c r="K69" s="287"/>
-      <c r="L69" s="287"/>
-      <c r="M69" s="287"/>
+      <c r="J69" s="315"/>
+      <c r="K69" s="315"/>
+      <c r="L69" s="315"/>
+      <c r="M69" s="315"/>
     </row>
     <row r="70" spans="3:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="284"/>
-      <c r="D70" s="285"/>
-      <c r="E70" s="285"/>
-      <c r="F70" s="285"/>
-      <c r="G70" s="286"/>
-      <c r="I70" s="287"/>
-      <c r="J70" s="287"/>
-      <c r="K70" s="287"/>
-      <c r="L70" s="287"/>
-      <c r="M70" s="287"/>
+      <c r="C70" s="312"/>
+      <c r="D70" s="313"/>
+      <c r="E70" s="313"/>
+      <c r="F70" s="313"/>
+      <c r="G70" s="314"/>
+      <c r="I70" s="315"/>
+      <c r="J70" s="315"/>
+      <c r="K70" s="315"/>
+      <c r="L70" s="315"/>
+      <c r="M70" s="315"/>
     </row>
     <row r="71" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13882,10 +13752,10 @@
       <c r="M76" s="55"/>
       <c r="N76" s="55"/>
       <c r="O76" s="55"/>
-      <c r="P76" s="280" t="s">
+      <c r="P76" s="296" t="s">
         <v>214</v>
       </c>
-      <c r="Q76" s="280"/>
+      <c r="Q76" s="296"/>
       <c r="R76" s="55"/>
       <c r="S76" s="55"/>
     </row>
@@ -14352,73 +14222,73 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AI56:AL56"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AI50:AL50"/>
-    <mergeCell ref="AI55:AL55"/>
-    <mergeCell ref="AC55:AD55"/>
-    <mergeCell ref="AA49:AB49"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="AD7:AN7"/>
-    <mergeCell ref="X5:AN5"/>
-    <mergeCell ref="Z6:AN6"/>
     <mergeCell ref="P76:Q76"/>
     <mergeCell ref="C69:G70"/>
     <mergeCell ref="I69:M70"/>
     <mergeCell ref="C2:T3"/>
     <mergeCell ref="Y6:Y8"/>
     <mergeCell ref="X6:X8"/>
+    <mergeCell ref="AA49:AB49"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="AD7:AN7"/>
+    <mergeCell ref="X5:AN5"/>
+    <mergeCell ref="Z6:AN6"/>
+    <mergeCell ref="AI56:AL56"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AI50:AL50"/>
+    <mergeCell ref="AI55:AL55"/>
+    <mergeCell ref="AC55:AD55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:V61">
-    <cfRule type="expression" dxfId="22" priority="7">
+    <cfRule type="expression" dxfId="12" priority="7">
       <formula>IF(ISBLANK($B$4), 0, SEARCH($B$4,$B6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK48">
-    <cfRule type="containsText" dxfId="21" priority="8" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH(("YES"),(AK9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK48">
-    <cfRule type="containsText" dxfId="20" priority="9" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH(("NO"),(AK9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y9:AN9 Y46:AC46 AD46:AL48 AC47:AC48 Y10:AL45 AM10:AN48">
-    <cfRule type="expression" dxfId="19" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>IF(ISBLANK($Z$4), 0, SEARCH($Z$4,$Y9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6:U61">
-    <cfRule type="containsText" dxfId="18" priority="11" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH(("NO"),(U6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6:U61">
-    <cfRule type="containsText" dxfId="17" priority="12" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH(("OK"),(U6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y10:Y45">
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>IF(AK10="YES",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q6:R61">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6:P61">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y9:AN48">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>IF(ISBLANK($AA$4), 0, SEARCH($AA$4,$Y9))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14432,7 +14302,7 @@
   <dimension ref="A2:W36"/>
   <sheetViews>
     <sheetView topLeftCell="L8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14452,86 +14322,86 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="302" t="s">
+      <c r="A2" s="318" t="s">
         <v>301</v>
       </c>
-      <c r="B2" s="302"/>
-      <c r="C2" s="302"/>
-      <c r="D2" s="302"/>
-      <c r="E2" s="302"/>
-      <c r="F2" s="302"/>
-      <c r="G2" s="302"/>
-      <c r="H2" s="302"/>
-      <c r="I2" s="302"/>
-      <c r="J2" s="302"/>
-      <c r="K2" s="302"/>
-      <c r="L2" s="302"/>
+      <c r="B2" s="318"/>
+      <c r="C2" s="318"/>
+      <c r="D2" s="318"/>
+      <c r="E2" s="318"/>
+      <c r="F2" s="318"/>
+      <c r="G2" s="318"/>
+      <c r="H2" s="318"/>
+      <c r="I2" s="318"/>
+      <c r="J2" s="318"/>
+      <c r="K2" s="318"/>
+      <c r="L2" s="318"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="302"/>
-      <c r="B3" s="302"/>
-      <c r="C3" s="302"/>
-      <c r="D3" s="302"/>
-      <c r="E3" s="302"/>
-      <c r="F3" s="302"/>
-      <c r="G3" s="302"/>
-      <c r="H3" s="302"/>
-      <c r="I3" s="302"/>
-      <c r="J3" s="302"/>
-      <c r="K3" s="302"/>
-      <c r="L3" s="302"/>
+      <c r="A3" s="318"/>
+      <c r="B3" s="318"/>
+      <c r="C3" s="318"/>
+      <c r="D3" s="318"/>
+      <c r="E3" s="318"/>
+      <c r="F3" s="318"/>
+      <c r="G3" s="318"/>
+      <c r="H3" s="318"/>
+      <c r="I3" s="318"/>
+      <c r="J3" s="318"/>
+      <c r="K3" s="318"/>
+      <c r="L3" s="318"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="287" t="s">
+      <c r="A5" s="315" t="s">
         <v>304</v>
       </c>
-      <c r="B5" s="287"/>
-      <c r="C5" s="287"/>
-      <c r="D5" s="287"/>
-      <c r="E5" s="287"/>
-      <c r="F5" s="287"/>
-      <c r="G5" s="287"/>
-      <c r="H5" s="287"/>
-      <c r="I5" s="287"/>
-      <c r="J5" s="287"/>
-      <c r="K5" s="287"/>
-      <c r="M5" s="287" t="s">
+      <c r="B5" s="315"/>
+      <c r="C5" s="315"/>
+      <c r="D5" s="315"/>
+      <c r="E5" s="315"/>
+      <c r="F5" s="315"/>
+      <c r="G5" s="315"/>
+      <c r="H5" s="315"/>
+      <c r="I5" s="315"/>
+      <c r="J5" s="315"/>
+      <c r="K5" s="315"/>
+      <c r="M5" s="315" t="s">
         <v>325</v>
       </c>
-      <c r="N5" s="287"/>
-      <c r="O5" s="287"/>
-      <c r="P5" s="287"/>
-      <c r="Q5" s="287"/>
-      <c r="R5" s="287"/>
-      <c r="S5" s="287"/>
-      <c r="T5" s="287"/>
-      <c r="U5" s="287"/>
-      <c r="V5" s="287"/>
-      <c r="W5" s="287"/>
+      <c r="N5" s="315"/>
+      <c r="O5" s="315"/>
+      <c r="P5" s="315"/>
+      <c r="Q5" s="315"/>
+      <c r="R5" s="315"/>
+      <c r="S5" s="315"/>
+      <c r="T5" s="315"/>
+      <c r="U5" s="315"/>
+      <c r="V5" s="315"/>
+      <c r="W5" s="315"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="287"/>
-      <c r="B6" s="287"/>
-      <c r="C6" s="287"/>
-      <c r="D6" s="287"/>
-      <c r="E6" s="287"/>
-      <c r="F6" s="287"/>
-      <c r="G6" s="287"/>
-      <c r="H6" s="287"/>
-      <c r="I6" s="287"/>
-      <c r="J6" s="287"/>
-      <c r="K6" s="287"/>
-      <c r="M6" s="287"/>
-      <c r="N6" s="287"/>
-      <c r="O6" s="287"/>
-      <c r="P6" s="287"/>
-      <c r="Q6" s="287"/>
-      <c r="R6" s="287"/>
-      <c r="S6" s="287"/>
-      <c r="T6" s="287"/>
-      <c r="U6" s="287"/>
-      <c r="V6" s="287"/>
-      <c r="W6" s="287"/>
+      <c r="A6" s="315"/>
+      <c r="B6" s="315"/>
+      <c r="C6" s="315"/>
+      <c r="D6" s="315"/>
+      <c r="E6" s="315"/>
+      <c r="F6" s="315"/>
+      <c r="G6" s="315"/>
+      <c r="H6" s="315"/>
+      <c r="I6" s="315"/>
+      <c r="J6" s="315"/>
+      <c r="K6" s="315"/>
+      <c r="M6" s="315"/>
+      <c r="N6" s="315"/>
+      <c r="O6" s="315"/>
+      <c r="P6" s="315"/>
+      <c r="Q6" s="315"/>
+      <c r="R6" s="315"/>
+      <c r="S6" s="315"/>
+      <c r="T6" s="315"/>
+      <c r="U6" s="315"/>
+      <c r="V6" s="315"/>
+      <c r="W6" s="315"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M7" s="251"/>
@@ -15144,9 +15014,15 @@
       <c r="N24" s="1">
         <v>16</v>
       </c>
-      <c r="O24" s="218"/>
-      <c r="P24" s="252"/>
-      <c r="Q24" s="213"/>
+      <c r="O24" s="218" t="s">
+        <v>345</v>
+      </c>
+      <c r="P24" s="252" t="s">
+        <v>342</v>
+      </c>
+      <c r="Q24" s="213">
+        <v>95000</v>
+      </c>
       <c r="R24" s="212"/>
       <c r="S24" s="251"/>
       <c r="T24" s="251"/>
@@ -15174,9 +15050,15 @@
       <c r="N25" s="1">
         <v>17</v>
       </c>
-      <c r="O25" s="218"/>
-      <c r="P25" s="252"/>
-      <c r="Q25" s="212"/>
+      <c r="O25" s="218" t="s">
+        <v>345</v>
+      </c>
+      <c r="P25" s="252" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q25" s="212">
+        <v>5000</v>
+      </c>
       <c r="R25" s="212"/>
       <c r="S25" s="251"/>
       <c r="T25" s="251"/>
@@ -15204,9 +15086,15 @@
       <c r="N26" s="1">
         <v>18</v>
       </c>
-      <c r="O26" s="218"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="212"/>
+      <c r="O26" s="218" t="s">
+        <v>345</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="Q26" s="212">
+        <v>100000</v>
+      </c>
       <c r="R26" s="212"/>
       <c r="S26" s="251"/>
       <c r="T26" s="251"/>
@@ -15404,7 +15292,7 @@
       </c>
       <c r="Q34" s="225">
         <f>SUM(Q9:Q33)</f>
-        <v>3381144.27</v>
+        <v>3581144.27</v>
       </c>
       <c r="R34" s="226">
         <f>SUM(R9:R33)</f>
@@ -15417,27 +15305,27 @@
       <c r="W34" s="251"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B35" s="307" t="s">
+      <c r="B35" s="323" t="s">
         <v>313</v>
       </c>
-      <c r="C35" s="308"/>
-      <c r="D35" s="309"/>
-      <c r="E35" s="303">
+      <c r="C35" s="324"/>
+      <c r="D35" s="325"/>
+      <c r="E35" s="319">
         <f>E34-F34</f>
         <v>2610871.1799999997</v>
       </c>
-      <c r="F35" s="304"/>
+      <c r="F35" s="320"/>
       <c r="M35" s="251"/>
-      <c r="N35" s="307" t="s">
+      <c r="N35" s="323" t="s">
         <v>313</v>
       </c>
-      <c r="O35" s="308"/>
-      <c r="P35" s="309"/>
-      <c r="Q35" s="303">
+      <c r="O35" s="324"/>
+      <c r="P35" s="325"/>
+      <c r="Q35" s="319">
         <f>Q34-R34</f>
-        <v>3306144.27</v>
-      </c>
-      <c r="R35" s="304"/>
+        <v>3506144.27</v>
+      </c>
+      <c r="R35" s="320"/>
       <c r="S35" s="251"/>
       <c r="T35" s="251"/>
       <c r="U35" s="251"/>
@@ -15445,17 +15333,17 @@
       <c r="W35" s="251"/>
     </row>
     <row r="36" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="310"/>
-      <c r="C36" s="311"/>
-      <c r="D36" s="312"/>
-      <c r="E36" s="305"/>
-      <c r="F36" s="306"/>
+      <c r="B36" s="326"/>
+      <c r="C36" s="327"/>
+      <c r="D36" s="328"/>
+      <c r="E36" s="321"/>
+      <c r="F36" s="322"/>
       <c r="M36" s="251"/>
-      <c r="N36" s="310"/>
-      <c r="O36" s="311"/>
-      <c r="P36" s="312"/>
-      <c r="Q36" s="305"/>
-      <c r="R36" s="306"/>
+      <c r="N36" s="326"/>
+      <c r="O36" s="327"/>
+      <c r="P36" s="328"/>
+      <c r="Q36" s="321"/>
+      <c r="R36" s="322"/>
       <c r="S36" s="251"/>
       <c r="T36" s="251"/>
       <c r="U36" s="251"/>
@@ -15504,17 +15392,17 @@
       <c r="A2" s="174"/>
       <c r="B2" s="175"/>
       <c r="C2" s="175"/>
-      <c r="D2" s="370" t="s">
+      <c r="D2" s="329" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="370"/>
-      <c r="F2" s="370"/>
-      <c r="G2" s="370"/>
-      <c r="H2" s="370"/>
-      <c r="I2" s="370"/>
-      <c r="J2" s="370"/>
-      <c r="K2" s="370"/>
-      <c r="L2" s="370"/>
+      <c r="E2" s="329"/>
+      <c r="F2" s="329"/>
+      <c r="G2" s="329"/>
+      <c r="H2" s="329"/>
+      <c r="I2" s="329"/>
+      <c r="J2" s="329"/>
+      <c r="K2" s="329"/>
+      <c r="L2" s="329"/>
       <c r="M2" s="176"/>
       <c r="N2" s="24"/>
     </row>
@@ -15532,205 +15420,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="178"/>
-      <c r="U3" s="313" t="s">
+      <c r="U3" s="379" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="314"/>
-      <c r="W3" s="315" t="s">
+      <c r="V3" s="380"/>
+      <c r="W3" s="381" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="314"/>
-      <c r="Y3" s="314"/>
-      <c r="Z3" s="314"/>
-      <c r="AA3" s="314"/>
-      <c r="AB3" s="314"/>
-      <c r="AC3" s="314"/>
-      <c r="AD3" s="316"/>
+      <c r="X3" s="380"/>
+      <c r="Y3" s="380"/>
+      <c r="Z3" s="380"/>
+      <c r="AA3" s="380"/>
+      <c r="AB3" s="380"/>
+      <c r="AC3" s="380"/>
+      <c r="AD3" s="382"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="177"/>
-      <c r="B4" s="374" t="s">
+      <c r="B4" s="344" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="375"/>
-      <c r="D4" s="375"/>
-      <c r="E4" s="375"/>
-      <c r="F4" s="375"/>
+      <c r="C4" s="345"/>
+      <c r="D4" s="345"/>
+      <c r="E4" s="345"/>
+      <c r="F4" s="345"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="322" t="s">
+      <c r="I4" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="293"/>
-      <c r="K4" s="293"/>
-      <c r="L4" s="293"/>
+      <c r="J4" s="306"/>
+      <c r="K4" s="306"/>
+      <c r="L4" s="306"/>
       <c r="M4" s="178"/>
-      <c r="U4" s="334" t="s">
+      <c r="U4" s="391" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="293"/>
-      <c r="W4" s="322" t="s">
+      <c r="V4" s="306"/>
+      <c r="W4" s="348" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="293"/>
-      <c r="Y4" s="293"/>
-      <c r="Z4" s="293"/>
-      <c r="AA4" s="293"/>
-      <c r="AB4" s="293"/>
-      <c r="AC4" s="293"/>
-      <c r="AD4" s="317"/>
+      <c r="X4" s="306"/>
+      <c r="Y4" s="306"/>
+      <c r="Z4" s="306"/>
+      <c r="AA4" s="306"/>
+      <c r="AB4" s="306"/>
+      <c r="AC4" s="306"/>
+      <c r="AD4" s="368"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="177"/>
       <c r="B5" s="339" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="293"/>
-      <c r="D5" s="293"/>
-      <c r="E5" s="293"/>
-      <c r="F5" s="293"/>
+      <c r="C5" s="306"/>
+      <c r="D5" s="306"/>
+      <c r="E5" s="306"/>
+      <c r="F5" s="306"/>
       <c r="G5" s="154">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="341" t="s">
+      <c r="I5" s="337" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="362"/>
-      <c r="K5" s="364">
+      <c r="J5" s="338"/>
+      <c r="K5" s="349">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="365"/>
+      <c r="L5" s="350"/>
       <c r="M5" s="178"/>
-      <c r="U5" s="335" t="s">
+      <c r="U5" s="375" t="s">
         <v>231</v>
       </c>
-      <c r="V5" s="336"/>
-      <c r="W5" s="341" t="s">
+      <c r="V5" s="376"/>
+      <c r="W5" s="337" t="s">
         <v>232</v>
       </c>
-      <c r="X5" s="342"/>
-      <c r="Y5" s="342"/>
-      <c r="Z5" s="342"/>
-      <c r="AA5" s="342"/>
-      <c r="AB5" s="342"/>
-      <c r="AC5" s="342"/>
-      <c r="AD5" s="343"/>
+      <c r="X5" s="362"/>
+      <c r="Y5" s="362"/>
+      <c r="Z5" s="362"/>
+      <c r="AA5" s="362"/>
+      <c r="AB5" s="362"/>
+      <c r="AC5" s="362"/>
+      <c r="AD5" s="363"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="177"/>
-      <c r="B6" s="332" t="s">
+      <c r="B6" s="331" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="333"/>
-      <c r="D6" s="333"/>
-      <c r="E6" s="333"/>
-      <c r="F6" s="333"/>
+      <c r="C6" s="332"/>
+      <c r="D6" s="332"/>
+      <c r="E6" s="332"/>
+      <c r="F6" s="332"/>
       <c r="G6" s="154">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="363" t="s">
+      <c r="I6" s="335" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="358"/>
-      <c r="K6" s="366">
+      <c r="J6" s="336"/>
+      <c r="K6" s="351">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="367"/>
+      <c r="L6" s="352"/>
       <c r="M6" s="178"/>
-      <c r="U6" s="337"/>
-      <c r="V6" s="338"/>
-      <c r="W6" s="323" t="s">
+      <c r="U6" s="377"/>
+      <c r="V6" s="378"/>
+      <c r="W6" s="364" t="s">
         <v>233</v>
       </c>
-      <c r="X6" s="324"/>
-      <c r="Y6" s="324"/>
-      <c r="Z6" s="324"/>
-      <c r="AA6" s="324"/>
-      <c r="AB6" s="324"/>
-      <c r="AC6" s="324"/>
-      <c r="AD6" s="325"/>
+      <c r="X6" s="365"/>
+      <c r="Y6" s="365"/>
+      <c r="Z6" s="365"/>
+      <c r="AA6" s="365"/>
+      <c r="AB6" s="365"/>
+      <c r="AC6" s="365"/>
+      <c r="AD6" s="366"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="177"/>
-      <c r="B7" s="344" t="s">
+      <c r="B7" s="342" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="345"/>
-      <c r="D7" s="345"/>
-      <c r="E7" s="345"/>
-      <c r="F7" s="358"/>
+      <c r="C7" s="343"/>
+      <c r="D7" s="343"/>
+      <c r="E7" s="343"/>
+      <c r="F7" s="336"/>
       <c r="G7" s="154">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="363" t="s">
+      <c r="I7" s="335" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="358"/>
-      <c r="K7" s="368">
+      <c r="J7" s="336"/>
+      <c r="K7" s="346">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="369"/>
+      <c r="L7" s="347"/>
       <c r="M7" s="178"/>
-      <c r="U7" s="320"/>
-      <c r="V7" s="321"/>
-      <c r="W7" s="322" t="s">
+      <c r="U7" s="383"/>
+      <c r="V7" s="384"/>
+      <c r="W7" s="348" t="s">
         <v>234</v>
       </c>
-      <c r="X7" s="293"/>
-      <c r="Y7" s="293"/>
-      <c r="Z7" s="293"/>
-      <c r="AA7" s="293"/>
-      <c r="AB7" s="293"/>
-      <c r="AC7" s="293"/>
-      <c r="AD7" s="317"/>
+      <c r="X7" s="306"/>
+      <c r="Y7" s="306"/>
+      <c r="Z7" s="306"/>
+      <c r="AA7" s="306"/>
+      <c r="AB7" s="306"/>
+      <c r="AC7" s="306"/>
+      <c r="AD7" s="368"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="177"/>
-      <c r="B8" s="372" t="s">
+      <c r="B8" s="340" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="373"/>
-      <c r="D8" s="373"/>
-      <c r="E8" s="373"/>
-      <c r="F8" s="373"/>
+      <c r="C8" s="341"/>
+      <c r="D8" s="341"/>
+      <c r="E8" s="341"/>
+      <c r="F8" s="341"/>
       <c r="G8" s="155">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="341" t="s">
+      <c r="I8" s="337" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="362"/>
-      <c r="K8" s="353">
+      <c r="J8" s="338"/>
+      <c r="K8" s="333">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="354"/>
+      <c r="L8" s="334"/>
       <c r="M8" s="178"/>
-      <c r="U8" s="328" t="s">
+      <c r="U8" s="387" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="329"/>
-      <c r="W8" s="323" t="s">
+      <c r="V8" s="388"/>
+      <c r="W8" s="364" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="324"/>
-      <c r="Y8" s="324"/>
-      <c r="Z8" s="324"/>
-      <c r="AA8" s="324"/>
-      <c r="AB8" s="324"/>
-      <c r="AC8" s="324"/>
-      <c r="AD8" s="325"/>
+      <c r="X8" s="365"/>
+      <c r="Y8" s="365"/>
+      <c r="Z8" s="365"/>
+      <c r="AA8" s="365"/>
+      <c r="AB8" s="365"/>
+      <c r="AC8" s="365"/>
+      <c r="AD8" s="366"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="177"/>
@@ -15746,28 +15634,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="178"/>
-      <c r="U9" s="330"/>
-      <c r="V9" s="331"/>
-      <c r="W9" s="323" t="s">
+      <c r="U9" s="389"/>
+      <c r="V9" s="390"/>
+      <c r="W9" s="364" t="s">
         <v>237</v>
       </c>
-      <c r="X9" s="324"/>
-      <c r="Y9" s="324"/>
-      <c r="Z9" s="324"/>
-      <c r="AA9" s="324"/>
-      <c r="AB9" s="324"/>
-      <c r="AC9" s="324"/>
-      <c r="AD9" s="325"/>
+      <c r="X9" s="365"/>
+      <c r="Y9" s="365"/>
+      <c r="Z9" s="365"/>
+      <c r="AA9" s="365"/>
+      <c r="AB9" s="365"/>
+      <c r="AC9" s="365"/>
+      <c r="AD9" s="366"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="177"/>
-      <c r="B10" s="293" t="s">
+      <c r="B10" s="306" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="293"/>
-      <c r="D10" s="293"/>
-      <c r="E10" s="293"/>
-      <c r="F10" s="293"/>
+      <c r="C10" s="306"/>
+      <c r="D10" s="306"/>
+      <c r="E10" s="306"/>
+      <c r="F10" s="306"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -15778,30 +15666,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="178"/>
-      <c r="U10" s="332" t="s">
+      <c r="U10" s="331" t="s">
         <v>243</v>
       </c>
-      <c r="V10" s="333"/>
-      <c r="W10" s="293" t="s">
+      <c r="V10" s="332"/>
+      <c r="W10" s="306" t="s">
         <v>257</v>
       </c>
-      <c r="X10" s="293"/>
-      <c r="Y10" s="293"/>
-      <c r="Z10" s="293"/>
-      <c r="AA10" s="293"/>
-      <c r="AB10" s="293"/>
-      <c r="AC10" s="293"/>
-      <c r="AD10" s="317"/>
+      <c r="X10" s="306"/>
+      <c r="Y10" s="306"/>
+      <c r="Z10" s="306"/>
+      <c r="AA10" s="306"/>
+      <c r="AB10" s="306"/>
+      <c r="AC10" s="306"/>
+      <c r="AD10" s="368"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="177"/>
-      <c r="B11" s="293" t="s">
+      <c r="B11" s="306" t="s">
         <v>254</v>
       </c>
-      <c r="C11" s="293"/>
-      <c r="D11" s="293"/>
-      <c r="E11" s="293"/>
-      <c r="F11" s="293"/>
+      <c r="C11" s="306"/>
+      <c r="D11" s="306"/>
+      <c r="E11" s="306"/>
+      <c r="F11" s="306"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -15811,30 +15699,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="178"/>
-      <c r="U11" s="332" t="s">
+      <c r="U11" s="331" t="s">
         <v>256</v>
       </c>
-      <c r="V11" s="333"/>
-      <c r="W11" s="326" t="s">
+      <c r="V11" s="332"/>
+      <c r="W11" s="385" t="s">
         <v>258</v>
       </c>
-      <c r="X11" s="326"/>
-      <c r="Y11" s="326"/>
-      <c r="Z11" s="326"/>
-      <c r="AA11" s="326"/>
-      <c r="AB11" s="326"/>
-      <c r="AC11" s="326"/>
-      <c r="AD11" s="327"/>
+      <c r="X11" s="385"/>
+      <c r="Y11" s="385"/>
+      <c r="Z11" s="385"/>
+      <c r="AA11" s="385"/>
+      <c r="AB11" s="385"/>
+      <c r="AC11" s="385"/>
+      <c r="AD11" s="386"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="177"/>
-      <c r="B12" s="371" t="s">
+      <c r="B12" s="330" t="s">
         <v>255</v>
       </c>
-      <c r="C12" s="371"/>
-      <c r="D12" s="371"/>
-      <c r="E12" s="371"/>
-      <c r="F12" s="371"/>
+      <c r="C12" s="330"/>
+      <c r="D12" s="330"/>
+      <c r="E12" s="330"/>
+      <c r="F12" s="330"/>
       <c r="G12" s="182">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -15845,16 +15733,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="178"/>
-      <c r="U12" s="332"/>
-      <c r="V12" s="333"/>
-      <c r="W12" s="293"/>
-      <c r="X12" s="293"/>
-      <c r="Y12" s="293"/>
-      <c r="Z12" s="293"/>
-      <c r="AA12" s="293"/>
-      <c r="AB12" s="293"/>
-      <c r="AC12" s="293"/>
-      <c r="AD12" s="317"/>
+      <c r="U12" s="331"/>
+      <c r="V12" s="332"/>
+      <c r="W12" s="306"/>
+      <c r="X12" s="306"/>
+      <c r="Y12" s="306"/>
+      <c r="Z12" s="306"/>
+      <c r="AA12" s="306"/>
+      <c r="AB12" s="306"/>
+      <c r="AC12" s="306"/>
+      <c r="AD12" s="368"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="179"/>
@@ -15870,53 +15758,53 @@
       <c r="K13" s="180"/>
       <c r="L13" s="180"/>
       <c r="M13" s="181"/>
-      <c r="U13" s="332"/>
-      <c r="V13" s="333"/>
-      <c r="W13" s="293"/>
-      <c r="X13" s="293"/>
-      <c r="Y13" s="293"/>
-      <c r="Z13" s="293"/>
-      <c r="AA13" s="293"/>
-      <c r="AB13" s="293"/>
-      <c r="AC13" s="293"/>
-      <c r="AD13" s="317"/>
+      <c r="U13" s="331"/>
+      <c r="V13" s="332"/>
+      <c r="W13" s="306"/>
+      <c r="X13" s="306"/>
+      <c r="Y13" s="306"/>
+      <c r="Z13" s="306"/>
+      <c r="AA13" s="306"/>
+      <c r="AB13" s="306"/>
+      <c r="AC13" s="306"/>
+      <c r="AD13" s="368"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="347"/>
-      <c r="V14" s="348"/>
-      <c r="W14" s="318"/>
-      <c r="X14" s="318"/>
-      <c r="Y14" s="318"/>
-      <c r="Z14" s="318"/>
-      <c r="AA14" s="318"/>
-      <c r="AB14" s="318"/>
-      <c r="AC14" s="318"/>
-      <c r="AD14" s="319"/>
+      <c r="U14" s="369"/>
+      <c r="V14" s="370"/>
+      <c r="W14" s="360"/>
+      <c r="X14" s="360"/>
+      <c r="Y14" s="360"/>
+      <c r="Z14" s="360"/>
+      <c r="AA14" s="360"/>
+      <c r="AB14" s="360"/>
+      <c r="AC14" s="360"/>
+      <c r="AD14" s="361"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="174"/>
       <c r="B18" s="175"/>
       <c r="C18" s="175"/>
-      <c r="D18" s="370" t="s">
+      <c r="D18" s="329" t="s">
         <v>249</v>
       </c>
-      <c r="E18" s="370"/>
-      <c r="F18" s="370"/>
-      <c r="G18" s="370"/>
-      <c r="H18" s="370"/>
-      <c r="I18" s="370"/>
-      <c r="J18" s="370"/>
-      <c r="K18" s="370"/>
-      <c r="L18" s="370"/>
+      <c r="E18" s="329"/>
+      <c r="F18" s="329"/>
+      <c r="G18" s="329"/>
+      <c r="H18" s="329"/>
+      <c r="I18" s="329"/>
+      <c r="J18" s="329"/>
+      <c r="K18" s="329"/>
+      <c r="L18" s="329"/>
       <c r="M18" s="176"/>
-      <c r="O18" s="349" t="s">
+      <c r="O18" s="371" t="s">
         <v>250</v>
       </c>
-      <c r="P18" s="350"/>
-      <c r="Q18" s="350"/>
-      <c r="R18" s="350"/>
-      <c r="S18" s="351"/>
+      <c r="P18" s="372"/>
+      <c r="Q18" s="372"/>
+      <c r="R18" s="372"/>
+      <c r="S18" s="373"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="177"/>
@@ -15924,10 +15812,10 @@
       <c r="O19" s="339" t="s">
         <v>251</v>
       </c>
-      <c r="P19" s="293"/>
-      <c r="Q19" s="293"/>
-      <c r="R19" s="293"/>
-      <c r="S19" s="317"/>
+      <c r="P19" s="306"/>
+      <c r="Q19" s="306"/>
+      <c r="R19" s="306"/>
+      <c r="S19" s="368"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="177"/>
@@ -15938,119 +15826,119 @@
       <c r="F20" s="202"/>
       <c r="G20" s="68"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="322" t="s">
+      <c r="I20" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="293"/>
-      <c r="K20" s="293"/>
-      <c r="L20" s="293"/>
+      <c r="J20" s="306"/>
+      <c r="K20" s="306"/>
+      <c r="L20" s="306"/>
       <c r="M20" s="178"/>
       <c r="O20" s="339" t="s">
         <v>252</v>
       </c>
-      <c r="P20" s="293"/>
-      <c r="Q20" s="293"/>
-      <c r="R20" s="293"/>
-      <c r="S20" s="317"/>
+      <c r="P20" s="306"/>
+      <c r="Q20" s="306"/>
+      <c r="R20" s="306"/>
+      <c r="S20" s="368"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="177"/>
-      <c r="B21" s="355" t="s">
+      <c r="B21" s="353" t="s">
         <v>297</v>
       </c>
-      <c r="C21" s="356"/>
-      <c r="D21" s="356"/>
-      <c r="E21" s="356"/>
-      <c r="F21" s="357"/>
+      <c r="C21" s="354"/>
+      <c r="D21" s="354"/>
+      <c r="E21" s="354"/>
+      <c r="F21" s="355"/>
       <c r="G21" s="70">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="341" t="s">
+      <c r="I21" s="337" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="362"/>
-      <c r="K21" s="364">
+      <c r="J21" s="338"/>
+      <c r="K21" s="349">
         <f>G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="L21" s="365"/>
+      <c r="L21" s="350"/>
       <c r="M21" s="178"/>
       <c r="N21" s="172"/>
-      <c r="O21" s="352" t="s">
+      <c r="O21" s="374" t="s">
         <v>259</v>
       </c>
-      <c r="P21" s="342"/>
-      <c r="Q21" s="342"/>
-      <c r="R21" s="342"/>
-      <c r="S21" s="343"/>
+      <c r="P21" s="362"/>
+      <c r="Q21" s="362"/>
+      <c r="R21" s="362"/>
+      <c r="S21" s="363"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="177"/>
-      <c r="B22" s="344" t="s">
+      <c r="B22" s="342" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="345"/>
-      <c r="D22" s="345"/>
-      <c r="E22" s="345"/>
-      <c r="F22" s="358"/>
+      <c r="C22" s="343"/>
+      <c r="D22" s="343"/>
+      <c r="E22" s="343"/>
+      <c r="F22" s="336"/>
       <c r="G22" s="154">
         <f>G21</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="363" t="s">
+      <c r="I22" s="335" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="358"/>
-      <c r="K22" s="366">
+      <c r="J22" s="336"/>
+      <c r="K22" s="351">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="L22" s="367"/>
+      <c r="L22" s="352"/>
       <c r="M22" s="178"/>
       <c r="N22" s="172"/>
-      <c r="O22" s="344" t="s">
+      <c r="O22" s="342" t="s">
         <v>260</v>
       </c>
-      <c r="P22" s="345"/>
-      <c r="Q22" s="345"/>
-      <c r="R22" s="345"/>
-      <c r="S22" s="346"/>
+      <c r="P22" s="343"/>
+      <c r="Q22" s="343"/>
+      <c r="R22" s="343"/>
+      <c r="S22" s="367"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="177"/>
-      <c r="B23" s="359" t="s">
+      <c r="B23" s="356" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="360"/>
-      <c r="D23" s="360"/>
-      <c r="E23" s="360"/>
-      <c r="F23" s="361"/>
+      <c r="C23" s="357"/>
+      <c r="D23" s="357"/>
+      <c r="E23" s="357"/>
+      <c r="F23" s="358"/>
       <c r="G23" s="155">
         <f>K24</f>
         <v>1568729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="363" t="s">
+      <c r="I23" s="335" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="358"/>
-      <c r="K23" s="368">
+      <c r="J23" s="336"/>
+      <c r="K23" s="346">
         <f>Pemasukkan!L31</f>
         <v>690000</v>
       </c>
-      <c r="L23" s="369"/>
+      <c r="L23" s="347"/>
       <c r="M23" s="178"/>
       <c r="N23" s="172"/>
-      <c r="O23" s="344" t="s">
+      <c r="O23" s="342" t="s">
         <v>261</v>
       </c>
-      <c r="P23" s="345"/>
-      <c r="Q23" s="345"/>
-      <c r="R23" s="345"/>
-      <c r="S23" s="346"/>
+      <c r="P23" s="343"/>
+      <c r="Q23" s="343"/>
+      <c r="R23" s="343"/>
+      <c r="S23" s="367"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="177"/>
@@ -16061,24 +15949,24 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="341" t="s">
+      <c r="I24" s="337" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="362"/>
-      <c r="K24" s="353">
+      <c r="J24" s="338"/>
+      <c r="K24" s="333">
         <f>(K21-K22)+K23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="L24" s="354"/>
+      <c r="L24" s="334"/>
       <c r="M24" s="178"/>
       <c r="N24" s="172"/>
-      <c r="O24" s="344" t="s">
+      <c r="O24" s="342" t="s">
         <v>262</v>
       </c>
-      <c r="P24" s="345"/>
-      <c r="Q24" s="345"/>
-      <c r="R24" s="345"/>
-      <c r="S24" s="346"/>
+      <c r="P24" s="343"/>
+      <c r="Q24" s="343"/>
+      <c r="R24" s="343"/>
+      <c r="S24" s="367"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="177"/>
@@ -16098,10 +15986,10 @@
       <c r="O25" s="339" t="s">
         <v>267</v>
       </c>
-      <c r="P25" s="293"/>
-      <c r="Q25" s="293"/>
-      <c r="R25" s="293"/>
-      <c r="S25" s="317"/>
+      <c r="P25" s="306"/>
+      <c r="Q25" s="306"/>
+      <c r="R25" s="306"/>
+      <c r="S25" s="368"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="177"/>
@@ -16118,11 +16006,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="178"/>
       <c r="N26" s="172"/>
-      <c r="O26" s="340"/>
-      <c r="P26" s="318"/>
-      <c r="Q26" s="318"/>
-      <c r="R26" s="318"/>
-      <c r="S26" s="319"/>
+      <c r="O26" s="359"/>
+      <c r="P26" s="360"/>
+      <c r="Q26" s="360"/>
+      <c r="R26" s="360"/>
+      <c r="S26" s="361"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="179"/>
@@ -16157,6 +16045,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:AD3"/>
+    <mergeCell ref="W12:AD12"/>
+    <mergeCell ref="W13:AD13"/>
+    <mergeCell ref="W14:AD14"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:AD7"/>
+    <mergeCell ref="W9:AD9"/>
+    <mergeCell ref="W10:AD10"/>
+    <mergeCell ref="W11:AD11"/>
+    <mergeCell ref="U8:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:AD4"/>
+    <mergeCell ref="W8:AD8"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="O25:S25"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="W5:AD5"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="O18:S18"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O23:S23"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
     <mergeCell ref="D2:L2"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
@@ -16173,53 +16108,6 @@
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="W5:AD5"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="O24:S24"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="O18:S18"/>
-    <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O23:S23"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="W4:AD4"/>
-    <mergeCell ref="W8:AD8"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="O25:S25"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:AD3"/>
-    <mergeCell ref="W12:AD12"/>
-    <mergeCell ref="W13:AD13"/>
-    <mergeCell ref="W14:AD14"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="W7:AD7"/>
-    <mergeCell ref="W9:AD9"/>
-    <mergeCell ref="W10:AD10"/>
-    <mergeCell ref="W11:AD11"/>
-    <mergeCell ref="U8:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U4:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -16253,44 +16141,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="385" t="s">
+      <c r="C2" s="392" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="386"/>
-      <c r="E2" s="386"/>
-      <c r="F2" s="386"/>
-      <c r="G2" s="386"/>
-      <c r="H2" s="386"/>
-      <c r="I2" s="386"/>
-      <c r="J2" s="386"/>
-      <c r="K2" s="386"/>
+      <c r="D2" s="393"/>
+      <c r="E2" s="393"/>
+      <c r="F2" s="393"/>
+      <c r="G2" s="393"/>
+      <c r="H2" s="393"/>
+      <c r="I2" s="393"/>
+      <c r="J2" s="393"/>
+      <c r="K2" s="393"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="386"/>
-      <c r="D3" s="386"/>
-      <c r="E3" s="386"/>
-      <c r="F3" s="386"/>
-      <c r="G3" s="386"/>
-      <c r="H3" s="386"/>
-      <c r="I3" s="386"/>
-      <c r="J3" s="386"/>
-      <c r="K3" s="386"/>
+      <c r="C3" s="393"/>
+      <c r="D3" s="393"/>
+      <c r="E3" s="393"/>
+      <c r="F3" s="393"/>
+      <c r="G3" s="393"/>
+      <c r="H3" s="393"/>
+      <c r="I3" s="393"/>
+      <c r="J3" s="393"/>
+      <c r="K3" s="393"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="378" t="s">
+      <c r="C5" s="400" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="378"/>
-      <c r="E5" s="378"/>
-      <c r="F5" s="378"/>
-      <c r="G5" s="378"/>
-      <c r="I5" s="378" t="s">
+      <c r="D5" s="400"/>
+      <c r="E5" s="400"/>
+      <c r="F5" s="400"/>
+      <c r="G5" s="400"/>
+      <c r="I5" s="400" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="378"/>
-      <c r="K5" s="378"/>
-      <c r="L5" s="378"/>
-      <c r="M5" s="378"/>
+      <c r="J5" s="400"/>
+      <c r="K5" s="400"/>
+      <c r="L5" s="400"/>
+      <c r="M5" s="400"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -16730,88 +16618,88 @@
       <c r="M28" s="172"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="374" t="s">
+      <c r="D29" s="344" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="375"/>
-      <c r="F29" s="379">
+      <c r="E29" s="345"/>
+      <c r="F29" s="394">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="380"/>
+      <c r="G29" s="395"/>
       <c r="I29" s="172"/>
-      <c r="J29" s="374" t="s">
+      <c r="J29" s="344" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="375"/>
-      <c r="L29" s="379">
+      <c r="K29" s="345"/>
+      <c r="L29" s="394">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="380"/>
+      <c r="M29" s="395"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="334" t="s">
+      <c r="D30" s="391" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="293"/>
-      <c r="F30" s="381">
+      <c r="E30" s="306"/>
+      <c r="F30" s="396">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="382"/>
+      <c r="G30" s="397"/>
       <c r="I30" s="172"/>
-      <c r="J30" s="334" t="s">
+      <c r="J30" s="391" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="293"/>
-      <c r="L30" s="381">
+      <c r="K30" s="306"/>
+      <c r="L30" s="396">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="382"/>
+      <c r="M30" s="397"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D31" s="339" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="293"/>
-      <c r="F31" s="383">
+      <c r="E31" s="306"/>
+      <c r="F31" s="401">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="384"/>
+      <c r="G31" s="402"/>
       <c r="I31" s="172"/>
       <c r="J31" s="339" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="293"/>
-      <c r="L31" s="383">
+      <c r="K31" s="306"/>
+      <c r="L31" s="401">
         <f>L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="384"/>
+      <c r="M31" s="402"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="372" t="s">
+      <c r="D32" s="340" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="373"/>
-      <c r="F32" s="376">
+      <c r="E32" s="341"/>
+      <c r="F32" s="398">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="377"/>
+      <c r="G32" s="399"/>
       <c r="I32" s="172"/>
-      <c r="J32" s="372" t="s">
+      <c r="J32" s="340" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="373"/>
-      <c r="L32" s="376">
+      <c r="K32" s="341"/>
+      <c r="L32" s="398">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="377"/>
+      <c r="M32" s="399"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17003,12 +16891,6 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C2:K3"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J29:K29"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="I5:M5"/>
@@ -17022,6 +16904,12 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J32:K32"/>
+    <mergeCell ref="C2:K3"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -17054,44 +16942,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="391" t="s">
+      <c r="C2" s="403" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="392"/>
-      <c r="E2" s="392"/>
-      <c r="F2" s="392"/>
-      <c r="G2" s="392"/>
-      <c r="H2" s="392"/>
-      <c r="I2" s="392"/>
-      <c r="J2" s="392"/>
-      <c r="K2" s="392"/>
+      <c r="D2" s="404"/>
+      <c r="E2" s="404"/>
+      <c r="F2" s="404"/>
+      <c r="G2" s="404"/>
+      <c r="H2" s="404"/>
+      <c r="I2" s="404"/>
+      <c r="J2" s="404"/>
+      <c r="K2" s="404"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="392"/>
-      <c r="D3" s="392"/>
-      <c r="E3" s="392"/>
-      <c r="F3" s="392"/>
-      <c r="G3" s="392"/>
-      <c r="H3" s="392"/>
-      <c r="I3" s="392"/>
-      <c r="J3" s="392"/>
-      <c r="K3" s="392"/>
+      <c r="C3" s="404"/>
+      <c r="D3" s="404"/>
+      <c r="E3" s="404"/>
+      <c r="F3" s="404"/>
+      <c r="G3" s="404"/>
+      <c r="H3" s="404"/>
+      <c r="I3" s="404"/>
+      <c r="J3" s="404"/>
+      <c r="K3" s="404"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="378" t="s">
+      <c r="C5" s="400" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="378"/>
-      <c r="E5" s="378"/>
-      <c r="F5" s="378"/>
-      <c r="G5" s="378"/>
-      <c r="I5" s="378" t="s">
+      <c r="D5" s="400"/>
+      <c r="E5" s="400"/>
+      <c r="F5" s="400"/>
+      <c r="G5" s="400"/>
+      <c r="I5" s="400" t="s">
         <v>246</v>
       </c>
-      <c r="J5" s="378"/>
-      <c r="K5" s="378"/>
-      <c r="L5" s="378"/>
-      <c r="M5" s="378"/>
+      <c r="J5" s="400"/>
+      <c r="K5" s="400"/>
+      <c r="L5" s="400"/>
+      <c r="M5" s="400"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -17575,88 +17463,88 @@
       <c r="M28" s="172"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="313" t="s">
+      <c r="D29" s="379" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="315"/>
-      <c r="F29" s="389">
+      <c r="E29" s="381"/>
+      <c r="F29" s="405">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="390"/>
+      <c r="G29" s="406"/>
       <c r="I29" s="172"/>
-      <c r="J29" s="313" t="s">
+      <c r="J29" s="379" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="315"/>
-      <c r="L29" s="389">
+      <c r="K29" s="381"/>
+      <c r="L29" s="405">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="390"/>
+      <c r="M29" s="406"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" s="339" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="293"/>
-      <c r="F30" s="381">
+      <c r="E30" s="306"/>
+      <c r="F30" s="396">
         <f>F27</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="382"/>
+      <c r="G30" s="397"/>
       <c r="I30" s="172"/>
       <c r="J30" s="339" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="293"/>
-      <c r="L30" s="381">
+      <c r="K30" s="306"/>
+      <c r="L30" s="396">
         <f>L27</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="382"/>
+      <c r="M30" s="397"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D31" s="339" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="293"/>
-      <c r="F31" s="383">
+      <c r="E31" s="306"/>
+      <c r="F31" s="401">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="384"/>
+      <c r="G31" s="402"/>
       <c r="I31" s="172"/>
       <c r="J31" s="339" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="293"/>
-      <c r="L31" s="383">
+      <c r="K31" s="306"/>
+      <c r="L31" s="401">
         <f>Pemasukkan!L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="384"/>
+      <c r="M31" s="402"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="372" t="s">
+      <c r="D32" s="340" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="373"/>
-      <c r="F32" s="387">
+      <c r="E32" s="341"/>
+      <c r="F32" s="407">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="388"/>
+      <c r="G32" s="408"/>
       <c r="I32" s="172"/>
-      <c r="J32" s="372" t="s">
+      <c r="J32" s="340" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="373"/>
-      <c r="L32" s="387">
+      <c r="K32" s="341"/>
+      <c r="L32" s="407">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="388"/>
+      <c r="M32" s="408"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17848,6 +17736,14 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
     <mergeCell ref="C2:K3"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
@@ -17859,14 +17755,6 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -17892,28 +17780,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="395" t="s">
+      <c r="C2" s="411" t="s">
         <v>230</v>
       </c>
-      <c r="D2" s="396"/>
-      <c r="E2" s="396"/>
-      <c r="F2" s="396"/>
-      <c r="G2" s="396"/>
-      <c r="H2" s="396"/>
-      <c r="I2" s="396"/>
-      <c r="J2" s="396"/>
-      <c r="K2" s="396"/>
+      <c r="D2" s="412"/>
+      <c r="E2" s="412"/>
+      <c r="F2" s="412"/>
+      <c r="G2" s="412"/>
+      <c r="H2" s="412"/>
+      <c r="I2" s="412"/>
+      <c r="J2" s="412"/>
+      <c r="K2" s="412"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="396"/>
-      <c r="D3" s="396"/>
-      <c r="E3" s="396"/>
-      <c r="F3" s="396"/>
-      <c r="G3" s="396"/>
-      <c r="H3" s="396"/>
-      <c r="I3" s="396"/>
-      <c r="J3" s="396"/>
-      <c r="K3" s="396"/>
+      <c r="C3" s="412"/>
+      <c r="D3" s="412"/>
+      <c r="E3" s="412"/>
+      <c r="F3" s="412"/>
+      <c r="G3" s="412"/>
+      <c r="H3" s="412"/>
+      <c r="I3" s="412"/>
+      <c r="J3" s="412"/>
+      <c r="K3" s="412"/>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="141"/>
@@ -18271,10 +18159,10 @@
     </row>
     <row r="29" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="141"/>
-      <c r="D29" s="397"/>
-      <c r="E29" s="397"/>
-      <c r="F29" s="398"/>
-      <c r="G29" s="398"/>
+      <c r="D29" s="413"/>
+      <c r="E29" s="413"/>
+      <c r="F29" s="414"/>
+      <c r="G29" s="414"/>
       <c r="H29" s="141"/>
       <c r="I29" s="141"/>
       <c r="J29" s="141"/>
@@ -18282,15 +18170,15 @@
     </row>
     <row r="30" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="24"/>
-      <c r="D30" s="399" t="s">
+      <c r="D30" s="415" t="s">
         <v>229</v>
       </c>
-      <c r="E30" s="400"/>
-      <c r="F30" s="401">
+      <c r="E30" s="416"/>
+      <c r="F30" s="417">
         <f>F27</f>
         <v>226000</v>
       </c>
-      <c r="G30" s="402"/>
+      <c r="G30" s="418"/>
       <c r="H30" s="141"/>
       <c r="I30" s="141"/>
       <c r="J30" s="141"/>
@@ -18305,10 +18193,10 @@
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="141"/>
-      <c r="D32" s="393"/>
-      <c r="E32" s="393"/>
-      <c r="F32" s="394"/>
-      <c r="G32" s="393"/>
+      <c r="D32" s="409"/>
+      <c r="E32" s="409"/>
+      <c r="F32" s="410"/>
+      <c r="G32" s="409"/>
       <c r="H32" s="141"/>
       <c r="I32" s="141"/>
       <c r="J32" s="141"/>
@@ -18345,17 +18233,17 @@
     <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="403" t="s">
+      <c r="C4" s="419" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="404"/>
+      <c r="D4" s="420"/>
       <c r="E4" s="27"/>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
-      <c r="H4" s="403" t="s">
+      <c r="H4" s="419" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="404"/>
+      <c r="I4" s="420"/>
       <c r="J4" s="35"/>
       <c r="K4" s="27"/>
     </row>
@@ -18482,17 +18370,17 @@
     <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26"/>
-      <c r="C17" s="403" t="s">
+      <c r="C17" s="419" t="s">
         <v>144</v>
       </c>
-      <c r="D17" s="404"/>
+      <c r="D17" s="420"/>
       <c r="E17" s="27"/>
       <c r="F17" s="26"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="403" t="s">
+      <c r="H17" s="419" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="404"/>
+      <c r="I17" s="420"/>
       <c r="J17" s="35"/>
       <c r="K17" s="27"/>
     </row>
@@ -18646,28 +18534,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="406" t="s">
+      <c r="B2" s="422" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="407"/>
-      <c r="D2" s="407"/>
-      <c r="E2" s="407"/>
-      <c r="F2" s="407"/>
-      <c r="G2" s="407"/>
-      <c r="H2" s="407"/>
-      <c r="I2" s="407"/>
-      <c r="J2" s="407"/>
+      <c r="C2" s="423"/>
+      <c r="D2" s="423"/>
+      <c r="E2" s="423"/>
+      <c r="F2" s="423"/>
+      <c r="G2" s="423"/>
+      <c r="H2" s="423"/>
+      <c r="I2" s="423"/>
+      <c r="J2" s="423"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="407"/>
-      <c r="C3" s="407"/>
-      <c r="D3" s="407"/>
-      <c r="E3" s="407"/>
-      <c r="F3" s="407"/>
-      <c r="G3" s="407"/>
-      <c r="H3" s="407"/>
-      <c r="I3" s="407"/>
-      <c r="J3" s="407"/>
+      <c r="B3" s="423"/>
+      <c r="C3" s="423"/>
+      <c r="D3" s="423"/>
+      <c r="E3" s="423"/>
+      <c r="F3" s="423"/>
+      <c r="G3" s="423"/>
+      <c r="H3" s="423"/>
+      <c r="I3" s="423"/>
+      <c r="J3" s="423"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -18688,10 +18576,10 @@
       <c r="G6" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="H6" s="322" t="s">
+      <c r="H6" s="348" t="s">
         <v>281</v>
       </c>
-      <c r="I6" s="293"/>
+      <c r="I6" s="306"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -18713,11 +18601,11 @@
       <c r="G7" s="195">
         <v>205000</v>
       </c>
-      <c r="H7" s="408">
+      <c r="H7" s="424">
         <f>F7-G7</f>
         <v>380000</v>
       </c>
-      <c r="I7" s="293"/>
+      <c r="I7" s="306"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="196"/>
@@ -18726,8 +18614,8 @@
       <c r="E8" s="197"/>
       <c r="F8" s="197"/>
       <c r="G8" s="197"/>
-      <c r="H8" s="405"/>
-      <c r="I8" s="405"/>
+      <c r="H8" s="421"/>
+      <c r="I8" s="421"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="196"/>
@@ -18738,11 +18626,11 @@
       <c r="G9" s="198" t="s">
         <v>282</v>
       </c>
-      <c r="H9" s="409">
+      <c r="H9" s="425">
         <f>H7</f>
         <v>380000</v>
       </c>
-      <c r="I9" s="410"/>
+      <c r="I9" s="426"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="196"/>
@@ -18751,8 +18639,8 @@
       <c r="E10" s="197"/>
       <c r="F10" s="197"/>
       <c r="G10" s="197"/>
-      <c r="H10" s="405"/>
-      <c r="I10" s="405"/>
+      <c r="H10" s="421"/>
+      <c r="I10" s="421"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="196"/>
@@ -18761,8 +18649,8 @@
       <c r="E11" s="197"/>
       <c r="F11" s="197"/>
       <c r="G11" s="197"/>
-      <c r="H11" s="405"/>
-      <c r="I11" s="405"/>
+      <c r="H11" s="421"/>
+      <c r="I11" s="421"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="196"/>
@@ -18771,8 +18659,8 @@
       <c r="E12" s="197"/>
       <c r="F12" s="197"/>
       <c r="G12" s="197"/>
-      <c r="H12" s="405"/>
-      <c r="I12" s="405"/>
+      <c r="H12" s="421"/>
+      <c r="I12" s="421"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="196"/>
@@ -18781,8 +18669,8 @@
       <c r="E13" s="197"/>
       <c r="F13" s="197"/>
       <c r="G13" s="197"/>
-      <c r="H13" s="405"/>
-      <c r="I13" s="405"/>
+      <c r="H13" s="421"/>
+      <c r="I13" s="421"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="196"/>
@@ -18791,8 +18679,8 @@
       <c r="E14" s="197"/>
       <c r="F14" s="197"/>
       <c r="G14" s="197"/>
-      <c r="H14" s="405"/>
-      <c r="I14" s="405"/>
+      <c r="H14" s="421"/>
+      <c r="I14" s="421"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="196"/>
@@ -18801,8 +18689,8 @@
       <c r="E15" s="197"/>
       <c r="F15" s="197"/>
       <c r="G15" s="197"/>
-      <c r="H15" s="405"/>
-      <c r="I15" s="405"/>
+      <c r="H15" s="421"/>
+      <c r="I15" s="421"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="196"/>
@@ -18811,8 +18699,8 @@
       <c r="E16" s="197"/>
       <c r="F16" s="197"/>
       <c r="G16" s="197"/>
-      <c r="H16" s="405"/>
-      <c r="I16" s="405"/>
+      <c r="H16" s="421"/>
+      <c r="I16" s="421"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="196"/>
@@ -18821,16 +18709,11 @@
       <c r="E17" s="197"/>
       <c r="F17" s="197"/>
       <c r="G17" s="197"/>
-      <c r="H17" s="405"/>
-      <c r="I17" s="405"/>
+      <c r="H17" s="421"/>
+      <c r="I17" s="421"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="H6:I6"/>
@@ -18839,6 +18722,11 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Pencatatan Pembayaran Pendaftaran Makrab 19
Ditambahkan sheet "Pembayaran Pendaftaran Makrab 19" untuk input Pembayaran Pendaftaran Makrab
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -10,19 +10,20 @@
     <sheet name="2018(NOT UPDATED)" sheetId="1" r:id="rId1"/>
     <sheet name="2019" sheetId="2" r:id="rId2"/>
     <sheet name="Sirkulasi" sheetId="10" r:id="rId3"/>
-    <sheet name="Hitung Pemasukan Pengeluaran" sheetId="8" r:id="rId4"/>
-    <sheet name="Pemasukkan" sheetId="6" r:id="rId5"/>
-    <sheet name="Pengeluaran" sheetId="4" r:id="rId6"/>
-    <sheet name="Inventaris" sheetId="7" r:id="rId7"/>
-    <sheet name="Lampiran Polo" sheetId="3" r:id="rId8"/>
-    <sheet name="Patch OH" sheetId="9" r:id="rId9"/>
+    <sheet name="Pembayaran Makrab 19" sheetId="11" r:id="rId4"/>
+    <sheet name="Hitung Pemasukan Pengeluaran" sheetId="8" r:id="rId5"/>
+    <sheet name="Pemasukkan" sheetId="6" r:id="rId6"/>
+    <sheet name="Pengeluaran" sheetId="4" r:id="rId7"/>
+    <sheet name="Inventaris" sheetId="7" r:id="rId8"/>
+    <sheet name="Lampiran Polo" sheetId="3" r:id="rId9"/>
+    <sheet name="Patch OH" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="362">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -1075,6 +1076,39 @@
   </si>
   <si>
     <t>DP Sewa Field</t>
+  </si>
+  <si>
+    <t>Nama</t>
+  </si>
+  <si>
+    <t>Metode</t>
+  </si>
+  <si>
+    <t>Devina</t>
+  </si>
+  <si>
+    <t>MABA</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
+  <si>
+    <t>Gazza Bryan Prilandi</t>
+  </si>
+  <si>
+    <t>Edi Pratbowo</t>
+  </si>
+  <si>
+    <t>Tunai</t>
+  </si>
+  <si>
+    <t>Chiko Permana Putra</t>
+  </si>
+  <si>
+    <t>Pendaftaran Makrab 19</t>
+  </si>
+  <si>
+    <t>`-</t>
   </si>
 </sst>
 </file>
@@ -1361,7 +1395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="78">
+  <borders count="79">
     <border>
       <left/>
       <right/>
@@ -2276,13 +2310,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="427">
+  <cellXfs count="434">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2885,19 +2930,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2905,9 +2939,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2923,37 +2962,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2961,29 +3002,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3018,6 +3066,156 @@
     <xf numFmtId="177" fontId="4" fillId="26" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3030,33 +3228,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3076,136 +3253,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3216,29 +3282,23 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3246,18 +3306,6 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3311,6 +3359,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="4" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3318,7 +3380,63 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4443,126 +4561,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="282" t="s">
+      <c r="A1" s="277" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="283"/>
-      <c r="C1" s="283"/>
-      <c r="D1" s="283"/>
-      <c r="E1" s="283"/>
-      <c r="F1" s="283"/>
-      <c r="G1" s="283"/>
-      <c r="H1" s="283"/>
-      <c r="I1" s="283"/>
-      <c r="J1" s="283"/>
-      <c r="K1" s="283"/>
-      <c r="L1" s="283"/>
-      <c r="M1" s="283"/>
-      <c r="N1" s="283"/>
-      <c r="O1" s="283"/>
-      <c r="P1" s="283"/>
-      <c r="Q1" s="283"/>
-      <c r="R1" s="283"/>
+      <c r="B1" s="278"/>
+      <c r="C1" s="278"/>
+      <c r="D1" s="278"/>
+      <c r="E1" s="278"/>
+      <c r="F1" s="278"/>
+      <c r="G1" s="278"/>
+      <c r="H1" s="278"/>
+      <c r="I1" s="278"/>
+      <c r="J1" s="278"/>
+      <c r="K1" s="278"/>
+      <c r="L1" s="278"/>
+      <c r="M1" s="278"/>
+      <c r="N1" s="278"/>
+      <c r="O1" s="278"/>
+      <c r="P1" s="278"/>
+      <c r="Q1" s="278"/>
+      <c r="R1" s="278"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="284"/>
-      <c r="B2" s="285"/>
-      <c r="C2" s="285"/>
-      <c r="D2" s="285"/>
-      <c r="E2" s="285"/>
-      <c r="F2" s="285"/>
-      <c r="G2" s="285"/>
-      <c r="H2" s="285"/>
-      <c r="I2" s="285"/>
-      <c r="J2" s="285"/>
-      <c r="K2" s="285"/>
-      <c r="L2" s="285"/>
-      <c r="M2" s="285"/>
-      <c r="N2" s="285"/>
-      <c r="O2" s="285"/>
-      <c r="P2" s="285"/>
-      <c r="Q2" s="285"/>
-      <c r="R2" s="285"/>
+      <c r="A2" s="279"/>
+      <c r="B2" s="280"/>
+      <c r="C2" s="280"/>
+      <c r="D2" s="280"/>
+      <c r="E2" s="280"/>
+      <c r="F2" s="280"/>
+      <c r="G2" s="280"/>
+      <c r="H2" s="280"/>
+      <c r="I2" s="280"/>
+      <c r="J2" s="280"/>
+      <c r="K2" s="280"/>
+      <c r="L2" s="280"/>
+      <c r="M2" s="280"/>
+      <c r="N2" s="280"/>
+      <c r="O2" s="280"/>
+      <c r="P2" s="280"/>
+      <c r="Q2" s="280"/>
+      <c r="R2" s="280"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="284"/>
-      <c r="B3" s="285"/>
-      <c r="C3" s="285"/>
-      <c r="D3" s="285"/>
-      <c r="E3" s="285"/>
-      <c r="F3" s="285"/>
-      <c r="G3" s="285"/>
-      <c r="H3" s="285"/>
-      <c r="I3" s="285"/>
-      <c r="J3" s="285"/>
-      <c r="K3" s="285"/>
-      <c r="L3" s="285"/>
-      <c r="M3" s="285"/>
-      <c r="N3" s="285"/>
-      <c r="O3" s="285"/>
-      <c r="P3" s="285"/>
-      <c r="Q3" s="285"/>
-      <c r="R3" s="285"/>
+      <c r="A3" s="279"/>
+      <c r="B3" s="280"/>
+      <c r="C3" s="280"/>
+      <c r="D3" s="280"/>
+      <c r="E3" s="280"/>
+      <c r="F3" s="280"/>
+      <c r="G3" s="280"/>
+      <c r="H3" s="280"/>
+      <c r="I3" s="280"/>
+      <c r="J3" s="280"/>
+      <c r="K3" s="280"/>
+      <c r="L3" s="280"/>
+      <c r="M3" s="280"/>
+      <c r="N3" s="280"/>
+      <c r="O3" s="280"/>
+      <c r="P3" s="280"/>
+      <c r="Q3" s="280"/>
+      <c r="R3" s="280"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="284"/>
-      <c r="B4" s="285"/>
-      <c r="C4" s="285"/>
-      <c r="D4" s="285"/>
-      <c r="E4" s="285"/>
-      <c r="F4" s="285"/>
-      <c r="G4" s="285"/>
-      <c r="H4" s="285"/>
-      <c r="I4" s="285"/>
-      <c r="J4" s="285"/>
-      <c r="K4" s="285"/>
-      <c r="L4" s="285"/>
-      <c r="M4" s="285"/>
-      <c r="N4" s="285"/>
-      <c r="O4" s="285"/>
-      <c r="P4" s="285"/>
-      <c r="Q4" s="285"/>
-      <c r="R4" s="285"/>
+      <c r="A4" s="279"/>
+      <c r="B4" s="280"/>
+      <c r="C4" s="280"/>
+      <c r="D4" s="280"/>
+      <c r="E4" s="280"/>
+      <c r="F4" s="280"/>
+      <c r="G4" s="280"/>
+      <c r="H4" s="280"/>
+      <c r="I4" s="280"/>
+      <c r="J4" s="280"/>
+      <c r="K4" s="280"/>
+      <c r="L4" s="280"/>
+      <c r="M4" s="280"/>
+      <c r="N4" s="280"/>
+      <c r="O4" s="280"/>
+      <c r="P4" s="280"/>
+      <c r="Q4" s="280"/>
+      <c r="R4" s="280"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="284"/>
-      <c r="B5" s="285"/>
-      <c r="C5" s="285"/>
-      <c r="D5" s="285"/>
-      <c r="E5" s="285"/>
-      <c r="F5" s="285"/>
-      <c r="G5" s="285"/>
-      <c r="H5" s="285"/>
-      <c r="I5" s="285"/>
-      <c r="J5" s="285"/>
-      <c r="K5" s="285"/>
-      <c r="L5" s="285"/>
-      <c r="M5" s="285"/>
-      <c r="N5" s="285"/>
-      <c r="O5" s="285"/>
-      <c r="P5" s="285"/>
-      <c r="Q5" s="285"/>
-      <c r="R5" s="285"/>
+      <c r="A5" s="279"/>
+      <c r="B5" s="280"/>
+      <c r="C5" s="280"/>
+      <c r="D5" s="280"/>
+      <c r="E5" s="280"/>
+      <c r="F5" s="280"/>
+      <c r="G5" s="280"/>
+      <c r="H5" s="280"/>
+      <c r="I5" s="280"/>
+      <c r="J5" s="280"/>
+      <c r="K5" s="280"/>
+      <c r="L5" s="280"/>
+      <c r="M5" s="280"/>
+      <c r="N5" s="280"/>
+      <c r="O5" s="280"/>
+      <c r="P5" s="280"/>
+      <c r="Q5" s="280"/>
+      <c r="R5" s="280"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="284"/>
-      <c r="B6" s="285"/>
-      <c r="C6" s="285"/>
-      <c r="D6" s="285"/>
-      <c r="E6" s="285"/>
-      <c r="F6" s="285"/>
-      <c r="G6" s="285"/>
-      <c r="H6" s="285"/>
-      <c r="I6" s="285"/>
-      <c r="J6" s="285"/>
-      <c r="K6" s="285"/>
-      <c r="L6" s="285"/>
-      <c r="M6" s="285"/>
-      <c r="N6" s="285"/>
-      <c r="O6" s="285"/>
-      <c r="P6" s="285"/>
-      <c r="Q6" s="285"/>
-      <c r="R6" s="285"/>
+      <c r="A6" s="279"/>
+      <c r="B6" s="280"/>
+      <c r="C6" s="280"/>
+      <c r="D6" s="280"/>
+      <c r="E6" s="280"/>
+      <c r="F6" s="280"/>
+      <c r="G6" s="280"/>
+      <c r="H6" s="280"/>
+      <c r="I6" s="280"/>
+      <c r="J6" s="280"/>
+      <c r="K6" s="280"/>
+      <c r="L6" s="280"/>
+      <c r="M6" s="280"/>
+      <c r="N6" s="280"/>
+      <c r="O6" s="280"/>
+      <c r="P6" s="280"/>
+      <c r="Q6" s="280"/>
+      <c r="R6" s="280"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -7507,58 +7625,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="287" t="s">
+      <c r="J79" s="285" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="288"/>
-      <c r="L79" s="288"/>
-      <c r="M79" s="288"/>
-      <c r="N79" s="289"/>
-      <c r="P79" s="295" t="s">
+      <c r="K79" s="286"/>
+      <c r="L79" s="286"/>
+      <c r="M79" s="286"/>
+      <c r="N79" s="287"/>
+      <c r="P79" s="293" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="288"/>
-      <c r="R79" s="288"/>
-      <c r="S79" s="289"/>
+      <c r="Q79" s="286"/>
+      <c r="R79" s="286"/>
+      <c r="S79" s="287"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="290" t="s">
+      <c r="J80" s="288" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="285"/>
-      <c r="L80" s="285"/>
-      <c r="M80" s="285"/>
-      <c r="N80" s="291"/>
-      <c r="P80" s="290" t="s">
+      <c r="K80" s="280"/>
+      <c r="L80" s="280"/>
+      <c r="M80" s="280"/>
+      <c r="N80" s="289"/>
+      <c r="P80" s="288" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="285"/>
-      <c r="R80" s="285"/>
-      <c r="S80" s="291"/>
+      <c r="Q80" s="280"/>
+      <c r="R80" s="280"/>
+      <c r="S80" s="289"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="292"/>
-      <c r="K81" s="293"/>
-      <c r="L81" s="293"/>
-      <c r="M81" s="293"/>
-      <c r="N81" s="294"/>
-      <c r="P81" s="292"/>
-      <c r="Q81" s="293"/>
-      <c r="R81" s="293"/>
-      <c r="S81" s="294"/>
+      <c r="J81" s="290"/>
+      <c r="K81" s="291"/>
+      <c r="L81" s="291"/>
+      <c r="M81" s="291"/>
+      <c r="N81" s="292"/>
+      <c r="P81" s="290"/>
+      <c r="Q81" s="291"/>
+      <c r="R81" s="291"/>
+      <c r="S81" s="292"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="286" t="s">
+      <c r="J82" s="283" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="277"/>
-      <c r="L82" s="278"/>
-      <c r="M82" s="286" t="s">
+      <c r="K82" s="284"/>
+      <c r="L82" s="282"/>
+      <c r="M82" s="283" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="278"/>
-      <c r="P82" s="286"/>
-      <c r="Q82" s="278"/>
+      <c r="N82" s="282"/>
+      <c r="P82" s="283"/>
+      <c r="Q82" s="282"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -7567,38 +7685,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="276" t="s">
+      <c r="J83" s="294" t="s">
         <v>70</v>
       </c>
-      <c r="K83" s="277"/>
-      <c r="L83" s="278"/>
-      <c r="M83" s="279">
+      <c r="K83" s="284"/>
+      <c r="L83" s="282"/>
+      <c r="M83" s="295">
         <v>7350000</v>
       </c>
-      <c r="N83" s="278"/>
-      <c r="P83" s="280" t="s">
+      <c r="N83" s="282"/>
+      <c r="P83" s="281" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="278"/>
+      <c r="Q83" s="282"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="276" t="s">
+      <c r="J84" s="294" t="s">
         <v>72</v>
       </c>
-      <c r="K84" s="277"/>
-      <c r="L84" s="278"/>
-      <c r="M84" s="281">
+      <c r="K84" s="284"/>
+      <c r="L84" s="282"/>
+      <c r="M84" s="296">
         <v>1100000</v>
       </c>
-      <c r="N84" s="278"/>
-      <c r="P84" s="280" t="s">
+      <c r="N84" s="282"/>
+      <c r="P84" s="281" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="278"/>
+      <c r="Q84" s="282"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -7607,39 +7725,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="276" t="s">
+      <c r="J85" s="294" t="s">
         <v>75</v>
       </c>
-      <c r="K85" s="277"/>
-      <c r="L85" s="278"/>
-      <c r="M85" s="279">
+      <c r="K85" s="284"/>
+      <c r="L85" s="282"/>
+      <c r="M85" s="295">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="278"/>
-      <c r="P85" s="280" t="s">
+      <c r="N85" s="282"/>
+      <c r="P85" s="281" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="278"/>
+      <c r="Q85" s="282"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="276" t="s">
+      <c r="J86" s="294" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="277"/>
-      <c r="L86" s="278"/>
-      <c r="M86" s="279">
+      <c r="K86" s="284"/>
+      <c r="L86" s="282"/>
+      <c r="M86" s="295">
         <v>8411850</v>
       </c>
-      <c r="N86" s="278"/>
-      <c r="P86" s="280" t="s">
+      <c r="N86" s="282"/>
+      <c r="P86" s="281" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="278"/>
+      <c r="Q86" s="282"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -7647,20 +7765,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="276" t="s">
+      <c r="J87" s="294" t="s">
         <v>79</v>
       </c>
-      <c r="K87" s="277"/>
-      <c r="L87" s="278"/>
-      <c r="M87" s="279">
+      <c r="K87" s="284"/>
+      <c r="L87" s="282"/>
+      <c r="M87" s="295">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="278"/>
-      <c r="P87" s="280" t="s">
+      <c r="N87" s="282"/>
+      <c r="P87" s="281" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="278"/>
+      <c r="Q87" s="282"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -7849,6 +7967,17 @@
   </sheetData>
   <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="23">
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="P86:Q86"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="M84:N84"/>
     <mergeCell ref="A1:R6"/>
     <mergeCell ref="P84:Q84"/>
     <mergeCell ref="J82:L82"/>
@@ -7861,38 +7990,27 @@
     <mergeCell ref="P83:Q83"/>
     <mergeCell ref="P82:Q82"/>
     <mergeCell ref="P80:S81"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="P86:Q86"/>
   </mergeCells>
   <conditionalFormatting sqref="T10:T52">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S52">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S51">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>$S$12=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7901,12 +8019,228 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="423" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" s="424"/>
+      <c r="D2" s="424"/>
+      <c r="E2" s="424"/>
+      <c r="F2" s="424"/>
+      <c r="G2" s="424"/>
+      <c r="H2" s="424"/>
+      <c r="I2" s="424"/>
+      <c r="J2" s="424"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="424"/>
+      <c r="C3" s="424"/>
+      <c r="D3" s="424"/>
+      <c r="E3" s="424"/>
+      <c r="F3" s="424"/>
+      <c r="G3" s="424"/>
+      <c r="H3" s="424"/>
+      <c r="I3" s="424"/>
+      <c r="J3" s="424"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H6" s="349" t="s">
+        <v>281</v>
+      </c>
+      <c r="I6" s="307"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D7" s="1">
+        <v>39</v>
+      </c>
+      <c r="E7" s="195">
+        <v>15000</v>
+      </c>
+      <c r="F7" s="195">
+        <f>D7*E7</f>
+        <v>585000</v>
+      </c>
+      <c r="G7" s="195">
+        <v>205000</v>
+      </c>
+      <c r="H7" s="425">
+        <f>F7-G7</f>
+        <v>380000</v>
+      </c>
+      <c r="I7" s="307"/>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="196"/>
+      <c r="C8" s="196"/>
+      <c r="D8" s="196"/>
+      <c r="E8" s="197"/>
+      <c r="F8" s="197"/>
+      <c r="G8" s="197"/>
+      <c r="H8" s="422"/>
+      <c r="I8" s="422"/>
+    </row>
+    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="196"/>
+      <c r="C9" s="196"/>
+      <c r="D9" s="196"/>
+      <c r="E9" s="197"/>
+      <c r="F9" s="197"/>
+      <c r="G9" s="198" t="s">
+        <v>282</v>
+      </c>
+      <c r="H9" s="426">
+        <f>H7</f>
+        <v>380000</v>
+      </c>
+      <c r="I9" s="427"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="196"/>
+      <c r="C10" s="196"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="197"/>
+      <c r="F10" s="197"/>
+      <c r="G10" s="197"/>
+      <c r="H10" s="422"/>
+      <c r="I10" s="422"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="196"/>
+      <c r="C11" s="196"/>
+      <c r="D11" s="196"/>
+      <c r="E11" s="197"/>
+      <c r="F11" s="197"/>
+      <c r="G11" s="197"/>
+      <c r="H11" s="422"/>
+      <c r="I11" s="422"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="196"/>
+      <c r="C12" s="196"/>
+      <c r="D12" s="196"/>
+      <c r="E12" s="197"/>
+      <c r="F12" s="197"/>
+      <c r="G12" s="197"/>
+      <c r="H12" s="422"/>
+      <c r="I12" s="422"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="196"/>
+      <c r="C13" s="196"/>
+      <c r="D13" s="196"/>
+      <c r="E13" s="197"/>
+      <c r="F13" s="197"/>
+      <c r="G13" s="197"/>
+      <c r="H13" s="422"/>
+      <c r="I13" s="422"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="196"/>
+      <c r="C14" s="196"/>
+      <c r="D14" s="196"/>
+      <c r="E14" s="197"/>
+      <c r="F14" s="197"/>
+      <c r="G14" s="197"/>
+      <c r="H14" s="422"/>
+      <c r="I14" s="422"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="196"/>
+      <c r="C15" s="196"/>
+      <c r="D15" s="196"/>
+      <c r="E15" s="197"/>
+      <c r="F15" s="197"/>
+      <c r="G15" s="197"/>
+      <c r="H15" s="422"/>
+      <c r="I15" s="422"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="196"/>
+      <c r="C16" s="196"/>
+      <c r="D16" s="196"/>
+      <c r="E16" s="197"/>
+      <c r="F16" s="197"/>
+      <c r="G16" s="197"/>
+      <c r="H16" s="422"/>
+      <c r="I16" s="422"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="196"/>
+      <c r="C17" s="196"/>
+      <c r="D17" s="196"/>
+      <c r="E17" s="197"/>
+      <c r="F17" s="197"/>
+      <c r="G17" s="197"/>
+      <c r="H17" s="422"/>
+      <c r="I17" s="422"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B2:J3"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BM266"/>
   <sheetViews>
     <sheetView defaultGridColor="0" colorId="8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7948,46 +8282,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="304" t="s">
+      <c r="C2" s="317" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="283"/>
-      <c r="E2" s="283"/>
-      <c r="F2" s="283"/>
-      <c r="G2" s="283"/>
-      <c r="H2" s="283"/>
-      <c r="I2" s="283"/>
-      <c r="J2" s="283"/>
-      <c r="K2" s="283"/>
-      <c r="L2" s="283"/>
-      <c r="M2" s="283"/>
-      <c r="N2" s="283"/>
-      <c r="O2" s="283"/>
-      <c r="P2" s="284"/>
-      <c r="Q2" s="284"/>
-      <c r="R2" s="284"/>
-      <c r="S2" s="283"/>
-      <c r="T2" s="283"/>
+      <c r="D2" s="278"/>
+      <c r="E2" s="278"/>
+      <c r="F2" s="278"/>
+      <c r="G2" s="278"/>
+      <c r="H2" s="278"/>
+      <c r="I2" s="278"/>
+      <c r="J2" s="278"/>
+      <c r="K2" s="278"/>
+      <c r="L2" s="278"/>
+      <c r="M2" s="278"/>
+      <c r="N2" s="278"/>
+      <c r="O2" s="278"/>
+      <c r="P2" s="279"/>
+      <c r="Q2" s="279"/>
+      <c r="R2" s="279"/>
+      <c r="S2" s="278"/>
+      <c r="T2" s="278"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="284"/>
-      <c r="D3" s="285"/>
-      <c r="E3" s="285"/>
-      <c r="F3" s="285"/>
-      <c r="G3" s="285"/>
-      <c r="H3" s="285"/>
-      <c r="I3" s="285"/>
-      <c r="J3" s="285"/>
-      <c r="K3" s="285"/>
-      <c r="L3" s="285"/>
-      <c r="M3" s="285"/>
-      <c r="N3" s="285"/>
-      <c r="O3" s="285"/>
-      <c r="P3" s="285"/>
-      <c r="Q3" s="285"/>
-      <c r="R3" s="285"/>
-      <c r="S3" s="285"/>
-      <c r="T3" s="285"/>
+      <c r="C3" s="279"/>
+      <c r="D3" s="280"/>
+      <c r="E3" s="280"/>
+      <c r="F3" s="280"/>
+      <c r="G3" s="280"/>
+      <c r="H3" s="280"/>
+      <c r="I3" s="280"/>
+      <c r="J3" s="280"/>
+      <c r="K3" s="280"/>
+      <c r="L3" s="280"/>
+      <c r="M3" s="280"/>
+      <c r="N3" s="280"/>
+      <c r="O3" s="280"/>
+      <c r="P3" s="280"/>
+      <c r="Q3" s="280"/>
+      <c r="R3" s="280"/>
+      <c r="S3" s="280"/>
+      <c r="T3" s="280"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8074,25 +8408,25 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="310" t="s">
+      <c r="X5" s="309" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="277"/>
-      <c r="Z5" s="277"/>
-      <c r="AA5" s="277"/>
-      <c r="AB5" s="277"/>
-      <c r="AC5" s="277"/>
-      <c r="AD5" s="277"/>
-      <c r="AE5" s="277"/>
-      <c r="AF5" s="277"/>
-      <c r="AG5" s="277"/>
-      <c r="AH5" s="277"/>
-      <c r="AI5" s="277"/>
-      <c r="AJ5" s="277"/>
-      <c r="AK5" s="277"/>
-      <c r="AL5" s="277"/>
-      <c r="AM5" s="277"/>
-      <c r="AN5" s="278"/>
+      <c r="Y5" s="284"/>
+      <c r="Z5" s="284"/>
+      <c r="AA5" s="284"/>
+      <c r="AB5" s="284"/>
+      <c r="AC5" s="284"/>
+      <c r="AD5" s="284"/>
+      <c r="AE5" s="284"/>
+      <c r="AF5" s="284"/>
+      <c r="AG5" s="284"/>
+      <c r="AH5" s="284"/>
+      <c r="AI5" s="284"/>
+      <c r="AJ5" s="284"/>
+      <c r="AK5" s="284"/>
+      <c r="AL5" s="284"/>
+      <c r="AM5" s="284"/>
+      <c r="AN5" s="282"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -8167,29 +8501,29 @@
       <c r="V6" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="X6" s="305" t="s">
+      <c r="X6" s="318" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="305" t="s">
+      <c r="Y6" s="318" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="309" t="s">
+      <c r="Z6" s="307" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="306"/>
-      <c r="AB6" s="306"/>
-      <c r="AC6" s="306"/>
-      <c r="AD6" s="306"/>
-      <c r="AE6" s="306"/>
-      <c r="AF6" s="306"/>
-      <c r="AG6" s="306"/>
-      <c r="AH6" s="306"/>
-      <c r="AI6" s="306"/>
-      <c r="AJ6" s="306"/>
-      <c r="AK6" s="306"/>
-      <c r="AL6" s="306"/>
-      <c r="AM6" s="306"/>
-      <c r="AN6" s="306"/>
+      <c r="AA6" s="308"/>
+      <c r="AB6" s="308"/>
+      <c r="AC6" s="308"/>
+      <c r="AD6" s="308"/>
+      <c r="AE6" s="308"/>
+      <c r="AF6" s="308"/>
+      <c r="AG6" s="308"/>
+      <c r="AH6" s="308"/>
+      <c r="AI6" s="308"/>
+      <c r="AJ6" s="308"/>
+      <c r="AK6" s="308"/>
+      <c r="AL6" s="308"/>
+      <c r="AM6" s="308"/>
+      <c r="AN6" s="308"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -8264,27 +8598,27 @@
       <c r="V7" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="X7" s="306"/>
-      <c r="Y7" s="306"/>
-      <c r="Z7" s="309" t="s">
+      <c r="X7" s="308"/>
+      <c r="Y7" s="308"/>
+      <c r="Z7" s="307" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="306"/>
-      <c r="AB7" s="306"/>
-      <c r="AC7" s="306"/>
-      <c r="AD7" s="309" t="s">
+      <c r="AA7" s="308"/>
+      <c r="AB7" s="308"/>
+      <c r="AC7" s="308"/>
+      <c r="AD7" s="307" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="306"/>
-      <c r="AF7" s="306"/>
-      <c r="AG7" s="306"/>
-      <c r="AH7" s="306"/>
-      <c r="AI7" s="306"/>
-      <c r="AJ7" s="306"/>
-      <c r="AK7" s="306"/>
-      <c r="AL7" s="306"/>
-      <c r="AM7" s="306"/>
-      <c r="AN7" s="306"/>
+      <c r="AE7" s="308"/>
+      <c r="AF7" s="308"/>
+      <c r="AG7" s="308"/>
+      <c r="AH7" s="308"/>
+      <c r="AI7" s="308"/>
+      <c r="AJ7" s="308"/>
+      <c r="AK7" s="308"/>
+      <c r="AL7" s="308"/>
+      <c r="AM7" s="308"/>
+      <c r="AN7" s="308"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -8334,8 +8668,8 @@
         <v>NO</v>
       </c>
       <c r="V8" s="13"/>
-      <c r="X8" s="306"/>
-      <c r="Y8" s="306"/>
+      <c r="X8" s="308"/>
+      <c r="Y8" s="308"/>
       <c r="Z8" s="153" t="s">
         <v>19</v>
       </c>
@@ -12946,10 +13280,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="307" t="s">
+      <c r="AA49" s="305" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="308"/>
+      <c r="AB49" s="306"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -13027,12 +13361,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="314" t="s">
+      <c r="AI50" s="301" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="315"/>
-      <c r="AK50" s="315"/>
-      <c r="AL50" s="316"/>
+      <c r="AJ50" s="302"/>
+      <c r="AK50" s="302"/>
+      <c r="AL50" s="303"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -13103,12 +13437,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="311" t="s">
+      <c r="AI51" s="298" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="312"/>
-      <c r="AK51" s="312"/>
-      <c r="AL51" s="313"/>
+      <c r="AJ51" s="299"/>
+      <c r="AK51" s="299"/>
+      <c r="AL51" s="300"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -13374,14 +13708,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="317"/>
-      <c r="AD55" s="317"/>
-      <c r="AI55" s="314" t="s">
+      <c r="AC55" s="304"/>
+      <c r="AD55" s="304"/>
+      <c r="AI55" s="301" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="315"/>
-      <c r="AK55" s="315"/>
-      <c r="AL55" s="316"/>
+      <c r="AJ55" s="302"/>
+      <c r="AK55" s="302"/>
+      <c r="AL55" s="303"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -13442,12 +13776,12 @@
         <v>NO</v>
       </c>
       <c r="V56" s="2"/>
-      <c r="AI56" s="296" t="s">
+      <c r="AI56" s="297" t="s">
         <v>168</v>
       </c>
-      <c r="AJ56" s="296"/>
-      <c r="AK56" s="296"/>
-      <c r="AL56" s="296"/>
+      <c r="AJ56" s="297"/>
+      <c r="AK56" s="297"/>
+      <c r="AL56" s="297"/>
       <c r="AM56" s="52">
         <f>AM50-AM55</f>
         <v>450000</v>
@@ -13696,32 +14030,32 @@
     <row r="67" spans="3:19" s="258" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="297" t="s">
+      <c r="C69" s="310" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="298"/>
-      <c r="E69" s="298"/>
-      <c r="F69" s="298"/>
-      <c r="G69" s="299"/>
-      <c r="I69" s="303" t="s">
+      <c r="D69" s="311"/>
+      <c r="E69" s="311"/>
+      <c r="F69" s="311"/>
+      <c r="G69" s="312"/>
+      <c r="I69" s="316" t="s">
         <v>178</v>
       </c>
-      <c r="J69" s="303"/>
-      <c r="K69" s="303"/>
-      <c r="L69" s="303"/>
-      <c r="M69" s="303"/>
+      <c r="J69" s="316"/>
+      <c r="K69" s="316"/>
+      <c r="L69" s="316"/>
+      <c r="M69" s="316"/>
     </row>
     <row r="70" spans="3:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="300"/>
-      <c r="D70" s="301"/>
-      <c r="E70" s="301"/>
-      <c r="F70" s="301"/>
-      <c r="G70" s="302"/>
-      <c r="I70" s="303"/>
-      <c r="J70" s="303"/>
-      <c r="K70" s="303"/>
-      <c r="L70" s="303"/>
-      <c r="M70" s="303"/>
+      <c r="C70" s="313"/>
+      <c r="D70" s="314"/>
+      <c r="E70" s="314"/>
+      <c r="F70" s="314"/>
+      <c r="G70" s="315"/>
+      <c r="I70" s="316"/>
+      <c r="J70" s="316"/>
+      <c r="K70" s="316"/>
+      <c r="L70" s="316"/>
+      <c r="M70" s="316"/>
     </row>
     <row r="71" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13742,10 +14076,10 @@
       <c r="M76" s="55"/>
       <c r="N76" s="55"/>
       <c r="O76" s="55"/>
-      <c r="P76" s="296" t="s">
+      <c r="P76" s="297" t="s">
         <v>214</v>
       </c>
-      <c r="Q76" s="296"/>
+      <c r="Q76" s="297"/>
       <c r="R76" s="55"/>
       <c r="S76" s="55"/>
     </row>
@@ -14212,73 +14546,73 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AI56:AL56"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AI50:AL50"/>
-    <mergeCell ref="AI55:AL55"/>
-    <mergeCell ref="AC55:AD55"/>
-    <mergeCell ref="AA49:AB49"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="AD7:AN7"/>
-    <mergeCell ref="X5:AN5"/>
-    <mergeCell ref="Z6:AN6"/>
     <mergeCell ref="P76:Q76"/>
     <mergeCell ref="C69:G70"/>
     <mergeCell ref="I69:M70"/>
     <mergeCell ref="C2:T3"/>
     <mergeCell ref="Y6:Y8"/>
     <mergeCell ref="X6:X8"/>
+    <mergeCell ref="AA49:AB49"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="AD7:AN7"/>
+    <mergeCell ref="X5:AN5"/>
+    <mergeCell ref="Z6:AN6"/>
+    <mergeCell ref="AI56:AL56"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AI50:AL50"/>
+    <mergeCell ref="AI55:AL55"/>
+    <mergeCell ref="AC55:AD55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:V61">
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="18" priority="7">
       <formula>IF(ISBLANK($B$4), 0, SEARCH($B$4,$B6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK48">
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH(("YES"),(AK9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK48">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH(("NO"),(AK9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y9:AN9 Y46:AC46 AD46:AL48 AC47:AC48 Y10:AL45 AM10:AN48">
-    <cfRule type="expression" dxfId="7" priority="10">
+    <cfRule type="expression" dxfId="15" priority="10">
       <formula>IF(ISBLANK($Z$4), 0, SEARCH($Z$4,$Y9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6:U61">
-    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH(("NO"),(U6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6:U61">
-    <cfRule type="containsText" dxfId="5" priority="12" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH(("OK"),(U6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y10:Y45">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>IF(AK10="YES",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q6:R61">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6:P61">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y9:AN48">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>IF(ISBLANK($AA$4), 0, SEARCH($AA$4,$Y9))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14291,8 +14625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="H16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14312,86 +14646,86 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="318" t="s">
+      <c r="A2" s="319" t="s">
         <v>301</v>
       </c>
-      <c r="B2" s="318"/>
-      <c r="C2" s="318"/>
-      <c r="D2" s="318"/>
-      <c r="E2" s="318"/>
-      <c r="F2" s="318"/>
-      <c r="G2" s="318"/>
-      <c r="H2" s="318"/>
-      <c r="I2" s="318"/>
-      <c r="J2" s="318"/>
-      <c r="K2" s="318"/>
-      <c r="L2" s="318"/>
+      <c r="B2" s="319"/>
+      <c r="C2" s="319"/>
+      <c r="D2" s="319"/>
+      <c r="E2" s="319"/>
+      <c r="F2" s="319"/>
+      <c r="G2" s="319"/>
+      <c r="H2" s="319"/>
+      <c r="I2" s="319"/>
+      <c r="J2" s="319"/>
+      <c r="K2" s="319"/>
+      <c r="L2" s="319"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="318"/>
-      <c r="B3" s="318"/>
-      <c r="C3" s="318"/>
-      <c r="D3" s="318"/>
-      <c r="E3" s="318"/>
-      <c r="F3" s="318"/>
-      <c r="G3" s="318"/>
-      <c r="H3" s="318"/>
-      <c r="I3" s="318"/>
-      <c r="J3" s="318"/>
-      <c r="K3" s="318"/>
-      <c r="L3" s="318"/>
+      <c r="A3" s="319"/>
+      <c r="B3" s="319"/>
+      <c r="C3" s="319"/>
+      <c r="D3" s="319"/>
+      <c r="E3" s="319"/>
+      <c r="F3" s="319"/>
+      <c r="G3" s="319"/>
+      <c r="H3" s="319"/>
+      <c r="I3" s="319"/>
+      <c r="J3" s="319"/>
+      <c r="K3" s="319"/>
+      <c r="L3" s="319"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="303" t="s">
+      <c r="A5" s="316" t="s">
         <v>304</v>
       </c>
-      <c r="B5" s="303"/>
-      <c r="C5" s="303"/>
-      <c r="D5" s="303"/>
-      <c r="E5" s="303"/>
-      <c r="F5" s="303"/>
-      <c r="G5" s="303"/>
-      <c r="H5" s="303"/>
-      <c r="I5" s="303"/>
-      <c r="J5" s="303"/>
-      <c r="K5" s="303"/>
-      <c r="M5" s="303" t="s">
+      <c r="B5" s="316"/>
+      <c r="C5" s="316"/>
+      <c r="D5" s="316"/>
+      <c r="E5" s="316"/>
+      <c r="F5" s="316"/>
+      <c r="G5" s="316"/>
+      <c r="H5" s="316"/>
+      <c r="I5" s="316"/>
+      <c r="J5" s="316"/>
+      <c r="K5" s="316"/>
+      <c r="M5" s="316" t="s">
         <v>325</v>
       </c>
-      <c r="N5" s="303"/>
-      <c r="O5" s="303"/>
-      <c r="P5" s="303"/>
-      <c r="Q5" s="303"/>
-      <c r="R5" s="303"/>
-      <c r="S5" s="303"/>
-      <c r="T5" s="303"/>
-      <c r="U5" s="303"/>
-      <c r="V5" s="303"/>
-      <c r="W5" s="303"/>
+      <c r="N5" s="316"/>
+      <c r="O5" s="316"/>
+      <c r="P5" s="316"/>
+      <c r="Q5" s="316"/>
+      <c r="R5" s="316"/>
+      <c r="S5" s="316"/>
+      <c r="T5" s="316"/>
+      <c r="U5" s="316"/>
+      <c r="V5" s="316"/>
+      <c r="W5" s="316"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="303"/>
-      <c r="B6" s="303"/>
-      <c r="C6" s="303"/>
-      <c r="D6" s="303"/>
-      <c r="E6" s="303"/>
-      <c r="F6" s="303"/>
-      <c r="G6" s="303"/>
-      <c r="H6" s="303"/>
-      <c r="I6" s="303"/>
-      <c r="J6" s="303"/>
-      <c r="K6" s="303"/>
-      <c r="M6" s="303"/>
-      <c r="N6" s="303"/>
-      <c r="O6" s="303"/>
-      <c r="P6" s="303"/>
-      <c r="Q6" s="303"/>
-      <c r="R6" s="303"/>
-      <c r="S6" s="303"/>
-      <c r="T6" s="303"/>
-      <c r="U6" s="303"/>
-      <c r="V6" s="303"/>
-      <c r="W6" s="303"/>
+      <c r="A6" s="316"/>
+      <c r="B6" s="316"/>
+      <c r="C6" s="316"/>
+      <c r="D6" s="316"/>
+      <c r="E6" s="316"/>
+      <c r="F6" s="316"/>
+      <c r="G6" s="316"/>
+      <c r="H6" s="316"/>
+      <c r="I6" s="316"/>
+      <c r="J6" s="316"/>
+      <c r="K6" s="316"/>
+      <c r="M6" s="316"/>
+      <c r="N6" s="316"/>
+      <c r="O6" s="316"/>
+      <c r="P6" s="316"/>
+      <c r="Q6" s="316"/>
+      <c r="R6" s="316"/>
+      <c r="S6" s="316"/>
+      <c r="T6" s="316"/>
+      <c r="U6" s="316"/>
+      <c r="V6" s="316"/>
+      <c r="W6" s="316"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M7" s="251"/>
@@ -15132,9 +15466,16 @@
       <c r="N28" s="1">
         <v>20</v>
       </c>
-      <c r="O28" s="218"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="212"/>
+      <c r="O28" s="431" t="s">
+        <v>123</v>
+      </c>
+      <c r="P28" s="276" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q28" s="212">
+        <f>'Pembayaran Makrab 19'!F40</f>
+        <v>500000</v>
+      </c>
       <c r="R28" s="212"/>
       <c r="S28" s="251"/>
       <c r="T28" s="251"/>
@@ -15248,8 +15589,8 @@
       <c r="N33" s="1">
         <v>25</v>
       </c>
-      <c r="O33" s="218">
-        <v>43770</v>
+      <c r="O33" s="211" t="s">
+        <v>361</v>
       </c>
       <c r="P33" s="252" t="s">
         <v>300</v>
@@ -15280,15 +15621,15 @@
       </c>
       <c r="M34" s="251"/>
       <c r="N34" s="196"/>
-      <c r="O34" s="223">
-        <v>43770</v>
+      <c r="O34" s="433" t="s">
+        <v>361</v>
       </c>
       <c r="P34" s="224" t="s">
         <v>317</v>
       </c>
       <c r="Q34" s="225">
         <f>SUM(Q9:Q33)</f>
-        <v>3581144.27</v>
+        <v>4081144.27</v>
       </c>
       <c r="R34" s="226">
         <f>SUM(R9:R33)</f>
@@ -15301,27 +15642,27 @@
       <c r="W34" s="251"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B35" s="323" t="s">
+      <c r="B35" s="324" t="s">
         <v>313</v>
       </c>
-      <c r="C35" s="324"/>
-      <c r="D35" s="325"/>
-      <c r="E35" s="319">
+      <c r="C35" s="325"/>
+      <c r="D35" s="326"/>
+      <c r="E35" s="320">
         <f>E34-F34</f>
         <v>2610871.1799999997</v>
       </c>
-      <c r="F35" s="320"/>
+      <c r="F35" s="321"/>
       <c r="M35" s="251"/>
-      <c r="N35" s="323" t="s">
+      <c r="N35" s="324" t="s">
         <v>313</v>
       </c>
-      <c r="O35" s="324"/>
-      <c r="P35" s="325"/>
-      <c r="Q35" s="319">
+      <c r="O35" s="325"/>
+      <c r="P35" s="326"/>
+      <c r="Q35" s="320">
         <f>Q34-R34</f>
-        <v>3006144.27</v>
-      </c>
-      <c r="R35" s="320"/>
+        <v>3506144.27</v>
+      </c>
+      <c r="R35" s="321"/>
       <c r="S35" s="251"/>
       <c r="T35" s="251"/>
       <c r="U35" s="251"/>
@@ -15329,17 +15670,17 @@
       <c r="W35" s="251"/>
     </row>
     <row r="36" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="326"/>
-      <c r="C36" s="327"/>
-      <c r="D36" s="328"/>
-      <c r="E36" s="321"/>
-      <c r="F36" s="322"/>
+      <c r="B36" s="327"/>
+      <c r="C36" s="328"/>
+      <c r="D36" s="329"/>
+      <c r="E36" s="322"/>
+      <c r="F36" s="323"/>
       <c r="M36" s="251"/>
-      <c r="N36" s="326"/>
-      <c r="O36" s="327"/>
-      <c r="P36" s="328"/>
-      <c r="Q36" s="321"/>
-      <c r="R36" s="322"/>
+      <c r="N36" s="327"/>
+      <c r="O36" s="328"/>
+      <c r="P36" s="329"/>
+      <c r="Q36" s="322"/>
+      <c r="R36" s="323"/>
       <c r="S36" s="251"/>
       <c r="T36" s="251"/>
       <c r="U36" s="251"/>
@@ -15362,6 +15703,433 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>351</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="428" t="s">
+        <v>352</v>
+      </c>
+      <c r="F3" s="57" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="57">
+        <v>1</v>
+      </c>
+      <c r="C4" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="D4" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="E4" s="57" t="s">
+        <v>355</v>
+      </c>
+      <c r="F4" s="56">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="57">
+        <v>2</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>356</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>354</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>355</v>
+      </c>
+      <c r="F5" s="56">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="57">
+        <v>3</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>357</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>354</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>358</v>
+      </c>
+      <c r="F6" s="56">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="57">
+        <v>4</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>359</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>354</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>358</v>
+      </c>
+      <c r="F7" s="56">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="57">
+        <v>5</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="56"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="57">
+        <v>6</v>
+      </c>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="56"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="57">
+        <v>7</v>
+      </c>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="56"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="57">
+        <v>8</v>
+      </c>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="56"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="57">
+        <v>9</v>
+      </c>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="56"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="57">
+        <v>10</v>
+      </c>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="56"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="57">
+        <v>11</v>
+      </c>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="56"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="57">
+        <v>12</v>
+      </c>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="56"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="57">
+        <v>13</v>
+      </c>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="56"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="57">
+        <v>14</v>
+      </c>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="56"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="57">
+        <v>15</v>
+      </c>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="56"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="57">
+        <v>16</v>
+      </c>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="56"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="57">
+        <v>17</v>
+      </c>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="56"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="57">
+        <v>18</v>
+      </c>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="56"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="57">
+        <v>19</v>
+      </c>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="56"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="57">
+        <v>20</v>
+      </c>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="56"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="57">
+        <v>21</v>
+      </c>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="56"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="57">
+        <v>22</v>
+      </c>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="56"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="57">
+        <v>23</v>
+      </c>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="56"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="57">
+        <v>24</v>
+      </c>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="56"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="57">
+        <v>25</v>
+      </c>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="56"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="57">
+        <v>26</v>
+      </c>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="56"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="57">
+        <v>27</v>
+      </c>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="56"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="57">
+        <v>28</v>
+      </c>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="56"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="57">
+        <v>29</v>
+      </c>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="56"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="57">
+        <v>30</v>
+      </c>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="56"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="57">
+        <v>31</v>
+      </c>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="56"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="57">
+        <v>32</v>
+      </c>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="56"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="57">
+        <v>33</v>
+      </c>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="56"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="57">
+        <v>34</v>
+      </c>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="56"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="57">
+        <v>35</v>
+      </c>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="56"/>
+    </row>
+    <row r="39" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="143">
+        <v>36</v>
+      </c>
+      <c r="C39" s="143"/>
+      <c r="D39" s="143"/>
+      <c r="E39" s="143"/>
+      <c r="F39" s="56"/>
+    </row>
+    <row r="40" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="429" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="430"/>
+      <c r="D40" s="430"/>
+      <c r="E40" s="427"/>
+      <c r="F40" s="432">
+        <f>SUM(F4:F39)</f>
+        <v>500000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B40:E40"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D4:D39">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="MABA">
+      <formula>NOT(ISERROR(SEARCH("MABA",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="SENIOR">
+      <formula>NOT(ISERROR(SEARCH("SENIOR",D4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E39">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Transfer">
+      <formula>NOT(ISERROR(SEARCH("Transfer",E4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Tunai">
+      <formula>NOT(ISERROR(SEARCH("Tunai",E4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD28"/>
   <sheetViews>
@@ -15388,17 +16156,17 @@
       <c r="A2" s="174"/>
       <c r="B2" s="175"/>
       <c r="C2" s="175"/>
-      <c r="D2" s="386" t="s">
+      <c r="D2" s="330" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="386"/>
-      <c r="F2" s="386"/>
-      <c r="G2" s="386"/>
-      <c r="H2" s="386"/>
-      <c r="I2" s="386"/>
-      <c r="J2" s="386"/>
-      <c r="K2" s="386"/>
-      <c r="L2" s="386"/>
+      <c r="E2" s="330"/>
+      <c r="F2" s="330"/>
+      <c r="G2" s="330"/>
+      <c r="H2" s="330"/>
+      <c r="I2" s="330"/>
+      <c r="J2" s="330"/>
+      <c r="K2" s="330"/>
+      <c r="L2" s="330"/>
       <c r="M2" s="176"/>
       <c r="N2" s="24"/>
     </row>
@@ -15416,205 +16184,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="178"/>
-      <c r="U3" s="329" t="s">
+      <c r="U3" s="380" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="330"/>
-      <c r="W3" s="331" t="s">
+      <c r="V3" s="381"/>
+      <c r="W3" s="382" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="330"/>
-      <c r="Y3" s="330"/>
-      <c r="Z3" s="330"/>
-      <c r="AA3" s="330"/>
-      <c r="AB3" s="330"/>
-      <c r="AC3" s="330"/>
-      <c r="AD3" s="332"/>
+      <c r="X3" s="381"/>
+      <c r="Y3" s="381"/>
+      <c r="Z3" s="381"/>
+      <c r="AA3" s="381"/>
+      <c r="AB3" s="381"/>
+      <c r="AC3" s="381"/>
+      <c r="AD3" s="383"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="177"/>
-      <c r="B4" s="390" t="s">
+      <c r="B4" s="345" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="391"/>
-      <c r="D4" s="391"/>
-      <c r="E4" s="391"/>
-      <c r="F4" s="391"/>
+      <c r="C4" s="346"/>
+      <c r="D4" s="346"/>
+      <c r="E4" s="346"/>
+      <c r="F4" s="346"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="338" t="s">
+      <c r="I4" s="349" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="309"/>
-      <c r="K4" s="309"/>
-      <c r="L4" s="309"/>
+      <c r="J4" s="307"/>
+      <c r="K4" s="307"/>
+      <c r="L4" s="307"/>
       <c r="M4" s="178"/>
-      <c r="U4" s="350" t="s">
+      <c r="U4" s="392" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="309"/>
-      <c r="W4" s="338" t="s">
+      <c r="V4" s="307"/>
+      <c r="W4" s="349" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="309"/>
-      <c r="Y4" s="309"/>
-      <c r="Z4" s="309"/>
-      <c r="AA4" s="309"/>
-      <c r="AB4" s="309"/>
-      <c r="AC4" s="309"/>
-      <c r="AD4" s="333"/>
+      <c r="X4" s="307"/>
+      <c r="Y4" s="307"/>
+      <c r="Z4" s="307"/>
+      <c r="AA4" s="307"/>
+      <c r="AB4" s="307"/>
+      <c r="AC4" s="307"/>
+      <c r="AD4" s="369"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="177"/>
-      <c r="B5" s="355" t="s">
+      <c r="B5" s="340" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="309"/>
-      <c r="D5" s="309"/>
-      <c r="E5" s="309"/>
-      <c r="F5" s="309"/>
+      <c r="C5" s="307"/>
+      <c r="D5" s="307"/>
+      <c r="E5" s="307"/>
+      <c r="F5" s="307"/>
       <c r="G5" s="154">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="357" t="s">
+      <c r="I5" s="338" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="378"/>
-      <c r="K5" s="380">
+      <c r="J5" s="339"/>
+      <c r="K5" s="350">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="381"/>
+      <c r="L5" s="351"/>
       <c r="M5" s="178"/>
-      <c r="U5" s="351" t="s">
+      <c r="U5" s="376" t="s">
         <v>231</v>
       </c>
-      <c r="V5" s="352"/>
-      <c r="W5" s="357" t="s">
+      <c r="V5" s="377"/>
+      <c r="W5" s="338" t="s">
         <v>232</v>
       </c>
-      <c r="X5" s="358"/>
-      <c r="Y5" s="358"/>
-      <c r="Z5" s="358"/>
-      <c r="AA5" s="358"/>
-      <c r="AB5" s="358"/>
-      <c r="AC5" s="358"/>
-      <c r="AD5" s="359"/>
+      <c r="X5" s="363"/>
+      <c r="Y5" s="363"/>
+      <c r="Z5" s="363"/>
+      <c r="AA5" s="363"/>
+      <c r="AB5" s="363"/>
+      <c r="AC5" s="363"/>
+      <c r="AD5" s="364"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="177"/>
-      <c r="B6" s="348" t="s">
+      <c r="B6" s="332" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="349"/>
-      <c r="D6" s="349"/>
-      <c r="E6" s="349"/>
-      <c r="F6" s="349"/>
+      <c r="C6" s="333"/>
+      <c r="D6" s="333"/>
+      <c r="E6" s="333"/>
+      <c r="F6" s="333"/>
       <c r="G6" s="154">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="379" t="s">
+      <c r="I6" s="336" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="374"/>
-      <c r="K6" s="382">
+      <c r="J6" s="337"/>
+      <c r="K6" s="352">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="383"/>
+      <c r="L6" s="353"/>
       <c r="M6" s="178"/>
-      <c r="U6" s="353"/>
-      <c r="V6" s="354"/>
-      <c r="W6" s="339" t="s">
+      <c r="U6" s="378"/>
+      <c r="V6" s="379"/>
+      <c r="W6" s="365" t="s">
         <v>233</v>
       </c>
-      <c r="X6" s="340"/>
-      <c r="Y6" s="340"/>
-      <c r="Z6" s="340"/>
-      <c r="AA6" s="340"/>
-      <c r="AB6" s="340"/>
-      <c r="AC6" s="340"/>
-      <c r="AD6" s="341"/>
+      <c r="X6" s="366"/>
+      <c r="Y6" s="366"/>
+      <c r="Z6" s="366"/>
+      <c r="AA6" s="366"/>
+      <c r="AB6" s="366"/>
+      <c r="AC6" s="366"/>
+      <c r="AD6" s="367"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="177"/>
-      <c r="B7" s="360" t="s">
+      <c r="B7" s="343" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="361"/>
-      <c r="D7" s="361"/>
-      <c r="E7" s="361"/>
-      <c r="F7" s="374"/>
+      <c r="C7" s="344"/>
+      <c r="D7" s="344"/>
+      <c r="E7" s="344"/>
+      <c r="F7" s="337"/>
       <c r="G7" s="154">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="379" t="s">
+      <c r="I7" s="336" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="374"/>
-      <c r="K7" s="384">
+      <c r="J7" s="337"/>
+      <c r="K7" s="347">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="385"/>
+      <c r="L7" s="348"/>
       <c r="M7" s="178"/>
-      <c r="U7" s="336"/>
-      <c r="V7" s="337"/>
-      <c r="W7" s="338" t="s">
+      <c r="U7" s="384"/>
+      <c r="V7" s="385"/>
+      <c r="W7" s="349" t="s">
         <v>234</v>
       </c>
-      <c r="X7" s="309"/>
-      <c r="Y7" s="309"/>
-      <c r="Z7" s="309"/>
-      <c r="AA7" s="309"/>
-      <c r="AB7" s="309"/>
-      <c r="AC7" s="309"/>
-      <c r="AD7" s="333"/>
+      <c r="X7" s="307"/>
+      <c r="Y7" s="307"/>
+      <c r="Z7" s="307"/>
+      <c r="AA7" s="307"/>
+      <c r="AB7" s="307"/>
+      <c r="AC7" s="307"/>
+      <c r="AD7" s="369"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="177"/>
-      <c r="B8" s="388" t="s">
+      <c r="B8" s="341" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="389"/>
-      <c r="D8" s="389"/>
-      <c r="E8" s="389"/>
-      <c r="F8" s="389"/>
+      <c r="C8" s="342"/>
+      <c r="D8" s="342"/>
+      <c r="E8" s="342"/>
+      <c r="F8" s="342"/>
       <c r="G8" s="155">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="357" t="s">
+      <c r="I8" s="338" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="378"/>
-      <c r="K8" s="369">
+      <c r="J8" s="339"/>
+      <c r="K8" s="334">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="370"/>
+      <c r="L8" s="335"/>
       <c r="M8" s="178"/>
-      <c r="U8" s="344" t="s">
+      <c r="U8" s="388" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="345"/>
-      <c r="W8" s="339" t="s">
+      <c r="V8" s="389"/>
+      <c r="W8" s="365" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="340"/>
-      <c r="Y8" s="340"/>
-      <c r="Z8" s="340"/>
-      <c r="AA8" s="340"/>
-      <c r="AB8" s="340"/>
-      <c r="AC8" s="340"/>
-      <c r="AD8" s="341"/>
+      <c r="X8" s="366"/>
+      <c r="Y8" s="366"/>
+      <c r="Z8" s="366"/>
+      <c r="AA8" s="366"/>
+      <c r="AB8" s="366"/>
+      <c r="AC8" s="366"/>
+      <c r="AD8" s="367"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="177"/>
@@ -15630,28 +16398,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="178"/>
-      <c r="U9" s="346"/>
-      <c r="V9" s="347"/>
-      <c r="W9" s="339" t="s">
+      <c r="U9" s="390"/>
+      <c r="V9" s="391"/>
+      <c r="W9" s="365" t="s">
         <v>237</v>
       </c>
-      <c r="X9" s="340"/>
-      <c r="Y9" s="340"/>
-      <c r="Z9" s="340"/>
-      <c r="AA9" s="340"/>
-      <c r="AB9" s="340"/>
-      <c r="AC9" s="340"/>
-      <c r="AD9" s="341"/>
+      <c r="X9" s="366"/>
+      <c r="Y9" s="366"/>
+      <c r="Z9" s="366"/>
+      <c r="AA9" s="366"/>
+      <c r="AB9" s="366"/>
+      <c r="AC9" s="366"/>
+      <c r="AD9" s="367"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="177"/>
-      <c r="B10" s="309" t="s">
+      <c r="B10" s="307" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="309"/>
-      <c r="D10" s="309"/>
-      <c r="E10" s="309"/>
-      <c r="F10" s="309"/>
+      <c r="C10" s="307"/>
+      <c r="D10" s="307"/>
+      <c r="E10" s="307"/>
+      <c r="F10" s="307"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -15662,30 +16430,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="178"/>
-      <c r="U10" s="348" t="s">
+      <c r="U10" s="332" t="s">
         <v>243</v>
       </c>
-      <c r="V10" s="349"/>
-      <c r="W10" s="309" t="s">
+      <c r="V10" s="333"/>
+      <c r="W10" s="307" t="s">
         <v>257</v>
       </c>
-      <c r="X10" s="309"/>
-      <c r="Y10" s="309"/>
-      <c r="Z10" s="309"/>
-      <c r="AA10" s="309"/>
-      <c r="AB10" s="309"/>
-      <c r="AC10" s="309"/>
-      <c r="AD10" s="333"/>
+      <c r="X10" s="307"/>
+      <c r="Y10" s="307"/>
+      <c r="Z10" s="307"/>
+      <c r="AA10" s="307"/>
+      <c r="AB10" s="307"/>
+      <c r="AC10" s="307"/>
+      <c r="AD10" s="369"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="177"/>
-      <c r="B11" s="309" t="s">
+      <c r="B11" s="307" t="s">
         <v>254</v>
       </c>
-      <c r="C11" s="309"/>
-      <c r="D11" s="309"/>
-      <c r="E11" s="309"/>
-      <c r="F11" s="309"/>
+      <c r="C11" s="307"/>
+      <c r="D11" s="307"/>
+      <c r="E11" s="307"/>
+      <c r="F11" s="307"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -15695,30 +16463,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="178"/>
-      <c r="U11" s="348" t="s">
+      <c r="U11" s="332" t="s">
         <v>256</v>
       </c>
-      <c r="V11" s="349"/>
-      <c r="W11" s="342" t="s">
+      <c r="V11" s="333"/>
+      <c r="W11" s="386" t="s">
         <v>258</v>
       </c>
-      <c r="X11" s="342"/>
-      <c r="Y11" s="342"/>
-      <c r="Z11" s="342"/>
-      <c r="AA11" s="342"/>
-      <c r="AB11" s="342"/>
-      <c r="AC11" s="342"/>
-      <c r="AD11" s="343"/>
+      <c r="X11" s="386"/>
+      <c r="Y11" s="386"/>
+      <c r="Z11" s="386"/>
+      <c r="AA11" s="386"/>
+      <c r="AB11" s="386"/>
+      <c r="AC11" s="386"/>
+      <c r="AD11" s="387"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="177"/>
-      <c r="B12" s="387" t="s">
+      <c r="B12" s="331" t="s">
         <v>255</v>
       </c>
-      <c r="C12" s="387"/>
-      <c r="D12" s="387"/>
-      <c r="E12" s="387"/>
-      <c r="F12" s="387"/>
+      <c r="C12" s="331"/>
+      <c r="D12" s="331"/>
+      <c r="E12" s="331"/>
+      <c r="F12" s="331"/>
       <c r="G12" s="182">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -15729,16 +16497,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="178"/>
-      <c r="U12" s="348"/>
-      <c r="V12" s="349"/>
-      <c r="W12" s="309"/>
-      <c r="X12" s="309"/>
-      <c r="Y12" s="309"/>
-      <c r="Z12" s="309"/>
-      <c r="AA12" s="309"/>
-      <c r="AB12" s="309"/>
-      <c r="AC12" s="309"/>
-      <c r="AD12" s="333"/>
+      <c r="U12" s="332"/>
+      <c r="V12" s="333"/>
+      <c r="W12" s="307"/>
+      <c r="X12" s="307"/>
+      <c r="Y12" s="307"/>
+      <c r="Z12" s="307"/>
+      <c r="AA12" s="307"/>
+      <c r="AB12" s="307"/>
+      <c r="AC12" s="307"/>
+      <c r="AD12" s="369"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="179"/>
@@ -15754,64 +16522,64 @@
       <c r="K13" s="180"/>
       <c r="L13" s="180"/>
       <c r="M13" s="181"/>
-      <c r="U13" s="348"/>
-      <c r="V13" s="349"/>
-      <c r="W13" s="309"/>
-      <c r="X13" s="309"/>
-      <c r="Y13" s="309"/>
-      <c r="Z13" s="309"/>
-      <c r="AA13" s="309"/>
-      <c r="AB13" s="309"/>
-      <c r="AC13" s="309"/>
-      <c r="AD13" s="333"/>
+      <c r="U13" s="332"/>
+      <c r="V13" s="333"/>
+      <c r="W13" s="307"/>
+      <c r="X13" s="307"/>
+      <c r="Y13" s="307"/>
+      <c r="Z13" s="307"/>
+      <c r="AA13" s="307"/>
+      <c r="AB13" s="307"/>
+      <c r="AC13" s="307"/>
+      <c r="AD13" s="369"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="363"/>
-      <c r="V14" s="364"/>
-      <c r="W14" s="334"/>
-      <c r="X14" s="334"/>
-      <c r="Y14" s="334"/>
-      <c r="Z14" s="334"/>
-      <c r="AA14" s="334"/>
-      <c r="AB14" s="334"/>
-      <c r="AC14" s="334"/>
-      <c r="AD14" s="335"/>
+      <c r="U14" s="370"/>
+      <c r="V14" s="371"/>
+      <c r="W14" s="361"/>
+      <c r="X14" s="361"/>
+      <c r="Y14" s="361"/>
+      <c r="Z14" s="361"/>
+      <c r="AA14" s="361"/>
+      <c r="AB14" s="361"/>
+      <c r="AC14" s="361"/>
+      <c r="AD14" s="362"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="174"/>
       <c r="B18" s="175"/>
       <c r="C18" s="175"/>
-      <c r="D18" s="386" t="s">
+      <c r="D18" s="330" t="s">
         <v>249</v>
       </c>
-      <c r="E18" s="386"/>
-      <c r="F18" s="386"/>
-      <c r="G18" s="386"/>
-      <c r="H18" s="386"/>
-      <c r="I18" s="386"/>
-      <c r="J18" s="386"/>
-      <c r="K18" s="386"/>
-      <c r="L18" s="386"/>
+      <c r="E18" s="330"/>
+      <c r="F18" s="330"/>
+      <c r="G18" s="330"/>
+      <c r="H18" s="330"/>
+      <c r="I18" s="330"/>
+      <c r="J18" s="330"/>
+      <c r="K18" s="330"/>
+      <c r="L18" s="330"/>
       <c r="M18" s="176"/>
-      <c r="O18" s="365" t="s">
+      <c r="O18" s="372" t="s">
         <v>250</v>
       </c>
-      <c r="P18" s="366"/>
-      <c r="Q18" s="366"/>
-      <c r="R18" s="366"/>
-      <c r="S18" s="367"/>
+      <c r="P18" s="373"/>
+      <c r="Q18" s="373"/>
+      <c r="R18" s="373"/>
+      <c r="S18" s="374"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="177"/>
       <c r="M19" s="178"/>
-      <c r="O19" s="355" t="s">
+      <c r="O19" s="340" t="s">
         <v>251</v>
       </c>
-      <c r="P19" s="309"/>
-      <c r="Q19" s="309"/>
-      <c r="R19" s="309"/>
-      <c r="S19" s="333"/>
+      <c r="P19" s="307"/>
+      <c r="Q19" s="307"/>
+      <c r="R19" s="307"/>
+      <c r="S19" s="369"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="177"/>
@@ -15822,119 +16590,119 @@
       <c r="F20" s="202"/>
       <c r="G20" s="68"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="338" t="s">
+      <c r="I20" s="349" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="309"/>
-      <c r="K20" s="309"/>
-      <c r="L20" s="309"/>
+      <c r="J20" s="307"/>
+      <c r="K20" s="307"/>
+      <c r="L20" s="307"/>
       <c r="M20" s="178"/>
-      <c r="O20" s="355" t="s">
+      <c r="O20" s="340" t="s">
         <v>252</v>
       </c>
-      <c r="P20" s="309"/>
-      <c r="Q20" s="309"/>
-      <c r="R20" s="309"/>
-      <c r="S20" s="333"/>
+      <c r="P20" s="307"/>
+      <c r="Q20" s="307"/>
+      <c r="R20" s="307"/>
+      <c r="S20" s="369"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="177"/>
-      <c r="B21" s="371" t="s">
+      <c r="B21" s="354" t="s">
         <v>297</v>
       </c>
-      <c r="C21" s="372"/>
-      <c r="D21" s="372"/>
-      <c r="E21" s="372"/>
-      <c r="F21" s="373"/>
+      <c r="C21" s="355"/>
+      <c r="D21" s="355"/>
+      <c r="E21" s="355"/>
+      <c r="F21" s="356"/>
       <c r="G21" s="70">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="357" t="s">
+      <c r="I21" s="338" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="378"/>
-      <c r="K21" s="380">
+      <c r="J21" s="339"/>
+      <c r="K21" s="350">
         <f>G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="L21" s="381"/>
+      <c r="L21" s="351"/>
       <c r="M21" s="178"/>
       <c r="N21" s="172"/>
-      <c r="O21" s="368" t="s">
+      <c r="O21" s="375" t="s">
         <v>259</v>
       </c>
-      <c r="P21" s="358"/>
-      <c r="Q21" s="358"/>
-      <c r="R21" s="358"/>
-      <c r="S21" s="359"/>
+      <c r="P21" s="363"/>
+      <c r="Q21" s="363"/>
+      <c r="R21" s="363"/>
+      <c r="S21" s="364"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="177"/>
-      <c r="B22" s="360" t="s">
+      <c r="B22" s="343" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="361"/>
-      <c r="D22" s="361"/>
-      <c r="E22" s="361"/>
-      <c r="F22" s="374"/>
+      <c r="C22" s="344"/>
+      <c r="D22" s="344"/>
+      <c r="E22" s="344"/>
+      <c r="F22" s="337"/>
       <c r="G22" s="154">
         <f>G21</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="379" t="s">
+      <c r="I22" s="336" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="374"/>
-      <c r="K22" s="382">
+      <c r="J22" s="337"/>
+      <c r="K22" s="352">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="L22" s="383"/>
+      <c r="L22" s="353"/>
       <c r="M22" s="178"/>
       <c r="N22" s="172"/>
-      <c r="O22" s="360" t="s">
+      <c r="O22" s="343" t="s">
         <v>260</v>
       </c>
-      <c r="P22" s="361"/>
-      <c r="Q22" s="361"/>
-      <c r="R22" s="361"/>
-      <c r="S22" s="362"/>
+      <c r="P22" s="344"/>
+      <c r="Q22" s="344"/>
+      <c r="R22" s="344"/>
+      <c r="S22" s="368"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="177"/>
-      <c r="B23" s="375" t="s">
+      <c r="B23" s="357" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="376"/>
-      <c r="D23" s="376"/>
-      <c r="E23" s="376"/>
-      <c r="F23" s="377"/>
+      <c r="C23" s="358"/>
+      <c r="D23" s="358"/>
+      <c r="E23" s="358"/>
+      <c r="F23" s="359"/>
       <c r="G23" s="155">
         <f>K24</f>
         <v>1568729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="379" t="s">
+      <c r="I23" s="336" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="374"/>
-      <c r="K23" s="384">
+      <c r="J23" s="337"/>
+      <c r="K23" s="347">
         <f>Pemasukkan!L31</f>
         <v>690000</v>
       </c>
-      <c r="L23" s="385"/>
+      <c r="L23" s="348"/>
       <c r="M23" s="178"/>
       <c r="N23" s="172"/>
-      <c r="O23" s="360" t="s">
+      <c r="O23" s="343" t="s">
         <v>261</v>
       </c>
-      <c r="P23" s="361"/>
-      <c r="Q23" s="361"/>
-      <c r="R23" s="361"/>
-      <c r="S23" s="362"/>
+      <c r="P23" s="344"/>
+      <c r="Q23" s="344"/>
+      <c r="R23" s="344"/>
+      <c r="S23" s="368"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="177"/>
@@ -15945,24 +16713,24 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="357" t="s">
+      <c r="I24" s="338" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="378"/>
-      <c r="K24" s="369">
+      <c r="J24" s="339"/>
+      <c r="K24" s="334">
         <f>(K21-K22)+K23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="L24" s="370"/>
+      <c r="L24" s="335"/>
       <c r="M24" s="178"/>
       <c r="N24" s="172"/>
-      <c r="O24" s="360" t="s">
+      <c r="O24" s="343" t="s">
         <v>262</v>
       </c>
-      <c r="P24" s="361"/>
-      <c r="Q24" s="361"/>
-      <c r="R24" s="361"/>
-      <c r="S24" s="362"/>
+      <c r="P24" s="344"/>
+      <c r="Q24" s="344"/>
+      <c r="R24" s="344"/>
+      <c r="S24" s="368"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="177"/>
@@ -15979,13 +16747,13 @@
       <c r="L25" s="24"/>
       <c r="M25" s="178"/>
       <c r="N25" s="172"/>
-      <c r="O25" s="355" t="s">
+      <c r="O25" s="340" t="s">
         <v>267</v>
       </c>
-      <c r="P25" s="309"/>
-      <c r="Q25" s="309"/>
-      <c r="R25" s="309"/>
-      <c r="S25" s="333"/>
+      <c r="P25" s="307"/>
+      <c r="Q25" s="307"/>
+      <c r="R25" s="307"/>
+      <c r="S25" s="369"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="177"/>
@@ -16002,11 +16770,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="178"/>
       <c r="N26" s="172"/>
-      <c r="O26" s="356"/>
-      <c r="P26" s="334"/>
-      <c r="Q26" s="334"/>
-      <c r="R26" s="334"/>
-      <c r="S26" s="335"/>
+      <c r="O26" s="360"/>
+      <c r="P26" s="361"/>
+      <c r="Q26" s="361"/>
+      <c r="R26" s="361"/>
+      <c r="S26" s="362"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="179"/>
@@ -16041,6 +16809,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:AD3"/>
+    <mergeCell ref="W12:AD12"/>
+    <mergeCell ref="W13:AD13"/>
+    <mergeCell ref="W14:AD14"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:AD7"/>
+    <mergeCell ref="W9:AD9"/>
+    <mergeCell ref="W10:AD10"/>
+    <mergeCell ref="W11:AD11"/>
+    <mergeCell ref="U8:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:AD4"/>
+    <mergeCell ref="W8:AD8"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="O25:S25"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="W5:AD5"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="O18:S18"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O23:S23"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
     <mergeCell ref="D2:L2"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
@@ -16057,53 +16872,6 @@
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="W5:AD5"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="O24:S24"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="O18:S18"/>
-    <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O23:S23"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="W4:AD4"/>
-    <mergeCell ref="W8:AD8"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="O25:S25"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:AD3"/>
-    <mergeCell ref="W12:AD12"/>
-    <mergeCell ref="W13:AD13"/>
-    <mergeCell ref="W14:AD14"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="W7:AD7"/>
-    <mergeCell ref="W9:AD9"/>
-    <mergeCell ref="W10:AD10"/>
-    <mergeCell ref="W11:AD11"/>
-    <mergeCell ref="U8:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U4:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -16111,7 +16879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:M220"/>
   <sheetViews>
@@ -16137,44 +16905,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="401" t="s">
+      <c r="C2" s="393" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="402"/>
-      <c r="E2" s="402"/>
-      <c r="F2" s="402"/>
-      <c r="G2" s="402"/>
-      <c r="H2" s="402"/>
-      <c r="I2" s="402"/>
-      <c r="J2" s="402"/>
-      <c r="K2" s="402"/>
+      <c r="D2" s="394"/>
+      <c r="E2" s="394"/>
+      <c r="F2" s="394"/>
+      <c r="G2" s="394"/>
+      <c r="H2" s="394"/>
+      <c r="I2" s="394"/>
+      <c r="J2" s="394"/>
+      <c r="K2" s="394"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="402"/>
-      <c r="D3" s="402"/>
-      <c r="E3" s="402"/>
-      <c r="F3" s="402"/>
-      <c r="G3" s="402"/>
-      <c r="H3" s="402"/>
-      <c r="I3" s="402"/>
-      <c r="J3" s="402"/>
-      <c r="K3" s="402"/>
+      <c r="C3" s="394"/>
+      <c r="D3" s="394"/>
+      <c r="E3" s="394"/>
+      <c r="F3" s="394"/>
+      <c r="G3" s="394"/>
+      <c r="H3" s="394"/>
+      <c r="I3" s="394"/>
+      <c r="J3" s="394"/>
+      <c r="K3" s="394"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="394" t="s">
+      <c r="C5" s="401" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="394"/>
-      <c r="E5" s="394"/>
-      <c r="F5" s="394"/>
-      <c r="G5" s="394"/>
-      <c r="I5" s="394" t="s">
+      <c r="D5" s="401"/>
+      <c r="E5" s="401"/>
+      <c r="F5" s="401"/>
+      <c r="G5" s="401"/>
+      <c r="I5" s="401" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="394"/>
-      <c r="K5" s="394"/>
-      <c r="L5" s="394"/>
-      <c r="M5" s="394"/>
+      <c r="J5" s="401"/>
+      <c r="K5" s="401"/>
+      <c r="L5" s="401"/>
+      <c r="M5" s="401"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -16614,20 +17382,20 @@
       <c r="M28" s="172"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="390" t="s">
+      <c r="D29" s="345" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="391"/>
+      <c r="E29" s="346"/>
       <c r="F29" s="395">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
       <c r="G29" s="396"/>
       <c r="I29" s="172"/>
-      <c r="J29" s="390" t="s">
+      <c r="J29" s="345" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="391"/>
+      <c r="K29" s="346"/>
       <c r="L29" s="395">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
@@ -16635,20 +17403,20 @@
       <c r="M29" s="396"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="350" t="s">
+      <c r="D30" s="392" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="309"/>
+      <c r="E30" s="307"/>
       <c r="F30" s="397">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
       <c r="G30" s="398"/>
       <c r="I30" s="172"/>
-      <c r="J30" s="350" t="s">
+      <c r="J30" s="392" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="309"/>
+      <c r="K30" s="307"/>
       <c r="L30" s="397">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
@@ -16656,46 +17424,46 @@
       <c r="M30" s="398"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="355" t="s">
+      <c r="D31" s="340" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="309"/>
-      <c r="F31" s="399">
+      <c r="E31" s="307"/>
+      <c r="F31" s="402">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="400"/>
+      <c r="G31" s="403"/>
       <c r="I31" s="172"/>
-      <c r="J31" s="355" t="s">
+      <c r="J31" s="340" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="309"/>
-      <c r="L31" s="399">
+      <c r="K31" s="307"/>
+      <c r="L31" s="402">
         <f>L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="400"/>
+      <c r="M31" s="403"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="388" t="s">
+      <c r="D32" s="341" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="389"/>
-      <c r="F32" s="392">
+      <c r="E32" s="342"/>
+      <c r="F32" s="399">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="393"/>
+      <c r="G32" s="400"/>
       <c r="I32" s="172"/>
-      <c r="J32" s="388" t="s">
+      <c r="J32" s="341" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="389"/>
-      <c r="L32" s="392">
+      <c r="K32" s="342"/>
+      <c r="L32" s="399">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="393"/>
+      <c r="M32" s="400"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16887,12 +17655,6 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C2:K3"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J29:K29"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="I5:M5"/>
@@ -16906,6 +17668,12 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J32:K32"/>
+    <mergeCell ref="C2:K3"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -16913,7 +17681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:M220"/>
   <sheetViews>
@@ -16938,44 +17706,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="407" t="s">
+      <c r="C2" s="404" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="408"/>
-      <c r="E2" s="408"/>
-      <c r="F2" s="408"/>
-      <c r="G2" s="408"/>
-      <c r="H2" s="408"/>
-      <c r="I2" s="408"/>
-      <c r="J2" s="408"/>
-      <c r="K2" s="408"/>
+      <c r="D2" s="405"/>
+      <c r="E2" s="405"/>
+      <c r="F2" s="405"/>
+      <c r="G2" s="405"/>
+      <c r="H2" s="405"/>
+      <c r="I2" s="405"/>
+      <c r="J2" s="405"/>
+      <c r="K2" s="405"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="408"/>
-      <c r="D3" s="408"/>
-      <c r="E3" s="408"/>
-      <c r="F3" s="408"/>
-      <c r="G3" s="408"/>
-      <c r="H3" s="408"/>
-      <c r="I3" s="408"/>
-      <c r="J3" s="408"/>
-      <c r="K3" s="408"/>
+      <c r="C3" s="405"/>
+      <c r="D3" s="405"/>
+      <c r="E3" s="405"/>
+      <c r="F3" s="405"/>
+      <c r="G3" s="405"/>
+      <c r="H3" s="405"/>
+      <c r="I3" s="405"/>
+      <c r="J3" s="405"/>
+      <c r="K3" s="405"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="394" t="s">
+      <c r="C5" s="401" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="394"/>
-      <c r="E5" s="394"/>
-      <c r="F5" s="394"/>
-      <c r="G5" s="394"/>
-      <c r="I5" s="394" t="s">
+      <c r="D5" s="401"/>
+      <c r="E5" s="401"/>
+      <c r="F5" s="401"/>
+      <c r="G5" s="401"/>
+      <c r="I5" s="401" t="s">
         <v>246</v>
       </c>
-      <c r="J5" s="394"/>
-      <c r="K5" s="394"/>
-      <c r="L5" s="394"/>
-      <c r="M5" s="394"/>
+      <c r="J5" s="401"/>
+      <c r="K5" s="401"/>
+      <c r="L5" s="401"/>
+      <c r="M5" s="401"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -17459,41 +18227,41 @@
       <c r="M28" s="172"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="329" t="s">
+      <c r="D29" s="380" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="331"/>
-      <c r="F29" s="405">
+      <c r="E29" s="382"/>
+      <c r="F29" s="406">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="406"/>
+      <c r="G29" s="407"/>
       <c r="I29" s="172"/>
-      <c r="J29" s="329" t="s">
+      <c r="J29" s="380" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="331"/>
-      <c r="L29" s="405">
+      <c r="K29" s="382"/>
+      <c r="L29" s="406">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="406"/>
+      <c r="M29" s="407"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="355" t="s">
+      <c r="D30" s="340" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="309"/>
+      <c r="E30" s="307"/>
       <c r="F30" s="397">
         <f>F27</f>
         <v>903300</v>
       </c>
       <c r="G30" s="398"/>
       <c r="I30" s="172"/>
-      <c r="J30" s="355" t="s">
+      <c r="J30" s="340" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="309"/>
+      <c r="K30" s="307"/>
       <c r="L30" s="397">
         <f>L27</f>
         <v>779000</v>
@@ -17501,46 +18269,46 @@
       <c r="M30" s="398"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="355" t="s">
+      <c r="D31" s="340" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="309"/>
-      <c r="F31" s="399">
+      <c r="E31" s="307"/>
+      <c r="F31" s="402">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="400"/>
+      <c r="G31" s="403"/>
       <c r="I31" s="172"/>
-      <c r="J31" s="355" t="s">
+      <c r="J31" s="340" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="309"/>
-      <c r="L31" s="399">
+      <c r="K31" s="307"/>
+      <c r="L31" s="402">
         <f>Pemasukkan!L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="400"/>
+      <c r="M31" s="403"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="388" t="s">
+      <c r="D32" s="341" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="389"/>
-      <c r="F32" s="403">
+      <c r="E32" s="342"/>
+      <c r="F32" s="408">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="404"/>
+      <c r="G32" s="409"/>
       <c r="I32" s="172"/>
-      <c r="J32" s="388" t="s">
+      <c r="J32" s="341" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="389"/>
-      <c r="L32" s="403">
+      <c r="K32" s="342"/>
+      <c r="L32" s="408">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="404"/>
+      <c r="M32" s="409"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17732,6 +18500,14 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
     <mergeCell ref="C2:K3"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
@@ -17743,14 +18519,6 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -17758,7 +18526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:K32"/>
   <sheetViews>
@@ -17776,28 +18544,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="411" t="s">
+      <c r="C2" s="412" t="s">
         <v>230</v>
       </c>
-      <c r="D2" s="412"/>
-      <c r="E2" s="412"/>
-      <c r="F2" s="412"/>
-      <c r="G2" s="412"/>
-      <c r="H2" s="412"/>
-      <c r="I2" s="412"/>
-      <c r="J2" s="412"/>
-      <c r="K2" s="412"/>
+      <c r="D2" s="413"/>
+      <c r="E2" s="413"/>
+      <c r="F2" s="413"/>
+      <c r="G2" s="413"/>
+      <c r="H2" s="413"/>
+      <c r="I2" s="413"/>
+      <c r="J2" s="413"/>
+      <c r="K2" s="413"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="412"/>
-      <c r="D3" s="412"/>
-      <c r="E3" s="412"/>
-      <c r="F3" s="412"/>
-      <c r="G3" s="412"/>
-      <c r="H3" s="412"/>
-      <c r="I3" s="412"/>
-      <c r="J3" s="412"/>
-      <c r="K3" s="412"/>
+      <c r="C3" s="413"/>
+      <c r="D3" s="413"/>
+      <c r="E3" s="413"/>
+      <c r="F3" s="413"/>
+      <c r="G3" s="413"/>
+      <c r="H3" s="413"/>
+      <c r="I3" s="413"/>
+      <c r="J3" s="413"/>
+      <c r="K3" s="413"/>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="141"/>
@@ -18155,10 +18923,10 @@
     </row>
     <row r="29" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="141"/>
-      <c r="D29" s="413"/>
-      <c r="E29" s="413"/>
-      <c r="F29" s="414"/>
-      <c r="G29" s="414"/>
+      <c r="D29" s="414"/>
+      <c r="E29" s="414"/>
+      <c r="F29" s="415"/>
+      <c r="G29" s="415"/>
       <c r="H29" s="141"/>
       <c r="I29" s="141"/>
       <c r="J29" s="141"/>
@@ -18166,15 +18934,15 @@
     </row>
     <row r="30" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="24"/>
-      <c r="D30" s="415" t="s">
+      <c r="D30" s="416" t="s">
         <v>229</v>
       </c>
-      <c r="E30" s="416"/>
-      <c r="F30" s="417">
+      <c r="E30" s="417"/>
+      <c r="F30" s="418">
         <f>F27</f>
         <v>226000</v>
       </c>
-      <c r="G30" s="418"/>
+      <c r="G30" s="419"/>
       <c r="H30" s="141"/>
       <c r="I30" s="141"/>
       <c r="J30" s="141"/>
@@ -18189,10 +18957,10 @@
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="141"/>
-      <c r="D32" s="409"/>
-      <c r="E32" s="409"/>
-      <c r="F32" s="410"/>
-      <c r="G32" s="409"/>
+      <c r="D32" s="410"/>
+      <c r="E32" s="410"/>
+      <c r="F32" s="411"/>
+      <c r="G32" s="410"/>
       <c r="H32" s="141"/>
       <c r="I32" s="141"/>
       <c r="J32" s="141"/>
@@ -18213,7 +18981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -18229,17 +18997,17 @@
     <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="419" t="s">
+      <c r="C4" s="420" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="420"/>
+      <c r="D4" s="421"/>
       <c r="E4" s="27"/>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
-      <c r="H4" s="419" t="s">
+      <c r="H4" s="420" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="420"/>
+      <c r="I4" s="421"/>
       <c r="J4" s="35"/>
       <c r="K4" s="27"/>
     </row>
@@ -18366,17 +19134,17 @@
     <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26"/>
-      <c r="C17" s="419" t="s">
+      <c r="C17" s="420" t="s">
         <v>144</v>
       </c>
-      <c r="D17" s="420"/>
+      <c r="D17" s="421"/>
       <c r="E17" s="27"/>
       <c r="F17" s="26"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="419" t="s">
+      <c r="H17" s="420" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="420"/>
+      <c r="I17" s="421"/>
       <c r="J17" s="35"/>
       <c r="K17" s="27"/>
     </row>
@@ -18511,220 +19279,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="422" t="s">
-        <v>276</v>
-      </c>
-      <c r="C2" s="423"/>
-      <c r="D2" s="423"/>
-      <c r="E2" s="423"/>
-      <c r="F2" s="423"/>
-      <c r="G2" s="423"/>
-      <c r="H2" s="423"/>
-      <c r="I2" s="423"/>
-      <c r="J2" s="423"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="423"/>
-      <c r="C3" s="423"/>
-      <c r="D3" s="423"/>
-      <c r="E3" s="423"/>
-      <c r="F3" s="423"/>
-      <c r="G3" s="423"/>
-      <c r="H3" s="423"/>
-      <c r="I3" s="423"/>
-      <c r="J3" s="423"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="H6" s="338" t="s">
-        <v>281</v>
-      </c>
-      <c r="I6" s="309"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D7" s="1">
-        <v>39</v>
-      </c>
-      <c r="E7" s="195">
-        <v>15000</v>
-      </c>
-      <c r="F7" s="195">
-        <f>D7*E7</f>
-        <v>585000</v>
-      </c>
-      <c r="G7" s="195">
-        <v>205000</v>
-      </c>
-      <c r="H7" s="424">
-        <f>F7-G7</f>
-        <v>380000</v>
-      </c>
-      <c r="I7" s="309"/>
-    </row>
-    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="196"/>
-      <c r="C8" s="196"/>
-      <c r="D8" s="196"/>
-      <c r="E8" s="197"/>
-      <c r="F8" s="197"/>
-      <c r="G8" s="197"/>
-      <c r="H8" s="421"/>
-      <c r="I8" s="421"/>
-    </row>
-    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="196"/>
-      <c r="C9" s="196"/>
-      <c r="D9" s="196"/>
-      <c r="E9" s="197"/>
-      <c r="F9" s="197"/>
-      <c r="G9" s="198" t="s">
-        <v>282</v>
-      </c>
-      <c r="H9" s="425">
-        <f>H7</f>
-        <v>380000</v>
-      </c>
-      <c r="I9" s="426"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="196"/>
-      <c r="C10" s="196"/>
-      <c r="D10" s="196"/>
-      <c r="E10" s="197"/>
-      <c r="F10" s="197"/>
-      <c r="G10" s="197"/>
-      <c r="H10" s="421"/>
-      <c r="I10" s="421"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="196"/>
-      <c r="C11" s="196"/>
-      <c r="D11" s="196"/>
-      <c r="E11" s="197"/>
-      <c r="F11" s="197"/>
-      <c r="G11" s="197"/>
-      <c r="H11" s="421"/>
-      <c r="I11" s="421"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="196"/>
-      <c r="C12" s="196"/>
-      <c r="D12" s="196"/>
-      <c r="E12" s="197"/>
-      <c r="F12" s="197"/>
-      <c r="G12" s="197"/>
-      <c r="H12" s="421"/>
-      <c r="I12" s="421"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="196"/>
-      <c r="C13" s="196"/>
-      <c r="D13" s="196"/>
-      <c r="E13" s="197"/>
-      <c r="F13" s="197"/>
-      <c r="G13" s="197"/>
-      <c r="H13" s="421"/>
-      <c r="I13" s="421"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="196"/>
-      <c r="C14" s="196"/>
-      <c r="D14" s="196"/>
-      <c r="E14" s="197"/>
-      <c r="F14" s="197"/>
-      <c r="G14" s="197"/>
-      <c r="H14" s="421"/>
-      <c r="I14" s="421"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="196"/>
-      <c r="C15" s="196"/>
-      <c r="D15" s="196"/>
-      <c r="E15" s="197"/>
-      <c r="F15" s="197"/>
-      <c r="G15" s="197"/>
-      <c r="H15" s="421"/>
-      <c r="I15" s="421"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="196"/>
-      <c r="C16" s="196"/>
-      <c r="D16" s="196"/>
-      <c r="E16" s="197"/>
-      <c r="F16" s="197"/>
-      <c r="G16" s="197"/>
-      <c r="H16" s="421"/>
-      <c r="I16" s="421"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="196"/>
-      <c r="C17" s="196"/>
-      <c r="D17" s="196"/>
-      <c r="E17" s="197"/>
-      <c r="F17" s="197"/>
-      <c r="G17" s="197"/>
-      <c r="H17" s="421"/>
-      <c r="I17" s="421"/>
-    </row>
-  </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B2:J3"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Yahya Bayar Makan untuk Makrab
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-630" yWindow="570" windowWidth="19815" windowHeight="7365" tabRatio="761" activeTab="1"/>
+    <workbookView xWindow="-630" yWindow="570" windowWidth="19815" windowHeight="7365" tabRatio="761" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2018(NOT UPDATED)" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="365">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -1115,6 +1115,9 @@
   </si>
   <si>
     <t>Simpanan 255k</t>
+  </si>
+  <si>
+    <t>Yahya(Makan doang)</t>
   </si>
 </sst>
 </file>
@@ -2947,29 +2950,20 @@
     <xf numFmtId="177" fontId="4" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2985,37 +2979,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3023,29 +3019,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3089,6 +3092,156 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3101,33 +3254,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3147,136 +3279,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3287,47 +3308,29 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4539,126 +4542,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="287" t="s">
+      <c r="A1" s="281" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="288"/>
-      <c r="C1" s="288"/>
-      <c r="D1" s="288"/>
-      <c r="E1" s="288"/>
-      <c r="F1" s="288"/>
-      <c r="G1" s="288"/>
-      <c r="H1" s="288"/>
-      <c r="I1" s="288"/>
-      <c r="J1" s="288"/>
-      <c r="K1" s="288"/>
-      <c r="L1" s="288"/>
-      <c r="M1" s="288"/>
-      <c r="N1" s="288"/>
-      <c r="O1" s="288"/>
-      <c r="P1" s="288"/>
-      <c r="Q1" s="288"/>
-      <c r="R1" s="288"/>
+      <c r="B1" s="282"/>
+      <c r="C1" s="282"/>
+      <c r="D1" s="282"/>
+      <c r="E1" s="282"/>
+      <c r="F1" s="282"/>
+      <c r="G1" s="282"/>
+      <c r="H1" s="282"/>
+      <c r="I1" s="282"/>
+      <c r="J1" s="282"/>
+      <c r="K1" s="282"/>
+      <c r="L1" s="282"/>
+      <c r="M1" s="282"/>
+      <c r="N1" s="282"/>
+      <c r="O1" s="282"/>
+      <c r="P1" s="282"/>
+      <c r="Q1" s="282"/>
+      <c r="R1" s="282"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="289"/>
-      <c r="B2" s="290"/>
-      <c r="C2" s="290"/>
-      <c r="D2" s="290"/>
-      <c r="E2" s="290"/>
-      <c r="F2" s="290"/>
-      <c r="G2" s="290"/>
-      <c r="H2" s="290"/>
-      <c r="I2" s="290"/>
-      <c r="J2" s="290"/>
-      <c r="K2" s="290"/>
-      <c r="L2" s="290"/>
-      <c r="M2" s="290"/>
-      <c r="N2" s="290"/>
-      <c r="O2" s="290"/>
-      <c r="P2" s="290"/>
-      <c r="Q2" s="290"/>
-      <c r="R2" s="290"/>
+      <c r="A2" s="283"/>
+      <c r="B2" s="284"/>
+      <c r="C2" s="284"/>
+      <c r="D2" s="284"/>
+      <c r="E2" s="284"/>
+      <c r="F2" s="284"/>
+      <c r="G2" s="284"/>
+      <c r="H2" s="284"/>
+      <c r="I2" s="284"/>
+      <c r="J2" s="284"/>
+      <c r="K2" s="284"/>
+      <c r="L2" s="284"/>
+      <c r="M2" s="284"/>
+      <c r="N2" s="284"/>
+      <c r="O2" s="284"/>
+      <c r="P2" s="284"/>
+      <c r="Q2" s="284"/>
+      <c r="R2" s="284"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="289"/>
-      <c r="B3" s="290"/>
-      <c r="C3" s="290"/>
-      <c r="D3" s="290"/>
-      <c r="E3" s="290"/>
-      <c r="F3" s="290"/>
-      <c r="G3" s="290"/>
-      <c r="H3" s="290"/>
-      <c r="I3" s="290"/>
-      <c r="J3" s="290"/>
-      <c r="K3" s="290"/>
-      <c r="L3" s="290"/>
-      <c r="M3" s="290"/>
-      <c r="N3" s="290"/>
-      <c r="O3" s="290"/>
-      <c r="P3" s="290"/>
-      <c r="Q3" s="290"/>
-      <c r="R3" s="290"/>
+      <c r="A3" s="283"/>
+      <c r="B3" s="284"/>
+      <c r="C3" s="284"/>
+      <c r="D3" s="284"/>
+      <c r="E3" s="284"/>
+      <c r="F3" s="284"/>
+      <c r="G3" s="284"/>
+      <c r="H3" s="284"/>
+      <c r="I3" s="284"/>
+      <c r="J3" s="284"/>
+      <c r="K3" s="284"/>
+      <c r="L3" s="284"/>
+      <c r="M3" s="284"/>
+      <c r="N3" s="284"/>
+      <c r="O3" s="284"/>
+      <c r="P3" s="284"/>
+      <c r="Q3" s="284"/>
+      <c r="R3" s="284"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="289"/>
-      <c r="B4" s="290"/>
-      <c r="C4" s="290"/>
-      <c r="D4" s="290"/>
-      <c r="E4" s="290"/>
-      <c r="F4" s="290"/>
-      <c r="G4" s="290"/>
-      <c r="H4" s="290"/>
-      <c r="I4" s="290"/>
-      <c r="J4" s="290"/>
-      <c r="K4" s="290"/>
-      <c r="L4" s="290"/>
-      <c r="M4" s="290"/>
-      <c r="N4" s="290"/>
-      <c r="O4" s="290"/>
-      <c r="P4" s="290"/>
-      <c r="Q4" s="290"/>
-      <c r="R4" s="290"/>
+      <c r="A4" s="283"/>
+      <c r="B4" s="284"/>
+      <c r="C4" s="284"/>
+      <c r="D4" s="284"/>
+      <c r="E4" s="284"/>
+      <c r="F4" s="284"/>
+      <c r="G4" s="284"/>
+      <c r="H4" s="284"/>
+      <c r="I4" s="284"/>
+      <c r="J4" s="284"/>
+      <c r="K4" s="284"/>
+      <c r="L4" s="284"/>
+      <c r="M4" s="284"/>
+      <c r="N4" s="284"/>
+      <c r="O4" s="284"/>
+      <c r="P4" s="284"/>
+      <c r="Q4" s="284"/>
+      <c r="R4" s="284"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="289"/>
-      <c r="B5" s="290"/>
-      <c r="C5" s="290"/>
-      <c r="D5" s="290"/>
-      <c r="E5" s="290"/>
-      <c r="F5" s="290"/>
-      <c r="G5" s="290"/>
-      <c r="H5" s="290"/>
-      <c r="I5" s="290"/>
-      <c r="J5" s="290"/>
-      <c r="K5" s="290"/>
-      <c r="L5" s="290"/>
-      <c r="M5" s="290"/>
-      <c r="N5" s="290"/>
-      <c r="O5" s="290"/>
-      <c r="P5" s="290"/>
-      <c r="Q5" s="290"/>
-      <c r="R5" s="290"/>
+      <c r="A5" s="283"/>
+      <c r="B5" s="284"/>
+      <c r="C5" s="284"/>
+      <c r="D5" s="284"/>
+      <c r="E5" s="284"/>
+      <c r="F5" s="284"/>
+      <c r="G5" s="284"/>
+      <c r="H5" s="284"/>
+      <c r="I5" s="284"/>
+      <c r="J5" s="284"/>
+      <c r="K5" s="284"/>
+      <c r="L5" s="284"/>
+      <c r="M5" s="284"/>
+      <c r="N5" s="284"/>
+      <c r="O5" s="284"/>
+      <c r="P5" s="284"/>
+      <c r="Q5" s="284"/>
+      <c r="R5" s="284"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="289"/>
-      <c r="B6" s="290"/>
-      <c r="C6" s="290"/>
-      <c r="D6" s="290"/>
-      <c r="E6" s="290"/>
-      <c r="F6" s="290"/>
-      <c r="G6" s="290"/>
-      <c r="H6" s="290"/>
-      <c r="I6" s="290"/>
-      <c r="J6" s="290"/>
-      <c r="K6" s="290"/>
-      <c r="L6" s="290"/>
-      <c r="M6" s="290"/>
-      <c r="N6" s="290"/>
-      <c r="O6" s="290"/>
-      <c r="P6" s="290"/>
-      <c r="Q6" s="290"/>
-      <c r="R6" s="290"/>
+      <c r="A6" s="283"/>
+      <c r="B6" s="284"/>
+      <c r="C6" s="284"/>
+      <c r="D6" s="284"/>
+      <c r="E6" s="284"/>
+      <c r="F6" s="284"/>
+      <c r="G6" s="284"/>
+      <c r="H6" s="284"/>
+      <c r="I6" s="284"/>
+      <c r="J6" s="284"/>
+      <c r="K6" s="284"/>
+      <c r="L6" s="284"/>
+      <c r="M6" s="284"/>
+      <c r="N6" s="284"/>
+      <c r="O6" s="284"/>
+      <c r="P6" s="284"/>
+      <c r="Q6" s="284"/>
+      <c r="R6" s="284"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -7603,58 +7606,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="292" t="s">
+      <c r="J79" s="289" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="293"/>
-      <c r="L79" s="293"/>
-      <c r="M79" s="293"/>
-      <c r="N79" s="294"/>
-      <c r="P79" s="300" t="s">
+      <c r="K79" s="290"/>
+      <c r="L79" s="290"/>
+      <c r="M79" s="290"/>
+      <c r="N79" s="291"/>
+      <c r="P79" s="297" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="293"/>
-      <c r="R79" s="293"/>
-      <c r="S79" s="294"/>
+      <c r="Q79" s="290"/>
+      <c r="R79" s="290"/>
+      <c r="S79" s="291"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="295" t="s">
+      <c r="J80" s="292" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="290"/>
-      <c r="L80" s="290"/>
-      <c r="M80" s="290"/>
-      <c r="N80" s="296"/>
-      <c r="P80" s="295" t="s">
+      <c r="K80" s="284"/>
+      <c r="L80" s="284"/>
+      <c r="M80" s="284"/>
+      <c r="N80" s="293"/>
+      <c r="P80" s="292" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="290"/>
-      <c r="R80" s="290"/>
-      <c r="S80" s="296"/>
+      <c r="Q80" s="284"/>
+      <c r="R80" s="284"/>
+      <c r="S80" s="293"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="297"/>
-      <c r="K81" s="298"/>
-      <c r="L81" s="298"/>
-      <c r="M81" s="298"/>
-      <c r="N81" s="299"/>
-      <c r="P81" s="297"/>
-      <c r="Q81" s="298"/>
-      <c r="R81" s="298"/>
-      <c r="S81" s="299"/>
+      <c r="J81" s="294"/>
+      <c r="K81" s="295"/>
+      <c r="L81" s="295"/>
+      <c r="M81" s="295"/>
+      <c r="N81" s="296"/>
+      <c r="P81" s="294"/>
+      <c r="Q81" s="295"/>
+      <c r="R81" s="295"/>
+      <c r="S81" s="296"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="291" t="s">
+      <c r="J82" s="287" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="282"/>
-      <c r="L82" s="283"/>
-      <c r="M82" s="291" t="s">
+      <c r="K82" s="288"/>
+      <c r="L82" s="286"/>
+      <c r="M82" s="287" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="283"/>
-      <c r="P82" s="291"/>
-      <c r="Q82" s="283"/>
+      <c r="N82" s="286"/>
+      <c r="P82" s="287"/>
+      <c r="Q82" s="286"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -7663,38 +7666,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="281" t="s">
+      <c r="J83" s="298" t="s">
         <v>70</v>
       </c>
-      <c r="K83" s="282"/>
-      <c r="L83" s="283"/>
-      <c r="M83" s="284">
+      <c r="K83" s="288"/>
+      <c r="L83" s="286"/>
+      <c r="M83" s="299">
         <v>7350000</v>
       </c>
-      <c r="N83" s="283"/>
+      <c r="N83" s="286"/>
       <c r="P83" s="285" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="283"/>
+      <c r="Q83" s="286"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="281" t="s">
+      <c r="J84" s="298" t="s">
         <v>72</v>
       </c>
-      <c r="K84" s="282"/>
-      <c r="L84" s="283"/>
-      <c r="M84" s="286">
+      <c r="K84" s="288"/>
+      <c r="L84" s="286"/>
+      <c r="M84" s="300">
         <v>1100000</v>
       </c>
-      <c r="N84" s="283"/>
+      <c r="N84" s="286"/>
       <c r="P84" s="285" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="283"/>
+      <c r="Q84" s="286"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -7703,39 +7706,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="281" t="s">
+      <c r="J85" s="298" t="s">
         <v>75</v>
       </c>
-      <c r="K85" s="282"/>
-      <c r="L85" s="283"/>
-      <c r="M85" s="284">
+      <c r="K85" s="288"/>
+      <c r="L85" s="286"/>
+      <c r="M85" s="299">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="283"/>
+      <c r="N85" s="286"/>
       <c r="P85" s="285" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="283"/>
+      <c r="Q85" s="286"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="281" t="s">
+      <c r="J86" s="298" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="282"/>
-      <c r="L86" s="283"/>
-      <c r="M86" s="284">
+      <c r="K86" s="288"/>
+      <c r="L86" s="286"/>
+      <c r="M86" s="299">
         <v>8411850</v>
       </c>
-      <c r="N86" s="283"/>
+      <c r="N86" s="286"/>
       <c r="P86" s="285" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="283"/>
+      <c r="Q86" s="286"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -7743,20 +7746,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="281" t="s">
+      <c r="J87" s="298" t="s">
         <v>79</v>
       </c>
-      <c r="K87" s="282"/>
-      <c r="L87" s="283"/>
-      <c r="M87" s="284">
+      <c r="K87" s="288"/>
+      <c r="L87" s="286"/>
+      <c r="M87" s="299">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="283"/>
+      <c r="N87" s="286"/>
       <c r="P87" s="285" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="283"/>
+      <c r="Q87" s="286"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -7945,6 +7948,17 @@
   </sheetData>
   <sheetProtection password="F879" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="23">
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="P86:Q86"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="M84:N84"/>
     <mergeCell ref="A1:R6"/>
     <mergeCell ref="P84:Q84"/>
     <mergeCell ref="J82:L82"/>
@@ -7957,17 +7971,6 @@
     <mergeCell ref="P83:Q83"/>
     <mergeCell ref="P82:Q82"/>
     <mergeCell ref="P80:S81"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="P86:Q86"/>
   </mergeCells>
   <conditionalFormatting sqref="T10:T52">
     <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
@@ -8056,10 +8059,10 @@
       <c r="G6" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="H6" s="346" t="s">
+      <c r="H6" s="356" t="s">
         <v>280</v>
       </c>
-      <c r="I6" s="314"/>
+      <c r="I6" s="311"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -8085,7 +8088,7 @@
         <f>F7-G7</f>
         <v>380000</v>
       </c>
-      <c r="I7" s="314"/>
+      <c r="I7" s="311"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="196"/>
@@ -8194,11 +8197,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="H6:I6"/>
@@ -8207,6 +8205,11 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8217,8 +8220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BM266"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="F31" colorId="8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V49" sqref="V49"/>
+    <sheetView defaultGridColor="0" topLeftCell="F31" colorId="8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8260,46 +8263,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="309" t="s">
+      <c r="C2" s="321" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="288"/>
-      <c r="E2" s="288"/>
-      <c r="F2" s="288"/>
-      <c r="G2" s="288"/>
-      <c r="H2" s="288"/>
-      <c r="I2" s="288"/>
-      <c r="J2" s="288"/>
-      <c r="K2" s="288"/>
-      <c r="L2" s="288"/>
-      <c r="M2" s="288"/>
-      <c r="N2" s="288"/>
-      <c r="O2" s="288"/>
-      <c r="P2" s="289"/>
-      <c r="Q2" s="289"/>
-      <c r="R2" s="289"/>
-      <c r="S2" s="288"/>
-      <c r="T2" s="288"/>
+      <c r="D2" s="282"/>
+      <c r="E2" s="282"/>
+      <c r="F2" s="282"/>
+      <c r="G2" s="282"/>
+      <c r="H2" s="282"/>
+      <c r="I2" s="282"/>
+      <c r="J2" s="282"/>
+      <c r="K2" s="282"/>
+      <c r="L2" s="282"/>
+      <c r="M2" s="282"/>
+      <c r="N2" s="282"/>
+      <c r="O2" s="282"/>
+      <c r="P2" s="283"/>
+      <c r="Q2" s="283"/>
+      <c r="R2" s="283"/>
+      <c r="S2" s="282"/>
+      <c r="T2" s="282"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="289"/>
-      <c r="D3" s="290"/>
-      <c r="E3" s="290"/>
-      <c r="F3" s="290"/>
-      <c r="G3" s="290"/>
-      <c r="H3" s="290"/>
-      <c r="I3" s="290"/>
-      <c r="J3" s="290"/>
-      <c r="K3" s="290"/>
-      <c r="L3" s="290"/>
-      <c r="M3" s="290"/>
-      <c r="N3" s="290"/>
-      <c r="O3" s="290"/>
-      <c r="P3" s="290"/>
-      <c r="Q3" s="290"/>
-      <c r="R3" s="290"/>
-      <c r="S3" s="290"/>
-      <c r="T3" s="290"/>
+      <c r="C3" s="283"/>
+      <c r="D3" s="284"/>
+      <c r="E3" s="284"/>
+      <c r="F3" s="284"/>
+      <c r="G3" s="284"/>
+      <c r="H3" s="284"/>
+      <c r="I3" s="284"/>
+      <c r="J3" s="284"/>
+      <c r="K3" s="284"/>
+      <c r="L3" s="284"/>
+      <c r="M3" s="284"/>
+      <c r="N3" s="284"/>
+      <c r="O3" s="284"/>
+      <c r="P3" s="284"/>
+      <c r="Q3" s="284"/>
+      <c r="R3" s="284"/>
+      <c r="S3" s="284"/>
+      <c r="T3" s="284"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8386,25 +8389,25 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="315" t="s">
+      <c r="X5" s="313" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="282"/>
-      <c r="Z5" s="282"/>
-      <c r="AA5" s="282"/>
-      <c r="AB5" s="282"/>
-      <c r="AC5" s="282"/>
-      <c r="AD5" s="282"/>
-      <c r="AE5" s="282"/>
-      <c r="AF5" s="282"/>
-      <c r="AG5" s="282"/>
-      <c r="AH5" s="282"/>
-      <c r="AI5" s="282"/>
-      <c r="AJ5" s="282"/>
-      <c r="AK5" s="282"/>
-      <c r="AL5" s="282"/>
-      <c r="AM5" s="282"/>
-      <c r="AN5" s="283"/>
+      <c r="Y5" s="288"/>
+      <c r="Z5" s="288"/>
+      <c r="AA5" s="288"/>
+      <c r="AB5" s="288"/>
+      <c r="AC5" s="288"/>
+      <c r="AD5" s="288"/>
+      <c r="AE5" s="288"/>
+      <c r="AF5" s="288"/>
+      <c r="AG5" s="288"/>
+      <c r="AH5" s="288"/>
+      <c r="AI5" s="288"/>
+      <c r="AJ5" s="288"/>
+      <c r="AK5" s="288"/>
+      <c r="AL5" s="288"/>
+      <c r="AM5" s="288"/>
+      <c r="AN5" s="286"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -8479,29 +8482,29 @@
       <c r="V6" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X6" s="310" t="s">
+      <c r="X6" s="322" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="310" t="s">
+      <c r="Y6" s="322" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="314" t="s">
+      <c r="Z6" s="311" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="311"/>
-      <c r="AB6" s="311"/>
-      <c r="AC6" s="311"/>
-      <c r="AD6" s="311"/>
-      <c r="AE6" s="311"/>
-      <c r="AF6" s="311"/>
-      <c r="AG6" s="311"/>
-      <c r="AH6" s="311"/>
-      <c r="AI6" s="311"/>
-      <c r="AJ6" s="311"/>
-      <c r="AK6" s="311"/>
-      <c r="AL6" s="311"/>
-      <c r="AM6" s="311"/>
-      <c r="AN6" s="311"/>
+      <c r="AA6" s="312"/>
+      <c r="AB6" s="312"/>
+      <c r="AC6" s="312"/>
+      <c r="AD6" s="312"/>
+      <c r="AE6" s="312"/>
+      <c r="AF6" s="312"/>
+      <c r="AG6" s="312"/>
+      <c r="AH6" s="312"/>
+      <c r="AI6" s="312"/>
+      <c r="AJ6" s="312"/>
+      <c r="AK6" s="312"/>
+      <c r="AL6" s="312"/>
+      <c r="AM6" s="312"/>
+      <c r="AN6" s="312"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -8576,27 +8579,27 @@
       <c r="V7" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X7" s="311"/>
-      <c r="Y7" s="311"/>
-      <c r="Z7" s="314" t="s">
+      <c r="X7" s="312"/>
+      <c r="Y7" s="312"/>
+      <c r="Z7" s="311" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="311"/>
-      <c r="AB7" s="311"/>
-      <c r="AC7" s="311"/>
-      <c r="AD7" s="314" t="s">
+      <c r="AA7" s="312"/>
+      <c r="AB7" s="312"/>
+      <c r="AC7" s="312"/>
+      <c r="AD7" s="311" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="311"/>
-      <c r="AF7" s="311"/>
-      <c r="AG7" s="311"/>
-      <c r="AH7" s="311"/>
-      <c r="AI7" s="311"/>
-      <c r="AJ7" s="311"/>
-      <c r="AK7" s="311"/>
-      <c r="AL7" s="311"/>
-      <c r="AM7" s="311"/>
-      <c r="AN7" s="311"/>
+      <c r="AE7" s="312"/>
+      <c r="AF7" s="312"/>
+      <c r="AG7" s="312"/>
+      <c r="AH7" s="312"/>
+      <c r="AI7" s="312"/>
+      <c r="AJ7" s="312"/>
+      <c r="AK7" s="312"/>
+      <c r="AL7" s="312"/>
+      <c r="AM7" s="312"/>
+      <c r="AN7" s="312"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -8646,8 +8649,8 @@
         <v>NO</v>
       </c>
       <c r="V8" s="13"/>
-      <c r="X8" s="311"/>
-      <c r="Y8" s="311"/>
+      <c r="X8" s="312"/>
+      <c r="Y8" s="312"/>
       <c r="Z8" s="153" t="s">
         <v>19</v>
       </c>
@@ -13258,10 +13261,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="312" t="s">
+      <c r="AA49" s="309" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="313"/>
+      <c r="AB49" s="310"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -13339,12 +13342,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="319" t="s">
+      <c r="AI50" s="305" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="320"/>
-      <c r="AK50" s="320"/>
-      <c r="AL50" s="321"/>
+      <c r="AJ50" s="306"/>
+      <c r="AK50" s="306"/>
+      <c r="AL50" s="307"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -13415,12 +13418,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="316" t="s">
+      <c r="AI51" s="302" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="317"/>
-      <c r="AK51" s="317"/>
-      <c r="AL51" s="318"/>
+      <c r="AJ51" s="303"/>
+      <c r="AK51" s="303"/>
+      <c r="AL51" s="304"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -13686,14 +13689,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="322"/>
-      <c r="AD55" s="322"/>
-      <c r="AI55" s="319" t="s">
+      <c r="AC55" s="308"/>
+      <c r="AD55" s="308"/>
+      <c r="AI55" s="305" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="320"/>
-      <c r="AK55" s="320"/>
-      <c r="AL55" s="321"/>
+      <c r="AJ55" s="306"/>
+      <c r="AK55" s="306"/>
+      <c r="AL55" s="307"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -14008,32 +14011,32 @@
     <row r="67" spans="3:19" s="258" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="302" t="s">
+      <c r="C69" s="314" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="303"/>
-      <c r="E69" s="303"/>
-      <c r="F69" s="303"/>
-      <c r="G69" s="304"/>
-      <c r="I69" s="308" t="s">
+      <c r="D69" s="315"/>
+      <c r="E69" s="315"/>
+      <c r="F69" s="315"/>
+      <c r="G69" s="316"/>
+      <c r="I69" s="320" t="s">
         <v>178</v>
       </c>
-      <c r="J69" s="308"/>
-      <c r="K69" s="308"/>
-      <c r="L69" s="308"/>
-      <c r="M69" s="308"/>
+      <c r="J69" s="320"/>
+      <c r="K69" s="320"/>
+      <c r="L69" s="320"/>
+      <c r="M69" s="320"/>
     </row>
     <row r="70" spans="3:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="305"/>
-      <c r="D70" s="306"/>
-      <c r="E70" s="306"/>
-      <c r="F70" s="306"/>
-      <c r="G70" s="307"/>
-      <c r="I70" s="308"/>
-      <c r="J70" s="308"/>
-      <c r="K70" s="308"/>
-      <c r="L70" s="308"/>
-      <c r="M70" s="308"/>
+      <c r="C70" s="317"/>
+      <c r="D70" s="318"/>
+      <c r="E70" s="318"/>
+      <c r="F70" s="318"/>
+      <c r="G70" s="319"/>
+      <c r="I70" s="320"/>
+      <c r="J70" s="320"/>
+      <c r="K70" s="320"/>
+      <c r="L70" s="320"/>
+      <c r="M70" s="320"/>
     </row>
     <row r="71" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14524,22 +14527,22 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AI56:AL56"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AI50:AL50"/>
-    <mergeCell ref="AI55:AL55"/>
-    <mergeCell ref="AC55:AD55"/>
-    <mergeCell ref="AA49:AB49"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="AD7:AN7"/>
-    <mergeCell ref="X5:AN5"/>
-    <mergeCell ref="Z6:AN6"/>
     <mergeCell ref="P76:Q76"/>
     <mergeCell ref="C69:G70"/>
     <mergeCell ref="I69:M70"/>
     <mergeCell ref="C2:T3"/>
     <mergeCell ref="Y6:Y8"/>
     <mergeCell ref="X6:X8"/>
+    <mergeCell ref="AA49:AB49"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="AD7:AN7"/>
+    <mergeCell ref="X5:AN5"/>
+    <mergeCell ref="Z6:AN6"/>
+    <mergeCell ref="AI56:AL56"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AI50:AL50"/>
+    <mergeCell ref="AI55:AL55"/>
+    <mergeCell ref="AC55:AD55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:V61">
     <cfRule type="expression" dxfId="14" priority="7">
@@ -14604,7 +14607,7 @@
   <dimension ref="A2:W36"/>
   <sheetViews>
     <sheetView topLeftCell="H16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14654,56 +14657,56 @@
       <c r="L3" s="323"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="308" t="s">
+      <c r="A5" s="320" t="s">
         <v>303</v>
       </c>
-      <c r="B5" s="308"/>
-      <c r="C5" s="308"/>
-      <c r="D5" s="308"/>
-      <c r="E5" s="308"/>
-      <c r="F5" s="308"/>
-      <c r="G5" s="308"/>
-      <c r="H5" s="308"/>
-      <c r="I5" s="308"/>
-      <c r="J5" s="308"/>
-      <c r="K5" s="308"/>
-      <c r="M5" s="308" t="s">
+      <c r="B5" s="320"/>
+      <c r="C5" s="320"/>
+      <c r="D5" s="320"/>
+      <c r="E5" s="320"/>
+      <c r="F5" s="320"/>
+      <c r="G5" s="320"/>
+      <c r="H5" s="320"/>
+      <c r="I5" s="320"/>
+      <c r="J5" s="320"/>
+      <c r="K5" s="320"/>
+      <c r="M5" s="320" t="s">
         <v>324</v>
       </c>
-      <c r="N5" s="308"/>
-      <c r="O5" s="308"/>
-      <c r="P5" s="308"/>
-      <c r="Q5" s="308"/>
-      <c r="R5" s="308"/>
-      <c r="S5" s="308"/>
-      <c r="T5" s="308"/>
-      <c r="U5" s="308"/>
-      <c r="V5" s="308"/>
-      <c r="W5" s="308"/>
+      <c r="N5" s="320"/>
+      <c r="O5" s="320"/>
+      <c r="P5" s="320"/>
+      <c r="Q5" s="320"/>
+      <c r="R5" s="320"/>
+      <c r="S5" s="320"/>
+      <c r="T5" s="320"/>
+      <c r="U5" s="320"/>
+      <c r="V5" s="320"/>
+      <c r="W5" s="320"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="308"/>
-      <c r="B6" s="308"/>
-      <c r="C6" s="308"/>
-      <c r="D6" s="308"/>
-      <c r="E6" s="308"/>
-      <c r="F6" s="308"/>
-      <c r="G6" s="308"/>
-      <c r="H6" s="308"/>
-      <c r="I6" s="308"/>
-      <c r="J6" s="308"/>
-      <c r="K6" s="308"/>
-      <c r="M6" s="308"/>
-      <c r="N6" s="308"/>
-      <c r="O6" s="308"/>
-      <c r="P6" s="308"/>
-      <c r="Q6" s="308"/>
-      <c r="R6" s="308"/>
-      <c r="S6" s="308"/>
-      <c r="T6" s="308"/>
-      <c r="U6" s="308"/>
-      <c r="V6" s="308"/>
-      <c r="W6" s="308"/>
+      <c r="A6" s="320"/>
+      <c r="B6" s="320"/>
+      <c r="C6" s="320"/>
+      <c r="D6" s="320"/>
+      <c r="E6" s="320"/>
+      <c r="F6" s="320"/>
+      <c r="G6" s="320"/>
+      <c r="H6" s="320"/>
+      <c r="I6" s="320"/>
+      <c r="J6" s="320"/>
+      <c r="K6" s="320"/>
+      <c r="M6" s="320"/>
+      <c r="N6" s="320"/>
+      <c r="O6" s="320"/>
+      <c r="P6" s="320"/>
+      <c r="Q6" s="320"/>
+      <c r="R6" s="320"/>
+      <c r="S6" s="320"/>
+      <c r="T6" s="320"/>
+      <c r="U6" s="320"/>
+      <c r="V6" s="320"/>
+      <c r="W6" s="320"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M7" s="251"/>
@@ -15452,7 +15455,7 @@
       </c>
       <c r="Q28" s="212">
         <f>'Pembayaran Makrab 19'!F40</f>
-        <v>600000</v>
+        <v>650000</v>
       </c>
       <c r="R28" s="212"/>
       <c r="S28" s="251"/>
@@ -15607,7 +15610,7 @@
       </c>
       <c r="Q34" s="225">
         <f>SUM(Q9:Q33)</f>
-        <v>4181144.27</v>
+        <v>4231144.2699999996</v>
       </c>
       <c r="R34" s="226">
         <f>SUM(R9:R33)</f>
@@ -15638,7 +15641,7 @@
       <c r="P35" s="330"/>
       <c r="Q35" s="324">
         <f>Q34-R34</f>
-        <v>3606144.27</v>
+        <v>3656144.2699999996</v>
       </c>
       <c r="R35" s="325"/>
       <c r="S35" s="251"/>
@@ -15684,8 +15687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15803,10 +15806,18 @@
       <c r="B9" s="57">
         <v>6</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="56"/>
+      <c r="C9" s="57" t="s">
+        <v>364</v>
+      </c>
+      <c r="D9" s="57" t="s">
+        <v>362</v>
+      </c>
+      <c r="E9" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="F9" s="56">
+        <v>50000</v>
+      </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="57">
@@ -16087,7 +16098,7 @@
       <c r="E40" s="336"/>
       <c r="F40" s="279">
         <f>SUM(F4:F39)</f>
-        <v>600000</v>
+        <v>650000</v>
       </c>
     </row>
   </sheetData>
@@ -16142,17 +16153,17 @@
       <c r="A2" s="174"/>
       <c r="B2" s="175"/>
       <c r="C2" s="175"/>
-      <c r="D2" s="394" t="s">
+      <c r="D2" s="337" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="394"/>
-      <c r="F2" s="394"/>
-      <c r="G2" s="394"/>
-      <c r="H2" s="394"/>
-      <c r="I2" s="394"/>
-      <c r="J2" s="394"/>
-      <c r="K2" s="394"/>
-      <c r="L2" s="394"/>
+      <c r="E2" s="337"/>
+      <c r="F2" s="337"/>
+      <c r="G2" s="337"/>
+      <c r="H2" s="337"/>
+      <c r="I2" s="337"/>
+      <c r="J2" s="337"/>
+      <c r="K2" s="337"/>
+      <c r="L2" s="337"/>
       <c r="M2" s="176"/>
       <c r="N2" s="24"/>
     </row>
@@ -16170,205 +16181,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="178"/>
-      <c r="U3" s="337" t="s">
+      <c r="U3" s="387" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="338"/>
-      <c r="W3" s="339" t="s">
+      <c r="V3" s="388"/>
+      <c r="W3" s="389" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="338"/>
-      <c r="Y3" s="338"/>
-      <c r="Z3" s="338"/>
-      <c r="AA3" s="338"/>
-      <c r="AB3" s="338"/>
-      <c r="AC3" s="338"/>
-      <c r="AD3" s="340"/>
+      <c r="X3" s="388"/>
+      <c r="Y3" s="388"/>
+      <c r="Z3" s="388"/>
+      <c r="AA3" s="388"/>
+      <c r="AB3" s="388"/>
+      <c r="AC3" s="388"/>
+      <c r="AD3" s="390"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="177"/>
-      <c r="B4" s="398" t="s">
+      <c r="B4" s="352" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="399"/>
-      <c r="D4" s="399"/>
-      <c r="E4" s="399"/>
-      <c r="F4" s="399"/>
+      <c r="C4" s="353"/>
+      <c r="D4" s="353"/>
+      <c r="E4" s="353"/>
+      <c r="F4" s="353"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="346" t="s">
+      <c r="I4" s="356" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="314"/>
-      <c r="K4" s="314"/>
-      <c r="L4" s="314"/>
+      <c r="J4" s="311"/>
+      <c r="K4" s="311"/>
+      <c r="L4" s="311"/>
       <c r="M4" s="178"/>
-      <c r="U4" s="358" t="s">
+      <c r="U4" s="399" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="314"/>
-      <c r="W4" s="346" t="s">
+      <c r="V4" s="311"/>
+      <c r="W4" s="356" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="314"/>
-      <c r="Y4" s="314"/>
-      <c r="Z4" s="314"/>
-      <c r="AA4" s="314"/>
-      <c r="AB4" s="314"/>
-      <c r="AC4" s="314"/>
-      <c r="AD4" s="341"/>
+      <c r="X4" s="311"/>
+      <c r="Y4" s="311"/>
+      <c r="Z4" s="311"/>
+      <c r="AA4" s="311"/>
+      <c r="AB4" s="311"/>
+      <c r="AC4" s="311"/>
+      <c r="AD4" s="376"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="177"/>
-      <c r="B5" s="363" t="s">
+      <c r="B5" s="347" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="314"/>
-      <c r="D5" s="314"/>
-      <c r="E5" s="314"/>
-      <c r="F5" s="314"/>
+      <c r="C5" s="311"/>
+      <c r="D5" s="311"/>
+      <c r="E5" s="311"/>
+      <c r="F5" s="311"/>
       <c r="G5" s="154">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="365" t="s">
+      <c r="I5" s="345" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="386"/>
-      <c r="K5" s="388">
+      <c r="J5" s="346"/>
+      <c r="K5" s="357">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="389"/>
+      <c r="L5" s="358"/>
       <c r="M5" s="178"/>
-      <c r="U5" s="359" t="s">
+      <c r="U5" s="383" t="s">
         <v>231</v>
       </c>
-      <c r="V5" s="360"/>
-      <c r="W5" s="365" t="s">
+      <c r="V5" s="384"/>
+      <c r="W5" s="345" t="s">
         <v>232</v>
       </c>
-      <c r="X5" s="366"/>
-      <c r="Y5" s="366"/>
-      <c r="Z5" s="366"/>
-      <c r="AA5" s="366"/>
-      <c r="AB5" s="366"/>
-      <c r="AC5" s="366"/>
-      <c r="AD5" s="367"/>
+      <c r="X5" s="370"/>
+      <c r="Y5" s="370"/>
+      <c r="Z5" s="370"/>
+      <c r="AA5" s="370"/>
+      <c r="AB5" s="370"/>
+      <c r="AC5" s="370"/>
+      <c r="AD5" s="371"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="177"/>
-      <c r="B6" s="356" t="s">
+      <c r="B6" s="339" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="357"/>
-      <c r="D6" s="357"/>
-      <c r="E6" s="357"/>
-      <c r="F6" s="357"/>
+      <c r="C6" s="340"/>
+      <c r="D6" s="340"/>
+      <c r="E6" s="340"/>
+      <c r="F6" s="340"/>
       <c r="G6" s="154">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="387" t="s">
+      <c r="I6" s="343" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="382"/>
-      <c r="K6" s="390">
+      <c r="J6" s="344"/>
+      <c r="K6" s="359">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="391"/>
+      <c r="L6" s="360"/>
       <c r="M6" s="178"/>
-      <c r="U6" s="361"/>
-      <c r="V6" s="362"/>
-      <c r="W6" s="347" t="s">
+      <c r="U6" s="385"/>
+      <c r="V6" s="386"/>
+      <c r="W6" s="372" t="s">
         <v>233</v>
       </c>
-      <c r="X6" s="348"/>
-      <c r="Y6" s="348"/>
-      <c r="Z6" s="348"/>
-      <c r="AA6" s="348"/>
-      <c r="AB6" s="348"/>
-      <c r="AC6" s="348"/>
-      <c r="AD6" s="349"/>
+      <c r="X6" s="373"/>
+      <c r="Y6" s="373"/>
+      <c r="Z6" s="373"/>
+      <c r="AA6" s="373"/>
+      <c r="AB6" s="373"/>
+      <c r="AC6" s="373"/>
+      <c r="AD6" s="374"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="177"/>
-      <c r="B7" s="368" t="s">
+      <c r="B7" s="350" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="369"/>
-      <c r="D7" s="369"/>
-      <c r="E7" s="369"/>
-      <c r="F7" s="382"/>
+      <c r="C7" s="351"/>
+      <c r="D7" s="351"/>
+      <c r="E7" s="351"/>
+      <c r="F7" s="344"/>
       <c r="G7" s="154">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="387" t="s">
+      <c r="I7" s="343" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="382"/>
-      <c r="K7" s="392">
+      <c r="J7" s="344"/>
+      <c r="K7" s="354">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="393"/>
+      <c r="L7" s="355"/>
       <c r="M7" s="178"/>
-      <c r="U7" s="344"/>
-      <c r="V7" s="345"/>
-      <c r="W7" s="346" t="s">
+      <c r="U7" s="391"/>
+      <c r="V7" s="392"/>
+      <c r="W7" s="356" t="s">
         <v>234</v>
       </c>
-      <c r="X7" s="314"/>
-      <c r="Y7" s="314"/>
-      <c r="Z7" s="314"/>
-      <c r="AA7" s="314"/>
-      <c r="AB7" s="314"/>
-      <c r="AC7" s="314"/>
-      <c r="AD7" s="341"/>
+      <c r="X7" s="311"/>
+      <c r="Y7" s="311"/>
+      <c r="Z7" s="311"/>
+      <c r="AA7" s="311"/>
+      <c r="AB7" s="311"/>
+      <c r="AC7" s="311"/>
+      <c r="AD7" s="376"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="177"/>
-      <c r="B8" s="396" t="s">
+      <c r="B8" s="348" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="397"/>
-      <c r="D8" s="397"/>
-      <c r="E8" s="397"/>
-      <c r="F8" s="397"/>
+      <c r="C8" s="349"/>
+      <c r="D8" s="349"/>
+      <c r="E8" s="349"/>
+      <c r="F8" s="349"/>
       <c r="G8" s="155">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="365" t="s">
+      <c r="I8" s="345" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="386"/>
-      <c r="K8" s="377">
+      <c r="J8" s="346"/>
+      <c r="K8" s="341">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="378"/>
+      <c r="L8" s="342"/>
       <c r="M8" s="178"/>
-      <c r="U8" s="352" t="s">
+      <c r="U8" s="395" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="353"/>
-      <c r="W8" s="347" t="s">
+      <c r="V8" s="396"/>
+      <c r="W8" s="372" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="348"/>
-      <c r="Y8" s="348"/>
-      <c r="Z8" s="348"/>
-      <c r="AA8" s="348"/>
-      <c r="AB8" s="348"/>
-      <c r="AC8" s="348"/>
-      <c r="AD8" s="349"/>
+      <c r="X8" s="373"/>
+      <c r="Y8" s="373"/>
+      <c r="Z8" s="373"/>
+      <c r="AA8" s="373"/>
+      <c r="AB8" s="373"/>
+      <c r="AC8" s="373"/>
+      <c r="AD8" s="374"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="177"/>
@@ -16384,28 +16395,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="178"/>
-      <c r="U9" s="354"/>
-      <c r="V9" s="355"/>
-      <c r="W9" s="347" t="s">
+      <c r="U9" s="397"/>
+      <c r="V9" s="398"/>
+      <c r="W9" s="372" t="s">
         <v>237</v>
       </c>
-      <c r="X9" s="348"/>
-      <c r="Y9" s="348"/>
-      <c r="Z9" s="348"/>
-      <c r="AA9" s="348"/>
-      <c r="AB9" s="348"/>
-      <c r="AC9" s="348"/>
-      <c r="AD9" s="349"/>
+      <c r="X9" s="373"/>
+      <c r="Y9" s="373"/>
+      <c r="Z9" s="373"/>
+      <c r="AA9" s="373"/>
+      <c r="AB9" s="373"/>
+      <c r="AC9" s="373"/>
+      <c r="AD9" s="374"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="177"/>
-      <c r="B10" s="314" t="s">
+      <c r="B10" s="311" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="314"/>
-      <c r="D10" s="314"/>
-      <c r="E10" s="314"/>
-      <c r="F10" s="314"/>
+      <c r="C10" s="311"/>
+      <c r="D10" s="311"/>
+      <c r="E10" s="311"/>
+      <c r="F10" s="311"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -16416,30 +16427,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="178"/>
-      <c r="U10" s="356" t="s">
+      <c r="U10" s="339" t="s">
         <v>243</v>
       </c>
-      <c r="V10" s="357"/>
-      <c r="W10" s="314" t="s">
+      <c r="V10" s="340"/>
+      <c r="W10" s="311" t="s">
         <v>257</v>
       </c>
-      <c r="X10" s="314"/>
-      <c r="Y10" s="314"/>
-      <c r="Z10" s="314"/>
-      <c r="AA10" s="314"/>
-      <c r="AB10" s="314"/>
-      <c r="AC10" s="314"/>
-      <c r="AD10" s="341"/>
+      <c r="X10" s="311"/>
+      <c r="Y10" s="311"/>
+      <c r="Z10" s="311"/>
+      <c r="AA10" s="311"/>
+      <c r="AB10" s="311"/>
+      <c r="AC10" s="311"/>
+      <c r="AD10" s="376"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="177"/>
-      <c r="B11" s="314" t="s">
+      <c r="B11" s="311" t="s">
         <v>254</v>
       </c>
-      <c r="C11" s="314"/>
-      <c r="D11" s="314"/>
-      <c r="E11" s="314"/>
-      <c r="F11" s="314"/>
+      <c r="C11" s="311"/>
+      <c r="D11" s="311"/>
+      <c r="E11" s="311"/>
+      <c r="F11" s="311"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -16449,30 +16460,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="178"/>
-      <c r="U11" s="356" t="s">
+      <c r="U11" s="339" t="s">
         <v>256</v>
       </c>
-      <c r="V11" s="357"/>
-      <c r="W11" s="350" t="s">
+      <c r="V11" s="340"/>
+      <c r="W11" s="393" t="s">
         <v>258</v>
       </c>
-      <c r="X11" s="350"/>
-      <c r="Y11" s="350"/>
-      <c r="Z11" s="350"/>
-      <c r="AA11" s="350"/>
-      <c r="AB11" s="350"/>
-      <c r="AC11" s="350"/>
-      <c r="AD11" s="351"/>
+      <c r="X11" s="393"/>
+      <c r="Y11" s="393"/>
+      <c r="Z11" s="393"/>
+      <c r="AA11" s="393"/>
+      <c r="AB11" s="393"/>
+      <c r="AC11" s="393"/>
+      <c r="AD11" s="394"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="177"/>
-      <c r="B12" s="395" t="s">
+      <c r="B12" s="338" t="s">
         <v>255</v>
       </c>
-      <c r="C12" s="395"/>
-      <c r="D12" s="395"/>
-      <c r="E12" s="395"/>
-      <c r="F12" s="395"/>
+      <c r="C12" s="338"/>
+      <c r="D12" s="338"/>
+      <c r="E12" s="338"/>
+      <c r="F12" s="338"/>
       <c r="G12" s="182">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -16483,16 +16494,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="178"/>
-      <c r="U12" s="356"/>
-      <c r="V12" s="357"/>
-      <c r="W12" s="314"/>
-      <c r="X12" s="314"/>
-      <c r="Y12" s="314"/>
-      <c r="Z12" s="314"/>
-      <c r="AA12" s="314"/>
-      <c r="AB12" s="314"/>
-      <c r="AC12" s="314"/>
-      <c r="AD12" s="341"/>
+      <c r="U12" s="339"/>
+      <c r="V12" s="340"/>
+      <c r="W12" s="311"/>
+      <c r="X12" s="311"/>
+      <c r="Y12" s="311"/>
+      <c r="Z12" s="311"/>
+      <c r="AA12" s="311"/>
+      <c r="AB12" s="311"/>
+      <c r="AC12" s="311"/>
+      <c r="AD12" s="376"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="179"/>
@@ -16508,64 +16519,64 @@
       <c r="K13" s="180"/>
       <c r="L13" s="180"/>
       <c r="M13" s="181"/>
-      <c r="U13" s="356"/>
-      <c r="V13" s="357"/>
-      <c r="W13" s="314"/>
-      <c r="X13" s="314"/>
-      <c r="Y13" s="314"/>
-      <c r="Z13" s="314"/>
-      <c r="AA13" s="314"/>
-      <c r="AB13" s="314"/>
-      <c r="AC13" s="314"/>
-      <c r="AD13" s="341"/>
+      <c r="U13" s="339"/>
+      <c r="V13" s="340"/>
+      <c r="W13" s="311"/>
+      <c r="X13" s="311"/>
+      <c r="Y13" s="311"/>
+      <c r="Z13" s="311"/>
+      <c r="AA13" s="311"/>
+      <c r="AB13" s="311"/>
+      <c r="AC13" s="311"/>
+      <c r="AD13" s="376"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="371"/>
-      <c r="V14" s="372"/>
-      <c r="W14" s="342"/>
-      <c r="X14" s="342"/>
-      <c r="Y14" s="342"/>
-      <c r="Z14" s="342"/>
-      <c r="AA14" s="342"/>
-      <c r="AB14" s="342"/>
-      <c r="AC14" s="342"/>
-      <c r="AD14" s="343"/>
+      <c r="U14" s="377"/>
+      <c r="V14" s="378"/>
+      <c r="W14" s="368"/>
+      <c r="X14" s="368"/>
+      <c r="Y14" s="368"/>
+      <c r="Z14" s="368"/>
+      <c r="AA14" s="368"/>
+      <c r="AB14" s="368"/>
+      <c r="AC14" s="368"/>
+      <c r="AD14" s="369"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="174"/>
       <c r="B18" s="175"/>
       <c r="C18" s="175"/>
-      <c r="D18" s="394" t="s">
+      <c r="D18" s="337" t="s">
         <v>249</v>
       </c>
-      <c r="E18" s="394"/>
-      <c r="F18" s="394"/>
-      <c r="G18" s="394"/>
-      <c r="H18" s="394"/>
-      <c r="I18" s="394"/>
-      <c r="J18" s="394"/>
-      <c r="K18" s="394"/>
-      <c r="L18" s="394"/>
+      <c r="E18" s="337"/>
+      <c r="F18" s="337"/>
+      <c r="G18" s="337"/>
+      <c r="H18" s="337"/>
+      <c r="I18" s="337"/>
+      <c r="J18" s="337"/>
+      <c r="K18" s="337"/>
+      <c r="L18" s="337"/>
       <c r="M18" s="176"/>
-      <c r="O18" s="373" t="s">
+      <c r="O18" s="379" t="s">
         <v>250</v>
       </c>
-      <c r="P18" s="374"/>
-      <c r="Q18" s="374"/>
-      <c r="R18" s="374"/>
-      <c r="S18" s="375"/>
+      <c r="P18" s="380"/>
+      <c r="Q18" s="380"/>
+      <c r="R18" s="380"/>
+      <c r="S18" s="381"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="177"/>
       <c r="M19" s="178"/>
-      <c r="O19" s="363" t="s">
+      <c r="O19" s="347" t="s">
         <v>251</v>
       </c>
-      <c r="P19" s="314"/>
-      <c r="Q19" s="314"/>
-      <c r="R19" s="314"/>
-      <c r="S19" s="341"/>
+      <c r="P19" s="311"/>
+      <c r="Q19" s="311"/>
+      <c r="R19" s="311"/>
+      <c r="S19" s="376"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="177"/>
@@ -16576,119 +16587,119 @@
       <c r="F20" s="202"/>
       <c r="G20" s="68"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="346" t="s">
+      <c r="I20" s="356" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="314"/>
-      <c r="K20" s="314"/>
-      <c r="L20" s="314"/>
+      <c r="J20" s="311"/>
+      <c r="K20" s="311"/>
+      <c r="L20" s="311"/>
       <c r="M20" s="178"/>
-      <c r="O20" s="363" t="s">
+      <c r="O20" s="347" t="s">
         <v>252</v>
       </c>
-      <c r="P20" s="314"/>
-      <c r="Q20" s="314"/>
-      <c r="R20" s="314"/>
-      <c r="S20" s="341"/>
+      <c r="P20" s="311"/>
+      <c r="Q20" s="311"/>
+      <c r="R20" s="311"/>
+      <c r="S20" s="376"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="177"/>
-      <c r="B21" s="379" t="s">
+      <c r="B21" s="361" t="s">
         <v>296</v>
       </c>
-      <c r="C21" s="380"/>
-      <c r="D21" s="380"/>
-      <c r="E21" s="380"/>
-      <c r="F21" s="381"/>
+      <c r="C21" s="362"/>
+      <c r="D21" s="362"/>
+      <c r="E21" s="362"/>
+      <c r="F21" s="363"/>
       <c r="G21" s="70">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="365" t="s">
+      <c r="I21" s="345" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="386"/>
-      <c r="K21" s="388">
+      <c r="J21" s="346"/>
+      <c r="K21" s="357">
         <f>G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="L21" s="389"/>
+      <c r="L21" s="358"/>
       <c r="M21" s="178"/>
       <c r="N21" s="172"/>
-      <c r="O21" s="376" t="s">
+      <c r="O21" s="382" t="s">
         <v>259</v>
       </c>
-      <c r="P21" s="366"/>
-      <c r="Q21" s="366"/>
-      <c r="R21" s="366"/>
-      <c r="S21" s="367"/>
+      <c r="P21" s="370"/>
+      <c r="Q21" s="370"/>
+      <c r="R21" s="370"/>
+      <c r="S21" s="371"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="177"/>
-      <c r="B22" s="368" t="s">
+      <c r="B22" s="350" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="369"/>
-      <c r="D22" s="369"/>
-      <c r="E22" s="369"/>
-      <c r="F22" s="382"/>
+      <c r="C22" s="351"/>
+      <c r="D22" s="351"/>
+      <c r="E22" s="351"/>
+      <c r="F22" s="344"/>
       <c r="G22" s="154">
         <f>G21</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="387" t="s">
+      <c r="I22" s="343" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="382"/>
-      <c r="K22" s="390">
+      <c r="J22" s="344"/>
+      <c r="K22" s="359">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="L22" s="391"/>
+      <c r="L22" s="360"/>
       <c r="M22" s="178"/>
       <c r="N22" s="172"/>
-      <c r="O22" s="368" t="s">
+      <c r="O22" s="350" t="s">
         <v>260</v>
       </c>
-      <c r="P22" s="369"/>
-      <c r="Q22" s="369"/>
-      <c r="R22" s="369"/>
-      <c r="S22" s="370"/>
+      <c r="P22" s="351"/>
+      <c r="Q22" s="351"/>
+      <c r="R22" s="351"/>
+      <c r="S22" s="375"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="177"/>
-      <c r="B23" s="383" t="s">
+      <c r="B23" s="364" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="384"/>
-      <c r="D23" s="384"/>
-      <c r="E23" s="384"/>
-      <c r="F23" s="385"/>
+      <c r="C23" s="365"/>
+      <c r="D23" s="365"/>
+      <c r="E23" s="365"/>
+      <c r="F23" s="366"/>
       <c r="G23" s="155">
         <f>K24</f>
         <v>1568729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="387" t="s">
+      <c r="I23" s="343" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="382"/>
-      <c r="K23" s="392">
+      <c r="J23" s="344"/>
+      <c r="K23" s="354">
         <f>Pemasukkan!L31</f>
         <v>690000</v>
       </c>
-      <c r="L23" s="393"/>
+      <c r="L23" s="355"/>
       <c r="M23" s="178"/>
       <c r="N23" s="172"/>
-      <c r="O23" s="368" t="s">
+      <c r="O23" s="350" t="s">
         <v>261</v>
       </c>
-      <c r="P23" s="369"/>
-      <c r="Q23" s="369"/>
-      <c r="R23" s="369"/>
-      <c r="S23" s="370"/>
+      <c r="P23" s="351"/>
+      <c r="Q23" s="351"/>
+      <c r="R23" s="351"/>
+      <c r="S23" s="375"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="177"/>
@@ -16699,24 +16710,24 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="365" t="s">
+      <c r="I24" s="345" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="386"/>
-      <c r="K24" s="377">
+      <c r="J24" s="346"/>
+      <c r="K24" s="341">
         <f>(K21-K22)+K23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="L24" s="378"/>
+      <c r="L24" s="342"/>
       <c r="M24" s="178"/>
       <c r="N24" s="172"/>
-      <c r="O24" s="368" t="s">
+      <c r="O24" s="350" t="s">
         <v>262</v>
       </c>
-      <c r="P24" s="369"/>
-      <c r="Q24" s="369"/>
-      <c r="R24" s="369"/>
-      <c r="S24" s="370"/>
+      <c r="P24" s="351"/>
+      <c r="Q24" s="351"/>
+      <c r="R24" s="351"/>
+      <c r="S24" s="375"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="177"/>
@@ -16733,13 +16744,13 @@
       <c r="L25" s="24"/>
       <c r="M25" s="178"/>
       <c r="N25" s="172"/>
-      <c r="O25" s="363" t="s">
+      <c r="O25" s="347" t="s">
         <v>267</v>
       </c>
-      <c r="P25" s="314"/>
-      <c r="Q25" s="314"/>
-      <c r="R25" s="314"/>
-      <c r="S25" s="341"/>
+      <c r="P25" s="311"/>
+      <c r="Q25" s="311"/>
+      <c r="R25" s="311"/>
+      <c r="S25" s="376"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="177"/>
@@ -16756,11 +16767,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="178"/>
       <c r="N26" s="172"/>
-      <c r="O26" s="364"/>
-      <c r="P26" s="342"/>
-      <c r="Q26" s="342"/>
-      <c r="R26" s="342"/>
-      <c r="S26" s="343"/>
+      <c r="O26" s="367"/>
+      <c r="P26" s="368"/>
+      <c r="Q26" s="368"/>
+      <c r="R26" s="368"/>
+      <c r="S26" s="369"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="179"/>
@@ -16795,6 +16806,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:AD3"/>
+    <mergeCell ref="W12:AD12"/>
+    <mergeCell ref="W13:AD13"/>
+    <mergeCell ref="W14:AD14"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:AD7"/>
+    <mergeCell ref="W9:AD9"/>
+    <mergeCell ref="W10:AD10"/>
+    <mergeCell ref="W11:AD11"/>
+    <mergeCell ref="U8:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:AD4"/>
+    <mergeCell ref="W8:AD8"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="O25:S25"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="W5:AD5"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="O18:S18"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O23:S23"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
     <mergeCell ref="D2:L2"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
@@ -16811,53 +16869,6 @@
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="W5:AD5"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="O24:S24"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="O18:S18"/>
-    <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O23:S23"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="W4:AD4"/>
-    <mergeCell ref="W8:AD8"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="O25:S25"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:AD3"/>
-    <mergeCell ref="W12:AD12"/>
-    <mergeCell ref="W13:AD13"/>
-    <mergeCell ref="W14:AD14"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="W7:AD7"/>
-    <mergeCell ref="W9:AD9"/>
-    <mergeCell ref="W10:AD10"/>
-    <mergeCell ref="W11:AD11"/>
-    <mergeCell ref="U8:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U4:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -16891,44 +16902,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="409" t="s">
+      <c r="C2" s="400" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="410"/>
-      <c r="E2" s="410"/>
-      <c r="F2" s="410"/>
-      <c r="G2" s="410"/>
-      <c r="H2" s="410"/>
-      <c r="I2" s="410"/>
-      <c r="J2" s="410"/>
-      <c r="K2" s="410"/>
+      <c r="D2" s="401"/>
+      <c r="E2" s="401"/>
+      <c r="F2" s="401"/>
+      <c r="G2" s="401"/>
+      <c r="H2" s="401"/>
+      <c r="I2" s="401"/>
+      <c r="J2" s="401"/>
+      <c r="K2" s="401"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="410"/>
-      <c r="D3" s="410"/>
-      <c r="E3" s="410"/>
-      <c r="F3" s="410"/>
-      <c r="G3" s="410"/>
-      <c r="H3" s="410"/>
-      <c r="I3" s="410"/>
-      <c r="J3" s="410"/>
-      <c r="K3" s="410"/>
+      <c r="C3" s="401"/>
+      <c r="D3" s="401"/>
+      <c r="E3" s="401"/>
+      <c r="F3" s="401"/>
+      <c r="G3" s="401"/>
+      <c r="H3" s="401"/>
+      <c r="I3" s="401"/>
+      <c r="J3" s="401"/>
+      <c r="K3" s="401"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="402" t="s">
+      <c r="C5" s="408" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="402"/>
-      <c r="E5" s="402"/>
-      <c r="F5" s="402"/>
-      <c r="G5" s="402"/>
-      <c r="I5" s="402" t="s">
+      <c r="D5" s="408"/>
+      <c r="E5" s="408"/>
+      <c r="F5" s="408"/>
+      <c r="G5" s="408"/>
+      <c r="I5" s="408" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="402"/>
-      <c r="K5" s="402"/>
-      <c r="L5" s="402"/>
-      <c r="M5" s="402"/>
+      <c r="J5" s="408"/>
+      <c r="K5" s="408"/>
+      <c r="L5" s="408"/>
+      <c r="M5" s="408"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -17368,88 +17379,88 @@
       <c r="M28" s="172"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="398" t="s">
+      <c r="D29" s="352" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="399"/>
-      <c r="F29" s="403">
+      <c r="E29" s="353"/>
+      <c r="F29" s="402">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="404"/>
+      <c r="G29" s="403"/>
       <c r="I29" s="172"/>
-      <c r="J29" s="398" t="s">
+      <c r="J29" s="352" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="399"/>
-      <c r="L29" s="403">
+      <c r="K29" s="353"/>
+      <c r="L29" s="402">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="404"/>
+      <c r="M29" s="403"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="358" t="s">
+      <c r="D30" s="399" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="314"/>
-      <c r="F30" s="405">
+      <c r="E30" s="311"/>
+      <c r="F30" s="404">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="406"/>
+      <c r="G30" s="405"/>
       <c r="I30" s="172"/>
-      <c r="J30" s="358" t="s">
+      <c r="J30" s="399" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="314"/>
-      <c r="L30" s="405">
+      <c r="K30" s="311"/>
+      <c r="L30" s="404">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="406"/>
+      <c r="M30" s="405"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="363" t="s">
+      <c r="D31" s="347" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="314"/>
-      <c r="F31" s="407">
+      <c r="E31" s="311"/>
+      <c r="F31" s="409">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="408"/>
+      <c r="G31" s="410"/>
       <c r="I31" s="172"/>
-      <c r="J31" s="363" t="s">
+      <c r="J31" s="347" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="314"/>
-      <c r="L31" s="407">
+      <c r="K31" s="311"/>
+      <c r="L31" s="409">
         <f>L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="408"/>
+      <c r="M31" s="410"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="396" t="s">
+      <c r="D32" s="348" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="397"/>
-      <c r="F32" s="400">
+      <c r="E32" s="349"/>
+      <c r="F32" s="406">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="401"/>
+      <c r="G32" s="407"/>
       <c r="I32" s="172"/>
-      <c r="J32" s="396" t="s">
+      <c r="J32" s="348" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="397"/>
-      <c r="L32" s="400">
+      <c r="K32" s="349"/>
+      <c r="L32" s="406">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="401"/>
+      <c r="M32" s="407"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17641,12 +17652,6 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C2:K3"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J29:K29"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="I5:M5"/>
@@ -17660,6 +17665,12 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J32:K32"/>
+    <mergeCell ref="C2:K3"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -17692,44 +17703,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="415" t="s">
+      <c r="C2" s="411" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="416"/>
-      <c r="E2" s="416"/>
-      <c r="F2" s="416"/>
-      <c r="G2" s="416"/>
-      <c r="H2" s="416"/>
-      <c r="I2" s="416"/>
-      <c r="J2" s="416"/>
-      <c r="K2" s="416"/>
+      <c r="D2" s="412"/>
+      <c r="E2" s="412"/>
+      <c r="F2" s="412"/>
+      <c r="G2" s="412"/>
+      <c r="H2" s="412"/>
+      <c r="I2" s="412"/>
+      <c r="J2" s="412"/>
+      <c r="K2" s="412"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="416"/>
-      <c r="D3" s="416"/>
-      <c r="E3" s="416"/>
-      <c r="F3" s="416"/>
-      <c r="G3" s="416"/>
-      <c r="H3" s="416"/>
-      <c r="I3" s="416"/>
-      <c r="J3" s="416"/>
-      <c r="K3" s="416"/>
+      <c r="C3" s="412"/>
+      <c r="D3" s="412"/>
+      <c r="E3" s="412"/>
+      <c r="F3" s="412"/>
+      <c r="G3" s="412"/>
+      <c r="H3" s="412"/>
+      <c r="I3" s="412"/>
+      <c r="J3" s="412"/>
+      <c r="K3" s="412"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="402" t="s">
+      <c r="C5" s="408" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="402"/>
-      <c r="E5" s="402"/>
-      <c r="F5" s="402"/>
-      <c r="G5" s="402"/>
-      <c r="I5" s="402" t="s">
+      <c r="D5" s="408"/>
+      <c r="E5" s="408"/>
+      <c r="F5" s="408"/>
+      <c r="G5" s="408"/>
+      <c r="I5" s="408" t="s">
         <v>246</v>
       </c>
-      <c r="J5" s="402"/>
-      <c r="K5" s="402"/>
-      <c r="L5" s="402"/>
-      <c r="M5" s="402"/>
+      <c r="J5" s="408"/>
+      <c r="K5" s="408"/>
+      <c r="L5" s="408"/>
+      <c r="M5" s="408"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -18213,20 +18224,20 @@
       <c r="M28" s="172"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="337" t="s">
+      <c r="D29" s="387" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="339"/>
+      <c r="E29" s="389"/>
       <c r="F29" s="413">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
       <c r="G29" s="414"/>
       <c r="I29" s="172"/>
-      <c r="J29" s="337" t="s">
+      <c r="J29" s="387" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="339"/>
+      <c r="K29" s="389"/>
       <c r="L29" s="413">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
@@ -18234,67 +18245,67 @@
       <c r="M29" s="414"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="363" t="s">
+      <c r="D30" s="347" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="314"/>
-      <c r="F30" s="405">
+      <c r="E30" s="311"/>
+      <c r="F30" s="404">
         <f>F27</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="406"/>
+      <c r="G30" s="405"/>
       <c r="I30" s="172"/>
-      <c r="J30" s="363" t="s">
+      <c r="J30" s="347" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="314"/>
-      <c r="L30" s="405">
+      <c r="K30" s="311"/>
+      <c r="L30" s="404">
         <f>L27</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="406"/>
+      <c r="M30" s="405"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="363" t="s">
+      <c r="D31" s="347" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="314"/>
-      <c r="F31" s="407">
+      <c r="E31" s="311"/>
+      <c r="F31" s="409">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="408"/>
+      <c r="G31" s="410"/>
       <c r="I31" s="172"/>
-      <c r="J31" s="363" t="s">
+      <c r="J31" s="347" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="314"/>
-      <c r="L31" s="407">
+      <c r="K31" s="311"/>
+      <c r="L31" s="409">
         <f>Pemasukkan!L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="408"/>
+      <c r="M31" s="410"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="396" t="s">
+      <c r="D32" s="348" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="397"/>
-      <c r="F32" s="411">
+      <c r="E32" s="349"/>
+      <c r="F32" s="415">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="412"/>
+      <c r="G32" s="416"/>
       <c r="I32" s="172"/>
-      <c r="J32" s="396" t="s">
+      <c r="J32" s="348" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="397"/>
-      <c r="L32" s="411">
+      <c r="K32" s="349"/>
+      <c r="L32" s="415">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="412"/>
+      <c r="M32" s="416"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18486,6 +18497,14 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
     <mergeCell ref="C2:K3"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
@@ -18497,14 +18516,6 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Khairul Bayar Uang Makrab,Perubahan pendataan
Data sirkulasi untuk makrab di pindah ke sheet Pembayaran Makrab
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="371">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -1118,6 +1118,24 @@
   </si>
   <si>
     <t>Yahya(Makan doang)</t>
+  </si>
+  <si>
+    <t>Khairul</t>
+  </si>
+  <si>
+    <t>Sumbangan KAS</t>
+  </si>
+  <si>
+    <t>Total Uang Makrab</t>
+  </si>
+  <si>
+    <t>Uang KAS Makrab</t>
+  </si>
+  <si>
+    <t>Sumbangan Makrab</t>
+  </si>
+  <si>
+    <t>UANG SUMBANGAN KAS UNTUK MAKRAB BELOM DI TARIK DARI ATM</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1159,7 @@
     <numFmt numFmtId="176" formatCode="[$IDR]\ #,##0_);\([$IDR]\ #,##0\)"/>
     <numFmt numFmtId="177" formatCode="dd\ mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1224,6 +1242,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2336,7 +2361,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="434">
+  <cellXfs count="439">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2950,6 +2975,13 @@
     <xf numFmtId="177" fontId="4" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3382,6 +3414,12 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4542,126 +4580,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="281" t="s">
+      <c r="A1" s="284" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="282"/>
-      <c r="C1" s="282"/>
-      <c r="D1" s="282"/>
-      <c r="E1" s="282"/>
-      <c r="F1" s="282"/>
-      <c r="G1" s="282"/>
-      <c r="H1" s="282"/>
-      <c r="I1" s="282"/>
-      <c r="J1" s="282"/>
-      <c r="K1" s="282"/>
-      <c r="L1" s="282"/>
-      <c r="M1" s="282"/>
-      <c r="N1" s="282"/>
-      <c r="O1" s="282"/>
-      <c r="P1" s="282"/>
-      <c r="Q1" s="282"/>
-      <c r="R1" s="282"/>
+      <c r="B1" s="285"/>
+      <c r="C1" s="285"/>
+      <c r="D1" s="285"/>
+      <c r="E1" s="285"/>
+      <c r="F1" s="285"/>
+      <c r="G1" s="285"/>
+      <c r="H1" s="285"/>
+      <c r="I1" s="285"/>
+      <c r="J1" s="285"/>
+      <c r="K1" s="285"/>
+      <c r="L1" s="285"/>
+      <c r="M1" s="285"/>
+      <c r="N1" s="285"/>
+      <c r="O1" s="285"/>
+      <c r="P1" s="285"/>
+      <c r="Q1" s="285"/>
+      <c r="R1" s="285"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="283"/>
-      <c r="B2" s="284"/>
-      <c r="C2" s="284"/>
-      <c r="D2" s="284"/>
-      <c r="E2" s="284"/>
-      <c r="F2" s="284"/>
-      <c r="G2" s="284"/>
-      <c r="H2" s="284"/>
-      <c r="I2" s="284"/>
-      <c r="J2" s="284"/>
-      <c r="K2" s="284"/>
-      <c r="L2" s="284"/>
-      <c r="M2" s="284"/>
-      <c r="N2" s="284"/>
-      <c r="O2" s="284"/>
-      <c r="P2" s="284"/>
-      <c r="Q2" s="284"/>
-      <c r="R2" s="284"/>
+      <c r="A2" s="286"/>
+      <c r="B2" s="287"/>
+      <c r="C2" s="287"/>
+      <c r="D2" s="287"/>
+      <c r="E2" s="287"/>
+      <c r="F2" s="287"/>
+      <c r="G2" s="287"/>
+      <c r="H2" s="287"/>
+      <c r="I2" s="287"/>
+      <c r="J2" s="287"/>
+      <c r="K2" s="287"/>
+      <c r="L2" s="287"/>
+      <c r="M2" s="287"/>
+      <c r="N2" s="287"/>
+      <c r="O2" s="287"/>
+      <c r="P2" s="287"/>
+      <c r="Q2" s="287"/>
+      <c r="R2" s="287"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="283"/>
-      <c r="B3" s="284"/>
-      <c r="C3" s="284"/>
-      <c r="D3" s="284"/>
-      <c r="E3" s="284"/>
-      <c r="F3" s="284"/>
-      <c r="G3" s="284"/>
-      <c r="H3" s="284"/>
-      <c r="I3" s="284"/>
-      <c r="J3" s="284"/>
-      <c r="K3" s="284"/>
-      <c r="L3" s="284"/>
-      <c r="M3" s="284"/>
-      <c r="N3" s="284"/>
-      <c r="O3" s="284"/>
-      <c r="P3" s="284"/>
-      <c r="Q3" s="284"/>
-      <c r="R3" s="284"/>
+      <c r="A3" s="286"/>
+      <c r="B3" s="287"/>
+      <c r="C3" s="287"/>
+      <c r="D3" s="287"/>
+      <c r="E3" s="287"/>
+      <c r="F3" s="287"/>
+      <c r="G3" s="287"/>
+      <c r="H3" s="287"/>
+      <c r="I3" s="287"/>
+      <c r="J3" s="287"/>
+      <c r="K3" s="287"/>
+      <c r="L3" s="287"/>
+      <c r="M3" s="287"/>
+      <c r="N3" s="287"/>
+      <c r="O3" s="287"/>
+      <c r="P3" s="287"/>
+      <c r="Q3" s="287"/>
+      <c r="R3" s="287"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="283"/>
-      <c r="B4" s="284"/>
-      <c r="C4" s="284"/>
-      <c r="D4" s="284"/>
-      <c r="E4" s="284"/>
-      <c r="F4" s="284"/>
-      <c r="G4" s="284"/>
-      <c r="H4" s="284"/>
-      <c r="I4" s="284"/>
-      <c r="J4" s="284"/>
-      <c r="K4" s="284"/>
-      <c r="L4" s="284"/>
-      <c r="M4" s="284"/>
-      <c r="N4" s="284"/>
-      <c r="O4" s="284"/>
-      <c r="P4" s="284"/>
-      <c r="Q4" s="284"/>
-      <c r="R4" s="284"/>
+      <c r="A4" s="286"/>
+      <c r="B4" s="287"/>
+      <c r="C4" s="287"/>
+      <c r="D4" s="287"/>
+      <c r="E4" s="287"/>
+      <c r="F4" s="287"/>
+      <c r="G4" s="287"/>
+      <c r="H4" s="287"/>
+      <c r="I4" s="287"/>
+      <c r="J4" s="287"/>
+      <c r="K4" s="287"/>
+      <c r="L4" s="287"/>
+      <c r="M4" s="287"/>
+      <c r="N4" s="287"/>
+      <c r="O4" s="287"/>
+      <c r="P4" s="287"/>
+      <c r="Q4" s="287"/>
+      <c r="R4" s="287"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="283"/>
-      <c r="B5" s="284"/>
-      <c r="C5" s="284"/>
-      <c r="D5" s="284"/>
-      <c r="E5" s="284"/>
-      <c r="F5" s="284"/>
-      <c r="G5" s="284"/>
-      <c r="H5" s="284"/>
-      <c r="I5" s="284"/>
-      <c r="J5" s="284"/>
-      <c r="K5" s="284"/>
-      <c r="L5" s="284"/>
-      <c r="M5" s="284"/>
-      <c r="N5" s="284"/>
-      <c r="O5" s="284"/>
-      <c r="P5" s="284"/>
-      <c r="Q5" s="284"/>
-      <c r="R5" s="284"/>
+      <c r="A5" s="286"/>
+      <c r="B5" s="287"/>
+      <c r="C5" s="287"/>
+      <c r="D5" s="287"/>
+      <c r="E5" s="287"/>
+      <c r="F5" s="287"/>
+      <c r="G5" s="287"/>
+      <c r="H5" s="287"/>
+      <c r="I5" s="287"/>
+      <c r="J5" s="287"/>
+      <c r="K5" s="287"/>
+      <c r="L5" s="287"/>
+      <c r="M5" s="287"/>
+      <c r="N5" s="287"/>
+      <c r="O5" s="287"/>
+      <c r="P5" s="287"/>
+      <c r="Q5" s="287"/>
+      <c r="R5" s="287"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="283"/>
-      <c r="B6" s="284"/>
-      <c r="C6" s="284"/>
-      <c r="D6" s="284"/>
-      <c r="E6" s="284"/>
-      <c r="F6" s="284"/>
-      <c r="G6" s="284"/>
-      <c r="H6" s="284"/>
-      <c r="I6" s="284"/>
-      <c r="J6" s="284"/>
-      <c r="K6" s="284"/>
-      <c r="L6" s="284"/>
-      <c r="M6" s="284"/>
-      <c r="N6" s="284"/>
-      <c r="O6" s="284"/>
-      <c r="P6" s="284"/>
-      <c r="Q6" s="284"/>
-      <c r="R6" s="284"/>
+      <c r="A6" s="286"/>
+      <c r="B6" s="287"/>
+      <c r="C6" s="287"/>
+      <c r="D6" s="287"/>
+      <c r="E6" s="287"/>
+      <c r="F6" s="287"/>
+      <c r="G6" s="287"/>
+      <c r="H6" s="287"/>
+      <c r="I6" s="287"/>
+      <c r="J6" s="287"/>
+      <c r="K6" s="287"/>
+      <c r="L6" s="287"/>
+      <c r="M6" s="287"/>
+      <c r="N6" s="287"/>
+      <c r="O6" s="287"/>
+      <c r="P6" s="287"/>
+      <c r="Q6" s="287"/>
+      <c r="R6" s="287"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -7606,58 +7644,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="289" t="s">
+      <c r="J79" s="292" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="290"/>
-      <c r="L79" s="290"/>
-      <c r="M79" s="290"/>
-      <c r="N79" s="291"/>
-      <c r="P79" s="297" t="s">
+      <c r="K79" s="293"/>
+      <c r="L79" s="293"/>
+      <c r="M79" s="293"/>
+      <c r="N79" s="294"/>
+      <c r="P79" s="300" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="290"/>
-      <c r="R79" s="290"/>
-      <c r="S79" s="291"/>
+      <c r="Q79" s="293"/>
+      <c r="R79" s="293"/>
+      <c r="S79" s="294"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="292" t="s">
+      <c r="J80" s="295" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="284"/>
-      <c r="L80" s="284"/>
-      <c r="M80" s="284"/>
-      <c r="N80" s="293"/>
-      <c r="P80" s="292" t="s">
+      <c r="K80" s="287"/>
+      <c r="L80" s="287"/>
+      <c r="M80" s="287"/>
+      <c r="N80" s="296"/>
+      <c r="P80" s="295" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="284"/>
-      <c r="R80" s="284"/>
-      <c r="S80" s="293"/>
+      <c r="Q80" s="287"/>
+      <c r="R80" s="287"/>
+      <c r="S80" s="296"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="294"/>
-      <c r="K81" s="295"/>
-      <c r="L81" s="295"/>
-      <c r="M81" s="295"/>
-      <c r="N81" s="296"/>
-      <c r="P81" s="294"/>
-      <c r="Q81" s="295"/>
-      <c r="R81" s="295"/>
-      <c r="S81" s="296"/>
+      <c r="J81" s="297"/>
+      <c r="K81" s="298"/>
+      <c r="L81" s="298"/>
+      <c r="M81" s="298"/>
+      <c r="N81" s="299"/>
+      <c r="P81" s="297"/>
+      <c r="Q81" s="298"/>
+      <c r="R81" s="298"/>
+      <c r="S81" s="299"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="287" t="s">
+      <c r="J82" s="290" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="288"/>
-      <c r="L82" s="286"/>
-      <c r="M82" s="287" t="s">
+      <c r="K82" s="291"/>
+      <c r="L82" s="289"/>
+      <c r="M82" s="290" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="286"/>
-      <c r="P82" s="287"/>
-      <c r="Q82" s="286"/>
+      <c r="N82" s="289"/>
+      <c r="P82" s="290"/>
+      <c r="Q82" s="289"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -7666,38 +7704,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="298" t="s">
+      <c r="J83" s="301" t="s">
         <v>70</v>
       </c>
-      <c r="K83" s="288"/>
-      <c r="L83" s="286"/>
-      <c r="M83" s="299">
+      <c r="K83" s="291"/>
+      <c r="L83" s="289"/>
+      <c r="M83" s="302">
         <v>7350000</v>
       </c>
-      <c r="N83" s="286"/>
-      <c r="P83" s="285" t="s">
+      <c r="N83" s="289"/>
+      <c r="P83" s="288" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="286"/>
+      <c r="Q83" s="289"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="298" t="s">
+      <c r="J84" s="301" t="s">
         <v>72</v>
       </c>
-      <c r="K84" s="288"/>
-      <c r="L84" s="286"/>
-      <c r="M84" s="300">
+      <c r="K84" s="291"/>
+      <c r="L84" s="289"/>
+      <c r="M84" s="303">
         <v>1100000</v>
       </c>
-      <c r="N84" s="286"/>
-      <c r="P84" s="285" t="s">
+      <c r="N84" s="289"/>
+      <c r="P84" s="288" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="286"/>
+      <c r="Q84" s="289"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -7706,39 +7744,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="298" t="s">
+      <c r="J85" s="301" t="s">
         <v>75</v>
       </c>
-      <c r="K85" s="288"/>
-      <c r="L85" s="286"/>
-      <c r="M85" s="299">
+      <c r="K85" s="291"/>
+      <c r="L85" s="289"/>
+      <c r="M85" s="302">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="286"/>
-      <c r="P85" s="285" t="s">
+      <c r="N85" s="289"/>
+      <c r="P85" s="288" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="286"/>
+      <c r="Q85" s="289"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="298" t="s">
+      <c r="J86" s="301" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="288"/>
-      <c r="L86" s="286"/>
-      <c r="M86" s="299">
+      <c r="K86" s="291"/>
+      <c r="L86" s="289"/>
+      <c r="M86" s="302">
         <v>8411850</v>
       </c>
-      <c r="N86" s="286"/>
-      <c r="P86" s="285" t="s">
+      <c r="N86" s="289"/>
+      <c r="P86" s="288" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="286"/>
+      <c r="Q86" s="289"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -7746,20 +7784,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="298" t="s">
+      <c r="J87" s="301" t="s">
         <v>79</v>
       </c>
-      <c r="K87" s="288"/>
-      <c r="L87" s="286"/>
-      <c r="M87" s="299">
+      <c r="K87" s="291"/>
+      <c r="L87" s="289"/>
+      <c r="M87" s="302">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="286"/>
-      <c r="P87" s="285" t="s">
+      <c r="N87" s="289"/>
+      <c r="P87" s="288" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="286"/>
+      <c r="Q87" s="289"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -8017,28 +8055,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="430" t="s">
+      <c r="B2" s="433" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="431"/>
-      <c r="D2" s="431"/>
-      <c r="E2" s="431"/>
-      <c r="F2" s="431"/>
-      <c r="G2" s="431"/>
-      <c r="H2" s="431"/>
-      <c r="I2" s="431"/>
-      <c r="J2" s="431"/>
+      <c r="C2" s="434"/>
+      <c r="D2" s="434"/>
+      <c r="E2" s="434"/>
+      <c r="F2" s="434"/>
+      <c r="G2" s="434"/>
+      <c r="H2" s="434"/>
+      <c r="I2" s="434"/>
+      <c r="J2" s="434"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="431"/>
-      <c r="C3" s="431"/>
-      <c r="D3" s="431"/>
-      <c r="E3" s="431"/>
-      <c r="F3" s="431"/>
-      <c r="G3" s="431"/>
-      <c r="H3" s="431"/>
-      <c r="I3" s="431"/>
-      <c r="J3" s="431"/>
+      <c r="B3" s="434"/>
+      <c r="C3" s="434"/>
+      <c r="D3" s="434"/>
+      <c r="E3" s="434"/>
+      <c r="F3" s="434"/>
+      <c r="G3" s="434"/>
+      <c r="H3" s="434"/>
+      <c r="I3" s="434"/>
+      <c r="J3" s="434"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -8059,10 +8097,10 @@
       <c r="G6" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="H6" s="356" t="s">
+      <c r="H6" s="359" t="s">
         <v>280</v>
       </c>
-      <c r="I6" s="311"/>
+      <c r="I6" s="314"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -8084,11 +8122,11 @@
       <c r="G7" s="195">
         <v>205000</v>
       </c>
-      <c r="H7" s="432">
+      <c r="H7" s="435">
         <f>F7-G7</f>
         <v>380000</v>
       </c>
-      <c r="I7" s="311"/>
+      <c r="I7" s="314"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="196"/>
@@ -8097,8 +8135,8 @@
       <c r="E8" s="197"/>
       <c r="F8" s="197"/>
       <c r="G8" s="197"/>
-      <c r="H8" s="429"/>
-      <c r="I8" s="429"/>
+      <c r="H8" s="432"/>
+      <c r="I8" s="432"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="196"/>
@@ -8109,11 +8147,11 @@
       <c r="G9" s="198" t="s">
         <v>281</v>
       </c>
-      <c r="H9" s="433">
+      <c r="H9" s="436">
         <f>H7</f>
         <v>380000</v>
       </c>
-      <c r="I9" s="336"/>
+      <c r="I9" s="339"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="196"/>
@@ -8122,8 +8160,8 @@
       <c r="E10" s="197"/>
       <c r="F10" s="197"/>
       <c r="G10" s="197"/>
-      <c r="H10" s="429"/>
-      <c r="I10" s="429"/>
+      <c r="H10" s="432"/>
+      <c r="I10" s="432"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="196"/>
@@ -8132,8 +8170,8 @@
       <c r="E11" s="197"/>
       <c r="F11" s="197"/>
       <c r="G11" s="197"/>
-      <c r="H11" s="429"/>
-      <c r="I11" s="429"/>
+      <c r="H11" s="432"/>
+      <c r="I11" s="432"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="196"/>
@@ -8142,8 +8180,8 @@
       <c r="E12" s="197"/>
       <c r="F12" s="197"/>
       <c r="G12" s="197"/>
-      <c r="H12" s="429"/>
-      <c r="I12" s="429"/>
+      <c r="H12" s="432"/>
+      <c r="I12" s="432"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="196"/>
@@ -8152,8 +8190,8 @@
       <c r="E13" s="197"/>
       <c r="F13" s="197"/>
       <c r="G13" s="197"/>
-      <c r="H13" s="429"/>
-      <c r="I13" s="429"/>
+      <c r="H13" s="432"/>
+      <c r="I13" s="432"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="196"/>
@@ -8162,8 +8200,8 @@
       <c r="E14" s="197"/>
       <c r="F14" s="197"/>
       <c r="G14" s="197"/>
-      <c r="H14" s="429"/>
-      <c r="I14" s="429"/>
+      <c r="H14" s="432"/>
+      <c r="I14" s="432"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="196"/>
@@ -8172,8 +8210,8 @@
       <c r="E15" s="197"/>
       <c r="F15" s="197"/>
       <c r="G15" s="197"/>
-      <c r="H15" s="429"/>
-      <c r="I15" s="429"/>
+      <c r="H15" s="432"/>
+      <c r="I15" s="432"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="196"/>
@@ -8182,8 +8220,8 @@
       <c r="E16" s="197"/>
       <c r="F16" s="197"/>
       <c r="G16" s="197"/>
-      <c r="H16" s="429"/>
-      <c r="I16" s="429"/>
+      <c r="H16" s="432"/>
+      <c r="I16" s="432"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="196"/>
@@ -8192,8 +8230,8 @@
       <c r="E17" s="197"/>
       <c r="F17" s="197"/>
       <c r="G17" s="197"/>
-      <c r="H17" s="429"/>
-      <c r="I17" s="429"/>
+      <c r="H17" s="432"/>
+      <c r="I17" s="432"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -8263,46 +8301,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="321" t="s">
+      <c r="C2" s="324" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="282"/>
-      <c r="E2" s="282"/>
-      <c r="F2" s="282"/>
-      <c r="G2" s="282"/>
-      <c r="H2" s="282"/>
-      <c r="I2" s="282"/>
-      <c r="J2" s="282"/>
-      <c r="K2" s="282"/>
-      <c r="L2" s="282"/>
-      <c r="M2" s="282"/>
-      <c r="N2" s="282"/>
-      <c r="O2" s="282"/>
-      <c r="P2" s="283"/>
-      <c r="Q2" s="283"/>
-      <c r="R2" s="283"/>
-      <c r="S2" s="282"/>
-      <c r="T2" s="282"/>
+      <c r="D2" s="285"/>
+      <c r="E2" s="285"/>
+      <c r="F2" s="285"/>
+      <c r="G2" s="285"/>
+      <c r="H2" s="285"/>
+      <c r="I2" s="285"/>
+      <c r="J2" s="285"/>
+      <c r="K2" s="285"/>
+      <c r="L2" s="285"/>
+      <c r="M2" s="285"/>
+      <c r="N2" s="285"/>
+      <c r="O2" s="285"/>
+      <c r="P2" s="286"/>
+      <c r="Q2" s="286"/>
+      <c r="R2" s="286"/>
+      <c r="S2" s="285"/>
+      <c r="T2" s="285"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="283"/>
-      <c r="D3" s="284"/>
-      <c r="E3" s="284"/>
-      <c r="F3" s="284"/>
-      <c r="G3" s="284"/>
-      <c r="H3" s="284"/>
-      <c r="I3" s="284"/>
-      <c r="J3" s="284"/>
-      <c r="K3" s="284"/>
-      <c r="L3" s="284"/>
-      <c r="M3" s="284"/>
-      <c r="N3" s="284"/>
-      <c r="O3" s="284"/>
-      <c r="P3" s="284"/>
-      <c r="Q3" s="284"/>
-      <c r="R3" s="284"/>
-      <c r="S3" s="284"/>
-      <c r="T3" s="284"/>
+      <c r="C3" s="286"/>
+      <c r="D3" s="287"/>
+      <c r="E3" s="287"/>
+      <c r="F3" s="287"/>
+      <c r="G3" s="287"/>
+      <c r="H3" s="287"/>
+      <c r="I3" s="287"/>
+      <c r="J3" s="287"/>
+      <c r="K3" s="287"/>
+      <c r="L3" s="287"/>
+      <c r="M3" s="287"/>
+      <c r="N3" s="287"/>
+      <c r="O3" s="287"/>
+      <c r="P3" s="287"/>
+      <c r="Q3" s="287"/>
+      <c r="R3" s="287"/>
+      <c r="S3" s="287"/>
+      <c r="T3" s="287"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8389,25 +8427,25 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="313" t="s">
+      <c r="X5" s="316" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="288"/>
-      <c r="Z5" s="288"/>
-      <c r="AA5" s="288"/>
-      <c r="AB5" s="288"/>
-      <c r="AC5" s="288"/>
-      <c r="AD5" s="288"/>
-      <c r="AE5" s="288"/>
-      <c r="AF5" s="288"/>
-      <c r="AG5" s="288"/>
-      <c r="AH5" s="288"/>
-      <c r="AI5" s="288"/>
-      <c r="AJ5" s="288"/>
-      <c r="AK5" s="288"/>
-      <c r="AL5" s="288"/>
-      <c r="AM5" s="288"/>
-      <c r="AN5" s="286"/>
+      <c r="Y5" s="291"/>
+      <c r="Z5" s="291"/>
+      <c r="AA5" s="291"/>
+      <c r="AB5" s="291"/>
+      <c r="AC5" s="291"/>
+      <c r="AD5" s="291"/>
+      <c r="AE5" s="291"/>
+      <c r="AF5" s="291"/>
+      <c r="AG5" s="291"/>
+      <c r="AH5" s="291"/>
+      <c r="AI5" s="291"/>
+      <c r="AJ5" s="291"/>
+      <c r="AK5" s="291"/>
+      <c r="AL5" s="291"/>
+      <c r="AM5" s="291"/>
+      <c r="AN5" s="289"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -8482,29 +8520,29 @@
       <c r="V6" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X6" s="322" t="s">
+      <c r="X6" s="325" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="322" t="s">
+      <c r="Y6" s="325" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="311" t="s">
+      <c r="Z6" s="314" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="312"/>
-      <c r="AB6" s="312"/>
-      <c r="AC6" s="312"/>
-      <c r="AD6" s="312"/>
-      <c r="AE6" s="312"/>
-      <c r="AF6" s="312"/>
-      <c r="AG6" s="312"/>
-      <c r="AH6" s="312"/>
-      <c r="AI6" s="312"/>
-      <c r="AJ6" s="312"/>
-      <c r="AK6" s="312"/>
-      <c r="AL6" s="312"/>
-      <c r="AM6" s="312"/>
-      <c r="AN6" s="312"/>
+      <c r="AA6" s="315"/>
+      <c r="AB6" s="315"/>
+      <c r="AC6" s="315"/>
+      <c r="AD6" s="315"/>
+      <c r="AE6" s="315"/>
+      <c r="AF6" s="315"/>
+      <c r="AG6" s="315"/>
+      <c r="AH6" s="315"/>
+      <c r="AI6" s="315"/>
+      <c r="AJ6" s="315"/>
+      <c r="AK6" s="315"/>
+      <c r="AL6" s="315"/>
+      <c r="AM6" s="315"/>
+      <c r="AN6" s="315"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -8579,27 +8617,27 @@
       <c r="V7" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X7" s="312"/>
-      <c r="Y7" s="312"/>
-      <c r="Z7" s="311" t="s">
+      <c r="X7" s="315"/>
+      <c r="Y7" s="315"/>
+      <c r="Z7" s="314" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="312"/>
-      <c r="AB7" s="312"/>
-      <c r="AC7" s="312"/>
-      <c r="AD7" s="311" t="s">
+      <c r="AA7" s="315"/>
+      <c r="AB7" s="315"/>
+      <c r="AC7" s="315"/>
+      <c r="AD7" s="314" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="312"/>
-      <c r="AF7" s="312"/>
-      <c r="AG7" s="312"/>
-      <c r="AH7" s="312"/>
-      <c r="AI7" s="312"/>
-      <c r="AJ7" s="312"/>
-      <c r="AK7" s="312"/>
-      <c r="AL7" s="312"/>
-      <c r="AM7" s="312"/>
-      <c r="AN7" s="312"/>
+      <c r="AE7" s="315"/>
+      <c r="AF7" s="315"/>
+      <c r="AG7" s="315"/>
+      <c r="AH7" s="315"/>
+      <c r="AI7" s="315"/>
+      <c r="AJ7" s="315"/>
+      <c r="AK7" s="315"/>
+      <c r="AL7" s="315"/>
+      <c r="AM7" s="315"/>
+      <c r="AN7" s="315"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -8649,8 +8687,8 @@
         <v>NO</v>
       </c>
       <c r="V8" s="13"/>
-      <c r="X8" s="312"/>
-      <c r="Y8" s="312"/>
+      <c r="X8" s="315"/>
+      <c r="Y8" s="315"/>
       <c r="Z8" s="153" t="s">
         <v>19</v>
       </c>
@@ -13261,10 +13299,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="309" t="s">
+      <c r="AA49" s="312" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="310"/>
+      <c r="AB49" s="313"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -13342,12 +13380,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="305" t="s">
+      <c r="AI50" s="308" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="306"/>
-      <c r="AK50" s="306"/>
-      <c r="AL50" s="307"/>
+      <c r="AJ50" s="309"/>
+      <c r="AK50" s="309"/>
+      <c r="AL50" s="310"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -13418,12 +13456,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="302" t="s">
+      <c r="AI51" s="305" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="303"/>
-      <c r="AK51" s="303"/>
-      <c r="AL51" s="304"/>
+      <c r="AJ51" s="306"/>
+      <c r="AK51" s="306"/>
+      <c r="AL51" s="307"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -13689,14 +13727,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="308"/>
-      <c r="AD55" s="308"/>
-      <c r="AI55" s="305" t="s">
+      <c r="AC55" s="311"/>
+      <c r="AD55" s="311"/>
+      <c r="AI55" s="308" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="306"/>
-      <c r="AK55" s="306"/>
-      <c r="AL55" s="307"/>
+      <c r="AJ55" s="309"/>
+      <c r="AK55" s="309"/>
+      <c r="AL55" s="310"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -13757,12 +13795,12 @@
         <v>NO</v>
       </c>
       <c r="V56" s="2"/>
-      <c r="AI56" s="301" t="s">
+      <c r="AI56" s="304" t="s">
         <v>168</v>
       </c>
-      <c r="AJ56" s="301"/>
-      <c r="AK56" s="301"/>
-      <c r="AL56" s="301"/>
+      <c r="AJ56" s="304"/>
+      <c r="AK56" s="304"/>
+      <c r="AL56" s="304"/>
       <c r="AM56" s="52">
         <f>AM50-AM55</f>
         <v>450000</v>
@@ -14011,32 +14049,32 @@
     <row r="67" spans="3:19" s="258" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="314" t="s">
+      <c r="C69" s="317" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="315"/>
-      <c r="E69" s="315"/>
-      <c r="F69" s="315"/>
-      <c r="G69" s="316"/>
-      <c r="I69" s="320" t="s">
+      <c r="D69" s="318"/>
+      <c r="E69" s="318"/>
+      <c r="F69" s="318"/>
+      <c r="G69" s="319"/>
+      <c r="I69" s="323" t="s">
         <v>178</v>
       </c>
-      <c r="J69" s="320"/>
-      <c r="K69" s="320"/>
-      <c r="L69" s="320"/>
-      <c r="M69" s="320"/>
+      <c r="J69" s="323"/>
+      <c r="K69" s="323"/>
+      <c r="L69" s="323"/>
+      <c r="M69" s="323"/>
     </row>
     <row r="70" spans="3:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="317"/>
-      <c r="D70" s="318"/>
-      <c r="E70" s="318"/>
-      <c r="F70" s="318"/>
-      <c r="G70" s="319"/>
-      <c r="I70" s="320"/>
-      <c r="J70" s="320"/>
-      <c r="K70" s="320"/>
-      <c r="L70" s="320"/>
-      <c r="M70" s="320"/>
+      <c r="C70" s="320"/>
+      <c r="D70" s="321"/>
+      <c r="E70" s="321"/>
+      <c r="F70" s="321"/>
+      <c r="G70" s="322"/>
+      <c r="I70" s="323"/>
+      <c r="J70" s="323"/>
+      <c r="K70" s="323"/>
+      <c r="L70" s="323"/>
+      <c r="M70" s="323"/>
     </row>
     <row r="71" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14057,10 +14095,10 @@
       <c r="M76" s="55"/>
       <c r="N76" s="55"/>
       <c r="O76" s="55"/>
-      <c r="P76" s="301" t="s">
+      <c r="P76" s="304" t="s">
         <v>214</v>
       </c>
-      <c r="Q76" s="301"/>
+      <c r="Q76" s="304"/>
       <c r="R76" s="55"/>
       <c r="S76" s="55"/>
     </row>
@@ -14606,8 +14644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W36"/>
   <sheetViews>
-    <sheetView topLeftCell="H16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView topLeftCell="H10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14627,86 +14665,86 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="323" t="s">
+      <c r="A2" s="326" t="s">
         <v>300</v>
       </c>
-      <c r="B2" s="323"/>
-      <c r="C2" s="323"/>
-      <c r="D2" s="323"/>
-      <c r="E2" s="323"/>
-      <c r="F2" s="323"/>
-      <c r="G2" s="323"/>
-      <c r="H2" s="323"/>
-      <c r="I2" s="323"/>
-      <c r="J2" s="323"/>
-      <c r="K2" s="323"/>
-      <c r="L2" s="323"/>
+      <c r="B2" s="326"/>
+      <c r="C2" s="326"/>
+      <c r="D2" s="326"/>
+      <c r="E2" s="326"/>
+      <c r="F2" s="326"/>
+      <c r="G2" s="326"/>
+      <c r="H2" s="326"/>
+      <c r="I2" s="326"/>
+      <c r="J2" s="326"/>
+      <c r="K2" s="326"/>
+      <c r="L2" s="326"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="323"/>
-      <c r="B3" s="323"/>
-      <c r="C3" s="323"/>
-      <c r="D3" s="323"/>
-      <c r="E3" s="323"/>
-      <c r="F3" s="323"/>
-      <c r="G3" s="323"/>
-      <c r="H3" s="323"/>
-      <c r="I3" s="323"/>
-      <c r="J3" s="323"/>
-      <c r="K3" s="323"/>
-      <c r="L3" s="323"/>
+      <c r="A3" s="326"/>
+      <c r="B3" s="326"/>
+      <c r="C3" s="326"/>
+      <c r="D3" s="326"/>
+      <c r="E3" s="326"/>
+      <c r="F3" s="326"/>
+      <c r="G3" s="326"/>
+      <c r="H3" s="326"/>
+      <c r="I3" s="326"/>
+      <c r="J3" s="326"/>
+      <c r="K3" s="326"/>
+      <c r="L3" s="326"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="320" t="s">
+      <c r="A5" s="323" t="s">
         <v>303</v>
       </c>
-      <c r="B5" s="320"/>
-      <c r="C5" s="320"/>
-      <c r="D5" s="320"/>
-      <c r="E5" s="320"/>
-      <c r="F5" s="320"/>
-      <c r="G5" s="320"/>
-      <c r="H5" s="320"/>
-      <c r="I5" s="320"/>
-      <c r="J5" s="320"/>
-      <c r="K5" s="320"/>
-      <c r="M5" s="320" t="s">
+      <c r="B5" s="323"/>
+      <c r="C5" s="323"/>
+      <c r="D5" s="323"/>
+      <c r="E5" s="323"/>
+      <c r="F5" s="323"/>
+      <c r="G5" s="323"/>
+      <c r="H5" s="323"/>
+      <c r="I5" s="323"/>
+      <c r="J5" s="323"/>
+      <c r="K5" s="323"/>
+      <c r="M5" s="323" t="s">
         <v>324</v>
       </c>
-      <c r="N5" s="320"/>
-      <c r="O5" s="320"/>
-      <c r="P5" s="320"/>
-      <c r="Q5" s="320"/>
-      <c r="R5" s="320"/>
-      <c r="S5" s="320"/>
-      <c r="T5" s="320"/>
-      <c r="U5" s="320"/>
-      <c r="V5" s="320"/>
-      <c r="W5" s="320"/>
+      <c r="N5" s="323"/>
+      <c r="O5" s="323"/>
+      <c r="P5" s="323"/>
+      <c r="Q5" s="323"/>
+      <c r="R5" s="323"/>
+      <c r="S5" s="323"/>
+      <c r="T5" s="323"/>
+      <c r="U5" s="323"/>
+      <c r="V5" s="323"/>
+      <c r="W5" s="323"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="320"/>
-      <c r="B6" s="320"/>
-      <c r="C6" s="320"/>
-      <c r="D6" s="320"/>
-      <c r="E6" s="320"/>
-      <c r="F6" s="320"/>
-      <c r="G6" s="320"/>
-      <c r="H6" s="320"/>
-      <c r="I6" s="320"/>
-      <c r="J6" s="320"/>
-      <c r="K6" s="320"/>
-      <c r="M6" s="320"/>
-      <c r="N6" s="320"/>
-      <c r="O6" s="320"/>
-      <c r="P6" s="320"/>
-      <c r="Q6" s="320"/>
-      <c r="R6" s="320"/>
-      <c r="S6" s="320"/>
-      <c r="T6" s="320"/>
-      <c r="U6" s="320"/>
-      <c r="V6" s="320"/>
-      <c r="W6" s="320"/>
+      <c r="A6" s="323"/>
+      <c r="B6" s="323"/>
+      <c r="C6" s="323"/>
+      <c r="D6" s="323"/>
+      <c r="E6" s="323"/>
+      <c r="F6" s="323"/>
+      <c r="G6" s="323"/>
+      <c r="H6" s="323"/>
+      <c r="I6" s="323"/>
+      <c r="J6" s="323"/>
+      <c r="K6" s="323"/>
+      <c r="M6" s="323"/>
+      <c r="N6" s="323"/>
+      <c r="O6" s="323"/>
+      <c r="P6" s="323"/>
+      <c r="Q6" s="323"/>
+      <c r="R6" s="323"/>
+      <c r="S6" s="323"/>
+      <c r="T6" s="323"/>
+      <c r="U6" s="323"/>
+      <c r="V6" s="323"/>
+      <c r="W6" s="323"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M7" s="251"/>
@@ -15419,15 +15457,15 @@
       <c r="N27" s="1">
         <v>19</v>
       </c>
-      <c r="O27" s="218" t="s">
-        <v>348</v>
+      <c r="O27" s="283" t="s">
+        <v>123</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="Q27" s="212"/>
       <c r="R27" s="212">
-        <v>500000</v>
+        <v>2000000</v>
       </c>
       <c r="S27" s="251"/>
       <c r="T27" s="251"/>
@@ -15447,16 +15485,9 @@
       <c r="N28" s="1">
         <v>20</v>
       </c>
-      <c r="O28" s="278" t="s">
-        <v>123</v>
-      </c>
-      <c r="P28" s="276" t="s">
-        <v>359</v>
-      </c>
-      <c r="Q28" s="212">
-        <f>'Pembayaran Makrab 19'!F40</f>
-        <v>650000</v>
-      </c>
+      <c r="O28" s="278"/>
+      <c r="P28" s="276"/>
+      <c r="Q28" s="212"/>
       <c r="R28" s="212"/>
       <c r="S28" s="251"/>
       <c r="T28" s="251"/>
@@ -15610,11 +15641,11 @@
       </c>
       <c r="Q34" s="225">
         <f>SUM(Q9:Q33)</f>
-        <v>4231144.2699999996</v>
+        <v>3581144.27</v>
       </c>
       <c r="R34" s="226">
         <f>SUM(R9:R33)</f>
-        <v>575000</v>
+        <v>2075000</v>
       </c>
       <c r="S34" s="251"/>
       <c r="T34" s="251"/>
@@ -15623,27 +15654,27 @@
       <c r="W34" s="251"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B35" s="328" t="s">
+      <c r="B35" s="331" t="s">
         <v>312</v>
       </c>
-      <c r="C35" s="329"/>
-      <c r="D35" s="330"/>
-      <c r="E35" s="324">
+      <c r="C35" s="332"/>
+      <c r="D35" s="333"/>
+      <c r="E35" s="327">
         <f>E34-F34</f>
         <v>2610871.1799999997</v>
       </c>
-      <c r="F35" s="325"/>
+      <c r="F35" s="328"/>
       <c r="M35" s="251"/>
-      <c r="N35" s="328" t="s">
+      <c r="N35" s="331" t="s">
         <v>312</v>
       </c>
-      <c r="O35" s="329"/>
-      <c r="P35" s="330"/>
-      <c r="Q35" s="324">
+      <c r="O35" s="332"/>
+      <c r="P35" s="333"/>
+      <c r="Q35" s="327">
         <f>Q34-R34</f>
-        <v>3656144.2699999996</v>
-      </c>
-      <c r="R35" s="325"/>
+        <v>1506144.27</v>
+      </c>
+      <c r="R35" s="328"/>
       <c r="S35" s="251"/>
       <c r="T35" s="251"/>
       <c r="U35" s="251"/>
@@ -15651,17 +15682,17 @@
       <c r="W35" s="251"/>
     </row>
     <row r="36" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="331"/>
-      <c r="C36" s="332"/>
-      <c r="D36" s="333"/>
-      <c r="E36" s="326"/>
-      <c r="F36" s="327"/>
+      <c r="B36" s="334"/>
+      <c r="C36" s="335"/>
+      <c r="D36" s="336"/>
+      <c r="E36" s="329"/>
+      <c r="F36" s="330"/>
       <c r="M36" s="251"/>
-      <c r="N36" s="331"/>
-      <c r="O36" s="332"/>
-      <c r="P36" s="333"/>
-      <c r="Q36" s="326"/>
-      <c r="R36" s="327"/>
+      <c r="N36" s="334"/>
+      <c r="O36" s="335"/>
+      <c r="P36" s="336"/>
+      <c r="Q36" s="329"/>
+      <c r="R36" s="330"/>
       <c r="S36" s="251"/>
       <c r="T36" s="251"/>
       <c r="U36" s="251"/>
@@ -15685,19 +15716,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F40"/>
+  <dimension ref="B3:O75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="3.85546875" customWidth="1"/>
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="22.140625" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -15823,10 +15855,18 @@
       <c r="B10" s="57">
         <v>7</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="56"/>
+      <c r="C10" s="57" t="s">
+        <v>365</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="F10" s="56">
+        <v>125000</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="57">
@@ -16026,7 +16066,7 @@
       <c r="E32" s="57"/>
       <c r="F32" s="56"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="57">
         <v>30</v>
       </c>
@@ -16035,7 +16075,7 @@
       <c r="E33" s="57"/>
       <c r="F33" s="56"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="57">
         <v>31</v>
       </c>
@@ -16044,7 +16084,7 @@
       <c r="E34" s="57"/>
       <c r="F34" s="56"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="57">
         <v>32</v>
       </c>
@@ -16053,7 +16093,7 @@
       <c r="E35" s="57"/>
       <c r="F35" s="56"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="57">
         <v>33</v>
       </c>
@@ -16062,7 +16102,7 @@
       <c r="E36" s="57"/>
       <c r="F36" s="56"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="57">
         <v>34</v>
       </c>
@@ -16071,7 +16111,7 @@
       <c r="E37" s="57"/>
       <c r="F37" s="56"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" s="57">
         <v>35</v>
       </c>
@@ -16080,7 +16120,7 @@
       <c r="E38" s="57"/>
       <c r="F38" s="56"/>
     </row>
-    <row r="39" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="143">
         <v>36</v>
       </c>
@@ -16089,21 +16129,562 @@
       <c r="E39" s="143"/>
       <c r="F39" s="56"/>
     </row>
-    <row r="40" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="334" t="s">
+    <row r="40" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="337" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="335"/>
-      <c r="D40" s="335"/>
-      <c r="E40" s="336"/>
+      <c r="C40" s="338"/>
+      <c r="D40" s="338"/>
+      <c r="E40" s="339"/>
       <c r="F40" s="279">
         <f>SUM(F4:F39)</f>
-        <v>650000</v>
-      </c>
+        <v>775000</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B44" s="323" t="s">
+        <v>368</v>
+      </c>
+      <c r="C44" s="323"/>
+      <c r="D44" s="323"/>
+      <c r="E44" s="323"/>
+      <c r="F44" s="323"/>
+      <c r="G44" s="323"/>
+      <c r="H44" s="323"/>
+      <c r="I44" s="323"/>
+      <c r="J44" s="323"/>
+      <c r="K44" s="323"/>
+      <c r="L44" s="323"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="323"/>
+      <c r="C45" s="323"/>
+      <c r="D45" s="323"/>
+      <c r="E45" s="323"/>
+      <c r="F45" s="323"/>
+      <c r="G45" s="323"/>
+      <c r="H45" s="323"/>
+      <c r="I45" s="323"/>
+      <c r="J45" s="323"/>
+      <c r="K45" s="323"/>
+      <c r="L45" s="323"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B46" s="281"/>
+      <c r="C46" s="205"/>
+      <c r="D46" s="216"/>
+      <c r="E46" s="205"/>
+      <c r="F46" s="281"/>
+      <c r="G46" s="217"/>
+      <c r="H46" s="281"/>
+      <c r="I46" s="281"/>
+      <c r="J46" s="281"/>
+      <c r="K46" s="281"/>
+      <c r="L46" s="281"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="281"/>
+      <c r="C47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="218" t="s">
+        <v>301</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="219" t="s">
+        <v>98</v>
+      </c>
+      <c r="G47" s="220" t="s">
+        <v>65</v>
+      </c>
+      <c r="H47" s="281"/>
+      <c r="I47" s="437" t="s">
+        <v>370</v>
+      </c>
+      <c r="J47" s="438"/>
+      <c r="K47" s="438"/>
+      <c r="L47" s="438"/>
+      <c r="M47" s="438"/>
+      <c r="N47" s="438"/>
+      <c r="O47" s="438"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="281"/>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="283" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="F48" s="212">
+        <v>2000000</v>
+      </c>
+      <c r="G48" s="213"/>
+      <c r="H48" s="281"/>
+      <c r="I48" s="438"/>
+      <c r="J48" s="438"/>
+      <c r="K48" s="438"/>
+      <c r="L48" s="438"/>
+      <c r="M48" s="438"/>
+      <c r="N48" s="438"/>
+      <c r="O48" s="438"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" s="281"/>
+      <c r="C49" s="1">
+        <v>2</v>
+      </c>
+      <c r="D49" s="218" t="s">
+        <v>348</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="F49" s="212"/>
+      <c r="G49" s="212">
+        <v>500000</v>
+      </c>
+      <c r="H49" s="281"/>
+      <c r="I49" s="438"/>
+      <c r="J49" s="438"/>
+      <c r="K49" s="438"/>
+      <c r="L49" s="438"/>
+      <c r="M49" s="438"/>
+      <c r="N49" s="438"/>
+      <c r="O49" s="438"/>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B50" s="281"/>
+      <c r="C50" s="1">
+        <v>3</v>
+      </c>
+      <c r="D50" s="278" t="s">
+        <v>123</v>
+      </c>
+      <c r="E50" s="282" t="s">
+        <v>359</v>
+      </c>
+      <c r="F50" s="212">
+        <f>F40</f>
+        <v>775000</v>
+      </c>
+      <c r="G50" s="212"/>
+      <c r="H50" s="281"/>
+      <c r="I50" s="438"/>
+      <c r="J50" s="438"/>
+      <c r="K50" s="438"/>
+      <c r="L50" s="438"/>
+      <c r="M50" s="438"/>
+      <c r="N50" s="438"/>
+      <c r="O50" s="438"/>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B51" s="281"/>
+      <c r="C51" s="1">
+        <v>4</v>
+      </c>
+      <c r="D51" s="211"/>
+      <c r="E51" s="66"/>
+      <c r="F51" s="212"/>
+      <c r="G51" s="213"/>
+      <c r="H51" s="281"/>
+      <c r="I51" s="438"/>
+      <c r="J51" s="438"/>
+      <c r="K51" s="438"/>
+      <c r="L51" s="438"/>
+      <c r="M51" s="438"/>
+      <c r="N51" s="438"/>
+      <c r="O51" s="438"/>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" s="281"/>
+      <c r="C52" s="1">
+        <v>5</v>
+      </c>
+      <c r="D52" s="211"/>
+      <c r="E52" s="66"/>
+      <c r="F52" s="254"/>
+      <c r="G52" s="213"/>
+      <c r="H52" s="281"/>
+      <c r="I52" s="438"/>
+      <c r="J52" s="438"/>
+      <c r="K52" s="438"/>
+      <c r="L52" s="438"/>
+      <c r="M52" s="438"/>
+      <c r="N52" s="438"/>
+      <c r="O52" s="438"/>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B53" s="281"/>
+      <c r="C53" s="1">
+        <v>6</v>
+      </c>
+      <c r="D53" s="211"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="212"/>
+      <c r="G53" s="213"/>
+      <c r="H53" s="281"/>
+      <c r="I53" s="438"/>
+      <c r="J53" s="438"/>
+      <c r="K53" s="438"/>
+      <c r="L53" s="438"/>
+      <c r="M53" s="438"/>
+      <c r="N53" s="438"/>
+      <c r="O53" s="438"/>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" s="281"/>
+      <c r="C54" s="1">
+        <v>7</v>
+      </c>
+      <c r="D54" s="218"/>
+      <c r="E54" s="282"/>
+      <c r="F54" s="212"/>
+      <c r="G54" s="213"/>
+      <c r="H54" s="281"/>
+      <c r="I54" s="281"/>
+      <c r="J54" s="281"/>
+      <c r="K54" s="281"/>
+      <c r="L54" s="281"/>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B55" s="281"/>
+      <c r="C55" s="1">
+        <v>8</v>
+      </c>
+      <c r="D55" s="218"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="213"/>
+      <c r="G55" s="212"/>
+      <c r="H55" s="281"/>
+      <c r="I55" s="281"/>
+      <c r="J55" s="281"/>
+      <c r="K55" s="281"/>
+      <c r="L55" s="281"/>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56" s="281"/>
+      <c r="C56" s="1">
+        <v>9</v>
+      </c>
+      <c r="D56" s="218"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="212"/>
+      <c r="G56" s="213"/>
+      <c r="H56" s="281"/>
+      <c r="I56" s="281"/>
+      <c r="J56" s="281"/>
+      <c r="K56" s="281"/>
+      <c r="L56" s="281"/>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B57" s="281"/>
+      <c r="C57" s="1">
+        <v>10</v>
+      </c>
+      <c r="D57" s="218"/>
+      <c r="E57" s="282"/>
+      <c r="F57" s="213"/>
+      <c r="G57" s="212"/>
+      <c r="H57" s="281"/>
+      <c r="I57" s="281"/>
+      <c r="J57" s="281"/>
+      <c r="K57" s="281"/>
+      <c r="L57" s="281"/>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B58" s="281"/>
+      <c r="C58" s="1">
+        <v>11</v>
+      </c>
+      <c r="D58" s="218"/>
+      <c r="E58" s="282"/>
+      <c r="F58" s="213"/>
+      <c r="G58" s="213"/>
+      <c r="H58" s="281"/>
+      <c r="I58" s="281"/>
+      <c r="J58" s="281"/>
+      <c r="K58" s="281"/>
+      <c r="L58" s="281"/>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B59" s="281"/>
+      <c r="C59" s="1">
+        <v>12</v>
+      </c>
+      <c r="D59" s="218"/>
+      <c r="E59" s="282"/>
+      <c r="F59" s="212"/>
+      <c r="G59" s="213"/>
+      <c r="H59" s="281"/>
+      <c r="I59" s="281"/>
+      <c r="J59" s="281"/>
+      <c r="K59" s="281"/>
+      <c r="L59" s="281"/>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B60" s="281"/>
+      <c r="C60" s="1">
+        <v>13</v>
+      </c>
+      <c r="D60" s="218"/>
+      <c r="E60" s="282"/>
+      <c r="F60" s="213"/>
+      <c r="G60" s="212"/>
+      <c r="H60" s="281"/>
+      <c r="I60" s="281"/>
+      <c r="J60" s="281"/>
+      <c r="K60" s="281"/>
+      <c r="L60" s="281"/>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B61" s="281"/>
+      <c r="C61" s="1">
+        <v>14</v>
+      </c>
+      <c r="D61" s="218"/>
+      <c r="E61" s="282"/>
+      <c r="F61" s="213"/>
+      <c r="G61" s="213"/>
+      <c r="H61" s="281"/>
+      <c r="I61" s="281"/>
+      <c r="J61" s="281"/>
+      <c r="K61" s="281"/>
+      <c r="L61" s="281"/>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B62" s="281"/>
+      <c r="C62" s="1">
+        <v>15</v>
+      </c>
+      <c r="D62" s="218"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="212"/>
+      <c r="G62" s="213"/>
+      <c r="H62" s="281"/>
+      <c r="I62" s="281"/>
+      <c r="J62" s="281"/>
+      <c r="K62" s="281"/>
+      <c r="L62" s="281"/>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B63" s="281"/>
+      <c r="C63" s="1">
+        <v>16</v>
+      </c>
+      <c r="D63" s="218"/>
+      <c r="E63" s="282"/>
+      <c r="F63" s="213"/>
+      <c r="G63" s="212"/>
+      <c r="H63" s="281"/>
+      <c r="I63" s="281"/>
+      <c r="J63" s="281"/>
+      <c r="K63" s="281"/>
+      <c r="L63" s="281"/>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B64" s="281"/>
+      <c r="C64" s="1">
+        <v>17</v>
+      </c>
+      <c r="D64" s="218"/>
+      <c r="E64" s="282"/>
+      <c r="F64" s="212"/>
+      <c r="G64" s="212"/>
+      <c r="H64" s="281"/>
+      <c r="I64" s="281"/>
+      <c r="J64" s="281"/>
+      <c r="K64" s="281"/>
+      <c r="L64" s="281"/>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B65" s="281"/>
+      <c r="C65" s="1">
+        <v>18</v>
+      </c>
+      <c r="D65" s="218"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="212"/>
+      <c r="G65" s="212"/>
+      <c r="H65" s="281"/>
+      <c r="I65" s="281"/>
+      <c r="J65" s="281"/>
+      <c r="K65" s="281"/>
+      <c r="L65" s="281"/>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B66" s="281"/>
+      <c r="C66" s="1">
+        <v>19</v>
+      </c>
+      <c r="D66" s="218"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="212"/>
+      <c r="G66" s="212"/>
+      <c r="H66" s="281"/>
+      <c r="I66" s="281"/>
+      <c r="J66" s="281"/>
+      <c r="K66" s="281"/>
+      <c r="L66" s="281"/>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B67" s="281"/>
+      <c r="C67" s="1">
+        <v>20</v>
+      </c>
+      <c r="D67" s="278"/>
+      <c r="E67" s="282"/>
+      <c r="F67" s="212"/>
+      <c r="G67" s="212"/>
+      <c r="H67" s="281"/>
+      <c r="I67" s="281"/>
+      <c r="J67" s="281"/>
+      <c r="K67" s="281"/>
+      <c r="L67" s="281"/>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B68" s="281"/>
+      <c r="C68" s="1">
+        <v>21</v>
+      </c>
+      <c r="D68" s="218"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="212"/>
+      <c r="G68" s="212"/>
+      <c r="H68" s="281"/>
+      <c r="I68" s="281"/>
+      <c r="J68" s="281"/>
+      <c r="K68" s="281"/>
+      <c r="L68" s="281"/>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B69" s="281"/>
+      <c r="C69" s="1">
+        <v>22</v>
+      </c>
+      <c r="D69" s="218"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="212"/>
+      <c r="G69" s="212"/>
+      <c r="H69" s="281"/>
+      <c r="I69" s="281"/>
+      <c r="J69" s="281"/>
+      <c r="K69" s="281"/>
+      <c r="L69" s="281"/>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B70" s="281"/>
+      <c r="C70" s="1">
+        <v>23</v>
+      </c>
+      <c r="D70" s="218"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="212"/>
+      <c r="G70" s="212"/>
+      <c r="H70" s="281"/>
+      <c r="I70" s="281"/>
+      <c r="J70" s="281"/>
+      <c r="K70" s="281"/>
+      <c r="L70" s="281"/>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B71" s="281"/>
+      <c r="C71" s="1">
+        <v>24</v>
+      </c>
+      <c r="D71" s="218"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="56"/>
+      <c r="G71" s="56"/>
+      <c r="H71" s="281"/>
+      <c r="I71" s="281"/>
+      <c r="J71" s="281"/>
+      <c r="K71" s="281"/>
+      <c r="L71" s="281"/>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B72" s="281"/>
+      <c r="C72" s="1">
+        <v>25</v>
+      </c>
+      <c r="D72" s="211" t="s">
+        <v>360</v>
+      </c>
+      <c r="E72" s="282" t="s">
+        <v>299</v>
+      </c>
+      <c r="F72" s="56"/>
+      <c r="G72" s="56"/>
+      <c r="H72" s="281"/>
+      <c r="I72" s="281"/>
+      <c r="J72" s="281"/>
+      <c r="K72" s="281"/>
+      <c r="L72" s="281"/>
+    </row>
+    <row r="73" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="281"/>
+      <c r="C73" s="196"/>
+      <c r="D73" s="280" t="s">
+        <v>360</v>
+      </c>
+      <c r="E73" s="224"/>
+      <c r="F73" s="225">
+        <f>SUM(F48:F72)</f>
+        <v>2775000</v>
+      </c>
+      <c r="G73" s="226">
+        <f>SUM(G48:G72)</f>
+        <v>500000</v>
+      </c>
+      <c r="H73" s="281"/>
+      <c r="I73" s="281"/>
+      <c r="J73" s="281"/>
+      <c r="K73" s="281"/>
+      <c r="L73" s="281"/>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B74" s="281"/>
+      <c r="C74" s="331" t="s">
+        <v>367</v>
+      </c>
+      <c r="D74" s="332"/>
+      <c r="E74" s="333"/>
+      <c r="F74" s="327">
+        <f>F73-G73</f>
+        <v>2275000</v>
+      </c>
+      <c r="G74" s="328"/>
+      <c r="H74" s="281"/>
+      <c r="I74" s="281"/>
+      <c r="J74" s="281"/>
+      <c r="K74" s="281"/>
+      <c r="L74" s="281"/>
+    </row>
+    <row r="75" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="281"/>
+      <c r="C75" s="334"/>
+      <c r="D75" s="335"/>
+      <c r="E75" s="336"/>
+      <c r="F75" s="329"/>
+      <c r="G75" s="330"/>
+      <c r="H75" s="281"/>
+      <c r="I75" s="281"/>
+      <c r="J75" s="281"/>
+      <c r="K75" s="281"/>
+      <c r="L75" s="281"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
+    <mergeCell ref="C74:E75"/>
+    <mergeCell ref="F74:G75"/>
     <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B44:L45"/>
+    <mergeCell ref="I47:O53"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:D39">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="MABA">
@@ -16153,17 +16734,17 @@
       <c r="A2" s="174"/>
       <c r="B2" s="175"/>
       <c r="C2" s="175"/>
-      <c r="D2" s="337" t="s">
+      <c r="D2" s="340" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="337"/>
-      <c r="F2" s="337"/>
-      <c r="G2" s="337"/>
-      <c r="H2" s="337"/>
-      <c r="I2" s="337"/>
-      <c r="J2" s="337"/>
-      <c r="K2" s="337"/>
-      <c r="L2" s="337"/>
+      <c r="E2" s="340"/>
+      <c r="F2" s="340"/>
+      <c r="G2" s="340"/>
+      <c r="H2" s="340"/>
+      <c r="I2" s="340"/>
+      <c r="J2" s="340"/>
+      <c r="K2" s="340"/>
+      <c r="L2" s="340"/>
       <c r="M2" s="176"/>
       <c r="N2" s="24"/>
     </row>
@@ -16181,205 +16762,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="178"/>
-      <c r="U3" s="387" t="s">
+      <c r="U3" s="390" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="388"/>
-      <c r="W3" s="389" t="s">
+      <c r="V3" s="391"/>
+      <c r="W3" s="392" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="388"/>
-      <c r="Y3" s="388"/>
-      <c r="Z3" s="388"/>
-      <c r="AA3" s="388"/>
-      <c r="AB3" s="388"/>
-      <c r="AC3" s="388"/>
-      <c r="AD3" s="390"/>
+      <c r="X3" s="391"/>
+      <c r="Y3" s="391"/>
+      <c r="Z3" s="391"/>
+      <c r="AA3" s="391"/>
+      <c r="AB3" s="391"/>
+      <c r="AC3" s="391"/>
+      <c r="AD3" s="393"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="177"/>
-      <c r="B4" s="352" t="s">
+      <c r="B4" s="355" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="353"/>
-      <c r="D4" s="353"/>
-      <c r="E4" s="353"/>
-      <c r="F4" s="353"/>
+      <c r="C4" s="356"/>
+      <c r="D4" s="356"/>
+      <c r="E4" s="356"/>
+      <c r="F4" s="356"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="356" t="s">
+      <c r="I4" s="359" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="311"/>
-      <c r="K4" s="311"/>
-      <c r="L4" s="311"/>
+      <c r="J4" s="314"/>
+      <c r="K4" s="314"/>
+      <c r="L4" s="314"/>
       <c r="M4" s="178"/>
-      <c r="U4" s="399" t="s">
+      <c r="U4" s="402" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="311"/>
-      <c r="W4" s="356" t="s">
+      <c r="V4" s="314"/>
+      <c r="W4" s="359" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="311"/>
-      <c r="Y4" s="311"/>
-      <c r="Z4" s="311"/>
-      <c r="AA4" s="311"/>
-      <c r="AB4" s="311"/>
-      <c r="AC4" s="311"/>
-      <c r="AD4" s="376"/>
+      <c r="X4" s="314"/>
+      <c r="Y4" s="314"/>
+      <c r="Z4" s="314"/>
+      <c r="AA4" s="314"/>
+      <c r="AB4" s="314"/>
+      <c r="AC4" s="314"/>
+      <c r="AD4" s="379"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="177"/>
-      <c r="B5" s="347" t="s">
+      <c r="B5" s="350" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="311"/>
-      <c r="D5" s="311"/>
-      <c r="E5" s="311"/>
-      <c r="F5" s="311"/>
+      <c r="C5" s="314"/>
+      <c r="D5" s="314"/>
+      <c r="E5" s="314"/>
+      <c r="F5" s="314"/>
       <c r="G5" s="154">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="345" t="s">
+      <c r="I5" s="348" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="346"/>
-      <c r="K5" s="357">
+      <c r="J5" s="349"/>
+      <c r="K5" s="360">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="358"/>
+      <c r="L5" s="361"/>
       <c r="M5" s="178"/>
-      <c r="U5" s="383" t="s">
+      <c r="U5" s="386" t="s">
         <v>231</v>
       </c>
-      <c r="V5" s="384"/>
-      <c r="W5" s="345" t="s">
+      <c r="V5" s="387"/>
+      <c r="W5" s="348" t="s">
         <v>232</v>
       </c>
-      <c r="X5" s="370"/>
-      <c r="Y5" s="370"/>
-      <c r="Z5" s="370"/>
-      <c r="AA5" s="370"/>
-      <c r="AB5" s="370"/>
-      <c r="AC5" s="370"/>
-      <c r="AD5" s="371"/>
+      <c r="X5" s="373"/>
+      <c r="Y5" s="373"/>
+      <c r="Z5" s="373"/>
+      <c r="AA5" s="373"/>
+      <c r="AB5" s="373"/>
+      <c r="AC5" s="373"/>
+      <c r="AD5" s="374"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="177"/>
-      <c r="B6" s="339" t="s">
+      <c r="B6" s="342" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="340"/>
-      <c r="D6" s="340"/>
-      <c r="E6" s="340"/>
-      <c r="F6" s="340"/>
+      <c r="C6" s="343"/>
+      <c r="D6" s="343"/>
+      <c r="E6" s="343"/>
+      <c r="F6" s="343"/>
       <c r="G6" s="154">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="343" t="s">
+      <c r="I6" s="346" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="344"/>
-      <c r="K6" s="359">
+      <c r="J6" s="347"/>
+      <c r="K6" s="362">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="360"/>
+      <c r="L6" s="363"/>
       <c r="M6" s="178"/>
-      <c r="U6" s="385"/>
-      <c r="V6" s="386"/>
-      <c r="W6" s="372" t="s">
+      <c r="U6" s="388"/>
+      <c r="V6" s="389"/>
+      <c r="W6" s="375" t="s">
         <v>233</v>
       </c>
-      <c r="X6" s="373"/>
-      <c r="Y6" s="373"/>
-      <c r="Z6" s="373"/>
-      <c r="AA6" s="373"/>
-      <c r="AB6" s="373"/>
-      <c r="AC6" s="373"/>
-      <c r="AD6" s="374"/>
+      <c r="X6" s="376"/>
+      <c r="Y6" s="376"/>
+      <c r="Z6" s="376"/>
+      <c r="AA6" s="376"/>
+      <c r="AB6" s="376"/>
+      <c r="AC6" s="376"/>
+      <c r="AD6" s="377"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="177"/>
-      <c r="B7" s="350" t="s">
+      <c r="B7" s="353" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="351"/>
-      <c r="D7" s="351"/>
-      <c r="E7" s="351"/>
-      <c r="F7" s="344"/>
+      <c r="C7" s="354"/>
+      <c r="D7" s="354"/>
+      <c r="E7" s="354"/>
+      <c r="F7" s="347"/>
       <c r="G7" s="154">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="343" t="s">
+      <c r="I7" s="346" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="344"/>
-      <c r="K7" s="354">
+      <c r="J7" s="347"/>
+      <c r="K7" s="357">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="355"/>
+      <c r="L7" s="358"/>
       <c r="M7" s="178"/>
-      <c r="U7" s="391"/>
-      <c r="V7" s="392"/>
-      <c r="W7" s="356" t="s">
+      <c r="U7" s="394"/>
+      <c r="V7" s="395"/>
+      <c r="W7" s="359" t="s">
         <v>234</v>
       </c>
-      <c r="X7" s="311"/>
-      <c r="Y7" s="311"/>
-      <c r="Z7" s="311"/>
-      <c r="AA7" s="311"/>
-      <c r="AB7" s="311"/>
-      <c r="AC7" s="311"/>
-      <c r="AD7" s="376"/>
+      <c r="X7" s="314"/>
+      <c r="Y7" s="314"/>
+      <c r="Z7" s="314"/>
+      <c r="AA7" s="314"/>
+      <c r="AB7" s="314"/>
+      <c r="AC7" s="314"/>
+      <c r="AD7" s="379"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="177"/>
-      <c r="B8" s="348" t="s">
+      <c r="B8" s="351" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="349"/>
-      <c r="D8" s="349"/>
-      <c r="E8" s="349"/>
-      <c r="F8" s="349"/>
+      <c r="C8" s="352"/>
+      <c r="D8" s="352"/>
+      <c r="E8" s="352"/>
+      <c r="F8" s="352"/>
       <c r="G8" s="155">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="345" t="s">
+      <c r="I8" s="348" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="346"/>
-      <c r="K8" s="341">
+      <c r="J8" s="349"/>
+      <c r="K8" s="344">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="342"/>
+      <c r="L8" s="345"/>
       <c r="M8" s="178"/>
-      <c r="U8" s="395" t="s">
+      <c r="U8" s="398" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="396"/>
-      <c r="W8" s="372" t="s">
+      <c r="V8" s="399"/>
+      <c r="W8" s="375" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="373"/>
-      <c r="Y8" s="373"/>
-      <c r="Z8" s="373"/>
-      <c r="AA8" s="373"/>
-      <c r="AB8" s="373"/>
-      <c r="AC8" s="373"/>
-      <c r="AD8" s="374"/>
+      <c r="X8" s="376"/>
+      <c r="Y8" s="376"/>
+      <c r="Z8" s="376"/>
+      <c r="AA8" s="376"/>
+      <c r="AB8" s="376"/>
+      <c r="AC8" s="376"/>
+      <c r="AD8" s="377"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="177"/>
@@ -16395,28 +16976,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="178"/>
-      <c r="U9" s="397"/>
-      <c r="V9" s="398"/>
-      <c r="W9" s="372" t="s">
+      <c r="U9" s="400"/>
+      <c r="V9" s="401"/>
+      <c r="W9" s="375" t="s">
         <v>237</v>
       </c>
-      <c r="X9" s="373"/>
-      <c r="Y9" s="373"/>
-      <c r="Z9" s="373"/>
-      <c r="AA9" s="373"/>
-      <c r="AB9" s="373"/>
-      <c r="AC9" s="373"/>
-      <c r="AD9" s="374"/>
+      <c r="X9" s="376"/>
+      <c r="Y9" s="376"/>
+      <c r="Z9" s="376"/>
+      <c r="AA9" s="376"/>
+      <c r="AB9" s="376"/>
+      <c r="AC9" s="376"/>
+      <c r="AD9" s="377"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="177"/>
-      <c r="B10" s="311" t="s">
+      <c r="B10" s="314" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="311"/>
-      <c r="D10" s="311"/>
-      <c r="E10" s="311"/>
-      <c r="F10" s="311"/>
+      <c r="C10" s="314"/>
+      <c r="D10" s="314"/>
+      <c r="E10" s="314"/>
+      <c r="F10" s="314"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -16427,30 +17008,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="178"/>
-      <c r="U10" s="339" t="s">
+      <c r="U10" s="342" t="s">
         <v>243</v>
       </c>
-      <c r="V10" s="340"/>
-      <c r="W10" s="311" t="s">
+      <c r="V10" s="343"/>
+      <c r="W10" s="314" t="s">
         <v>257</v>
       </c>
-      <c r="X10" s="311"/>
-      <c r="Y10" s="311"/>
-      <c r="Z10" s="311"/>
-      <c r="AA10" s="311"/>
-      <c r="AB10" s="311"/>
-      <c r="AC10" s="311"/>
-      <c r="AD10" s="376"/>
+      <c r="X10" s="314"/>
+      <c r="Y10" s="314"/>
+      <c r="Z10" s="314"/>
+      <c r="AA10" s="314"/>
+      <c r="AB10" s="314"/>
+      <c r="AC10" s="314"/>
+      <c r="AD10" s="379"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="177"/>
-      <c r="B11" s="311" t="s">
+      <c r="B11" s="314" t="s">
         <v>254</v>
       </c>
-      <c r="C11" s="311"/>
-      <c r="D11" s="311"/>
-      <c r="E11" s="311"/>
-      <c r="F11" s="311"/>
+      <c r="C11" s="314"/>
+      <c r="D11" s="314"/>
+      <c r="E11" s="314"/>
+      <c r="F11" s="314"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -16460,30 +17041,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="178"/>
-      <c r="U11" s="339" t="s">
+      <c r="U11" s="342" t="s">
         <v>256</v>
       </c>
-      <c r="V11" s="340"/>
-      <c r="W11" s="393" t="s">
+      <c r="V11" s="343"/>
+      <c r="W11" s="396" t="s">
         <v>258</v>
       </c>
-      <c r="X11" s="393"/>
-      <c r="Y11" s="393"/>
-      <c r="Z11" s="393"/>
-      <c r="AA11" s="393"/>
-      <c r="AB11" s="393"/>
-      <c r="AC11" s="393"/>
-      <c r="AD11" s="394"/>
+      <c r="X11" s="396"/>
+      <c r="Y11" s="396"/>
+      <c r="Z11" s="396"/>
+      <c r="AA11" s="396"/>
+      <c r="AB11" s="396"/>
+      <c r="AC11" s="396"/>
+      <c r="AD11" s="397"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="177"/>
-      <c r="B12" s="338" t="s">
+      <c r="B12" s="341" t="s">
         <v>255</v>
       </c>
-      <c r="C12" s="338"/>
-      <c r="D12" s="338"/>
-      <c r="E12" s="338"/>
-      <c r="F12" s="338"/>
+      <c r="C12" s="341"/>
+      <c r="D12" s="341"/>
+      <c r="E12" s="341"/>
+      <c r="F12" s="341"/>
       <c r="G12" s="182">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -16494,16 +17075,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="178"/>
-      <c r="U12" s="339"/>
-      <c r="V12" s="340"/>
-      <c r="W12" s="311"/>
-      <c r="X12" s="311"/>
-      <c r="Y12" s="311"/>
-      <c r="Z12" s="311"/>
-      <c r="AA12" s="311"/>
-      <c r="AB12" s="311"/>
-      <c r="AC12" s="311"/>
-      <c r="AD12" s="376"/>
+      <c r="U12" s="342"/>
+      <c r="V12" s="343"/>
+      <c r="W12" s="314"/>
+      <c r="X12" s="314"/>
+      <c r="Y12" s="314"/>
+      <c r="Z12" s="314"/>
+      <c r="AA12" s="314"/>
+      <c r="AB12" s="314"/>
+      <c r="AC12" s="314"/>
+      <c r="AD12" s="379"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="179"/>
@@ -16519,64 +17100,64 @@
       <c r="K13" s="180"/>
       <c r="L13" s="180"/>
       <c r="M13" s="181"/>
-      <c r="U13" s="339"/>
-      <c r="V13" s="340"/>
-      <c r="W13" s="311"/>
-      <c r="X13" s="311"/>
-      <c r="Y13" s="311"/>
-      <c r="Z13" s="311"/>
-      <c r="AA13" s="311"/>
-      <c r="AB13" s="311"/>
-      <c r="AC13" s="311"/>
-      <c r="AD13" s="376"/>
+      <c r="U13" s="342"/>
+      <c r="V13" s="343"/>
+      <c r="W13" s="314"/>
+      <c r="X13" s="314"/>
+      <c r="Y13" s="314"/>
+      <c r="Z13" s="314"/>
+      <c r="AA13" s="314"/>
+      <c r="AB13" s="314"/>
+      <c r="AC13" s="314"/>
+      <c r="AD13" s="379"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="377"/>
-      <c r="V14" s="378"/>
-      <c r="W14" s="368"/>
-      <c r="X14" s="368"/>
-      <c r="Y14" s="368"/>
-      <c r="Z14" s="368"/>
-      <c r="AA14" s="368"/>
-      <c r="AB14" s="368"/>
-      <c r="AC14" s="368"/>
-      <c r="AD14" s="369"/>
+      <c r="U14" s="380"/>
+      <c r="V14" s="381"/>
+      <c r="W14" s="371"/>
+      <c r="X14" s="371"/>
+      <c r="Y14" s="371"/>
+      <c r="Z14" s="371"/>
+      <c r="AA14" s="371"/>
+      <c r="AB14" s="371"/>
+      <c r="AC14" s="371"/>
+      <c r="AD14" s="372"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="174"/>
       <c r="B18" s="175"/>
       <c r="C18" s="175"/>
-      <c r="D18" s="337" t="s">
+      <c r="D18" s="340" t="s">
         <v>249</v>
       </c>
-      <c r="E18" s="337"/>
-      <c r="F18" s="337"/>
-      <c r="G18" s="337"/>
-      <c r="H18" s="337"/>
-      <c r="I18" s="337"/>
-      <c r="J18" s="337"/>
-      <c r="K18" s="337"/>
-      <c r="L18" s="337"/>
+      <c r="E18" s="340"/>
+      <c r="F18" s="340"/>
+      <c r="G18" s="340"/>
+      <c r="H18" s="340"/>
+      <c r="I18" s="340"/>
+      <c r="J18" s="340"/>
+      <c r="K18" s="340"/>
+      <c r="L18" s="340"/>
       <c r="M18" s="176"/>
-      <c r="O18" s="379" t="s">
+      <c r="O18" s="382" t="s">
         <v>250</v>
       </c>
-      <c r="P18" s="380"/>
-      <c r="Q18" s="380"/>
-      <c r="R18" s="380"/>
-      <c r="S18" s="381"/>
+      <c r="P18" s="383"/>
+      <c r="Q18" s="383"/>
+      <c r="R18" s="383"/>
+      <c r="S18" s="384"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="177"/>
       <c r="M19" s="178"/>
-      <c r="O19" s="347" t="s">
+      <c r="O19" s="350" t="s">
         <v>251</v>
       </c>
-      <c r="P19" s="311"/>
-      <c r="Q19" s="311"/>
-      <c r="R19" s="311"/>
-      <c r="S19" s="376"/>
+      <c r="P19" s="314"/>
+      <c r="Q19" s="314"/>
+      <c r="R19" s="314"/>
+      <c r="S19" s="379"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="177"/>
@@ -16587,119 +17168,119 @@
       <c r="F20" s="202"/>
       <c r="G20" s="68"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="356" t="s">
+      <c r="I20" s="359" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="311"/>
-      <c r="K20" s="311"/>
-      <c r="L20" s="311"/>
+      <c r="J20" s="314"/>
+      <c r="K20" s="314"/>
+      <c r="L20" s="314"/>
       <c r="M20" s="178"/>
-      <c r="O20" s="347" t="s">
+      <c r="O20" s="350" t="s">
         <v>252</v>
       </c>
-      <c r="P20" s="311"/>
-      <c r="Q20" s="311"/>
-      <c r="R20" s="311"/>
-      <c r="S20" s="376"/>
+      <c r="P20" s="314"/>
+      <c r="Q20" s="314"/>
+      <c r="R20" s="314"/>
+      <c r="S20" s="379"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="177"/>
-      <c r="B21" s="361" t="s">
+      <c r="B21" s="364" t="s">
         <v>296</v>
       </c>
-      <c r="C21" s="362"/>
-      <c r="D21" s="362"/>
-      <c r="E21" s="362"/>
-      <c r="F21" s="363"/>
+      <c r="C21" s="365"/>
+      <c r="D21" s="365"/>
+      <c r="E21" s="365"/>
+      <c r="F21" s="366"/>
       <c r="G21" s="70">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="345" t="s">
+      <c r="I21" s="348" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="346"/>
-      <c r="K21" s="357">
+      <c r="J21" s="349"/>
+      <c r="K21" s="360">
         <f>G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="L21" s="358"/>
+      <c r="L21" s="361"/>
       <c r="M21" s="178"/>
       <c r="N21" s="172"/>
-      <c r="O21" s="382" t="s">
+      <c r="O21" s="385" t="s">
         <v>259</v>
       </c>
-      <c r="P21" s="370"/>
-      <c r="Q21" s="370"/>
-      <c r="R21" s="370"/>
-      <c r="S21" s="371"/>
+      <c r="P21" s="373"/>
+      <c r="Q21" s="373"/>
+      <c r="R21" s="373"/>
+      <c r="S21" s="374"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="177"/>
-      <c r="B22" s="350" t="s">
+      <c r="B22" s="353" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="351"/>
-      <c r="D22" s="351"/>
-      <c r="E22" s="351"/>
-      <c r="F22" s="344"/>
+      <c r="C22" s="354"/>
+      <c r="D22" s="354"/>
+      <c r="E22" s="354"/>
+      <c r="F22" s="347"/>
       <c r="G22" s="154">
         <f>G21</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="343" t="s">
+      <c r="I22" s="346" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="344"/>
-      <c r="K22" s="359">
+      <c r="J22" s="347"/>
+      <c r="K22" s="362">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="L22" s="360"/>
+      <c r="L22" s="363"/>
       <c r="M22" s="178"/>
       <c r="N22" s="172"/>
-      <c r="O22" s="350" t="s">
+      <c r="O22" s="353" t="s">
         <v>260</v>
       </c>
-      <c r="P22" s="351"/>
-      <c r="Q22" s="351"/>
-      <c r="R22" s="351"/>
-      <c r="S22" s="375"/>
+      <c r="P22" s="354"/>
+      <c r="Q22" s="354"/>
+      <c r="R22" s="354"/>
+      <c r="S22" s="378"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="177"/>
-      <c r="B23" s="364" t="s">
+      <c r="B23" s="367" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="365"/>
-      <c r="D23" s="365"/>
-      <c r="E23" s="365"/>
-      <c r="F23" s="366"/>
+      <c r="C23" s="368"/>
+      <c r="D23" s="368"/>
+      <c r="E23" s="368"/>
+      <c r="F23" s="369"/>
       <c r="G23" s="155">
         <f>K24</f>
         <v>1568729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="343" t="s">
+      <c r="I23" s="346" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="344"/>
-      <c r="K23" s="354">
+      <c r="J23" s="347"/>
+      <c r="K23" s="357">
         <f>Pemasukkan!L31</f>
         <v>690000</v>
       </c>
-      <c r="L23" s="355"/>
+      <c r="L23" s="358"/>
       <c r="M23" s="178"/>
       <c r="N23" s="172"/>
-      <c r="O23" s="350" t="s">
+      <c r="O23" s="353" t="s">
         <v>261</v>
       </c>
-      <c r="P23" s="351"/>
-      <c r="Q23" s="351"/>
-      <c r="R23" s="351"/>
-      <c r="S23" s="375"/>
+      <c r="P23" s="354"/>
+      <c r="Q23" s="354"/>
+      <c r="R23" s="354"/>
+      <c r="S23" s="378"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="177"/>
@@ -16710,24 +17291,24 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="345" t="s">
+      <c r="I24" s="348" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="346"/>
-      <c r="K24" s="341">
+      <c r="J24" s="349"/>
+      <c r="K24" s="344">
         <f>(K21-K22)+K23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="L24" s="342"/>
+      <c r="L24" s="345"/>
       <c r="M24" s="178"/>
       <c r="N24" s="172"/>
-      <c r="O24" s="350" t="s">
+      <c r="O24" s="353" t="s">
         <v>262</v>
       </c>
-      <c r="P24" s="351"/>
-      <c r="Q24" s="351"/>
-      <c r="R24" s="351"/>
-      <c r="S24" s="375"/>
+      <c r="P24" s="354"/>
+      <c r="Q24" s="354"/>
+      <c r="R24" s="354"/>
+      <c r="S24" s="378"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="177"/>
@@ -16744,13 +17325,13 @@
       <c r="L25" s="24"/>
       <c r="M25" s="178"/>
       <c r="N25" s="172"/>
-      <c r="O25" s="347" t="s">
+      <c r="O25" s="350" t="s">
         <v>267</v>
       </c>
-      <c r="P25" s="311"/>
-      <c r="Q25" s="311"/>
-      <c r="R25" s="311"/>
-      <c r="S25" s="376"/>
+      <c r="P25" s="314"/>
+      <c r="Q25" s="314"/>
+      <c r="R25" s="314"/>
+      <c r="S25" s="379"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="177"/>
@@ -16767,11 +17348,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="178"/>
       <c r="N26" s="172"/>
-      <c r="O26" s="367"/>
-      <c r="P26" s="368"/>
-      <c r="Q26" s="368"/>
-      <c r="R26" s="368"/>
-      <c r="S26" s="369"/>
+      <c r="O26" s="370"/>
+      <c r="P26" s="371"/>
+      <c r="Q26" s="371"/>
+      <c r="R26" s="371"/>
+      <c r="S26" s="372"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="179"/>
@@ -16902,44 +17483,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="400" t="s">
+      <c r="C2" s="403" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="401"/>
-      <c r="E2" s="401"/>
-      <c r="F2" s="401"/>
-      <c r="G2" s="401"/>
-      <c r="H2" s="401"/>
-      <c r="I2" s="401"/>
-      <c r="J2" s="401"/>
-      <c r="K2" s="401"/>
+      <c r="D2" s="404"/>
+      <c r="E2" s="404"/>
+      <c r="F2" s="404"/>
+      <c r="G2" s="404"/>
+      <c r="H2" s="404"/>
+      <c r="I2" s="404"/>
+      <c r="J2" s="404"/>
+      <c r="K2" s="404"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="401"/>
-      <c r="D3" s="401"/>
-      <c r="E3" s="401"/>
-      <c r="F3" s="401"/>
-      <c r="G3" s="401"/>
-      <c r="H3" s="401"/>
-      <c r="I3" s="401"/>
-      <c r="J3" s="401"/>
-      <c r="K3" s="401"/>
+      <c r="C3" s="404"/>
+      <c r="D3" s="404"/>
+      <c r="E3" s="404"/>
+      <c r="F3" s="404"/>
+      <c r="G3" s="404"/>
+      <c r="H3" s="404"/>
+      <c r="I3" s="404"/>
+      <c r="J3" s="404"/>
+      <c r="K3" s="404"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="408" t="s">
+      <c r="C5" s="411" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="408"/>
-      <c r="E5" s="408"/>
-      <c r="F5" s="408"/>
-      <c r="G5" s="408"/>
-      <c r="I5" s="408" t="s">
+      <c r="D5" s="411"/>
+      <c r="E5" s="411"/>
+      <c r="F5" s="411"/>
+      <c r="G5" s="411"/>
+      <c r="I5" s="411" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="408"/>
-      <c r="K5" s="408"/>
-      <c r="L5" s="408"/>
-      <c r="M5" s="408"/>
+      <c r="J5" s="411"/>
+      <c r="K5" s="411"/>
+      <c r="L5" s="411"/>
+      <c r="M5" s="411"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -17379,88 +17960,88 @@
       <c r="M28" s="172"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="352" t="s">
+      <c r="D29" s="355" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="353"/>
-      <c r="F29" s="402">
+      <c r="E29" s="356"/>
+      <c r="F29" s="405">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="403"/>
+      <c r="G29" s="406"/>
       <c r="I29" s="172"/>
-      <c r="J29" s="352" t="s">
+      <c r="J29" s="355" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="353"/>
-      <c r="L29" s="402">
+      <c r="K29" s="356"/>
+      <c r="L29" s="405">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="403"/>
+      <c r="M29" s="406"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="399" t="s">
+      <c r="D30" s="402" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="311"/>
-      <c r="F30" s="404">
+      <c r="E30" s="314"/>
+      <c r="F30" s="407">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="405"/>
+      <c r="G30" s="408"/>
       <c r="I30" s="172"/>
-      <c r="J30" s="399" t="s">
+      <c r="J30" s="402" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="311"/>
-      <c r="L30" s="404">
+      <c r="K30" s="314"/>
+      <c r="L30" s="407">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="405"/>
+      <c r="M30" s="408"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="347" t="s">
+      <c r="D31" s="350" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="311"/>
-      <c r="F31" s="409">
+      <c r="E31" s="314"/>
+      <c r="F31" s="412">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="410"/>
+      <c r="G31" s="413"/>
       <c r="I31" s="172"/>
-      <c r="J31" s="347" t="s">
+      <c r="J31" s="350" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="311"/>
-      <c r="L31" s="409">
+      <c r="K31" s="314"/>
+      <c r="L31" s="412">
         <f>L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="410"/>
+      <c r="M31" s="413"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="348" t="s">
+      <c r="D32" s="351" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="349"/>
-      <c r="F32" s="406">
+      <c r="E32" s="352"/>
+      <c r="F32" s="409">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="407"/>
+      <c r="G32" s="410"/>
       <c r="I32" s="172"/>
-      <c r="J32" s="348" t="s">
+      <c r="J32" s="351" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="349"/>
-      <c r="L32" s="406">
+      <c r="K32" s="352"/>
+      <c r="L32" s="409">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="407"/>
+      <c r="M32" s="410"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17703,44 +18284,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="411" t="s">
+      <c r="C2" s="414" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="412"/>
-      <c r="E2" s="412"/>
-      <c r="F2" s="412"/>
-      <c r="G2" s="412"/>
-      <c r="H2" s="412"/>
-      <c r="I2" s="412"/>
-      <c r="J2" s="412"/>
-      <c r="K2" s="412"/>
+      <c r="D2" s="415"/>
+      <c r="E2" s="415"/>
+      <c r="F2" s="415"/>
+      <c r="G2" s="415"/>
+      <c r="H2" s="415"/>
+      <c r="I2" s="415"/>
+      <c r="J2" s="415"/>
+      <c r="K2" s="415"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="412"/>
-      <c r="D3" s="412"/>
-      <c r="E3" s="412"/>
-      <c r="F3" s="412"/>
-      <c r="G3" s="412"/>
-      <c r="H3" s="412"/>
-      <c r="I3" s="412"/>
-      <c r="J3" s="412"/>
-      <c r="K3" s="412"/>
+      <c r="C3" s="415"/>
+      <c r="D3" s="415"/>
+      <c r="E3" s="415"/>
+      <c r="F3" s="415"/>
+      <c r="G3" s="415"/>
+      <c r="H3" s="415"/>
+      <c r="I3" s="415"/>
+      <c r="J3" s="415"/>
+      <c r="K3" s="415"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="408" t="s">
+      <c r="C5" s="411" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="408"/>
-      <c r="E5" s="408"/>
-      <c r="F5" s="408"/>
-      <c r="G5" s="408"/>
-      <c r="I5" s="408" t="s">
+      <c r="D5" s="411"/>
+      <c r="E5" s="411"/>
+      <c r="F5" s="411"/>
+      <c r="G5" s="411"/>
+      <c r="I5" s="411" t="s">
         <v>246</v>
       </c>
-      <c r="J5" s="408"/>
-      <c r="K5" s="408"/>
-      <c r="L5" s="408"/>
-      <c r="M5" s="408"/>
+      <c r="J5" s="411"/>
+      <c r="K5" s="411"/>
+      <c r="L5" s="411"/>
+      <c r="M5" s="411"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -18224,88 +18805,88 @@
       <c r="M28" s="172"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="387" t="s">
+      <c r="D29" s="390" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="389"/>
-      <c r="F29" s="413">
+      <c r="E29" s="392"/>
+      <c r="F29" s="416">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="414"/>
+      <c r="G29" s="417"/>
       <c r="I29" s="172"/>
-      <c r="J29" s="387" t="s">
+      <c r="J29" s="390" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="389"/>
-      <c r="L29" s="413">
+      <c r="K29" s="392"/>
+      <c r="L29" s="416">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="414"/>
+      <c r="M29" s="417"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="347" t="s">
+      <c r="D30" s="350" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="311"/>
-      <c r="F30" s="404">
+      <c r="E30" s="314"/>
+      <c r="F30" s="407">
         <f>F27</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="405"/>
+      <c r="G30" s="408"/>
       <c r="I30" s="172"/>
-      <c r="J30" s="347" t="s">
+      <c r="J30" s="350" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="311"/>
-      <c r="L30" s="404">
+      <c r="K30" s="314"/>
+      <c r="L30" s="407">
         <f>L27</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="405"/>
+      <c r="M30" s="408"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="347" t="s">
+      <c r="D31" s="350" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="311"/>
-      <c r="F31" s="409">
+      <c r="E31" s="314"/>
+      <c r="F31" s="412">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="410"/>
+      <c r="G31" s="413"/>
       <c r="I31" s="172"/>
-      <c r="J31" s="347" t="s">
+      <c r="J31" s="350" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="311"/>
-      <c r="L31" s="409">
+      <c r="K31" s="314"/>
+      <c r="L31" s="412">
         <f>Pemasukkan!L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="410"/>
+      <c r="M31" s="413"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="348" t="s">
+      <c r="D32" s="351" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="349"/>
-      <c r="F32" s="415">
+      <c r="E32" s="352"/>
+      <c r="F32" s="418">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="416"/>
+      <c r="G32" s="419"/>
       <c r="I32" s="172"/>
-      <c r="J32" s="348" t="s">
+      <c r="J32" s="351" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="349"/>
-      <c r="L32" s="415">
+      <c r="K32" s="352"/>
+      <c r="L32" s="418">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="416"/>
+      <c r="M32" s="419"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18541,28 +19122,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="419" t="s">
+      <c r="C2" s="422" t="s">
         <v>230</v>
       </c>
-      <c r="D2" s="420"/>
-      <c r="E2" s="420"/>
-      <c r="F2" s="420"/>
-      <c r="G2" s="420"/>
-      <c r="H2" s="420"/>
-      <c r="I2" s="420"/>
-      <c r="J2" s="420"/>
-      <c r="K2" s="420"/>
+      <c r="D2" s="423"/>
+      <c r="E2" s="423"/>
+      <c r="F2" s="423"/>
+      <c r="G2" s="423"/>
+      <c r="H2" s="423"/>
+      <c r="I2" s="423"/>
+      <c r="J2" s="423"/>
+      <c r="K2" s="423"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="420"/>
-      <c r="D3" s="420"/>
-      <c r="E3" s="420"/>
-      <c r="F3" s="420"/>
-      <c r="G3" s="420"/>
-      <c r="H3" s="420"/>
-      <c r="I3" s="420"/>
-      <c r="J3" s="420"/>
-      <c r="K3" s="420"/>
+      <c r="C3" s="423"/>
+      <c r="D3" s="423"/>
+      <c r="E3" s="423"/>
+      <c r="F3" s="423"/>
+      <c r="G3" s="423"/>
+      <c r="H3" s="423"/>
+      <c r="I3" s="423"/>
+      <c r="J3" s="423"/>
+      <c r="K3" s="423"/>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="141"/>
@@ -18920,10 +19501,10 @@
     </row>
     <row r="29" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="141"/>
-      <c r="D29" s="421"/>
-      <c r="E29" s="421"/>
-      <c r="F29" s="422"/>
-      <c r="G29" s="422"/>
+      <c r="D29" s="424"/>
+      <c r="E29" s="424"/>
+      <c r="F29" s="425"/>
+      <c r="G29" s="425"/>
       <c r="H29" s="141"/>
       <c r="I29" s="141"/>
       <c r="J29" s="141"/>
@@ -18931,15 +19512,15 @@
     </row>
     <row r="30" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="24"/>
-      <c r="D30" s="423" t="s">
+      <c r="D30" s="426" t="s">
         <v>229</v>
       </c>
-      <c r="E30" s="424"/>
-      <c r="F30" s="425">
+      <c r="E30" s="427"/>
+      <c r="F30" s="428">
         <f>F27</f>
         <v>226000</v>
       </c>
-      <c r="G30" s="426"/>
+      <c r="G30" s="429"/>
       <c r="H30" s="141"/>
       <c r="I30" s="141"/>
       <c r="J30" s="141"/>
@@ -18954,10 +19535,10 @@
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="141"/>
-      <c r="D32" s="417"/>
-      <c r="E32" s="417"/>
-      <c r="F32" s="418"/>
-      <c r="G32" s="417"/>
+      <c r="D32" s="420"/>
+      <c r="E32" s="420"/>
+      <c r="F32" s="421"/>
+      <c r="G32" s="420"/>
       <c r="H32" s="141"/>
       <c r="I32" s="141"/>
       <c r="J32" s="141"/>
@@ -18994,17 +19575,17 @@
     <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="427" t="s">
+      <c r="C4" s="430" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="428"/>
+      <c r="D4" s="431"/>
       <c r="E4" s="27"/>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
-      <c r="H4" s="427" t="s">
+      <c r="H4" s="430" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="428"/>
+      <c r="I4" s="431"/>
       <c r="J4" s="35"/>
       <c r="K4" s="27"/>
     </row>
@@ -19131,17 +19712,17 @@
     <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26"/>
-      <c r="C17" s="427" t="s">
+      <c r="C17" s="430" t="s">
         <v>144</v>
       </c>
-      <c r="D17" s="428"/>
+      <c r="D17" s="431"/>
       <c r="E17" s="27"/>
       <c r="F17" s="26"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="427" t="s">
+      <c r="H17" s="430" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="428"/>
+      <c r="I17" s="431"/>
       <c r="J17" s="35"/>
       <c r="K17" s="27"/>
     </row>

</xml_diff>

<commit_message>
fix format nama tabel pembayaran makrab 19
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -2400,7 +2400,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="443">
+  <cellXfs count="442">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3000,7 +3000,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3021,10 +3020,10 @@
     <xf numFmtId="177" fontId="4" fillId="26" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -4670,126 +4669,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="294" t="s">
+      <c r="A1" s="293" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="295"/>
-      <c r="C1" s="295"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="295"/>
-      <c r="F1" s="295"/>
-      <c r="G1" s="295"/>
-      <c r="H1" s="295"/>
-      <c r="I1" s="295"/>
-      <c r="J1" s="295"/>
-      <c r="K1" s="295"/>
-      <c r="L1" s="295"/>
-      <c r="M1" s="295"/>
-      <c r="N1" s="295"/>
-      <c r="O1" s="295"/>
-      <c r="P1" s="295"/>
-      <c r="Q1" s="295"/>
-      <c r="R1" s="295"/>
+      <c r="B1" s="294"/>
+      <c r="C1" s="294"/>
+      <c r="D1" s="294"/>
+      <c r="E1" s="294"/>
+      <c r="F1" s="294"/>
+      <c r="G1" s="294"/>
+      <c r="H1" s="294"/>
+      <c r="I1" s="294"/>
+      <c r="J1" s="294"/>
+      <c r="K1" s="294"/>
+      <c r="L1" s="294"/>
+      <c r="M1" s="294"/>
+      <c r="N1" s="294"/>
+      <c r="O1" s="294"/>
+      <c r="P1" s="294"/>
+      <c r="Q1" s="294"/>
+      <c r="R1" s="294"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="296"/>
-      <c r="B2" s="297"/>
-      <c r="C2" s="297"/>
-      <c r="D2" s="297"/>
-      <c r="E2" s="297"/>
-      <c r="F2" s="297"/>
-      <c r="G2" s="297"/>
-      <c r="H2" s="297"/>
-      <c r="I2" s="297"/>
-      <c r="J2" s="297"/>
-      <c r="K2" s="297"/>
-      <c r="L2" s="297"/>
-      <c r="M2" s="297"/>
-      <c r="N2" s="297"/>
-      <c r="O2" s="297"/>
-      <c r="P2" s="297"/>
-      <c r="Q2" s="297"/>
-      <c r="R2" s="297"/>
+      <c r="A2" s="295"/>
+      <c r="B2" s="296"/>
+      <c r="C2" s="296"/>
+      <c r="D2" s="296"/>
+      <c r="E2" s="296"/>
+      <c r="F2" s="296"/>
+      <c r="G2" s="296"/>
+      <c r="H2" s="296"/>
+      <c r="I2" s="296"/>
+      <c r="J2" s="296"/>
+      <c r="K2" s="296"/>
+      <c r="L2" s="296"/>
+      <c r="M2" s="296"/>
+      <c r="N2" s="296"/>
+      <c r="O2" s="296"/>
+      <c r="P2" s="296"/>
+      <c r="Q2" s="296"/>
+      <c r="R2" s="296"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="296"/>
-      <c r="B3" s="297"/>
-      <c r="C3" s="297"/>
-      <c r="D3" s="297"/>
-      <c r="E3" s="297"/>
-      <c r="F3" s="297"/>
-      <c r="G3" s="297"/>
-      <c r="H3" s="297"/>
-      <c r="I3" s="297"/>
-      <c r="J3" s="297"/>
-      <c r="K3" s="297"/>
-      <c r="L3" s="297"/>
-      <c r="M3" s="297"/>
-      <c r="N3" s="297"/>
-      <c r="O3" s="297"/>
-      <c r="P3" s="297"/>
-      <c r="Q3" s="297"/>
-      <c r="R3" s="297"/>
+      <c r="A3" s="295"/>
+      <c r="B3" s="296"/>
+      <c r="C3" s="296"/>
+      <c r="D3" s="296"/>
+      <c r="E3" s="296"/>
+      <c r="F3" s="296"/>
+      <c r="G3" s="296"/>
+      <c r="H3" s="296"/>
+      <c r="I3" s="296"/>
+      <c r="J3" s="296"/>
+      <c r="K3" s="296"/>
+      <c r="L3" s="296"/>
+      <c r="M3" s="296"/>
+      <c r="N3" s="296"/>
+      <c r="O3" s="296"/>
+      <c r="P3" s="296"/>
+      <c r="Q3" s="296"/>
+      <c r="R3" s="296"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="296"/>
-      <c r="B4" s="297"/>
-      <c r="C4" s="297"/>
-      <c r="D4" s="297"/>
-      <c r="E4" s="297"/>
-      <c r="F4" s="297"/>
-      <c r="G4" s="297"/>
-      <c r="H4" s="297"/>
-      <c r="I4" s="297"/>
-      <c r="J4" s="297"/>
-      <c r="K4" s="297"/>
-      <c r="L4" s="297"/>
-      <c r="M4" s="297"/>
-      <c r="N4" s="297"/>
-      <c r="O4" s="297"/>
-      <c r="P4" s="297"/>
-      <c r="Q4" s="297"/>
-      <c r="R4" s="297"/>
+      <c r="A4" s="295"/>
+      <c r="B4" s="296"/>
+      <c r="C4" s="296"/>
+      <c r="D4" s="296"/>
+      <c r="E4" s="296"/>
+      <c r="F4" s="296"/>
+      <c r="G4" s="296"/>
+      <c r="H4" s="296"/>
+      <c r="I4" s="296"/>
+      <c r="J4" s="296"/>
+      <c r="K4" s="296"/>
+      <c r="L4" s="296"/>
+      <c r="M4" s="296"/>
+      <c r="N4" s="296"/>
+      <c r="O4" s="296"/>
+      <c r="P4" s="296"/>
+      <c r="Q4" s="296"/>
+      <c r="R4" s="296"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="296"/>
-      <c r="B5" s="297"/>
-      <c r="C5" s="297"/>
-      <c r="D5" s="297"/>
-      <c r="E5" s="297"/>
-      <c r="F5" s="297"/>
-      <c r="G5" s="297"/>
-      <c r="H5" s="297"/>
-      <c r="I5" s="297"/>
-      <c r="J5" s="297"/>
-      <c r="K5" s="297"/>
-      <c r="L5" s="297"/>
-      <c r="M5" s="297"/>
-      <c r="N5" s="297"/>
-      <c r="O5" s="297"/>
-      <c r="P5" s="297"/>
-      <c r="Q5" s="297"/>
-      <c r="R5" s="297"/>
+      <c r="A5" s="295"/>
+      <c r="B5" s="296"/>
+      <c r="C5" s="296"/>
+      <c r="D5" s="296"/>
+      <c r="E5" s="296"/>
+      <c r="F5" s="296"/>
+      <c r="G5" s="296"/>
+      <c r="H5" s="296"/>
+      <c r="I5" s="296"/>
+      <c r="J5" s="296"/>
+      <c r="K5" s="296"/>
+      <c r="L5" s="296"/>
+      <c r="M5" s="296"/>
+      <c r="N5" s="296"/>
+      <c r="O5" s="296"/>
+      <c r="P5" s="296"/>
+      <c r="Q5" s="296"/>
+      <c r="R5" s="296"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="296"/>
-      <c r="B6" s="297"/>
-      <c r="C6" s="297"/>
-      <c r="D6" s="297"/>
-      <c r="E6" s="297"/>
-      <c r="F6" s="297"/>
-      <c r="G6" s="297"/>
-      <c r="H6" s="297"/>
-      <c r="I6" s="297"/>
-      <c r="J6" s="297"/>
-      <c r="K6" s="297"/>
-      <c r="L6" s="297"/>
-      <c r="M6" s="297"/>
-      <c r="N6" s="297"/>
-      <c r="O6" s="297"/>
-      <c r="P6" s="297"/>
-      <c r="Q6" s="297"/>
-      <c r="R6" s="297"/>
+      <c r="A6" s="295"/>
+      <c r="B6" s="296"/>
+      <c r="C6" s="296"/>
+      <c r="D6" s="296"/>
+      <c r="E6" s="296"/>
+      <c r="F6" s="296"/>
+      <c r="G6" s="296"/>
+      <c r="H6" s="296"/>
+      <c r="I6" s="296"/>
+      <c r="J6" s="296"/>
+      <c r="K6" s="296"/>
+      <c r="L6" s="296"/>
+      <c r="M6" s="296"/>
+      <c r="N6" s="296"/>
+      <c r="O6" s="296"/>
+      <c r="P6" s="296"/>
+      <c r="Q6" s="296"/>
+      <c r="R6" s="296"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -7896,58 +7895,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="299" t="s">
+      <c r="J79" s="298" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="300"/>
-      <c r="L79" s="300"/>
-      <c r="M79" s="300"/>
-      <c r="N79" s="301"/>
-      <c r="P79" s="307" t="s">
+      <c r="K79" s="299"/>
+      <c r="L79" s="299"/>
+      <c r="M79" s="299"/>
+      <c r="N79" s="300"/>
+      <c r="P79" s="306" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="300"/>
-      <c r="R79" s="300"/>
-      <c r="S79" s="301"/>
+      <c r="Q79" s="299"/>
+      <c r="R79" s="299"/>
+      <c r="S79" s="300"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="302" t="s">
+      <c r="J80" s="301" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="297"/>
-      <c r="L80" s="297"/>
-      <c r="M80" s="297"/>
-      <c r="N80" s="303"/>
-      <c r="P80" s="302" t="s">
+      <c r="K80" s="296"/>
+      <c r="L80" s="296"/>
+      <c r="M80" s="296"/>
+      <c r="N80" s="302"/>
+      <c r="P80" s="301" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="297"/>
-      <c r="R80" s="297"/>
-      <c r="S80" s="303"/>
+      <c r="Q80" s="296"/>
+      <c r="R80" s="296"/>
+      <c r="S80" s="302"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="304"/>
-      <c r="K81" s="305"/>
-      <c r="L81" s="305"/>
-      <c r="M81" s="305"/>
-      <c r="N81" s="306"/>
-      <c r="P81" s="304"/>
-      <c r="Q81" s="305"/>
-      <c r="R81" s="305"/>
-      <c r="S81" s="306"/>
+      <c r="J81" s="303"/>
+      <c r="K81" s="304"/>
+      <c r="L81" s="304"/>
+      <c r="M81" s="304"/>
+      <c r="N81" s="305"/>
+      <c r="P81" s="303"/>
+      <c r="Q81" s="304"/>
+      <c r="R81" s="304"/>
+      <c r="S81" s="305"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="298" t="s">
+      <c r="J82" s="297" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="289"/>
-      <c r="L82" s="290"/>
-      <c r="M82" s="298" t="s">
+      <c r="K82" s="288"/>
+      <c r="L82" s="289"/>
+      <c r="M82" s="297" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="290"/>
-      <c r="P82" s="298"/>
-      <c r="Q82" s="290"/>
+      <c r="N82" s="289"/>
+      <c r="P82" s="297"/>
+      <c r="Q82" s="289"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -7956,38 +7955,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="288" t="s">
+      <c r="J83" s="287" t="s">
         <v>70</v>
       </c>
-      <c r="K83" s="289"/>
-      <c r="L83" s="290"/>
-      <c r="M83" s="291">
+      <c r="K83" s="288"/>
+      <c r="L83" s="289"/>
+      <c r="M83" s="290">
         <v>7350000</v>
       </c>
-      <c r="N83" s="290"/>
-      <c r="P83" s="292" t="s">
+      <c r="N83" s="289"/>
+      <c r="P83" s="291" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="290"/>
+      <c r="Q83" s="289"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="288" t="s">
+      <c r="J84" s="287" t="s">
         <v>72</v>
       </c>
-      <c r="K84" s="289"/>
-      <c r="L84" s="290"/>
-      <c r="M84" s="293">
+      <c r="K84" s="288"/>
+      <c r="L84" s="289"/>
+      <c r="M84" s="292">
         <v>1100000</v>
       </c>
-      <c r="N84" s="290"/>
-      <c r="P84" s="292" t="s">
+      <c r="N84" s="289"/>
+      <c r="P84" s="291" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="290"/>
+      <c r="Q84" s="289"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -7996,39 +7995,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="288" t="s">
+      <c r="J85" s="287" t="s">
         <v>75</v>
       </c>
-      <c r="K85" s="289"/>
-      <c r="L85" s="290"/>
-      <c r="M85" s="291">
+      <c r="K85" s="288"/>
+      <c r="L85" s="289"/>
+      <c r="M85" s="290">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="290"/>
-      <c r="P85" s="292" t="s">
+      <c r="N85" s="289"/>
+      <c r="P85" s="291" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="290"/>
+      <c r="Q85" s="289"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="288" t="s">
+      <c r="J86" s="287" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="289"/>
-      <c r="L86" s="290"/>
-      <c r="M86" s="291">
+      <c r="K86" s="288"/>
+      <c r="L86" s="289"/>
+      <c r="M86" s="290">
         <v>8411850</v>
       </c>
-      <c r="N86" s="290"/>
-      <c r="P86" s="292" t="s">
+      <c r="N86" s="289"/>
+      <c r="P86" s="291" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="290"/>
+      <c r="Q86" s="289"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -8036,20 +8035,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="288" t="s">
+      <c r="J87" s="287" t="s">
         <v>79</v>
       </c>
-      <c r="K87" s="289"/>
-      <c r="L87" s="290"/>
-      <c r="M87" s="291">
+      <c r="K87" s="288"/>
+      <c r="L87" s="289"/>
+      <c r="M87" s="290">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="290"/>
-      <c r="P87" s="292" t="s">
+      <c r="N87" s="289"/>
+      <c r="P87" s="291" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="290"/>
+      <c r="Q87" s="289"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -8306,28 +8305,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="439" t="s">
+      <c r="B2" s="438" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="440"/>
-      <c r="D2" s="440"/>
-      <c r="E2" s="440"/>
-      <c r="F2" s="440"/>
-      <c r="G2" s="440"/>
-      <c r="H2" s="440"/>
-      <c r="I2" s="440"/>
-      <c r="J2" s="440"/>
+      <c r="C2" s="439"/>
+      <c r="D2" s="439"/>
+      <c r="E2" s="439"/>
+      <c r="F2" s="439"/>
+      <c r="G2" s="439"/>
+      <c r="H2" s="439"/>
+      <c r="I2" s="439"/>
+      <c r="J2" s="439"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="440"/>
-      <c r="C3" s="440"/>
-      <c r="D3" s="440"/>
-      <c r="E3" s="440"/>
-      <c r="F3" s="440"/>
-      <c r="G3" s="440"/>
-      <c r="H3" s="440"/>
-      <c r="I3" s="440"/>
-      <c r="J3" s="440"/>
+      <c r="B3" s="439"/>
+      <c r="C3" s="439"/>
+      <c r="D3" s="439"/>
+      <c r="E3" s="439"/>
+      <c r="F3" s="439"/>
+      <c r="G3" s="439"/>
+      <c r="H3" s="439"/>
+      <c r="I3" s="439"/>
+      <c r="J3" s="439"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -8348,10 +8347,10 @@
       <c r="G6" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="H6" s="355" t="s">
+      <c r="H6" s="354" t="s">
         <v>280</v>
       </c>
-      <c r="I6" s="321"/>
+      <c r="I6" s="320"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -8373,11 +8372,11 @@
       <c r="G7" s="193">
         <v>205000</v>
       </c>
-      <c r="H7" s="441">
+      <c r="H7" s="440">
         <f>F7-G7</f>
         <v>380000</v>
       </c>
-      <c r="I7" s="321"/>
+      <c r="I7" s="320"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="194"/>
@@ -8386,8 +8385,8 @@
       <c r="E8" s="195"/>
       <c r="F8" s="195"/>
       <c r="G8" s="195"/>
-      <c r="H8" s="438"/>
-      <c r="I8" s="438"/>
+      <c r="H8" s="437"/>
+      <c r="I8" s="437"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="194"/>
@@ -8398,11 +8397,11 @@
       <c r="G9" s="196" t="s">
         <v>281</v>
       </c>
-      <c r="H9" s="442">
+      <c r="H9" s="441">
         <f>H7</f>
         <v>380000</v>
       </c>
-      <c r="I9" s="345"/>
+      <c r="I9" s="344"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="194"/>
@@ -8411,8 +8410,8 @@
       <c r="E10" s="195"/>
       <c r="F10" s="195"/>
       <c r="G10" s="195"/>
-      <c r="H10" s="438"/>
-      <c r="I10" s="438"/>
+      <c r="H10" s="437"/>
+      <c r="I10" s="437"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="194"/>
@@ -8421,8 +8420,8 @@
       <c r="E11" s="195"/>
       <c r="F11" s="195"/>
       <c r="G11" s="195"/>
-      <c r="H11" s="438"/>
-      <c r="I11" s="438"/>
+      <c r="H11" s="437"/>
+      <c r="I11" s="437"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="194"/>
@@ -8431,8 +8430,8 @@
       <c r="E12" s="195"/>
       <c r="F12" s="195"/>
       <c r="G12" s="195"/>
-      <c r="H12" s="438"/>
-      <c r="I12" s="438"/>
+      <c r="H12" s="437"/>
+      <c r="I12" s="437"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="194"/>
@@ -8441,8 +8440,8 @@
       <c r="E13" s="195"/>
       <c r="F13" s="195"/>
       <c r="G13" s="195"/>
-      <c r="H13" s="438"/>
-      <c r="I13" s="438"/>
+      <c r="H13" s="437"/>
+      <c r="I13" s="437"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="194"/>
@@ -8451,8 +8450,8 @@
       <c r="E14" s="195"/>
       <c r="F14" s="195"/>
       <c r="G14" s="195"/>
-      <c r="H14" s="438"/>
-      <c r="I14" s="438"/>
+      <c r="H14" s="437"/>
+      <c r="I14" s="437"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="194"/>
@@ -8461,8 +8460,8 @@
       <c r="E15" s="195"/>
       <c r="F15" s="195"/>
       <c r="G15" s="195"/>
-      <c r="H15" s="438"/>
-      <c r="I15" s="438"/>
+      <c r="H15" s="437"/>
+      <c r="I15" s="437"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="194"/>
@@ -8471,8 +8470,8 @@
       <c r="E16" s="195"/>
       <c r="F16" s="195"/>
       <c r="G16" s="195"/>
-      <c r="H16" s="438"/>
-      <c r="I16" s="438"/>
+      <c r="H16" s="437"/>
+      <c r="I16" s="437"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="194"/>
@@ -8481,8 +8480,8 @@
       <c r="E17" s="195"/>
       <c r="F17" s="195"/>
       <c r="G17" s="195"/>
-      <c r="H17" s="438"/>
-      <c r="I17" s="438"/>
+      <c r="H17" s="437"/>
+      <c r="I17" s="437"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -8552,46 +8551,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="316" t="s">
+      <c r="C2" s="315" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="295"/>
-      <c r="E2" s="295"/>
-      <c r="F2" s="295"/>
-      <c r="G2" s="295"/>
-      <c r="H2" s="295"/>
-      <c r="I2" s="295"/>
-      <c r="J2" s="295"/>
-      <c r="K2" s="295"/>
-      <c r="L2" s="295"/>
-      <c r="M2" s="295"/>
-      <c r="N2" s="295"/>
-      <c r="O2" s="295"/>
-      <c r="P2" s="296"/>
-      <c r="Q2" s="296"/>
-      <c r="R2" s="296"/>
-      <c r="S2" s="295"/>
-      <c r="T2" s="295"/>
+      <c r="D2" s="294"/>
+      <c r="E2" s="294"/>
+      <c r="F2" s="294"/>
+      <c r="G2" s="294"/>
+      <c r="H2" s="294"/>
+      <c r="I2" s="294"/>
+      <c r="J2" s="294"/>
+      <c r="K2" s="294"/>
+      <c r="L2" s="294"/>
+      <c r="M2" s="294"/>
+      <c r="N2" s="294"/>
+      <c r="O2" s="294"/>
+      <c r="P2" s="295"/>
+      <c r="Q2" s="295"/>
+      <c r="R2" s="295"/>
+      <c r="S2" s="294"/>
+      <c r="T2" s="294"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="296"/>
-      <c r="D3" s="297"/>
-      <c r="E3" s="297"/>
-      <c r="F3" s="297"/>
-      <c r="G3" s="297"/>
-      <c r="H3" s="297"/>
-      <c r="I3" s="297"/>
-      <c r="J3" s="297"/>
-      <c r="K3" s="297"/>
-      <c r="L3" s="297"/>
-      <c r="M3" s="297"/>
-      <c r="N3" s="297"/>
-      <c r="O3" s="297"/>
-      <c r="P3" s="297"/>
-      <c r="Q3" s="297"/>
-      <c r="R3" s="297"/>
-      <c r="S3" s="297"/>
-      <c r="T3" s="297"/>
+      <c r="C3" s="295"/>
+      <c r="D3" s="296"/>
+      <c r="E3" s="296"/>
+      <c r="F3" s="296"/>
+      <c r="G3" s="296"/>
+      <c r="H3" s="296"/>
+      <c r="I3" s="296"/>
+      <c r="J3" s="296"/>
+      <c r="K3" s="296"/>
+      <c r="L3" s="296"/>
+      <c r="M3" s="296"/>
+      <c r="N3" s="296"/>
+      <c r="O3" s="296"/>
+      <c r="P3" s="296"/>
+      <c r="Q3" s="296"/>
+      <c r="R3" s="296"/>
+      <c r="S3" s="296"/>
+      <c r="T3" s="296"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8678,25 +8677,25 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="322" t="s">
+      <c r="X5" s="321" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="289"/>
-      <c r="Z5" s="289"/>
-      <c r="AA5" s="289"/>
-      <c r="AB5" s="289"/>
-      <c r="AC5" s="289"/>
-      <c r="AD5" s="289"/>
-      <c r="AE5" s="289"/>
-      <c r="AF5" s="289"/>
-      <c r="AG5" s="289"/>
-      <c r="AH5" s="289"/>
-      <c r="AI5" s="289"/>
-      <c r="AJ5" s="289"/>
-      <c r="AK5" s="289"/>
-      <c r="AL5" s="289"/>
-      <c r="AM5" s="289"/>
-      <c r="AN5" s="290"/>
+      <c r="Y5" s="288"/>
+      <c r="Z5" s="288"/>
+      <c r="AA5" s="288"/>
+      <c r="AB5" s="288"/>
+      <c r="AC5" s="288"/>
+      <c r="AD5" s="288"/>
+      <c r="AE5" s="288"/>
+      <c r="AF5" s="288"/>
+      <c r="AG5" s="288"/>
+      <c r="AH5" s="288"/>
+      <c r="AI5" s="288"/>
+      <c r="AJ5" s="288"/>
+      <c r="AK5" s="288"/>
+      <c r="AL5" s="288"/>
+      <c r="AM5" s="288"/>
+      <c r="AN5" s="289"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -8771,29 +8770,29 @@
       <c r="V6" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X6" s="317" t="s">
+      <c r="X6" s="316" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="317" t="s">
+      <c r="Y6" s="316" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="321" t="s">
+      <c r="Z6" s="320" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="318"/>
-      <c r="AB6" s="318"/>
-      <c r="AC6" s="318"/>
-      <c r="AD6" s="318"/>
-      <c r="AE6" s="318"/>
-      <c r="AF6" s="318"/>
-      <c r="AG6" s="318"/>
-      <c r="AH6" s="318"/>
-      <c r="AI6" s="318"/>
-      <c r="AJ6" s="318"/>
-      <c r="AK6" s="318"/>
-      <c r="AL6" s="318"/>
-      <c r="AM6" s="318"/>
-      <c r="AN6" s="318"/>
+      <c r="AA6" s="317"/>
+      <c r="AB6" s="317"/>
+      <c r="AC6" s="317"/>
+      <c r="AD6" s="317"/>
+      <c r="AE6" s="317"/>
+      <c r="AF6" s="317"/>
+      <c r="AG6" s="317"/>
+      <c r="AH6" s="317"/>
+      <c r="AI6" s="317"/>
+      <c r="AJ6" s="317"/>
+      <c r="AK6" s="317"/>
+      <c r="AL6" s="317"/>
+      <c r="AM6" s="317"/>
+      <c r="AN6" s="317"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -8868,27 +8867,27 @@
       <c r="V7" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X7" s="318"/>
-      <c r="Y7" s="318"/>
-      <c r="Z7" s="321" t="s">
+      <c r="X7" s="317"/>
+      <c r="Y7" s="317"/>
+      <c r="Z7" s="320" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="318"/>
-      <c r="AB7" s="318"/>
-      <c r="AC7" s="318"/>
-      <c r="AD7" s="321" t="s">
+      <c r="AA7" s="317"/>
+      <c r="AB7" s="317"/>
+      <c r="AC7" s="317"/>
+      <c r="AD7" s="320" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="318"/>
-      <c r="AF7" s="318"/>
-      <c r="AG7" s="318"/>
-      <c r="AH7" s="318"/>
-      <c r="AI7" s="318"/>
-      <c r="AJ7" s="318"/>
-      <c r="AK7" s="318"/>
-      <c r="AL7" s="318"/>
-      <c r="AM7" s="318"/>
-      <c r="AN7" s="318"/>
+      <c r="AE7" s="317"/>
+      <c r="AF7" s="317"/>
+      <c r="AG7" s="317"/>
+      <c r="AH7" s="317"/>
+      <c r="AI7" s="317"/>
+      <c r="AJ7" s="317"/>
+      <c r="AK7" s="317"/>
+      <c r="AL7" s="317"/>
+      <c r="AM7" s="317"/>
+      <c r="AN7" s="317"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -8938,8 +8937,8 @@
         <v>NO</v>
       </c>
       <c r="V8" s="13"/>
-      <c r="X8" s="318"/>
-      <c r="Y8" s="318"/>
+      <c r="X8" s="317"/>
+      <c r="Y8" s="317"/>
       <c r="Z8" s="151" t="s">
         <v>19</v>
       </c>
@@ -13550,10 +13549,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="319" t="s">
+      <c r="AA49" s="318" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="320"/>
+      <c r="AB49" s="319"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -13631,12 +13630,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="326" t="s">
+      <c r="AI50" s="325" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="327"/>
-      <c r="AK50" s="327"/>
-      <c r="AL50" s="328"/>
+      <c r="AJ50" s="326"/>
+      <c r="AK50" s="326"/>
+      <c r="AL50" s="327"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -13707,12 +13706,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="323" t="s">
+      <c r="AI51" s="322" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="324"/>
-      <c r="AK51" s="324"/>
-      <c r="AL51" s="325"/>
+      <c r="AJ51" s="323"/>
+      <c r="AK51" s="323"/>
+      <c r="AL51" s="324"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -13978,14 +13977,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="329"/>
-      <c r="AD55" s="329"/>
-      <c r="AI55" s="326" t="s">
+      <c r="AC55" s="328"/>
+      <c r="AD55" s="328"/>
+      <c r="AI55" s="325" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="327"/>
-      <c r="AK55" s="327"/>
-      <c r="AL55" s="328"/>
+      <c r="AJ55" s="326"/>
+      <c r="AK55" s="326"/>
+      <c r="AL55" s="327"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -14048,12 +14047,12 @@
         <v>NO</v>
       </c>
       <c r="V56" s="2"/>
-      <c r="AI56" s="308" t="s">
+      <c r="AI56" s="307" t="s">
         <v>168</v>
       </c>
-      <c r="AJ56" s="308"/>
-      <c r="AK56" s="308"/>
-      <c r="AL56" s="308"/>
+      <c r="AJ56" s="307"/>
+      <c r="AK56" s="307"/>
+      <c r="AL56" s="307"/>
       <c r="AM56" s="52">
         <f>AM50-AM55</f>
         <v>450000</v>
@@ -14302,32 +14301,32 @@
     <row r="67" spans="3:19" s="256" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="309" t="s">
+      <c r="C69" s="308" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="310"/>
-      <c r="E69" s="310"/>
-      <c r="F69" s="310"/>
-      <c r="G69" s="311"/>
-      <c r="I69" s="315" t="s">
+      <c r="D69" s="309"/>
+      <c r="E69" s="309"/>
+      <c r="F69" s="309"/>
+      <c r="G69" s="310"/>
+      <c r="I69" s="314" t="s">
         <v>178</v>
       </c>
-      <c r="J69" s="315"/>
-      <c r="K69" s="315"/>
-      <c r="L69" s="315"/>
-      <c r="M69" s="315"/>
+      <c r="J69" s="314"/>
+      <c r="K69" s="314"/>
+      <c r="L69" s="314"/>
+      <c r="M69" s="314"/>
     </row>
     <row r="70" spans="3:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="312"/>
-      <c r="D70" s="313"/>
-      <c r="E70" s="313"/>
-      <c r="F70" s="313"/>
-      <c r="G70" s="314"/>
-      <c r="I70" s="315"/>
-      <c r="J70" s="315"/>
-      <c r="K70" s="315"/>
-      <c r="L70" s="315"/>
-      <c r="M70" s="315"/>
+      <c r="C70" s="311"/>
+      <c r="D70" s="312"/>
+      <c r="E70" s="312"/>
+      <c r="F70" s="312"/>
+      <c r="G70" s="313"/>
+      <c r="I70" s="314"/>
+      <c r="J70" s="314"/>
+      <c r="K70" s="314"/>
+      <c r="L70" s="314"/>
+      <c r="M70" s="314"/>
     </row>
     <row r="71" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14348,10 +14347,10 @@
       <c r="M76" s="55"/>
       <c r="N76" s="55"/>
       <c r="O76" s="55"/>
-      <c r="P76" s="308" t="s">
+      <c r="P76" s="307" t="s">
         <v>214</v>
       </c>
-      <c r="Q76" s="308"/>
+      <c r="Q76" s="307"/>
       <c r="R76" s="55"/>
       <c r="S76" s="55"/>
     </row>
@@ -14923,86 +14922,86 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="330" t="s">
+      <c r="A2" s="329" t="s">
         <v>300</v>
       </c>
-      <c r="B2" s="330"/>
-      <c r="C2" s="330"/>
-      <c r="D2" s="330"/>
-      <c r="E2" s="330"/>
-      <c r="F2" s="330"/>
-      <c r="G2" s="330"/>
-      <c r="H2" s="330"/>
-      <c r="I2" s="330"/>
-      <c r="J2" s="330"/>
-      <c r="K2" s="330"/>
-      <c r="L2" s="330"/>
+      <c r="B2" s="329"/>
+      <c r="C2" s="329"/>
+      <c r="D2" s="329"/>
+      <c r="E2" s="329"/>
+      <c r="F2" s="329"/>
+      <c r="G2" s="329"/>
+      <c r="H2" s="329"/>
+      <c r="I2" s="329"/>
+      <c r="J2" s="329"/>
+      <c r="K2" s="329"/>
+      <c r="L2" s="329"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="330"/>
-      <c r="B3" s="330"/>
-      <c r="C3" s="330"/>
-      <c r="D3" s="330"/>
-      <c r="E3" s="330"/>
-      <c r="F3" s="330"/>
-      <c r="G3" s="330"/>
-      <c r="H3" s="330"/>
-      <c r="I3" s="330"/>
-      <c r="J3" s="330"/>
-      <c r="K3" s="330"/>
-      <c r="L3" s="330"/>
+      <c r="A3" s="329"/>
+      <c r="B3" s="329"/>
+      <c r="C3" s="329"/>
+      <c r="D3" s="329"/>
+      <c r="E3" s="329"/>
+      <c r="F3" s="329"/>
+      <c r="G3" s="329"/>
+      <c r="H3" s="329"/>
+      <c r="I3" s="329"/>
+      <c r="J3" s="329"/>
+      <c r="K3" s="329"/>
+      <c r="L3" s="329"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="315" t="s">
+      <c r="A5" s="314" t="s">
         <v>303</v>
       </c>
-      <c r="B5" s="315"/>
-      <c r="C5" s="315"/>
-      <c r="D5" s="315"/>
-      <c r="E5" s="315"/>
-      <c r="F5" s="315"/>
-      <c r="G5" s="315"/>
-      <c r="H5" s="315"/>
-      <c r="I5" s="315"/>
-      <c r="J5" s="315"/>
-      <c r="K5" s="315"/>
-      <c r="M5" s="315" t="s">
+      <c r="B5" s="314"/>
+      <c r="C5" s="314"/>
+      <c r="D5" s="314"/>
+      <c r="E5" s="314"/>
+      <c r="F5" s="314"/>
+      <c r="G5" s="314"/>
+      <c r="H5" s="314"/>
+      <c r="I5" s="314"/>
+      <c r="J5" s="314"/>
+      <c r="K5" s="314"/>
+      <c r="M5" s="314" t="s">
         <v>324</v>
       </c>
-      <c r="N5" s="315"/>
-      <c r="O5" s="315"/>
-      <c r="P5" s="315"/>
-      <c r="Q5" s="315"/>
-      <c r="R5" s="315"/>
-      <c r="S5" s="315"/>
-      <c r="T5" s="315"/>
-      <c r="U5" s="315"/>
-      <c r="V5" s="315"/>
-      <c r="W5" s="315"/>
+      <c r="N5" s="314"/>
+      <c r="O5" s="314"/>
+      <c r="P5" s="314"/>
+      <c r="Q5" s="314"/>
+      <c r="R5" s="314"/>
+      <c r="S5" s="314"/>
+      <c r="T5" s="314"/>
+      <c r="U5" s="314"/>
+      <c r="V5" s="314"/>
+      <c r="W5" s="314"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="315"/>
-      <c r="B6" s="315"/>
-      <c r="C6" s="315"/>
-      <c r="D6" s="315"/>
-      <c r="E6" s="315"/>
-      <c r="F6" s="315"/>
-      <c r="G6" s="315"/>
-      <c r="H6" s="315"/>
-      <c r="I6" s="315"/>
-      <c r="J6" s="315"/>
-      <c r="K6" s="315"/>
-      <c r="M6" s="315"/>
-      <c r="N6" s="315"/>
-      <c r="O6" s="315"/>
-      <c r="P6" s="315"/>
-      <c r="Q6" s="315"/>
-      <c r="R6" s="315"/>
-      <c r="S6" s="315"/>
-      <c r="T6" s="315"/>
-      <c r="U6" s="315"/>
-      <c r="V6" s="315"/>
-      <c r="W6" s="315"/>
+      <c r="A6" s="314"/>
+      <c r="B6" s="314"/>
+      <c r="C6" s="314"/>
+      <c r="D6" s="314"/>
+      <c r="E6" s="314"/>
+      <c r="F6" s="314"/>
+      <c r="G6" s="314"/>
+      <c r="H6" s="314"/>
+      <c r="I6" s="314"/>
+      <c r="J6" s="314"/>
+      <c r="K6" s="314"/>
+      <c r="M6" s="314"/>
+      <c r="N6" s="314"/>
+      <c r="O6" s="314"/>
+      <c r="P6" s="314"/>
+      <c r="Q6" s="314"/>
+      <c r="R6" s="314"/>
+      <c r="S6" s="314"/>
+      <c r="T6" s="314"/>
+      <c r="U6" s="314"/>
+      <c r="V6" s="314"/>
+      <c r="W6" s="314"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M7" s="249"/>
@@ -15715,7 +15714,7 @@
       <c r="N27" s="1">
         <v>19</v>
       </c>
-      <c r="O27" s="280" t="s">
+      <c r="O27" s="279" t="s">
         <v>123</v>
       </c>
       <c r="P27" s="1" t="s">
@@ -15743,7 +15742,7 @@
       <c r="N28" s="1">
         <v>20</v>
       </c>
-      <c r="O28" s="276"/>
+      <c r="O28" s="275"/>
       <c r="P28" s="274"/>
       <c r="Q28" s="210"/>
       <c r="R28" s="210"/>
@@ -15891,7 +15890,7 @@
       </c>
       <c r="M34" s="249"/>
       <c r="N34" s="194"/>
-      <c r="O34" s="277" t="s">
+      <c r="O34" s="276" t="s">
         <v>359</v>
       </c>
       <c r="P34" s="222" t="s">
@@ -15912,27 +15911,27 @@
       <c r="W34" s="249"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B35" s="335" t="s">
+      <c r="B35" s="334" t="s">
         <v>312</v>
       </c>
-      <c r="C35" s="336"/>
-      <c r="D35" s="337"/>
-      <c r="E35" s="331">
+      <c r="C35" s="335"/>
+      <c r="D35" s="336"/>
+      <c r="E35" s="330">
         <f>E34-F34</f>
         <v>2610871.1799999997</v>
       </c>
-      <c r="F35" s="332"/>
+      <c r="F35" s="331"/>
       <c r="M35" s="249"/>
-      <c r="N35" s="335" t="s">
+      <c r="N35" s="334" t="s">
         <v>312</v>
       </c>
-      <c r="O35" s="336"/>
-      <c r="P35" s="337"/>
-      <c r="Q35" s="331">
+      <c r="O35" s="335"/>
+      <c r="P35" s="336"/>
+      <c r="Q35" s="330">
         <f>Q34-R34</f>
         <v>1506144.27</v>
       </c>
-      <c r="R35" s="332"/>
+      <c r="R35" s="331"/>
       <c r="S35" s="249"/>
       <c r="T35" s="249"/>
       <c r="U35" s="249"/>
@@ -15940,17 +15939,17 @@
       <c r="W35" s="249"/>
     </row>
     <row r="36" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="338"/>
-      <c r="C36" s="339"/>
-      <c r="D36" s="340"/>
-      <c r="E36" s="333"/>
-      <c r="F36" s="334"/>
+      <c r="B36" s="337"/>
+      <c r="C36" s="338"/>
+      <c r="D36" s="339"/>
+      <c r="E36" s="332"/>
+      <c r="F36" s="333"/>
       <c r="M36" s="249"/>
-      <c r="N36" s="338"/>
-      <c r="O36" s="339"/>
-      <c r="P36" s="340"/>
-      <c r="Q36" s="333"/>
-      <c r="R36" s="334"/>
+      <c r="N36" s="337"/>
+      <c r="O36" s="338"/>
+      <c r="P36" s="339"/>
+      <c r="Q36" s="332"/>
+      <c r="R36" s="333"/>
       <c r="S36" s="249"/>
       <c r="T36" s="249"/>
       <c r="U36" s="249"/>
@@ -15976,8 +15975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:P75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15986,7 +15985,7 @@
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" style="281" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="280" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
     <col min="10" max="10" width="17.140625" customWidth="1"/>
@@ -15994,28 +15993,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="275" t="s">
+      <c r="E3" s="133" t="s">
         <v>350</v>
       </c>
       <c r="F3" s="284" t="s">
         <v>378</v>
       </c>
-      <c r="G3" s="57" t="s">
+      <c r="G3" s="1" t="s">
         <v>180</v>
       </c>
       <c r="J3" s="59" t="s">
         <v>373</v>
       </c>
-      <c r="K3" s="286" t="s">
+      <c r="K3" s="285" t="s">
         <v>374</v>
       </c>
     </row>
@@ -16682,64 +16681,64 @@
       </c>
     </row>
     <row r="40" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="343" t="s">
+      <c r="B40" s="342" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="344"/>
-      <c r="D40" s="344"/>
-      <c r="E40" s="344"/>
-      <c r="F40" s="345"/>
-      <c r="G40" s="287">
+      <c r="C40" s="343"/>
+      <c r="D40" s="343"/>
+      <c r="E40" s="343"/>
+      <c r="F40" s="344"/>
+      <c r="G40" s="286">
         <f>SUM(G4:G39)</f>
         <v>2750000</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="315" t="s">
+      <c r="B44" s="314" t="s">
         <v>366</v>
       </c>
-      <c r="C44" s="315"/>
-      <c r="D44" s="315"/>
-      <c r="E44" s="315"/>
-      <c r="F44" s="315"/>
-      <c r="G44" s="315"/>
-      <c r="H44" s="315"/>
-      <c r="I44" s="315"/>
-      <c r="J44" s="315"/>
-      <c r="K44" s="315"/>
-      <c r="L44" s="315"/>
-      <c r="M44" s="315"/>
+      <c r="C44" s="314"/>
+      <c r="D44" s="314"/>
+      <c r="E44" s="314"/>
+      <c r="F44" s="314"/>
+      <c r="G44" s="314"/>
+      <c r="H44" s="314"/>
+      <c r="I44" s="314"/>
+      <c r="J44" s="314"/>
+      <c r="K44" s="314"/>
+      <c r="L44" s="314"/>
+      <c r="M44" s="314"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="315"/>
-      <c r="C45" s="315"/>
-      <c r="D45" s="315"/>
-      <c r="E45" s="315"/>
-      <c r="F45" s="315"/>
-      <c r="G45" s="315"/>
-      <c r="H45" s="315"/>
-      <c r="I45" s="315"/>
-      <c r="J45" s="315"/>
-      <c r="K45" s="315"/>
-      <c r="L45" s="315"/>
-      <c r="M45" s="315"/>
+      <c r="B45" s="314"/>
+      <c r="C45" s="314"/>
+      <c r="D45" s="314"/>
+      <c r="E45" s="314"/>
+      <c r="F45" s="314"/>
+      <c r="G45" s="314"/>
+      <c r="H45" s="314"/>
+      <c r="I45" s="314"/>
+      <c r="J45" s="314"/>
+      <c r="K45" s="314"/>
+      <c r="L45" s="314"/>
+      <c r="M45" s="314"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B46" s="278"/>
+      <c r="B46" s="277"/>
       <c r="C46" s="203"/>
       <c r="D46" s="214"/>
       <c r="E46" s="203"/>
       <c r="F46" s="203"/>
-      <c r="G46" s="278"/>
+      <c r="G46" s="277"/>
       <c r="H46" s="215"/>
-      <c r="I46" s="278"/>
-      <c r="J46" s="278"/>
-      <c r="K46" s="278"/>
-      <c r="L46" s="278"/>
-      <c r="M46" s="278"/>
+      <c r="I46" s="277"/>
+      <c r="J46" s="277"/>
+      <c r="K46" s="277"/>
+      <c r="L46" s="277"/>
+      <c r="M46" s="277"/>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="278"/>
+      <c r="B47" s="277"/>
       <c r="C47" s="1" t="s">
         <v>1</v>
       </c>
@@ -16756,23 +16755,23 @@
       <c r="H47" s="218" t="s">
         <v>65</v>
       </c>
-      <c r="I47" s="278"/>
-      <c r="J47" s="341" t="s">
+      <c r="I47" s="277"/>
+      <c r="J47" s="340" t="s">
         <v>368</v>
       </c>
-      <c r="K47" s="342"/>
-      <c r="L47" s="342"/>
-      <c r="M47" s="342"/>
-      <c r="N47" s="342"/>
-      <c r="O47" s="342"/>
-      <c r="P47" s="342"/>
+      <c r="K47" s="341"/>
+      <c r="L47" s="341"/>
+      <c r="M47" s="341"/>
+      <c r="N47" s="341"/>
+      <c r="O47" s="341"/>
+      <c r="P47" s="341"/>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B48" s="278"/>
+      <c r="B48" s="277"/>
       <c r="C48" s="1">
         <v>1</v>
       </c>
-      <c r="D48" s="280" t="s">
+      <c r="D48" s="279" t="s">
         <v>123</v>
       </c>
       <c r="E48" s="1" t="s">
@@ -16783,17 +16782,17 @@
         <v>2000000</v>
       </c>
       <c r="H48" s="211"/>
-      <c r="I48" s="278"/>
-      <c r="J48" s="342"/>
-      <c r="K48" s="342"/>
-      <c r="L48" s="342"/>
-      <c r="M48" s="342"/>
-      <c r="N48" s="342"/>
-      <c r="O48" s="342"/>
-      <c r="P48" s="342"/>
+      <c r="I48" s="277"/>
+      <c r="J48" s="341"/>
+      <c r="K48" s="341"/>
+      <c r="L48" s="341"/>
+      <c r="M48" s="341"/>
+      <c r="N48" s="341"/>
+      <c r="O48" s="341"/>
+      <c r="P48" s="341"/>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B49" s="278"/>
+      <c r="B49" s="277"/>
       <c r="C49" s="1">
         <v>2</v>
       </c>
@@ -16808,43 +16807,43 @@
       <c r="H49" s="210">
         <v>500000</v>
       </c>
-      <c r="I49" s="278"/>
-      <c r="J49" s="342"/>
-      <c r="K49" s="342"/>
-      <c r="L49" s="342"/>
-      <c r="M49" s="342"/>
-      <c r="N49" s="342"/>
-      <c r="O49" s="342"/>
-      <c r="P49" s="342"/>
+      <c r="I49" s="277"/>
+      <c r="J49" s="341"/>
+      <c r="K49" s="341"/>
+      <c r="L49" s="341"/>
+      <c r="M49" s="341"/>
+      <c r="N49" s="341"/>
+      <c r="O49" s="341"/>
+      <c r="P49" s="341"/>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B50" s="278"/>
+      <c r="B50" s="277"/>
       <c r="C50" s="1">
         <v>3</v>
       </c>
-      <c r="D50" s="276" t="s">
+      <c r="D50" s="275" t="s">
         <v>123</v>
       </c>
-      <c r="E50" s="279" t="s">
+      <c r="E50" s="278" t="s">
         <v>358</v>
       </c>
-      <c r="F50" s="285"/>
+      <c r="F50" s="283"/>
       <c r="G50" s="210">
         <f>G40</f>
         <v>2750000</v>
       </c>
       <c r="H50" s="210"/>
-      <c r="I50" s="278"/>
-      <c r="J50" s="342"/>
-      <c r="K50" s="342"/>
-      <c r="L50" s="342"/>
-      <c r="M50" s="342"/>
-      <c r="N50" s="342"/>
-      <c r="O50" s="342"/>
-      <c r="P50" s="342"/>
+      <c r="I50" s="277"/>
+      <c r="J50" s="341"/>
+      <c r="K50" s="341"/>
+      <c r="L50" s="341"/>
+      <c r="M50" s="341"/>
+      <c r="N50" s="341"/>
+      <c r="O50" s="341"/>
+      <c r="P50" s="341"/>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B51" s="278"/>
+      <c r="B51" s="277"/>
       <c r="C51" s="1">
         <v>4</v>
       </c>
@@ -16853,17 +16852,17 @@
       <c r="F51" s="66"/>
       <c r="G51" s="210"/>
       <c r="H51" s="211"/>
-      <c r="I51" s="278"/>
-      <c r="J51" s="342"/>
-      <c r="K51" s="342"/>
-      <c r="L51" s="342"/>
-      <c r="M51" s="342"/>
-      <c r="N51" s="342"/>
-      <c r="O51" s="342"/>
-      <c r="P51" s="342"/>
+      <c r="I51" s="277"/>
+      <c r="J51" s="341"/>
+      <c r="K51" s="341"/>
+      <c r="L51" s="341"/>
+      <c r="M51" s="341"/>
+      <c r="N51" s="341"/>
+      <c r="O51" s="341"/>
+      <c r="P51" s="341"/>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B52" s="278"/>
+      <c r="B52" s="277"/>
       <c r="C52" s="1">
         <v>5</v>
       </c>
@@ -16872,17 +16871,17 @@
       <c r="F52" s="66"/>
       <c r="G52" s="252"/>
       <c r="H52" s="211"/>
-      <c r="I52" s="278"/>
-      <c r="J52" s="342"/>
-      <c r="K52" s="342"/>
-      <c r="L52" s="342"/>
-      <c r="M52" s="342"/>
-      <c r="N52" s="342"/>
-      <c r="O52" s="342"/>
-      <c r="P52" s="342"/>
+      <c r="I52" s="277"/>
+      <c r="J52" s="341"/>
+      <c r="K52" s="341"/>
+      <c r="L52" s="341"/>
+      <c r="M52" s="341"/>
+      <c r="N52" s="341"/>
+      <c r="O52" s="341"/>
+      <c r="P52" s="341"/>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B53" s="278"/>
+      <c r="B53" s="277"/>
       <c r="C53" s="1">
         <v>6</v>
       </c>
@@ -16891,33 +16890,33 @@
       <c r="F53" s="1"/>
       <c r="G53" s="210"/>
       <c r="H53" s="211"/>
-      <c r="I53" s="278"/>
-      <c r="J53" s="342"/>
-      <c r="K53" s="342"/>
-      <c r="L53" s="342"/>
-      <c r="M53" s="342"/>
-      <c r="N53" s="342"/>
-      <c r="O53" s="342"/>
-      <c r="P53" s="342"/>
+      <c r="I53" s="277"/>
+      <c r="J53" s="341"/>
+      <c r="K53" s="341"/>
+      <c r="L53" s="341"/>
+      <c r="M53" s="341"/>
+      <c r="N53" s="341"/>
+      <c r="O53" s="341"/>
+      <c r="P53" s="341"/>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="278"/>
+      <c r="B54" s="277"/>
       <c r="C54" s="1">
         <v>7</v>
       </c>
       <c r="D54" s="216"/>
-      <c r="E54" s="279"/>
-      <c r="F54" s="285"/>
+      <c r="E54" s="278"/>
+      <c r="F54" s="283"/>
       <c r="G54" s="210"/>
       <c r="H54" s="211"/>
-      <c r="I54" s="278"/>
-      <c r="J54" s="278"/>
-      <c r="K54" s="278"/>
-      <c r="L54" s="278"/>
-      <c r="M54" s="278"/>
+      <c r="I54" s="277"/>
+      <c r="J54" s="277"/>
+      <c r="K54" s="277"/>
+      <c r="L54" s="277"/>
+      <c r="M54" s="277"/>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="278"/>
+      <c r="B55" s="277"/>
       <c r="C55" s="1">
         <v>8</v>
       </c>
@@ -16926,14 +16925,14 @@
       <c r="F55" s="1"/>
       <c r="G55" s="211"/>
       <c r="H55" s="210"/>
-      <c r="I55" s="278"/>
-      <c r="J55" s="278"/>
-      <c r="K55" s="278"/>
-      <c r="L55" s="278"/>
-      <c r="M55" s="278"/>
+      <c r="I55" s="277"/>
+      <c r="J55" s="277"/>
+      <c r="K55" s="277"/>
+      <c r="L55" s="277"/>
+      <c r="M55" s="277"/>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B56" s="278"/>
+      <c r="B56" s="277"/>
       <c r="C56" s="1">
         <v>9</v>
       </c>
@@ -16942,94 +16941,94 @@
       <c r="F56" s="1"/>
       <c r="G56" s="210"/>
       <c r="H56" s="211"/>
-      <c r="I56" s="278"/>
-      <c r="J56" s="278"/>
-      <c r="K56" s="278"/>
-      <c r="L56" s="278"/>
-      <c r="M56" s="278"/>
+      <c r="I56" s="277"/>
+      <c r="J56" s="277"/>
+      <c r="K56" s="277"/>
+      <c r="L56" s="277"/>
+      <c r="M56" s="277"/>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B57" s="278"/>
+      <c r="B57" s="277"/>
       <c r="C57" s="1">
         <v>10</v>
       </c>
       <c r="D57" s="216"/>
-      <c r="E57" s="279"/>
-      <c r="F57" s="285"/>
+      <c r="E57" s="278"/>
+      <c r="F57" s="283"/>
       <c r="G57" s="211"/>
       <c r="H57" s="210"/>
-      <c r="I57" s="278"/>
-      <c r="J57" s="278"/>
-      <c r="K57" s="278"/>
-      <c r="L57" s="278"/>
-      <c r="M57" s="278"/>
+      <c r="I57" s="277"/>
+      <c r="J57" s="277"/>
+      <c r="K57" s="277"/>
+      <c r="L57" s="277"/>
+      <c r="M57" s="277"/>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B58" s="278"/>
+      <c r="B58" s="277"/>
       <c r="C58" s="1">
         <v>11</v>
       </c>
       <c r="D58" s="216"/>
-      <c r="E58" s="279"/>
-      <c r="F58" s="285"/>
+      <c r="E58" s="278"/>
+      <c r="F58" s="283"/>
       <c r="G58" s="211"/>
       <c r="H58" s="211"/>
-      <c r="I58" s="278"/>
-      <c r="J58" s="278"/>
-      <c r="K58" s="278"/>
-      <c r="L58" s="278"/>
-      <c r="M58" s="278"/>
+      <c r="I58" s="277"/>
+      <c r="J58" s="277"/>
+      <c r="K58" s="277"/>
+      <c r="L58" s="277"/>
+      <c r="M58" s="277"/>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B59" s="278"/>
+      <c r="B59" s="277"/>
       <c r="C59" s="1">
         <v>12</v>
       </c>
       <c r="D59" s="216"/>
-      <c r="E59" s="279"/>
-      <c r="F59" s="285"/>
+      <c r="E59" s="278"/>
+      <c r="F59" s="283"/>
       <c r="G59" s="210"/>
       <c r="H59" s="211"/>
-      <c r="I59" s="278"/>
-      <c r="J59" s="278"/>
-      <c r="K59" s="278"/>
-      <c r="L59" s="278"/>
-      <c r="M59" s="278"/>
+      <c r="I59" s="277"/>
+      <c r="J59" s="277"/>
+      <c r="K59" s="277"/>
+      <c r="L59" s="277"/>
+      <c r="M59" s="277"/>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B60" s="278"/>
+      <c r="B60" s="277"/>
       <c r="C60" s="1">
         <v>13</v>
       </c>
       <c r="D60" s="216"/>
-      <c r="E60" s="279"/>
-      <c r="F60" s="285"/>
+      <c r="E60" s="278"/>
+      <c r="F60" s="283"/>
       <c r="G60" s="211"/>
       <c r="H60" s="210"/>
-      <c r="I60" s="278"/>
-      <c r="J60" s="278"/>
-      <c r="K60" s="278"/>
-      <c r="L60" s="278"/>
-      <c r="M60" s="278"/>
+      <c r="I60" s="277"/>
+      <c r="J60" s="277"/>
+      <c r="K60" s="277"/>
+      <c r="L60" s="277"/>
+      <c r="M60" s="277"/>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B61" s="278"/>
+      <c r="B61" s="277"/>
       <c r="C61" s="1">
         <v>14</v>
       </c>
       <c r="D61" s="216"/>
-      <c r="E61" s="279"/>
-      <c r="F61" s="285"/>
+      <c r="E61" s="278"/>
+      <c r="F61" s="283"/>
       <c r="G61" s="211"/>
       <c r="H61" s="211"/>
-      <c r="I61" s="278"/>
-      <c r="J61" s="278"/>
-      <c r="K61" s="278"/>
-      <c r="L61" s="278"/>
-      <c r="M61" s="278"/>
+      <c r="I61" s="277"/>
+      <c r="J61" s="277"/>
+      <c r="K61" s="277"/>
+      <c r="L61" s="277"/>
+      <c r="M61" s="277"/>
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B62" s="278"/>
+      <c r="B62" s="277"/>
       <c r="C62" s="1">
         <v>15</v>
       </c>
@@ -17038,46 +17037,46 @@
       <c r="F62" s="1"/>
       <c r="G62" s="210"/>
       <c r="H62" s="211"/>
-      <c r="I62" s="278"/>
-      <c r="J62" s="278"/>
-      <c r="K62" s="278"/>
-      <c r="L62" s="278"/>
-      <c r="M62" s="278"/>
+      <c r="I62" s="277"/>
+      <c r="J62" s="277"/>
+      <c r="K62" s="277"/>
+      <c r="L62" s="277"/>
+      <c r="M62" s="277"/>
     </row>
     <row r="63" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B63" s="278"/>
+      <c r="B63" s="277"/>
       <c r="C63" s="1">
         <v>16</v>
       </c>
       <c r="D63" s="216"/>
-      <c r="E63" s="279"/>
-      <c r="F63" s="285"/>
+      <c r="E63" s="278"/>
+      <c r="F63" s="283"/>
       <c r="G63" s="211"/>
       <c r="H63" s="210"/>
-      <c r="I63" s="278"/>
-      <c r="J63" s="278"/>
-      <c r="K63" s="278"/>
-      <c r="L63" s="278"/>
-      <c r="M63" s="278"/>
+      <c r="I63" s="277"/>
+      <c r="J63" s="277"/>
+      <c r="K63" s="277"/>
+      <c r="L63" s="277"/>
+      <c r="M63" s="277"/>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B64" s="278"/>
+      <c r="B64" s="277"/>
       <c r="C64" s="1">
         <v>17</v>
       </c>
       <c r="D64" s="216"/>
-      <c r="E64" s="279"/>
-      <c r="F64" s="285"/>
+      <c r="E64" s="278"/>
+      <c r="F64" s="283"/>
       <c r="G64" s="210"/>
       <c r="H64" s="210"/>
-      <c r="I64" s="278"/>
-      <c r="J64" s="278"/>
-      <c r="K64" s="278"/>
-      <c r="L64" s="278"/>
-      <c r="M64" s="278"/>
+      <c r="I64" s="277"/>
+      <c r="J64" s="277"/>
+      <c r="K64" s="277"/>
+      <c r="L64" s="277"/>
+      <c r="M64" s="277"/>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B65" s="278"/>
+      <c r="B65" s="277"/>
       <c r="C65" s="1">
         <v>18</v>
       </c>
@@ -17086,14 +17085,14 @@
       <c r="F65" s="1"/>
       <c r="G65" s="210"/>
       <c r="H65" s="210"/>
-      <c r="I65" s="278"/>
-      <c r="J65" s="278"/>
-      <c r="K65" s="278"/>
-      <c r="L65" s="278"/>
-      <c r="M65" s="278"/>
+      <c r="I65" s="277"/>
+      <c r="J65" s="277"/>
+      <c r="K65" s="277"/>
+      <c r="L65" s="277"/>
+      <c r="M65" s="277"/>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="278"/>
+      <c r="B66" s="277"/>
       <c r="C66" s="1">
         <v>19</v>
       </c>
@@ -17102,30 +17101,30 @@
       <c r="F66" s="1"/>
       <c r="G66" s="210"/>
       <c r="H66" s="210"/>
-      <c r="I66" s="278"/>
-      <c r="J66" s="278"/>
-      <c r="K66" s="278"/>
-      <c r="L66" s="278"/>
-      <c r="M66" s="278"/>
+      <c r="I66" s="277"/>
+      <c r="J66" s="277"/>
+      <c r="K66" s="277"/>
+      <c r="L66" s="277"/>
+      <c r="M66" s="277"/>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B67" s="278"/>
+      <c r="B67" s="277"/>
       <c r="C67" s="1">
         <v>20</v>
       </c>
-      <c r="D67" s="276"/>
-      <c r="E67" s="279"/>
-      <c r="F67" s="285"/>
+      <c r="D67" s="275"/>
+      <c r="E67" s="278"/>
+      <c r="F67" s="283"/>
       <c r="G67" s="210"/>
       <c r="H67" s="210"/>
-      <c r="I67" s="278"/>
-      <c r="J67" s="278"/>
-      <c r="K67" s="278"/>
-      <c r="L67" s="278"/>
-      <c r="M67" s="278"/>
+      <c r="I67" s="277"/>
+      <c r="J67" s="277"/>
+      <c r="K67" s="277"/>
+      <c r="L67" s="277"/>
+      <c r="M67" s="277"/>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B68" s="278"/>
+      <c r="B68" s="277"/>
       <c r="C68" s="1">
         <v>21</v>
       </c>
@@ -17134,14 +17133,14 @@
       <c r="F68" s="1"/>
       <c r="G68" s="210"/>
       <c r="H68" s="210"/>
-      <c r="I68" s="278"/>
-      <c r="J68" s="278"/>
-      <c r="K68" s="278"/>
-      <c r="L68" s="278"/>
-      <c r="M68" s="278"/>
+      <c r="I68" s="277"/>
+      <c r="J68" s="277"/>
+      <c r="K68" s="277"/>
+      <c r="L68" s="277"/>
+      <c r="M68" s="277"/>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B69" s="278"/>
+      <c r="B69" s="277"/>
       <c r="C69" s="1">
         <v>22</v>
       </c>
@@ -17150,14 +17149,14 @@
       <c r="F69" s="1"/>
       <c r="G69" s="210"/>
       <c r="H69" s="210"/>
-      <c r="I69" s="278"/>
-      <c r="J69" s="278"/>
-      <c r="K69" s="278"/>
-      <c r="L69" s="278"/>
-      <c r="M69" s="278"/>
+      <c r="I69" s="277"/>
+      <c r="J69" s="277"/>
+      <c r="K69" s="277"/>
+      <c r="L69" s="277"/>
+      <c r="M69" s="277"/>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B70" s="278"/>
+      <c r="B70" s="277"/>
       <c r="C70" s="1">
         <v>23</v>
       </c>
@@ -17166,14 +17165,14 @@
       <c r="F70" s="1"/>
       <c r="G70" s="210"/>
       <c r="H70" s="210"/>
-      <c r="I70" s="278"/>
-      <c r="J70" s="278"/>
-      <c r="K70" s="278"/>
-      <c r="L70" s="278"/>
-      <c r="M70" s="278"/>
+      <c r="I70" s="277"/>
+      <c r="J70" s="277"/>
+      <c r="K70" s="277"/>
+      <c r="L70" s="277"/>
+      <c r="M70" s="277"/>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B71" s="278"/>
+      <c r="B71" s="277"/>
       <c r="C71" s="1">
         <v>24</v>
       </c>
@@ -17182,36 +17181,36 @@
       <c r="F71" s="1"/>
       <c r="G71" s="56"/>
       <c r="H71" s="56"/>
-      <c r="I71" s="278"/>
-      <c r="J71" s="278"/>
-      <c r="K71" s="278"/>
-      <c r="L71" s="278"/>
-      <c r="M71" s="278"/>
+      <c r="I71" s="277"/>
+      <c r="J71" s="277"/>
+      <c r="K71" s="277"/>
+      <c r="L71" s="277"/>
+      <c r="M71" s="277"/>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B72" s="278"/>
+      <c r="B72" s="277"/>
       <c r="C72" s="1">
         <v>25</v>
       </c>
       <c r="D72" s="209" t="s">
         <v>359</v>
       </c>
-      <c r="E72" s="279" t="s">
+      <c r="E72" s="278" t="s">
         <v>299</v>
       </c>
-      <c r="F72" s="285"/>
+      <c r="F72" s="283"/>
       <c r="G72" s="56"/>
       <c r="H72" s="56"/>
-      <c r="I72" s="278"/>
-      <c r="J72" s="278"/>
-      <c r="K72" s="278"/>
-      <c r="L72" s="278"/>
-      <c r="M72" s="278"/>
+      <c r="I72" s="277"/>
+      <c r="J72" s="277"/>
+      <c r="K72" s="277"/>
+      <c r="L72" s="277"/>
+      <c r="M72" s="277"/>
     </row>
     <row r="73" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="278"/>
+      <c r="B73" s="277"/>
       <c r="C73" s="194"/>
-      <c r="D73" s="277" t="s">
+      <c r="D73" s="276" t="s">
         <v>359</v>
       </c>
       <c r="E73" s="222"/>
@@ -17224,44 +17223,44 @@
         <f>SUM(H48:H72)</f>
         <v>500000</v>
       </c>
-      <c r="I73" s="278"/>
-      <c r="J73" s="278"/>
-      <c r="K73" s="278"/>
-      <c r="L73" s="278"/>
-      <c r="M73" s="278"/>
+      <c r="I73" s="277"/>
+      <c r="J73" s="277"/>
+      <c r="K73" s="277"/>
+      <c r="L73" s="277"/>
+      <c r="M73" s="277"/>
     </row>
     <row r="74" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B74" s="278"/>
-      <c r="C74" s="335" t="s">
+      <c r="B74" s="277"/>
+      <c r="C74" s="334" t="s">
         <v>365</v>
       </c>
-      <c r="D74" s="336"/>
-      <c r="E74" s="337"/>
-      <c r="F74" s="282"/>
-      <c r="G74" s="331">
+      <c r="D74" s="335"/>
+      <c r="E74" s="336"/>
+      <c r="F74" s="281"/>
+      <c r="G74" s="330">
         <f>G73-H73</f>
         <v>4250000</v>
       </c>
-      <c r="H74" s="332"/>
-      <c r="I74" s="278"/>
-      <c r="J74" s="278"/>
-      <c r="K74" s="278"/>
-      <c r="L74" s="278"/>
-      <c r="M74" s="278"/>
+      <c r="H74" s="331"/>
+      <c r="I74" s="277"/>
+      <c r="J74" s="277"/>
+      <c r="K74" s="277"/>
+      <c r="L74" s="277"/>
+      <c r="M74" s="277"/>
     </row>
     <row r="75" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="278"/>
-      <c r="C75" s="338"/>
-      <c r="D75" s="339"/>
-      <c r="E75" s="340"/>
-      <c r="F75" s="283"/>
-      <c r="G75" s="333"/>
-      <c r="H75" s="334"/>
-      <c r="I75" s="278"/>
-      <c r="J75" s="278"/>
-      <c r="K75" s="278"/>
-      <c r="L75" s="278"/>
-      <c r="M75" s="278"/>
+      <c r="B75" s="277"/>
+      <c r="C75" s="337"/>
+      <c r="D75" s="338"/>
+      <c r="E75" s="339"/>
+      <c r="F75" s="282"/>
+      <c r="G75" s="332"/>
+      <c r="H75" s="333"/>
+      <c r="I75" s="277"/>
+      <c r="J75" s="277"/>
+      <c r="K75" s="277"/>
+      <c r="L75" s="277"/>
+      <c r="M75" s="277"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -17341,17 +17340,17 @@
       <c r="A2" s="172"/>
       <c r="B2" s="173"/>
       <c r="C2" s="173"/>
-      <c r="D2" s="403" t="s">
+      <c r="D2" s="402" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="403"/>
-      <c r="F2" s="403"/>
-      <c r="G2" s="403"/>
-      <c r="H2" s="403"/>
-      <c r="I2" s="403"/>
-      <c r="J2" s="403"/>
-      <c r="K2" s="403"/>
-      <c r="L2" s="403"/>
+      <c r="E2" s="402"/>
+      <c r="F2" s="402"/>
+      <c r="G2" s="402"/>
+      <c r="H2" s="402"/>
+      <c r="I2" s="402"/>
+      <c r="J2" s="402"/>
+      <c r="K2" s="402"/>
+      <c r="L2" s="402"/>
       <c r="M2" s="174"/>
       <c r="N2" s="24"/>
     </row>
@@ -17369,205 +17368,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="176"/>
-      <c r="U3" s="346" t="s">
+      <c r="U3" s="345" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="347"/>
-      <c r="W3" s="348" t="s">
+      <c r="V3" s="346"/>
+      <c r="W3" s="347" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="347"/>
-      <c r="Y3" s="347"/>
-      <c r="Z3" s="347"/>
-      <c r="AA3" s="347"/>
-      <c r="AB3" s="347"/>
-      <c r="AC3" s="347"/>
-      <c r="AD3" s="349"/>
+      <c r="X3" s="346"/>
+      <c r="Y3" s="346"/>
+      <c r="Z3" s="346"/>
+      <c r="AA3" s="346"/>
+      <c r="AB3" s="346"/>
+      <c r="AC3" s="346"/>
+      <c r="AD3" s="348"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="175"/>
-      <c r="B4" s="407" t="s">
+      <c r="B4" s="406" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="408"/>
-      <c r="D4" s="408"/>
-      <c r="E4" s="408"/>
-      <c r="F4" s="408"/>
+      <c r="C4" s="407"/>
+      <c r="D4" s="407"/>
+      <c r="E4" s="407"/>
+      <c r="F4" s="407"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="355" t="s">
+      <c r="I4" s="354" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="321"/>
-      <c r="K4" s="321"/>
-      <c r="L4" s="321"/>
+      <c r="J4" s="320"/>
+      <c r="K4" s="320"/>
+      <c r="L4" s="320"/>
       <c r="M4" s="176"/>
-      <c r="U4" s="367" t="s">
+      <c r="U4" s="366" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="321"/>
-      <c r="W4" s="355" t="s">
+      <c r="V4" s="320"/>
+      <c r="W4" s="354" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="321"/>
-      <c r="Y4" s="321"/>
-      <c r="Z4" s="321"/>
-      <c r="AA4" s="321"/>
-      <c r="AB4" s="321"/>
-      <c r="AC4" s="321"/>
-      <c r="AD4" s="350"/>
+      <c r="X4" s="320"/>
+      <c r="Y4" s="320"/>
+      <c r="Z4" s="320"/>
+      <c r="AA4" s="320"/>
+      <c r="AB4" s="320"/>
+      <c r="AC4" s="320"/>
+      <c r="AD4" s="349"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="175"/>
-      <c r="B5" s="372" t="s">
+      <c r="B5" s="371" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="321"/>
-      <c r="D5" s="321"/>
-      <c r="E5" s="321"/>
-      <c r="F5" s="321"/>
+      <c r="C5" s="320"/>
+      <c r="D5" s="320"/>
+      <c r="E5" s="320"/>
+      <c r="F5" s="320"/>
       <c r="G5" s="152">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="374" t="s">
+      <c r="I5" s="373" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="395"/>
-      <c r="K5" s="397">
+      <c r="J5" s="394"/>
+      <c r="K5" s="396">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="398"/>
+      <c r="L5" s="397"/>
       <c r="M5" s="176"/>
-      <c r="U5" s="368" t="s">
+      <c r="U5" s="367" t="s">
         <v>231</v>
       </c>
-      <c r="V5" s="369"/>
-      <c r="W5" s="374" t="s">
+      <c r="V5" s="368"/>
+      <c r="W5" s="373" t="s">
         <v>232</v>
       </c>
-      <c r="X5" s="375"/>
-      <c r="Y5" s="375"/>
-      <c r="Z5" s="375"/>
-      <c r="AA5" s="375"/>
-      <c r="AB5" s="375"/>
-      <c r="AC5" s="375"/>
-      <c r="AD5" s="376"/>
+      <c r="X5" s="374"/>
+      <c r="Y5" s="374"/>
+      <c r="Z5" s="374"/>
+      <c r="AA5" s="374"/>
+      <c r="AB5" s="374"/>
+      <c r="AC5" s="374"/>
+      <c r="AD5" s="375"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="175"/>
-      <c r="B6" s="365" t="s">
+      <c r="B6" s="364" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="366"/>
-      <c r="D6" s="366"/>
-      <c r="E6" s="366"/>
-      <c r="F6" s="366"/>
+      <c r="C6" s="365"/>
+      <c r="D6" s="365"/>
+      <c r="E6" s="365"/>
+      <c r="F6" s="365"/>
       <c r="G6" s="152">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="396" t="s">
+      <c r="I6" s="395" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="391"/>
-      <c r="K6" s="399">
+      <c r="J6" s="390"/>
+      <c r="K6" s="398">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="400"/>
+      <c r="L6" s="399"/>
       <c r="M6" s="176"/>
-      <c r="U6" s="370"/>
-      <c r="V6" s="371"/>
-      <c r="W6" s="356" t="s">
+      <c r="U6" s="369"/>
+      <c r="V6" s="370"/>
+      <c r="W6" s="355" t="s">
         <v>233</v>
       </c>
-      <c r="X6" s="357"/>
-      <c r="Y6" s="357"/>
-      <c r="Z6" s="357"/>
-      <c r="AA6" s="357"/>
-      <c r="AB6" s="357"/>
-      <c r="AC6" s="357"/>
-      <c r="AD6" s="358"/>
+      <c r="X6" s="356"/>
+      <c r="Y6" s="356"/>
+      <c r="Z6" s="356"/>
+      <c r="AA6" s="356"/>
+      <c r="AB6" s="356"/>
+      <c r="AC6" s="356"/>
+      <c r="AD6" s="357"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="175"/>
-      <c r="B7" s="377" t="s">
+      <c r="B7" s="376" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="378"/>
-      <c r="D7" s="378"/>
-      <c r="E7" s="378"/>
-      <c r="F7" s="391"/>
+      <c r="C7" s="377"/>
+      <c r="D7" s="377"/>
+      <c r="E7" s="377"/>
+      <c r="F7" s="390"/>
       <c r="G7" s="152">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="396" t="s">
+      <c r="I7" s="395" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="391"/>
-      <c r="K7" s="401">
+      <c r="J7" s="390"/>
+      <c r="K7" s="400">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="402"/>
+      <c r="L7" s="401"/>
       <c r="M7" s="176"/>
-      <c r="U7" s="353"/>
-      <c r="V7" s="354"/>
-      <c r="W7" s="355" t="s">
+      <c r="U7" s="352"/>
+      <c r="V7" s="353"/>
+      <c r="W7" s="354" t="s">
         <v>234</v>
       </c>
-      <c r="X7" s="321"/>
-      <c r="Y7" s="321"/>
-      <c r="Z7" s="321"/>
-      <c r="AA7" s="321"/>
-      <c r="AB7" s="321"/>
-      <c r="AC7" s="321"/>
-      <c r="AD7" s="350"/>
+      <c r="X7" s="320"/>
+      <c r="Y7" s="320"/>
+      <c r="Z7" s="320"/>
+      <c r="AA7" s="320"/>
+      <c r="AB7" s="320"/>
+      <c r="AC7" s="320"/>
+      <c r="AD7" s="349"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="175"/>
-      <c r="B8" s="405" t="s">
+      <c r="B8" s="404" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="406"/>
-      <c r="D8" s="406"/>
-      <c r="E8" s="406"/>
-      <c r="F8" s="406"/>
+      <c r="C8" s="405"/>
+      <c r="D8" s="405"/>
+      <c r="E8" s="405"/>
+      <c r="F8" s="405"/>
       <c r="G8" s="153">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="374" t="s">
+      <c r="I8" s="373" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="395"/>
-      <c r="K8" s="386">
+      <c r="J8" s="394"/>
+      <c r="K8" s="385">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="387"/>
+      <c r="L8" s="386"/>
       <c r="M8" s="176"/>
-      <c r="U8" s="361" t="s">
+      <c r="U8" s="360" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="362"/>
-      <c r="W8" s="356" t="s">
+      <c r="V8" s="361"/>
+      <c r="W8" s="355" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="357"/>
-      <c r="Y8" s="357"/>
-      <c r="Z8" s="357"/>
-      <c r="AA8" s="357"/>
-      <c r="AB8" s="357"/>
-      <c r="AC8" s="357"/>
-      <c r="AD8" s="358"/>
+      <c r="X8" s="356"/>
+      <c r="Y8" s="356"/>
+      <c r="Z8" s="356"/>
+      <c r="AA8" s="356"/>
+      <c r="AB8" s="356"/>
+      <c r="AC8" s="356"/>
+      <c r="AD8" s="357"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="175"/>
@@ -17583,28 +17582,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="176"/>
-      <c r="U9" s="363"/>
-      <c r="V9" s="364"/>
-      <c r="W9" s="356" t="s">
+      <c r="U9" s="362"/>
+      <c r="V9" s="363"/>
+      <c r="W9" s="355" t="s">
         <v>237</v>
       </c>
-      <c r="X9" s="357"/>
-      <c r="Y9" s="357"/>
-      <c r="Z9" s="357"/>
-      <c r="AA9" s="357"/>
-      <c r="AB9" s="357"/>
-      <c r="AC9" s="357"/>
-      <c r="AD9" s="358"/>
+      <c r="X9" s="356"/>
+      <c r="Y9" s="356"/>
+      <c r="Z9" s="356"/>
+      <c r="AA9" s="356"/>
+      <c r="AB9" s="356"/>
+      <c r="AC9" s="356"/>
+      <c r="AD9" s="357"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="175"/>
-      <c r="B10" s="321" t="s">
+      <c r="B10" s="320" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="321"/>
-      <c r="D10" s="321"/>
-      <c r="E10" s="321"/>
-      <c r="F10" s="321"/>
+      <c r="C10" s="320"/>
+      <c r="D10" s="320"/>
+      <c r="E10" s="320"/>
+      <c r="F10" s="320"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -17615,30 +17614,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="176"/>
-      <c r="U10" s="365" t="s">
+      <c r="U10" s="364" t="s">
         <v>243</v>
       </c>
-      <c r="V10" s="366"/>
-      <c r="W10" s="321" t="s">
+      <c r="V10" s="365"/>
+      <c r="W10" s="320" t="s">
         <v>257</v>
       </c>
-      <c r="X10" s="321"/>
-      <c r="Y10" s="321"/>
-      <c r="Z10" s="321"/>
-      <c r="AA10" s="321"/>
-      <c r="AB10" s="321"/>
-      <c r="AC10" s="321"/>
-      <c r="AD10" s="350"/>
+      <c r="X10" s="320"/>
+      <c r="Y10" s="320"/>
+      <c r="Z10" s="320"/>
+      <c r="AA10" s="320"/>
+      <c r="AB10" s="320"/>
+      <c r="AC10" s="320"/>
+      <c r="AD10" s="349"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="175"/>
-      <c r="B11" s="321" t="s">
+      <c r="B11" s="320" t="s">
         <v>254</v>
       </c>
-      <c r="C11" s="321"/>
-      <c r="D11" s="321"/>
-      <c r="E11" s="321"/>
-      <c r="F11" s="321"/>
+      <c r="C11" s="320"/>
+      <c r="D11" s="320"/>
+      <c r="E11" s="320"/>
+      <c r="F11" s="320"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -17648,30 +17647,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="176"/>
-      <c r="U11" s="365" t="s">
+      <c r="U11" s="364" t="s">
         <v>256</v>
       </c>
-      <c r="V11" s="366"/>
-      <c r="W11" s="359" t="s">
+      <c r="V11" s="365"/>
+      <c r="W11" s="358" t="s">
         <v>258</v>
       </c>
-      <c r="X11" s="359"/>
-      <c r="Y11" s="359"/>
-      <c r="Z11" s="359"/>
-      <c r="AA11" s="359"/>
-      <c r="AB11" s="359"/>
-      <c r="AC11" s="359"/>
-      <c r="AD11" s="360"/>
+      <c r="X11" s="358"/>
+      <c r="Y11" s="358"/>
+      <c r="Z11" s="358"/>
+      <c r="AA11" s="358"/>
+      <c r="AB11" s="358"/>
+      <c r="AC11" s="358"/>
+      <c r="AD11" s="359"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="175"/>
-      <c r="B12" s="404" t="s">
+      <c r="B12" s="403" t="s">
         <v>255</v>
       </c>
-      <c r="C12" s="404"/>
-      <c r="D12" s="404"/>
-      <c r="E12" s="404"/>
-      <c r="F12" s="404"/>
+      <c r="C12" s="403"/>
+      <c r="D12" s="403"/>
+      <c r="E12" s="403"/>
+      <c r="F12" s="403"/>
       <c r="G12" s="180">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -17682,16 +17681,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="176"/>
-      <c r="U12" s="365"/>
-      <c r="V12" s="366"/>
-      <c r="W12" s="321"/>
-      <c r="X12" s="321"/>
-      <c r="Y12" s="321"/>
-      <c r="Z12" s="321"/>
-      <c r="AA12" s="321"/>
-      <c r="AB12" s="321"/>
-      <c r="AC12" s="321"/>
-      <c r="AD12" s="350"/>
+      <c r="U12" s="364"/>
+      <c r="V12" s="365"/>
+      <c r="W12" s="320"/>
+      <c r="X12" s="320"/>
+      <c r="Y12" s="320"/>
+      <c r="Z12" s="320"/>
+      <c r="AA12" s="320"/>
+      <c r="AB12" s="320"/>
+      <c r="AC12" s="320"/>
+      <c r="AD12" s="349"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="177"/>
@@ -17707,64 +17706,64 @@
       <c r="K13" s="178"/>
       <c r="L13" s="178"/>
       <c r="M13" s="179"/>
-      <c r="U13" s="365"/>
-      <c r="V13" s="366"/>
-      <c r="W13" s="321"/>
-      <c r="X13" s="321"/>
-      <c r="Y13" s="321"/>
-      <c r="Z13" s="321"/>
-      <c r="AA13" s="321"/>
-      <c r="AB13" s="321"/>
-      <c r="AC13" s="321"/>
-      <c r="AD13" s="350"/>
+      <c r="U13" s="364"/>
+      <c r="V13" s="365"/>
+      <c r="W13" s="320"/>
+      <c r="X13" s="320"/>
+      <c r="Y13" s="320"/>
+      <c r="Z13" s="320"/>
+      <c r="AA13" s="320"/>
+      <c r="AB13" s="320"/>
+      <c r="AC13" s="320"/>
+      <c r="AD13" s="349"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="380"/>
-      <c r="V14" s="381"/>
-      <c r="W14" s="351"/>
-      <c r="X14" s="351"/>
-      <c r="Y14" s="351"/>
-      <c r="Z14" s="351"/>
-      <c r="AA14" s="351"/>
-      <c r="AB14" s="351"/>
-      <c r="AC14" s="351"/>
-      <c r="AD14" s="352"/>
+      <c r="U14" s="379"/>
+      <c r="V14" s="380"/>
+      <c r="W14" s="350"/>
+      <c r="X14" s="350"/>
+      <c r="Y14" s="350"/>
+      <c r="Z14" s="350"/>
+      <c r="AA14" s="350"/>
+      <c r="AB14" s="350"/>
+      <c r="AC14" s="350"/>
+      <c r="AD14" s="351"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="172"/>
       <c r="B18" s="173"/>
       <c r="C18" s="173"/>
-      <c r="D18" s="403" t="s">
+      <c r="D18" s="402" t="s">
         <v>249</v>
       </c>
-      <c r="E18" s="403"/>
-      <c r="F18" s="403"/>
-      <c r="G18" s="403"/>
-      <c r="H18" s="403"/>
-      <c r="I18" s="403"/>
-      <c r="J18" s="403"/>
-      <c r="K18" s="403"/>
-      <c r="L18" s="403"/>
+      <c r="E18" s="402"/>
+      <c r="F18" s="402"/>
+      <c r="G18" s="402"/>
+      <c r="H18" s="402"/>
+      <c r="I18" s="402"/>
+      <c r="J18" s="402"/>
+      <c r="K18" s="402"/>
+      <c r="L18" s="402"/>
       <c r="M18" s="174"/>
-      <c r="O18" s="382" t="s">
+      <c r="O18" s="381" t="s">
         <v>250</v>
       </c>
-      <c r="P18" s="383"/>
-      <c r="Q18" s="383"/>
-      <c r="R18" s="383"/>
-      <c r="S18" s="384"/>
+      <c r="P18" s="382"/>
+      <c r="Q18" s="382"/>
+      <c r="R18" s="382"/>
+      <c r="S18" s="383"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="175"/>
       <c r="M19" s="176"/>
-      <c r="O19" s="372" t="s">
+      <c r="O19" s="371" t="s">
         <v>251</v>
       </c>
-      <c r="P19" s="321"/>
-      <c r="Q19" s="321"/>
-      <c r="R19" s="321"/>
-      <c r="S19" s="350"/>
+      <c r="P19" s="320"/>
+      <c r="Q19" s="320"/>
+      <c r="R19" s="320"/>
+      <c r="S19" s="349"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="175"/>
@@ -17775,119 +17774,119 @@
       <c r="F20" s="200"/>
       <c r="G20" s="68"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="355" t="s">
+      <c r="I20" s="354" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="321"/>
-      <c r="K20" s="321"/>
-      <c r="L20" s="321"/>
+      <c r="J20" s="320"/>
+      <c r="K20" s="320"/>
+      <c r="L20" s="320"/>
       <c r="M20" s="176"/>
-      <c r="O20" s="372" t="s">
+      <c r="O20" s="371" t="s">
         <v>252</v>
       </c>
-      <c r="P20" s="321"/>
-      <c r="Q20" s="321"/>
-      <c r="R20" s="321"/>
-      <c r="S20" s="350"/>
+      <c r="P20" s="320"/>
+      <c r="Q20" s="320"/>
+      <c r="R20" s="320"/>
+      <c r="S20" s="349"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="175"/>
-      <c r="B21" s="388" t="s">
+      <c r="B21" s="387" t="s">
         <v>296</v>
       </c>
-      <c r="C21" s="389"/>
-      <c r="D21" s="389"/>
-      <c r="E21" s="389"/>
-      <c r="F21" s="390"/>
+      <c r="C21" s="388"/>
+      <c r="D21" s="388"/>
+      <c r="E21" s="388"/>
+      <c r="F21" s="389"/>
       <c r="G21" s="70">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="374" t="s">
+      <c r="I21" s="373" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="395"/>
-      <c r="K21" s="397">
+      <c r="J21" s="394"/>
+      <c r="K21" s="396">
         <f>G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="L21" s="398"/>
+      <c r="L21" s="397"/>
       <c r="M21" s="176"/>
       <c r="N21" s="170"/>
-      <c r="O21" s="385" t="s">
+      <c r="O21" s="384" t="s">
         <v>259</v>
       </c>
-      <c r="P21" s="375"/>
-      <c r="Q21" s="375"/>
-      <c r="R21" s="375"/>
-      <c r="S21" s="376"/>
+      <c r="P21" s="374"/>
+      <c r="Q21" s="374"/>
+      <c r="R21" s="374"/>
+      <c r="S21" s="375"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="175"/>
-      <c r="B22" s="377" t="s">
+      <c r="B22" s="376" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="378"/>
-      <c r="D22" s="378"/>
-      <c r="E22" s="378"/>
-      <c r="F22" s="391"/>
+      <c r="C22" s="377"/>
+      <c r="D22" s="377"/>
+      <c r="E22" s="377"/>
+      <c r="F22" s="390"/>
       <c r="G22" s="152">
         <f>G21</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="396" t="s">
+      <c r="I22" s="395" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="391"/>
-      <c r="K22" s="399">
+      <c r="J22" s="390"/>
+      <c r="K22" s="398">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="L22" s="400"/>
+      <c r="L22" s="399"/>
       <c r="M22" s="176"/>
       <c r="N22" s="170"/>
-      <c r="O22" s="377" t="s">
+      <c r="O22" s="376" t="s">
         <v>260</v>
       </c>
-      <c r="P22" s="378"/>
-      <c r="Q22" s="378"/>
-      <c r="R22" s="378"/>
-      <c r="S22" s="379"/>
+      <c r="P22" s="377"/>
+      <c r="Q22" s="377"/>
+      <c r="R22" s="377"/>
+      <c r="S22" s="378"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="175"/>
-      <c r="B23" s="392" t="s">
+      <c r="B23" s="391" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="393"/>
-      <c r="D23" s="393"/>
-      <c r="E23" s="393"/>
-      <c r="F23" s="394"/>
+      <c r="C23" s="392"/>
+      <c r="D23" s="392"/>
+      <c r="E23" s="392"/>
+      <c r="F23" s="393"/>
       <c r="G23" s="153">
         <f>K24</f>
         <v>1568729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="396" t="s">
+      <c r="I23" s="395" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="391"/>
-      <c r="K23" s="401">
+      <c r="J23" s="390"/>
+      <c r="K23" s="400">
         <f>Pemasukkan!L31</f>
         <v>690000</v>
       </c>
-      <c r="L23" s="402"/>
+      <c r="L23" s="401"/>
       <c r="M23" s="176"/>
       <c r="N23" s="170"/>
-      <c r="O23" s="377" t="s">
+      <c r="O23" s="376" t="s">
         <v>261</v>
       </c>
-      <c r="P23" s="378"/>
-      <c r="Q23" s="378"/>
-      <c r="R23" s="378"/>
-      <c r="S23" s="379"/>
+      <c r="P23" s="377"/>
+      <c r="Q23" s="377"/>
+      <c r="R23" s="377"/>
+      <c r="S23" s="378"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="175"/>
@@ -17898,24 +17897,24 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="374" t="s">
+      <c r="I24" s="373" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="395"/>
-      <c r="K24" s="386">
+      <c r="J24" s="394"/>
+      <c r="K24" s="385">
         <f>(K21-K22)+K23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="L24" s="387"/>
+      <c r="L24" s="386"/>
       <c r="M24" s="176"/>
       <c r="N24" s="170"/>
-      <c r="O24" s="377" t="s">
+      <c r="O24" s="376" t="s">
         <v>262</v>
       </c>
-      <c r="P24" s="378"/>
-      <c r="Q24" s="378"/>
-      <c r="R24" s="378"/>
-      <c r="S24" s="379"/>
+      <c r="P24" s="377"/>
+      <c r="Q24" s="377"/>
+      <c r="R24" s="377"/>
+      <c r="S24" s="378"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="175"/>
@@ -17932,13 +17931,13 @@
       <c r="L25" s="24"/>
       <c r="M25" s="176"/>
       <c r="N25" s="170"/>
-      <c r="O25" s="372" t="s">
+      <c r="O25" s="371" t="s">
         <v>267</v>
       </c>
-      <c r="P25" s="321"/>
-      <c r="Q25" s="321"/>
-      <c r="R25" s="321"/>
-      <c r="S25" s="350"/>
+      <c r="P25" s="320"/>
+      <c r="Q25" s="320"/>
+      <c r="R25" s="320"/>
+      <c r="S25" s="349"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="175"/>
@@ -17955,11 +17954,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="176"/>
       <c r="N26" s="170"/>
-      <c r="O26" s="373"/>
-      <c r="P26" s="351"/>
-      <c r="Q26" s="351"/>
-      <c r="R26" s="351"/>
-      <c r="S26" s="352"/>
+      <c r="O26" s="372"/>
+      <c r="P26" s="350"/>
+      <c r="Q26" s="350"/>
+      <c r="R26" s="350"/>
+      <c r="S26" s="351"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="177"/>
@@ -18090,44 +18089,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="418" t="s">
+      <c r="C2" s="417" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="419"/>
-      <c r="E2" s="419"/>
-      <c r="F2" s="419"/>
-      <c r="G2" s="419"/>
-      <c r="H2" s="419"/>
-      <c r="I2" s="419"/>
-      <c r="J2" s="419"/>
-      <c r="K2" s="419"/>
+      <c r="D2" s="418"/>
+      <c r="E2" s="418"/>
+      <c r="F2" s="418"/>
+      <c r="G2" s="418"/>
+      <c r="H2" s="418"/>
+      <c r="I2" s="418"/>
+      <c r="J2" s="418"/>
+      <c r="K2" s="418"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="419"/>
-      <c r="D3" s="419"/>
-      <c r="E3" s="419"/>
-      <c r="F3" s="419"/>
-      <c r="G3" s="419"/>
-      <c r="H3" s="419"/>
-      <c r="I3" s="419"/>
-      <c r="J3" s="419"/>
-      <c r="K3" s="419"/>
+      <c r="C3" s="418"/>
+      <c r="D3" s="418"/>
+      <c r="E3" s="418"/>
+      <c r="F3" s="418"/>
+      <c r="G3" s="418"/>
+      <c r="H3" s="418"/>
+      <c r="I3" s="418"/>
+      <c r="J3" s="418"/>
+      <c r="K3" s="418"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="411" t="s">
+      <c r="C5" s="410" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="411"/>
-      <c r="E5" s="411"/>
-      <c r="F5" s="411"/>
-      <c r="G5" s="411"/>
-      <c r="I5" s="411" t="s">
+      <c r="D5" s="410"/>
+      <c r="E5" s="410"/>
+      <c r="F5" s="410"/>
+      <c r="G5" s="410"/>
+      <c r="I5" s="410" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="411"/>
-      <c r="K5" s="411"/>
-      <c r="L5" s="411"/>
-      <c r="M5" s="411"/>
+      <c r="J5" s="410"/>
+      <c r="K5" s="410"/>
+      <c r="L5" s="410"/>
+      <c r="M5" s="410"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -18567,88 +18566,88 @@
       <c r="M28" s="170"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="407" t="s">
+      <c r="D29" s="406" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="408"/>
-      <c r="F29" s="412">
+      <c r="E29" s="407"/>
+      <c r="F29" s="411">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="413"/>
+      <c r="G29" s="412"/>
       <c r="I29" s="170"/>
-      <c r="J29" s="407" t="s">
+      <c r="J29" s="406" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="408"/>
-      <c r="L29" s="412">
+      <c r="K29" s="407"/>
+      <c r="L29" s="411">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="413"/>
+      <c r="M29" s="412"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="367" t="s">
+      <c r="D30" s="366" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="321"/>
-      <c r="F30" s="414">
+      <c r="E30" s="320"/>
+      <c r="F30" s="413">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="415"/>
+      <c r="G30" s="414"/>
       <c r="I30" s="170"/>
-      <c r="J30" s="367" t="s">
+      <c r="J30" s="366" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="321"/>
-      <c r="L30" s="414">
+      <c r="K30" s="320"/>
+      <c r="L30" s="413">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="415"/>
+      <c r="M30" s="414"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="372" t="s">
+      <c r="D31" s="371" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="321"/>
-      <c r="F31" s="416">
+      <c r="E31" s="320"/>
+      <c r="F31" s="415">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="417"/>
+      <c r="G31" s="416"/>
       <c r="I31" s="170"/>
-      <c r="J31" s="372" t="s">
+      <c r="J31" s="371" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="321"/>
-      <c r="L31" s="416">
+      <c r="K31" s="320"/>
+      <c r="L31" s="415">
         <f>L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="417"/>
+      <c r="M31" s="416"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="405" t="s">
+      <c r="D32" s="404" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="406"/>
-      <c r="F32" s="409">
+      <c r="E32" s="405"/>
+      <c r="F32" s="408">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="410"/>
+      <c r="G32" s="409"/>
       <c r="I32" s="170"/>
-      <c r="J32" s="405" t="s">
+      <c r="J32" s="404" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="406"/>
-      <c r="L32" s="409">
+      <c r="K32" s="405"/>
+      <c r="L32" s="408">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="410"/>
+      <c r="M32" s="409"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18891,44 +18890,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="424" t="s">
+      <c r="C2" s="423" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="425"/>
-      <c r="E2" s="425"/>
-      <c r="F2" s="425"/>
-      <c r="G2" s="425"/>
-      <c r="H2" s="425"/>
-      <c r="I2" s="425"/>
-      <c r="J2" s="425"/>
-      <c r="K2" s="425"/>
+      <c r="D2" s="424"/>
+      <c r="E2" s="424"/>
+      <c r="F2" s="424"/>
+      <c r="G2" s="424"/>
+      <c r="H2" s="424"/>
+      <c r="I2" s="424"/>
+      <c r="J2" s="424"/>
+      <c r="K2" s="424"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="425"/>
-      <c r="D3" s="425"/>
-      <c r="E3" s="425"/>
-      <c r="F3" s="425"/>
-      <c r="G3" s="425"/>
-      <c r="H3" s="425"/>
-      <c r="I3" s="425"/>
-      <c r="J3" s="425"/>
-      <c r="K3" s="425"/>
+      <c r="C3" s="424"/>
+      <c r="D3" s="424"/>
+      <c r="E3" s="424"/>
+      <c r="F3" s="424"/>
+      <c r="G3" s="424"/>
+      <c r="H3" s="424"/>
+      <c r="I3" s="424"/>
+      <c r="J3" s="424"/>
+      <c r="K3" s="424"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="411" t="s">
+      <c r="C5" s="410" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="411"/>
-      <c r="E5" s="411"/>
-      <c r="F5" s="411"/>
-      <c r="G5" s="411"/>
-      <c r="I5" s="411" t="s">
+      <c r="D5" s="410"/>
+      <c r="E5" s="410"/>
+      <c r="F5" s="410"/>
+      <c r="G5" s="410"/>
+      <c r="I5" s="410" t="s">
         <v>246</v>
       </c>
-      <c r="J5" s="411"/>
-      <c r="K5" s="411"/>
-      <c r="L5" s="411"/>
-      <c r="M5" s="411"/>
+      <c r="J5" s="410"/>
+      <c r="K5" s="410"/>
+      <c r="L5" s="410"/>
+      <c r="M5" s="410"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -19412,88 +19411,88 @@
       <c r="M28" s="170"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="346" t="s">
+      <c r="D29" s="345" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="348"/>
-      <c r="F29" s="422">
+      <c r="E29" s="347"/>
+      <c r="F29" s="421">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="423"/>
+      <c r="G29" s="422"/>
       <c r="I29" s="170"/>
-      <c r="J29" s="346" t="s">
+      <c r="J29" s="345" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="348"/>
-      <c r="L29" s="422">
+      <c r="K29" s="347"/>
+      <c r="L29" s="421">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="423"/>
+      <c r="M29" s="422"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="372" t="s">
+      <c r="D30" s="371" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="321"/>
-      <c r="F30" s="414">
+      <c r="E30" s="320"/>
+      <c r="F30" s="413">
         <f>F27</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="415"/>
+      <c r="G30" s="414"/>
       <c r="I30" s="170"/>
-      <c r="J30" s="372" t="s">
+      <c r="J30" s="371" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="321"/>
-      <c r="L30" s="414">
+      <c r="K30" s="320"/>
+      <c r="L30" s="413">
         <f>L27</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="415"/>
+      <c r="M30" s="414"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="372" t="s">
+      <c r="D31" s="371" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="321"/>
-      <c r="F31" s="416">
+      <c r="E31" s="320"/>
+      <c r="F31" s="415">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="417"/>
+      <c r="G31" s="416"/>
       <c r="I31" s="170"/>
-      <c r="J31" s="372" t="s">
+      <c r="J31" s="371" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="321"/>
-      <c r="L31" s="416">
+      <c r="K31" s="320"/>
+      <c r="L31" s="415">
         <f>Pemasukkan!L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="417"/>
+      <c r="M31" s="416"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="405" t="s">
+      <c r="D32" s="404" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="406"/>
-      <c r="F32" s="420">
+      <c r="E32" s="405"/>
+      <c r="F32" s="419">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="421"/>
+      <c r="G32" s="420"/>
       <c r="I32" s="170"/>
-      <c r="J32" s="405" t="s">
+      <c r="J32" s="404" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="406"/>
-      <c r="L32" s="420">
+      <c r="K32" s="405"/>
+      <c r="L32" s="419">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="421"/>
+      <c r="M32" s="420"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19729,28 +19728,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="428" t="s">
+      <c r="C2" s="427" t="s">
         <v>230</v>
       </c>
-      <c r="D2" s="429"/>
-      <c r="E2" s="429"/>
-      <c r="F2" s="429"/>
-      <c r="G2" s="429"/>
-      <c r="H2" s="429"/>
-      <c r="I2" s="429"/>
-      <c r="J2" s="429"/>
-      <c r="K2" s="429"/>
+      <c r="D2" s="428"/>
+      <c r="E2" s="428"/>
+      <c r="F2" s="428"/>
+      <c r="G2" s="428"/>
+      <c r="H2" s="428"/>
+      <c r="I2" s="428"/>
+      <c r="J2" s="428"/>
+      <c r="K2" s="428"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="429"/>
-      <c r="D3" s="429"/>
-      <c r="E3" s="429"/>
-      <c r="F3" s="429"/>
-      <c r="G3" s="429"/>
-      <c r="H3" s="429"/>
-      <c r="I3" s="429"/>
-      <c r="J3" s="429"/>
-      <c r="K3" s="429"/>
+      <c r="C3" s="428"/>
+      <c r="D3" s="428"/>
+      <c r="E3" s="428"/>
+      <c r="F3" s="428"/>
+      <c r="G3" s="428"/>
+      <c r="H3" s="428"/>
+      <c r="I3" s="428"/>
+      <c r="J3" s="428"/>
+      <c r="K3" s="428"/>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="139"/>
@@ -20108,10 +20107,10 @@
     </row>
     <row r="29" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="139"/>
-      <c r="D29" s="430"/>
-      <c r="E29" s="430"/>
-      <c r="F29" s="431"/>
-      <c r="G29" s="431"/>
+      <c r="D29" s="429"/>
+      <c r="E29" s="429"/>
+      <c r="F29" s="430"/>
+      <c r="G29" s="430"/>
       <c r="H29" s="139"/>
       <c r="I29" s="139"/>
       <c r="J29" s="139"/>
@@ -20119,15 +20118,15 @@
     </row>
     <row r="30" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="24"/>
-      <c r="D30" s="432" t="s">
+      <c r="D30" s="431" t="s">
         <v>229</v>
       </c>
-      <c r="E30" s="433"/>
-      <c r="F30" s="434">
+      <c r="E30" s="432"/>
+      <c r="F30" s="433">
         <f>F27</f>
         <v>226000</v>
       </c>
-      <c r="G30" s="435"/>
+      <c r="G30" s="434"/>
       <c r="H30" s="139"/>
       <c r="I30" s="139"/>
       <c r="J30" s="139"/>
@@ -20142,10 +20141,10 @@
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="139"/>
-      <c r="D32" s="426"/>
-      <c r="E32" s="426"/>
-      <c r="F32" s="427"/>
-      <c r="G32" s="426"/>
+      <c r="D32" s="425"/>
+      <c r="E32" s="425"/>
+      <c r="F32" s="426"/>
+      <c r="G32" s="425"/>
       <c r="H32" s="139"/>
       <c r="I32" s="139"/>
       <c r="J32" s="139"/>
@@ -20182,17 +20181,17 @@
     <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="436" t="s">
+      <c r="C4" s="435" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="437"/>
+      <c r="D4" s="436"/>
       <c r="E4" s="27"/>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
-      <c r="H4" s="436" t="s">
+      <c r="H4" s="435" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="437"/>
+      <c r="I4" s="436"/>
       <c r="J4" s="35"/>
       <c r="K4" s="27"/>
     </row>
@@ -20319,17 +20318,17 @@
     <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26"/>
-      <c r="C17" s="436" t="s">
+      <c r="C17" s="435" t="s">
         <v>144</v>
       </c>
-      <c r="D17" s="437"/>
+      <c r="D17" s="436"/>
       <c r="E17" s="27"/>
       <c r="F17" s="26"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="436" t="s">
+      <c r="H17" s="435" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="437"/>
+      <c r="I17" s="436"/>
       <c r="J17" s="35"/>
       <c r="K17" s="27"/>
     </row>

</xml_diff>

<commit_message>
Bayar Makrab Amir, Sulthon, Adhika
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="385">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -1175,6 +1175,9 @@
   </si>
   <si>
     <t>Nursagita I</t>
+  </si>
+  <si>
+    <t>Sulthon Muhamad Arief</t>
   </si>
 </sst>
 </file>
@@ -3028,29 +3031,20 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3066,37 +3060,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3104,29 +3100,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3176,6 +3179,156 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3188,33 +3341,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3234,136 +3366,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3374,47 +3395,29 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4669,126 +4672,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="293" t="s">
+      <c r="A1" s="287" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="294"/>
-      <c r="C1" s="294"/>
-      <c r="D1" s="294"/>
-      <c r="E1" s="294"/>
-      <c r="F1" s="294"/>
-      <c r="G1" s="294"/>
-      <c r="H1" s="294"/>
-      <c r="I1" s="294"/>
-      <c r="J1" s="294"/>
-      <c r="K1" s="294"/>
-      <c r="L1" s="294"/>
-      <c r="M1" s="294"/>
-      <c r="N1" s="294"/>
-      <c r="O1" s="294"/>
-      <c r="P1" s="294"/>
-      <c r="Q1" s="294"/>
-      <c r="R1" s="294"/>
+      <c r="B1" s="288"/>
+      <c r="C1" s="288"/>
+      <c r="D1" s="288"/>
+      <c r="E1" s="288"/>
+      <c r="F1" s="288"/>
+      <c r="G1" s="288"/>
+      <c r="H1" s="288"/>
+      <c r="I1" s="288"/>
+      <c r="J1" s="288"/>
+      <c r="K1" s="288"/>
+      <c r="L1" s="288"/>
+      <c r="M1" s="288"/>
+      <c r="N1" s="288"/>
+      <c r="O1" s="288"/>
+      <c r="P1" s="288"/>
+      <c r="Q1" s="288"/>
+      <c r="R1" s="288"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="295"/>
-      <c r="B2" s="296"/>
-      <c r="C2" s="296"/>
-      <c r="D2" s="296"/>
-      <c r="E2" s="296"/>
-      <c r="F2" s="296"/>
-      <c r="G2" s="296"/>
-      <c r="H2" s="296"/>
-      <c r="I2" s="296"/>
-      <c r="J2" s="296"/>
-      <c r="K2" s="296"/>
-      <c r="L2" s="296"/>
-      <c r="M2" s="296"/>
-      <c r="N2" s="296"/>
-      <c r="O2" s="296"/>
-      <c r="P2" s="296"/>
-      <c r="Q2" s="296"/>
-      <c r="R2" s="296"/>
+      <c r="A2" s="289"/>
+      <c r="B2" s="290"/>
+      <c r="C2" s="290"/>
+      <c r="D2" s="290"/>
+      <c r="E2" s="290"/>
+      <c r="F2" s="290"/>
+      <c r="G2" s="290"/>
+      <c r="H2" s="290"/>
+      <c r="I2" s="290"/>
+      <c r="J2" s="290"/>
+      <c r="K2" s="290"/>
+      <c r="L2" s="290"/>
+      <c r="M2" s="290"/>
+      <c r="N2" s="290"/>
+      <c r="O2" s="290"/>
+      <c r="P2" s="290"/>
+      <c r="Q2" s="290"/>
+      <c r="R2" s="290"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="295"/>
-      <c r="B3" s="296"/>
-      <c r="C3" s="296"/>
-      <c r="D3" s="296"/>
-      <c r="E3" s="296"/>
-      <c r="F3" s="296"/>
-      <c r="G3" s="296"/>
-      <c r="H3" s="296"/>
-      <c r="I3" s="296"/>
-      <c r="J3" s="296"/>
-      <c r="K3" s="296"/>
-      <c r="L3" s="296"/>
-      <c r="M3" s="296"/>
-      <c r="N3" s="296"/>
-      <c r="O3" s="296"/>
-      <c r="P3" s="296"/>
-      <c r="Q3" s="296"/>
-      <c r="R3" s="296"/>
+      <c r="A3" s="289"/>
+      <c r="B3" s="290"/>
+      <c r="C3" s="290"/>
+      <c r="D3" s="290"/>
+      <c r="E3" s="290"/>
+      <c r="F3" s="290"/>
+      <c r="G3" s="290"/>
+      <c r="H3" s="290"/>
+      <c r="I3" s="290"/>
+      <c r="J3" s="290"/>
+      <c r="K3" s="290"/>
+      <c r="L3" s="290"/>
+      <c r="M3" s="290"/>
+      <c r="N3" s="290"/>
+      <c r="O3" s="290"/>
+      <c r="P3" s="290"/>
+      <c r="Q3" s="290"/>
+      <c r="R3" s="290"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="295"/>
-      <c r="B4" s="296"/>
-      <c r="C4" s="296"/>
-      <c r="D4" s="296"/>
-      <c r="E4" s="296"/>
-      <c r="F4" s="296"/>
-      <c r="G4" s="296"/>
-      <c r="H4" s="296"/>
-      <c r="I4" s="296"/>
-      <c r="J4" s="296"/>
-      <c r="K4" s="296"/>
-      <c r="L4" s="296"/>
-      <c r="M4" s="296"/>
-      <c r="N4" s="296"/>
-      <c r="O4" s="296"/>
-      <c r="P4" s="296"/>
-      <c r="Q4" s="296"/>
-      <c r="R4" s="296"/>
+      <c r="A4" s="289"/>
+      <c r="B4" s="290"/>
+      <c r="C4" s="290"/>
+      <c r="D4" s="290"/>
+      <c r="E4" s="290"/>
+      <c r="F4" s="290"/>
+      <c r="G4" s="290"/>
+      <c r="H4" s="290"/>
+      <c r="I4" s="290"/>
+      <c r="J4" s="290"/>
+      <c r="K4" s="290"/>
+      <c r="L4" s="290"/>
+      <c r="M4" s="290"/>
+      <c r="N4" s="290"/>
+      <c r="O4" s="290"/>
+      <c r="P4" s="290"/>
+      <c r="Q4" s="290"/>
+      <c r="R4" s="290"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="295"/>
-      <c r="B5" s="296"/>
-      <c r="C5" s="296"/>
-      <c r="D5" s="296"/>
-      <c r="E5" s="296"/>
-      <c r="F5" s="296"/>
-      <c r="G5" s="296"/>
-      <c r="H5" s="296"/>
-      <c r="I5" s="296"/>
-      <c r="J5" s="296"/>
-      <c r="K5" s="296"/>
-      <c r="L5" s="296"/>
-      <c r="M5" s="296"/>
-      <c r="N5" s="296"/>
-      <c r="O5" s="296"/>
-      <c r="P5" s="296"/>
-      <c r="Q5" s="296"/>
-      <c r="R5" s="296"/>
+      <c r="A5" s="289"/>
+      <c r="B5" s="290"/>
+      <c r="C5" s="290"/>
+      <c r="D5" s="290"/>
+      <c r="E5" s="290"/>
+      <c r="F5" s="290"/>
+      <c r="G5" s="290"/>
+      <c r="H5" s="290"/>
+      <c r="I5" s="290"/>
+      <c r="J5" s="290"/>
+      <c r="K5" s="290"/>
+      <c r="L5" s="290"/>
+      <c r="M5" s="290"/>
+      <c r="N5" s="290"/>
+      <c r="O5" s="290"/>
+      <c r="P5" s="290"/>
+      <c r="Q5" s="290"/>
+      <c r="R5" s="290"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="295"/>
-      <c r="B6" s="296"/>
-      <c r="C6" s="296"/>
-      <c r="D6" s="296"/>
-      <c r="E6" s="296"/>
-      <c r="F6" s="296"/>
-      <c r="G6" s="296"/>
-      <c r="H6" s="296"/>
-      <c r="I6" s="296"/>
-      <c r="J6" s="296"/>
-      <c r="K6" s="296"/>
-      <c r="L6" s="296"/>
-      <c r="M6" s="296"/>
-      <c r="N6" s="296"/>
-      <c r="O6" s="296"/>
-      <c r="P6" s="296"/>
-      <c r="Q6" s="296"/>
-      <c r="R6" s="296"/>
+      <c r="A6" s="289"/>
+      <c r="B6" s="290"/>
+      <c r="C6" s="290"/>
+      <c r="D6" s="290"/>
+      <c r="E6" s="290"/>
+      <c r="F6" s="290"/>
+      <c r="G6" s="290"/>
+      <c r="H6" s="290"/>
+      <c r="I6" s="290"/>
+      <c r="J6" s="290"/>
+      <c r="K6" s="290"/>
+      <c r="L6" s="290"/>
+      <c r="M6" s="290"/>
+      <c r="N6" s="290"/>
+      <c r="O6" s="290"/>
+      <c r="P6" s="290"/>
+      <c r="Q6" s="290"/>
+      <c r="R6" s="290"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -7895,58 +7898,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="298" t="s">
+      <c r="J79" s="295" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="299"/>
-      <c r="L79" s="299"/>
-      <c r="M79" s="299"/>
-      <c r="N79" s="300"/>
-      <c r="P79" s="306" t="s">
+      <c r="K79" s="296"/>
+      <c r="L79" s="296"/>
+      <c r="M79" s="296"/>
+      <c r="N79" s="297"/>
+      <c r="P79" s="303" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="299"/>
-      <c r="R79" s="299"/>
-      <c r="S79" s="300"/>
+      <c r="Q79" s="296"/>
+      <c r="R79" s="296"/>
+      <c r="S79" s="297"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="301" t="s">
+      <c r="J80" s="298" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="296"/>
-      <c r="L80" s="296"/>
-      <c r="M80" s="296"/>
-      <c r="N80" s="302"/>
-      <c r="P80" s="301" t="s">
+      <c r="K80" s="290"/>
+      <c r="L80" s="290"/>
+      <c r="M80" s="290"/>
+      <c r="N80" s="299"/>
+      <c r="P80" s="298" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="296"/>
-      <c r="R80" s="296"/>
-      <c r="S80" s="302"/>
+      <c r="Q80" s="290"/>
+      <c r="R80" s="290"/>
+      <c r="S80" s="299"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="303"/>
-      <c r="K81" s="304"/>
-      <c r="L81" s="304"/>
-      <c r="M81" s="304"/>
-      <c r="N81" s="305"/>
-      <c r="P81" s="303"/>
-      <c r="Q81" s="304"/>
-      <c r="R81" s="304"/>
-      <c r="S81" s="305"/>
+      <c r="J81" s="300"/>
+      <c r="K81" s="301"/>
+      <c r="L81" s="301"/>
+      <c r="M81" s="301"/>
+      <c r="N81" s="302"/>
+      <c r="P81" s="300"/>
+      <c r="Q81" s="301"/>
+      <c r="R81" s="301"/>
+      <c r="S81" s="302"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="297" t="s">
+      <c r="J82" s="293" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="288"/>
-      <c r="L82" s="289"/>
-      <c r="M82" s="297" t="s">
+      <c r="K82" s="294"/>
+      <c r="L82" s="292"/>
+      <c r="M82" s="293" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="289"/>
-      <c r="P82" s="297"/>
-      <c r="Q82" s="289"/>
+      <c r="N82" s="292"/>
+      <c r="P82" s="293"/>
+      <c r="Q82" s="292"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -7955,38 +7958,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="287" t="s">
+      <c r="J83" s="304" t="s">
         <v>70</v>
       </c>
-      <c r="K83" s="288"/>
-      <c r="L83" s="289"/>
-      <c r="M83" s="290">
+      <c r="K83" s="294"/>
+      <c r="L83" s="292"/>
+      <c r="M83" s="305">
         <v>7350000</v>
       </c>
-      <c r="N83" s="289"/>
+      <c r="N83" s="292"/>
       <c r="P83" s="291" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="289"/>
+      <c r="Q83" s="292"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="287" t="s">
+      <c r="J84" s="304" t="s">
         <v>72</v>
       </c>
-      <c r="K84" s="288"/>
-      <c r="L84" s="289"/>
-      <c r="M84" s="292">
+      <c r="K84" s="294"/>
+      <c r="L84" s="292"/>
+      <c r="M84" s="306">
         <v>1100000</v>
       </c>
-      <c r="N84" s="289"/>
+      <c r="N84" s="292"/>
       <c r="P84" s="291" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="289"/>
+      <c r="Q84" s="292"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -7995,39 +7998,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="287" t="s">
+      <c r="J85" s="304" t="s">
         <v>75</v>
       </c>
-      <c r="K85" s="288"/>
-      <c r="L85" s="289"/>
-      <c r="M85" s="290">
+      <c r="K85" s="294"/>
+      <c r="L85" s="292"/>
+      <c r="M85" s="305">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="289"/>
+      <c r="N85" s="292"/>
       <c r="P85" s="291" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="289"/>
+      <c r="Q85" s="292"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="287" t="s">
+      <c r="J86" s="304" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="288"/>
-      <c r="L86" s="289"/>
-      <c r="M86" s="290">
+      <c r="K86" s="294"/>
+      <c r="L86" s="292"/>
+      <c r="M86" s="305">
         <v>8411850</v>
       </c>
-      <c r="N86" s="289"/>
+      <c r="N86" s="292"/>
       <c r="P86" s="291" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="289"/>
+      <c r="Q86" s="292"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -8035,20 +8038,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="287" t="s">
+      <c r="J87" s="304" t="s">
         <v>79</v>
       </c>
-      <c r="K87" s="288"/>
-      <c r="L87" s="289"/>
-      <c r="M87" s="290">
+      <c r="K87" s="294"/>
+      <c r="L87" s="292"/>
+      <c r="M87" s="305">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="289"/>
+      <c r="N87" s="292"/>
       <c r="P87" s="291" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="289"/>
+      <c r="Q87" s="292"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -8236,6 +8239,17 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="P86:Q86"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="M84:N84"/>
     <mergeCell ref="A1:R6"/>
     <mergeCell ref="P84:Q84"/>
     <mergeCell ref="J82:L82"/>
@@ -8248,17 +8262,6 @@
     <mergeCell ref="P83:Q83"/>
     <mergeCell ref="P82:Q82"/>
     <mergeCell ref="P80:S81"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="P86:Q86"/>
   </mergeCells>
   <conditionalFormatting sqref="T10:T69">
     <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
@@ -8347,10 +8350,10 @@
       <c r="G6" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="H6" s="354" t="s">
+      <c r="H6" s="364" t="s">
         <v>280</v>
       </c>
-      <c r="I6" s="320"/>
+      <c r="I6" s="317"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -8376,7 +8379,7 @@
         <f>F7-G7</f>
         <v>380000</v>
       </c>
-      <c r="I7" s="320"/>
+      <c r="I7" s="317"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="194"/>
@@ -8485,11 +8488,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="H6:I6"/>
@@ -8498,6 +8496,11 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8551,46 +8554,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="315" t="s">
+      <c r="C2" s="327" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="294"/>
-      <c r="E2" s="294"/>
-      <c r="F2" s="294"/>
-      <c r="G2" s="294"/>
-      <c r="H2" s="294"/>
-      <c r="I2" s="294"/>
-      <c r="J2" s="294"/>
-      <c r="K2" s="294"/>
-      <c r="L2" s="294"/>
-      <c r="M2" s="294"/>
-      <c r="N2" s="294"/>
-      <c r="O2" s="294"/>
-      <c r="P2" s="295"/>
-      <c r="Q2" s="295"/>
-      <c r="R2" s="295"/>
-      <c r="S2" s="294"/>
-      <c r="T2" s="294"/>
+      <c r="D2" s="288"/>
+      <c r="E2" s="288"/>
+      <c r="F2" s="288"/>
+      <c r="G2" s="288"/>
+      <c r="H2" s="288"/>
+      <c r="I2" s="288"/>
+      <c r="J2" s="288"/>
+      <c r="K2" s="288"/>
+      <c r="L2" s="288"/>
+      <c r="M2" s="288"/>
+      <c r="N2" s="288"/>
+      <c r="O2" s="288"/>
+      <c r="P2" s="289"/>
+      <c r="Q2" s="289"/>
+      <c r="R2" s="289"/>
+      <c r="S2" s="288"/>
+      <c r="T2" s="288"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="295"/>
-      <c r="D3" s="296"/>
-      <c r="E3" s="296"/>
-      <c r="F3" s="296"/>
-      <c r="G3" s="296"/>
-      <c r="H3" s="296"/>
-      <c r="I3" s="296"/>
-      <c r="J3" s="296"/>
-      <c r="K3" s="296"/>
-      <c r="L3" s="296"/>
-      <c r="M3" s="296"/>
-      <c r="N3" s="296"/>
-      <c r="O3" s="296"/>
-      <c r="P3" s="296"/>
-      <c r="Q3" s="296"/>
-      <c r="R3" s="296"/>
-      <c r="S3" s="296"/>
-      <c r="T3" s="296"/>
+      <c r="C3" s="289"/>
+      <c r="D3" s="290"/>
+      <c r="E3" s="290"/>
+      <c r="F3" s="290"/>
+      <c r="G3" s="290"/>
+      <c r="H3" s="290"/>
+      <c r="I3" s="290"/>
+      <c r="J3" s="290"/>
+      <c r="K3" s="290"/>
+      <c r="L3" s="290"/>
+      <c r="M3" s="290"/>
+      <c r="N3" s="290"/>
+      <c r="O3" s="290"/>
+      <c r="P3" s="290"/>
+      <c r="Q3" s="290"/>
+      <c r="R3" s="290"/>
+      <c r="S3" s="290"/>
+      <c r="T3" s="290"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8677,25 +8680,25 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="321" t="s">
+      <c r="X5" s="319" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="288"/>
-      <c r="Z5" s="288"/>
-      <c r="AA5" s="288"/>
-      <c r="AB5" s="288"/>
-      <c r="AC5" s="288"/>
-      <c r="AD5" s="288"/>
-      <c r="AE5" s="288"/>
-      <c r="AF5" s="288"/>
-      <c r="AG5" s="288"/>
-      <c r="AH5" s="288"/>
-      <c r="AI5" s="288"/>
-      <c r="AJ5" s="288"/>
-      <c r="AK5" s="288"/>
-      <c r="AL5" s="288"/>
-      <c r="AM5" s="288"/>
-      <c r="AN5" s="289"/>
+      <c r="Y5" s="294"/>
+      <c r="Z5" s="294"/>
+      <c r="AA5" s="294"/>
+      <c r="AB5" s="294"/>
+      <c r="AC5" s="294"/>
+      <c r="AD5" s="294"/>
+      <c r="AE5" s="294"/>
+      <c r="AF5" s="294"/>
+      <c r="AG5" s="294"/>
+      <c r="AH5" s="294"/>
+      <c r="AI5" s="294"/>
+      <c r="AJ5" s="294"/>
+      <c r="AK5" s="294"/>
+      <c r="AL5" s="294"/>
+      <c r="AM5" s="294"/>
+      <c r="AN5" s="292"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -8770,29 +8773,29 @@
       <c r="V6" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X6" s="316" t="s">
+      <c r="X6" s="328" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="316" t="s">
+      <c r="Y6" s="328" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="320" t="s">
+      <c r="Z6" s="317" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="317"/>
-      <c r="AB6" s="317"/>
-      <c r="AC6" s="317"/>
-      <c r="AD6" s="317"/>
-      <c r="AE6" s="317"/>
-      <c r="AF6" s="317"/>
-      <c r="AG6" s="317"/>
-      <c r="AH6" s="317"/>
-      <c r="AI6" s="317"/>
-      <c r="AJ6" s="317"/>
-      <c r="AK6" s="317"/>
-      <c r="AL6" s="317"/>
-      <c r="AM6" s="317"/>
-      <c r="AN6" s="317"/>
+      <c r="AA6" s="318"/>
+      <c r="AB6" s="318"/>
+      <c r="AC6" s="318"/>
+      <c r="AD6" s="318"/>
+      <c r="AE6" s="318"/>
+      <c r="AF6" s="318"/>
+      <c r="AG6" s="318"/>
+      <c r="AH6" s="318"/>
+      <c r="AI6" s="318"/>
+      <c r="AJ6" s="318"/>
+      <c r="AK6" s="318"/>
+      <c r="AL6" s="318"/>
+      <c r="AM6" s="318"/>
+      <c r="AN6" s="318"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -8867,27 +8870,27 @@
       <c r="V7" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X7" s="317"/>
-      <c r="Y7" s="317"/>
-      <c r="Z7" s="320" t="s">
+      <c r="X7" s="318"/>
+      <c r="Y7" s="318"/>
+      <c r="Z7" s="317" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="317"/>
-      <c r="AB7" s="317"/>
-      <c r="AC7" s="317"/>
-      <c r="AD7" s="320" t="s">
+      <c r="AA7" s="318"/>
+      <c r="AB7" s="318"/>
+      <c r="AC7" s="318"/>
+      <c r="AD7" s="317" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="317"/>
-      <c r="AF7" s="317"/>
-      <c r="AG7" s="317"/>
-      <c r="AH7" s="317"/>
-      <c r="AI7" s="317"/>
-      <c r="AJ7" s="317"/>
-      <c r="AK7" s="317"/>
-      <c r="AL7" s="317"/>
-      <c r="AM7" s="317"/>
-      <c r="AN7" s="317"/>
+      <c r="AE7" s="318"/>
+      <c r="AF7" s="318"/>
+      <c r="AG7" s="318"/>
+      <c r="AH7" s="318"/>
+      <c r="AI7" s="318"/>
+      <c r="AJ7" s="318"/>
+      <c r="AK7" s="318"/>
+      <c r="AL7" s="318"/>
+      <c r="AM7" s="318"/>
+      <c r="AN7" s="318"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -8937,8 +8940,8 @@
         <v>NO</v>
       </c>
       <c r="V8" s="13"/>
-      <c r="X8" s="317"/>
-      <c r="Y8" s="317"/>
+      <c r="X8" s="318"/>
+      <c r="Y8" s="318"/>
       <c r="Z8" s="151" t="s">
         <v>19</v>
       </c>
@@ -13549,10 +13552,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="318" t="s">
+      <c r="AA49" s="315" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="319"/>
+      <c r="AB49" s="316"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -13630,12 +13633,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="325" t="s">
+      <c r="AI50" s="311" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="326"/>
-      <c r="AK50" s="326"/>
-      <c r="AL50" s="327"/>
+      <c r="AJ50" s="312"/>
+      <c r="AK50" s="312"/>
+      <c r="AL50" s="313"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -13706,12 +13709,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="322" t="s">
+      <c r="AI51" s="308" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="323"/>
-      <c r="AK51" s="323"/>
-      <c r="AL51" s="324"/>
+      <c r="AJ51" s="309"/>
+      <c r="AK51" s="309"/>
+      <c r="AL51" s="310"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -13977,14 +13980,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="328"/>
-      <c r="AD55" s="328"/>
-      <c r="AI55" s="325" t="s">
+      <c r="AC55" s="314"/>
+      <c r="AD55" s="314"/>
+      <c r="AI55" s="311" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="326"/>
-      <c r="AK55" s="326"/>
-      <c r="AL55" s="327"/>
+      <c r="AJ55" s="312"/>
+      <c r="AK55" s="312"/>
+      <c r="AL55" s="313"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -14301,32 +14304,32 @@
     <row r="67" spans="3:19" s="256" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="308" t="s">
+      <c r="C69" s="320" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="309"/>
-      <c r="E69" s="309"/>
-      <c r="F69" s="309"/>
-      <c r="G69" s="310"/>
-      <c r="I69" s="314" t="s">
+      <c r="D69" s="321"/>
+      <c r="E69" s="321"/>
+      <c r="F69" s="321"/>
+      <c r="G69" s="322"/>
+      <c r="I69" s="326" t="s">
         <v>178</v>
       </c>
-      <c r="J69" s="314"/>
-      <c r="K69" s="314"/>
-      <c r="L69" s="314"/>
-      <c r="M69" s="314"/>
+      <c r="J69" s="326"/>
+      <c r="K69" s="326"/>
+      <c r="L69" s="326"/>
+      <c r="M69" s="326"/>
     </row>
     <row r="70" spans="3:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="311"/>
-      <c r="D70" s="312"/>
-      <c r="E70" s="312"/>
-      <c r="F70" s="312"/>
-      <c r="G70" s="313"/>
-      <c r="I70" s="314"/>
-      <c r="J70" s="314"/>
-      <c r="K70" s="314"/>
-      <c r="L70" s="314"/>
-      <c r="M70" s="314"/>
+      <c r="C70" s="323"/>
+      <c r="D70" s="324"/>
+      <c r="E70" s="324"/>
+      <c r="F70" s="324"/>
+      <c r="G70" s="325"/>
+      <c r="I70" s="326"/>
+      <c r="J70" s="326"/>
+      <c r="K70" s="326"/>
+      <c r="L70" s="326"/>
+      <c r="M70" s="326"/>
     </row>
     <row r="71" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14817,22 +14820,22 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AI56:AL56"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AI50:AL50"/>
-    <mergeCell ref="AI55:AL55"/>
-    <mergeCell ref="AC55:AD55"/>
-    <mergeCell ref="AA49:AB49"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="AD7:AN7"/>
-    <mergeCell ref="X5:AN5"/>
-    <mergeCell ref="Z6:AN6"/>
     <mergeCell ref="P76:Q76"/>
     <mergeCell ref="C69:G70"/>
     <mergeCell ref="I69:M70"/>
     <mergeCell ref="C2:T3"/>
     <mergeCell ref="Y6:Y8"/>
     <mergeCell ref="X6:X8"/>
+    <mergeCell ref="AA49:AB49"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="AD7:AN7"/>
+    <mergeCell ref="X5:AN5"/>
+    <mergeCell ref="Z6:AN6"/>
+    <mergeCell ref="AI56:AL56"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AI50:AL50"/>
+    <mergeCell ref="AI55:AL55"/>
+    <mergeCell ref="AC55:AD55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:V61">
     <cfRule type="expression" dxfId="20" priority="8">
@@ -14952,56 +14955,56 @@
       <c r="L3" s="329"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="314" t="s">
+      <c r="A5" s="326" t="s">
         <v>303</v>
       </c>
-      <c r="B5" s="314"/>
-      <c r="C5" s="314"/>
-      <c r="D5" s="314"/>
-      <c r="E5" s="314"/>
-      <c r="F5" s="314"/>
-      <c r="G5" s="314"/>
-      <c r="H5" s="314"/>
-      <c r="I5" s="314"/>
-      <c r="J5" s="314"/>
-      <c r="K5" s="314"/>
-      <c r="M5" s="314" t="s">
+      <c r="B5" s="326"/>
+      <c r="C5" s="326"/>
+      <c r="D5" s="326"/>
+      <c r="E5" s="326"/>
+      <c r="F5" s="326"/>
+      <c r="G5" s="326"/>
+      <c r="H5" s="326"/>
+      <c r="I5" s="326"/>
+      <c r="J5" s="326"/>
+      <c r="K5" s="326"/>
+      <c r="M5" s="326" t="s">
         <v>324</v>
       </c>
-      <c r="N5" s="314"/>
-      <c r="O5" s="314"/>
-      <c r="P5" s="314"/>
-      <c r="Q5" s="314"/>
-      <c r="R5" s="314"/>
-      <c r="S5" s="314"/>
-      <c r="T5" s="314"/>
-      <c r="U5" s="314"/>
-      <c r="V5" s="314"/>
-      <c r="W5" s="314"/>
+      <c r="N5" s="326"/>
+      <c r="O5" s="326"/>
+      <c r="P5" s="326"/>
+      <c r="Q5" s="326"/>
+      <c r="R5" s="326"/>
+      <c r="S5" s="326"/>
+      <c r="T5" s="326"/>
+      <c r="U5" s="326"/>
+      <c r="V5" s="326"/>
+      <c r="W5" s="326"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="314"/>
-      <c r="B6" s="314"/>
-      <c r="C6" s="314"/>
-      <c r="D6" s="314"/>
-      <c r="E6" s="314"/>
-      <c r="F6" s="314"/>
-      <c r="G6" s="314"/>
-      <c r="H6" s="314"/>
-      <c r="I6" s="314"/>
-      <c r="J6" s="314"/>
-      <c r="K6" s="314"/>
-      <c r="M6" s="314"/>
-      <c r="N6" s="314"/>
-      <c r="O6" s="314"/>
-      <c r="P6" s="314"/>
-      <c r="Q6" s="314"/>
-      <c r="R6" s="314"/>
-      <c r="S6" s="314"/>
-      <c r="T6" s="314"/>
-      <c r="U6" s="314"/>
-      <c r="V6" s="314"/>
-      <c r="W6" s="314"/>
+      <c r="A6" s="326"/>
+      <c r="B6" s="326"/>
+      <c r="C6" s="326"/>
+      <c r="D6" s="326"/>
+      <c r="E6" s="326"/>
+      <c r="F6" s="326"/>
+      <c r="G6" s="326"/>
+      <c r="H6" s="326"/>
+      <c r="I6" s="326"/>
+      <c r="J6" s="326"/>
+      <c r="K6" s="326"/>
+      <c r="M6" s="326"/>
+      <c r="N6" s="326"/>
+      <c r="O6" s="326"/>
+      <c r="P6" s="326"/>
+      <c r="Q6" s="326"/>
+      <c r="R6" s="326"/>
+      <c r="S6" s="326"/>
+      <c r="T6" s="326"/>
+      <c r="U6" s="326"/>
+      <c r="V6" s="326"/>
+      <c r="W6" s="326"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M7" s="249"/>
@@ -15975,8 +15978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:P75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16502,39 +16505,63 @@
       <c r="B26" s="57">
         <v>23</v>
       </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
+      <c r="C26" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="E26" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="F26" s="57" t="s">
+        <v>379</v>
+      </c>
       <c r="G26" s="56">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="57">
         <v>24</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
+      <c r="C27" s="57" t="s">
+        <v>384</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>352</v>
+      </c>
+      <c r="E27" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="F27" s="57" t="s">
+        <v>379</v>
+      </c>
       <c r="G27" s="56">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>125000</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="57">
         <v>25</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
+      <c r="C28" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" s="57" t="s">
+        <v>372</v>
+      </c>
+      <c r="E28" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="F28" s="57" t="s">
+        <v>379</v>
+      </c>
       <c r="G28" s="56">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -16690,38 +16717,38 @@
       <c r="F40" s="344"/>
       <c r="G40" s="286">
         <f>SUM(G4:G39)</f>
-        <v>2750000</v>
+        <v>3125000</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="314" t="s">
+      <c r="B44" s="326" t="s">
         <v>366</v>
       </c>
-      <c r="C44" s="314"/>
-      <c r="D44" s="314"/>
-      <c r="E44" s="314"/>
-      <c r="F44" s="314"/>
-      <c r="G44" s="314"/>
-      <c r="H44" s="314"/>
-      <c r="I44" s="314"/>
-      <c r="J44" s="314"/>
-      <c r="K44" s="314"/>
-      <c r="L44" s="314"/>
-      <c r="M44" s="314"/>
+      <c r="C44" s="326"/>
+      <c r="D44" s="326"/>
+      <c r="E44" s="326"/>
+      <c r="F44" s="326"/>
+      <c r="G44" s="326"/>
+      <c r="H44" s="326"/>
+      <c r="I44" s="326"/>
+      <c r="J44" s="326"/>
+      <c r="K44" s="326"/>
+      <c r="L44" s="326"/>
+      <c r="M44" s="326"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="314"/>
-      <c r="C45" s="314"/>
-      <c r="D45" s="314"/>
-      <c r="E45" s="314"/>
-      <c r="F45" s="314"/>
-      <c r="G45" s="314"/>
-      <c r="H45" s="314"/>
-      <c r="I45" s="314"/>
-      <c r="J45" s="314"/>
-      <c r="K45" s="314"/>
-      <c r="L45" s="314"/>
-      <c r="M45" s="314"/>
+      <c r="B45" s="326"/>
+      <c r="C45" s="326"/>
+      <c r="D45" s="326"/>
+      <c r="E45" s="326"/>
+      <c r="F45" s="326"/>
+      <c r="G45" s="326"/>
+      <c r="H45" s="326"/>
+      <c r="I45" s="326"/>
+      <c r="J45" s="326"/>
+      <c r="K45" s="326"/>
+      <c r="L45" s="326"/>
+      <c r="M45" s="326"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="277"/>
@@ -16830,7 +16857,7 @@
       <c r="F50" s="283"/>
       <c r="G50" s="210">
         <f>G40</f>
-        <v>2750000</v>
+        <v>3125000</v>
       </c>
       <c r="H50" s="210"/>
       <c r="I50" s="277"/>
@@ -17217,7 +17244,7 @@
       <c r="F73" s="222"/>
       <c r="G73" s="223">
         <f>SUM(G48:G72)</f>
-        <v>4750000</v>
+        <v>5125000</v>
       </c>
       <c r="H73" s="224">
         <f>SUM(H48:H72)</f>
@@ -17239,7 +17266,7 @@
       <c r="F74" s="281"/>
       <c r="G74" s="330">
         <f>G73-H73</f>
-        <v>4250000</v>
+        <v>4625000</v>
       </c>
       <c r="H74" s="331"/>
       <c r="I74" s="277"/>
@@ -17340,17 +17367,17 @@
       <c r="A2" s="172"/>
       <c r="B2" s="173"/>
       <c r="C2" s="173"/>
-      <c r="D2" s="402" t="s">
+      <c r="D2" s="345" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="402"/>
-      <c r="F2" s="402"/>
-      <c r="G2" s="402"/>
-      <c r="H2" s="402"/>
-      <c r="I2" s="402"/>
-      <c r="J2" s="402"/>
-      <c r="K2" s="402"/>
-      <c r="L2" s="402"/>
+      <c r="E2" s="345"/>
+      <c r="F2" s="345"/>
+      <c r="G2" s="345"/>
+      <c r="H2" s="345"/>
+      <c r="I2" s="345"/>
+      <c r="J2" s="345"/>
+      <c r="K2" s="345"/>
+      <c r="L2" s="345"/>
       <c r="M2" s="174"/>
       <c r="N2" s="24"/>
     </row>
@@ -17368,205 +17395,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="176"/>
-      <c r="U3" s="345" t="s">
+      <c r="U3" s="395" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="346"/>
-      <c r="W3" s="347" t="s">
+      <c r="V3" s="396"/>
+      <c r="W3" s="397" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="346"/>
-      <c r="Y3" s="346"/>
-      <c r="Z3" s="346"/>
-      <c r="AA3" s="346"/>
-      <c r="AB3" s="346"/>
-      <c r="AC3" s="346"/>
-      <c r="AD3" s="348"/>
+      <c r="X3" s="396"/>
+      <c r="Y3" s="396"/>
+      <c r="Z3" s="396"/>
+      <c r="AA3" s="396"/>
+      <c r="AB3" s="396"/>
+      <c r="AC3" s="396"/>
+      <c r="AD3" s="398"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="175"/>
-      <c r="B4" s="406" t="s">
+      <c r="B4" s="360" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="407"/>
-      <c r="D4" s="407"/>
-      <c r="E4" s="407"/>
-      <c r="F4" s="407"/>
+      <c r="C4" s="361"/>
+      <c r="D4" s="361"/>
+      <c r="E4" s="361"/>
+      <c r="F4" s="361"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="354" t="s">
+      <c r="I4" s="364" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="320"/>
-      <c r="K4" s="320"/>
-      <c r="L4" s="320"/>
+      <c r="J4" s="317"/>
+      <c r="K4" s="317"/>
+      <c r="L4" s="317"/>
       <c r="M4" s="176"/>
-      <c r="U4" s="366" t="s">
+      <c r="U4" s="407" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="320"/>
-      <c r="W4" s="354" t="s">
+      <c r="V4" s="317"/>
+      <c r="W4" s="364" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="320"/>
-      <c r="Y4" s="320"/>
-      <c r="Z4" s="320"/>
-      <c r="AA4" s="320"/>
-      <c r="AB4" s="320"/>
-      <c r="AC4" s="320"/>
-      <c r="AD4" s="349"/>
+      <c r="X4" s="317"/>
+      <c r="Y4" s="317"/>
+      <c r="Z4" s="317"/>
+      <c r="AA4" s="317"/>
+      <c r="AB4" s="317"/>
+      <c r="AC4" s="317"/>
+      <c r="AD4" s="384"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="175"/>
-      <c r="B5" s="371" t="s">
+      <c r="B5" s="355" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="320"/>
-      <c r="D5" s="320"/>
-      <c r="E5" s="320"/>
-      <c r="F5" s="320"/>
+      <c r="C5" s="317"/>
+      <c r="D5" s="317"/>
+      <c r="E5" s="317"/>
+      <c r="F5" s="317"/>
       <c r="G5" s="152">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="373" t="s">
+      <c r="I5" s="353" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="394"/>
-      <c r="K5" s="396">
+      <c r="J5" s="354"/>
+      <c r="K5" s="365">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="397"/>
+      <c r="L5" s="366"/>
       <c r="M5" s="176"/>
-      <c r="U5" s="367" t="s">
+      <c r="U5" s="391" t="s">
         <v>231</v>
       </c>
-      <c r="V5" s="368"/>
-      <c r="W5" s="373" t="s">
+      <c r="V5" s="392"/>
+      <c r="W5" s="353" t="s">
         <v>232</v>
       </c>
-      <c r="X5" s="374"/>
-      <c r="Y5" s="374"/>
-      <c r="Z5" s="374"/>
-      <c r="AA5" s="374"/>
-      <c r="AB5" s="374"/>
-      <c r="AC5" s="374"/>
-      <c r="AD5" s="375"/>
+      <c r="X5" s="378"/>
+      <c r="Y5" s="378"/>
+      <c r="Z5" s="378"/>
+      <c r="AA5" s="378"/>
+      <c r="AB5" s="378"/>
+      <c r="AC5" s="378"/>
+      <c r="AD5" s="379"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="175"/>
-      <c r="B6" s="364" t="s">
+      <c r="B6" s="347" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="365"/>
-      <c r="D6" s="365"/>
-      <c r="E6" s="365"/>
-      <c r="F6" s="365"/>
+      <c r="C6" s="348"/>
+      <c r="D6" s="348"/>
+      <c r="E6" s="348"/>
+      <c r="F6" s="348"/>
       <c r="G6" s="152">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="395" t="s">
+      <c r="I6" s="351" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="390"/>
-      <c r="K6" s="398">
+      <c r="J6" s="352"/>
+      <c r="K6" s="367">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="399"/>
+      <c r="L6" s="368"/>
       <c r="M6" s="176"/>
-      <c r="U6" s="369"/>
-      <c r="V6" s="370"/>
-      <c r="W6" s="355" t="s">
+      <c r="U6" s="393"/>
+      <c r="V6" s="394"/>
+      <c r="W6" s="380" t="s">
         <v>233</v>
       </c>
-      <c r="X6" s="356"/>
-      <c r="Y6" s="356"/>
-      <c r="Z6" s="356"/>
-      <c r="AA6" s="356"/>
-      <c r="AB6" s="356"/>
-      <c r="AC6" s="356"/>
-      <c r="AD6" s="357"/>
+      <c r="X6" s="381"/>
+      <c r="Y6" s="381"/>
+      <c r="Z6" s="381"/>
+      <c r="AA6" s="381"/>
+      <c r="AB6" s="381"/>
+      <c r="AC6" s="381"/>
+      <c r="AD6" s="382"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="175"/>
-      <c r="B7" s="376" t="s">
+      <c r="B7" s="358" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="377"/>
-      <c r="D7" s="377"/>
-      <c r="E7" s="377"/>
-      <c r="F7" s="390"/>
+      <c r="C7" s="359"/>
+      <c r="D7" s="359"/>
+      <c r="E7" s="359"/>
+      <c r="F7" s="352"/>
       <c r="G7" s="152">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="395" t="s">
+      <c r="I7" s="351" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="390"/>
-      <c r="K7" s="400">
+      <c r="J7" s="352"/>
+      <c r="K7" s="362">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="401"/>
+      <c r="L7" s="363"/>
       <c r="M7" s="176"/>
-      <c r="U7" s="352"/>
-      <c r="V7" s="353"/>
-      <c r="W7" s="354" t="s">
+      <c r="U7" s="399"/>
+      <c r="V7" s="400"/>
+      <c r="W7" s="364" t="s">
         <v>234</v>
       </c>
-      <c r="X7" s="320"/>
-      <c r="Y7" s="320"/>
-      <c r="Z7" s="320"/>
-      <c r="AA7" s="320"/>
-      <c r="AB7" s="320"/>
-      <c r="AC7" s="320"/>
-      <c r="AD7" s="349"/>
+      <c r="X7" s="317"/>
+      <c r="Y7" s="317"/>
+      <c r="Z7" s="317"/>
+      <c r="AA7" s="317"/>
+      <c r="AB7" s="317"/>
+      <c r="AC7" s="317"/>
+      <c r="AD7" s="384"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="175"/>
-      <c r="B8" s="404" t="s">
+      <c r="B8" s="356" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="405"/>
-      <c r="D8" s="405"/>
-      <c r="E8" s="405"/>
-      <c r="F8" s="405"/>
+      <c r="C8" s="357"/>
+      <c r="D8" s="357"/>
+      <c r="E8" s="357"/>
+      <c r="F8" s="357"/>
       <c r="G8" s="153">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="373" t="s">
+      <c r="I8" s="353" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="394"/>
-      <c r="K8" s="385">
+      <c r="J8" s="354"/>
+      <c r="K8" s="349">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="386"/>
+      <c r="L8" s="350"/>
       <c r="M8" s="176"/>
-      <c r="U8" s="360" t="s">
+      <c r="U8" s="403" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="361"/>
-      <c r="W8" s="355" t="s">
+      <c r="V8" s="404"/>
+      <c r="W8" s="380" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="356"/>
-      <c r="Y8" s="356"/>
-      <c r="Z8" s="356"/>
-      <c r="AA8" s="356"/>
-      <c r="AB8" s="356"/>
-      <c r="AC8" s="356"/>
-      <c r="AD8" s="357"/>
+      <c r="X8" s="381"/>
+      <c r="Y8" s="381"/>
+      <c r="Z8" s="381"/>
+      <c r="AA8" s="381"/>
+      <c r="AB8" s="381"/>
+      <c r="AC8" s="381"/>
+      <c r="AD8" s="382"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="175"/>
@@ -17582,28 +17609,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="176"/>
-      <c r="U9" s="362"/>
-      <c r="V9" s="363"/>
-      <c r="W9" s="355" t="s">
+      <c r="U9" s="405"/>
+      <c r="V9" s="406"/>
+      <c r="W9" s="380" t="s">
         <v>237</v>
       </c>
-      <c r="X9" s="356"/>
-      <c r="Y9" s="356"/>
-      <c r="Z9" s="356"/>
-      <c r="AA9" s="356"/>
-      <c r="AB9" s="356"/>
-      <c r="AC9" s="356"/>
-      <c r="AD9" s="357"/>
+      <c r="X9" s="381"/>
+      <c r="Y9" s="381"/>
+      <c r="Z9" s="381"/>
+      <c r="AA9" s="381"/>
+      <c r="AB9" s="381"/>
+      <c r="AC9" s="381"/>
+      <c r="AD9" s="382"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="175"/>
-      <c r="B10" s="320" t="s">
+      <c r="B10" s="317" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="320"/>
-      <c r="D10" s="320"/>
-      <c r="E10" s="320"/>
-      <c r="F10" s="320"/>
+      <c r="C10" s="317"/>
+      <c r="D10" s="317"/>
+      <c r="E10" s="317"/>
+      <c r="F10" s="317"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -17614,30 +17641,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="176"/>
-      <c r="U10" s="364" t="s">
+      <c r="U10" s="347" t="s">
         <v>243</v>
       </c>
-      <c r="V10" s="365"/>
-      <c r="W10" s="320" t="s">
+      <c r="V10" s="348"/>
+      <c r="W10" s="317" t="s">
         <v>257</v>
       </c>
-      <c r="X10" s="320"/>
-      <c r="Y10" s="320"/>
-      <c r="Z10" s="320"/>
-      <c r="AA10" s="320"/>
-      <c r="AB10" s="320"/>
-      <c r="AC10" s="320"/>
-      <c r="AD10" s="349"/>
+      <c r="X10" s="317"/>
+      <c r="Y10" s="317"/>
+      <c r="Z10" s="317"/>
+      <c r="AA10" s="317"/>
+      <c r="AB10" s="317"/>
+      <c r="AC10" s="317"/>
+      <c r="AD10" s="384"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="175"/>
-      <c r="B11" s="320" t="s">
+      <c r="B11" s="317" t="s">
         <v>254</v>
       </c>
-      <c r="C11" s="320"/>
-      <c r="D11" s="320"/>
-      <c r="E11" s="320"/>
-      <c r="F11" s="320"/>
+      <c r="C11" s="317"/>
+      <c r="D11" s="317"/>
+      <c r="E11" s="317"/>
+      <c r="F11" s="317"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -17647,30 +17674,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="176"/>
-      <c r="U11" s="364" t="s">
+      <c r="U11" s="347" t="s">
         <v>256</v>
       </c>
-      <c r="V11" s="365"/>
-      <c r="W11" s="358" t="s">
+      <c r="V11" s="348"/>
+      <c r="W11" s="401" t="s">
         <v>258</v>
       </c>
-      <c r="X11" s="358"/>
-      <c r="Y11" s="358"/>
-      <c r="Z11" s="358"/>
-      <c r="AA11" s="358"/>
-      <c r="AB11" s="358"/>
-      <c r="AC11" s="358"/>
-      <c r="AD11" s="359"/>
+      <c r="X11" s="401"/>
+      <c r="Y11" s="401"/>
+      <c r="Z11" s="401"/>
+      <c r="AA11" s="401"/>
+      <c r="AB11" s="401"/>
+      <c r="AC11" s="401"/>
+      <c r="AD11" s="402"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="175"/>
-      <c r="B12" s="403" t="s">
+      <c r="B12" s="346" t="s">
         <v>255</v>
       </c>
-      <c r="C12" s="403"/>
-      <c r="D12" s="403"/>
-      <c r="E12" s="403"/>
-      <c r="F12" s="403"/>
+      <c r="C12" s="346"/>
+      <c r="D12" s="346"/>
+      <c r="E12" s="346"/>
+      <c r="F12" s="346"/>
       <c r="G12" s="180">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -17681,16 +17708,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="176"/>
-      <c r="U12" s="364"/>
-      <c r="V12" s="365"/>
-      <c r="W12" s="320"/>
-      <c r="X12" s="320"/>
-      <c r="Y12" s="320"/>
-      <c r="Z12" s="320"/>
-      <c r="AA12" s="320"/>
-      <c r="AB12" s="320"/>
-      <c r="AC12" s="320"/>
-      <c r="AD12" s="349"/>
+      <c r="U12" s="347"/>
+      <c r="V12" s="348"/>
+      <c r="W12" s="317"/>
+      <c r="X12" s="317"/>
+      <c r="Y12" s="317"/>
+      <c r="Z12" s="317"/>
+      <c r="AA12" s="317"/>
+      <c r="AB12" s="317"/>
+      <c r="AC12" s="317"/>
+      <c r="AD12" s="384"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="177"/>
@@ -17706,64 +17733,64 @@
       <c r="K13" s="178"/>
       <c r="L13" s="178"/>
       <c r="M13" s="179"/>
-      <c r="U13" s="364"/>
-      <c r="V13" s="365"/>
-      <c r="W13" s="320"/>
-      <c r="X13" s="320"/>
-      <c r="Y13" s="320"/>
-      <c r="Z13" s="320"/>
-      <c r="AA13" s="320"/>
-      <c r="AB13" s="320"/>
-      <c r="AC13" s="320"/>
-      <c r="AD13" s="349"/>
+      <c r="U13" s="347"/>
+      <c r="V13" s="348"/>
+      <c r="W13" s="317"/>
+      <c r="X13" s="317"/>
+      <c r="Y13" s="317"/>
+      <c r="Z13" s="317"/>
+      <c r="AA13" s="317"/>
+      <c r="AB13" s="317"/>
+      <c r="AC13" s="317"/>
+      <c r="AD13" s="384"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="379"/>
-      <c r="V14" s="380"/>
-      <c r="W14" s="350"/>
-      <c r="X14" s="350"/>
-      <c r="Y14" s="350"/>
-      <c r="Z14" s="350"/>
-      <c r="AA14" s="350"/>
-      <c r="AB14" s="350"/>
-      <c r="AC14" s="350"/>
-      <c r="AD14" s="351"/>
+      <c r="U14" s="385"/>
+      <c r="V14" s="386"/>
+      <c r="W14" s="376"/>
+      <c r="X14" s="376"/>
+      <c r="Y14" s="376"/>
+      <c r="Z14" s="376"/>
+      <c r="AA14" s="376"/>
+      <c r="AB14" s="376"/>
+      <c r="AC14" s="376"/>
+      <c r="AD14" s="377"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="172"/>
       <c r="B18" s="173"/>
       <c r="C18" s="173"/>
-      <c r="D18" s="402" t="s">
+      <c r="D18" s="345" t="s">
         <v>249</v>
       </c>
-      <c r="E18" s="402"/>
-      <c r="F18" s="402"/>
-      <c r="G18" s="402"/>
-      <c r="H18" s="402"/>
-      <c r="I18" s="402"/>
-      <c r="J18" s="402"/>
-      <c r="K18" s="402"/>
-      <c r="L18" s="402"/>
+      <c r="E18" s="345"/>
+      <c r="F18" s="345"/>
+      <c r="G18" s="345"/>
+      <c r="H18" s="345"/>
+      <c r="I18" s="345"/>
+      <c r="J18" s="345"/>
+      <c r="K18" s="345"/>
+      <c r="L18" s="345"/>
       <c r="M18" s="174"/>
-      <c r="O18" s="381" t="s">
+      <c r="O18" s="387" t="s">
         <v>250</v>
       </c>
-      <c r="P18" s="382"/>
-      <c r="Q18" s="382"/>
-      <c r="R18" s="382"/>
-      <c r="S18" s="383"/>
+      <c r="P18" s="388"/>
+      <c r="Q18" s="388"/>
+      <c r="R18" s="388"/>
+      <c r="S18" s="389"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="175"/>
       <c r="M19" s="176"/>
-      <c r="O19" s="371" t="s">
+      <c r="O19" s="355" t="s">
         <v>251</v>
       </c>
-      <c r="P19" s="320"/>
-      <c r="Q19" s="320"/>
-      <c r="R19" s="320"/>
-      <c r="S19" s="349"/>
+      <c r="P19" s="317"/>
+      <c r="Q19" s="317"/>
+      <c r="R19" s="317"/>
+      <c r="S19" s="384"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="175"/>
@@ -17774,119 +17801,119 @@
       <c r="F20" s="200"/>
       <c r="G20" s="68"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="354" t="s">
+      <c r="I20" s="364" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="320"/>
-      <c r="K20" s="320"/>
-      <c r="L20" s="320"/>
+      <c r="J20" s="317"/>
+      <c r="K20" s="317"/>
+      <c r="L20" s="317"/>
       <c r="M20" s="176"/>
-      <c r="O20" s="371" t="s">
+      <c r="O20" s="355" t="s">
         <v>252</v>
       </c>
-      <c r="P20" s="320"/>
-      <c r="Q20" s="320"/>
-      <c r="R20" s="320"/>
-      <c r="S20" s="349"/>
+      <c r="P20" s="317"/>
+      <c r="Q20" s="317"/>
+      <c r="R20" s="317"/>
+      <c r="S20" s="384"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="175"/>
-      <c r="B21" s="387" t="s">
+      <c r="B21" s="369" t="s">
         <v>296</v>
       </c>
-      <c r="C21" s="388"/>
-      <c r="D21" s="388"/>
-      <c r="E21" s="388"/>
-      <c r="F21" s="389"/>
+      <c r="C21" s="370"/>
+      <c r="D21" s="370"/>
+      <c r="E21" s="370"/>
+      <c r="F21" s="371"/>
       <c r="G21" s="70">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="373" t="s">
+      <c r="I21" s="353" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="394"/>
-      <c r="K21" s="396">
+      <c r="J21" s="354"/>
+      <c r="K21" s="365">
         <f>G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="L21" s="397"/>
+      <c r="L21" s="366"/>
       <c r="M21" s="176"/>
       <c r="N21" s="170"/>
-      <c r="O21" s="384" t="s">
+      <c r="O21" s="390" t="s">
         <v>259</v>
       </c>
-      <c r="P21" s="374"/>
-      <c r="Q21" s="374"/>
-      <c r="R21" s="374"/>
-      <c r="S21" s="375"/>
+      <c r="P21" s="378"/>
+      <c r="Q21" s="378"/>
+      <c r="R21" s="378"/>
+      <c r="S21" s="379"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="175"/>
-      <c r="B22" s="376" t="s">
+      <c r="B22" s="358" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="377"/>
-      <c r="D22" s="377"/>
-      <c r="E22" s="377"/>
-      <c r="F22" s="390"/>
+      <c r="C22" s="359"/>
+      <c r="D22" s="359"/>
+      <c r="E22" s="359"/>
+      <c r="F22" s="352"/>
       <c r="G22" s="152">
         <f>G21</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="395" t="s">
+      <c r="I22" s="351" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="390"/>
-      <c r="K22" s="398">
+      <c r="J22" s="352"/>
+      <c r="K22" s="367">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="L22" s="399"/>
+      <c r="L22" s="368"/>
       <c r="M22" s="176"/>
       <c r="N22" s="170"/>
-      <c r="O22" s="376" t="s">
+      <c r="O22" s="358" t="s">
         <v>260</v>
       </c>
-      <c r="P22" s="377"/>
-      <c r="Q22" s="377"/>
-      <c r="R22" s="377"/>
-      <c r="S22" s="378"/>
+      <c r="P22" s="359"/>
+      <c r="Q22" s="359"/>
+      <c r="R22" s="359"/>
+      <c r="S22" s="383"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="175"/>
-      <c r="B23" s="391" t="s">
+      <c r="B23" s="372" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="392"/>
-      <c r="D23" s="392"/>
-      <c r="E23" s="392"/>
-      <c r="F23" s="393"/>
+      <c r="C23" s="373"/>
+      <c r="D23" s="373"/>
+      <c r="E23" s="373"/>
+      <c r="F23" s="374"/>
       <c r="G23" s="153">
         <f>K24</f>
         <v>1568729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="395" t="s">
+      <c r="I23" s="351" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="390"/>
-      <c r="K23" s="400">
+      <c r="J23" s="352"/>
+      <c r="K23" s="362">
         <f>Pemasukkan!L31</f>
         <v>690000</v>
       </c>
-      <c r="L23" s="401"/>
+      <c r="L23" s="363"/>
       <c r="M23" s="176"/>
       <c r="N23" s="170"/>
-      <c r="O23" s="376" t="s">
+      <c r="O23" s="358" t="s">
         <v>261</v>
       </c>
-      <c r="P23" s="377"/>
-      <c r="Q23" s="377"/>
-      <c r="R23" s="377"/>
-      <c r="S23" s="378"/>
+      <c r="P23" s="359"/>
+      <c r="Q23" s="359"/>
+      <c r="R23" s="359"/>
+      <c r="S23" s="383"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="175"/>
@@ -17897,24 +17924,24 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="373" t="s">
+      <c r="I24" s="353" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="394"/>
-      <c r="K24" s="385">
+      <c r="J24" s="354"/>
+      <c r="K24" s="349">
         <f>(K21-K22)+K23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="L24" s="386"/>
+      <c r="L24" s="350"/>
       <c r="M24" s="176"/>
       <c r="N24" s="170"/>
-      <c r="O24" s="376" t="s">
+      <c r="O24" s="358" t="s">
         <v>262</v>
       </c>
-      <c r="P24" s="377"/>
-      <c r="Q24" s="377"/>
-      <c r="R24" s="377"/>
-      <c r="S24" s="378"/>
+      <c r="P24" s="359"/>
+      <c r="Q24" s="359"/>
+      <c r="R24" s="359"/>
+      <c r="S24" s="383"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="175"/>
@@ -17931,13 +17958,13 @@
       <c r="L25" s="24"/>
       <c r="M25" s="176"/>
       <c r="N25" s="170"/>
-      <c r="O25" s="371" t="s">
+      <c r="O25" s="355" t="s">
         <v>267</v>
       </c>
-      <c r="P25" s="320"/>
-      <c r="Q25" s="320"/>
-      <c r="R25" s="320"/>
-      <c r="S25" s="349"/>
+      <c r="P25" s="317"/>
+      <c r="Q25" s="317"/>
+      <c r="R25" s="317"/>
+      <c r="S25" s="384"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="175"/>
@@ -17954,11 +17981,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="176"/>
       <c r="N26" s="170"/>
-      <c r="O26" s="372"/>
-      <c r="P26" s="350"/>
-      <c r="Q26" s="350"/>
-      <c r="R26" s="350"/>
-      <c r="S26" s="351"/>
+      <c r="O26" s="375"/>
+      <c r="P26" s="376"/>
+      <c r="Q26" s="376"/>
+      <c r="R26" s="376"/>
+      <c r="S26" s="377"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="177"/>
@@ -17993,6 +18020,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:AD3"/>
+    <mergeCell ref="W12:AD12"/>
+    <mergeCell ref="W13:AD13"/>
+    <mergeCell ref="W14:AD14"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:AD7"/>
+    <mergeCell ref="W9:AD9"/>
+    <mergeCell ref="W10:AD10"/>
+    <mergeCell ref="W11:AD11"/>
+    <mergeCell ref="U8:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:AD4"/>
+    <mergeCell ref="W8:AD8"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="O25:S25"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="W5:AD5"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="O18:S18"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O23:S23"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
     <mergeCell ref="D2:L2"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
@@ -18009,53 +18083,6 @@
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="W5:AD5"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="O24:S24"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="O18:S18"/>
-    <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O23:S23"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="W4:AD4"/>
-    <mergeCell ref="W8:AD8"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="O25:S25"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:AD3"/>
-    <mergeCell ref="W12:AD12"/>
-    <mergeCell ref="W13:AD13"/>
-    <mergeCell ref="W14:AD14"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="W7:AD7"/>
-    <mergeCell ref="W9:AD9"/>
-    <mergeCell ref="W10:AD10"/>
-    <mergeCell ref="W11:AD11"/>
-    <mergeCell ref="U8:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U4:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -18089,44 +18116,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="417" t="s">
+      <c r="C2" s="408" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="418"/>
-      <c r="E2" s="418"/>
-      <c r="F2" s="418"/>
-      <c r="G2" s="418"/>
-      <c r="H2" s="418"/>
-      <c r="I2" s="418"/>
-      <c r="J2" s="418"/>
-      <c r="K2" s="418"/>
+      <c r="D2" s="409"/>
+      <c r="E2" s="409"/>
+      <c r="F2" s="409"/>
+      <c r="G2" s="409"/>
+      <c r="H2" s="409"/>
+      <c r="I2" s="409"/>
+      <c r="J2" s="409"/>
+      <c r="K2" s="409"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="418"/>
-      <c r="D3" s="418"/>
-      <c r="E3" s="418"/>
-      <c r="F3" s="418"/>
-      <c r="G3" s="418"/>
-      <c r="H3" s="418"/>
-      <c r="I3" s="418"/>
-      <c r="J3" s="418"/>
-      <c r="K3" s="418"/>
+      <c r="C3" s="409"/>
+      <c r="D3" s="409"/>
+      <c r="E3" s="409"/>
+      <c r="F3" s="409"/>
+      <c r="G3" s="409"/>
+      <c r="H3" s="409"/>
+      <c r="I3" s="409"/>
+      <c r="J3" s="409"/>
+      <c r="K3" s="409"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="410" t="s">
+      <c r="C5" s="416" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="410"/>
-      <c r="E5" s="410"/>
-      <c r="F5" s="410"/>
-      <c r="G5" s="410"/>
-      <c r="I5" s="410" t="s">
+      <c r="D5" s="416"/>
+      <c r="E5" s="416"/>
+      <c r="F5" s="416"/>
+      <c r="G5" s="416"/>
+      <c r="I5" s="416" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="410"/>
-      <c r="K5" s="410"/>
-      <c r="L5" s="410"/>
-      <c r="M5" s="410"/>
+      <c r="J5" s="416"/>
+      <c r="K5" s="416"/>
+      <c r="L5" s="416"/>
+      <c r="M5" s="416"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -18566,88 +18593,88 @@
       <c r="M28" s="170"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="406" t="s">
+      <c r="D29" s="360" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="407"/>
-      <c r="F29" s="411">
+      <c r="E29" s="361"/>
+      <c r="F29" s="410">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="412"/>
+      <c r="G29" s="411"/>
       <c r="I29" s="170"/>
-      <c r="J29" s="406" t="s">
+      <c r="J29" s="360" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="407"/>
-      <c r="L29" s="411">
+      <c r="K29" s="361"/>
+      <c r="L29" s="410">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="412"/>
+      <c r="M29" s="411"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="366" t="s">
+      <c r="D30" s="407" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="320"/>
-      <c r="F30" s="413">
+      <c r="E30" s="317"/>
+      <c r="F30" s="412">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="414"/>
+      <c r="G30" s="413"/>
       <c r="I30" s="170"/>
-      <c r="J30" s="366" t="s">
+      <c r="J30" s="407" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="320"/>
-      <c r="L30" s="413">
+      <c r="K30" s="317"/>
+      <c r="L30" s="412">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="414"/>
+      <c r="M30" s="413"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="371" t="s">
+      <c r="D31" s="355" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="320"/>
-      <c r="F31" s="415">
+      <c r="E31" s="317"/>
+      <c r="F31" s="417">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="416"/>
+      <c r="G31" s="418"/>
       <c r="I31" s="170"/>
-      <c r="J31" s="371" t="s">
+      <c r="J31" s="355" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="320"/>
-      <c r="L31" s="415">
+      <c r="K31" s="317"/>
+      <c r="L31" s="417">
         <f>L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="416"/>
+      <c r="M31" s="418"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="404" t="s">
+      <c r="D32" s="356" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="405"/>
-      <c r="F32" s="408">
+      <c r="E32" s="357"/>
+      <c r="F32" s="414">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="409"/>
+      <c r="G32" s="415"/>
       <c r="I32" s="170"/>
-      <c r="J32" s="404" t="s">
+      <c r="J32" s="356" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="405"/>
-      <c r="L32" s="408">
+      <c r="K32" s="357"/>
+      <c r="L32" s="414">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="409"/>
+      <c r="M32" s="415"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18839,12 +18866,6 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C2:K3"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J29:K29"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="I5:M5"/>
@@ -18858,6 +18879,12 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J32:K32"/>
+    <mergeCell ref="C2:K3"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -18890,44 +18917,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="423" t="s">
+      <c r="C2" s="419" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="424"/>
-      <c r="E2" s="424"/>
-      <c r="F2" s="424"/>
-      <c r="G2" s="424"/>
-      <c r="H2" s="424"/>
-      <c r="I2" s="424"/>
-      <c r="J2" s="424"/>
-      <c r="K2" s="424"/>
+      <c r="D2" s="420"/>
+      <c r="E2" s="420"/>
+      <c r="F2" s="420"/>
+      <c r="G2" s="420"/>
+      <c r="H2" s="420"/>
+      <c r="I2" s="420"/>
+      <c r="J2" s="420"/>
+      <c r="K2" s="420"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="424"/>
-      <c r="D3" s="424"/>
-      <c r="E3" s="424"/>
-      <c r="F3" s="424"/>
-      <c r="G3" s="424"/>
-      <c r="H3" s="424"/>
-      <c r="I3" s="424"/>
-      <c r="J3" s="424"/>
-      <c r="K3" s="424"/>
+      <c r="C3" s="420"/>
+      <c r="D3" s="420"/>
+      <c r="E3" s="420"/>
+      <c r="F3" s="420"/>
+      <c r="G3" s="420"/>
+      <c r="H3" s="420"/>
+      <c r="I3" s="420"/>
+      <c r="J3" s="420"/>
+      <c r="K3" s="420"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="410" t="s">
+      <c r="C5" s="416" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="410"/>
-      <c r="E5" s="410"/>
-      <c r="F5" s="410"/>
-      <c r="G5" s="410"/>
-      <c r="I5" s="410" t="s">
+      <c r="D5" s="416"/>
+      <c r="E5" s="416"/>
+      <c r="F5" s="416"/>
+      <c r="G5" s="416"/>
+      <c r="I5" s="416" t="s">
         <v>246</v>
       </c>
-      <c r="J5" s="410"/>
-      <c r="K5" s="410"/>
-      <c r="L5" s="410"/>
-      <c r="M5" s="410"/>
+      <c r="J5" s="416"/>
+      <c r="K5" s="416"/>
+      <c r="L5" s="416"/>
+      <c r="M5" s="416"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -19411,20 +19438,20 @@
       <c r="M28" s="170"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="345" t="s">
+      <c r="D29" s="395" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="347"/>
+      <c r="E29" s="397"/>
       <c r="F29" s="421">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
       <c r="G29" s="422"/>
       <c r="I29" s="170"/>
-      <c r="J29" s="345" t="s">
+      <c r="J29" s="395" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="347"/>
+      <c r="K29" s="397"/>
       <c r="L29" s="421">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
@@ -19432,67 +19459,67 @@
       <c r="M29" s="422"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="371" t="s">
+      <c r="D30" s="355" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="320"/>
-      <c r="F30" s="413">
+      <c r="E30" s="317"/>
+      <c r="F30" s="412">
         <f>F27</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="414"/>
+      <c r="G30" s="413"/>
       <c r="I30" s="170"/>
-      <c r="J30" s="371" t="s">
+      <c r="J30" s="355" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="320"/>
-      <c r="L30" s="413">
+      <c r="K30" s="317"/>
+      <c r="L30" s="412">
         <f>L27</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="414"/>
+      <c r="M30" s="413"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="371" t="s">
+      <c r="D31" s="355" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="320"/>
-      <c r="F31" s="415">
+      <c r="E31" s="317"/>
+      <c r="F31" s="417">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="416"/>
+      <c r="G31" s="418"/>
       <c r="I31" s="170"/>
-      <c r="J31" s="371" t="s">
+      <c r="J31" s="355" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="320"/>
-      <c r="L31" s="415">
+      <c r="K31" s="317"/>
+      <c r="L31" s="417">
         <f>Pemasukkan!L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="416"/>
+      <c r="M31" s="418"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="404" t="s">
+      <c r="D32" s="356" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="405"/>
-      <c r="F32" s="419">
+      <c r="E32" s="357"/>
+      <c r="F32" s="423">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="420"/>
+      <c r="G32" s="424"/>
       <c r="I32" s="170"/>
-      <c r="J32" s="404" t="s">
+      <c r="J32" s="356" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="405"/>
-      <c r="L32" s="419">
+      <c r="K32" s="357"/>
+      <c r="L32" s="423">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="420"/>
+      <c r="M32" s="424"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19684,6 +19711,14 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
     <mergeCell ref="C2:K3"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
@@ -19695,14 +19730,6 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Bayar Makrab Adit,Ilham Rasyid Adrian,Alex
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="386">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -1178,6 +1178,9 @@
   </si>
   <si>
     <t>Sulthon Muhamad Arief</t>
+  </si>
+  <si>
+    <t>Ilham Rasyid Adrian</t>
   </si>
 </sst>
 </file>
@@ -3031,20 +3034,29 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3060,39 +3072,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3100,36 +3110,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3179,193 +3182,220 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3374,31 +3404,16 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3406,18 +3421,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4672,126 +4675,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="287" t="s">
+      <c r="A1" s="293" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="288"/>
-      <c r="C1" s="288"/>
-      <c r="D1" s="288"/>
-      <c r="E1" s="288"/>
-      <c r="F1" s="288"/>
-      <c r="G1" s="288"/>
-      <c r="H1" s="288"/>
-      <c r="I1" s="288"/>
-      <c r="J1" s="288"/>
-      <c r="K1" s="288"/>
-      <c r="L1" s="288"/>
-      <c r="M1" s="288"/>
-      <c r="N1" s="288"/>
-      <c r="O1" s="288"/>
-      <c r="P1" s="288"/>
-      <c r="Q1" s="288"/>
-      <c r="R1" s="288"/>
+      <c r="B1" s="294"/>
+      <c r="C1" s="294"/>
+      <c r="D1" s="294"/>
+      <c r="E1" s="294"/>
+      <c r="F1" s="294"/>
+      <c r="G1" s="294"/>
+      <c r="H1" s="294"/>
+      <c r="I1" s="294"/>
+      <c r="J1" s="294"/>
+      <c r="K1" s="294"/>
+      <c r="L1" s="294"/>
+      <c r="M1" s="294"/>
+      <c r="N1" s="294"/>
+      <c r="O1" s="294"/>
+      <c r="P1" s="294"/>
+      <c r="Q1" s="294"/>
+      <c r="R1" s="294"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="289"/>
-      <c r="B2" s="290"/>
-      <c r="C2" s="290"/>
-      <c r="D2" s="290"/>
-      <c r="E2" s="290"/>
-      <c r="F2" s="290"/>
-      <c r="G2" s="290"/>
-      <c r="H2" s="290"/>
-      <c r="I2" s="290"/>
-      <c r="J2" s="290"/>
-      <c r="K2" s="290"/>
-      <c r="L2" s="290"/>
-      <c r="M2" s="290"/>
-      <c r="N2" s="290"/>
-      <c r="O2" s="290"/>
-      <c r="P2" s="290"/>
-      <c r="Q2" s="290"/>
-      <c r="R2" s="290"/>
+      <c r="A2" s="295"/>
+      <c r="B2" s="296"/>
+      <c r="C2" s="296"/>
+      <c r="D2" s="296"/>
+      <c r="E2" s="296"/>
+      <c r="F2" s="296"/>
+      <c r="G2" s="296"/>
+      <c r="H2" s="296"/>
+      <c r="I2" s="296"/>
+      <c r="J2" s="296"/>
+      <c r="K2" s="296"/>
+      <c r="L2" s="296"/>
+      <c r="M2" s="296"/>
+      <c r="N2" s="296"/>
+      <c r="O2" s="296"/>
+      <c r="P2" s="296"/>
+      <c r="Q2" s="296"/>
+      <c r="R2" s="296"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="289"/>
-      <c r="B3" s="290"/>
-      <c r="C3" s="290"/>
-      <c r="D3" s="290"/>
-      <c r="E3" s="290"/>
-      <c r="F3" s="290"/>
-      <c r="G3" s="290"/>
-      <c r="H3" s="290"/>
-      <c r="I3" s="290"/>
-      <c r="J3" s="290"/>
-      <c r="K3" s="290"/>
-      <c r="L3" s="290"/>
-      <c r="M3" s="290"/>
-      <c r="N3" s="290"/>
-      <c r="O3" s="290"/>
-      <c r="P3" s="290"/>
-      <c r="Q3" s="290"/>
-      <c r="R3" s="290"/>
+      <c r="A3" s="295"/>
+      <c r="B3" s="296"/>
+      <c r="C3" s="296"/>
+      <c r="D3" s="296"/>
+      <c r="E3" s="296"/>
+      <c r="F3" s="296"/>
+      <c r="G3" s="296"/>
+      <c r="H3" s="296"/>
+      <c r="I3" s="296"/>
+      <c r="J3" s="296"/>
+      <c r="K3" s="296"/>
+      <c r="L3" s="296"/>
+      <c r="M3" s="296"/>
+      <c r="N3" s="296"/>
+      <c r="O3" s="296"/>
+      <c r="P3" s="296"/>
+      <c r="Q3" s="296"/>
+      <c r="R3" s="296"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="289"/>
-      <c r="B4" s="290"/>
-      <c r="C4" s="290"/>
-      <c r="D4" s="290"/>
-      <c r="E4" s="290"/>
-      <c r="F4" s="290"/>
-      <c r="G4" s="290"/>
-      <c r="H4" s="290"/>
-      <c r="I4" s="290"/>
-      <c r="J4" s="290"/>
-      <c r="K4" s="290"/>
-      <c r="L4" s="290"/>
-      <c r="M4" s="290"/>
-      <c r="N4" s="290"/>
-      <c r="O4" s="290"/>
-      <c r="P4" s="290"/>
-      <c r="Q4" s="290"/>
-      <c r="R4" s="290"/>
+      <c r="A4" s="295"/>
+      <c r="B4" s="296"/>
+      <c r="C4" s="296"/>
+      <c r="D4" s="296"/>
+      <c r="E4" s="296"/>
+      <c r="F4" s="296"/>
+      <c r="G4" s="296"/>
+      <c r="H4" s="296"/>
+      <c r="I4" s="296"/>
+      <c r="J4" s="296"/>
+      <c r="K4" s="296"/>
+      <c r="L4" s="296"/>
+      <c r="M4" s="296"/>
+      <c r="N4" s="296"/>
+      <c r="O4" s="296"/>
+      <c r="P4" s="296"/>
+      <c r="Q4" s="296"/>
+      <c r="R4" s="296"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="289"/>
-      <c r="B5" s="290"/>
-      <c r="C5" s="290"/>
-      <c r="D5" s="290"/>
-      <c r="E5" s="290"/>
-      <c r="F5" s="290"/>
-      <c r="G5" s="290"/>
-      <c r="H5" s="290"/>
-      <c r="I5" s="290"/>
-      <c r="J5" s="290"/>
-      <c r="K5" s="290"/>
-      <c r="L5" s="290"/>
-      <c r="M5" s="290"/>
-      <c r="N5" s="290"/>
-      <c r="O5" s="290"/>
-      <c r="P5" s="290"/>
-      <c r="Q5" s="290"/>
-      <c r="R5" s="290"/>
+      <c r="A5" s="295"/>
+      <c r="B5" s="296"/>
+      <c r="C5" s="296"/>
+      <c r="D5" s="296"/>
+      <c r="E5" s="296"/>
+      <c r="F5" s="296"/>
+      <c r="G5" s="296"/>
+      <c r="H5" s="296"/>
+      <c r="I5" s="296"/>
+      <c r="J5" s="296"/>
+      <c r="K5" s="296"/>
+      <c r="L5" s="296"/>
+      <c r="M5" s="296"/>
+      <c r="N5" s="296"/>
+      <c r="O5" s="296"/>
+      <c r="P5" s="296"/>
+      <c r="Q5" s="296"/>
+      <c r="R5" s="296"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="289"/>
-      <c r="B6" s="290"/>
-      <c r="C6" s="290"/>
-      <c r="D6" s="290"/>
-      <c r="E6" s="290"/>
-      <c r="F6" s="290"/>
-      <c r="G6" s="290"/>
-      <c r="H6" s="290"/>
-      <c r="I6" s="290"/>
-      <c r="J6" s="290"/>
-      <c r="K6" s="290"/>
-      <c r="L6" s="290"/>
-      <c r="M6" s="290"/>
-      <c r="N6" s="290"/>
-      <c r="O6" s="290"/>
-      <c r="P6" s="290"/>
-      <c r="Q6" s="290"/>
-      <c r="R6" s="290"/>
+      <c r="A6" s="295"/>
+      <c r="B6" s="296"/>
+      <c r="C6" s="296"/>
+      <c r="D6" s="296"/>
+      <c r="E6" s="296"/>
+      <c r="F6" s="296"/>
+      <c r="G6" s="296"/>
+      <c r="H6" s="296"/>
+      <c r="I6" s="296"/>
+      <c r="J6" s="296"/>
+      <c r="K6" s="296"/>
+      <c r="L6" s="296"/>
+      <c r="M6" s="296"/>
+      <c r="N6" s="296"/>
+      <c r="O6" s="296"/>
+      <c r="P6" s="296"/>
+      <c r="Q6" s="296"/>
+      <c r="R6" s="296"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -7898,58 +7901,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="295" t="s">
+      <c r="J79" s="298" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="296"/>
-      <c r="L79" s="296"/>
-      <c r="M79" s="296"/>
-      <c r="N79" s="297"/>
-      <c r="P79" s="303" t="s">
+      <c r="K79" s="299"/>
+      <c r="L79" s="299"/>
+      <c r="M79" s="299"/>
+      <c r="N79" s="300"/>
+      <c r="P79" s="306" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="296"/>
-      <c r="R79" s="296"/>
-      <c r="S79" s="297"/>
+      <c r="Q79" s="299"/>
+      <c r="R79" s="299"/>
+      <c r="S79" s="300"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="298" t="s">
+      <c r="J80" s="301" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="290"/>
-      <c r="L80" s="290"/>
-      <c r="M80" s="290"/>
-      <c r="N80" s="299"/>
-      <c r="P80" s="298" t="s">
+      <c r="K80" s="296"/>
+      <c r="L80" s="296"/>
+      <c r="M80" s="296"/>
+      <c r="N80" s="302"/>
+      <c r="P80" s="301" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="290"/>
-      <c r="R80" s="290"/>
-      <c r="S80" s="299"/>
+      <c r="Q80" s="296"/>
+      <c r="R80" s="296"/>
+      <c r="S80" s="302"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="300"/>
-      <c r="K81" s="301"/>
-      <c r="L81" s="301"/>
-      <c r="M81" s="301"/>
-      <c r="N81" s="302"/>
-      <c r="P81" s="300"/>
-      <c r="Q81" s="301"/>
-      <c r="R81" s="301"/>
-      <c r="S81" s="302"/>
+      <c r="J81" s="303"/>
+      <c r="K81" s="304"/>
+      <c r="L81" s="304"/>
+      <c r="M81" s="304"/>
+      <c r="N81" s="305"/>
+      <c r="P81" s="303"/>
+      <c r="Q81" s="304"/>
+      <c r="R81" s="304"/>
+      <c r="S81" s="305"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="293" t="s">
+      <c r="J82" s="297" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="294"/>
-      <c r="L82" s="292"/>
-      <c r="M82" s="293" t="s">
+      <c r="K82" s="288"/>
+      <c r="L82" s="289"/>
+      <c r="M82" s="297" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="292"/>
-      <c r="P82" s="293"/>
-      <c r="Q82" s="292"/>
+      <c r="N82" s="289"/>
+      <c r="P82" s="297"/>
+      <c r="Q82" s="289"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -7958,38 +7961,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="304" t="s">
+      <c r="J83" s="287" t="s">
         <v>70</v>
       </c>
-      <c r="K83" s="294"/>
-      <c r="L83" s="292"/>
-      <c r="M83" s="305">
+      <c r="K83" s="288"/>
+      <c r="L83" s="289"/>
+      <c r="M83" s="290">
         <v>7350000</v>
       </c>
-      <c r="N83" s="292"/>
+      <c r="N83" s="289"/>
       <c r="P83" s="291" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="292"/>
+      <c r="Q83" s="289"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="304" t="s">
+      <c r="J84" s="287" t="s">
         <v>72</v>
       </c>
-      <c r="K84" s="294"/>
-      <c r="L84" s="292"/>
-      <c r="M84" s="306">
+      <c r="K84" s="288"/>
+      <c r="L84" s="289"/>
+      <c r="M84" s="292">
         <v>1100000</v>
       </c>
-      <c r="N84" s="292"/>
+      <c r="N84" s="289"/>
       <c r="P84" s="291" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="292"/>
+      <c r="Q84" s="289"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -7998,39 +8001,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="304" t="s">
+      <c r="J85" s="287" t="s">
         <v>75</v>
       </c>
-      <c r="K85" s="294"/>
-      <c r="L85" s="292"/>
-      <c r="M85" s="305">
+      <c r="K85" s="288"/>
+      <c r="L85" s="289"/>
+      <c r="M85" s="290">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="292"/>
+      <c r="N85" s="289"/>
       <c r="P85" s="291" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="292"/>
+      <c r="Q85" s="289"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="304" t="s">
+      <c r="J86" s="287" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="294"/>
-      <c r="L86" s="292"/>
-      <c r="M86" s="305">
+      <c r="K86" s="288"/>
+      <c r="L86" s="289"/>
+      <c r="M86" s="290">
         <v>8411850</v>
       </c>
-      <c r="N86" s="292"/>
+      <c r="N86" s="289"/>
       <c r="P86" s="291" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="292"/>
+      <c r="Q86" s="289"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -8038,20 +8041,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="304" t="s">
+      <c r="J87" s="287" t="s">
         <v>79</v>
       </c>
-      <c r="K87" s="294"/>
-      <c r="L87" s="292"/>
-      <c r="M87" s="305">
+      <c r="K87" s="288"/>
+      <c r="L87" s="289"/>
+      <c r="M87" s="290">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="292"/>
+      <c r="N87" s="289"/>
       <c r="P87" s="291" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="292"/>
+      <c r="Q87" s="289"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -8239,17 +8242,6 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="P86:Q86"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="M84:N84"/>
     <mergeCell ref="A1:R6"/>
     <mergeCell ref="P84:Q84"/>
     <mergeCell ref="J82:L82"/>
@@ -8262,6 +8254,17 @@
     <mergeCell ref="P83:Q83"/>
     <mergeCell ref="P82:Q82"/>
     <mergeCell ref="P80:S81"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="P86:Q86"/>
   </mergeCells>
   <conditionalFormatting sqref="T10:T69">
     <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
@@ -8350,10 +8353,10 @@
       <c r="G6" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="H6" s="364" t="s">
+      <c r="H6" s="354" t="s">
         <v>280</v>
       </c>
-      <c r="I6" s="317"/>
+      <c r="I6" s="320"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -8379,7 +8382,7 @@
         <f>F7-G7</f>
         <v>380000</v>
       </c>
-      <c r="I7" s="317"/>
+      <c r="I7" s="320"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="194"/>
@@ -8488,6 +8491,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="H6:I6"/>
@@ -8496,11 +8504,6 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8554,46 +8557,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="327" t="s">
+      <c r="C2" s="315" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="288"/>
-      <c r="E2" s="288"/>
-      <c r="F2" s="288"/>
-      <c r="G2" s="288"/>
-      <c r="H2" s="288"/>
-      <c r="I2" s="288"/>
-      <c r="J2" s="288"/>
-      <c r="K2" s="288"/>
-      <c r="L2" s="288"/>
-      <c r="M2" s="288"/>
-      <c r="N2" s="288"/>
-      <c r="O2" s="288"/>
-      <c r="P2" s="289"/>
-      <c r="Q2" s="289"/>
-      <c r="R2" s="289"/>
-      <c r="S2" s="288"/>
-      <c r="T2" s="288"/>
+      <c r="D2" s="294"/>
+      <c r="E2" s="294"/>
+      <c r="F2" s="294"/>
+      <c r="G2" s="294"/>
+      <c r="H2" s="294"/>
+      <c r="I2" s="294"/>
+      <c r="J2" s="294"/>
+      <c r="K2" s="294"/>
+      <c r="L2" s="294"/>
+      <c r="M2" s="294"/>
+      <c r="N2" s="294"/>
+      <c r="O2" s="294"/>
+      <c r="P2" s="295"/>
+      <c r="Q2" s="295"/>
+      <c r="R2" s="295"/>
+      <c r="S2" s="294"/>
+      <c r="T2" s="294"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="289"/>
-      <c r="D3" s="290"/>
-      <c r="E3" s="290"/>
-      <c r="F3" s="290"/>
-      <c r="G3" s="290"/>
-      <c r="H3" s="290"/>
-      <c r="I3" s="290"/>
-      <c r="J3" s="290"/>
-      <c r="K3" s="290"/>
-      <c r="L3" s="290"/>
-      <c r="M3" s="290"/>
-      <c r="N3" s="290"/>
-      <c r="O3" s="290"/>
-      <c r="P3" s="290"/>
-      <c r="Q3" s="290"/>
-      <c r="R3" s="290"/>
-      <c r="S3" s="290"/>
-      <c r="T3" s="290"/>
+      <c r="C3" s="295"/>
+      <c r="D3" s="296"/>
+      <c r="E3" s="296"/>
+      <c r="F3" s="296"/>
+      <c r="G3" s="296"/>
+      <c r="H3" s="296"/>
+      <c r="I3" s="296"/>
+      <c r="J3" s="296"/>
+      <c r="K3" s="296"/>
+      <c r="L3" s="296"/>
+      <c r="M3" s="296"/>
+      <c r="N3" s="296"/>
+      <c r="O3" s="296"/>
+      <c r="P3" s="296"/>
+      <c r="Q3" s="296"/>
+      <c r="R3" s="296"/>
+      <c r="S3" s="296"/>
+      <c r="T3" s="296"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8680,25 +8683,25 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="319" t="s">
+      <c r="X5" s="321" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="294"/>
-      <c r="Z5" s="294"/>
-      <c r="AA5" s="294"/>
-      <c r="AB5" s="294"/>
-      <c r="AC5" s="294"/>
-      <c r="AD5" s="294"/>
-      <c r="AE5" s="294"/>
-      <c r="AF5" s="294"/>
-      <c r="AG5" s="294"/>
-      <c r="AH5" s="294"/>
-      <c r="AI5" s="294"/>
-      <c r="AJ5" s="294"/>
-      <c r="AK5" s="294"/>
-      <c r="AL5" s="294"/>
-      <c r="AM5" s="294"/>
-      <c r="AN5" s="292"/>
+      <c r="Y5" s="288"/>
+      <c r="Z5" s="288"/>
+      <c r="AA5" s="288"/>
+      <c r="AB5" s="288"/>
+      <c r="AC5" s="288"/>
+      <c r="AD5" s="288"/>
+      <c r="AE5" s="288"/>
+      <c r="AF5" s="288"/>
+      <c r="AG5" s="288"/>
+      <c r="AH5" s="288"/>
+      <c r="AI5" s="288"/>
+      <c r="AJ5" s="288"/>
+      <c r="AK5" s="288"/>
+      <c r="AL5" s="288"/>
+      <c r="AM5" s="288"/>
+      <c r="AN5" s="289"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -8773,29 +8776,29 @@
       <c r="V6" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X6" s="328" t="s">
+      <c r="X6" s="316" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="328" t="s">
+      <c r="Y6" s="316" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="317" t="s">
+      <c r="Z6" s="320" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="318"/>
-      <c r="AB6" s="318"/>
-      <c r="AC6" s="318"/>
-      <c r="AD6" s="318"/>
-      <c r="AE6" s="318"/>
-      <c r="AF6" s="318"/>
-      <c r="AG6" s="318"/>
-      <c r="AH6" s="318"/>
-      <c r="AI6" s="318"/>
-      <c r="AJ6" s="318"/>
-      <c r="AK6" s="318"/>
-      <c r="AL6" s="318"/>
-      <c r="AM6" s="318"/>
-      <c r="AN6" s="318"/>
+      <c r="AA6" s="317"/>
+      <c r="AB6" s="317"/>
+      <c r="AC6" s="317"/>
+      <c r="AD6" s="317"/>
+      <c r="AE6" s="317"/>
+      <c r="AF6" s="317"/>
+      <c r="AG6" s="317"/>
+      <c r="AH6" s="317"/>
+      <c r="AI6" s="317"/>
+      <c r="AJ6" s="317"/>
+      <c r="AK6" s="317"/>
+      <c r="AL6" s="317"/>
+      <c r="AM6" s="317"/>
+      <c r="AN6" s="317"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -8870,27 +8873,27 @@
       <c r="V7" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X7" s="318"/>
-      <c r="Y7" s="318"/>
-      <c r="Z7" s="317" t="s">
+      <c r="X7" s="317"/>
+      <c r="Y7" s="317"/>
+      <c r="Z7" s="320" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="318"/>
-      <c r="AB7" s="318"/>
-      <c r="AC7" s="318"/>
-      <c r="AD7" s="317" t="s">
+      <c r="AA7" s="317"/>
+      <c r="AB7" s="317"/>
+      <c r="AC7" s="317"/>
+      <c r="AD7" s="320" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="318"/>
-      <c r="AF7" s="318"/>
-      <c r="AG7" s="318"/>
-      <c r="AH7" s="318"/>
-      <c r="AI7" s="318"/>
-      <c r="AJ7" s="318"/>
-      <c r="AK7" s="318"/>
-      <c r="AL7" s="318"/>
-      <c r="AM7" s="318"/>
-      <c r="AN7" s="318"/>
+      <c r="AE7" s="317"/>
+      <c r="AF7" s="317"/>
+      <c r="AG7" s="317"/>
+      <c r="AH7" s="317"/>
+      <c r="AI7" s="317"/>
+      <c r="AJ7" s="317"/>
+      <c r="AK7" s="317"/>
+      <c r="AL7" s="317"/>
+      <c r="AM7" s="317"/>
+      <c r="AN7" s="317"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -8940,8 +8943,8 @@
         <v>NO</v>
       </c>
       <c r="V8" s="13"/>
-      <c r="X8" s="318"/>
-      <c r="Y8" s="318"/>
+      <c r="X8" s="317"/>
+      <c r="Y8" s="317"/>
       <c r="Z8" s="151" t="s">
         <v>19</v>
       </c>
@@ -13552,10 +13555,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="315" t="s">
+      <c r="AA49" s="318" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="316"/>
+      <c r="AB49" s="319"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -13633,12 +13636,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="311" t="s">
+      <c r="AI50" s="325" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="312"/>
-      <c r="AK50" s="312"/>
-      <c r="AL50" s="313"/>
+      <c r="AJ50" s="326"/>
+      <c r="AK50" s="326"/>
+      <c r="AL50" s="327"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -13709,12 +13712,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="308" t="s">
+      <c r="AI51" s="322" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="309"/>
-      <c r="AK51" s="309"/>
-      <c r="AL51" s="310"/>
+      <c r="AJ51" s="323"/>
+      <c r="AK51" s="323"/>
+      <c r="AL51" s="324"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -13980,14 +13983,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="314"/>
-      <c r="AD55" s="314"/>
-      <c r="AI55" s="311" t="s">
+      <c r="AC55" s="328"/>
+      <c r="AD55" s="328"/>
+      <c r="AI55" s="325" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="312"/>
-      <c r="AK55" s="312"/>
-      <c r="AL55" s="313"/>
+      <c r="AJ55" s="326"/>
+      <c r="AK55" s="326"/>
+      <c r="AL55" s="327"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -14304,32 +14307,32 @@
     <row r="67" spans="3:19" s="256" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="320" t="s">
+      <c r="C69" s="308" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="321"/>
-      <c r="E69" s="321"/>
-      <c r="F69" s="321"/>
-      <c r="G69" s="322"/>
-      <c r="I69" s="326" t="s">
+      <c r="D69" s="309"/>
+      <c r="E69" s="309"/>
+      <c r="F69" s="309"/>
+      <c r="G69" s="310"/>
+      <c r="I69" s="314" t="s">
         <v>178</v>
       </c>
-      <c r="J69" s="326"/>
-      <c r="K69" s="326"/>
-      <c r="L69" s="326"/>
-      <c r="M69" s="326"/>
+      <c r="J69" s="314"/>
+      <c r="K69" s="314"/>
+      <c r="L69" s="314"/>
+      <c r="M69" s="314"/>
     </row>
     <row r="70" spans="3:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="323"/>
-      <c r="D70" s="324"/>
-      <c r="E70" s="324"/>
-      <c r="F70" s="324"/>
-      <c r="G70" s="325"/>
-      <c r="I70" s="326"/>
-      <c r="J70" s="326"/>
-      <c r="K70" s="326"/>
-      <c r="L70" s="326"/>
-      <c r="M70" s="326"/>
+      <c r="C70" s="311"/>
+      <c r="D70" s="312"/>
+      <c r="E70" s="312"/>
+      <c r="F70" s="312"/>
+      <c r="G70" s="313"/>
+      <c r="I70" s="314"/>
+      <c r="J70" s="314"/>
+      <c r="K70" s="314"/>
+      <c r="L70" s="314"/>
+      <c r="M70" s="314"/>
     </row>
     <row r="71" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14820,22 +14823,22 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AI56:AL56"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AI50:AL50"/>
+    <mergeCell ref="AI55:AL55"/>
+    <mergeCell ref="AC55:AD55"/>
+    <mergeCell ref="AA49:AB49"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="AD7:AN7"/>
+    <mergeCell ref="X5:AN5"/>
+    <mergeCell ref="Z6:AN6"/>
     <mergeCell ref="P76:Q76"/>
     <mergeCell ref="C69:G70"/>
     <mergeCell ref="I69:M70"/>
     <mergeCell ref="C2:T3"/>
     <mergeCell ref="Y6:Y8"/>
     <mergeCell ref="X6:X8"/>
-    <mergeCell ref="AA49:AB49"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="AD7:AN7"/>
-    <mergeCell ref="X5:AN5"/>
-    <mergeCell ref="Z6:AN6"/>
-    <mergeCell ref="AI56:AL56"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AI50:AL50"/>
-    <mergeCell ref="AI55:AL55"/>
-    <mergeCell ref="AC55:AD55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:V61">
     <cfRule type="expression" dxfId="20" priority="8">
@@ -14955,56 +14958,56 @@
       <c r="L3" s="329"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="326" t="s">
+      <c r="A5" s="314" t="s">
         <v>303</v>
       </c>
-      <c r="B5" s="326"/>
-      <c r="C5" s="326"/>
-      <c r="D5" s="326"/>
-      <c r="E5" s="326"/>
-      <c r="F5" s="326"/>
-      <c r="G5" s="326"/>
-      <c r="H5" s="326"/>
-      <c r="I5" s="326"/>
-      <c r="J5" s="326"/>
-      <c r="K5" s="326"/>
-      <c r="M5" s="326" t="s">
+      <c r="B5" s="314"/>
+      <c r="C5" s="314"/>
+      <c r="D5" s="314"/>
+      <c r="E5" s="314"/>
+      <c r="F5" s="314"/>
+      <c r="G5" s="314"/>
+      <c r="H5" s="314"/>
+      <c r="I5" s="314"/>
+      <c r="J5" s="314"/>
+      <c r="K5" s="314"/>
+      <c r="M5" s="314" t="s">
         <v>324</v>
       </c>
-      <c r="N5" s="326"/>
-      <c r="O5" s="326"/>
-      <c r="P5" s="326"/>
-      <c r="Q5" s="326"/>
-      <c r="R5" s="326"/>
-      <c r="S5" s="326"/>
-      <c r="T5" s="326"/>
-      <c r="U5" s="326"/>
-      <c r="V5" s="326"/>
-      <c r="W5" s="326"/>
+      <c r="N5" s="314"/>
+      <c r="O5" s="314"/>
+      <c r="P5" s="314"/>
+      <c r="Q5" s="314"/>
+      <c r="R5" s="314"/>
+      <c r="S5" s="314"/>
+      <c r="T5" s="314"/>
+      <c r="U5" s="314"/>
+      <c r="V5" s="314"/>
+      <c r="W5" s="314"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="326"/>
-      <c r="B6" s="326"/>
-      <c r="C6" s="326"/>
-      <c r="D6" s="326"/>
-      <c r="E6" s="326"/>
-      <c r="F6" s="326"/>
-      <c r="G6" s="326"/>
-      <c r="H6" s="326"/>
-      <c r="I6" s="326"/>
-      <c r="J6" s="326"/>
-      <c r="K6" s="326"/>
-      <c r="M6" s="326"/>
-      <c r="N6" s="326"/>
-      <c r="O6" s="326"/>
-      <c r="P6" s="326"/>
-      <c r="Q6" s="326"/>
-      <c r="R6" s="326"/>
-      <c r="S6" s="326"/>
-      <c r="T6" s="326"/>
-      <c r="U6" s="326"/>
-      <c r="V6" s="326"/>
-      <c r="W6" s="326"/>
+      <c r="A6" s="314"/>
+      <c r="B6" s="314"/>
+      <c r="C6" s="314"/>
+      <c r="D6" s="314"/>
+      <c r="E6" s="314"/>
+      <c r="F6" s="314"/>
+      <c r="G6" s="314"/>
+      <c r="H6" s="314"/>
+      <c r="I6" s="314"/>
+      <c r="J6" s="314"/>
+      <c r="K6" s="314"/>
+      <c r="M6" s="314"/>
+      <c r="N6" s="314"/>
+      <c r="O6" s="314"/>
+      <c r="P6" s="314"/>
+      <c r="Q6" s="314"/>
+      <c r="R6" s="314"/>
+      <c r="S6" s="314"/>
+      <c r="T6" s="314"/>
+      <c r="U6" s="314"/>
+      <c r="V6" s="314"/>
+      <c r="W6" s="314"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M7" s="249"/>
@@ -15979,7 +15982,7 @@
   <dimension ref="B3:P75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16568,39 +16571,63 @@
       <c r="B29" s="57">
         <v>26</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
+      <c r="C29" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="E29" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="F29" s="57" t="s">
+        <v>379</v>
+      </c>
       <c r="G29" s="56">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="57">
         <v>27</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
+      <c r="C30" s="57" t="s">
+        <v>385</v>
+      </c>
+      <c r="D30" s="57" t="s">
+        <v>352</v>
+      </c>
+      <c r="E30" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="F30" s="57" t="s">
+        <v>379</v>
+      </c>
       <c r="G30" s="56">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>125000</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="57">
         <v>28</v>
       </c>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
+      <c r="C31" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="E31" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="F31" s="57" t="s">
+        <v>379</v>
+      </c>
       <c r="G31" s="56">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
@@ -16717,38 +16744,38 @@
       <c r="F40" s="344"/>
       <c r="G40" s="286">
         <f>SUM(G4:G39)</f>
-        <v>3125000</v>
+        <v>3550000</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="326" t="s">
+      <c r="B44" s="314" t="s">
         <v>366</v>
       </c>
-      <c r="C44" s="326"/>
-      <c r="D44" s="326"/>
-      <c r="E44" s="326"/>
-      <c r="F44" s="326"/>
-      <c r="G44" s="326"/>
-      <c r="H44" s="326"/>
-      <c r="I44" s="326"/>
-      <c r="J44" s="326"/>
-      <c r="K44" s="326"/>
-      <c r="L44" s="326"/>
-      <c r="M44" s="326"/>
+      <c r="C44" s="314"/>
+      <c r="D44" s="314"/>
+      <c r="E44" s="314"/>
+      <c r="F44" s="314"/>
+      <c r="G44" s="314"/>
+      <c r="H44" s="314"/>
+      <c r="I44" s="314"/>
+      <c r="J44" s="314"/>
+      <c r="K44" s="314"/>
+      <c r="L44" s="314"/>
+      <c r="M44" s="314"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="326"/>
-      <c r="C45" s="326"/>
-      <c r="D45" s="326"/>
-      <c r="E45" s="326"/>
-      <c r="F45" s="326"/>
-      <c r="G45" s="326"/>
-      <c r="H45" s="326"/>
-      <c r="I45" s="326"/>
-      <c r="J45" s="326"/>
-      <c r="K45" s="326"/>
-      <c r="L45" s="326"/>
-      <c r="M45" s="326"/>
+      <c r="B45" s="314"/>
+      <c r="C45" s="314"/>
+      <c r="D45" s="314"/>
+      <c r="E45" s="314"/>
+      <c r="F45" s="314"/>
+      <c r="G45" s="314"/>
+      <c r="H45" s="314"/>
+      <c r="I45" s="314"/>
+      <c r="J45" s="314"/>
+      <c r="K45" s="314"/>
+      <c r="L45" s="314"/>
+      <c r="M45" s="314"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="277"/>
@@ -16857,7 +16884,7 @@
       <c r="F50" s="283"/>
       <c r="G50" s="210">
         <f>G40</f>
-        <v>3125000</v>
+        <v>3550000</v>
       </c>
       <c r="H50" s="210"/>
       <c r="I50" s="277"/>
@@ -17244,7 +17271,7 @@
       <c r="F73" s="222"/>
       <c r="G73" s="223">
         <f>SUM(G48:G72)</f>
-        <v>5125000</v>
+        <v>5550000</v>
       </c>
       <c r="H73" s="224">
         <f>SUM(H48:H72)</f>
@@ -17266,7 +17293,7 @@
       <c r="F74" s="281"/>
       <c r="G74" s="330">
         <f>G73-H73</f>
-        <v>4625000</v>
+        <v>5050000</v>
       </c>
       <c r="H74" s="331"/>
       <c r="I74" s="277"/>
@@ -17367,17 +17394,17 @@
       <c r="A2" s="172"/>
       <c r="B2" s="173"/>
       <c r="C2" s="173"/>
-      <c r="D2" s="345" t="s">
+      <c r="D2" s="402" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="345"/>
-      <c r="F2" s="345"/>
-      <c r="G2" s="345"/>
-      <c r="H2" s="345"/>
-      <c r="I2" s="345"/>
-      <c r="J2" s="345"/>
-      <c r="K2" s="345"/>
-      <c r="L2" s="345"/>
+      <c r="E2" s="402"/>
+      <c r="F2" s="402"/>
+      <c r="G2" s="402"/>
+      <c r="H2" s="402"/>
+      <c r="I2" s="402"/>
+      <c r="J2" s="402"/>
+      <c r="K2" s="402"/>
+      <c r="L2" s="402"/>
       <c r="M2" s="174"/>
       <c r="N2" s="24"/>
     </row>
@@ -17395,205 +17422,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="176"/>
-      <c r="U3" s="395" t="s">
+      <c r="U3" s="345" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="396"/>
-      <c r="W3" s="397" t="s">
+      <c r="V3" s="346"/>
+      <c r="W3" s="347" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="396"/>
-      <c r="Y3" s="396"/>
-      <c r="Z3" s="396"/>
-      <c r="AA3" s="396"/>
-      <c r="AB3" s="396"/>
-      <c r="AC3" s="396"/>
-      <c r="AD3" s="398"/>
+      <c r="X3" s="346"/>
+      <c r="Y3" s="346"/>
+      <c r="Z3" s="346"/>
+      <c r="AA3" s="346"/>
+      <c r="AB3" s="346"/>
+      <c r="AC3" s="346"/>
+      <c r="AD3" s="348"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="175"/>
-      <c r="B4" s="360" t="s">
+      <c r="B4" s="406" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="361"/>
-      <c r="D4" s="361"/>
-      <c r="E4" s="361"/>
-      <c r="F4" s="361"/>
+      <c r="C4" s="407"/>
+      <c r="D4" s="407"/>
+      <c r="E4" s="407"/>
+      <c r="F4" s="407"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="364" t="s">
+      <c r="I4" s="354" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="317"/>
-      <c r="K4" s="317"/>
-      <c r="L4" s="317"/>
+      <c r="J4" s="320"/>
+      <c r="K4" s="320"/>
+      <c r="L4" s="320"/>
       <c r="M4" s="176"/>
-      <c r="U4" s="407" t="s">
+      <c r="U4" s="366" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="317"/>
-      <c r="W4" s="364" t="s">
+      <c r="V4" s="320"/>
+      <c r="W4" s="354" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="317"/>
-      <c r="Y4" s="317"/>
-      <c r="Z4" s="317"/>
-      <c r="AA4" s="317"/>
-      <c r="AB4" s="317"/>
-      <c r="AC4" s="317"/>
-      <c r="AD4" s="384"/>
+      <c r="X4" s="320"/>
+      <c r="Y4" s="320"/>
+      <c r="Z4" s="320"/>
+      <c r="AA4" s="320"/>
+      <c r="AB4" s="320"/>
+      <c r="AC4" s="320"/>
+      <c r="AD4" s="349"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="175"/>
-      <c r="B5" s="355" t="s">
+      <c r="B5" s="371" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="317"/>
-      <c r="D5" s="317"/>
-      <c r="E5" s="317"/>
-      <c r="F5" s="317"/>
+      <c r="C5" s="320"/>
+      <c r="D5" s="320"/>
+      <c r="E5" s="320"/>
+      <c r="F5" s="320"/>
       <c r="G5" s="152">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="353" t="s">
+      <c r="I5" s="373" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="354"/>
-      <c r="K5" s="365">
+      <c r="J5" s="394"/>
+      <c r="K5" s="396">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="366"/>
+      <c r="L5" s="397"/>
       <c r="M5" s="176"/>
-      <c r="U5" s="391" t="s">
+      <c r="U5" s="367" t="s">
         <v>231</v>
       </c>
-      <c r="V5" s="392"/>
-      <c r="W5" s="353" t="s">
+      <c r="V5" s="368"/>
+      <c r="W5" s="373" t="s">
         <v>232</v>
       </c>
-      <c r="X5" s="378"/>
-      <c r="Y5" s="378"/>
-      <c r="Z5" s="378"/>
-      <c r="AA5" s="378"/>
-      <c r="AB5" s="378"/>
-      <c r="AC5" s="378"/>
-      <c r="AD5" s="379"/>
+      <c r="X5" s="374"/>
+      <c r="Y5" s="374"/>
+      <c r="Z5" s="374"/>
+      <c r="AA5" s="374"/>
+      <c r="AB5" s="374"/>
+      <c r="AC5" s="374"/>
+      <c r="AD5" s="375"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="175"/>
-      <c r="B6" s="347" t="s">
+      <c r="B6" s="364" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="348"/>
-      <c r="D6" s="348"/>
-      <c r="E6" s="348"/>
-      <c r="F6" s="348"/>
+      <c r="C6" s="365"/>
+      <c r="D6" s="365"/>
+      <c r="E6" s="365"/>
+      <c r="F6" s="365"/>
       <c r="G6" s="152">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="351" t="s">
+      <c r="I6" s="395" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="352"/>
-      <c r="K6" s="367">
+      <c r="J6" s="390"/>
+      <c r="K6" s="398">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="368"/>
+      <c r="L6" s="399"/>
       <c r="M6" s="176"/>
-      <c r="U6" s="393"/>
-      <c r="V6" s="394"/>
-      <c r="W6" s="380" t="s">
+      <c r="U6" s="369"/>
+      <c r="V6" s="370"/>
+      <c r="W6" s="355" t="s">
         <v>233</v>
       </c>
-      <c r="X6" s="381"/>
-      <c r="Y6" s="381"/>
-      <c r="Z6" s="381"/>
-      <c r="AA6" s="381"/>
-      <c r="AB6" s="381"/>
-      <c r="AC6" s="381"/>
-      <c r="AD6" s="382"/>
+      <c r="X6" s="356"/>
+      <c r="Y6" s="356"/>
+      <c r="Z6" s="356"/>
+      <c r="AA6" s="356"/>
+      <c r="AB6" s="356"/>
+      <c r="AC6" s="356"/>
+      <c r="AD6" s="357"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="175"/>
-      <c r="B7" s="358" t="s">
+      <c r="B7" s="376" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="359"/>
-      <c r="D7" s="359"/>
-      <c r="E7" s="359"/>
-      <c r="F7" s="352"/>
+      <c r="C7" s="377"/>
+      <c r="D7" s="377"/>
+      <c r="E7" s="377"/>
+      <c r="F7" s="390"/>
       <c r="G7" s="152">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="351" t="s">
+      <c r="I7" s="395" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="352"/>
-      <c r="K7" s="362">
+      <c r="J7" s="390"/>
+      <c r="K7" s="400">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="363"/>
+      <c r="L7" s="401"/>
       <c r="M7" s="176"/>
-      <c r="U7" s="399"/>
-      <c r="V7" s="400"/>
-      <c r="W7" s="364" t="s">
+      <c r="U7" s="352"/>
+      <c r="V7" s="353"/>
+      <c r="W7" s="354" t="s">
         <v>234</v>
       </c>
-      <c r="X7" s="317"/>
-      <c r="Y7" s="317"/>
-      <c r="Z7" s="317"/>
-      <c r="AA7" s="317"/>
-      <c r="AB7" s="317"/>
-      <c r="AC7" s="317"/>
-      <c r="AD7" s="384"/>
+      <c r="X7" s="320"/>
+      <c r="Y7" s="320"/>
+      <c r="Z7" s="320"/>
+      <c r="AA7" s="320"/>
+      <c r="AB7" s="320"/>
+      <c r="AC7" s="320"/>
+      <c r="AD7" s="349"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="175"/>
-      <c r="B8" s="356" t="s">
+      <c r="B8" s="404" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="357"/>
-      <c r="D8" s="357"/>
-      <c r="E8" s="357"/>
-      <c r="F8" s="357"/>
+      <c r="C8" s="405"/>
+      <c r="D8" s="405"/>
+      <c r="E8" s="405"/>
+      <c r="F8" s="405"/>
       <c r="G8" s="153">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="353" t="s">
+      <c r="I8" s="373" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="354"/>
-      <c r="K8" s="349">
+      <c r="J8" s="394"/>
+      <c r="K8" s="385">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="350"/>
+      <c r="L8" s="386"/>
       <c r="M8" s="176"/>
-      <c r="U8" s="403" t="s">
+      <c r="U8" s="360" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="404"/>
-      <c r="W8" s="380" t="s">
+      <c r="V8" s="361"/>
+      <c r="W8" s="355" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="381"/>
-      <c r="Y8" s="381"/>
-      <c r="Z8" s="381"/>
-      <c r="AA8" s="381"/>
-      <c r="AB8" s="381"/>
-      <c r="AC8" s="381"/>
-      <c r="AD8" s="382"/>
+      <c r="X8" s="356"/>
+      <c r="Y8" s="356"/>
+      <c r="Z8" s="356"/>
+      <c r="AA8" s="356"/>
+      <c r="AB8" s="356"/>
+      <c r="AC8" s="356"/>
+      <c r="AD8" s="357"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="175"/>
@@ -17609,28 +17636,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="176"/>
-      <c r="U9" s="405"/>
-      <c r="V9" s="406"/>
-      <c r="W9" s="380" t="s">
+      <c r="U9" s="362"/>
+      <c r="V9" s="363"/>
+      <c r="W9" s="355" t="s">
         <v>237</v>
       </c>
-      <c r="X9" s="381"/>
-      <c r="Y9" s="381"/>
-      <c r="Z9" s="381"/>
-      <c r="AA9" s="381"/>
-      <c r="AB9" s="381"/>
-      <c r="AC9" s="381"/>
-      <c r="AD9" s="382"/>
+      <c r="X9" s="356"/>
+      <c r="Y9" s="356"/>
+      <c r="Z9" s="356"/>
+      <c r="AA9" s="356"/>
+      <c r="AB9" s="356"/>
+      <c r="AC9" s="356"/>
+      <c r="AD9" s="357"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="175"/>
-      <c r="B10" s="317" t="s">
+      <c r="B10" s="320" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="317"/>
-      <c r="D10" s="317"/>
-      <c r="E10" s="317"/>
-      <c r="F10" s="317"/>
+      <c r="C10" s="320"/>
+      <c r="D10" s="320"/>
+      <c r="E10" s="320"/>
+      <c r="F10" s="320"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -17641,30 +17668,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="176"/>
-      <c r="U10" s="347" t="s">
+      <c r="U10" s="364" t="s">
         <v>243</v>
       </c>
-      <c r="V10" s="348"/>
-      <c r="W10" s="317" t="s">
+      <c r="V10" s="365"/>
+      <c r="W10" s="320" t="s">
         <v>257</v>
       </c>
-      <c r="X10" s="317"/>
-      <c r="Y10" s="317"/>
-      <c r="Z10" s="317"/>
-      <c r="AA10" s="317"/>
-      <c r="AB10" s="317"/>
-      <c r="AC10" s="317"/>
-      <c r="AD10" s="384"/>
+      <c r="X10" s="320"/>
+      <c r="Y10" s="320"/>
+      <c r="Z10" s="320"/>
+      <c r="AA10" s="320"/>
+      <c r="AB10" s="320"/>
+      <c r="AC10" s="320"/>
+      <c r="AD10" s="349"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="175"/>
-      <c r="B11" s="317" t="s">
+      <c r="B11" s="320" t="s">
         <v>254</v>
       </c>
-      <c r="C11" s="317"/>
-      <c r="D11" s="317"/>
-      <c r="E11" s="317"/>
-      <c r="F11" s="317"/>
+      <c r="C11" s="320"/>
+      <c r="D11" s="320"/>
+      <c r="E11" s="320"/>
+      <c r="F11" s="320"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -17674,30 +17701,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="176"/>
-      <c r="U11" s="347" t="s">
+      <c r="U11" s="364" t="s">
         <v>256</v>
       </c>
-      <c r="V11" s="348"/>
-      <c r="W11" s="401" t="s">
+      <c r="V11" s="365"/>
+      <c r="W11" s="358" t="s">
         <v>258</v>
       </c>
-      <c r="X11" s="401"/>
-      <c r="Y11" s="401"/>
-      <c r="Z11" s="401"/>
-      <c r="AA11" s="401"/>
-      <c r="AB11" s="401"/>
-      <c r="AC11" s="401"/>
-      <c r="AD11" s="402"/>
+      <c r="X11" s="358"/>
+      <c r="Y11" s="358"/>
+      <c r="Z11" s="358"/>
+      <c r="AA11" s="358"/>
+      <c r="AB11" s="358"/>
+      <c r="AC11" s="358"/>
+      <c r="AD11" s="359"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="175"/>
-      <c r="B12" s="346" t="s">
+      <c r="B12" s="403" t="s">
         <v>255</v>
       </c>
-      <c r="C12" s="346"/>
-      <c r="D12" s="346"/>
-      <c r="E12" s="346"/>
-      <c r="F12" s="346"/>
+      <c r="C12" s="403"/>
+      <c r="D12" s="403"/>
+      <c r="E12" s="403"/>
+      <c r="F12" s="403"/>
       <c r="G12" s="180">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -17708,16 +17735,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="176"/>
-      <c r="U12" s="347"/>
-      <c r="V12" s="348"/>
-      <c r="W12" s="317"/>
-      <c r="X12" s="317"/>
-      <c r="Y12" s="317"/>
-      <c r="Z12" s="317"/>
-      <c r="AA12" s="317"/>
-      <c r="AB12" s="317"/>
-      <c r="AC12" s="317"/>
-      <c r="AD12" s="384"/>
+      <c r="U12" s="364"/>
+      <c r="V12" s="365"/>
+      <c r="W12" s="320"/>
+      <c r="X12" s="320"/>
+      <c r="Y12" s="320"/>
+      <c r="Z12" s="320"/>
+      <c r="AA12" s="320"/>
+      <c r="AB12" s="320"/>
+      <c r="AC12" s="320"/>
+      <c r="AD12" s="349"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="177"/>
@@ -17733,64 +17760,64 @@
       <c r="K13" s="178"/>
       <c r="L13" s="178"/>
       <c r="M13" s="179"/>
-      <c r="U13" s="347"/>
-      <c r="V13" s="348"/>
-      <c r="W13" s="317"/>
-      <c r="X13" s="317"/>
-      <c r="Y13" s="317"/>
-      <c r="Z13" s="317"/>
-      <c r="AA13" s="317"/>
-      <c r="AB13" s="317"/>
-      <c r="AC13" s="317"/>
-      <c r="AD13" s="384"/>
+      <c r="U13" s="364"/>
+      <c r="V13" s="365"/>
+      <c r="W13" s="320"/>
+      <c r="X13" s="320"/>
+      <c r="Y13" s="320"/>
+      <c r="Z13" s="320"/>
+      <c r="AA13" s="320"/>
+      <c r="AB13" s="320"/>
+      <c r="AC13" s="320"/>
+      <c r="AD13" s="349"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="385"/>
-      <c r="V14" s="386"/>
-      <c r="W14" s="376"/>
-      <c r="X14" s="376"/>
-      <c r="Y14" s="376"/>
-      <c r="Z14" s="376"/>
-      <c r="AA14" s="376"/>
-      <c r="AB14" s="376"/>
-      <c r="AC14" s="376"/>
-      <c r="AD14" s="377"/>
+      <c r="U14" s="379"/>
+      <c r="V14" s="380"/>
+      <c r="W14" s="350"/>
+      <c r="X14" s="350"/>
+      <c r="Y14" s="350"/>
+      <c r="Z14" s="350"/>
+      <c r="AA14" s="350"/>
+      <c r="AB14" s="350"/>
+      <c r="AC14" s="350"/>
+      <c r="AD14" s="351"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="172"/>
       <c r="B18" s="173"/>
       <c r="C18" s="173"/>
-      <c r="D18" s="345" t="s">
+      <c r="D18" s="402" t="s">
         <v>249</v>
       </c>
-      <c r="E18" s="345"/>
-      <c r="F18" s="345"/>
-      <c r="G18" s="345"/>
-      <c r="H18" s="345"/>
-      <c r="I18" s="345"/>
-      <c r="J18" s="345"/>
-      <c r="K18" s="345"/>
-      <c r="L18" s="345"/>
+      <c r="E18" s="402"/>
+      <c r="F18" s="402"/>
+      <c r="G18" s="402"/>
+      <c r="H18" s="402"/>
+      <c r="I18" s="402"/>
+      <c r="J18" s="402"/>
+      <c r="K18" s="402"/>
+      <c r="L18" s="402"/>
       <c r="M18" s="174"/>
-      <c r="O18" s="387" t="s">
+      <c r="O18" s="381" t="s">
         <v>250</v>
       </c>
-      <c r="P18" s="388"/>
-      <c r="Q18" s="388"/>
-      <c r="R18" s="388"/>
-      <c r="S18" s="389"/>
+      <c r="P18" s="382"/>
+      <c r="Q18" s="382"/>
+      <c r="R18" s="382"/>
+      <c r="S18" s="383"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="175"/>
       <c r="M19" s="176"/>
-      <c r="O19" s="355" t="s">
+      <c r="O19" s="371" t="s">
         <v>251</v>
       </c>
-      <c r="P19" s="317"/>
-      <c r="Q19" s="317"/>
-      <c r="R19" s="317"/>
-      <c r="S19" s="384"/>
+      <c r="P19" s="320"/>
+      <c r="Q19" s="320"/>
+      <c r="R19" s="320"/>
+      <c r="S19" s="349"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="175"/>
@@ -17801,119 +17828,119 @@
       <c r="F20" s="200"/>
       <c r="G20" s="68"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="364" t="s">
+      <c r="I20" s="354" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="317"/>
-      <c r="K20" s="317"/>
-      <c r="L20" s="317"/>
+      <c r="J20" s="320"/>
+      <c r="K20" s="320"/>
+      <c r="L20" s="320"/>
       <c r="M20" s="176"/>
-      <c r="O20" s="355" t="s">
+      <c r="O20" s="371" t="s">
         <v>252</v>
       </c>
-      <c r="P20" s="317"/>
-      <c r="Q20" s="317"/>
-      <c r="R20" s="317"/>
-      <c r="S20" s="384"/>
+      <c r="P20" s="320"/>
+      <c r="Q20" s="320"/>
+      <c r="R20" s="320"/>
+      <c r="S20" s="349"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="175"/>
-      <c r="B21" s="369" t="s">
+      <c r="B21" s="387" t="s">
         <v>296</v>
       </c>
-      <c r="C21" s="370"/>
-      <c r="D21" s="370"/>
-      <c r="E21" s="370"/>
-      <c r="F21" s="371"/>
+      <c r="C21" s="388"/>
+      <c r="D21" s="388"/>
+      <c r="E21" s="388"/>
+      <c r="F21" s="389"/>
       <c r="G21" s="70">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="353" t="s">
+      <c r="I21" s="373" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="354"/>
-      <c r="K21" s="365">
+      <c r="J21" s="394"/>
+      <c r="K21" s="396">
         <f>G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="L21" s="366"/>
+      <c r="L21" s="397"/>
       <c r="M21" s="176"/>
       <c r="N21" s="170"/>
-      <c r="O21" s="390" t="s">
+      <c r="O21" s="384" t="s">
         <v>259</v>
       </c>
-      <c r="P21" s="378"/>
-      <c r="Q21" s="378"/>
-      <c r="R21" s="378"/>
-      <c r="S21" s="379"/>
+      <c r="P21" s="374"/>
+      <c r="Q21" s="374"/>
+      <c r="R21" s="374"/>
+      <c r="S21" s="375"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="175"/>
-      <c r="B22" s="358" t="s">
+      <c r="B22" s="376" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="359"/>
-      <c r="D22" s="359"/>
-      <c r="E22" s="359"/>
-      <c r="F22" s="352"/>
+      <c r="C22" s="377"/>
+      <c r="D22" s="377"/>
+      <c r="E22" s="377"/>
+      <c r="F22" s="390"/>
       <c r="G22" s="152">
         <f>G21</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="351" t="s">
+      <c r="I22" s="395" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="352"/>
-      <c r="K22" s="367">
+      <c r="J22" s="390"/>
+      <c r="K22" s="398">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="L22" s="368"/>
+      <c r="L22" s="399"/>
       <c r="M22" s="176"/>
       <c r="N22" s="170"/>
-      <c r="O22" s="358" t="s">
+      <c r="O22" s="376" t="s">
         <v>260</v>
       </c>
-      <c r="P22" s="359"/>
-      <c r="Q22" s="359"/>
-      <c r="R22" s="359"/>
-      <c r="S22" s="383"/>
+      <c r="P22" s="377"/>
+      <c r="Q22" s="377"/>
+      <c r="R22" s="377"/>
+      <c r="S22" s="378"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="175"/>
-      <c r="B23" s="372" t="s">
+      <c r="B23" s="391" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="373"/>
-      <c r="D23" s="373"/>
-      <c r="E23" s="373"/>
-      <c r="F23" s="374"/>
+      <c r="C23" s="392"/>
+      <c r="D23" s="392"/>
+      <c r="E23" s="392"/>
+      <c r="F23" s="393"/>
       <c r="G23" s="153">
         <f>K24</f>
         <v>1568729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="351" t="s">
+      <c r="I23" s="395" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="352"/>
-      <c r="K23" s="362">
+      <c r="J23" s="390"/>
+      <c r="K23" s="400">
         <f>Pemasukkan!L31</f>
         <v>690000</v>
       </c>
-      <c r="L23" s="363"/>
+      <c r="L23" s="401"/>
       <c r="M23" s="176"/>
       <c r="N23" s="170"/>
-      <c r="O23" s="358" t="s">
+      <c r="O23" s="376" t="s">
         <v>261</v>
       </c>
-      <c r="P23" s="359"/>
-      <c r="Q23" s="359"/>
-      <c r="R23" s="359"/>
-      <c r="S23" s="383"/>
+      <c r="P23" s="377"/>
+      <c r="Q23" s="377"/>
+      <c r="R23" s="377"/>
+      <c r="S23" s="378"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="175"/>
@@ -17924,24 +17951,24 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="353" t="s">
+      <c r="I24" s="373" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="354"/>
-      <c r="K24" s="349">
+      <c r="J24" s="394"/>
+      <c r="K24" s="385">
         <f>(K21-K22)+K23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="L24" s="350"/>
+      <c r="L24" s="386"/>
       <c r="M24" s="176"/>
       <c r="N24" s="170"/>
-      <c r="O24" s="358" t="s">
+      <c r="O24" s="376" t="s">
         <v>262</v>
       </c>
-      <c r="P24" s="359"/>
-      <c r="Q24" s="359"/>
-      <c r="R24" s="359"/>
-      <c r="S24" s="383"/>
+      <c r="P24" s="377"/>
+      <c r="Q24" s="377"/>
+      <c r="R24" s="377"/>
+      <c r="S24" s="378"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="175"/>
@@ -17958,13 +17985,13 @@
       <c r="L25" s="24"/>
       <c r="M25" s="176"/>
       <c r="N25" s="170"/>
-      <c r="O25" s="355" t="s">
+      <c r="O25" s="371" t="s">
         <v>267</v>
       </c>
-      <c r="P25" s="317"/>
-      <c r="Q25" s="317"/>
-      <c r="R25" s="317"/>
-      <c r="S25" s="384"/>
+      <c r="P25" s="320"/>
+      <c r="Q25" s="320"/>
+      <c r="R25" s="320"/>
+      <c r="S25" s="349"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="175"/>
@@ -17981,11 +18008,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="176"/>
       <c r="N26" s="170"/>
-      <c r="O26" s="375"/>
-      <c r="P26" s="376"/>
-      <c r="Q26" s="376"/>
-      <c r="R26" s="376"/>
-      <c r="S26" s="377"/>
+      <c r="O26" s="372"/>
+      <c r="P26" s="350"/>
+      <c r="Q26" s="350"/>
+      <c r="R26" s="350"/>
+      <c r="S26" s="351"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="177"/>
@@ -18020,6 +18047,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="D18:L18"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="W5:AD5"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="O18:S18"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O23:S23"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="W4:AD4"/>
+    <mergeCell ref="W8:AD8"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="O25:S25"/>
     <mergeCell ref="U3:V3"/>
     <mergeCell ref="W3:AD3"/>
     <mergeCell ref="W12:AD12"/>
@@ -18036,53 +18110,6 @@
     <mergeCell ref="U12:V12"/>
     <mergeCell ref="U13:V13"/>
     <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:AD4"/>
-    <mergeCell ref="W8:AD8"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="O25:S25"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="W5:AD5"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="O24:S24"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="O18:S18"/>
-    <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O23:S23"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="D18:L18"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -18116,44 +18143,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="408" t="s">
+      <c r="C2" s="417" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="409"/>
-      <c r="E2" s="409"/>
-      <c r="F2" s="409"/>
-      <c r="G2" s="409"/>
-      <c r="H2" s="409"/>
-      <c r="I2" s="409"/>
-      <c r="J2" s="409"/>
-      <c r="K2" s="409"/>
+      <c r="D2" s="418"/>
+      <c r="E2" s="418"/>
+      <c r="F2" s="418"/>
+      <c r="G2" s="418"/>
+      <c r="H2" s="418"/>
+      <c r="I2" s="418"/>
+      <c r="J2" s="418"/>
+      <c r="K2" s="418"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="409"/>
-      <c r="D3" s="409"/>
-      <c r="E3" s="409"/>
-      <c r="F3" s="409"/>
-      <c r="G3" s="409"/>
-      <c r="H3" s="409"/>
-      <c r="I3" s="409"/>
-      <c r="J3" s="409"/>
-      <c r="K3" s="409"/>
+      <c r="C3" s="418"/>
+      <c r="D3" s="418"/>
+      <c r="E3" s="418"/>
+      <c r="F3" s="418"/>
+      <c r="G3" s="418"/>
+      <c r="H3" s="418"/>
+      <c r="I3" s="418"/>
+      <c r="J3" s="418"/>
+      <c r="K3" s="418"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="416" t="s">
+      <c r="C5" s="410" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="416"/>
-      <c r="E5" s="416"/>
-      <c r="F5" s="416"/>
-      <c r="G5" s="416"/>
-      <c r="I5" s="416" t="s">
+      <c r="D5" s="410"/>
+      <c r="E5" s="410"/>
+      <c r="F5" s="410"/>
+      <c r="G5" s="410"/>
+      <c r="I5" s="410" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="416"/>
-      <c r="K5" s="416"/>
-      <c r="L5" s="416"/>
-      <c r="M5" s="416"/>
+      <c r="J5" s="410"/>
+      <c r="K5" s="410"/>
+      <c r="L5" s="410"/>
+      <c r="M5" s="410"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -18593,88 +18620,88 @@
       <c r="M28" s="170"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="360" t="s">
+      <c r="D29" s="406" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="361"/>
-      <c r="F29" s="410">
+      <c r="E29" s="407"/>
+      <c r="F29" s="411">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="411"/>
+      <c r="G29" s="412"/>
       <c r="I29" s="170"/>
-      <c r="J29" s="360" t="s">
+      <c r="J29" s="406" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="361"/>
-      <c r="L29" s="410">
+      <c r="K29" s="407"/>
+      <c r="L29" s="411">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="411"/>
+      <c r="M29" s="412"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="407" t="s">
+      <c r="D30" s="366" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="317"/>
-      <c r="F30" s="412">
+      <c r="E30" s="320"/>
+      <c r="F30" s="413">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="413"/>
+      <c r="G30" s="414"/>
       <c r="I30" s="170"/>
-      <c r="J30" s="407" t="s">
+      <c r="J30" s="366" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="317"/>
-      <c r="L30" s="412">
+      <c r="K30" s="320"/>
+      <c r="L30" s="413">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="413"/>
+      <c r="M30" s="414"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="355" t="s">
+      <c r="D31" s="371" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="317"/>
-      <c r="F31" s="417">
+      <c r="E31" s="320"/>
+      <c r="F31" s="415">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="418"/>
+      <c r="G31" s="416"/>
       <c r="I31" s="170"/>
-      <c r="J31" s="355" t="s">
+      <c r="J31" s="371" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="317"/>
-      <c r="L31" s="417">
+      <c r="K31" s="320"/>
+      <c r="L31" s="415">
         <f>L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="418"/>
+      <c r="M31" s="416"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="356" t="s">
+      <c r="D32" s="404" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="357"/>
-      <c r="F32" s="414">
+      <c r="E32" s="405"/>
+      <c r="F32" s="408">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="415"/>
+      <c r="G32" s="409"/>
       <c r="I32" s="170"/>
-      <c r="J32" s="356" t="s">
+      <c r="J32" s="404" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="357"/>
-      <c r="L32" s="414">
+      <c r="K32" s="405"/>
+      <c r="L32" s="408">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="415"/>
+      <c r="M32" s="409"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18866,6 +18893,12 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C2:K3"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J29:K29"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="I5:M5"/>
@@ -18879,12 +18912,6 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J32:K32"/>
-    <mergeCell ref="C2:K3"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -18917,44 +18944,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="419" t="s">
+      <c r="C2" s="423" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="420"/>
-      <c r="E2" s="420"/>
-      <c r="F2" s="420"/>
-      <c r="G2" s="420"/>
-      <c r="H2" s="420"/>
-      <c r="I2" s="420"/>
-      <c r="J2" s="420"/>
-      <c r="K2" s="420"/>
+      <c r="D2" s="424"/>
+      <c r="E2" s="424"/>
+      <c r="F2" s="424"/>
+      <c r="G2" s="424"/>
+      <c r="H2" s="424"/>
+      <c r="I2" s="424"/>
+      <c r="J2" s="424"/>
+      <c r="K2" s="424"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="420"/>
-      <c r="D3" s="420"/>
-      <c r="E3" s="420"/>
-      <c r="F3" s="420"/>
-      <c r="G3" s="420"/>
-      <c r="H3" s="420"/>
-      <c r="I3" s="420"/>
-      <c r="J3" s="420"/>
-      <c r="K3" s="420"/>
+      <c r="C3" s="424"/>
+      <c r="D3" s="424"/>
+      <c r="E3" s="424"/>
+      <c r="F3" s="424"/>
+      <c r="G3" s="424"/>
+      <c r="H3" s="424"/>
+      <c r="I3" s="424"/>
+      <c r="J3" s="424"/>
+      <c r="K3" s="424"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="416" t="s">
+      <c r="C5" s="410" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="416"/>
-      <c r="E5" s="416"/>
-      <c r="F5" s="416"/>
-      <c r="G5" s="416"/>
-      <c r="I5" s="416" t="s">
+      <c r="D5" s="410"/>
+      <c r="E5" s="410"/>
+      <c r="F5" s="410"/>
+      <c r="G5" s="410"/>
+      <c r="I5" s="410" t="s">
         <v>246</v>
       </c>
-      <c r="J5" s="416"/>
-      <c r="K5" s="416"/>
-      <c r="L5" s="416"/>
-      <c r="M5" s="416"/>
+      <c r="J5" s="410"/>
+      <c r="K5" s="410"/>
+      <c r="L5" s="410"/>
+      <c r="M5" s="410"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -19438,20 +19465,20 @@
       <c r="M28" s="170"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="395" t="s">
+      <c r="D29" s="345" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="397"/>
+      <c r="E29" s="347"/>
       <c r="F29" s="421">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
       <c r="G29" s="422"/>
       <c r="I29" s="170"/>
-      <c r="J29" s="395" t="s">
+      <c r="J29" s="345" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="397"/>
+      <c r="K29" s="347"/>
       <c r="L29" s="421">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
@@ -19459,67 +19486,67 @@
       <c r="M29" s="422"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="355" t="s">
+      <c r="D30" s="371" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="317"/>
-      <c r="F30" s="412">
+      <c r="E30" s="320"/>
+      <c r="F30" s="413">
         <f>F27</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="413"/>
+      <c r="G30" s="414"/>
       <c r="I30" s="170"/>
-      <c r="J30" s="355" t="s">
+      <c r="J30" s="371" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="317"/>
-      <c r="L30" s="412">
+      <c r="K30" s="320"/>
+      <c r="L30" s="413">
         <f>L27</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="413"/>
+      <c r="M30" s="414"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="355" t="s">
+      <c r="D31" s="371" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="317"/>
-      <c r="F31" s="417">
+      <c r="E31" s="320"/>
+      <c r="F31" s="415">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="418"/>
+      <c r="G31" s="416"/>
       <c r="I31" s="170"/>
-      <c r="J31" s="355" t="s">
+      <c r="J31" s="371" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="317"/>
-      <c r="L31" s="417">
+      <c r="K31" s="320"/>
+      <c r="L31" s="415">
         <f>Pemasukkan!L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="418"/>
+      <c r="M31" s="416"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="356" t="s">
+      <c r="D32" s="404" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="357"/>
-      <c r="F32" s="423">
+      <c r="E32" s="405"/>
+      <c r="F32" s="419">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="424"/>
+      <c r="G32" s="420"/>
       <c r="I32" s="170"/>
-      <c r="J32" s="356" t="s">
+      <c r="J32" s="404" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="357"/>
-      <c r="L32" s="423">
+      <c r="K32" s="405"/>
+      <c r="L32" s="419">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="424"/>
+      <c r="M32" s="420"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19711,14 +19738,6 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
     <mergeCell ref="C2:K3"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
@@ -19730,6 +19749,14 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Sirkulasi Pembayaran Makrab 19
Bayar Tiket masuk kleresede (mobil)
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="392">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -1190,6 +1190,15 @@
   </si>
   <si>
     <t>Print Keperluan TM</t>
+  </si>
+  <si>
+    <t>15 Februari 2020</t>
+  </si>
+  <si>
+    <t>Tiket Masuk Mobil ke Kleresede</t>
+  </si>
+  <si>
+    <t>UANG MAKRAB MASIH HUTANG KE RAPLI 2RB UNTUK TIKET MASUK KLERESEDE</t>
   </si>
 </sst>
 </file>
@@ -2415,7 +2424,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="440">
+  <cellXfs count="441">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3037,20 +3046,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3066,39 +3084,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3106,36 +3122,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3185,193 +3194,220 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3380,31 +3416,16 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3413,18 +3434,6 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3475,6 +3484,9 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3482,36 +3494,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <fill>
         <patternFill>
@@ -4707,126 +4690,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="285" t="s">
+      <c r="A1" s="291" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="286"/>
-      <c r="C1" s="286"/>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
-      <c r="N1" s="286"/>
-      <c r="O1" s="286"/>
-      <c r="P1" s="286"/>
-      <c r="Q1" s="286"/>
-      <c r="R1" s="286"/>
+      <c r="B1" s="292"/>
+      <c r="C1" s="292"/>
+      <c r="D1" s="292"/>
+      <c r="E1" s="292"/>
+      <c r="F1" s="292"/>
+      <c r="G1" s="292"/>
+      <c r="H1" s="292"/>
+      <c r="I1" s="292"/>
+      <c r="J1" s="292"/>
+      <c r="K1" s="292"/>
+      <c r="L1" s="292"/>
+      <c r="M1" s="292"/>
+      <c r="N1" s="292"/>
+      <c r="O1" s="292"/>
+      <c r="P1" s="292"/>
+      <c r="Q1" s="292"/>
+      <c r="R1" s="292"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="287"/>
-      <c r="B2" s="288"/>
-      <c r="C2" s="288"/>
-      <c r="D2" s="288"/>
-      <c r="E2" s="288"/>
-      <c r="F2" s="288"/>
-      <c r="G2" s="288"/>
-      <c r="H2" s="288"/>
-      <c r="I2" s="288"/>
-      <c r="J2" s="288"/>
-      <c r="K2" s="288"/>
-      <c r="L2" s="288"/>
-      <c r="M2" s="288"/>
-      <c r="N2" s="288"/>
-      <c r="O2" s="288"/>
-      <c r="P2" s="288"/>
-      <c r="Q2" s="288"/>
-      <c r="R2" s="288"/>
+      <c r="A2" s="293"/>
+      <c r="B2" s="294"/>
+      <c r="C2" s="294"/>
+      <c r="D2" s="294"/>
+      <c r="E2" s="294"/>
+      <c r="F2" s="294"/>
+      <c r="G2" s="294"/>
+      <c r="H2" s="294"/>
+      <c r="I2" s="294"/>
+      <c r="J2" s="294"/>
+      <c r="K2" s="294"/>
+      <c r="L2" s="294"/>
+      <c r="M2" s="294"/>
+      <c r="N2" s="294"/>
+      <c r="O2" s="294"/>
+      <c r="P2" s="294"/>
+      <c r="Q2" s="294"/>
+      <c r="R2" s="294"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="287"/>
-      <c r="B3" s="288"/>
-      <c r="C3" s="288"/>
-      <c r="D3" s="288"/>
-      <c r="E3" s="288"/>
-      <c r="F3" s="288"/>
-      <c r="G3" s="288"/>
-      <c r="H3" s="288"/>
-      <c r="I3" s="288"/>
-      <c r="J3" s="288"/>
-      <c r="K3" s="288"/>
-      <c r="L3" s="288"/>
-      <c r="M3" s="288"/>
-      <c r="N3" s="288"/>
-      <c r="O3" s="288"/>
-      <c r="P3" s="288"/>
-      <c r="Q3" s="288"/>
-      <c r="R3" s="288"/>
+      <c r="A3" s="293"/>
+      <c r="B3" s="294"/>
+      <c r="C3" s="294"/>
+      <c r="D3" s="294"/>
+      <c r="E3" s="294"/>
+      <c r="F3" s="294"/>
+      <c r="G3" s="294"/>
+      <c r="H3" s="294"/>
+      <c r="I3" s="294"/>
+      <c r="J3" s="294"/>
+      <c r="K3" s="294"/>
+      <c r="L3" s="294"/>
+      <c r="M3" s="294"/>
+      <c r="N3" s="294"/>
+      <c r="O3" s="294"/>
+      <c r="P3" s="294"/>
+      <c r="Q3" s="294"/>
+      <c r="R3" s="294"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="287"/>
-      <c r="B4" s="288"/>
-      <c r="C4" s="288"/>
-      <c r="D4" s="288"/>
-      <c r="E4" s="288"/>
-      <c r="F4" s="288"/>
-      <c r="G4" s="288"/>
-      <c r="H4" s="288"/>
-      <c r="I4" s="288"/>
-      <c r="J4" s="288"/>
-      <c r="K4" s="288"/>
-      <c r="L4" s="288"/>
-      <c r="M4" s="288"/>
-      <c r="N4" s="288"/>
-      <c r="O4" s="288"/>
-      <c r="P4" s="288"/>
-      <c r="Q4" s="288"/>
-      <c r="R4" s="288"/>
+      <c r="A4" s="293"/>
+      <c r="B4" s="294"/>
+      <c r="C4" s="294"/>
+      <c r="D4" s="294"/>
+      <c r="E4" s="294"/>
+      <c r="F4" s="294"/>
+      <c r="G4" s="294"/>
+      <c r="H4" s="294"/>
+      <c r="I4" s="294"/>
+      <c r="J4" s="294"/>
+      <c r="K4" s="294"/>
+      <c r="L4" s="294"/>
+      <c r="M4" s="294"/>
+      <c r="N4" s="294"/>
+      <c r="O4" s="294"/>
+      <c r="P4" s="294"/>
+      <c r="Q4" s="294"/>
+      <c r="R4" s="294"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="287"/>
-      <c r="B5" s="288"/>
-      <c r="C5" s="288"/>
-      <c r="D5" s="288"/>
-      <c r="E5" s="288"/>
-      <c r="F5" s="288"/>
-      <c r="G5" s="288"/>
-      <c r="H5" s="288"/>
-      <c r="I5" s="288"/>
-      <c r="J5" s="288"/>
-      <c r="K5" s="288"/>
-      <c r="L5" s="288"/>
-      <c r="M5" s="288"/>
-      <c r="N5" s="288"/>
-      <c r="O5" s="288"/>
-      <c r="P5" s="288"/>
-      <c r="Q5" s="288"/>
-      <c r="R5" s="288"/>
+      <c r="A5" s="293"/>
+      <c r="B5" s="294"/>
+      <c r="C5" s="294"/>
+      <c r="D5" s="294"/>
+      <c r="E5" s="294"/>
+      <c r="F5" s="294"/>
+      <c r="G5" s="294"/>
+      <c r="H5" s="294"/>
+      <c r="I5" s="294"/>
+      <c r="J5" s="294"/>
+      <c r="K5" s="294"/>
+      <c r="L5" s="294"/>
+      <c r="M5" s="294"/>
+      <c r="N5" s="294"/>
+      <c r="O5" s="294"/>
+      <c r="P5" s="294"/>
+      <c r="Q5" s="294"/>
+      <c r="R5" s="294"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="287"/>
-      <c r="B6" s="288"/>
-      <c r="C6" s="288"/>
-      <c r="D6" s="288"/>
-      <c r="E6" s="288"/>
-      <c r="F6" s="288"/>
-      <c r="G6" s="288"/>
-      <c r="H6" s="288"/>
-      <c r="I6" s="288"/>
-      <c r="J6" s="288"/>
-      <c r="K6" s="288"/>
-      <c r="L6" s="288"/>
-      <c r="M6" s="288"/>
-      <c r="N6" s="288"/>
-      <c r="O6" s="288"/>
-      <c r="P6" s="288"/>
-      <c r="Q6" s="288"/>
-      <c r="R6" s="288"/>
+      <c r="A6" s="293"/>
+      <c r="B6" s="294"/>
+      <c r="C6" s="294"/>
+      <c r="D6" s="294"/>
+      <c r="E6" s="294"/>
+      <c r="F6" s="294"/>
+      <c r="G6" s="294"/>
+      <c r="H6" s="294"/>
+      <c r="I6" s="294"/>
+      <c r="J6" s="294"/>
+      <c r="K6" s="294"/>
+      <c r="L6" s="294"/>
+      <c r="M6" s="294"/>
+      <c r="N6" s="294"/>
+      <c r="O6" s="294"/>
+      <c r="P6" s="294"/>
+      <c r="Q6" s="294"/>
+      <c r="R6" s="294"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -7933,58 +7916,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="293" t="s">
+      <c r="J79" s="296" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="294"/>
-      <c r="L79" s="294"/>
-      <c r="M79" s="294"/>
-      <c r="N79" s="295"/>
-      <c r="P79" s="301" t="s">
+      <c r="K79" s="297"/>
+      <c r="L79" s="297"/>
+      <c r="M79" s="297"/>
+      <c r="N79" s="298"/>
+      <c r="P79" s="304" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="294"/>
-      <c r="R79" s="294"/>
-      <c r="S79" s="295"/>
+      <c r="Q79" s="297"/>
+      <c r="R79" s="297"/>
+      <c r="S79" s="298"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="296" t="s">
+      <c r="J80" s="299" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="288"/>
-      <c r="L80" s="288"/>
-      <c r="M80" s="288"/>
-      <c r="N80" s="297"/>
-      <c r="P80" s="296" t="s">
+      <c r="K80" s="294"/>
+      <c r="L80" s="294"/>
+      <c r="M80" s="294"/>
+      <c r="N80" s="300"/>
+      <c r="P80" s="299" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="288"/>
-      <c r="R80" s="288"/>
-      <c r="S80" s="297"/>
+      <c r="Q80" s="294"/>
+      <c r="R80" s="294"/>
+      <c r="S80" s="300"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="298"/>
-      <c r="K81" s="299"/>
-      <c r="L81" s="299"/>
-      <c r="M81" s="299"/>
-      <c r="N81" s="300"/>
-      <c r="P81" s="298"/>
-      <c r="Q81" s="299"/>
-      <c r="R81" s="299"/>
-      <c r="S81" s="300"/>
+      <c r="J81" s="301"/>
+      <c r="K81" s="302"/>
+      <c r="L81" s="302"/>
+      <c r="M81" s="302"/>
+      <c r="N81" s="303"/>
+      <c r="P81" s="301"/>
+      <c r="Q81" s="302"/>
+      <c r="R81" s="302"/>
+      <c r="S81" s="303"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="291" t="s">
+      <c r="J82" s="295" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="292"/>
-      <c r="L82" s="290"/>
-      <c r="M82" s="291" t="s">
+      <c r="K82" s="286"/>
+      <c r="L82" s="287"/>
+      <c r="M82" s="295" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="290"/>
-      <c r="P82" s="291"/>
-      <c r="Q82" s="290"/>
+      <c r="N82" s="287"/>
+      <c r="P82" s="295"/>
+      <c r="Q82" s="287"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -7993,38 +7976,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="302" t="s">
+      <c r="J83" s="285" t="s">
         <v>70</v>
       </c>
-      <c r="K83" s="292"/>
-      <c r="L83" s="290"/>
-      <c r="M83" s="303">
+      <c r="K83" s="286"/>
+      <c r="L83" s="287"/>
+      <c r="M83" s="288">
         <v>7350000</v>
       </c>
-      <c r="N83" s="290"/>
+      <c r="N83" s="287"/>
       <c r="P83" s="289" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="290"/>
+      <c r="Q83" s="287"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="302" t="s">
+      <c r="J84" s="285" t="s">
         <v>72</v>
       </c>
-      <c r="K84" s="292"/>
-      <c r="L84" s="290"/>
-      <c r="M84" s="304">
+      <c r="K84" s="286"/>
+      <c r="L84" s="287"/>
+      <c r="M84" s="290">
         <v>1100000</v>
       </c>
-      <c r="N84" s="290"/>
+      <c r="N84" s="287"/>
       <c r="P84" s="289" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="290"/>
+      <c r="Q84" s="287"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -8033,39 +8016,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="302" t="s">
+      <c r="J85" s="285" t="s">
         <v>75</v>
       </c>
-      <c r="K85" s="292"/>
-      <c r="L85" s="290"/>
-      <c r="M85" s="303">
+      <c r="K85" s="286"/>
+      <c r="L85" s="287"/>
+      <c r="M85" s="288">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="290"/>
+      <c r="N85" s="287"/>
       <c r="P85" s="289" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="290"/>
+      <c r="Q85" s="287"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="302" t="s">
+      <c r="J86" s="285" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="292"/>
-      <c r="L86" s="290"/>
-      <c r="M86" s="303">
+      <c r="K86" s="286"/>
+      <c r="L86" s="287"/>
+      <c r="M86" s="288">
         <v>8411850</v>
       </c>
-      <c r="N86" s="290"/>
+      <c r="N86" s="287"/>
       <c r="P86" s="289" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="290"/>
+      <c r="Q86" s="287"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -8073,20 +8056,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="302" t="s">
+      <c r="J87" s="285" t="s">
         <v>79</v>
       </c>
-      <c r="K87" s="292"/>
-      <c r="L87" s="290"/>
-      <c r="M87" s="303">
+      <c r="K87" s="286"/>
+      <c r="L87" s="287"/>
+      <c r="M87" s="288">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="290"/>
+      <c r="N87" s="287"/>
       <c r="P87" s="289" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="290"/>
+      <c r="Q87" s="287"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -8274,17 +8257,6 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="P86:Q86"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="M84:N84"/>
     <mergeCell ref="A1:R6"/>
     <mergeCell ref="P84:Q84"/>
     <mergeCell ref="J82:L82"/>
@@ -8297,27 +8269,38 @@
     <mergeCell ref="P83:Q83"/>
     <mergeCell ref="P82:Q82"/>
     <mergeCell ref="P80:S81"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="P86:Q86"/>
   </mergeCells>
   <conditionalFormatting sqref="T10:T69">
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S69">
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S69">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>$S$12=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8385,10 +8368,10 @@
       <c r="G6" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="H6" s="362" t="s">
+      <c r="H6" s="352" t="s">
         <v>280</v>
       </c>
-      <c r="I6" s="315"/>
+      <c r="I6" s="318"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -8414,7 +8397,7 @@
         <f>F7-G7</f>
         <v>380000</v>
       </c>
-      <c r="I7" s="315"/>
+      <c r="I7" s="318"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="194"/>
@@ -8523,6 +8506,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="H6:I6"/>
@@ -8531,11 +8519,6 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8589,46 +8572,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="325" t="s">
+      <c r="C2" s="313" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="286"/>
-      <c r="E2" s="286"/>
-      <c r="F2" s="286"/>
-      <c r="G2" s="286"/>
-      <c r="H2" s="286"/>
-      <c r="I2" s="286"/>
-      <c r="J2" s="286"/>
-      <c r="K2" s="286"/>
-      <c r="L2" s="286"/>
-      <c r="M2" s="286"/>
-      <c r="N2" s="286"/>
-      <c r="O2" s="286"/>
-      <c r="P2" s="287"/>
-      <c r="Q2" s="287"/>
-      <c r="R2" s="287"/>
-      <c r="S2" s="286"/>
-      <c r="T2" s="286"/>
+      <c r="D2" s="292"/>
+      <c r="E2" s="292"/>
+      <c r="F2" s="292"/>
+      <c r="G2" s="292"/>
+      <c r="H2" s="292"/>
+      <c r="I2" s="292"/>
+      <c r="J2" s="292"/>
+      <c r="K2" s="292"/>
+      <c r="L2" s="292"/>
+      <c r="M2" s="292"/>
+      <c r="N2" s="292"/>
+      <c r="O2" s="292"/>
+      <c r="P2" s="293"/>
+      <c r="Q2" s="293"/>
+      <c r="R2" s="293"/>
+      <c r="S2" s="292"/>
+      <c r="T2" s="292"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="287"/>
-      <c r="D3" s="288"/>
-      <c r="E3" s="288"/>
-      <c r="F3" s="288"/>
-      <c r="G3" s="288"/>
-      <c r="H3" s="288"/>
-      <c r="I3" s="288"/>
-      <c r="J3" s="288"/>
-      <c r="K3" s="288"/>
-      <c r="L3" s="288"/>
-      <c r="M3" s="288"/>
-      <c r="N3" s="288"/>
-      <c r="O3" s="288"/>
-      <c r="P3" s="288"/>
-      <c r="Q3" s="288"/>
-      <c r="R3" s="288"/>
-      <c r="S3" s="288"/>
-      <c r="T3" s="288"/>
+      <c r="C3" s="293"/>
+      <c r="D3" s="294"/>
+      <c r="E3" s="294"/>
+      <c r="F3" s="294"/>
+      <c r="G3" s="294"/>
+      <c r="H3" s="294"/>
+      <c r="I3" s="294"/>
+      <c r="J3" s="294"/>
+      <c r="K3" s="294"/>
+      <c r="L3" s="294"/>
+      <c r="M3" s="294"/>
+      <c r="N3" s="294"/>
+      <c r="O3" s="294"/>
+      <c r="P3" s="294"/>
+      <c r="Q3" s="294"/>
+      <c r="R3" s="294"/>
+      <c r="S3" s="294"/>
+      <c r="T3" s="294"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8715,25 +8698,25 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="317" t="s">
+      <c r="X5" s="319" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="292"/>
-      <c r="Z5" s="292"/>
-      <c r="AA5" s="292"/>
-      <c r="AB5" s="292"/>
-      <c r="AC5" s="292"/>
-      <c r="AD5" s="292"/>
-      <c r="AE5" s="292"/>
-      <c r="AF5" s="292"/>
-      <c r="AG5" s="292"/>
-      <c r="AH5" s="292"/>
-      <c r="AI5" s="292"/>
-      <c r="AJ5" s="292"/>
-      <c r="AK5" s="292"/>
-      <c r="AL5" s="292"/>
-      <c r="AM5" s="292"/>
-      <c r="AN5" s="290"/>
+      <c r="Y5" s="286"/>
+      <c r="Z5" s="286"/>
+      <c r="AA5" s="286"/>
+      <c r="AB5" s="286"/>
+      <c r="AC5" s="286"/>
+      <c r="AD5" s="286"/>
+      <c r="AE5" s="286"/>
+      <c r="AF5" s="286"/>
+      <c r="AG5" s="286"/>
+      <c r="AH5" s="286"/>
+      <c r="AI5" s="286"/>
+      <c r="AJ5" s="286"/>
+      <c r="AK5" s="286"/>
+      <c r="AL5" s="286"/>
+      <c r="AM5" s="286"/>
+      <c r="AN5" s="287"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -8808,29 +8791,29 @@
       <c r="V6" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X6" s="326" t="s">
+      <c r="X6" s="314" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="326" t="s">
+      <c r="Y6" s="314" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="315" t="s">
+      <c r="Z6" s="318" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="316"/>
-      <c r="AB6" s="316"/>
-      <c r="AC6" s="316"/>
-      <c r="AD6" s="316"/>
-      <c r="AE6" s="316"/>
-      <c r="AF6" s="316"/>
-      <c r="AG6" s="316"/>
-      <c r="AH6" s="316"/>
-      <c r="AI6" s="316"/>
-      <c r="AJ6" s="316"/>
-      <c r="AK6" s="316"/>
-      <c r="AL6" s="316"/>
-      <c r="AM6" s="316"/>
-      <c r="AN6" s="316"/>
+      <c r="AA6" s="315"/>
+      <c r="AB6" s="315"/>
+      <c r="AC6" s="315"/>
+      <c r="AD6" s="315"/>
+      <c r="AE6" s="315"/>
+      <c r="AF6" s="315"/>
+      <c r="AG6" s="315"/>
+      <c r="AH6" s="315"/>
+      <c r="AI6" s="315"/>
+      <c r="AJ6" s="315"/>
+      <c r="AK6" s="315"/>
+      <c r="AL6" s="315"/>
+      <c r="AM6" s="315"/>
+      <c r="AN6" s="315"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -8905,27 +8888,27 @@
       <c r="V7" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X7" s="316"/>
-      <c r="Y7" s="316"/>
-      <c r="Z7" s="315" t="s">
+      <c r="X7" s="315"/>
+      <c r="Y7" s="315"/>
+      <c r="Z7" s="318" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="316"/>
-      <c r="AB7" s="316"/>
-      <c r="AC7" s="316"/>
-      <c r="AD7" s="315" t="s">
+      <c r="AA7" s="315"/>
+      <c r="AB7" s="315"/>
+      <c r="AC7" s="315"/>
+      <c r="AD7" s="318" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="316"/>
-      <c r="AF7" s="316"/>
-      <c r="AG7" s="316"/>
-      <c r="AH7" s="316"/>
-      <c r="AI7" s="316"/>
-      <c r="AJ7" s="316"/>
-      <c r="AK7" s="316"/>
-      <c r="AL7" s="316"/>
-      <c r="AM7" s="316"/>
-      <c r="AN7" s="316"/>
+      <c r="AE7" s="315"/>
+      <c r="AF7" s="315"/>
+      <c r="AG7" s="315"/>
+      <c r="AH7" s="315"/>
+      <c r="AI7" s="315"/>
+      <c r="AJ7" s="315"/>
+      <c r="AK7" s="315"/>
+      <c r="AL7" s="315"/>
+      <c r="AM7" s="315"/>
+      <c r="AN7" s="315"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -8975,8 +8958,8 @@
         <v>NO</v>
       </c>
       <c r="V8" s="13"/>
-      <c r="X8" s="316"/>
-      <c r="Y8" s="316"/>
+      <c r="X8" s="315"/>
+      <c r="Y8" s="315"/>
       <c r="Z8" s="151" t="s">
         <v>19</v>
       </c>
@@ -13587,10 +13570,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="313" t="s">
+      <c r="AA49" s="316" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="314"/>
+      <c r="AB49" s="317"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -13668,12 +13651,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="309" t="s">
+      <c r="AI50" s="323" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="310"/>
-      <c r="AK50" s="310"/>
-      <c r="AL50" s="311"/>
+      <c r="AJ50" s="324"/>
+      <c r="AK50" s="324"/>
+      <c r="AL50" s="325"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -13744,12 +13727,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="306" t="s">
+      <c r="AI51" s="320" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="307"/>
-      <c r="AK51" s="307"/>
-      <c r="AL51" s="308"/>
+      <c r="AJ51" s="321"/>
+      <c r="AK51" s="321"/>
+      <c r="AL51" s="322"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -14015,14 +13998,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="312"/>
-      <c r="AD55" s="312"/>
-      <c r="AI55" s="309" t="s">
+      <c r="AC55" s="326"/>
+      <c r="AD55" s="326"/>
+      <c r="AI55" s="323" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="310"/>
-      <c r="AK55" s="310"/>
-      <c r="AL55" s="311"/>
+      <c r="AJ55" s="324"/>
+      <c r="AK55" s="324"/>
+      <c r="AL55" s="325"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -14355,32 +14338,32 @@
     <row r="67" spans="3:19" s="256" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="318" t="s">
+      <c r="C69" s="306" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="319"/>
-      <c r="E69" s="319"/>
-      <c r="F69" s="319"/>
-      <c r="G69" s="320"/>
-      <c r="I69" s="324" t="s">
+      <c r="D69" s="307"/>
+      <c r="E69" s="307"/>
+      <c r="F69" s="307"/>
+      <c r="G69" s="308"/>
+      <c r="I69" s="312" t="s">
         <v>178</v>
       </c>
-      <c r="J69" s="324"/>
-      <c r="K69" s="324"/>
-      <c r="L69" s="324"/>
-      <c r="M69" s="324"/>
+      <c r="J69" s="312"/>
+      <c r="K69" s="312"/>
+      <c r="L69" s="312"/>
+      <c r="M69" s="312"/>
     </row>
     <row r="70" spans="3:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="321"/>
-      <c r="D70" s="322"/>
-      <c r="E70" s="322"/>
-      <c r="F70" s="322"/>
-      <c r="G70" s="323"/>
-      <c r="I70" s="324"/>
-      <c r="J70" s="324"/>
-      <c r="K70" s="324"/>
-      <c r="L70" s="324"/>
-      <c r="M70" s="324"/>
+      <c r="C70" s="309"/>
+      <c r="D70" s="310"/>
+      <c r="E70" s="310"/>
+      <c r="F70" s="310"/>
+      <c r="G70" s="311"/>
+      <c r="I70" s="312"/>
+      <c r="J70" s="312"/>
+      <c r="K70" s="312"/>
+      <c r="L70" s="312"/>
+      <c r="M70" s="312"/>
     </row>
     <row r="71" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14871,78 +14854,78 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AI56:AL56"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AI50:AL50"/>
+    <mergeCell ref="AI55:AL55"/>
+    <mergeCell ref="AC55:AD55"/>
+    <mergeCell ref="AA49:AB49"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="AD7:AN7"/>
+    <mergeCell ref="X5:AN5"/>
+    <mergeCell ref="Z6:AN6"/>
     <mergeCell ref="P76:Q76"/>
     <mergeCell ref="C69:G70"/>
     <mergeCell ref="I69:M70"/>
     <mergeCell ref="C2:T3"/>
     <mergeCell ref="Y6:Y8"/>
     <mergeCell ref="X6:X8"/>
-    <mergeCell ref="AA49:AB49"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="AD7:AN7"/>
-    <mergeCell ref="X5:AN5"/>
-    <mergeCell ref="Z6:AN6"/>
-    <mergeCell ref="AI56:AL56"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AI50:AL50"/>
-    <mergeCell ref="AI55:AL55"/>
-    <mergeCell ref="AC55:AD55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:V61">
-    <cfRule type="expression" dxfId="24" priority="8">
+    <cfRule type="expression" dxfId="20" priority="8">
       <formula>IF(ISBLANK($B$4), 0, SEARCH($B$4,$B6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK48">
-    <cfRule type="containsText" dxfId="23" priority="9" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="19" priority="9" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH(("YES"),(AK9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK48">
-    <cfRule type="containsText" dxfId="22" priority="10" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="18" priority="10" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH(("NO"),(AK9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y9:AN9 Y46:AC46 AD46:AL48 AC47:AC48 Y10:AL45 AM10:AN48">
-    <cfRule type="expression" dxfId="21" priority="11">
+    <cfRule type="expression" dxfId="17" priority="11">
       <formula>IF(ISBLANK($Z$4), 0, SEARCH($Z$4,$Y9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6:U61">
-    <cfRule type="containsText" dxfId="20" priority="12" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH(("NO"),(U6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6:U61">
-    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH(("OK"),(U6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y10:Y45">
-    <cfRule type="expression" dxfId="18" priority="7">
+    <cfRule type="expression" dxfId="14" priority="7">
       <formula>IF(AK10="YES",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q6:R61">
-    <cfRule type="cellIs" dxfId="17" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6:P61">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y9:AN48">
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>IF(ISBLANK($AA$4), 0, SEARCH($AA$4,$Y9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6:O61">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThanOrEqual">
       <formula>200</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15006,56 +14989,56 @@
       <c r="L3" s="327"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="324" t="s">
+      <c r="A5" s="312" t="s">
         <v>303</v>
       </c>
-      <c r="B5" s="324"/>
-      <c r="C5" s="324"/>
-      <c r="D5" s="324"/>
-      <c r="E5" s="324"/>
-      <c r="F5" s="324"/>
-      <c r="G5" s="324"/>
-      <c r="H5" s="324"/>
-      <c r="I5" s="324"/>
-      <c r="J5" s="324"/>
-      <c r="K5" s="324"/>
-      <c r="M5" s="324" t="s">
+      <c r="B5" s="312"/>
+      <c r="C5" s="312"/>
+      <c r="D5" s="312"/>
+      <c r="E5" s="312"/>
+      <c r="F5" s="312"/>
+      <c r="G5" s="312"/>
+      <c r="H5" s="312"/>
+      <c r="I5" s="312"/>
+      <c r="J5" s="312"/>
+      <c r="K5" s="312"/>
+      <c r="M5" s="312" t="s">
         <v>324</v>
       </c>
-      <c r="N5" s="324"/>
-      <c r="O5" s="324"/>
-      <c r="P5" s="324"/>
-      <c r="Q5" s="324"/>
-      <c r="R5" s="324"/>
-      <c r="S5" s="324"/>
-      <c r="T5" s="324"/>
-      <c r="U5" s="324"/>
-      <c r="V5" s="324"/>
-      <c r="W5" s="324"/>
+      <c r="N5" s="312"/>
+      <c r="O5" s="312"/>
+      <c r="P5" s="312"/>
+      <c r="Q5" s="312"/>
+      <c r="R5" s="312"/>
+      <c r="S5" s="312"/>
+      <c r="T5" s="312"/>
+      <c r="U5" s="312"/>
+      <c r="V5" s="312"/>
+      <c r="W5" s="312"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="324"/>
-      <c r="B6" s="324"/>
-      <c r="C6" s="324"/>
-      <c r="D6" s="324"/>
-      <c r="E6" s="324"/>
-      <c r="F6" s="324"/>
-      <c r="G6" s="324"/>
-      <c r="H6" s="324"/>
-      <c r="I6" s="324"/>
-      <c r="J6" s="324"/>
-      <c r="K6" s="324"/>
-      <c r="M6" s="324"/>
-      <c r="N6" s="324"/>
-      <c r="O6" s="324"/>
-      <c r="P6" s="324"/>
-      <c r="Q6" s="324"/>
-      <c r="R6" s="324"/>
-      <c r="S6" s="324"/>
-      <c r="T6" s="324"/>
-      <c r="U6" s="324"/>
-      <c r="V6" s="324"/>
-      <c r="W6" s="324"/>
+      <c r="A6" s="312"/>
+      <c r="B6" s="312"/>
+      <c r="C6" s="312"/>
+      <c r="D6" s="312"/>
+      <c r="E6" s="312"/>
+      <c r="F6" s="312"/>
+      <c r="G6" s="312"/>
+      <c r="H6" s="312"/>
+      <c r="I6" s="312"/>
+      <c r="J6" s="312"/>
+      <c r="K6" s="312"/>
+      <c r="M6" s="312"/>
+      <c r="N6" s="312"/>
+      <c r="O6" s="312"/>
+      <c r="P6" s="312"/>
+      <c r="Q6" s="312"/>
+      <c r="R6" s="312"/>
+      <c r="S6" s="312"/>
+      <c r="T6" s="312"/>
+      <c r="U6" s="312"/>
+      <c r="V6" s="312"/>
+      <c r="W6" s="312"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M7" s="249"/>
@@ -16029,8 +16012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16044,7 +16027,7 @@
     <col min="8" max="8" width="16" customWidth="1"/>
     <col min="10" max="10" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="28" customWidth="1"/>
+    <col min="12" max="12" width="33.42578125" customWidth="1"/>
     <col min="13" max="13" width="28.140625" customWidth="1"/>
     <col min="14" max="14" width="32.5703125" customWidth="1"/>
   </cols>
@@ -16068,19 +16051,19 @@
       <c r="G3" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I3" s="324" t="s">
+      <c r="I3" s="312" t="s">
         <v>366</v>
       </c>
-      <c r="J3" s="324"/>
-      <c r="K3" s="324"/>
-      <c r="L3" s="324"/>
-      <c r="M3" s="324"/>
-      <c r="N3" s="324"/>
-      <c r="O3" s="324"/>
-      <c r="P3" s="324"/>
-      <c r="Q3" s="324"/>
-      <c r="R3" s="324"/>
-      <c r="S3" s="324"/>
+      <c r="J3" s="312"/>
+      <c r="K3" s="312"/>
+      <c r="L3" s="312"/>
+      <c r="M3" s="312"/>
+      <c r="N3" s="312"/>
+      <c r="O3" s="312"/>
+      <c r="P3" s="312"/>
+      <c r="Q3" s="312"/>
+      <c r="R3" s="312"/>
+      <c r="S3" s="312"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="57">
@@ -16102,17 +16085,17 @@
         <f>IF(ISNUMBER(SEARCH("SENIOR DISKON",D4)),100000,IF(ISNUMBER(SEARCH("SENIOR",D4)),150000,IF(ISNUMBER(SEARCH("MABA",D4)),125000,0)))</f>
         <v>125000</v>
       </c>
-      <c r="I4" s="324"/>
-      <c r="J4" s="324"/>
-      <c r="K4" s="324"/>
-      <c r="L4" s="324"/>
-      <c r="M4" s="324"/>
-      <c r="N4" s="324"/>
-      <c r="O4" s="324"/>
-      <c r="P4" s="324"/>
-      <c r="Q4" s="324"/>
-      <c r="R4" s="324"/>
-      <c r="S4" s="324"/>
+      <c r="I4" s="312"/>
+      <c r="J4" s="312"/>
+      <c r="K4" s="312"/>
+      <c r="L4" s="312"/>
+      <c r="M4" s="312"/>
+      <c r="N4" s="312"/>
+      <c r="O4" s="312"/>
+      <c r="P4" s="312"/>
+      <c r="Q4" s="312"/>
+      <c r="R4" s="312"/>
+      <c r="S4" s="312"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="57">
@@ -16433,10 +16416,16 @@
       <c r="J12" s="1">
         <v>6</v>
       </c>
-      <c r="K12" s="209"/>
-      <c r="L12" s="1"/>
+      <c r="K12" s="209" t="s">
+        <v>389</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>390</v>
+      </c>
       <c r="M12" s="210"/>
-      <c r="N12" s="211"/>
+      <c r="N12" s="211">
+        <v>13000</v>
+      </c>
       <c r="O12" s="277"/>
       <c r="P12" s="339"/>
       <c r="Q12" s="339"/>
@@ -16543,10 +16532,14 @@
       <c r="M15" s="210"/>
       <c r="N15" s="211"/>
       <c r="O15" s="277"/>
-      <c r="P15" s="277"/>
-      <c r="Q15" s="277"/>
-      <c r="R15" s="277"/>
-      <c r="S15" s="277"/>
+      <c r="P15" s="440" t="s">
+        <v>391</v>
+      </c>
+      <c r="Q15" s="440"/>
+      <c r="R15" s="440"/>
+      <c r="S15" s="440"/>
+      <c r="T15" s="440"/>
+      <c r="U15" s="440"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" s="57">
@@ -16577,12 +16570,14 @@
       <c r="M16" s="211"/>
       <c r="N16" s="210"/>
       <c r="O16" s="277"/>
-      <c r="P16" s="277"/>
-      <c r="Q16" s="277"/>
-      <c r="R16" s="277"/>
-      <c r="S16" s="277"/>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="P16" s="440"/>
+      <c r="Q16" s="440"/>
+      <c r="R16" s="440"/>
+      <c r="S16" s="440"/>
+      <c r="T16" s="440"/>
+      <c r="U16" s="440"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="57">
         <v>14</v>
       </c>
@@ -16611,12 +16606,14 @@
       <c r="M17" s="211"/>
       <c r="N17" s="211"/>
       <c r="O17" s="277"/>
-      <c r="P17" s="277"/>
-      <c r="Q17" s="277"/>
-      <c r="R17" s="277"/>
-      <c r="S17" s="277"/>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="P17" s="440"/>
+      <c r="Q17" s="440"/>
+      <c r="R17" s="440"/>
+      <c r="S17" s="440"/>
+      <c r="T17" s="440"/>
+      <c r="U17" s="440"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="57">
         <v>15</v>
       </c>
@@ -16650,7 +16647,7 @@
       <c r="R18" s="277"/>
       <c r="S18" s="277"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" s="57">
         <v>16</v>
       </c>
@@ -16684,7 +16681,7 @@
       <c r="R19" s="277"/>
       <c r="S19" s="277"/>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20" s="57">
         <v>17</v>
       </c>
@@ -16718,7 +16715,7 @@
       <c r="R20" s="277"/>
       <c r="S20" s="277"/>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="57">
         <v>18</v>
       </c>
@@ -16752,7 +16749,7 @@
       <c r="R21" s="277"/>
       <c r="S21" s="277"/>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" s="57">
         <v>19</v>
       </c>
@@ -16786,7 +16783,7 @@
       <c r="R22" s="277"/>
       <c r="S22" s="277"/>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B23" s="57">
         <v>20</v>
       </c>
@@ -16820,7 +16817,7 @@
       <c r="R23" s="277"/>
       <c r="S23" s="277"/>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B24" s="57">
         <v>21</v>
       </c>
@@ -16854,7 +16851,7 @@
       <c r="R24" s="277"/>
       <c r="S24" s="277"/>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B25" s="57">
         <v>22</v>
       </c>
@@ -16888,7 +16885,7 @@
       <c r="R25" s="277"/>
       <c r="S25" s="277"/>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B26" s="57">
         <v>23</v>
       </c>
@@ -16922,7 +16919,7 @@
       <c r="R26" s="277"/>
       <c r="S26" s="277"/>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B27" s="57">
         <v>24</v>
       </c>
@@ -16956,7 +16953,7 @@
       <c r="R27" s="277"/>
       <c r="S27" s="277"/>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B28" s="57">
         <v>25</v>
       </c>
@@ -16990,7 +16987,7 @@
       <c r="R28" s="277"/>
       <c r="S28" s="277"/>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B29" s="57">
         <v>26</v>
       </c>
@@ -17024,7 +17021,7 @@
       <c r="R29" s="277"/>
       <c r="S29" s="277"/>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B30" s="57">
         <v>27</v>
       </c>
@@ -17058,7 +17055,7 @@
       <c r="R30" s="277"/>
       <c r="S30" s="277"/>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B31" s="57">
         <v>28</v>
       </c>
@@ -17096,7 +17093,7 @@
       <c r="R31" s="277"/>
       <c r="S31" s="277"/>
     </row>
-    <row r="32" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="57">
         <v>29</v>
       </c>
@@ -17128,7 +17125,7 @@
       </c>
       <c r="N32" s="224">
         <f>SUM(N7:N31)</f>
-        <v>527000</v>
+        <v>540000</v>
       </c>
       <c r="O32" s="277"/>
       <c r="P32" s="277"/>
@@ -17164,7 +17161,7 @@
       <c r="L33" s="334"/>
       <c r="M33" s="328">
         <f>M32-N32</f>
-        <v>6323000</v>
+        <v>6310000</v>
       </c>
       <c r="N33" s="329"/>
       <c r="O33" s="277"/>
@@ -17431,48 +17428,49 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="J33:L34"/>
     <mergeCell ref="M33:N34"/>
     <mergeCell ref="I3:S4"/>
     <mergeCell ref="P6:V12"/>
     <mergeCell ref="B47:F47"/>
+    <mergeCell ref="P15:U17"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:D46">
     <cfRule type="expression" priority="5">
       <formula>IF(ISNUMBER(SEARCH("SENIOR DISKON",$G$4:$G$46)),"100000",IF(ISNUMBER(SEARCH("SENIOR",$G$4:$G$46)),"150000","125000"))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="SENIOR DISKON">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="SENIOR DISKON">
       <formula>NOT(ISERROR(SEARCH("SENIOR DISKON",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="SENIOR">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="SENIOR">
       <formula>NOT(ISERROR(SEARCH("SENIOR",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="MABA">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="MABA">
       <formula>NOT(ISERROR(SEARCH("MABA",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:F46">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Tunai">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Tunai">
       <formula>NOT(ISERROR(SEARCH("Tunai",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="Transfer">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Transfer">
       <formula>NOT(ISERROR(SEARCH("Transfer",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G46">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>150000</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>100000</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>125000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F46">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"LUNAS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17508,17 +17506,17 @@
       <c r="A2" s="172"/>
       <c r="B2" s="173"/>
       <c r="C2" s="173"/>
-      <c r="D2" s="343" t="s">
+      <c r="D2" s="400" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="343"/>
-      <c r="F2" s="343"/>
-      <c r="G2" s="343"/>
-      <c r="H2" s="343"/>
-      <c r="I2" s="343"/>
-      <c r="J2" s="343"/>
-      <c r="K2" s="343"/>
-      <c r="L2" s="343"/>
+      <c r="E2" s="400"/>
+      <c r="F2" s="400"/>
+      <c r="G2" s="400"/>
+      <c r="H2" s="400"/>
+      <c r="I2" s="400"/>
+      <c r="J2" s="400"/>
+      <c r="K2" s="400"/>
+      <c r="L2" s="400"/>
       <c r="M2" s="174"/>
       <c r="N2" s="24"/>
     </row>
@@ -17536,205 +17534,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="176"/>
-      <c r="U3" s="393" t="s">
+      <c r="U3" s="343" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="394"/>
-      <c r="W3" s="395" t="s">
+      <c r="V3" s="344"/>
+      <c r="W3" s="345" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="394"/>
-      <c r="Y3" s="394"/>
-      <c r="Z3" s="394"/>
-      <c r="AA3" s="394"/>
-      <c r="AB3" s="394"/>
-      <c r="AC3" s="394"/>
-      <c r="AD3" s="396"/>
+      <c r="X3" s="344"/>
+      <c r="Y3" s="344"/>
+      <c r="Z3" s="344"/>
+      <c r="AA3" s="344"/>
+      <c r="AB3" s="344"/>
+      <c r="AC3" s="344"/>
+      <c r="AD3" s="346"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="175"/>
-      <c r="B4" s="358" t="s">
+      <c r="B4" s="404" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="359"/>
-      <c r="D4" s="359"/>
-      <c r="E4" s="359"/>
-      <c r="F4" s="359"/>
+      <c r="C4" s="405"/>
+      <c r="D4" s="405"/>
+      <c r="E4" s="405"/>
+      <c r="F4" s="405"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="362" t="s">
+      <c r="I4" s="352" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="315"/>
-      <c r="K4" s="315"/>
-      <c r="L4" s="315"/>
+      <c r="J4" s="318"/>
+      <c r="K4" s="318"/>
+      <c r="L4" s="318"/>
       <c r="M4" s="176"/>
-      <c r="U4" s="405" t="s">
+      <c r="U4" s="364" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="315"/>
-      <c r="W4" s="362" t="s">
+      <c r="V4" s="318"/>
+      <c r="W4" s="352" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="315"/>
-      <c r="Y4" s="315"/>
-      <c r="Z4" s="315"/>
-      <c r="AA4" s="315"/>
-      <c r="AB4" s="315"/>
-      <c r="AC4" s="315"/>
-      <c r="AD4" s="382"/>
+      <c r="X4" s="318"/>
+      <c r="Y4" s="318"/>
+      <c r="Z4" s="318"/>
+      <c r="AA4" s="318"/>
+      <c r="AB4" s="318"/>
+      <c r="AC4" s="318"/>
+      <c r="AD4" s="347"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="175"/>
-      <c r="B5" s="353" t="s">
+      <c r="B5" s="369" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="315"/>
-      <c r="D5" s="315"/>
-      <c r="E5" s="315"/>
-      <c r="F5" s="315"/>
+      <c r="C5" s="318"/>
+      <c r="D5" s="318"/>
+      <c r="E5" s="318"/>
+      <c r="F5" s="318"/>
       <c r="G5" s="152">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="351" t="s">
+      <c r="I5" s="371" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="352"/>
-      <c r="K5" s="363">
+      <c r="J5" s="392"/>
+      <c r="K5" s="394">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="364"/>
+      <c r="L5" s="395"/>
       <c r="M5" s="176"/>
-      <c r="U5" s="389" t="s">
+      <c r="U5" s="365" t="s">
         <v>231</v>
       </c>
-      <c r="V5" s="390"/>
-      <c r="W5" s="351" t="s">
+      <c r="V5" s="366"/>
+      <c r="W5" s="371" t="s">
         <v>232</v>
       </c>
-      <c r="X5" s="376"/>
-      <c r="Y5" s="376"/>
-      <c r="Z5" s="376"/>
-      <c r="AA5" s="376"/>
-      <c r="AB5" s="376"/>
-      <c r="AC5" s="376"/>
-      <c r="AD5" s="377"/>
+      <c r="X5" s="372"/>
+      <c r="Y5" s="372"/>
+      <c r="Z5" s="372"/>
+      <c r="AA5" s="372"/>
+      <c r="AB5" s="372"/>
+      <c r="AC5" s="372"/>
+      <c r="AD5" s="373"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="175"/>
-      <c r="B6" s="345" t="s">
+      <c r="B6" s="362" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="346"/>
-      <c r="D6" s="346"/>
-      <c r="E6" s="346"/>
-      <c r="F6" s="346"/>
+      <c r="C6" s="363"/>
+      <c r="D6" s="363"/>
+      <c r="E6" s="363"/>
+      <c r="F6" s="363"/>
       <c r="G6" s="152">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="349" t="s">
+      <c r="I6" s="393" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="350"/>
-      <c r="K6" s="365">
+      <c r="J6" s="388"/>
+      <c r="K6" s="396">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="366"/>
+      <c r="L6" s="397"/>
       <c r="M6" s="176"/>
-      <c r="U6" s="391"/>
-      <c r="V6" s="392"/>
-      <c r="W6" s="378" t="s">
+      <c r="U6" s="367"/>
+      <c r="V6" s="368"/>
+      <c r="W6" s="353" t="s">
         <v>233</v>
       </c>
-      <c r="X6" s="379"/>
-      <c r="Y6" s="379"/>
-      <c r="Z6" s="379"/>
-      <c r="AA6" s="379"/>
-      <c r="AB6" s="379"/>
-      <c r="AC6" s="379"/>
-      <c r="AD6" s="380"/>
+      <c r="X6" s="354"/>
+      <c r="Y6" s="354"/>
+      <c r="Z6" s="354"/>
+      <c r="AA6" s="354"/>
+      <c r="AB6" s="354"/>
+      <c r="AC6" s="354"/>
+      <c r="AD6" s="355"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="175"/>
-      <c r="B7" s="356" t="s">
+      <c r="B7" s="374" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="357"/>
-      <c r="D7" s="357"/>
-      <c r="E7" s="357"/>
-      <c r="F7" s="350"/>
+      <c r="C7" s="375"/>
+      <c r="D7" s="375"/>
+      <c r="E7" s="375"/>
+      <c r="F7" s="388"/>
       <c r="G7" s="152">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="349" t="s">
+      <c r="I7" s="393" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="350"/>
-      <c r="K7" s="360">
+      <c r="J7" s="388"/>
+      <c r="K7" s="398">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="361"/>
+      <c r="L7" s="399"/>
       <c r="M7" s="176"/>
-      <c r="U7" s="397"/>
-      <c r="V7" s="398"/>
-      <c r="W7" s="362" t="s">
+      <c r="U7" s="350"/>
+      <c r="V7" s="351"/>
+      <c r="W7" s="352" t="s">
         <v>234</v>
       </c>
-      <c r="X7" s="315"/>
-      <c r="Y7" s="315"/>
-      <c r="Z7" s="315"/>
-      <c r="AA7" s="315"/>
-      <c r="AB7" s="315"/>
-      <c r="AC7" s="315"/>
-      <c r="AD7" s="382"/>
+      <c r="X7" s="318"/>
+      <c r="Y7" s="318"/>
+      <c r="Z7" s="318"/>
+      <c r="AA7" s="318"/>
+      <c r="AB7" s="318"/>
+      <c r="AC7" s="318"/>
+      <c r="AD7" s="347"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="175"/>
-      <c r="B8" s="354" t="s">
+      <c r="B8" s="402" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="355"/>
-      <c r="D8" s="355"/>
-      <c r="E8" s="355"/>
-      <c r="F8" s="355"/>
+      <c r="C8" s="403"/>
+      <c r="D8" s="403"/>
+      <c r="E8" s="403"/>
+      <c r="F8" s="403"/>
       <c r="G8" s="153">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="351" t="s">
+      <c r="I8" s="371" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="352"/>
-      <c r="K8" s="347">
+      <c r="J8" s="392"/>
+      <c r="K8" s="383">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="348"/>
+      <c r="L8" s="384"/>
       <c r="M8" s="176"/>
-      <c r="U8" s="401" t="s">
+      <c r="U8" s="358" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="402"/>
-      <c r="W8" s="378" t="s">
+      <c r="V8" s="359"/>
+      <c r="W8" s="353" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="379"/>
-      <c r="Y8" s="379"/>
-      <c r="Z8" s="379"/>
-      <c r="AA8" s="379"/>
-      <c r="AB8" s="379"/>
-      <c r="AC8" s="379"/>
-      <c r="AD8" s="380"/>
+      <c r="X8" s="354"/>
+      <c r="Y8" s="354"/>
+      <c r="Z8" s="354"/>
+      <c r="AA8" s="354"/>
+      <c r="AB8" s="354"/>
+      <c r="AC8" s="354"/>
+      <c r="AD8" s="355"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="175"/>
@@ -17750,28 +17748,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="176"/>
-      <c r="U9" s="403"/>
-      <c r="V9" s="404"/>
-      <c r="W9" s="378" t="s">
+      <c r="U9" s="360"/>
+      <c r="V9" s="361"/>
+      <c r="W9" s="353" t="s">
         <v>237</v>
       </c>
-      <c r="X9" s="379"/>
-      <c r="Y9" s="379"/>
-      <c r="Z9" s="379"/>
-      <c r="AA9" s="379"/>
-      <c r="AB9" s="379"/>
-      <c r="AC9" s="379"/>
-      <c r="AD9" s="380"/>
+      <c r="X9" s="354"/>
+      <c r="Y9" s="354"/>
+      <c r="Z9" s="354"/>
+      <c r="AA9" s="354"/>
+      <c r="AB9" s="354"/>
+      <c r="AC9" s="354"/>
+      <c r="AD9" s="355"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="175"/>
-      <c r="B10" s="315" t="s">
+      <c r="B10" s="318" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="315"/>
-      <c r="D10" s="315"/>
-      <c r="E10" s="315"/>
-      <c r="F10" s="315"/>
+      <c r="C10" s="318"/>
+      <c r="D10" s="318"/>
+      <c r="E10" s="318"/>
+      <c r="F10" s="318"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -17782,30 +17780,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="176"/>
-      <c r="U10" s="345" t="s">
+      <c r="U10" s="362" t="s">
         <v>243</v>
       </c>
-      <c r="V10" s="346"/>
-      <c r="W10" s="315" t="s">
+      <c r="V10" s="363"/>
+      <c r="W10" s="318" t="s">
         <v>257</v>
       </c>
-      <c r="X10" s="315"/>
-      <c r="Y10" s="315"/>
-      <c r="Z10" s="315"/>
-      <c r="AA10" s="315"/>
-      <c r="AB10" s="315"/>
-      <c r="AC10" s="315"/>
-      <c r="AD10" s="382"/>
+      <c r="X10" s="318"/>
+      <c r="Y10" s="318"/>
+      <c r="Z10" s="318"/>
+      <c r="AA10" s="318"/>
+      <c r="AB10" s="318"/>
+      <c r="AC10" s="318"/>
+      <c r="AD10" s="347"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="175"/>
-      <c r="B11" s="315" t="s">
+      <c r="B11" s="318" t="s">
         <v>254</v>
       </c>
-      <c r="C11" s="315"/>
-      <c r="D11" s="315"/>
-      <c r="E11" s="315"/>
-      <c r="F11" s="315"/>
+      <c r="C11" s="318"/>
+      <c r="D11" s="318"/>
+      <c r="E11" s="318"/>
+      <c r="F11" s="318"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -17815,30 +17813,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="176"/>
-      <c r="U11" s="345" t="s">
+      <c r="U11" s="362" t="s">
         <v>256</v>
       </c>
-      <c r="V11" s="346"/>
-      <c r="W11" s="399" t="s">
+      <c r="V11" s="363"/>
+      <c r="W11" s="356" t="s">
         <v>258</v>
       </c>
-      <c r="X11" s="399"/>
-      <c r="Y11" s="399"/>
-      <c r="Z11" s="399"/>
-      <c r="AA11" s="399"/>
-      <c r="AB11" s="399"/>
-      <c r="AC11" s="399"/>
-      <c r="AD11" s="400"/>
+      <c r="X11" s="356"/>
+      <c r="Y11" s="356"/>
+      <c r="Z11" s="356"/>
+      <c r="AA11" s="356"/>
+      <c r="AB11" s="356"/>
+      <c r="AC11" s="356"/>
+      <c r="AD11" s="357"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="175"/>
-      <c r="B12" s="344" t="s">
+      <c r="B12" s="401" t="s">
         <v>255</v>
       </c>
-      <c r="C12" s="344"/>
-      <c r="D12" s="344"/>
-      <c r="E12" s="344"/>
-      <c r="F12" s="344"/>
+      <c r="C12" s="401"/>
+      <c r="D12" s="401"/>
+      <c r="E12" s="401"/>
+      <c r="F12" s="401"/>
       <c r="G12" s="180">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -17849,16 +17847,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="176"/>
-      <c r="U12" s="345"/>
-      <c r="V12" s="346"/>
-      <c r="W12" s="315"/>
-      <c r="X12" s="315"/>
-      <c r="Y12" s="315"/>
-      <c r="Z12" s="315"/>
-      <c r="AA12" s="315"/>
-      <c r="AB12" s="315"/>
-      <c r="AC12" s="315"/>
-      <c r="AD12" s="382"/>
+      <c r="U12" s="362"/>
+      <c r="V12" s="363"/>
+      <c r="W12" s="318"/>
+      <c r="X12" s="318"/>
+      <c r="Y12" s="318"/>
+      <c r="Z12" s="318"/>
+      <c r="AA12" s="318"/>
+      <c r="AB12" s="318"/>
+      <c r="AC12" s="318"/>
+      <c r="AD12" s="347"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="177"/>
@@ -17874,64 +17872,64 @@
       <c r="K13" s="178"/>
       <c r="L13" s="178"/>
       <c r="M13" s="179"/>
-      <c r="U13" s="345"/>
-      <c r="V13" s="346"/>
-      <c r="W13" s="315"/>
-      <c r="X13" s="315"/>
-      <c r="Y13" s="315"/>
-      <c r="Z13" s="315"/>
-      <c r="AA13" s="315"/>
-      <c r="AB13" s="315"/>
-      <c r="AC13" s="315"/>
-      <c r="AD13" s="382"/>
+      <c r="U13" s="362"/>
+      <c r="V13" s="363"/>
+      <c r="W13" s="318"/>
+      <c r="X13" s="318"/>
+      <c r="Y13" s="318"/>
+      <c r="Z13" s="318"/>
+      <c r="AA13" s="318"/>
+      <c r="AB13" s="318"/>
+      <c r="AC13" s="318"/>
+      <c r="AD13" s="347"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="383"/>
-      <c r="V14" s="384"/>
-      <c r="W14" s="374"/>
-      <c r="X14" s="374"/>
-      <c r="Y14" s="374"/>
-      <c r="Z14" s="374"/>
-      <c r="AA14" s="374"/>
-      <c r="AB14" s="374"/>
-      <c r="AC14" s="374"/>
-      <c r="AD14" s="375"/>
+      <c r="U14" s="377"/>
+      <c r="V14" s="378"/>
+      <c r="W14" s="348"/>
+      <c r="X14" s="348"/>
+      <c r="Y14" s="348"/>
+      <c r="Z14" s="348"/>
+      <c r="AA14" s="348"/>
+      <c r="AB14" s="348"/>
+      <c r="AC14" s="348"/>
+      <c r="AD14" s="349"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="172"/>
       <c r="B18" s="173"/>
       <c r="C18" s="173"/>
-      <c r="D18" s="343" t="s">
+      <c r="D18" s="400" t="s">
         <v>249</v>
       </c>
-      <c r="E18" s="343"/>
-      <c r="F18" s="343"/>
-      <c r="G18" s="343"/>
-      <c r="H18" s="343"/>
-      <c r="I18" s="343"/>
-      <c r="J18" s="343"/>
-      <c r="K18" s="343"/>
-      <c r="L18" s="343"/>
+      <c r="E18" s="400"/>
+      <c r="F18" s="400"/>
+      <c r="G18" s="400"/>
+      <c r="H18" s="400"/>
+      <c r="I18" s="400"/>
+      <c r="J18" s="400"/>
+      <c r="K18" s="400"/>
+      <c r="L18" s="400"/>
       <c r="M18" s="174"/>
-      <c r="O18" s="385" t="s">
+      <c r="O18" s="379" t="s">
         <v>250</v>
       </c>
-      <c r="P18" s="386"/>
-      <c r="Q18" s="386"/>
-      <c r="R18" s="386"/>
-      <c r="S18" s="387"/>
+      <c r="P18" s="380"/>
+      <c r="Q18" s="380"/>
+      <c r="R18" s="380"/>
+      <c r="S18" s="381"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="175"/>
       <c r="M19" s="176"/>
-      <c r="O19" s="353" t="s">
+      <c r="O19" s="369" t="s">
         <v>251</v>
       </c>
-      <c r="P19" s="315"/>
-      <c r="Q19" s="315"/>
-      <c r="R19" s="315"/>
-      <c r="S19" s="382"/>
+      <c r="P19" s="318"/>
+      <c r="Q19" s="318"/>
+      <c r="R19" s="318"/>
+      <c r="S19" s="347"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="175"/>
@@ -17942,119 +17940,119 @@
       <c r="F20" s="200"/>
       <c r="G20" s="68"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="362" t="s">
+      <c r="I20" s="352" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="315"/>
-      <c r="K20" s="315"/>
-      <c r="L20" s="315"/>
+      <c r="J20" s="318"/>
+      <c r="K20" s="318"/>
+      <c r="L20" s="318"/>
       <c r="M20" s="176"/>
-      <c r="O20" s="353" t="s">
+      <c r="O20" s="369" t="s">
         <v>252</v>
       </c>
-      <c r="P20" s="315"/>
-      <c r="Q20" s="315"/>
-      <c r="R20" s="315"/>
-      <c r="S20" s="382"/>
+      <c r="P20" s="318"/>
+      <c r="Q20" s="318"/>
+      <c r="R20" s="318"/>
+      <c r="S20" s="347"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="175"/>
-      <c r="B21" s="367" t="s">
+      <c r="B21" s="385" t="s">
         <v>296</v>
       </c>
-      <c r="C21" s="368"/>
-      <c r="D21" s="368"/>
-      <c r="E21" s="368"/>
-      <c r="F21" s="369"/>
+      <c r="C21" s="386"/>
+      <c r="D21" s="386"/>
+      <c r="E21" s="386"/>
+      <c r="F21" s="387"/>
       <c r="G21" s="70">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="351" t="s">
+      <c r="I21" s="371" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="352"/>
-      <c r="K21" s="363">
+      <c r="J21" s="392"/>
+      <c r="K21" s="394">
         <f>G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="L21" s="364"/>
+      <c r="L21" s="395"/>
       <c r="M21" s="176"/>
       <c r="N21" s="170"/>
-      <c r="O21" s="388" t="s">
+      <c r="O21" s="382" t="s">
         <v>259</v>
       </c>
-      <c r="P21" s="376"/>
-      <c r="Q21" s="376"/>
-      <c r="R21" s="376"/>
-      <c r="S21" s="377"/>
+      <c r="P21" s="372"/>
+      <c r="Q21" s="372"/>
+      <c r="R21" s="372"/>
+      <c r="S21" s="373"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="175"/>
-      <c r="B22" s="356" t="s">
+      <c r="B22" s="374" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="357"/>
-      <c r="D22" s="357"/>
-      <c r="E22" s="357"/>
-      <c r="F22" s="350"/>
+      <c r="C22" s="375"/>
+      <c r="D22" s="375"/>
+      <c r="E22" s="375"/>
+      <c r="F22" s="388"/>
       <c r="G22" s="152">
         <f>G21</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="349" t="s">
+      <c r="I22" s="393" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="350"/>
-      <c r="K22" s="365">
+      <c r="J22" s="388"/>
+      <c r="K22" s="396">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="L22" s="366"/>
+      <c r="L22" s="397"/>
       <c r="M22" s="176"/>
       <c r="N22" s="170"/>
-      <c r="O22" s="356" t="s">
+      <c r="O22" s="374" t="s">
         <v>260</v>
       </c>
-      <c r="P22" s="357"/>
-      <c r="Q22" s="357"/>
-      <c r="R22" s="357"/>
-      <c r="S22" s="381"/>
+      <c r="P22" s="375"/>
+      <c r="Q22" s="375"/>
+      <c r="R22" s="375"/>
+      <c r="S22" s="376"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="175"/>
-      <c r="B23" s="370" t="s">
+      <c r="B23" s="389" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="371"/>
-      <c r="D23" s="371"/>
-      <c r="E23" s="371"/>
-      <c r="F23" s="372"/>
+      <c r="C23" s="390"/>
+      <c r="D23" s="390"/>
+      <c r="E23" s="390"/>
+      <c r="F23" s="391"/>
       <c r="G23" s="153">
         <f>K24</f>
         <v>1568729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="349" t="s">
+      <c r="I23" s="393" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="350"/>
-      <c r="K23" s="360">
+      <c r="J23" s="388"/>
+      <c r="K23" s="398">
         <f>Pemasukkan!L31</f>
         <v>690000</v>
       </c>
-      <c r="L23" s="361"/>
+      <c r="L23" s="399"/>
       <c r="M23" s="176"/>
       <c r="N23" s="170"/>
-      <c r="O23" s="356" t="s">
+      <c r="O23" s="374" t="s">
         <v>261</v>
       </c>
-      <c r="P23" s="357"/>
-      <c r="Q23" s="357"/>
-      <c r="R23" s="357"/>
-      <c r="S23" s="381"/>
+      <c r="P23" s="375"/>
+      <c r="Q23" s="375"/>
+      <c r="R23" s="375"/>
+      <c r="S23" s="376"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="175"/>
@@ -18065,24 +18063,24 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="351" t="s">
+      <c r="I24" s="371" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="352"/>
-      <c r="K24" s="347">
+      <c r="J24" s="392"/>
+      <c r="K24" s="383">
         <f>(K21-K22)+K23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="L24" s="348"/>
+      <c r="L24" s="384"/>
       <c r="M24" s="176"/>
       <c r="N24" s="170"/>
-      <c r="O24" s="356" t="s">
+      <c r="O24" s="374" t="s">
         <v>262</v>
       </c>
-      <c r="P24" s="357"/>
-      <c r="Q24" s="357"/>
-      <c r="R24" s="357"/>
-      <c r="S24" s="381"/>
+      <c r="P24" s="375"/>
+      <c r="Q24" s="375"/>
+      <c r="R24" s="375"/>
+      <c r="S24" s="376"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="175"/>
@@ -18099,13 +18097,13 @@
       <c r="L25" s="24"/>
       <c r="M25" s="176"/>
       <c r="N25" s="170"/>
-      <c r="O25" s="353" t="s">
+      <c r="O25" s="369" t="s">
         <v>267</v>
       </c>
-      <c r="P25" s="315"/>
-      <c r="Q25" s="315"/>
-      <c r="R25" s="315"/>
-      <c r="S25" s="382"/>
+      <c r="P25" s="318"/>
+      <c r="Q25" s="318"/>
+      <c r="R25" s="318"/>
+      <c r="S25" s="347"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="175"/>
@@ -18122,11 +18120,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="176"/>
       <c r="N26" s="170"/>
-      <c r="O26" s="373"/>
-      <c r="P26" s="374"/>
-      <c r="Q26" s="374"/>
-      <c r="R26" s="374"/>
-      <c r="S26" s="375"/>
+      <c r="O26" s="370"/>
+      <c r="P26" s="348"/>
+      <c r="Q26" s="348"/>
+      <c r="R26" s="348"/>
+      <c r="S26" s="349"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="177"/>
@@ -18161,6 +18159,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="D18:L18"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="W5:AD5"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="O18:S18"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O23:S23"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="W4:AD4"/>
+    <mergeCell ref="W8:AD8"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="O25:S25"/>
     <mergeCell ref="U3:V3"/>
     <mergeCell ref="W3:AD3"/>
     <mergeCell ref="W12:AD12"/>
@@ -18177,53 +18222,6 @@
     <mergeCell ref="U12:V12"/>
     <mergeCell ref="U13:V13"/>
     <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:AD4"/>
-    <mergeCell ref="W8:AD8"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="O25:S25"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="W5:AD5"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="O24:S24"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="O18:S18"/>
-    <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O23:S23"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="D18:L18"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -18257,44 +18255,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="406" t="s">
+      <c r="C2" s="415" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="407"/>
-      <c r="E2" s="407"/>
-      <c r="F2" s="407"/>
-      <c r="G2" s="407"/>
-      <c r="H2" s="407"/>
-      <c r="I2" s="407"/>
-      <c r="J2" s="407"/>
-      <c r="K2" s="407"/>
+      <c r="D2" s="416"/>
+      <c r="E2" s="416"/>
+      <c r="F2" s="416"/>
+      <c r="G2" s="416"/>
+      <c r="H2" s="416"/>
+      <c r="I2" s="416"/>
+      <c r="J2" s="416"/>
+      <c r="K2" s="416"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="407"/>
-      <c r="D3" s="407"/>
-      <c r="E3" s="407"/>
-      <c r="F3" s="407"/>
-      <c r="G3" s="407"/>
-      <c r="H3" s="407"/>
-      <c r="I3" s="407"/>
-      <c r="J3" s="407"/>
-      <c r="K3" s="407"/>
+      <c r="C3" s="416"/>
+      <c r="D3" s="416"/>
+      <c r="E3" s="416"/>
+      <c r="F3" s="416"/>
+      <c r="G3" s="416"/>
+      <c r="H3" s="416"/>
+      <c r="I3" s="416"/>
+      <c r="J3" s="416"/>
+      <c r="K3" s="416"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="414" t="s">
+      <c r="C5" s="408" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="414"/>
-      <c r="E5" s="414"/>
-      <c r="F5" s="414"/>
-      <c r="G5" s="414"/>
-      <c r="I5" s="414" t="s">
+      <c r="D5" s="408"/>
+      <c r="E5" s="408"/>
+      <c r="F5" s="408"/>
+      <c r="G5" s="408"/>
+      <c r="I5" s="408" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="414"/>
-      <c r="K5" s="414"/>
-      <c r="L5" s="414"/>
-      <c r="M5" s="414"/>
+      <c r="J5" s="408"/>
+      <c r="K5" s="408"/>
+      <c r="L5" s="408"/>
+      <c r="M5" s="408"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -18734,88 +18732,88 @@
       <c r="M28" s="170"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="358" t="s">
+      <c r="D29" s="404" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="359"/>
-      <c r="F29" s="408">
+      <c r="E29" s="405"/>
+      <c r="F29" s="409">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="409"/>
+      <c r="G29" s="410"/>
       <c r="I29" s="170"/>
-      <c r="J29" s="358" t="s">
+      <c r="J29" s="404" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="359"/>
-      <c r="L29" s="408">
+      <c r="K29" s="405"/>
+      <c r="L29" s="409">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="409"/>
+      <c r="M29" s="410"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="405" t="s">
+      <c r="D30" s="364" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="315"/>
-      <c r="F30" s="410">
+      <c r="E30" s="318"/>
+      <c r="F30" s="411">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="411"/>
+      <c r="G30" s="412"/>
       <c r="I30" s="170"/>
-      <c r="J30" s="405" t="s">
+      <c r="J30" s="364" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="315"/>
-      <c r="L30" s="410">
+      <c r="K30" s="318"/>
+      <c r="L30" s="411">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="411"/>
+      <c r="M30" s="412"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="353" t="s">
+      <c r="D31" s="369" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="315"/>
-      <c r="F31" s="415">
+      <c r="E31" s="318"/>
+      <c r="F31" s="413">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="416"/>
+      <c r="G31" s="414"/>
       <c r="I31" s="170"/>
-      <c r="J31" s="353" t="s">
+      <c r="J31" s="369" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="315"/>
-      <c r="L31" s="415">
+      <c r="K31" s="318"/>
+      <c r="L31" s="413">
         <f>L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="416"/>
+      <c r="M31" s="414"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="354" t="s">
+      <c r="D32" s="402" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="355"/>
-      <c r="F32" s="412">
+      <c r="E32" s="403"/>
+      <c r="F32" s="406">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="413"/>
+      <c r="G32" s="407"/>
       <c r="I32" s="170"/>
-      <c r="J32" s="354" t="s">
+      <c r="J32" s="402" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="355"/>
-      <c r="L32" s="412">
+      <c r="K32" s="403"/>
+      <c r="L32" s="406">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="413"/>
+      <c r="M32" s="407"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19007,6 +19005,12 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C2:K3"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J29:K29"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="I5:M5"/>
@@ -19020,12 +19024,6 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J32:K32"/>
-    <mergeCell ref="C2:K3"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -19058,44 +19056,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="417" t="s">
+      <c r="C2" s="421" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="418"/>
-      <c r="E2" s="418"/>
-      <c r="F2" s="418"/>
-      <c r="G2" s="418"/>
-      <c r="H2" s="418"/>
-      <c r="I2" s="418"/>
-      <c r="J2" s="418"/>
-      <c r="K2" s="418"/>
+      <c r="D2" s="422"/>
+      <c r="E2" s="422"/>
+      <c r="F2" s="422"/>
+      <c r="G2" s="422"/>
+      <c r="H2" s="422"/>
+      <c r="I2" s="422"/>
+      <c r="J2" s="422"/>
+      <c r="K2" s="422"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="418"/>
-      <c r="D3" s="418"/>
-      <c r="E3" s="418"/>
-      <c r="F3" s="418"/>
-      <c r="G3" s="418"/>
-      <c r="H3" s="418"/>
-      <c r="I3" s="418"/>
-      <c r="J3" s="418"/>
-      <c r="K3" s="418"/>
+      <c r="C3" s="422"/>
+      <c r="D3" s="422"/>
+      <c r="E3" s="422"/>
+      <c r="F3" s="422"/>
+      <c r="G3" s="422"/>
+      <c r="H3" s="422"/>
+      <c r="I3" s="422"/>
+      <c r="J3" s="422"/>
+      <c r="K3" s="422"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="414" t="s">
+      <c r="C5" s="408" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="414"/>
-      <c r="E5" s="414"/>
-      <c r="F5" s="414"/>
-      <c r="G5" s="414"/>
-      <c r="I5" s="414" t="s">
+      <c r="D5" s="408"/>
+      <c r="E5" s="408"/>
+      <c r="F5" s="408"/>
+      <c r="G5" s="408"/>
+      <c r="I5" s="408" t="s">
         <v>246</v>
       </c>
-      <c r="J5" s="414"/>
-      <c r="K5" s="414"/>
-      <c r="L5" s="414"/>
-      <c r="M5" s="414"/>
+      <c r="J5" s="408"/>
+      <c r="K5" s="408"/>
+      <c r="L5" s="408"/>
+      <c r="M5" s="408"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -19579,20 +19577,20 @@
       <c r="M28" s="170"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="393" t="s">
+      <c r="D29" s="343" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="395"/>
+      <c r="E29" s="345"/>
       <c r="F29" s="419">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
       <c r="G29" s="420"/>
       <c r="I29" s="170"/>
-      <c r="J29" s="393" t="s">
+      <c r="J29" s="343" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="395"/>
+      <c r="K29" s="345"/>
       <c r="L29" s="419">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
@@ -19600,67 +19598,67 @@
       <c r="M29" s="420"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="353" t="s">
+      <c r="D30" s="369" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="315"/>
-      <c r="F30" s="410">
+      <c r="E30" s="318"/>
+      <c r="F30" s="411">
         <f>F27</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="411"/>
+      <c r="G30" s="412"/>
       <c r="I30" s="170"/>
-      <c r="J30" s="353" t="s">
+      <c r="J30" s="369" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="315"/>
-      <c r="L30" s="410">
+      <c r="K30" s="318"/>
+      <c r="L30" s="411">
         <f>L27</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="411"/>
+      <c r="M30" s="412"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="353" t="s">
+      <c r="D31" s="369" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="315"/>
-      <c r="F31" s="415">
+      <c r="E31" s="318"/>
+      <c r="F31" s="413">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="416"/>
+      <c r="G31" s="414"/>
       <c r="I31" s="170"/>
-      <c r="J31" s="353" t="s">
+      <c r="J31" s="369" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="315"/>
-      <c r="L31" s="415">
+      <c r="K31" s="318"/>
+      <c r="L31" s="413">
         <f>Pemasukkan!L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="416"/>
+      <c r="M31" s="414"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="354" t="s">
+      <c r="D32" s="402" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="355"/>
-      <c r="F32" s="421">
+      <c r="E32" s="403"/>
+      <c r="F32" s="417">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="422"/>
+      <c r="G32" s="418"/>
       <c r="I32" s="170"/>
-      <c r="J32" s="354" t="s">
+      <c r="J32" s="402" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="355"/>
-      <c r="L32" s="421">
+      <c r="K32" s="403"/>
+      <c r="L32" s="417">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="422"/>
+      <c r="M32" s="418"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19852,14 +19850,6 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
     <mergeCell ref="C2:K3"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
@@ -19871,6 +19861,14 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Bayar Makrab Gagas, Once, Ghazi
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="394">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -1199,6 +1199,12 @@
   </si>
   <si>
     <t>UANG MAKRAB MASIH HUTANG KE RAPLI 2RB UNTUK TIKET MASUK KLERESEDE</t>
+  </si>
+  <si>
+    <t>Gagas</t>
+  </si>
+  <si>
+    <t>Ghazi</t>
   </si>
 </sst>
 </file>
@@ -3046,29 +3052,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3084,37 +3081,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3122,29 +3121,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3194,6 +3200,159 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3206,33 +3365,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3252,136 +3390,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3392,29 +3419,23 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3422,18 +3443,6 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3484,9 +3493,6 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4690,126 +4696,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="291" t="s">
+      <c r="A1" s="285" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="292"/>
-      <c r="C1" s="292"/>
-      <c r="D1" s="292"/>
-      <c r="E1" s="292"/>
-      <c r="F1" s="292"/>
-      <c r="G1" s="292"/>
-      <c r="H1" s="292"/>
-      <c r="I1" s="292"/>
-      <c r="J1" s="292"/>
-      <c r="K1" s="292"/>
-      <c r="L1" s="292"/>
-      <c r="M1" s="292"/>
-      <c r="N1" s="292"/>
-      <c r="O1" s="292"/>
-      <c r="P1" s="292"/>
-      <c r="Q1" s="292"/>
-      <c r="R1" s="292"/>
+      <c r="B1" s="286"/>
+      <c r="C1" s="286"/>
+      <c r="D1" s="286"/>
+      <c r="E1" s="286"/>
+      <c r="F1" s="286"/>
+      <c r="G1" s="286"/>
+      <c r="H1" s="286"/>
+      <c r="I1" s="286"/>
+      <c r="J1" s="286"/>
+      <c r="K1" s="286"/>
+      <c r="L1" s="286"/>
+      <c r="M1" s="286"/>
+      <c r="N1" s="286"/>
+      <c r="O1" s="286"/>
+      <c r="P1" s="286"/>
+      <c r="Q1" s="286"/>
+      <c r="R1" s="286"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="293"/>
-      <c r="B2" s="294"/>
-      <c r="C2" s="294"/>
-      <c r="D2" s="294"/>
-      <c r="E2" s="294"/>
-      <c r="F2" s="294"/>
-      <c r="G2" s="294"/>
-      <c r="H2" s="294"/>
-      <c r="I2" s="294"/>
-      <c r="J2" s="294"/>
-      <c r="K2" s="294"/>
-      <c r="L2" s="294"/>
-      <c r="M2" s="294"/>
-      <c r="N2" s="294"/>
-      <c r="O2" s="294"/>
-      <c r="P2" s="294"/>
-      <c r="Q2" s="294"/>
-      <c r="R2" s="294"/>
+      <c r="A2" s="287"/>
+      <c r="B2" s="288"/>
+      <c r="C2" s="288"/>
+      <c r="D2" s="288"/>
+      <c r="E2" s="288"/>
+      <c r="F2" s="288"/>
+      <c r="G2" s="288"/>
+      <c r="H2" s="288"/>
+      <c r="I2" s="288"/>
+      <c r="J2" s="288"/>
+      <c r="K2" s="288"/>
+      <c r="L2" s="288"/>
+      <c r="M2" s="288"/>
+      <c r="N2" s="288"/>
+      <c r="O2" s="288"/>
+      <c r="P2" s="288"/>
+      <c r="Q2" s="288"/>
+      <c r="R2" s="288"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="293"/>
-      <c r="B3" s="294"/>
-      <c r="C3" s="294"/>
-      <c r="D3" s="294"/>
-      <c r="E3" s="294"/>
-      <c r="F3" s="294"/>
-      <c r="G3" s="294"/>
-      <c r="H3" s="294"/>
-      <c r="I3" s="294"/>
-      <c r="J3" s="294"/>
-      <c r="K3" s="294"/>
-      <c r="L3" s="294"/>
-      <c r="M3" s="294"/>
-      <c r="N3" s="294"/>
-      <c r="O3" s="294"/>
-      <c r="P3" s="294"/>
-      <c r="Q3" s="294"/>
-      <c r="R3" s="294"/>
+      <c r="A3" s="287"/>
+      <c r="B3" s="288"/>
+      <c r="C3" s="288"/>
+      <c r="D3" s="288"/>
+      <c r="E3" s="288"/>
+      <c r="F3" s="288"/>
+      <c r="G3" s="288"/>
+      <c r="H3" s="288"/>
+      <c r="I3" s="288"/>
+      <c r="J3" s="288"/>
+      <c r="K3" s="288"/>
+      <c r="L3" s="288"/>
+      <c r="M3" s="288"/>
+      <c r="N3" s="288"/>
+      <c r="O3" s="288"/>
+      <c r="P3" s="288"/>
+      <c r="Q3" s="288"/>
+      <c r="R3" s="288"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="293"/>
-      <c r="B4" s="294"/>
-      <c r="C4" s="294"/>
-      <c r="D4" s="294"/>
-      <c r="E4" s="294"/>
-      <c r="F4" s="294"/>
-      <c r="G4" s="294"/>
-      <c r="H4" s="294"/>
-      <c r="I4" s="294"/>
-      <c r="J4" s="294"/>
-      <c r="K4" s="294"/>
-      <c r="L4" s="294"/>
-      <c r="M4" s="294"/>
-      <c r="N4" s="294"/>
-      <c r="O4" s="294"/>
-      <c r="P4" s="294"/>
-      <c r="Q4" s="294"/>
-      <c r="R4" s="294"/>
+      <c r="A4" s="287"/>
+      <c r="B4" s="288"/>
+      <c r="C4" s="288"/>
+      <c r="D4" s="288"/>
+      <c r="E4" s="288"/>
+      <c r="F4" s="288"/>
+      <c r="G4" s="288"/>
+      <c r="H4" s="288"/>
+      <c r="I4" s="288"/>
+      <c r="J4" s="288"/>
+      <c r="K4" s="288"/>
+      <c r="L4" s="288"/>
+      <c r="M4" s="288"/>
+      <c r="N4" s="288"/>
+      <c r="O4" s="288"/>
+      <c r="P4" s="288"/>
+      <c r="Q4" s="288"/>
+      <c r="R4" s="288"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="293"/>
-      <c r="B5" s="294"/>
-      <c r="C5" s="294"/>
-      <c r="D5" s="294"/>
-      <c r="E5" s="294"/>
-      <c r="F5" s="294"/>
-      <c r="G5" s="294"/>
-      <c r="H5" s="294"/>
-      <c r="I5" s="294"/>
-      <c r="J5" s="294"/>
-      <c r="K5" s="294"/>
-      <c r="L5" s="294"/>
-      <c r="M5" s="294"/>
-      <c r="N5" s="294"/>
-      <c r="O5" s="294"/>
-      <c r="P5" s="294"/>
-      <c r="Q5" s="294"/>
-      <c r="R5" s="294"/>
+      <c r="A5" s="287"/>
+      <c r="B5" s="288"/>
+      <c r="C5" s="288"/>
+      <c r="D5" s="288"/>
+      <c r="E5" s="288"/>
+      <c r="F5" s="288"/>
+      <c r="G5" s="288"/>
+      <c r="H5" s="288"/>
+      <c r="I5" s="288"/>
+      <c r="J5" s="288"/>
+      <c r="K5" s="288"/>
+      <c r="L5" s="288"/>
+      <c r="M5" s="288"/>
+      <c r="N5" s="288"/>
+      <c r="O5" s="288"/>
+      <c r="P5" s="288"/>
+      <c r="Q5" s="288"/>
+      <c r="R5" s="288"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="293"/>
-      <c r="B6" s="294"/>
-      <c r="C6" s="294"/>
-      <c r="D6" s="294"/>
-      <c r="E6" s="294"/>
-      <c r="F6" s="294"/>
-      <c r="G6" s="294"/>
-      <c r="H6" s="294"/>
-      <c r="I6" s="294"/>
-      <c r="J6" s="294"/>
-      <c r="K6" s="294"/>
-      <c r="L6" s="294"/>
-      <c r="M6" s="294"/>
-      <c r="N6" s="294"/>
-      <c r="O6" s="294"/>
-      <c r="P6" s="294"/>
-      <c r="Q6" s="294"/>
-      <c r="R6" s="294"/>
+      <c r="A6" s="287"/>
+      <c r="B6" s="288"/>
+      <c r="C6" s="288"/>
+      <c r="D6" s="288"/>
+      <c r="E6" s="288"/>
+      <c r="F6" s="288"/>
+      <c r="G6" s="288"/>
+      <c r="H6" s="288"/>
+      <c r="I6" s="288"/>
+      <c r="J6" s="288"/>
+      <c r="K6" s="288"/>
+      <c r="L6" s="288"/>
+      <c r="M6" s="288"/>
+      <c r="N6" s="288"/>
+      <c r="O6" s="288"/>
+      <c r="P6" s="288"/>
+      <c r="Q6" s="288"/>
+      <c r="R6" s="288"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -7916,58 +7922,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="296" t="s">
+      <c r="J79" s="293" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="297"/>
-      <c r="L79" s="297"/>
-      <c r="M79" s="297"/>
-      <c r="N79" s="298"/>
-      <c r="P79" s="304" t="s">
+      <c r="K79" s="294"/>
+      <c r="L79" s="294"/>
+      <c r="M79" s="294"/>
+      <c r="N79" s="295"/>
+      <c r="P79" s="301" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="297"/>
-      <c r="R79" s="297"/>
-      <c r="S79" s="298"/>
+      <c r="Q79" s="294"/>
+      <c r="R79" s="294"/>
+      <c r="S79" s="295"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="299" t="s">
+      <c r="J80" s="296" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="294"/>
-      <c r="L80" s="294"/>
-      <c r="M80" s="294"/>
-      <c r="N80" s="300"/>
-      <c r="P80" s="299" t="s">
+      <c r="K80" s="288"/>
+      <c r="L80" s="288"/>
+      <c r="M80" s="288"/>
+      <c r="N80" s="297"/>
+      <c r="P80" s="296" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="294"/>
-      <c r="R80" s="294"/>
-      <c r="S80" s="300"/>
+      <c r="Q80" s="288"/>
+      <c r="R80" s="288"/>
+      <c r="S80" s="297"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="301"/>
-      <c r="K81" s="302"/>
-      <c r="L81" s="302"/>
-      <c r="M81" s="302"/>
-      <c r="N81" s="303"/>
-      <c r="P81" s="301"/>
-      <c r="Q81" s="302"/>
-      <c r="R81" s="302"/>
-      <c r="S81" s="303"/>
+      <c r="J81" s="298"/>
+      <c r="K81" s="299"/>
+      <c r="L81" s="299"/>
+      <c r="M81" s="299"/>
+      <c r="N81" s="300"/>
+      <c r="P81" s="298"/>
+      <c r="Q81" s="299"/>
+      <c r="R81" s="299"/>
+      <c r="S81" s="300"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="295" t="s">
+      <c r="J82" s="291" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="286"/>
-      <c r="L82" s="287"/>
-      <c r="M82" s="295" t="s">
+      <c r="K82" s="292"/>
+      <c r="L82" s="290"/>
+      <c r="M82" s="291" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="287"/>
-      <c r="P82" s="295"/>
-      <c r="Q82" s="287"/>
+      <c r="N82" s="290"/>
+      <c r="P82" s="291"/>
+      <c r="Q82" s="290"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -7976,38 +7982,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="285" t="s">
+      <c r="J83" s="302" t="s">
         <v>70</v>
       </c>
-      <c r="K83" s="286"/>
-      <c r="L83" s="287"/>
-      <c r="M83" s="288">
+      <c r="K83" s="292"/>
+      <c r="L83" s="290"/>
+      <c r="M83" s="303">
         <v>7350000</v>
       </c>
-      <c r="N83" s="287"/>
+      <c r="N83" s="290"/>
       <c r="P83" s="289" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="287"/>
+      <c r="Q83" s="290"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="285" t="s">
+      <c r="J84" s="302" t="s">
         <v>72</v>
       </c>
-      <c r="K84" s="286"/>
-      <c r="L84" s="287"/>
-      <c r="M84" s="290">
+      <c r="K84" s="292"/>
+      <c r="L84" s="290"/>
+      <c r="M84" s="304">
         <v>1100000</v>
       </c>
-      <c r="N84" s="287"/>
+      <c r="N84" s="290"/>
       <c r="P84" s="289" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="287"/>
+      <c r="Q84" s="290"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -8016,39 +8022,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="285" t="s">
+      <c r="J85" s="302" t="s">
         <v>75</v>
       </c>
-      <c r="K85" s="286"/>
-      <c r="L85" s="287"/>
-      <c r="M85" s="288">
+      <c r="K85" s="292"/>
+      <c r="L85" s="290"/>
+      <c r="M85" s="303">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="287"/>
+      <c r="N85" s="290"/>
       <c r="P85" s="289" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="287"/>
+      <c r="Q85" s="290"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="285" t="s">
+      <c r="J86" s="302" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="286"/>
-      <c r="L86" s="287"/>
-      <c r="M86" s="288">
+      <c r="K86" s="292"/>
+      <c r="L86" s="290"/>
+      <c r="M86" s="303">
         <v>8411850</v>
       </c>
-      <c r="N86" s="287"/>
+      <c r="N86" s="290"/>
       <c r="P86" s="289" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="287"/>
+      <c r="Q86" s="290"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -8056,20 +8062,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="285" t="s">
+      <c r="J87" s="302" t="s">
         <v>79</v>
       </c>
-      <c r="K87" s="286"/>
-      <c r="L87" s="287"/>
-      <c r="M87" s="288">
+      <c r="K87" s="292"/>
+      <c r="L87" s="290"/>
+      <c r="M87" s="303">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="287"/>
+      <c r="N87" s="290"/>
       <c r="P87" s="289" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="287"/>
+      <c r="Q87" s="290"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -8257,6 +8263,17 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="P86:Q86"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="M84:N84"/>
     <mergeCell ref="A1:R6"/>
     <mergeCell ref="P84:Q84"/>
     <mergeCell ref="J82:L82"/>
@@ -8269,17 +8286,6 @@
     <mergeCell ref="P83:Q83"/>
     <mergeCell ref="P82:Q82"/>
     <mergeCell ref="P80:S81"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="P86:Q86"/>
   </mergeCells>
   <conditionalFormatting sqref="T10:T69">
     <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
@@ -8326,28 +8332,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="436" t="s">
+      <c r="B2" s="437" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="437"/>
-      <c r="D2" s="437"/>
-      <c r="E2" s="437"/>
-      <c r="F2" s="437"/>
-      <c r="G2" s="437"/>
-      <c r="H2" s="437"/>
-      <c r="I2" s="437"/>
-      <c r="J2" s="437"/>
+      <c r="C2" s="438"/>
+      <c r="D2" s="438"/>
+      <c r="E2" s="438"/>
+      <c r="F2" s="438"/>
+      <c r="G2" s="438"/>
+      <c r="H2" s="438"/>
+      <c r="I2" s="438"/>
+      <c r="J2" s="438"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="437"/>
-      <c r="C3" s="437"/>
-      <c r="D3" s="437"/>
-      <c r="E3" s="437"/>
-      <c r="F3" s="437"/>
-      <c r="G3" s="437"/>
-      <c r="H3" s="437"/>
-      <c r="I3" s="437"/>
-      <c r="J3" s="437"/>
+      <c r="B3" s="438"/>
+      <c r="C3" s="438"/>
+      <c r="D3" s="438"/>
+      <c r="E3" s="438"/>
+      <c r="F3" s="438"/>
+      <c r="G3" s="438"/>
+      <c r="H3" s="438"/>
+      <c r="I3" s="438"/>
+      <c r="J3" s="438"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -8368,10 +8374,10 @@
       <c r="G6" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="H6" s="352" t="s">
+      <c r="H6" s="363" t="s">
         <v>280</v>
       </c>
-      <c r="I6" s="318"/>
+      <c r="I6" s="315"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -8393,11 +8399,11 @@
       <c r="G7" s="193">
         <v>205000</v>
       </c>
-      <c r="H7" s="438">
+      <c r="H7" s="439">
         <f>F7-G7</f>
         <v>380000</v>
       </c>
-      <c r="I7" s="318"/>
+      <c r="I7" s="315"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="194"/>
@@ -8406,8 +8412,8 @@
       <c r="E8" s="195"/>
       <c r="F8" s="195"/>
       <c r="G8" s="195"/>
-      <c r="H8" s="435"/>
-      <c r="I8" s="435"/>
+      <c r="H8" s="436"/>
+      <c r="I8" s="436"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="194"/>
@@ -8418,7 +8424,7 @@
       <c r="G9" s="196" t="s">
         <v>281</v>
       </c>
-      <c r="H9" s="439">
+      <c r="H9" s="440">
         <f>H7</f>
         <v>380000</v>
       </c>
@@ -8431,8 +8437,8 @@
       <c r="E10" s="195"/>
       <c r="F10" s="195"/>
       <c r="G10" s="195"/>
-      <c r="H10" s="435"/>
-      <c r="I10" s="435"/>
+      <c r="H10" s="436"/>
+      <c r="I10" s="436"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="194"/>
@@ -8441,8 +8447,8 @@
       <c r="E11" s="195"/>
       <c r="F11" s="195"/>
       <c r="G11" s="195"/>
-      <c r="H11" s="435"/>
-      <c r="I11" s="435"/>
+      <c r="H11" s="436"/>
+      <c r="I11" s="436"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="194"/>
@@ -8451,8 +8457,8 @@
       <c r="E12" s="195"/>
       <c r="F12" s="195"/>
       <c r="G12" s="195"/>
-      <c r="H12" s="435"/>
-      <c r="I12" s="435"/>
+      <c r="H12" s="436"/>
+      <c r="I12" s="436"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="194"/>
@@ -8461,8 +8467,8 @@
       <c r="E13" s="195"/>
       <c r="F13" s="195"/>
       <c r="G13" s="195"/>
-      <c r="H13" s="435"/>
-      <c r="I13" s="435"/>
+      <c r="H13" s="436"/>
+      <c r="I13" s="436"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="194"/>
@@ -8471,8 +8477,8 @@
       <c r="E14" s="195"/>
       <c r="F14" s="195"/>
       <c r="G14" s="195"/>
-      <c r="H14" s="435"/>
-      <c r="I14" s="435"/>
+      <c r="H14" s="436"/>
+      <c r="I14" s="436"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="194"/>
@@ -8481,8 +8487,8 @@
       <c r="E15" s="195"/>
       <c r="F15" s="195"/>
       <c r="G15" s="195"/>
-      <c r="H15" s="435"/>
-      <c r="I15" s="435"/>
+      <c r="H15" s="436"/>
+      <c r="I15" s="436"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="194"/>
@@ -8491,8 +8497,8 @@
       <c r="E16" s="195"/>
       <c r="F16" s="195"/>
       <c r="G16" s="195"/>
-      <c r="H16" s="435"/>
-      <c r="I16" s="435"/>
+      <c r="H16" s="436"/>
+      <c r="I16" s="436"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="194"/>
@@ -8501,16 +8507,11 @@
       <c r="E17" s="195"/>
       <c r="F17" s="195"/>
       <c r="G17" s="195"/>
-      <c r="H17" s="435"/>
-      <c r="I17" s="435"/>
+      <c r="H17" s="436"/>
+      <c r="I17" s="436"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="H6:I6"/>
@@ -8519,6 +8520,11 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8572,46 +8578,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="313" t="s">
+      <c r="C2" s="325" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="292"/>
-      <c r="E2" s="292"/>
-      <c r="F2" s="292"/>
-      <c r="G2" s="292"/>
-      <c r="H2" s="292"/>
-      <c r="I2" s="292"/>
-      <c r="J2" s="292"/>
-      <c r="K2" s="292"/>
-      <c r="L2" s="292"/>
-      <c r="M2" s="292"/>
-      <c r="N2" s="292"/>
-      <c r="O2" s="292"/>
-      <c r="P2" s="293"/>
-      <c r="Q2" s="293"/>
-      <c r="R2" s="293"/>
-      <c r="S2" s="292"/>
-      <c r="T2" s="292"/>
+      <c r="D2" s="286"/>
+      <c r="E2" s="286"/>
+      <c r="F2" s="286"/>
+      <c r="G2" s="286"/>
+      <c r="H2" s="286"/>
+      <c r="I2" s="286"/>
+      <c r="J2" s="286"/>
+      <c r="K2" s="286"/>
+      <c r="L2" s="286"/>
+      <c r="M2" s="286"/>
+      <c r="N2" s="286"/>
+      <c r="O2" s="286"/>
+      <c r="P2" s="287"/>
+      <c r="Q2" s="287"/>
+      <c r="R2" s="287"/>
+      <c r="S2" s="286"/>
+      <c r="T2" s="286"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="293"/>
-      <c r="D3" s="294"/>
-      <c r="E3" s="294"/>
-      <c r="F3" s="294"/>
-      <c r="G3" s="294"/>
-      <c r="H3" s="294"/>
-      <c r="I3" s="294"/>
-      <c r="J3" s="294"/>
-      <c r="K3" s="294"/>
-      <c r="L3" s="294"/>
-      <c r="M3" s="294"/>
-      <c r="N3" s="294"/>
-      <c r="O3" s="294"/>
-      <c r="P3" s="294"/>
-      <c r="Q3" s="294"/>
-      <c r="R3" s="294"/>
-      <c r="S3" s="294"/>
-      <c r="T3" s="294"/>
+      <c r="C3" s="287"/>
+      <c r="D3" s="288"/>
+      <c r="E3" s="288"/>
+      <c r="F3" s="288"/>
+      <c r="G3" s="288"/>
+      <c r="H3" s="288"/>
+      <c r="I3" s="288"/>
+      <c r="J3" s="288"/>
+      <c r="K3" s="288"/>
+      <c r="L3" s="288"/>
+      <c r="M3" s="288"/>
+      <c r="N3" s="288"/>
+      <c r="O3" s="288"/>
+      <c r="P3" s="288"/>
+      <c r="Q3" s="288"/>
+      <c r="R3" s="288"/>
+      <c r="S3" s="288"/>
+      <c r="T3" s="288"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8698,25 +8704,25 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="319" t="s">
+      <c r="X5" s="317" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="286"/>
-      <c r="Z5" s="286"/>
-      <c r="AA5" s="286"/>
-      <c r="AB5" s="286"/>
-      <c r="AC5" s="286"/>
-      <c r="AD5" s="286"/>
-      <c r="AE5" s="286"/>
-      <c r="AF5" s="286"/>
-      <c r="AG5" s="286"/>
-      <c r="AH5" s="286"/>
-      <c r="AI5" s="286"/>
-      <c r="AJ5" s="286"/>
-      <c r="AK5" s="286"/>
-      <c r="AL5" s="286"/>
-      <c r="AM5" s="286"/>
-      <c r="AN5" s="287"/>
+      <c r="Y5" s="292"/>
+      <c r="Z5" s="292"/>
+      <c r="AA5" s="292"/>
+      <c r="AB5" s="292"/>
+      <c r="AC5" s="292"/>
+      <c r="AD5" s="292"/>
+      <c r="AE5" s="292"/>
+      <c r="AF5" s="292"/>
+      <c r="AG5" s="292"/>
+      <c r="AH5" s="292"/>
+      <c r="AI5" s="292"/>
+      <c r="AJ5" s="292"/>
+      <c r="AK5" s="292"/>
+      <c r="AL5" s="292"/>
+      <c r="AM5" s="292"/>
+      <c r="AN5" s="290"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -8791,29 +8797,29 @@
       <c r="V6" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X6" s="314" t="s">
+      <c r="X6" s="326" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="314" t="s">
+      <c r="Y6" s="326" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="318" t="s">
+      <c r="Z6" s="315" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="315"/>
-      <c r="AB6" s="315"/>
-      <c r="AC6" s="315"/>
-      <c r="AD6" s="315"/>
-      <c r="AE6" s="315"/>
-      <c r="AF6" s="315"/>
-      <c r="AG6" s="315"/>
-      <c r="AH6" s="315"/>
-      <c r="AI6" s="315"/>
-      <c r="AJ6" s="315"/>
-      <c r="AK6" s="315"/>
-      <c r="AL6" s="315"/>
-      <c r="AM6" s="315"/>
-      <c r="AN6" s="315"/>
+      <c r="AA6" s="316"/>
+      <c r="AB6" s="316"/>
+      <c r="AC6" s="316"/>
+      <c r="AD6" s="316"/>
+      <c r="AE6" s="316"/>
+      <c r="AF6" s="316"/>
+      <c r="AG6" s="316"/>
+      <c r="AH6" s="316"/>
+      <c r="AI6" s="316"/>
+      <c r="AJ6" s="316"/>
+      <c r="AK6" s="316"/>
+      <c r="AL6" s="316"/>
+      <c r="AM6" s="316"/>
+      <c r="AN6" s="316"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -8888,27 +8894,27 @@
       <c r="V7" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X7" s="315"/>
-      <c r="Y7" s="315"/>
-      <c r="Z7" s="318" t="s">
+      <c r="X7" s="316"/>
+      <c r="Y7" s="316"/>
+      <c r="Z7" s="315" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="315"/>
-      <c r="AB7" s="315"/>
-      <c r="AC7" s="315"/>
-      <c r="AD7" s="318" t="s">
+      <c r="AA7" s="316"/>
+      <c r="AB7" s="316"/>
+      <c r="AC7" s="316"/>
+      <c r="AD7" s="315" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="315"/>
-      <c r="AF7" s="315"/>
-      <c r="AG7" s="315"/>
-      <c r="AH7" s="315"/>
-      <c r="AI7" s="315"/>
-      <c r="AJ7" s="315"/>
-      <c r="AK7" s="315"/>
-      <c r="AL7" s="315"/>
-      <c r="AM7" s="315"/>
-      <c r="AN7" s="315"/>
+      <c r="AE7" s="316"/>
+      <c r="AF7" s="316"/>
+      <c r="AG7" s="316"/>
+      <c r="AH7" s="316"/>
+      <c r="AI7" s="316"/>
+      <c r="AJ7" s="316"/>
+      <c r="AK7" s="316"/>
+      <c r="AL7" s="316"/>
+      <c r="AM7" s="316"/>
+      <c r="AN7" s="316"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -8958,8 +8964,8 @@
         <v>NO</v>
       </c>
       <c r="V8" s="13"/>
-      <c r="X8" s="315"/>
-      <c r="Y8" s="315"/>
+      <c r="X8" s="316"/>
+      <c r="Y8" s="316"/>
       <c r="Z8" s="151" t="s">
         <v>19</v>
       </c>
@@ -13570,10 +13576,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="316" t="s">
+      <c r="AA49" s="313" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="317"/>
+      <c r="AB49" s="314"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -13651,12 +13657,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="323" t="s">
+      <c r="AI50" s="309" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="324"/>
-      <c r="AK50" s="324"/>
-      <c r="AL50" s="325"/>
+      <c r="AJ50" s="310"/>
+      <c r="AK50" s="310"/>
+      <c r="AL50" s="311"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -13727,12 +13733,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="320" t="s">
+      <c r="AI51" s="306" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="321"/>
-      <c r="AK51" s="321"/>
-      <c r="AL51" s="322"/>
+      <c r="AJ51" s="307"/>
+      <c r="AK51" s="307"/>
+      <c r="AL51" s="308"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -13998,14 +14004,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="326"/>
-      <c r="AD55" s="326"/>
-      <c r="AI55" s="323" t="s">
+      <c r="AC55" s="312"/>
+      <c r="AD55" s="312"/>
+      <c r="AI55" s="309" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="324"/>
-      <c r="AK55" s="324"/>
-      <c r="AL55" s="325"/>
+      <c r="AJ55" s="310"/>
+      <c r="AK55" s="310"/>
+      <c r="AL55" s="311"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -14338,32 +14344,32 @@
     <row r="67" spans="3:19" s="256" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="306" t="s">
+      <c r="C69" s="318" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="307"/>
-      <c r="E69" s="307"/>
-      <c r="F69" s="307"/>
-      <c r="G69" s="308"/>
-      <c r="I69" s="312" t="s">
+      <c r="D69" s="319"/>
+      <c r="E69" s="319"/>
+      <c r="F69" s="319"/>
+      <c r="G69" s="320"/>
+      <c r="I69" s="324" t="s">
         <v>178</v>
       </c>
-      <c r="J69" s="312"/>
-      <c r="K69" s="312"/>
-      <c r="L69" s="312"/>
-      <c r="M69" s="312"/>
+      <c r="J69" s="324"/>
+      <c r="K69" s="324"/>
+      <c r="L69" s="324"/>
+      <c r="M69" s="324"/>
     </row>
     <row r="70" spans="3:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="309"/>
-      <c r="D70" s="310"/>
-      <c r="E70" s="310"/>
-      <c r="F70" s="310"/>
-      <c r="G70" s="311"/>
-      <c r="I70" s="312"/>
-      <c r="J70" s="312"/>
-      <c r="K70" s="312"/>
-      <c r="L70" s="312"/>
-      <c r="M70" s="312"/>
+      <c r="C70" s="321"/>
+      <c r="D70" s="322"/>
+      <c r="E70" s="322"/>
+      <c r="F70" s="322"/>
+      <c r="G70" s="323"/>
+      <c r="I70" s="324"/>
+      <c r="J70" s="324"/>
+      <c r="K70" s="324"/>
+      <c r="L70" s="324"/>
+      <c r="M70" s="324"/>
     </row>
     <row r="71" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14854,22 +14860,22 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AI56:AL56"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AI50:AL50"/>
-    <mergeCell ref="AI55:AL55"/>
-    <mergeCell ref="AC55:AD55"/>
-    <mergeCell ref="AA49:AB49"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="AD7:AN7"/>
-    <mergeCell ref="X5:AN5"/>
-    <mergeCell ref="Z6:AN6"/>
     <mergeCell ref="P76:Q76"/>
     <mergeCell ref="C69:G70"/>
     <mergeCell ref="I69:M70"/>
     <mergeCell ref="C2:T3"/>
     <mergeCell ref="Y6:Y8"/>
     <mergeCell ref="X6:X8"/>
+    <mergeCell ref="AA49:AB49"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="AD7:AN7"/>
+    <mergeCell ref="X5:AN5"/>
+    <mergeCell ref="Z6:AN6"/>
+    <mergeCell ref="AI56:AL56"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AI50:AL50"/>
+    <mergeCell ref="AI55:AL55"/>
+    <mergeCell ref="AC55:AD55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:V61">
     <cfRule type="expression" dxfId="20" priority="8">
@@ -14989,56 +14995,56 @@
       <c r="L3" s="327"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="312" t="s">
+      <c r="A5" s="324" t="s">
         <v>303</v>
       </c>
-      <c r="B5" s="312"/>
-      <c r="C5" s="312"/>
-      <c r="D5" s="312"/>
-      <c r="E5" s="312"/>
-      <c r="F5" s="312"/>
-      <c r="G5" s="312"/>
-      <c r="H5" s="312"/>
-      <c r="I5" s="312"/>
-      <c r="J5" s="312"/>
-      <c r="K5" s="312"/>
-      <c r="M5" s="312" t="s">
+      <c r="B5" s="324"/>
+      <c r="C5" s="324"/>
+      <c r="D5" s="324"/>
+      <c r="E5" s="324"/>
+      <c r="F5" s="324"/>
+      <c r="G5" s="324"/>
+      <c r="H5" s="324"/>
+      <c r="I5" s="324"/>
+      <c r="J5" s="324"/>
+      <c r="K5" s="324"/>
+      <c r="M5" s="324" t="s">
         <v>324</v>
       </c>
-      <c r="N5" s="312"/>
-      <c r="O5" s="312"/>
-      <c r="P5" s="312"/>
-      <c r="Q5" s="312"/>
-      <c r="R5" s="312"/>
-      <c r="S5" s="312"/>
-      <c r="T5" s="312"/>
-      <c r="U5" s="312"/>
-      <c r="V5" s="312"/>
-      <c r="W5" s="312"/>
+      <c r="N5" s="324"/>
+      <c r="O5" s="324"/>
+      <c r="P5" s="324"/>
+      <c r="Q5" s="324"/>
+      <c r="R5" s="324"/>
+      <c r="S5" s="324"/>
+      <c r="T5" s="324"/>
+      <c r="U5" s="324"/>
+      <c r="V5" s="324"/>
+      <c r="W5" s="324"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="312"/>
-      <c r="B6" s="312"/>
-      <c r="C6" s="312"/>
-      <c r="D6" s="312"/>
-      <c r="E6" s="312"/>
-      <c r="F6" s="312"/>
-      <c r="G6" s="312"/>
-      <c r="H6" s="312"/>
-      <c r="I6" s="312"/>
-      <c r="J6" s="312"/>
-      <c r="K6" s="312"/>
-      <c r="M6" s="312"/>
-      <c r="N6" s="312"/>
-      <c r="O6" s="312"/>
-      <c r="P6" s="312"/>
-      <c r="Q6" s="312"/>
-      <c r="R6" s="312"/>
-      <c r="S6" s="312"/>
-      <c r="T6" s="312"/>
-      <c r="U6" s="312"/>
-      <c r="V6" s="312"/>
-      <c r="W6" s="312"/>
+      <c r="A6" s="324"/>
+      <c r="B6" s="324"/>
+      <c r="C6" s="324"/>
+      <c r="D6" s="324"/>
+      <c r="E6" s="324"/>
+      <c r="F6" s="324"/>
+      <c r="G6" s="324"/>
+      <c r="H6" s="324"/>
+      <c r="I6" s="324"/>
+      <c r="J6" s="324"/>
+      <c r="K6" s="324"/>
+      <c r="M6" s="324"/>
+      <c r="N6" s="324"/>
+      <c r="O6" s="324"/>
+      <c r="P6" s="324"/>
+      <c r="Q6" s="324"/>
+      <c r="R6" s="324"/>
+      <c r="S6" s="324"/>
+      <c r="T6" s="324"/>
+      <c r="U6" s="324"/>
+      <c r="V6" s="324"/>
+      <c r="W6" s="324"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M7" s="249"/>
@@ -16012,8 +16018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16051,19 +16057,19 @@
       <c r="G3" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I3" s="312" t="s">
+      <c r="I3" s="324" t="s">
         <v>366</v>
       </c>
-      <c r="J3" s="312"/>
-      <c r="K3" s="312"/>
-      <c r="L3" s="312"/>
-      <c r="M3" s="312"/>
-      <c r="N3" s="312"/>
-      <c r="O3" s="312"/>
-      <c r="P3" s="312"/>
-      <c r="Q3" s="312"/>
-      <c r="R3" s="312"/>
-      <c r="S3" s="312"/>
+      <c r="J3" s="324"/>
+      <c r="K3" s="324"/>
+      <c r="L3" s="324"/>
+      <c r="M3" s="324"/>
+      <c r="N3" s="324"/>
+      <c r="O3" s="324"/>
+      <c r="P3" s="324"/>
+      <c r="Q3" s="324"/>
+      <c r="R3" s="324"/>
+      <c r="S3" s="324"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="57">
@@ -16085,17 +16091,17 @@
         <f>IF(ISNUMBER(SEARCH("SENIOR DISKON",D4)),100000,IF(ISNUMBER(SEARCH("SENIOR",D4)),150000,IF(ISNUMBER(SEARCH("MABA",D4)),125000,0)))</f>
         <v>125000</v>
       </c>
-      <c r="I4" s="312"/>
-      <c r="J4" s="312"/>
-      <c r="K4" s="312"/>
-      <c r="L4" s="312"/>
-      <c r="M4" s="312"/>
-      <c r="N4" s="312"/>
-      <c r="O4" s="312"/>
-      <c r="P4" s="312"/>
-      <c r="Q4" s="312"/>
-      <c r="R4" s="312"/>
-      <c r="S4" s="312"/>
+      <c r="I4" s="324"/>
+      <c r="J4" s="324"/>
+      <c r="K4" s="324"/>
+      <c r="L4" s="324"/>
+      <c r="M4" s="324"/>
+      <c r="N4" s="324"/>
+      <c r="O4" s="324"/>
+      <c r="P4" s="324"/>
+      <c r="Q4" s="324"/>
+      <c r="R4" s="324"/>
+      <c r="S4" s="324"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="57">
@@ -16294,7 +16300,7 @@
       </c>
       <c r="M9" s="210">
         <f>G47</f>
-        <v>4850000</v>
+        <v>5250000</v>
       </c>
       <c r="N9" s="210"/>
       <c r="O9" s="277"/>
@@ -16532,14 +16538,14 @@
       <c r="M15" s="210"/>
       <c r="N15" s="211"/>
       <c r="O15" s="277"/>
-      <c r="P15" s="440" t="s">
+      <c r="P15" s="343" t="s">
         <v>391</v>
       </c>
-      <c r="Q15" s="440"/>
-      <c r="R15" s="440"/>
-      <c r="S15" s="440"/>
-      <c r="T15" s="440"/>
-      <c r="U15" s="440"/>
+      <c r="Q15" s="343"/>
+      <c r="R15" s="343"/>
+      <c r="S15" s="343"/>
+      <c r="T15" s="343"/>
+      <c r="U15" s="343"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" s="57">
@@ -16570,12 +16576,12 @@
       <c r="M16" s="211"/>
       <c r="N16" s="210"/>
       <c r="O16" s="277"/>
-      <c r="P16" s="440"/>
-      <c r="Q16" s="440"/>
-      <c r="R16" s="440"/>
-      <c r="S16" s="440"/>
-      <c r="T16" s="440"/>
-      <c r="U16" s="440"/>
+      <c r="P16" s="343"/>
+      <c r="Q16" s="343"/>
+      <c r="R16" s="343"/>
+      <c r="S16" s="343"/>
+      <c r="T16" s="343"/>
+      <c r="U16" s="343"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="57">
@@ -16606,12 +16612,12 @@
       <c r="M17" s="211"/>
       <c r="N17" s="211"/>
       <c r="O17" s="277"/>
-      <c r="P17" s="440"/>
-      <c r="Q17" s="440"/>
-      <c r="R17" s="440"/>
-      <c r="S17" s="440"/>
-      <c r="T17" s="440"/>
-      <c r="U17" s="440"/>
+      <c r="P17" s="343"/>
+      <c r="Q17" s="343"/>
+      <c r="R17" s="343"/>
+      <c r="S17" s="343"/>
+      <c r="T17" s="343"/>
+      <c r="U17" s="343"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="57">
@@ -17121,7 +17127,7 @@
       <c r="L32" s="222"/>
       <c r="M32" s="223">
         <f>SUM(M7:M31)</f>
-        <v>6850000</v>
+        <v>7250000</v>
       </c>
       <c r="N32" s="224">
         <f>SUM(N7:N31)</f>
@@ -17161,7 +17167,7 @@
       <c r="L33" s="334"/>
       <c r="M33" s="328">
         <f>M32-N32</f>
-        <v>6310000</v>
+        <v>6710000</v>
       </c>
       <c r="N33" s="329"/>
       <c r="O33" s="277"/>
@@ -17353,39 +17359,63 @@
       <c r="B42" s="57">
         <v>39</v>
       </c>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="57"/>
+      <c r="C42" s="57" t="s">
+        <v>392</v>
+      </c>
+      <c r="D42" s="57" t="s">
+        <v>352</v>
+      </c>
+      <c r="E42" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="F42" s="57" t="s">
+        <v>377</v>
+      </c>
       <c r="G42" s="56">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>125000</v>
       </c>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B43" s="57">
         <v>40</v>
       </c>
-      <c r="C43" s="57"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
-      <c r="F43" s="57"/>
+      <c r="C43" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="E43" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="F43" s="57" t="s">
+        <v>377</v>
+      </c>
       <c r="G43" s="56">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="44" spans="2:19" s="283" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="57">
         <v>41</v>
       </c>
-      <c r="C44" s="57"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="57"/>
+      <c r="C44" s="57" t="s">
+        <v>393</v>
+      </c>
+      <c r="D44" s="57" t="s">
+        <v>352</v>
+      </c>
+      <c r="E44" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="F44" s="57" t="s">
+        <v>377</v>
+      </c>
       <c r="G44" s="56">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>125000</v>
       </c>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.25">
@@ -17424,7 +17454,7 @@
       <c r="F47" s="342"/>
       <c r="G47" s="282">
         <f>SUM(G4:G46)</f>
-        <v>4850000</v>
+        <v>5250000</v>
       </c>
     </row>
   </sheetData>
@@ -17506,17 +17536,17 @@
       <c r="A2" s="172"/>
       <c r="B2" s="173"/>
       <c r="C2" s="173"/>
-      <c r="D2" s="400" t="s">
+      <c r="D2" s="344" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="400"/>
-      <c r="F2" s="400"/>
-      <c r="G2" s="400"/>
-      <c r="H2" s="400"/>
-      <c r="I2" s="400"/>
-      <c r="J2" s="400"/>
-      <c r="K2" s="400"/>
-      <c r="L2" s="400"/>
+      <c r="E2" s="344"/>
+      <c r="F2" s="344"/>
+      <c r="G2" s="344"/>
+      <c r="H2" s="344"/>
+      <c r="I2" s="344"/>
+      <c r="J2" s="344"/>
+      <c r="K2" s="344"/>
+      <c r="L2" s="344"/>
       <c r="M2" s="174"/>
       <c r="N2" s="24"/>
     </row>
@@ -17534,205 +17564,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="176"/>
-      <c r="U3" s="343" t="s">
+      <c r="U3" s="394" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="344"/>
-      <c r="W3" s="345" t="s">
+      <c r="V3" s="395"/>
+      <c r="W3" s="396" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="344"/>
-      <c r="Y3" s="344"/>
-      <c r="Z3" s="344"/>
-      <c r="AA3" s="344"/>
-      <c r="AB3" s="344"/>
-      <c r="AC3" s="344"/>
-      <c r="AD3" s="346"/>
+      <c r="X3" s="395"/>
+      <c r="Y3" s="395"/>
+      <c r="Z3" s="395"/>
+      <c r="AA3" s="395"/>
+      <c r="AB3" s="395"/>
+      <c r="AC3" s="395"/>
+      <c r="AD3" s="397"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="175"/>
-      <c r="B4" s="404" t="s">
+      <c r="B4" s="359" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="405"/>
-      <c r="D4" s="405"/>
-      <c r="E4" s="405"/>
-      <c r="F4" s="405"/>
+      <c r="C4" s="360"/>
+      <c r="D4" s="360"/>
+      <c r="E4" s="360"/>
+      <c r="F4" s="360"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="352" t="s">
+      <c r="I4" s="363" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="318"/>
-      <c r="K4" s="318"/>
-      <c r="L4" s="318"/>
+      <c r="J4" s="315"/>
+      <c r="K4" s="315"/>
+      <c r="L4" s="315"/>
       <c r="M4" s="176"/>
-      <c r="U4" s="364" t="s">
+      <c r="U4" s="406" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="318"/>
-      <c r="W4" s="352" t="s">
+      <c r="V4" s="315"/>
+      <c r="W4" s="363" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="318"/>
-      <c r="Y4" s="318"/>
-      <c r="Z4" s="318"/>
-      <c r="AA4" s="318"/>
-      <c r="AB4" s="318"/>
-      <c r="AC4" s="318"/>
-      <c r="AD4" s="347"/>
+      <c r="X4" s="315"/>
+      <c r="Y4" s="315"/>
+      <c r="Z4" s="315"/>
+      <c r="AA4" s="315"/>
+      <c r="AB4" s="315"/>
+      <c r="AC4" s="315"/>
+      <c r="AD4" s="383"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="175"/>
-      <c r="B5" s="369" t="s">
+      <c r="B5" s="354" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="318"/>
-      <c r="D5" s="318"/>
-      <c r="E5" s="318"/>
-      <c r="F5" s="318"/>
+      <c r="C5" s="315"/>
+      <c r="D5" s="315"/>
+      <c r="E5" s="315"/>
+      <c r="F5" s="315"/>
       <c r="G5" s="152">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="371" t="s">
+      <c r="I5" s="352" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="392"/>
-      <c r="K5" s="394">
+      <c r="J5" s="353"/>
+      <c r="K5" s="364">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="395"/>
+      <c r="L5" s="365"/>
       <c r="M5" s="176"/>
-      <c r="U5" s="365" t="s">
+      <c r="U5" s="390" t="s">
         <v>231</v>
       </c>
-      <c r="V5" s="366"/>
-      <c r="W5" s="371" t="s">
+      <c r="V5" s="391"/>
+      <c r="W5" s="352" t="s">
         <v>232</v>
       </c>
-      <c r="X5" s="372"/>
-      <c r="Y5" s="372"/>
-      <c r="Z5" s="372"/>
-      <c r="AA5" s="372"/>
-      <c r="AB5" s="372"/>
-      <c r="AC5" s="372"/>
-      <c r="AD5" s="373"/>
+      <c r="X5" s="377"/>
+      <c r="Y5" s="377"/>
+      <c r="Z5" s="377"/>
+      <c r="AA5" s="377"/>
+      <c r="AB5" s="377"/>
+      <c r="AC5" s="377"/>
+      <c r="AD5" s="378"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="175"/>
-      <c r="B6" s="362" t="s">
+      <c r="B6" s="346" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="363"/>
-      <c r="D6" s="363"/>
-      <c r="E6" s="363"/>
-      <c r="F6" s="363"/>
+      <c r="C6" s="347"/>
+      <c r="D6" s="347"/>
+      <c r="E6" s="347"/>
+      <c r="F6" s="347"/>
       <c r="G6" s="152">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="393" t="s">
+      <c r="I6" s="350" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="388"/>
-      <c r="K6" s="396">
+      <c r="J6" s="351"/>
+      <c r="K6" s="366">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="397"/>
+      <c r="L6" s="367"/>
       <c r="M6" s="176"/>
-      <c r="U6" s="367"/>
-      <c r="V6" s="368"/>
-      <c r="W6" s="353" t="s">
+      <c r="U6" s="392"/>
+      <c r="V6" s="393"/>
+      <c r="W6" s="379" t="s">
         <v>233</v>
       </c>
-      <c r="X6" s="354"/>
-      <c r="Y6" s="354"/>
-      <c r="Z6" s="354"/>
-      <c r="AA6" s="354"/>
-      <c r="AB6" s="354"/>
-      <c r="AC6" s="354"/>
-      <c r="AD6" s="355"/>
+      <c r="X6" s="380"/>
+      <c r="Y6" s="380"/>
+      <c r="Z6" s="380"/>
+      <c r="AA6" s="380"/>
+      <c r="AB6" s="380"/>
+      <c r="AC6" s="380"/>
+      <c r="AD6" s="381"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="175"/>
-      <c r="B7" s="374" t="s">
+      <c r="B7" s="357" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="375"/>
-      <c r="D7" s="375"/>
-      <c r="E7" s="375"/>
-      <c r="F7" s="388"/>
+      <c r="C7" s="358"/>
+      <c r="D7" s="358"/>
+      <c r="E7" s="358"/>
+      <c r="F7" s="351"/>
       <c r="G7" s="152">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="393" t="s">
+      <c r="I7" s="350" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="388"/>
-      <c r="K7" s="398">
+      <c r="J7" s="351"/>
+      <c r="K7" s="361">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="399"/>
+      <c r="L7" s="362"/>
       <c r="M7" s="176"/>
-      <c r="U7" s="350"/>
-      <c r="V7" s="351"/>
-      <c r="W7" s="352" t="s">
+      <c r="U7" s="398"/>
+      <c r="V7" s="399"/>
+      <c r="W7" s="363" t="s">
         <v>234</v>
       </c>
-      <c r="X7" s="318"/>
-      <c r="Y7" s="318"/>
-      <c r="Z7" s="318"/>
-      <c r="AA7" s="318"/>
-      <c r="AB7" s="318"/>
-      <c r="AC7" s="318"/>
-      <c r="AD7" s="347"/>
+      <c r="X7" s="315"/>
+      <c r="Y7" s="315"/>
+      <c r="Z7" s="315"/>
+      <c r="AA7" s="315"/>
+      <c r="AB7" s="315"/>
+      <c r="AC7" s="315"/>
+      <c r="AD7" s="383"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="175"/>
-      <c r="B8" s="402" t="s">
+      <c r="B8" s="355" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="403"/>
-      <c r="D8" s="403"/>
-      <c r="E8" s="403"/>
-      <c r="F8" s="403"/>
+      <c r="C8" s="356"/>
+      <c r="D8" s="356"/>
+      <c r="E8" s="356"/>
+      <c r="F8" s="356"/>
       <c r="G8" s="153">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="371" t="s">
+      <c r="I8" s="352" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="392"/>
-      <c r="K8" s="383">
+      <c r="J8" s="353"/>
+      <c r="K8" s="348">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="384"/>
+      <c r="L8" s="349"/>
       <c r="M8" s="176"/>
-      <c r="U8" s="358" t="s">
+      <c r="U8" s="402" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="359"/>
-      <c r="W8" s="353" t="s">
+      <c r="V8" s="403"/>
+      <c r="W8" s="379" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="354"/>
-      <c r="Y8" s="354"/>
-      <c r="Z8" s="354"/>
-      <c r="AA8" s="354"/>
-      <c r="AB8" s="354"/>
-      <c r="AC8" s="354"/>
-      <c r="AD8" s="355"/>
+      <c r="X8" s="380"/>
+      <c r="Y8" s="380"/>
+      <c r="Z8" s="380"/>
+      <c r="AA8" s="380"/>
+      <c r="AB8" s="380"/>
+      <c r="AC8" s="380"/>
+      <c r="AD8" s="381"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="175"/>
@@ -17748,28 +17778,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="176"/>
-      <c r="U9" s="360"/>
-      <c r="V9" s="361"/>
-      <c r="W9" s="353" t="s">
+      <c r="U9" s="404"/>
+      <c r="V9" s="405"/>
+      <c r="W9" s="379" t="s">
         <v>237</v>
       </c>
-      <c r="X9" s="354"/>
-      <c r="Y9" s="354"/>
-      <c r="Z9" s="354"/>
-      <c r="AA9" s="354"/>
-      <c r="AB9" s="354"/>
-      <c r="AC9" s="354"/>
-      <c r="AD9" s="355"/>
+      <c r="X9" s="380"/>
+      <c r="Y9" s="380"/>
+      <c r="Z9" s="380"/>
+      <c r="AA9" s="380"/>
+      <c r="AB9" s="380"/>
+      <c r="AC9" s="380"/>
+      <c r="AD9" s="381"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="175"/>
-      <c r="B10" s="318" t="s">
+      <c r="B10" s="315" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="318"/>
-      <c r="D10" s="318"/>
-      <c r="E10" s="318"/>
-      <c r="F10" s="318"/>
+      <c r="C10" s="315"/>
+      <c r="D10" s="315"/>
+      <c r="E10" s="315"/>
+      <c r="F10" s="315"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -17780,30 +17810,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="176"/>
-      <c r="U10" s="362" t="s">
+      <c r="U10" s="346" t="s">
         <v>243</v>
       </c>
-      <c r="V10" s="363"/>
-      <c r="W10" s="318" t="s">
+      <c r="V10" s="347"/>
+      <c r="W10" s="315" t="s">
         <v>257</v>
       </c>
-      <c r="X10" s="318"/>
-      <c r="Y10" s="318"/>
-      <c r="Z10" s="318"/>
-      <c r="AA10" s="318"/>
-      <c r="AB10" s="318"/>
-      <c r="AC10" s="318"/>
-      <c r="AD10" s="347"/>
+      <c r="X10" s="315"/>
+      <c r="Y10" s="315"/>
+      <c r="Z10" s="315"/>
+      <c r="AA10" s="315"/>
+      <c r="AB10" s="315"/>
+      <c r="AC10" s="315"/>
+      <c r="AD10" s="383"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="175"/>
-      <c r="B11" s="318" t="s">
+      <c r="B11" s="315" t="s">
         <v>254</v>
       </c>
-      <c r="C11" s="318"/>
-      <c r="D11" s="318"/>
-      <c r="E11" s="318"/>
-      <c r="F11" s="318"/>
+      <c r="C11" s="315"/>
+      <c r="D11" s="315"/>
+      <c r="E11" s="315"/>
+      <c r="F11" s="315"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -17813,30 +17843,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="176"/>
-      <c r="U11" s="362" t="s">
+      <c r="U11" s="346" t="s">
         <v>256</v>
       </c>
-      <c r="V11" s="363"/>
-      <c r="W11" s="356" t="s">
+      <c r="V11" s="347"/>
+      <c r="W11" s="400" t="s">
         <v>258</v>
       </c>
-      <c r="X11" s="356"/>
-      <c r="Y11" s="356"/>
-      <c r="Z11" s="356"/>
-      <c r="AA11" s="356"/>
-      <c r="AB11" s="356"/>
-      <c r="AC11" s="356"/>
-      <c r="AD11" s="357"/>
+      <c r="X11" s="400"/>
+      <c r="Y11" s="400"/>
+      <c r="Z11" s="400"/>
+      <c r="AA11" s="400"/>
+      <c r="AB11" s="400"/>
+      <c r="AC11" s="400"/>
+      <c r="AD11" s="401"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="175"/>
-      <c r="B12" s="401" t="s">
+      <c r="B12" s="345" t="s">
         <v>255</v>
       </c>
-      <c r="C12" s="401"/>
-      <c r="D12" s="401"/>
-      <c r="E12" s="401"/>
-      <c r="F12" s="401"/>
+      <c r="C12" s="345"/>
+      <c r="D12" s="345"/>
+      <c r="E12" s="345"/>
+      <c r="F12" s="345"/>
       <c r="G12" s="180">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -17847,16 +17877,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="176"/>
-      <c r="U12" s="362"/>
-      <c r="V12" s="363"/>
-      <c r="W12" s="318"/>
-      <c r="X12" s="318"/>
-      <c r="Y12" s="318"/>
-      <c r="Z12" s="318"/>
-      <c r="AA12" s="318"/>
-      <c r="AB12" s="318"/>
-      <c r="AC12" s="318"/>
-      <c r="AD12" s="347"/>
+      <c r="U12" s="346"/>
+      <c r="V12" s="347"/>
+      <c r="W12" s="315"/>
+      <c r="X12" s="315"/>
+      <c r="Y12" s="315"/>
+      <c r="Z12" s="315"/>
+      <c r="AA12" s="315"/>
+      <c r="AB12" s="315"/>
+      <c r="AC12" s="315"/>
+      <c r="AD12" s="383"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="177"/>
@@ -17872,64 +17902,64 @@
       <c r="K13" s="178"/>
       <c r="L13" s="178"/>
       <c r="M13" s="179"/>
-      <c r="U13" s="362"/>
-      <c r="V13" s="363"/>
-      <c r="W13" s="318"/>
-      <c r="X13" s="318"/>
-      <c r="Y13" s="318"/>
-      <c r="Z13" s="318"/>
-      <c r="AA13" s="318"/>
-      <c r="AB13" s="318"/>
-      <c r="AC13" s="318"/>
-      <c r="AD13" s="347"/>
+      <c r="U13" s="346"/>
+      <c r="V13" s="347"/>
+      <c r="W13" s="315"/>
+      <c r="X13" s="315"/>
+      <c r="Y13" s="315"/>
+      <c r="Z13" s="315"/>
+      <c r="AA13" s="315"/>
+      <c r="AB13" s="315"/>
+      <c r="AC13" s="315"/>
+      <c r="AD13" s="383"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="377"/>
-      <c r="V14" s="378"/>
-      <c r="W14" s="348"/>
-      <c r="X14" s="348"/>
-      <c r="Y14" s="348"/>
-      <c r="Z14" s="348"/>
-      <c r="AA14" s="348"/>
-      <c r="AB14" s="348"/>
-      <c r="AC14" s="348"/>
-      <c r="AD14" s="349"/>
+      <c r="U14" s="384"/>
+      <c r="V14" s="385"/>
+      <c r="W14" s="375"/>
+      <c r="X14" s="375"/>
+      <c r="Y14" s="375"/>
+      <c r="Z14" s="375"/>
+      <c r="AA14" s="375"/>
+      <c r="AB14" s="375"/>
+      <c r="AC14" s="375"/>
+      <c r="AD14" s="376"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="172"/>
       <c r="B18" s="173"/>
       <c r="C18" s="173"/>
-      <c r="D18" s="400" t="s">
+      <c r="D18" s="344" t="s">
         <v>249</v>
       </c>
-      <c r="E18" s="400"/>
-      <c r="F18" s="400"/>
-      <c r="G18" s="400"/>
-      <c r="H18" s="400"/>
-      <c r="I18" s="400"/>
-      <c r="J18" s="400"/>
-      <c r="K18" s="400"/>
-      <c r="L18" s="400"/>
+      <c r="E18" s="344"/>
+      <c r="F18" s="344"/>
+      <c r="G18" s="344"/>
+      <c r="H18" s="344"/>
+      <c r="I18" s="344"/>
+      <c r="J18" s="344"/>
+      <c r="K18" s="344"/>
+      <c r="L18" s="344"/>
       <c r="M18" s="174"/>
-      <c r="O18" s="379" t="s">
+      <c r="O18" s="386" t="s">
         <v>250</v>
       </c>
-      <c r="P18" s="380"/>
-      <c r="Q18" s="380"/>
-      <c r="R18" s="380"/>
-      <c r="S18" s="381"/>
+      <c r="P18" s="387"/>
+      <c r="Q18" s="387"/>
+      <c r="R18" s="387"/>
+      <c r="S18" s="388"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="175"/>
       <c r="M19" s="176"/>
-      <c r="O19" s="369" t="s">
+      <c r="O19" s="354" t="s">
         <v>251</v>
       </c>
-      <c r="P19" s="318"/>
-      <c r="Q19" s="318"/>
-      <c r="R19" s="318"/>
-      <c r="S19" s="347"/>
+      <c r="P19" s="315"/>
+      <c r="Q19" s="315"/>
+      <c r="R19" s="315"/>
+      <c r="S19" s="383"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="175"/>
@@ -17940,119 +17970,119 @@
       <c r="F20" s="200"/>
       <c r="G20" s="68"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="352" t="s">
+      <c r="I20" s="363" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="318"/>
-      <c r="K20" s="318"/>
-      <c r="L20" s="318"/>
+      <c r="J20" s="315"/>
+      <c r="K20" s="315"/>
+      <c r="L20" s="315"/>
       <c r="M20" s="176"/>
-      <c r="O20" s="369" t="s">
+      <c r="O20" s="354" t="s">
         <v>252</v>
       </c>
-      <c r="P20" s="318"/>
-      <c r="Q20" s="318"/>
-      <c r="R20" s="318"/>
-      <c r="S20" s="347"/>
+      <c r="P20" s="315"/>
+      <c r="Q20" s="315"/>
+      <c r="R20" s="315"/>
+      <c r="S20" s="383"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="175"/>
-      <c r="B21" s="385" t="s">
+      <c r="B21" s="368" t="s">
         <v>296</v>
       </c>
-      <c r="C21" s="386"/>
-      <c r="D21" s="386"/>
-      <c r="E21" s="386"/>
-      <c r="F21" s="387"/>
+      <c r="C21" s="369"/>
+      <c r="D21" s="369"/>
+      <c r="E21" s="369"/>
+      <c r="F21" s="370"/>
       <c r="G21" s="70">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="371" t="s">
+      <c r="I21" s="352" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="392"/>
-      <c r="K21" s="394">
+      <c r="J21" s="353"/>
+      <c r="K21" s="364">
         <f>G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="L21" s="395"/>
+      <c r="L21" s="365"/>
       <c r="M21" s="176"/>
       <c r="N21" s="170"/>
-      <c r="O21" s="382" t="s">
+      <c r="O21" s="389" t="s">
         <v>259</v>
       </c>
-      <c r="P21" s="372"/>
-      <c r="Q21" s="372"/>
-      <c r="R21" s="372"/>
-      <c r="S21" s="373"/>
+      <c r="P21" s="377"/>
+      <c r="Q21" s="377"/>
+      <c r="R21" s="377"/>
+      <c r="S21" s="378"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="175"/>
-      <c r="B22" s="374" t="s">
+      <c r="B22" s="357" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="375"/>
-      <c r="D22" s="375"/>
-      <c r="E22" s="375"/>
-      <c r="F22" s="388"/>
+      <c r="C22" s="358"/>
+      <c r="D22" s="358"/>
+      <c r="E22" s="358"/>
+      <c r="F22" s="351"/>
       <c r="G22" s="152">
         <f>G21</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="393" t="s">
+      <c r="I22" s="350" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="388"/>
-      <c r="K22" s="396">
+      <c r="J22" s="351"/>
+      <c r="K22" s="366">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="L22" s="397"/>
+      <c r="L22" s="367"/>
       <c r="M22" s="176"/>
       <c r="N22" s="170"/>
-      <c r="O22" s="374" t="s">
+      <c r="O22" s="357" t="s">
         <v>260</v>
       </c>
-      <c r="P22" s="375"/>
-      <c r="Q22" s="375"/>
-      <c r="R22" s="375"/>
-      <c r="S22" s="376"/>
+      <c r="P22" s="358"/>
+      <c r="Q22" s="358"/>
+      <c r="R22" s="358"/>
+      <c r="S22" s="382"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="175"/>
-      <c r="B23" s="389" t="s">
+      <c r="B23" s="371" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="390"/>
-      <c r="D23" s="390"/>
-      <c r="E23" s="390"/>
-      <c r="F23" s="391"/>
+      <c r="C23" s="372"/>
+      <c r="D23" s="372"/>
+      <c r="E23" s="372"/>
+      <c r="F23" s="373"/>
       <c r="G23" s="153">
         <f>K24</f>
         <v>1568729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="393" t="s">
+      <c r="I23" s="350" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="388"/>
-      <c r="K23" s="398">
+      <c r="J23" s="351"/>
+      <c r="K23" s="361">
         <f>Pemasukkan!L31</f>
         <v>690000</v>
       </c>
-      <c r="L23" s="399"/>
+      <c r="L23" s="362"/>
       <c r="M23" s="176"/>
       <c r="N23" s="170"/>
-      <c r="O23" s="374" t="s">
+      <c r="O23" s="357" t="s">
         <v>261</v>
       </c>
-      <c r="P23" s="375"/>
-      <c r="Q23" s="375"/>
-      <c r="R23" s="375"/>
-      <c r="S23" s="376"/>
+      <c r="P23" s="358"/>
+      <c r="Q23" s="358"/>
+      <c r="R23" s="358"/>
+      <c r="S23" s="382"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="175"/>
@@ -18063,24 +18093,24 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="371" t="s">
+      <c r="I24" s="352" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="392"/>
-      <c r="K24" s="383">
+      <c r="J24" s="353"/>
+      <c r="K24" s="348">
         <f>(K21-K22)+K23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="L24" s="384"/>
+      <c r="L24" s="349"/>
       <c r="M24" s="176"/>
       <c r="N24" s="170"/>
-      <c r="O24" s="374" t="s">
+      <c r="O24" s="357" t="s">
         <v>262</v>
       </c>
-      <c r="P24" s="375"/>
-      <c r="Q24" s="375"/>
-      <c r="R24" s="375"/>
-      <c r="S24" s="376"/>
+      <c r="P24" s="358"/>
+      <c r="Q24" s="358"/>
+      <c r="R24" s="358"/>
+      <c r="S24" s="382"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="175"/>
@@ -18097,13 +18127,13 @@
       <c r="L25" s="24"/>
       <c r="M25" s="176"/>
       <c r="N25" s="170"/>
-      <c r="O25" s="369" t="s">
+      <c r="O25" s="354" t="s">
         <v>267</v>
       </c>
-      <c r="P25" s="318"/>
-      <c r="Q25" s="318"/>
-      <c r="R25" s="318"/>
-      <c r="S25" s="347"/>
+      <c r="P25" s="315"/>
+      <c r="Q25" s="315"/>
+      <c r="R25" s="315"/>
+      <c r="S25" s="383"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="175"/>
@@ -18120,11 +18150,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="176"/>
       <c r="N26" s="170"/>
-      <c r="O26" s="370"/>
-      <c r="P26" s="348"/>
-      <c r="Q26" s="348"/>
-      <c r="R26" s="348"/>
-      <c r="S26" s="349"/>
+      <c r="O26" s="374"/>
+      <c r="P26" s="375"/>
+      <c r="Q26" s="375"/>
+      <c r="R26" s="375"/>
+      <c r="S26" s="376"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="177"/>
@@ -18159,6 +18189,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:AD3"/>
+    <mergeCell ref="W12:AD12"/>
+    <mergeCell ref="W13:AD13"/>
+    <mergeCell ref="W14:AD14"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:AD7"/>
+    <mergeCell ref="W9:AD9"/>
+    <mergeCell ref="W10:AD10"/>
+    <mergeCell ref="W11:AD11"/>
+    <mergeCell ref="U8:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:AD4"/>
+    <mergeCell ref="W8:AD8"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="O25:S25"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="W5:AD5"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="O18:S18"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O23:S23"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
     <mergeCell ref="D2:L2"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
@@ -18175,53 +18252,6 @@
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="W5:AD5"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="O24:S24"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="O18:S18"/>
-    <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O23:S23"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="W4:AD4"/>
-    <mergeCell ref="W8:AD8"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="O25:S25"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:AD3"/>
-    <mergeCell ref="W12:AD12"/>
-    <mergeCell ref="W13:AD13"/>
-    <mergeCell ref="W14:AD14"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="W7:AD7"/>
-    <mergeCell ref="W9:AD9"/>
-    <mergeCell ref="W10:AD10"/>
-    <mergeCell ref="W11:AD11"/>
-    <mergeCell ref="U8:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U4:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -18255,44 +18285,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="415" t="s">
+      <c r="C2" s="407" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="416"/>
-      <c r="E2" s="416"/>
-      <c r="F2" s="416"/>
-      <c r="G2" s="416"/>
-      <c r="H2" s="416"/>
-      <c r="I2" s="416"/>
-      <c r="J2" s="416"/>
-      <c r="K2" s="416"/>
+      <c r="D2" s="408"/>
+      <c r="E2" s="408"/>
+      <c r="F2" s="408"/>
+      <c r="G2" s="408"/>
+      <c r="H2" s="408"/>
+      <c r="I2" s="408"/>
+      <c r="J2" s="408"/>
+      <c r="K2" s="408"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="416"/>
-      <c r="D3" s="416"/>
-      <c r="E3" s="416"/>
-      <c r="F3" s="416"/>
-      <c r="G3" s="416"/>
-      <c r="H3" s="416"/>
-      <c r="I3" s="416"/>
-      <c r="J3" s="416"/>
-      <c r="K3" s="416"/>
+      <c r="C3" s="408"/>
+      <c r="D3" s="408"/>
+      <c r="E3" s="408"/>
+      <c r="F3" s="408"/>
+      <c r="G3" s="408"/>
+      <c r="H3" s="408"/>
+      <c r="I3" s="408"/>
+      <c r="J3" s="408"/>
+      <c r="K3" s="408"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="408" t="s">
+      <c r="C5" s="415" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="408"/>
-      <c r="E5" s="408"/>
-      <c r="F5" s="408"/>
-      <c r="G5" s="408"/>
-      <c r="I5" s="408" t="s">
+      <c r="D5" s="415"/>
+      <c r="E5" s="415"/>
+      <c r="F5" s="415"/>
+      <c r="G5" s="415"/>
+      <c r="I5" s="415" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="408"/>
-      <c r="K5" s="408"/>
-      <c r="L5" s="408"/>
-      <c r="M5" s="408"/>
+      <c r="J5" s="415"/>
+      <c r="K5" s="415"/>
+      <c r="L5" s="415"/>
+      <c r="M5" s="415"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -18732,20 +18762,20 @@
       <c r="M28" s="170"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="404" t="s">
+      <c r="D29" s="359" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="405"/>
+      <c r="E29" s="360"/>
       <c r="F29" s="409">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
       <c r="G29" s="410"/>
       <c r="I29" s="170"/>
-      <c r="J29" s="404" t="s">
+      <c r="J29" s="359" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="405"/>
+      <c r="K29" s="360"/>
       <c r="L29" s="409">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
@@ -18753,20 +18783,20 @@
       <c r="M29" s="410"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="364" t="s">
+      <c r="D30" s="406" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="318"/>
+      <c r="E30" s="315"/>
       <c r="F30" s="411">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
       <c r="G30" s="412"/>
       <c r="I30" s="170"/>
-      <c r="J30" s="364" t="s">
+      <c r="J30" s="406" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="318"/>
+      <c r="K30" s="315"/>
       <c r="L30" s="411">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
@@ -18774,46 +18804,46 @@
       <c r="M30" s="412"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="369" t="s">
+      <c r="D31" s="354" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="318"/>
-      <c r="F31" s="413">
+      <c r="E31" s="315"/>
+      <c r="F31" s="416">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="414"/>
+      <c r="G31" s="417"/>
       <c r="I31" s="170"/>
-      <c r="J31" s="369" t="s">
+      <c r="J31" s="354" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="318"/>
-      <c r="L31" s="413">
+      <c r="K31" s="315"/>
+      <c r="L31" s="416">
         <f>L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="414"/>
+      <c r="M31" s="417"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="402" t="s">
+      <c r="D32" s="355" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="403"/>
-      <c r="F32" s="406">
+      <c r="E32" s="356"/>
+      <c r="F32" s="413">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="407"/>
+      <c r="G32" s="414"/>
       <c r="I32" s="170"/>
-      <c r="J32" s="402" t="s">
+      <c r="J32" s="355" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="403"/>
-      <c r="L32" s="406">
+      <c r="K32" s="356"/>
+      <c r="L32" s="413">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="407"/>
+      <c r="M32" s="414"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19005,12 +19035,6 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C2:K3"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J29:K29"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="I5:M5"/>
@@ -19024,6 +19048,12 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J32:K32"/>
+    <mergeCell ref="C2:K3"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -19056,44 +19086,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="421" t="s">
+      <c r="C2" s="418" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="422"/>
-      <c r="E2" s="422"/>
-      <c r="F2" s="422"/>
-      <c r="G2" s="422"/>
-      <c r="H2" s="422"/>
-      <c r="I2" s="422"/>
-      <c r="J2" s="422"/>
-      <c r="K2" s="422"/>
+      <c r="D2" s="419"/>
+      <c r="E2" s="419"/>
+      <c r="F2" s="419"/>
+      <c r="G2" s="419"/>
+      <c r="H2" s="419"/>
+      <c r="I2" s="419"/>
+      <c r="J2" s="419"/>
+      <c r="K2" s="419"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="422"/>
-      <c r="D3" s="422"/>
-      <c r="E3" s="422"/>
-      <c r="F3" s="422"/>
-      <c r="G3" s="422"/>
-      <c r="H3" s="422"/>
-      <c r="I3" s="422"/>
-      <c r="J3" s="422"/>
-      <c r="K3" s="422"/>
+      <c r="C3" s="419"/>
+      <c r="D3" s="419"/>
+      <c r="E3" s="419"/>
+      <c r="F3" s="419"/>
+      <c r="G3" s="419"/>
+      <c r="H3" s="419"/>
+      <c r="I3" s="419"/>
+      <c r="J3" s="419"/>
+      <c r="K3" s="419"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="408" t="s">
+      <c r="C5" s="415" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="408"/>
-      <c r="E5" s="408"/>
-      <c r="F5" s="408"/>
-      <c r="G5" s="408"/>
-      <c r="I5" s="408" t="s">
+      <c r="D5" s="415"/>
+      <c r="E5" s="415"/>
+      <c r="F5" s="415"/>
+      <c r="G5" s="415"/>
+      <c r="I5" s="415" t="s">
         <v>246</v>
       </c>
-      <c r="J5" s="408"/>
-      <c r="K5" s="408"/>
-      <c r="L5" s="408"/>
-      <c r="M5" s="408"/>
+      <c r="J5" s="415"/>
+      <c r="K5" s="415"/>
+      <c r="L5" s="415"/>
+      <c r="M5" s="415"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -19577,41 +19607,41 @@
       <c r="M28" s="170"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="343" t="s">
+      <c r="D29" s="394" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="345"/>
-      <c r="F29" s="419">
+      <c r="E29" s="396"/>
+      <c r="F29" s="420">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="420"/>
+      <c r="G29" s="421"/>
       <c r="I29" s="170"/>
-      <c r="J29" s="343" t="s">
+      <c r="J29" s="394" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="345"/>
-      <c r="L29" s="419">
+      <c r="K29" s="396"/>
+      <c r="L29" s="420">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="420"/>
+      <c r="M29" s="421"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="369" t="s">
+      <c r="D30" s="354" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="318"/>
+      <c r="E30" s="315"/>
       <c r="F30" s="411">
         <f>F27</f>
         <v>903300</v>
       </c>
       <c r="G30" s="412"/>
       <c r="I30" s="170"/>
-      <c r="J30" s="369" t="s">
+      <c r="J30" s="354" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="318"/>
+      <c r="K30" s="315"/>
       <c r="L30" s="411">
         <f>L27</f>
         <v>779000</v>
@@ -19619,46 +19649,46 @@
       <c r="M30" s="412"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="369" t="s">
+      <c r="D31" s="354" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="318"/>
-      <c r="F31" s="413">
+      <c r="E31" s="315"/>
+      <c r="F31" s="416">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="414"/>
+      <c r="G31" s="417"/>
       <c r="I31" s="170"/>
-      <c r="J31" s="369" t="s">
+      <c r="J31" s="354" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="318"/>
-      <c r="L31" s="413">
+      <c r="K31" s="315"/>
+      <c r="L31" s="416">
         <f>Pemasukkan!L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="414"/>
+      <c r="M31" s="417"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="402" t="s">
+      <c r="D32" s="355" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="403"/>
-      <c r="F32" s="417">
+      <c r="E32" s="356"/>
+      <c r="F32" s="422">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="418"/>
+      <c r="G32" s="423"/>
       <c r="I32" s="170"/>
-      <c r="J32" s="402" t="s">
+      <c r="J32" s="355" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="403"/>
-      <c r="L32" s="417">
+      <c r="K32" s="356"/>
+      <c r="L32" s="422">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="418"/>
+      <c r="M32" s="423"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19850,6 +19880,14 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
     <mergeCell ref="C2:K3"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
@@ -19861,14 +19899,6 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -19894,28 +19924,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="425" t="s">
+      <c r="C2" s="426" t="s">
         <v>230</v>
       </c>
-      <c r="D2" s="426"/>
-      <c r="E2" s="426"/>
-      <c r="F2" s="426"/>
-      <c r="G2" s="426"/>
-      <c r="H2" s="426"/>
-      <c r="I2" s="426"/>
-      <c r="J2" s="426"/>
-      <c r="K2" s="426"/>
+      <c r="D2" s="427"/>
+      <c r="E2" s="427"/>
+      <c r="F2" s="427"/>
+      <c r="G2" s="427"/>
+      <c r="H2" s="427"/>
+      <c r="I2" s="427"/>
+      <c r="J2" s="427"/>
+      <c r="K2" s="427"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="426"/>
-      <c r="D3" s="426"/>
-      <c r="E3" s="426"/>
-      <c r="F3" s="426"/>
-      <c r="G3" s="426"/>
-      <c r="H3" s="426"/>
-      <c r="I3" s="426"/>
-      <c r="J3" s="426"/>
-      <c r="K3" s="426"/>
+      <c r="C3" s="427"/>
+      <c r="D3" s="427"/>
+      <c r="E3" s="427"/>
+      <c r="F3" s="427"/>
+      <c r="G3" s="427"/>
+      <c r="H3" s="427"/>
+      <c r="I3" s="427"/>
+      <c r="J3" s="427"/>
+      <c r="K3" s="427"/>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="139"/>
@@ -20273,10 +20303,10 @@
     </row>
     <row r="29" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="139"/>
-      <c r="D29" s="427"/>
-      <c r="E29" s="427"/>
-      <c r="F29" s="428"/>
-      <c r="G29" s="428"/>
+      <c r="D29" s="428"/>
+      <c r="E29" s="428"/>
+      <c r="F29" s="429"/>
+      <c r="G29" s="429"/>
       <c r="H29" s="139"/>
       <c r="I29" s="139"/>
       <c r="J29" s="139"/>
@@ -20284,15 +20314,15 @@
     </row>
     <row r="30" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="24"/>
-      <c r="D30" s="429" t="s">
+      <c r="D30" s="430" t="s">
         <v>229</v>
       </c>
-      <c r="E30" s="430"/>
-      <c r="F30" s="431">
+      <c r="E30" s="431"/>
+      <c r="F30" s="432">
         <f>F27</f>
         <v>226000</v>
       </c>
-      <c r="G30" s="432"/>
+      <c r="G30" s="433"/>
       <c r="H30" s="139"/>
       <c r="I30" s="139"/>
       <c r="J30" s="139"/>
@@ -20307,10 +20337,10 @@
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="139"/>
-      <c r="D32" s="423"/>
-      <c r="E32" s="423"/>
-      <c r="F32" s="424"/>
-      <c r="G32" s="423"/>
+      <c r="D32" s="424"/>
+      <c r="E32" s="424"/>
+      <c r="F32" s="425"/>
+      <c r="G32" s="424"/>
       <c r="H32" s="139"/>
       <c r="I32" s="139"/>
       <c r="J32" s="139"/>
@@ -20347,17 +20377,17 @@
     <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="433" t="s">
+      <c r="C4" s="434" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="434"/>
+      <c r="D4" s="435"/>
       <c r="E4" s="27"/>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
-      <c r="H4" s="433" t="s">
+      <c r="H4" s="434" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="434"/>
+      <c r="I4" s="435"/>
       <c r="J4" s="35"/>
       <c r="K4" s="27"/>
     </row>
@@ -20484,17 +20514,17 @@
     <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26"/>
-      <c r="C17" s="433" t="s">
+      <c r="C17" s="434" t="s">
         <v>144</v>
       </c>
-      <c r="D17" s="434"/>
+      <c r="D17" s="435"/>
       <c r="E17" s="27"/>
       <c r="F17" s="26"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="433" t="s">
+      <c r="H17" s="434" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="434"/>
+      <c r="I17" s="435"/>
       <c r="J17" s="35"/>
       <c r="K17" s="27"/>
     </row>

</xml_diff>

<commit_message>
Tambahan bkolom pada pembayaran makrab 19
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -2430,7 +2430,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="441">
+  <cellXfs count="442">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3052,20 +3052,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3081,39 +3091,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3121,36 +3129,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3203,193 +3204,220 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3398,31 +3426,16 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3430,18 +3443,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3500,7 +3501,28 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="29">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4696,126 +4718,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="285" t="s">
+      <c r="A1" s="292" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="286"/>
-      <c r="C1" s="286"/>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
-      <c r="N1" s="286"/>
-      <c r="O1" s="286"/>
-      <c r="P1" s="286"/>
-      <c r="Q1" s="286"/>
-      <c r="R1" s="286"/>
+      <c r="B1" s="293"/>
+      <c r="C1" s="293"/>
+      <c r="D1" s="293"/>
+      <c r="E1" s="293"/>
+      <c r="F1" s="293"/>
+      <c r="G1" s="293"/>
+      <c r="H1" s="293"/>
+      <c r="I1" s="293"/>
+      <c r="J1" s="293"/>
+      <c r="K1" s="293"/>
+      <c r="L1" s="293"/>
+      <c r="M1" s="293"/>
+      <c r="N1" s="293"/>
+      <c r="O1" s="293"/>
+      <c r="P1" s="293"/>
+      <c r="Q1" s="293"/>
+      <c r="R1" s="293"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="287"/>
-      <c r="B2" s="288"/>
-      <c r="C2" s="288"/>
-      <c r="D2" s="288"/>
-      <c r="E2" s="288"/>
-      <c r="F2" s="288"/>
-      <c r="G2" s="288"/>
-      <c r="H2" s="288"/>
-      <c r="I2" s="288"/>
-      <c r="J2" s="288"/>
-      <c r="K2" s="288"/>
-      <c r="L2" s="288"/>
-      <c r="M2" s="288"/>
-      <c r="N2" s="288"/>
-      <c r="O2" s="288"/>
-      <c r="P2" s="288"/>
-      <c r="Q2" s="288"/>
-      <c r="R2" s="288"/>
+      <c r="A2" s="294"/>
+      <c r="B2" s="295"/>
+      <c r="C2" s="295"/>
+      <c r="D2" s="295"/>
+      <c r="E2" s="295"/>
+      <c r="F2" s="295"/>
+      <c r="G2" s="295"/>
+      <c r="H2" s="295"/>
+      <c r="I2" s="295"/>
+      <c r="J2" s="295"/>
+      <c r="K2" s="295"/>
+      <c r="L2" s="295"/>
+      <c r="M2" s="295"/>
+      <c r="N2" s="295"/>
+      <c r="O2" s="295"/>
+      <c r="P2" s="295"/>
+      <c r="Q2" s="295"/>
+      <c r="R2" s="295"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="287"/>
-      <c r="B3" s="288"/>
-      <c r="C3" s="288"/>
-      <c r="D3" s="288"/>
-      <c r="E3" s="288"/>
-      <c r="F3" s="288"/>
-      <c r="G3" s="288"/>
-      <c r="H3" s="288"/>
-      <c r="I3" s="288"/>
-      <c r="J3" s="288"/>
-      <c r="K3" s="288"/>
-      <c r="L3" s="288"/>
-      <c r="M3" s="288"/>
-      <c r="N3" s="288"/>
-      <c r="O3" s="288"/>
-      <c r="P3" s="288"/>
-      <c r="Q3" s="288"/>
-      <c r="R3" s="288"/>
+      <c r="A3" s="294"/>
+      <c r="B3" s="295"/>
+      <c r="C3" s="295"/>
+      <c r="D3" s="295"/>
+      <c r="E3" s="295"/>
+      <c r="F3" s="295"/>
+      <c r="G3" s="295"/>
+      <c r="H3" s="295"/>
+      <c r="I3" s="295"/>
+      <c r="J3" s="295"/>
+      <c r="K3" s="295"/>
+      <c r="L3" s="295"/>
+      <c r="M3" s="295"/>
+      <c r="N3" s="295"/>
+      <c r="O3" s="295"/>
+      <c r="P3" s="295"/>
+      <c r="Q3" s="295"/>
+      <c r="R3" s="295"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="287"/>
-      <c r="B4" s="288"/>
-      <c r="C4" s="288"/>
-      <c r="D4" s="288"/>
-      <c r="E4" s="288"/>
-      <c r="F4" s="288"/>
-      <c r="G4" s="288"/>
-      <c r="H4" s="288"/>
-      <c r="I4" s="288"/>
-      <c r="J4" s="288"/>
-      <c r="K4" s="288"/>
-      <c r="L4" s="288"/>
-      <c r="M4" s="288"/>
-      <c r="N4" s="288"/>
-      <c r="O4" s="288"/>
-      <c r="P4" s="288"/>
-      <c r="Q4" s="288"/>
-      <c r="R4" s="288"/>
+      <c r="A4" s="294"/>
+      <c r="B4" s="295"/>
+      <c r="C4" s="295"/>
+      <c r="D4" s="295"/>
+      <c r="E4" s="295"/>
+      <c r="F4" s="295"/>
+      <c r="G4" s="295"/>
+      <c r="H4" s="295"/>
+      <c r="I4" s="295"/>
+      <c r="J4" s="295"/>
+      <c r="K4" s="295"/>
+      <c r="L4" s="295"/>
+      <c r="M4" s="295"/>
+      <c r="N4" s="295"/>
+      <c r="O4" s="295"/>
+      <c r="P4" s="295"/>
+      <c r="Q4" s="295"/>
+      <c r="R4" s="295"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="287"/>
-      <c r="B5" s="288"/>
-      <c r="C5" s="288"/>
-      <c r="D5" s="288"/>
-      <c r="E5" s="288"/>
-      <c r="F5" s="288"/>
-      <c r="G5" s="288"/>
-      <c r="H5" s="288"/>
-      <c r="I5" s="288"/>
-      <c r="J5" s="288"/>
-      <c r="K5" s="288"/>
-      <c r="L5" s="288"/>
-      <c r="M5" s="288"/>
-      <c r="N5" s="288"/>
-      <c r="O5" s="288"/>
-      <c r="P5" s="288"/>
-      <c r="Q5" s="288"/>
-      <c r="R5" s="288"/>
+      <c r="A5" s="294"/>
+      <c r="B5" s="295"/>
+      <c r="C5" s="295"/>
+      <c r="D5" s="295"/>
+      <c r="E5" s="295"/>
+      <c r="F5" s="295"/>
+      <c r="G5" s="295"/>
+      <c r="H5" s="295"/>
+      <c r="I5" s="295"/>
+      <c r="J5" s="295"/>
+      <c r="K5" s="295"/>
+      <c r="L5" s="295"/>
+      <c r="M5" s="295"/>
+      <c r="N5" s="295"/>
+      <c r="O5" s="295"/>
+      <c r="P5" s="295"/>
+      <c r="Q5" s="295"/>
+      <c r="R5" s="295"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="287"/>
-      <c r="B6" s="288"/>
-      <c r="C6" s="288"/>
-      <c r="D6" s="288"/>
-      <c r="E6" s="288"/>
-      <c r="F6" s="288"/>
-      <c r="G6" s="288"/>
-      <c r="H6" s="288"/>
-      <c r="I6" s="288"/>
-      <c r="J6" s="288"/>
-      <c r="K6" s="288"/>
-      <c r="L6" s="288"/>
-      <c r="M6" s="288"/>
-      <c r="N6" s="288"/>
-      <c r="O6" s="288"/>
-      <c r="P6" s="288"/>
-      <c r="Q6" s="288"/>
-      <c r="R6" s="288"/>
+      <c r="A6" s="294"/>
+      <c r="B6" s="295"/>
+      <c r="C6" s="295"/>
+      <c r="D6" s="295"/>
+      <c r="E6" s="295"/>
+      <c r="F6" s="295"/>
+      <c r="G6" s="295"/>
+      <c r="H6" s="295"/>
+      <c r="I6" s="295"/>
+      <c r="J6" s="295"/>
+      <c r="K6" s="295"/>
+      <c r="L6" s="295"/>
+      <c r="M6" s="295"/>
+      <c r="N6" s="295"/>
+      <c r="O6" s="295"/>
+      <c r="P6" s="295"/>
+      <c r="Q6" s="295"/>
+      <c r="R6" s="295"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -7922,58 +7944,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="293" t="s">
+      <c r="J79" s="297" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="294"/>
-      <c r="L79" s="294"/>
-      <c r="M79" s="294"/>
-      <c r="N79" s="295"/>
-      <c r="P79" s="301" t="s">
+      <c r="K79" s="298"/>
+      <c r="L79" s="298"/>
+      <c r="M79" s="298"/>
+      <c r="N79" s="299"/>
+      <c r="P79" s="305" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="294"/>
-      <c r="R79" s="294"/>
-      <c r="S79" s="295"/>
+      <c r="Q79" s="298"/>
+      <c r="R79" s="298"/>
+      <c r="S79" s="299"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="296" t="s">
+      <c r="J80" s="300" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="288"/>
-      <c r="L80" s="288"/>
-      <c r="M80" s="288"/>
-      <c r="N80" s="297"/>
-      <c r="P80" s="296" t="s">
+      <c r="K80" s="295"/>
+      <c r="L80" s="295"/>
+      <c r="M80" s="295"/>
+      <c r="N80" s="301"/>
+      <c r="P80" s="300" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="288"/>
-      <c r="R80" s="288"/>
-      <c r="S80" s="297"/>
+      <c r="Q80" s="295"/>
+      <c r="R80" s="295"/>
+      <c r="S80" s="301"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="298"/>
-      <c r="K81" s="299"/>
-      <c r="L81" s="299"/>
-      <c r="M81" s="299"/>
-      <c r="N81" s="300"/>
-      <c r="P81" s="298"/>
-      <c r="Q81" s="299"/>
-      <c r="R81" s="299"/>
-      <c r="S81" s="300"/>
+      <c r="J81" s="302"/>
+      <c r="K81" s="303"/>
+      <c r="L81" s="303"/>
+      <c r="M81" s="303"/>
+      <c r="N81" s="304"/>
+      <c r="P81" s="302"/>
+      <c r="Q81" s="303"/>
+      <c r="R81" s="303"/>
+      <c r="S81" s="304"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="291" t="s">
+      <c r="J82" s="296" t="s">
         <v>19</v>
       </c>
-      <c r="K82" s="292"/>
-      <c r="L82" s="290"/>
-      <c r="M82" s="291" t="s">
+      <c r="K82" s="287"/>
+      <c r="L82" s="288"/>
+      <c r="M82" s="296" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="290"/>
-      <c r="P82" s="291"/>
-      <c r="Q82" s="290"/>
+      <c r="N82" s="288"/>
+      <c r="P82" s="296"/>
+      <c r="Q82" s="288"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -7982,38 +8004,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="302" t="s">
+      <c r="J83" s="286" t="s">
         <v>70</v>
       </c>
-      <c r="K83" s="292"/>
-      <c r="L83" s="290"/>
-      <c r="M83" s="303">
+      <c r="K83" s="287"/>
+      <c r="L83" s="288"/>
+      <c r="M83" s="289">
         <v>7350000</v>
       </c>
-      <c r="N83" s="290"/>
-      <c r="P83" s="289" t="s">
+      <c r="N83" s="288"/>
+      <c r="P83" s="290" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="290"/>
+      <c r="Q83" s="288"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="302" t="s">
+      <c r="J84" s="286" t="s">
         <v>72</v>
       </c>
-      <c r="K84" s="292"/>
-      <c r="L84" s="290"/>
-      <c r="M84" s="304">
+      <c r="K84" s="287"/>
+      <c r="L84" s="288"/>
+      <c r="M84" s="291">
         <v>1100000</v>
       </c>
-      <c r="N84" s="290"/>
-      <c r="P84" s="289" t="s">
+      <c r="N84" s="288"/>
+      <c r="P84" s="290" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="290"/>
+      <c r="Q84" s="288"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -8022,39 +8044,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="302" t="s">
+      <c r="J85" s="286" t="s">
         <v>75</v>
       </c>
-      <c r="K85" s="292"/>
-      <c r="L85" s="290"/>
-      <c r="M85" s="303">
+      <c r="K85" s="287"/>
+      <c r="L85" s="288"/>
+      <c r="M85" s="289">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="290"/>
-      <c r="P85" s="289" t="s">
+      <c r="N85" s="288"/>
+      <c r="P85" s="290" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="290"/>
+      <c r="Q85" s="288"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="302" t="s">
+      <c r="J86" s="286" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="292"/>
-      <c r="L86" s="290"/>
-      <c r="M86" s="303">
+      <c r="K86" s="287"/>
+      <c r="L86" s="288"/>
+      <c r="M86" s="289">
         <v>8411850</v>
       </c>
-      <c r="N86" s="290"/>
-      <c r="P86" s="289" t="s">
+      <c r="N86" s="288"/>
+      <c r="P86" s="290" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="290"/>
+      <c r="Q86" s="288"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -8062,20 +8084,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="302" t="s">
+      <c r="J87" s="286" t="s">
         <v>79</v>
       </c>
-      <c r="K87" s="292"/>
-      <c r="L87" s="290"/>
-      <c r="M87" s="303">
+      <c r="K87" s="287"/>
+      <c r="L87" s="288"/>
+      <c r="M87" s="289">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="290"/>
-      <c r="P87" s="289" t="s">
+      <c r="N87" s="288"/>
+      <c r="P87" s="290" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="290"/>
+      <c r="Q87" s="288"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -8263,17 +8285,6 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="P86:Q86"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="M84:N84"/>
     <mergeCell ref="A1:R6"/>
     <mergeCell ref="P84:Q84"/>
     <mergeCell ref="J82:L82"/>
@@ -8286,27 +8297,38 @@
     <mergeCell ref="P83:Q83"/>
     <mergeCell ref="P82:Q82"/>
     <mergeCell ref="P80:S81"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="P86:Q86"/>
   </mergeCells>
   <conditionalFormatting sqref="T10:T69">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S69">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S69">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>$S$12=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8332,28 +8354,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="437" t="s">
+      <c r="B2" s="438" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="438"/>
-      <c r="D2" s="438"/>
-      <c r="E2" s="438"/>
-      <c r="F2" s="438"/>
-      <c r="G2" s="438"/>
-      <c r="H2" s="438"/>
-      <c r="I2" s="438"/>
-      <c r="J2" s="438"/>
+      <c r="C2" s="439"/>
+      <c r="D2" s="439"/>
+      <c r="E2" s="439"/>
+      <c r="F2" s="439"/>
+      <c r="G2" s="439"/>
+      <c r="H2" s="439"/>
+      <c r="I2" s="439"/>
+      <c r="J2" s="439"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="438"/>
-      <c r="C3" s="438"/>
-      <c r="D3" s="438"/>
-      <c r="E3" s="438"/>
-      <c r="F3" s="438"/>
-      <c r="G3" s="438"/>
-      <c r="H3" s="438"/>
-      <c r="I3" s="438"/>
-      <c r="J3" s="438"/>
+      <c r="B3" s="439"/>
+      <c r="C3" s="439"/>
+      <c r="D3" s="439"/>
+      <c r="E3" s="439"/>
+      <c r="F3" s="439"/>
+      <c r="G3" s="439"/>
+      <c r="H3" s="439"/>
+      <c r="I3" s="439"/>
+      <c r="J3" s="439"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -8374,10 +8396,10 @@
       <c r="G6" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="H6" s="363" t="s">
+      <c r="H6" s="354" t="s">
         <v>280</v>
       </c>
-      <c r="I6" s="315"/>
+      <c r="I6" s="319"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -8399,11 +8421,11 @@
       <c r="G7" s="193">
         <v>205000</v>
       </c>
-      <c r="H7" s="439">
+      <c r="H7" s="440">
         <f>F7-G7</f>
         <v>380000</v>
       </c>
-      <c r="I7" s="315"/>
+      <c r="I7" s="319"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="194"/>
@@ -8412,8 +8434,8 @@
       <c r="E8" s="195"/>
       <c r="F8" s="195"/>
       <c r="G8" s="195"/>
-      <c r="H8" s="436"/>
-      <c r="I8" s="436"/>
+      <c r="H8" s="437"/>
+      <c r="I8" s="437"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="194"/>
@@ -8424,11 +8446,11 @@
       <c r="G9" s="196" t="s">
         <v>281</v>
       </c>
-      <c r="H9" s="440">
+      <c r="H9" s="441">
         <f>H7</f>
         <v>380000</v>
       </c>
-      <c r="I9" s="342"/>
+      <c r="I9" s="343"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="194"/>
@@ -8437,8 +8459,8 @@
       <c r="E10" s="195"/>
       <c r="F10" s="195"/>
       <c r="G10" s="195"/>
-      <c r="H10" s="436"/>
-      <c r="I10" s="436"/>
+      <c r="H10" s="437"/>
+      <c r="I10" s="437"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="194"/>
@@ -8447,8 +8469,8 @@
       <c r="E11" s="195"/>
       <c r="F11" s="195"/>
       <c r="G11" s="195"/>
-      <c r="H11" s="436"/>
-      <c r="I11" s="436"/>
+      <c r="H11" s="437"/>
+      <c r="I11" s="437"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="194"/>
@@ -8457,8 +8479,8 @@
       <c r="E12" s="195"/>
       <c r="F12" s="195"/>
       <c r="G12" s="195"/>
-      <c r="H12" s="436"/>
-      <c r="I12" s="436"/>
+      <c r="H12" s="437"/>
+      <c r="I12" s="437"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="194"/>
@@ -8467,8 +8489,8 @@
       <c r="E13" s="195"/>
       <c r="F13" s="195"/>
       <c r="G13" s="195"/>
-      <c r="H13" s="436"/>
-      <c r="I13" s="436"/>
+      <c r="H13" s="437"/>
+      <c r="I13" s="437"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="194"/>
@@ -8477,8 +8499,8 @@
       <c r="E14" s="195"/>
       <c r="F14" s="195"/>
       <c r="G14" s="195"/>
-      <c r="H14" s="436"/>
-      <c r="I14" s="436"/>
+      <c r="H14" s="437"/>
+      <c r="I14" s="437"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="194"/>
@@ -8487,8 +8509,8 @@
       <c r="E15" s="195"/>
       <c r="F15" s="195"/>
       <c r="G15" s="195"/>
-      <c r="H15" s="436"/>
-      <c r="I15" s="436"/>
+      <c r="H15" s="437"/>
+      <c r="I15" s="437"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="194"/>
@@ -8497,8 +8519,8 @@
       <c r="E16" s="195"/>
       <c r="F16" s="195"/>
       <c r="G16" s="195"/>
-      <c r="H16" s="436"/>
-      <c r="I16" s="436"/>
+      <c r="H16" s="437"/>
+      <c r="I16" s="437"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="194"/>
@@ -8507,11 +8529,16 @@
       <c r="E17" s="195"/>
       <c r="F17" s="195"/>
       <c r="G17" s="195"/>
-      <c r="H17" s="436"/>
-      <c r="I17" s="436"/>
+      <c r="H17" s="437"/>
+      <c r="I17" s="437"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="H6:I6"/>
@@ -8520,11 +8547,6 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8578,46 +8600,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="325" t="s">
+      <c r="C2" s="314" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="286"/>
-      <c r="E2" s="286"/>
-      <c r="F2" s="286"/>
-      <c r="G2" s="286"/>
-      <c r="H2" s="286"/>
-      <c r="I2" s="286"/>
-      <c r="J2" s="286"/>
-      <c r="K2" s="286"/>
-      <c r="L2" s="286"/>
-      <c r="M2" s="286"/>
-      <c r="N2" s="286"/>
-      <c r="O2" s="286"/>
-      <c r="P2" s="287"/>
-      <c r="Q2" s="287"/>
-      <c r="R2" s="287"/>
-      <c r="S2" s="286"/>
-      <c r="T2" s="286"/>
+      <c r="D2" s="293"/>
+      <c r="E2" s="293"/>
+      <c r="F2" s="293"/>
+      <c r="G2" s="293"/>
+      <c r="H2" s="293"/>
+      <c r="I2" s="293"/>
+      <c r="J2" s="293"/>
+      <c r="K2" s="293"/>
+      <c r="L2" s="293"/>
+      <c r="M2" s="293"/>
+      <c r="N2" s="293"/>
+      <c r="O2" s="293"/>
+      <c r="P2" s="294"/>
+      <c r="Q2" s="294"/>
+      <c r="R2" s="294"/>
+      <c r="S2" s="293"/>
+      <c r="T2" s="293"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="287"/>
-      <c r="D3" s="288"/>
-      <c r="E3" s="288"/>
-      <c r="F3" s="288"/>
-      <c r="G3" s="288"/>
-      <c r="H3" s="288"/>
-      <c r="I3" s="288"/>
-      <c r="J3" s="288"/>
-      <c r="K3" s="288"/>
-      <c r="L3" s="288"/>
-      <c r="M3" s="288"/>
-      <c r="N3" s="288"/>
-      <c r="O3" s="288"/>
-      <c r="P3" s="288"/>
-      <c r="Q3" s="288"/>
-      <c r="R3" s="288"/>
-      <c r="S3" s="288"/>
-      <c r="T3" s="288"/>
+      <c r="C3" s="294"/>
+      <c r="D3" s="295"/>
+      <c r="E3" s="295"/>
+      <c r="F3" s="295"/>
+      <c r="G3" s="295"/>
+      <c r="H3" s="295"/>
+      <c r="I3" s="295"/>
+      <c r="J3" s="295"/>
+      <c r="K3" s="295"/>
+      <c r="L3" s="295"/>
+      <c r="M3" s="295"/>
+      <c r="N3" s="295"/>
+      <c r="O3" s="295"/>
+      <c r="P3" s="295"/>
+      <c r="Q3" s="295"/>
+      <c r="R3" s="295"/>
+      <c r="S3" s="295"/>
+      <c r="T3" s="295"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8704,25 +8726,25 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="317" t="s">
+      <c r="X5" s="320" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="292"/>
-      <c r="Z5" s="292"/>
-      <c r="AA5" s="292"/>
-      <c r="AB5" s="292"/>
-      <c r="AC5" s="292"/>
-      <c r="AD5" s="292"/>
-      <c r="AE5" s="292"/>
-      <c r="AF5" s="292"/>
-      <c r="AG5" s="292"/>
-      <c r="AH5" s="292"/>
-      <c r="AI5" s="292"/>
-      <c r="AJ5" s="292"/>
-      <c r="AK5" s="292"/>
-      <c r="AL5" s="292"/>
-      <c r="AM5" s="292"/>
-      <c r="AN5" s="290"/>
+      <c r="Y5" s="287"/>
+      <c r="Z5" s="287"/>
+      <c r="AA5" s="287"/>
+      <c r="AB5" s="287"/>
+      <c r="AC5" s="287"/>
+      <c r="AD5" s="287"/>
+      <c r="AE5" s="287"/>
+      <c r="AF5" s="287"/>
+      <c r="AG5" s="287"/>
+      <c r="AH5" s="287"/>
+      <c r="AI5" s="287"/>
+      <c r="AJ5" s="287"/>
+      <c r="AK5" s="287"/>
+      <c r="AL5" s="287"/>
+      <c r="AM5" s="287"/>
+      <c r="AN5" s="288"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -8797,13 +8819,13 @@
       <c r="V6" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X6" s="326" t="s">
+      <c r="X6" s="315" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="326" t="s">
+      <c r="Y6" s="315" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="315" t="s">
+      <c r="Z6" s="319" t="s">
         <v>86</v>
       </c>
       <c r="AA6" s="316"/>
@@ -8896,13 +8918,13 @@
       </c>
       <c r="X7" s="316"/>
       <c r="Y7" s="316"/>
-      <c r="Z7" s="315" t="s">
+      <c r="Z7" s="319" t="s">
         <v>87</v>
       </c>
       <c r="AA7" s="316"/>
       <c r="AB7" s="316"/>
       <c r="AC7" s="316"/>
-      <c r="AD7" s="315" t="s">
+      <c r="AD7" s="319" t="s">
         <v>88</v>
       </c>
       <c r="AE7" s="316"/>
@@ -13576,10 +13598,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="313" t="s">
+      <c r="AA49" s="317" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="314"/>
+      <c r="AB49" s="318"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -13657,12 +13679,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="309" t="s">
+      <c r="AI50" s="324" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="310"/>
-      <c r="AK50" s="310"/>
-      <c r="AL50" s="311"/>
+      <c r="AJ50" s="325"/>
+      <c r="AK50" s="325"/>
+      <c r="AL50" s="326"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -13733,12 +13755,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="306" t="s">
+      <c r="AI51" s="321" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="307"/>
-      <c r="AK51" s="307"/>
-      <c r="AL51" s="308"/>
+      <c r="AJ51" s="322"/>
+      <c r="AK51" s="322"/>
+      <c r="AL51" s="323"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -14004,14 +14026,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="312"/>
-      <c r="AD55" s="312"/>
-      <c r="AI55" s="309" t="s">
+      <c r="AC55" s="327"/>
+      <c r="AD55" s="327"/>
+      <c r="AI55" s="324" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="310"/>
-      <c r="AK55" s="310"/>
-      <c r="AL55" s="311"/>
+      <c r="AJ55" s="325"/>
+      <c r="AK55" s="325"/>
+      <c r="AL55" s="326"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -14090,12 +14112,12 @@
         <v>OK</v>
       </c>
       <c r="V56" s="2"/>
-      <c r="AI56" s="305" t="s">
+      <c r="AI56" s="306" t="s">
         <v>168</v>
       </c>
-      <c r="AJ56" s="305"/>
-      <c r="AK56" s="305"/>
-      <c r="AL56" s="305"/>
+      <c r="AJ56" s="306"/>
+      <c r="AK56" s="306"/>
+      <c r="AL56" s="306"/>
       <c r="AM56" s="52">
         <f>AM50-AM55</f>
         <v>450000</v>
@@ -14344,32 +14366,32 @@
     <row r="67" spans="3:19" s="256" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="318" t="s">
+      <c r="C69" s="307" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="319"/>
-      <c r="E69" s="319"/>
-      <c r="F69" s="319"/>
-      <c r="G69" s="320"/>
-      <c r="I69" s="324" t="s">
+      <c r="D69" s="308"/>
+      <c r="E69" s="308"/>
+      <c r="F69" s="308"/>
+      <c r="G69" s="309"/>
+      <c r="I69" s="313" t="s">
         <v>178</v>
       </c>
-      <c r="J69" s="324"/>
-      <c r="K69" s="324"/>
-      <c r="L69" s="324"/>
-      <c r="M69" s="324"/>
+      <c r="J69" s="313"/>
+      <c r="K69" s="313"/>
+      <c r="L69" s="313"/>
+      <c r="M69" s="313"/>
     </row>
     <row r="70" spans="3:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="321"/>
-      <c r="D70" s="322"/>
-      <c r="E70" s="322"/>
-      <c r="F70" s="322"/>
-      <c r="G70" s="323"/>
-      <c r="I70" s="324"/>
-      <c r="J70" s="324"/>
-      <c r="K70" s="324"/>
-      <c r="L70" s="324"/>
-      <c r="M70" s="324"/>
+      <c r="C70" s="310"/>
+      <c r="D70" s="311"/>
+      <c r="E70" s="311"/>
+      <c r="F70" s="311"/>
+      <c r="G70" s="312"/>
+      <c r="I70" s="313"/>
+      <c r="J70" s="313"/>
+      <c r="K70" s="313"/>
+      <c r="L70" s="313"/>
+      <c r="M70" s="313"/>
     </row>
     <row r="71" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14390,10 +14412,10 @@
       <c r="M76" s="55"/>
       <c r="N76" s="55"/>
       <c r="O76" s="55"/>
-      <c r="P76" s="305" t="s">
+      <c r="P76" s="306" t="s">
         <v>214</v>
       </c>
-      <c r="Q76" s="305"/>
+      <c r="Q76" s="306"/>
       <c r="R76" s="55"/>
       <c r="S76" s="55"/>
     </row>
@@ -14860,78 +14882,78 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AI56:AL56"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AI50:AL50"/>
+    <mergeCell ref="AI55:AL55"/>
+    <mergeCell ref="AC55:AD55"/>
+    <mergeCell ref="AA49:AB49"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="AD7:AN7"/>
+    <mergeCell ref="X5:AN5"/>
+    <mergeCell ref="Z6:AN6"/>
     <mergeCell ref="P76:Q76"/>
     <mergeCell ref="C69:G70"/>
     <mergeCell ref="I69:M70"/>
     <mergeCell ref="C2:T3"/>
     <mergeCell ref="Y6:Y8"/>
     <mergeCell ref="X6:X8"/>
-    <mergeCell ref="AA49:AB49"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="AD7:AN7"/>
-    <mergeCell ref="X5:AN5"/>
-    <mergeCell ref="Z6:AN6"/>
-    <mergeCell ref="AI56:AL56"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AI50:AL50"/>
-    <mergeCell ref="AI55:AL55"/>
-    <mergeCell ref="AC55:AD55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:V61">
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="23" priority="8">
       <formula>IF(ISBLANK($B$4), 0, SEARCH($B$4,$B6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK48">
-    <cfRule type="containsText" dxfId="19" priority="9" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="22" priority="9" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH(("YES"),(AK9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK9:AK48">
-    <cfRule type="containsText" dxfId="18" priority="10" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="21" priority="10" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH(("NO"),(AK9))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y9:AN9 Y46:AC46 AD46:AL48 AC47:AC48 Y10:AL45 AM10:AN48">
-    <cfRule type="expression" dxfId="17" priority="11">
+    <cfRule type="expression" dxfId="20" priority="11">
       <formula>IF(ISBLANK($Z$4), 0, SEARCH($Z$4,$Y9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6:U61">
-    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="19" priority="12" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH(("NO"),(U6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6:U61">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="18" priority="13" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH(("OK"),(U6))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y10:Y45">
-    <cfRule type="expression" dxfId="14" priority="7">
+    <cfRule type="expression" dxfId="17" priority="7">
       <formula>IF(AK10="YES",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q6:R61">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6:P61">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y9:AN48">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>IF(ISBLANK($AA$4), 0, SEARCH($AA$4,$Y9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6:O61">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThanOrEqual">
       <formula>200</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14965,86 +14987,86 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="327" t="s">
+      <c r="A2" s="328" t="s">
         <v>300</v>
       </c>
-      <c r="B2" s="327"/>
-      <c r="C2" s="327"/>
-      <c r="D2" s="327"/>
-      <c r="E2" s="327"/>
-      <c r="F2" s="327"/>
-      <c r="G2" s="327"/>
-      <c r="H2" s="327"/>
-      <c r="I2" s="327"/>
-      <c r="J2" s="327"/>
-      <c r="K2" s="327"/>
-      <c r="L2" s="327"/>
+      <c r="B2" s="328"/>
+      <c r="C2" s="328"/>
+      <c r="D2" s="328"/>
+      <c r="E2" s="328"/>
+      <c r="F2" s="328"/>
+      <c r="G2" s="328"/>
+      <c r="H2" s="328"/>
+      <c r="I2" s="328"/>
+      <c r="J2" s="328"/>
+      <c r="K2" s="328"/>
+      <c r="L2" s="328"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="327"/>
-      <c r="B3" s="327"/>
-      <c r="C3" s="327"/>
-      <c r="D3" s="327"/>
-      <c r="E3" s="327"/>
-      <c r="F3" s="327"/>
-      <c r="G3" s="327"/>
-      <c r="H3" s="327"/>
-      <c r="I3" s="327"/>
-      <c r="J3" s="327"/>
-      <c r="K3" s="327"/>
-      <c r="L3" s="327"/>
+      <c r="A3" s="328"/>
+      <c r="B3" s="328"/>
+      <c r="C3" s="328"/>
+      <c r="D3" s="328"/>
+      <c r="E3" s="328"/>
+      <c r="F3" s="328"/>
+      <c r="G3" s="328"/>
+      <c r="H3" s="328"/>
+      <c r="I3" s="328"/>
+      <c r="J3" s="328"/>
+      <c r="K3" s="328"/>
+      <c r="L3" s="328"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="324" t="s">
+      <c r="A5" s="313" t="s">
         <v>303</v>
       </c>
-      <c r="B5" s="324"/>
-      <c r="C5" s="324"/>
-      <c r="D5" s="324"/>
-      <c r="E5" s="324"/>
-      <c r="F5" s="324"/>
-      <c r="G5" s="324"/>
-      <c r="H5" s="324"/>
-      <c r="I5" s="324"/>
-      <c r="J5" s="324"/>
-      <c r="K5" s="324"/>
-      <c r="M5" s="324" t="s">
+      <c r="B5" s="313"/>
+      <c r="C5" s="313"/>
+      <c r="D5" s="313"/>
+      <c r="E5" s="313"/>
+      <c r="F5" s="313"/>
+      <c r="G5" s="313"/>
+      <c r="H5" s="313"/>
+      <c r="I5" s="313"/>
+      <c r="J5" s="313"/>
+      <c r="K5" s="313"/>
+      <c r="M5" s="313" t="s">
         <v>324</v>
       </c>
-      <c r="N5" s="324"/>
-      <c r="O5" s="324"/>
-      <c r="P5" s="324"/>
-      <c r="Q5" s="324"/>
-      <c r="R5" s="324"/>
-      <c r="S5" s="324"/>
-      <c r="T5" s="324"/>
-      <c r="U5" s="324"/>
-      <c r="V5" s="324"/>
-      <c r="W5" s="324"/>
+      <c r="N5" s="313"/>
+      <c r="O5" s="313"/>
+      <c r="P5" s="313"/>
+      <c r="Q5" s="313"/>
+      <c r="R5" s="313"/>
+      <c r="S5" s="313"/>
+      <c r="T5" s="313"/>
+      <c r="U5" s="313"/>
+      <c r="V5" s="313"/>
+      <c r="W5" s="313"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="324"/>
-      <c r="B6" s="324"/>
-      <c r="C6" s="324"/>
-      <c r="D6" s="324"/>
-      <c r="E6" s="324"/>
-      <c r="F6" s="324"/>
-      <c r="G6" s="324"/>
-      <c r="H6" s="324"/>
-      <c r="I6" s="324"/>
-      <c r="J6" s="324"/>
-      <c r="K6" s="324"/>
-      <c r="M6" s="324"/>
-      <c r="N6" s="324"/>
-      <c r="O6" s="324"/>
-      <c r="P6" s="324"/>
-      <c r="Q6" s="324"/>
-      <c r="R6" s="324"/>
-      <c r="S6" s="324"/>
-      <c r="T6" s="324"/>
-      <c r="U6" s="324"/>
-      <c r="V6" s="324"/>
-      <c r="W6" s="324"/>
+      <c r="A6" s="313"/>
+      <c r="B6" s="313"/>
+      <c r="C6" s="313"/>
+      <c r="D6" s="313"/>
+      <c r="E6" s="313"/>
+      <c r="F6" s="313"/>
+      <c r="G6" s="313"/>
+      <c r="H6" s="313"/>
+      <c r="I6" s="313"/>
+      <c r="J6" s="313"/>
+      <c r="K6" s="313"/>
+      <c r="M6" s="313"/>
+      <c r="N6" s="313"/>
+      <c r="O6" s="313"/>
+      <c r="P6" s="313"/>
+      <c r="Q6" s="313"/>
+      <c r="R6" s="313"/>
+      <c r="S6" s="313"/>
+      <c r="T6" s="313"/>
+      <c r="U6" s="313"/>
+      <c r="V6" s="313"/>
+      <c r="W6" s="313"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M7" s="249"/>
@@ -15954,27 +15976,27 @@
       <c r="W34" s="249"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B35" s="332" t="s">
+      <c r="B35" s="333" t="s">
         <v>312</v>
       </c>
-      <c r="C35" s="333"/>
-      <c r="D35" s="334"/>
-      <c r="E35" s="328">
+      <c r="C35" s="334"/>
+      <c r="D35" s="335"/>
+      <c r="E35" s="329">
         <f>E34-F34</f>
         <v>2610871.1799999997</v>
       </c>
-      <c r="F35" s="329"/>
+      <c r="F35" s="330"/>
       <c r="M35" s="249"/>
-      <c r="N35" s="332" t="s">
+      <c r="N35" s="333" t="s">
         <v>312</v>
       </c>
-      <c r="O35" s="333"/>
-      <c r="P35" s="334"/>
-      <c r="Q35" s="328">
+      <c r="O35" s="334"/>
+      <c r="P35" s="335"/>
+      <c r="Q35" s="329">
         <f>Q34-R34</f>
         <v>1506144.27</v>
       </c>
-      <c r="R35" s="329"/>
+      <c r="R35" s="330"/>
       <c r="S35" s="249"/>
       <c r="T35" s="249"/>
       <c r="U35" s="249"/>
@@ -15982,17 +16004,17 @@
       <c r="W35" s="249"/>
     </row>
     <row r="36" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="335"/>
-      <c r="C36" s="336"/>
-      <c r="D36" s="337"/>
-      <c r="E36" s="330"/>
-      <c r="F36" s="331"/>
+      <c r="B36" s="336"/>
+      <c r="C36" s="337"/>
+      <c r="D36" s="338"/>
+      <c r="E36" s="331"/>
+      <c r="F36" s="332"/>
       <c r="M36" s="249"/>
-      <c r="N36" s="335"/>
-      <c r="O36" s="336"/>
-      <c r="P36" s="337"/>
-      <c r="Q36" s="330"/>
-      <c r="R36" s="331"/>
+      <c r="N36" s="336"/>
+      <c r="O36" s="337"/>
+      <c r="P36" s="338"/>
+      <c r="Q36" s="331"/>
+      <c r="R36" s="332"/>
       <c r="S36" s="249"/>
       <c r="T36" s="249"/>
       <c r="U36" s="249"/>
@@ -16016,10 +16038,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:V47"/>
+  <dimension ref="B3:V57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16057,19 +16079,19 @@
       <c r="G3" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I3" s="324" t="s">
+      <c r="I3" s="313" t="s">
         <v>366</v>
       </c>
-      <c r="J3" s="324"/>
-      <c r="K3" s="324"/>
-      <c r="L3" s="324"/>
-      <c r="M3" s="324"/>
-      <c r="N3" s="324"/>
-      <c r="O3" s="324"/>
-      <c r="P3" s="324"/>
-      <c r="Q3" s="324"/>
-      <c r="R3" s="324"/>
-      <c r="S3" s="324"/>
+      <c r="J3" s="313"/>
+      <c r="K3" s="313"/>
+      <c r="L3" s="313"/>
+      <c r="M3" s="313"/>
+      <c r="N3" s="313"/>
+      <c r="O3" s="313"/>
+      <c r="P3" s="313"/>
+      <c r="Q3" s="313"/>
+      <c r="R3" s="313"/>
+      <c r="S3" s="313"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="57">
@@ -16091,17 +16113,17 @@
         <f>IF(ISNUMBER(SEARCH("SENIOR DISKON",D4)),100000,IF(ISNUMBER(SEARCH("SENIOR",D4)),150000,IF(ISNUMBER(SEARCH("MABA",D4)),125000,0)))</f>
         <v>125000</v>
       </c>
-      <c r="I4" s="324"/>
-      <c r="J4" s="324"/>
-      <c r="K4" s="324"/>
-      <c r="L4" s="324"/>
-      <c r="M4" s="324"/>
-      <c r="N4" s="324"/>
-      <c r="O4" s="324"/>
-      <c r="P4" s="324"/>
-      <c r="Q4" s="324"/>
-      <c r="R4" s="324"/>
-      <c r="S4" s="324"/>
+      <c r="I4" s="313"/>
+      <c r="J4" s="313"/>
+      <c r="K4" s="313"/>
+      <c r="L4" s="313"/>
+      <c r="M4" s="313"/>
+      <c r="N4" s="313"/>
+      <c r="O4" s="313"/>
+      <c r="P4" s="313"/>
+      <c r="Q4" s="313"/>
+      <c r="R4" s="313"/>
+      <c r="S4" s="313"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="57">
@@ -16120,7 +16142,7 @@
         <v>377</v>
       </c>
       <c r="G5" s="56">
-        <f t="shared" ref="G5:G46" si="0">IF(ISNUMBER(SEARCH("SENIOR DISKON",D5)),100000,IF(ISNUMBER(SEARCH("SENIOR",D5)),150000,IF(ISNUMBER(SEARCH("MABA",D5)),125000,0)))</f>
+        <f t="shared" ref="G5:G56" si="0">IF(ISNUMBER(SEARCH("SENIOR DISKON",D5)),100000,IF(ISNUMBER(SEARCH("SENIOR",D5)),150000,IF(ISNUMBER(SEARCH("MABA",D5)),125000,0)))</f>
         <v>125000</v>
       </c>
       <c r="I5" s="277"/>
@@ -16172,15 +16194,15 @@
         <v>65</v>
       </c>
       <c r="O6" s="277"/>
-      <c r="P6" s="338" t="s">
+      <c r="P6" s="339" t="s">
         <v>368</v>
       </c>
-      <c r="Q6" s="339"/>
-      <c r="R6" s="339"/>
-      <c r="S6" s="339"/>
-      <c r="T6" s="339"/>
-      <c r="U6" s="339"/>
-      <c r="V6" s="339"/>
+      <c r="Q6" s="340"/>
+      <c r="R6" s="340"/>
+      <c r="S6" s="340"/>
+      <c r="T6" s="340"/>
+      <c r="U6" s="340"/>
+      <c r="V6" s="340"/>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="57">
@@ -16217,13 +16239,13 @@
       </c>
       <c r="N7" s="211"/>
       <c r="O7" s="277"/>
-      <c r="P7" s="339"/>
-      <c r="Q7" s="339"/>
-      <c r="R7" s="339"/>
-      <c r="S7" s="339"/>
-      <c r="T7" s="339"/>
-      <c r="U7" s="339"/>
-      <c r="V7" s="339"/>
+      <c r="P7" s="340"/>
+      <c r="Q7" s="340"/>
+      <c r="R7" s="340"/>
+      <c r="S7" s="340"/>
+      <c r="T7" s="340"/>
+      <c r="U7" s="340"/>
+      <c r="V7" s="340"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="57">
@@ -16260,13 +16282,13 @@
         <v>500000</v>
       </c>
       <c r="O8" s="277"/>
-      <c r="P8" s="339"/>
-      <c r="Q8" s="339"/>
-      <c r="R8" s="339"/>
-      <c r="S8" s="339"/>
-      <c r="T8" s="339"/>
-      <c r="U8" s="339"/>
-      <c r="V8" s="339"/>
+      <c r="P8" s="340"/>
+      <c r="Q8" s="340"/>
+      <c r="R8" s="340"/>
+      <c r="S8" s="340"/>
+      <c r="T8" s="340"/>
+      <c r="U8" s="340"/>
+      <c r="V8" s="340"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="57">
@@ -16299,18 +16321,18 @@
         <v>358</v>
       </c>
       <c r="M9" s="210">
-        <f>G47</f>
+        <f>G57</f>
         <v>5250000</v>
       </c>
       <c r="N9" s="210"/>
       <c r="O9" s="277"/>
-      <c r="P9" s="339"/>
-      <c r="Q9" s="339"/>
-      <c r="R9" s="339"/>
-      <c r="S9" s="339"/>
-      <c r="T9" s="339"/>
-      <c r="U9" s="339"/>
-      <c r="V9" s="339"/>
+      <c r="P9" s="340"/>
+      <c r="Q9" s="340"/>
+      <c r="R9" s="340"/>
+      <c r="S9" s="340"/>
+      <c r="T9" s="340"/>
+      <c r="U9" s="340"/>
+      <c r="V9" s="340"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="57">
@@ -16347,13 +16369,13 @@
         <v>1500</v>
       </c>
       <c r="O10" s="277"/>
-      <c r="P10" s="339"/>
-      <c r="Q10" s="339"/>
-      <c r="R10" s="339"/>
-      <c r="S10" s="339"/>
-      <c r="T10" s="339"/>
-      <c r="U10" s="339"/>
-      <c r="V10" s="339"/>
+      <c r="P10" s="340"/>
+      <c r="Q10" s="340"/>
+      <c r="R10" s="340"/>
+      <c r="S10" s="340"/>
+      <c r="T10" s="340"/>
+      <c r="U10" s="340"/>
+      <c r="V10" s="340"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" s="57">
@@ -16390,13 +16412,13 @@
         <v>25500</v>
       </c>
       <c r="O11" s="277"/>
-      <c r="P11" s="339"/>
-      <c r="Q11" s="339"/>
-      <c r="R11" s="339"/>
-      <c r="S11" s="339"/>
-      <c r="T11" s="339"/>
-      <c r="U11" s="339"/>
-      <c r="V11" s="339"/>
+      <c r="P11" s="340"/>
+      <c r="Q11" s="340"/>
+      <c r="R11" s="340"/>
+      <c r="S11" s="340"/>
+      <c r="T11" s="340"/>
+      <c r="U11" s="340"/>
+      <c r="V11" s="340"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="57">
@@ -16433,13 +16455,13 @@
         <v>13000</v>
       </c>
       <c r="O12" s="277"/>
-      <c r="P12" s="339"/>
-      <c r="Q12" s="339"/>
-      <c r="R12" s="339"/>
-      <c r="S12" s="339"/>
-      <c r="T12" s="339"/>
-      <c r="U12" s="339"/>
-      <c r="V12" s="339"/>
+      <c r="P12" s="340"/>
+      <c r="Q12" s="340"/>
+      <c r="R12" s="340"/>
+      <c r="S12" s="340"/>
+      <c r="T12" s="340"/>
+      <c r="U12" s="340"/>
+      <c r="V12" s="340"/>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="57">
@@ -16538,14 +16560,14 @@
       <c r="M15" s="210"/>
       <c r="N15" s="211"/>
       <c r="O15" s="277"/>
-      <c r="P15" s="343" t="s">
+      <c r="P15" s="344" t="s">
         <v>391</v>
       </c>
-      <c r="Q15" s="343"/>
-      <c r="R15" s="343"/>
-      <c r="S15" s="343"/>
-      <c r="T15" s="343"/>
-      <c r="U15" s="343"/>
+      <c r="Q15" s="344"/>
+      <c r="R15" s="344"/>
+      <c r="S15" s="344"/>
+      <c r="T15" s="344"/>
+      <c r="U15" s="344"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" s="57">
@@ -16576,12 +16598,12 @@
       <c r="M16" s="211"/>
       <c r="N16" s="210"/>
       <c r="O16" s="277"/>
-      <c r="P16" s="343"/>
-      <c r="Q16" s="343"/>
-      <c r="R16" s="343"/>
-      <c r="S16" s="343"/>
-      <c r="T16" s="343"/>
-      <c r="U16" s="343"/>
+      <c r="P16" s="344"/>
+      <c r="Q16" s="344"/>
+      <c r="R16" s="344"/>
+      <c r="S16" s="344"/>
+      <c r="T16" s="344"/>
+      <c r="U16" s="344"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="57">
@@ -16612,12 +16634,12 @@
       <c r="M17" s="211"/>
       <c r="N17" s="211"/>
       <c r="O17" s="277"/>
-      <c r="P17" s="343"/>
-      <c r="Q17" s="343"/>
-      <c r="R17" s="343"/>
-      <c r="S17" s="343"/>
-      <c r="T17" s="343"/>
-      <c r="U17" s="343"/>
+      <c r="P17" s="344"/>
+      <c r="Q17" s="344"/>
+      <c r="R17" s="344"/>
+      <c r="S17" s="344"/>
+      <c r="T17" s="344"/>
+      <c r="U17" s="344"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="57">
@@ -17160,16 +17182,16 @@
         <v>100000</v>
       </c>
       <c r="I33" s="277"/>
-      <c r="J33" s="332" t="s">
+      <c r="J33" s="333" t="s">
         <v>365</v>
       </c>
-      <c r="K33" s="333"/>
-      <c r="L33" s="334"/>
-      <c r="M33" s="328">
+      <c r="K33" s="334"/>
+      <c r="L33" s="335"/>
+      <c r="M33" s="329">
         <f>M32-N32</f>
         <v>6710000</v>
       </c>
-      <c r="N33" s="329"/>
+      <c r="N33" s="330"/>
       <c r="O33" s="277"/>
       <c r="P33" s="277"/>
       <c r="Q33" s="277"/>
@@ -17197,11 +17219,11 @@
         <v>150000</v>
       </c>
       <c r="I34" s="277"/>
-      <c r="J34" s="335"/>
-      <c r="K34" s="336"/>
-      <c r="L34" s="337"/>
-      <c r="M34" s="330"/>
-      <c r="N34" s="331"/>
+      <c r="J34" s="336"/>
+      <c r="K34" s="337"/>
+      <c r="L34" s="338"/>
+      <c r="M34" s="331"/>
+      <c r="N34" s="332"/>
       <c r="O34" s="277"/>
       <c r="P34" s="277"/>
       <c r="Q34" s="277"/>
@@ -17418,7 +17440,7 @@
         <v>125000</v>
       </c>
     </row>
-    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:19" s="285" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="57">
         <v>42</v>
       </c>
@@ -17431,29 +17453,159 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:19" s="285" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="57">
         <v>43</v>
       </c>
-      <c r="C46" s="141"/>
-      <c r="D46" s="141"/>
-      <c r="E46" s="141"/>
-      <c r="F46" s="141"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
       <c r="G46" s="56">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="340" t="s">
+    <row r="47" spans="2:19" s="285" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="57">
+        <v>44</v>
+      </c>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:19" s="285" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="57">
+        <v>45</v>
+      </c>
+      <c r="C48" s="57"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" s="285" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="57">
+        <v>46</v>
+      </c>
+      <c r="C49" s="57"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" s="285" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="57">
+        <v>47</v>
+      </c>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" s="285" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="57">
+        <v>48</v>
+      </c>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" s="285" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="57">
+        <v>49</v>
+      </c>
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" s="285" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="57">
+        <v>50</v>
+      </c>
+      <c r="C53" s="57"/>
+      <c r="D53" s="57"/>
+      <c r="E53" s="57"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" s="285" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="57">
+        <v>51</v>
+      </c>
+      <c r="C54" s="57"/>
+      <c r="D54" s="57"/>
+      <c r="E54" s="57"/>
+      <c r="F54" s="57"/>
+      <c r="G54" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="57">
+        <v>52</v>
+      </c>
+      <c r="C55" s="57"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="57"/>
+      <c r="G55" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="57">
+        <v>53</v>
+      </c>
+      <c r="C56" s="141"/>
+      <c r="D56" s="141"/>
+      <c r="E56" s="141"/>
+      <c r="F56" s="141"/>
+      <c r="G56" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="341" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="341"/>
-      <c r="D47" s="341"/>
-      <c r="E47" s="341"/>
-      <c r="F47" s="342"/>
-      <c r="G47" s="282">
-        <f>SUM(G4:G46)</f>
+      <c r="C57" s="342"/>
+      <c r="D57" s="342"/>
+      <c r="E57" s="342"/>
+      <c r="F57" s="343"/>
+      <c r="G57" s="282">
+        <f>SUM(G4:G56)</f>
         <v>5250000</v>
       </c>
     </row>
@@ -17463,44 +17615,44 @@
     <mergeCell ref="M33:N34"/>
     <mergeCell ref="I3:S4"/>
     <mergeCell ref="P6:V12"/>
-    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B57:F57"/>
     <mergeCell ref="P15:U17"/>
   </mergeCells>
-  <conditionalFormatting sqref="D4:D46">
+  <conditionalFormatting sqref="D4:D56">
     <cfRule type="expression" priority="5">
-      <formula>IF(ISNUMBER(SEARCH("SENIOR DISKON",$G$4:$G$46)),"100000",IF(ISNUMBER(SEARCH("SENIOR",$G$4:$G$46)),"150000","125000"))</formula>
+      <formula>IF(ISNUMBER(SEARCH("SENIOR DISKON",$G$4:$G$56)),"100000",IF(ISNUMBER(SEARCH("SENIOR",$G$4:$G$56)),"150000","125000"))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="SENIOR DISKON">
+    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="SENIOR DISKON">
       <formula>NOT(ISERROR(SEARCH("SENIOR DISKON",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="SENIOR">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="SENIOR">
       <formula>NOT(ISERROR(SEARCH("SENIOR",D4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="MABA">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="MABA">
       <formula>NOT(ISERROR(SEARCH("MABA",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:F46">
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Tunai">
+  <conditionalFormatting sqref="E4:F56">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Tunai">
       <formula>NOT(ISERROR(SEARCH("Tunai",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Transfer">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Transfer">
       <formula>NOT(ISERROR(SEARCH("Transfer",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G46">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+  <conditionalFormatting sqref="G4:G56">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>150000</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>100000</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>125000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F46">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="F4:F56">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"LUNAS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17536,17 +17688,17 @@
       <c r="A2" s="172"/>
       <c r="B2" s="173"/>
       <c r="C2" s="173"/>
-      <c r="D2" s="344" t="s">
+      <c r="D2" s="402" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="344"/>
-      <c r="F2" s="344"/>
-      <c r="G2" s="344"/>
-      <c r="H2" s="344"/>
-      <c r="I2" s="344"/>
-      <c r="J2" s="344"/>
-      <c r="K2" s="344"/>
-      <c r="L2" s="344"/>
+      <c r="E2" s="402"/>
+      <c r="F2" s="402"/>
+      <c r="G2" s="402"/>
+      <c r="H2" s="402"/>
+      <c r="I2" s="402"/>
+      <c r="J2" s="402"/>
+      <c r="K2" s="402"/>
+      <c r="L2" s="402"/>
       <c r="M2" s="174"/>
       <c r="N2" s="24"/>
     </row>
@@ -17564,205 +17716,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="176"/>
-      <c r="U3" s="394" t="s">
+      <c r="U3" s="345" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="395"/>
-      <c r="W3" s="396" t="s">
+      <c r="V3" s="346"/>
+      <c r="W3" s="347" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="395"/>
-      <c r="Y3" s="395"/>
-      <c r="Z3" s="395"/>
-      <c r="AA3" s="395"/>
-      <c r="AB3" s="395"/>
-      <c r="AC3" s="395"/>
-      <c r="AD3" s="397"/>
+      <c r="X3" s="346"/>
+      <c r="Y3" s="346"/>
+      <c r="Z3" s="346"/>
+      <c r="AA3" s="346"/>
+      <c r="AB3" s="346"/>
+      <c r="AC3" s="346"/>
+      <c r="AD3" s="348"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="175"/>
-      <c r="B4" s="359" t="s">
+      <c r="B4" s="406" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="360"/>
-      <c r="F4" s="360"/>
+      <c r="C4" s="407"/>
+      <c r="D4" s="407"/>
+      <c r="E4" s="407"/>
+      <c r="F4" s="407"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="363" t="s">
+      <c r="I4" s="354" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="315"/>
-      <c r="K4" s="315"/>
-      <c r="L4" s="315"/>
+      <c r="J4" s="319"/>
+      <c r="K4" s="319"/>
+      <c r="L4" s="319"/>
       <c r="M4" s="176"/>
-      <c r="U4" s="406" t="s">
+      <c r="U4" s="366" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="315"/>
-      <c r="W4" s="363" t="s">
+      <c r="V4" s="319"/>
+      <c r="W4" s="354" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="315"/>
-      <c r="Y4" s="315"/>
-      <c r="Z4" s="315"/>
-      <c r="AA4" s="315"/>
-      <c r="AB4" s="315"/>
-      <c r="AC4" s="315"/>
-      <c r="AD4" s="383"/>
+      <c r="X4" s="319"/>
+      <c r="Y4" s="319"/>
+      <c r="Z4" s="319"/>
+      <c r="AA4" s="319"/>
+      <c r="AB4" s="319"/>
+      <c r="AC4" s="319"/>
+      <c r="AD4" s="349"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="175"/>
-      <c r="B5" s="354" t="s">
+      <c r="B5" s="371" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="315"/>
-      <c r="D5" s="315"/>
-      <c r="E5" s="315"/>
-      <c r="F5" s="315"/>
+      <c r="C5" s="319"/>
+      <c r="D5" s="319"/>
+      <c r="E5" s="319"/>
+      <c r="F5" s="319"/>
       <c r="G5" s="152">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="352" t="s">
+      <c r="I5" s="373" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="353"/>
-      <c r="K5" s="364">
+      <c r="J5" s="394"/>
+      <c r="K5" s="396">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="365"/>
+      <c r="L5" s="397"/>
       <c r="M5" s="176"/>
-      <c r="U5" s="390" t="s">
+      <c r="U5" s="367" t="s">
         <v>231</v>
       </c>
-      <c r="V5" s="391"/>
-      <c r="W5" s="352" t="s">
+      <c r="V5" s="368"/>
+      <c r="W5" s="373" t="s">
         <v>232</v>
       </c>
-      <c r="X5" s="377"/>
-      <c r="Y5" s="377"/>
-      <c r="Z5" s="377"/>
-      <c r="AA5" s="377"/>
-      <c r="AB5" s="377"/>
-      <c r="AC5" s="377"/>
-      <c r="AD5" s="378"/>
+      <c r="X5" s="374"/>
+      <c r="Y5" s="374"/>
+      <c r="Z5" s="374"/>
+      <c r="AA5" s="374"/>
+      <c r="AB5" s="374"/>
+      <c r="AC5" s="374"/>
+      <c r="AD5" s="375"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="175"/>
-      <c r="B6" s="346" t="s">
+      <c r="B6" s="364" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="347"/>
-      <c r="D6" s="347"/>
-      <c r="E6" s="347"/>
-      <c r="F6" s="347"/>
+      <c r="C6" s="365"/>
+      <c r="D6" s="365"/>
+      <c r="E6" s="365"/>
+      <c r="F6" s="365"/>
       <c r="G6" s="152">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="350" t="s">
+      <c r="I6" s="395" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="351"/>
-      <c r="K6" s="366">
+      <c r="J6" s="390"/>
+      <c r="K6" s="398">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="367"/>
+      <c r="L6" s="399"/>
       <c r="M6" s="176"/>
-      <c r="U6" s="392"/>
-      <c r="V6" s="393"/>
-      <c r="W6" s="379" t="s">
+      <c r="U6" s="369"/>
+      <c r="V6" s="370"/>
+      <c r="W6" s="355" t="s">
         <v>233</v>
       </c>
-      <c r="X6" s="380"/>
-      <c r="Y6" s="380"/>
-      <c r="Z6" s="380"/>
-      <c r="AA6" s="380"/>
-      <c r="AB6" s="380"/>
-      <c r="AC6" s="380"/>
-      <c r="AD6" s="381"/>
+      <c r="X6" s="356"/>
+      <c r="Y6" s="356"/>
+      <c r="Z6" s="356"/>
+      <c r="AA6" s="356"/>
+      <c r="AB6" s="356"/>
+      <c r="AC6" s="356"/>
+      <c r="AD6" s="357"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="175"/>
-      <c r="B7" s="357" t="s">
+      <c r="B7" s="376" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="358"/>
-      <c r="D7" s="358"/>
-      <c r="E7" s="358"/>
-      <c r="F7" s="351"/>
+      <c r="C7" s="377"/>
+      <c r="D7" s="377"/>
+      <c r="E7" s="377"/>
+      <c r="F7" s="390"/>
       <c r="G7" s="152">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="350" t="s">
+      <c r="I7" s="395" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="351"/>
-      <c r="K7" s="361">
+      <c r="J7" s="390"/>
+      <c r="K7" s="400">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="362"/>
+      <c r="L7" s="401"/>
       <c r="M7" s="176"/>
-      <c r="U7" s="398"/>
-      <c r="V7" s="399"/>
-      <c r="W7" s="363" t="s">
+      <c r="U7" s="352"/>
+      <c r="V7" s="353"/>
+      <c r="W7" s="354" t="s">
         <v>234</v>
       </c>
-      <c r="X7" s="315"/>
-      <c r="Y7" s="315"/>
-      <c r="Z7" s="315"/>
-      <c r="AA7" s="315"/>
-      <c r="AB7" s="315"/>
-      <c r="AC7" s="315"/>
-      <c r="AD7" s="383"/>
+      <c r="X7" s="319"/>
+      <c r="Y7" s="319"/>
+      <c r="Z7" s="319"/>
+      <c r="AA7" s="319"/>
+      <c r="AB7" s="319"/>
+      <c r="AC7" s="319"/>
+      <c r="AD7" s="349"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="175"/>
-      <c r="B8" s="355" t="s">
+      <c r="B8" s="404" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="356"/>
-      <c r="D8" s="356"/>
-      <c r="E8" s="356"/>
-      <c r="F8" s="356"/>
+      <c r="C8" s="405"/>
+      <c r="D8" s="405"/>
+      <c r="E8" s="405"/>
+      <c r="F8" s="405"/>
       <c r="G8" s="153">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="352" t="s">
+      <c r="I8" s="373" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="353"/>
-      <c r="K8" s="348">
+      <c r="J8" s="394"/>
+      <c r="K8" s="385">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="349"/>
+      <c r="L8" s="386"/>
       <c r="M8" s="176"/>
-      <c r="U8" s="402" t="s">
+      <c r="U8" s="360" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="403"/>
-      <c r="W8" s="379" t="s">
+      <c r="V8" s="361"/>
+      <c r="W8" s="355" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="380"/>
-      <c r="Y8" s="380"/>
-      <c r="Z8" s="380"/>
-      <c r="AA8" s="380"/>
-      <c r="AB8" s="380"/>
-      <c r="AC8" s="380"/>
-      <c r="AD8" s="381"/>
+      <c r="X8" s="356"/>
+      <c r="Y8" s="356"/>
+      <c r="Z8" s="356"/>
+      <c r="AA8" s="356"/>
+      <c r="AB8" s="356"/>
+      <c r="AC8" s="356"/>
+      <c r="AD8" s="357"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="175"/>
@@ -17778,28 +17930,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="176"/>
-      <c r="U9" s="404"/>
-      <c r="V9" s="405"/>
-      <c r="W9" s="379" t="s">
+      <c r="U9" s="362"/>
+      <c r="V9" s="363"/>
+      <c r="W9" s="355" t="s">
         <v>237</v>
       </c>
-      <c r="X9" s="380"/>
-      <c r="Y9" s="380"/>
-      <c r="Z9" s="380"/>
-      <c r="AA9" s="380"/>
-      <c r="AB9" s="380"/>
-      <c r="AC9" s="380"/>
-      <c r="AD9" s="381"/>
+      <c r="X9" s="356"/>
+      <c r="Y9" s="356"/>
+      <c r="Z9" s="356"/>
+      <c r="AA9" s="356"/>
+      <c r="AB9" s="356"/>
+      <c r="AC9" s="356"/>
+      <c r="AD9" s="357"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="175"/>
-      <c r="B10" s="315" t="s">
+      <c r="B10" s="319" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="315"/>
-      <c r="D10" s="315"/>
-      <c r="E10" s="315"/>
-      <c r="F10" s="315"/>
+      <c r="C10" s="319"/>
+      <c r="D10" s="319"/>
+      <c r="E10" s="319"/>
+      <c r="F10" s="319"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -17810,30 +17962,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="176"/>
-      <c r="U10" s="346" t="s">
+      <c r="U10" s="364" t="s">
         <v>243</v>
       </c>
-      <c r="V10" s="347"/>
-      <c r="W10" s="315" t="s">
+      <c r="V10" s="365"/>
+      <c r="W10" s="319" t="s">
         <v>257</v>
       </c>
-      <c r="X10" s="315"/>
-      <c r="Y10" s="315"/>
-      <c r="Z10" s="315"/>
-      <c r="AA10" s="315"/>
-      <c r="AB10" s="315"/>
-      <c r="AC10" s="315"/>
-      <c r="AD10" s="383"/>
+      <c r="X10" s="319"/>
+      <c r="Y10" s="319"/>
+      <c r="Z10" s="319"/>
+      <c r="AA10" s="319"/>
+      <c r="AB10" s="319"/>
+      <c r="AC10" s="319"/>
+      <c r="AD10" s="349"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="175"/>
-      <c r="B11" s="315" t="s">
+      <c r="B11" s="319" t="s">
         <v>254</v>
       </c>
-      <c r="C11" s="315"/>
-      <c r="D11" s="315"/>
-      <c r="E11" s="315"/>
-      <c r="F11" s="315"/>
+      <c r="C11" s="319"/>
+      <c r="D11" s="319"/>
+      <c r="E11" s="319"/>
+      <c r="F11" s="319"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -17843,30 +17995,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="176"/>
-      <c r="U11" s="346" t="s">
+      <c r="U11" s="364" t="s">
         <v>256</v>
       </c>
-      <c r="V11" s="347"/>
-      <c r="W11" s="400" t="s">
+      <c r="V11" s="365"/>
+      <c r="W11" s="358" t="s">
         <v>258</v>
       </c>
-      <c r="X11" s="400"/>
-      <c r="Y11" s="400"/>
-      <c r="Z11" s="400"/>
-      <c r="AA11" s="400"/>
-      <c r="AB11" s="400"/>
-      <c r="AC11" s="400"/>
-      <c r="AD11" s="401"/>
+      <c r="X11" s="358"/>
+      <c r="Y11" s="358"/>
+      <c r="Z11" s="358"/>
+      <c r="AA11" s="358"/>
+      <c r="AB11" s="358"/>
+      <c r="AC11" s="358"/>
+      <c r="AD11" s="359"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="175"/>
-      <c r="B12" s="345" t="s">
+      <c r="B12" s="403" t="s">
         <v>255</v>
       </c>
-      <c r="C12" s="345"/>
-      <c r="D12" s="345"/>
-      <c r="E12" s="345"/>
-      <c r="F12" s="345"/>
+      <c r="C12" s="403"/>
+      <c r="D12" s="403"/>
+      <c r="E12" s="403"/>
+      <c r="F12" s="403"/>
       <c r="G12" s="180">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -17877,16 +18029,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="176"/>
-      <c r="U12" s="346"/>
-      <c r="V12" s="347"/>
-      <c r="W12" s="315"/>
-      <c r="X12" s="315"/>
-      <c r="Y12" s="315"/>
-      <c r="Z12" s="315"/>
-      <c r="AA12" s="315"/>
-      <c r="AB12" s="315"/>
-      <c r="AC12" s="315"/>
-      <c r="AD12" s="383"/>
+      <c r="U12" s="364"/>
+      <c r="V12" s="365"/>
+      <c r="W12" s="319"/>
+      <c r="X12" s="319"/>
+      <c r="Y12" s="319"/>
+      <c r="Z12" s="319"/>
+      <c r="AA12" s="319"/>
+      <c r="AB12" s="319"/>
+      <c r="AC12" s="319"/>
+      <c r="AD12" s="349"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="177"/>
@@ -17902,64 +18054,64 @@
       <c r="K13" s="178"/>
       <c r="L13" s="178"/>
       <c r="M13" s="179"/>
-      <c r="U13" s="346"/>
-      <c r="V13" s="347"/>
-      <c r="W13" s="315"/>
-      <c r="X13" s="315"/>
-      <c r="Y13" s="315"/>
-      <c r="Z13" s="315"/>
-      <c r="AA13" s="315"/>
-      <c r="AB13" s="315"/>
-      <c r="AC13" s="315"/>
-      <c r="AD13" s="383"/>
+      <c r="U13" s="364"/>
+      <c r="V13" s="365"/>
+      <c r="W13" s="319"/>
+      <c r="X13" s="319"/>
+      <c r="Y13" s="319"/>
+      <c r="Z13" s="319"/>
+      <c r="AA13" s="319"/>
+      <c r="AB13" s="319"/>
+      <c r="AC13" s="319"/>
+      <c r="AD13" s="349"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="U14" s="384"/>
-      <c r="V14" s="385"/>
-      <c r="W14" s="375"/>
-      <c r="X14" s="375"/>
-      <c r="Y14" s="375"/>
-      <c r="Z14" s="375"/>
-      <c r="AA14" s="375"/>
-      <c r="AB14" s="375"/>
-      <c r="AC14" s="375"/>
-      <c r="AD14" s="376"/>
+      <c r="U14" s="379"/>
+      <c r="V14" s="380"/>
+      <c r="W14" s="350"/>
+      <c r="X14" s="350"/>
+      <c r="Y14" s="350"/>
+      <c r="Z14" s="350"/>
+      <c r="AA14" s="350"/>
+      <c r="AB14" s="350"/>
+      <c r="AC14" s="350"/>
+      <c r="AD14" s="351"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="172"/>
       <c r="B18" s="173"/>
       <c r="C18" s="173"/>
-      <c r="D18" s="344" t="s">
+      <c r="D18" s="402" t="s">
         <v>249</v>
       </c>
-      <c r="E18" s="344"/>
-      <c r="F18" s="344"/>
-      <c r="G18" s="344"/>
-      <c r="H18" s="344"/>
-      <c r="I18" s="344"/>
-      <c r="J18" s="344"/>
-      <c r="K18" s="344"/>
-      <c r="L18" s="344"/>
+      <c r="E18" s="402"/>
+      <c r="F18" s="402"/>
+      <c r="G18" s="402"/>
+      <c r="H18" s="402"/>
+      <c r="I18" s="402"/>
+      <c r="J18" s="402"/>
+      <c r="K18" s="402"/>
+      <c r="L18" s="402"/>
       <c r="M18" s="174"/>
-      <c r="O18" s="386" t="s">
+      <c r="O18" s="381" t="s">
         <v>250</v>
       </c>
-      <c r="P18" s="387"/>
-      <c r="Q18" s="387"/>
-      <c r="R18" s="387"/>
-      <c r="S18" s="388"/>
+      <c r="P18" s="382"/>
+      <c r="Q18" s="382"/>
+      <c r="R18" s="382"/>
+      <c r="S18" s="383"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="175"/>
       <c r="M19" s="176"/>
-      <c r="O19" s="354" t="s">
+      <c r="O19" s="371" t="s">
         <v>251</v>
       </c>
-      <c r="P19" s="315"/>
-      <c r="Q19" s="315"/>
-      <c r="R19" s="315"/>
-      <c r="S19" s="383"/>
+      <c r="P19" s="319"/>
+      <c r="Q19" s="319"/>
+      <c r="R19" s="319"/>
+      <c r="S19" s="349"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="175"/>
@@ -17970,119 +18122,119 @@
       <c r="F20" s="200"/>
       <c r="G20" s="68"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="363" t="s">
+      <c r="I20" s="354" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="315"/>
-      <c r="K20" s="315"/>
-      <c r="L20" s="315"/>
+      <c r="J20" s="319"/>
+      <c r="K20" s="319"/>
+      <c r="L20" s="319"/>
       <c r="M20" s="176"/>
-      <c r="O20" s="354" t="s">
+      <c r="O20" s="371" t="s">
         <v>252</v>
       </c>
-      <c r="P20" s="315"/>
-      <c r="Q20" s="315"/>
-      <c r="R20" s="315"/>
-      <c r="S20" s="383"/>
+      <c r="P20" s="319"/>
+      <c r="Q20" s="319"/>
+      <c r="R20" s="319"/>
+      <c r="S20" s="349"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="175"/>
-      <c r="B21" s="368" t="s">
+      <c r="B21" s="387" t="s">
         <v>296</v>
       </c>
-      <c r="C21" s="369"/>
-      <c r="D21" s="369"/>
-      <c r="E21" s="369"/>
-      <c r="F21" s="370"/>
+      <c r="C21" s="388"/>
+      <c r="D21" s="388"/>
+      <c r="E21" s="388"/>
+      <c r="F21" s="389"/>
       <c r="G21" s="70">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="352" t="s">
+      <c r="I21" s="373" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="353"/>
-      <c r="K21" s="364">
+      <c r="J21" s="394"/>
+      <c r="K21" s="396">
         <f>G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="L21" s="365"/>
+      <c r="L21" s="397"/>
       <c r="M21" s="176"/>
       <c r="N21" s="170"/>
-      <c r="O21" s="389" t="s">
+      <c r="O21" s="384" t="s">
         <v>259</v>
       </c>
-      <c r="P21" s="377"/>
-      <c r="Q21" s="377"/>
-      <c r="R21" s="377"/>
-      <c r="S21" s="378"/>
+      <c r="P21" s="374"/>
+      <c r="Q21" s="374"/>
+      <c r="R21" s="374"/>
+      <c r="S21" s="375"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="175"/>
-      <c r="B22" s="357" t="s">
+      <c r="B22" s="376" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="358"/>
-      <c r="D22" s="358"/>
-      <c r="E22" s="358"/>
-      <c r="F22" s="351"/>
+      <c r="C22" s="377"/>
+      <c r="D22" s="377"/>
+      <c r="E22" s="377"/>
+      <c r="F22" s="390"/>
       <c r="G22" s="152">
         <f>G21</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="350" t="s">
+      <c r="I22" s="395" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="351"/>
-      <c r="K22" s="366">
+      <c r="J22" s="390"/>
+      <c r="K22" s="398">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="L22" s="367"/>
+      <c r="L22" s="399"/>
       <c r="M22" s="176"/>
       <c r="N22" s="170"/>
-      <c r="O22" s="357" t="s">
+      <c r="O22" s="376" t="s">
         <v>260</v>
       </c>
-      <c r="P22" s="358"/>
-      <c r="Q22" s="358"/>
-      <c r="R22" s="358"/>
-      <c r="S22" s="382"/>
+      <c r="P22" s="377"/>
+      <c r="Q22" s="377"/>
+      <c r="R22" s="377"/>
+      <c r="S22" s="378"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="175"/>
-      <c r="B23" s="371" t="s">
+      <c r="B23" s="391" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="372"/>
-      <c r="D23" s="372"/>
-      <c r="E23" s="372"/>
-      <c r="F23" s="373"/>
+      <c r="C23" s="392"/>
+      <c r="D23" s="392"/>
+      <c r="E23" s="392"/>
+      <c r="F23" s="393"/>
       <c r="G23" s="153">
         <f>K24</f>
         <v>1568729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="350" t="s">
+      <c r="I23" s="395" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="351"/>
-      <c r="K23" s="361">
+      <c r="J23" s="390"/>
+      <c r="K23" s="400">
         <f>Pemasukkan!L31</f>
         <v>690000</v>
       </c>
-      <c r="L23" s="362"/>
+      <c r="L23" s="401"/>
       <c r="M23" s="176"/>
       <c r="N23" s="170"/>
-      <c r="O23" s="357" t="s">
+      <c r="O23" s="376" t="s">
         <v>261</v>
       </c>
-      <c r="P23" s="358"/>
-      <c r="Q23" s="358"/>
-      <c r="R23" s="358"/>
-      <c r="S23" s="382"/>
+      <c r="P23" s="377"/>
+      <c r="Q23" s="377"/>
+      <c r="R23" s="377"/>
+      <c r="S23" s="378"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="175"/>
@@ -18093,24 +18245,24 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="352" t="s">
+      <c r="I24" s="373" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="353"/>
-      <c r="K24" s="348">
+      <c r="J24" s="394"/>
+      <c r="K24" s="385">
         <f>(K21-K22)+K23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="L24" s="349"/>
+      <c r="L24" s="386"/>
       <c r="M24" s="176"/>
       <c r="N24" s="170"/>
-      <c r="O24" s="357" t="s">
+      <c r="O24" s="376" t="s">
         <v>262</v>
       </c>
-      <c r="P24" s="358"/>
-      <c r="Q24" s="358"/>
-      <c r="R24" s="358"/>
-      <c r="S24" s="382"/>
+      <c r="P24" s="377"/>
+      <c r="Q24" s="377"/>
+      <c r="R24" s="377"/>
+      <c r="S24" s="378"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="175"/>
@@ -18127,13 +18279,13 @@
       <c r="L25" s="24"/>
       <c r="M25" s="176"/>
       <c r="N25" s="170"/>
-      <c r="O25" s="354" t="s">
+      <c r="O25" s="371" t="s">
         <v>267</v>
       </c>
-      <c r="P25" s="315"/>
-      <c r="Q25" s="315"/>
-      <c r="R25" s="315"/>
-      <c r="S25" s="383"/>
+      <c r="P25" s="319"/>
+      <c r="Q25" s="319"/>
+      <c r="R25" s="319"/>
+      <c r="S25" s="349"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="175"/>
@@ -18150,11 +18302,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="176"/>
       <c r="N26" s="170"/>
-      <c r="O26" s="374"/>
-      <c r="P26" s="375"/>
-      <c r="Q26" s="375"/>
-      <c r="R26" s="375"/>
-      <c r="S26" s="376"/>
+      <c r="O26" s="372"/>
+      <c r="P26" s="350"/>
+      <c r="Q26" s="350"/>
+      <c r="R26" s="350"/>
+      <c r="S26" s="351"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="177"/>
@@ -18189,6 +18341,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="D18:L18"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="W5:AD5"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="O18:S18"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O23:S23"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="W4:AD4"/>
+    <mergeCell ref="W8:AD8"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="O25:S25"/>
     <mergeCell ref="U3:V3"/>
     <mergeCell ref="W3:AD3"/>
     <mergeCell ref="W12:AD12"/>
@@ -18205,53 +18404,6 @@
     <mergeCell ref="U12:V12"/>
     <mergeCell ref="U13:V13"/>
     <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:AD4"/>
-    <mergeCell ref="W8:AD8"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="O25:S25"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="W5:AD5"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="O24:S24"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="O18:S18"/>
-    <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O23:S23"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="D18:L18"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -18285,44 +18437,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="407" t="s">
+      <c r="C2" s="417" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="408"/>
-      <c r="E2" s="408"/>
-      <c r="F2" s="408"/>
-      <c r="G2" s="408"/>
-      <c r="H2" s="408"/>
-      <c r="I2" s="408"/>
-      <c r="J2" s="408"/>
-      <c r="K2" s="408"/>
+      <c r="D2" s="418"/>
+      <c r="E2" s="418"/>
+      <c r="F2" s="418"/>
+      <c r="G2" s="418"/>
+      <c r="H2" s="418"/>
+      <c r="I2" s="418"/>
+      <c r="J2" s="418"/>
+      <c r="K2" s="418"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="408"/>
-      <c r="D3" s="408"/>
-      <c r="E3" s="408"/>
-      <c r="F3" s="408"/>
-      <c r="G3" s="408"/>
-      <c r="H3" s="408"/>
-      <c r="I3" s="408"/>
-      <c r="J3" s="408"/>
-      <c r="K3" s="408"/>
+      <c r="C3" s="418"/>
+      <c r="D3" s="418"/>
+      <c r="E3" s="418"/>
+      <c r="F3" s="418"/>
+      <c r="G3" s="418"/>
+      <c r="H3" s="418"/>
+      <c r="I3" s="418"/>
+      <c r="J3" s="418"/>
+      <c r="K3" s="418"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="415" t="s">
+      <c r="C5" s="410" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="415"/>
-      <c r="E5" s="415"/>
-      <c r="F5" s="415"/>
-      <c r="G5" s="415"/>
-      <c r="I5" s="415" t="s">
+      <c r="D5" s="410"/>
+      <c r="E5" s="410"/>
+      <c r="F5" s="410"/>
+      <c r="G5" s="410"/>
+      <c r="I5" s="410" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="415"/>
-      <c r="K5" s="415"/>
-      <c r="L5" s="415"/>
-      <c r="M5" s="415"/>
+      <c r="J5" s="410"/>
+      <c r="K5" s="410"/>
+      <c r="L5" s="410"/>
+      <c r="M5" s="410"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -18762,88 +18914,88 @@
       <c r="M28" s="170"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="359" t="s">
+      <c r="D29" s="406" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="360"/>
-      <c r="F29" s="409">
+      <c r="E29" s="407"/>
+      <c r="F29" s="411">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="410"/>
+      <c r="G29" s="412"/>
       <c r="I29" s="170"/>
-      <c r="J29" s="359" t="s">
+      <c r="J29" s="406" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="360"/>
-      <c r="L29" s="409">
+      <c r="K29" s="407"/>
+      <c r="L29" s="411">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="410"/>
+      <c r="M29" s="412"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="406" t="s">
+      <c r="D30" s="366" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="315"/>
-      <c r="F30" s="411">
+      <c r="E30" s="319"/>
+      <c r="F30" s="413">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="412"/>
+      <c r="G30" s="414"/>
       <c r="I30" s="170"/>
-      <c r="J30" s="406" t="s">
+      <c r="J30" s="366" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="315"/>
-      <c r="L30" s="411">
+      <c r="K30" s="319"/>
+      <c r="L30" s="413">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="412"/>
+      <c r="M30" s="414"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="354" t="s">
+      <c r="D31" s="371" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="315"/>
-      <c r="F31" s="416">
+      <c r="E31" s="319"/>
+      <c r="F31" s="415">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="417"/>
+      <c r="G31" s="416"/>
       <c r="I31" s="170"/>
-      <c r="J31" s="354" t="s">
+      <c r="J31" s="371" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="315"/>
-      <c r="L31" s="416">
+      <c r="K31" s="319"/>
+      <c r="L31" s="415">
         <f>L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="417"/>
+      <c r="M31" s="416"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="355" t="s">
+      <c r="D32" s="404" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="356"/>
-      <c r="F32" s="413">
+      <c r="E32" s="405"/>
+      <c r="F32" s="408">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="414"/>
+      <c r="G32" s="409"/>
       <c r="I32" s="170"/>
-      <c r="J32" s="355" t="s">
+      <c r="J32" s="404" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="356"/>
-      <c r="L32" s="413">
+      <c r="K32" s="405"/>
+      <c r="L32" s="408">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="414"/>
+      <c r="M32" s="409"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19035,6 +19187,12 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C2:K3"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J29:K29"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="I5:M5"/>
@@ -19048,12 +19206,6 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J32:K32"/>
-    <mergeCell ref="C2:K3"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -19086,44 +19238,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="418" t="s">
+      <c r="C2" s="423" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="419"/>
-      <c r="E2" s="419"/>
-      <c r="F2" s="419"/>
-      <c r="G2" s="419"/>
-      <c r="H2" s="419"/>
-      <c r="I2" s="419"/>
-      <c r="J2" s="419"/>
-      <c r="K2" s="419"/>
+      <c r="D2" s="424"/>
+      <c r="E2" s="424"/>
+      <c r="F2" s="424"/>
+      <c r="G2" s="424"/>
+      <c r="H2" s="424"/>
+      <c r="I2" s="424"/>
+      <c r="J2" s="424"/>
+      <c r="K2" s="424"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="419"/>
-      <c r="D3" s="419"/>
-      <c r="E3" s="419"/>
-      <c r="F3" s="419"/>
-      <c r="G3" s="419"/>
-      <c r="H3" s="419"/>
-      <c r="I3" s="419"/>
-      <c r="J3" s="419"/>
-      <c r="K3" s="419"/>
+      <c r="C3" s="424"/>
+      <c r="D3" s="424"/>
+      <c r="E3" s="424"/>
+      <c r="F3" s="424"/>
+      <c r="G3" s="424"/>
+      <c r="H3" s="424"/>
+      <c r="I3" s="424"/>
+      <c r="J3" s="424"/>
+      <c r="K3" s="424"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="415" t="s">
+      <c r="C5" s="410" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="415"/>
-      <c r="E5" s="415"/>
-      <c r="F5" s="415"/>
-      <c r="G5" s="415"/>
-      <c r="I5" s="415" t="s">
+      <c r="D5" s="410"/>
+      <c r="E5" s="410"/>
+      <c r="F5" s="410"/>
+      <c r="G5" s="410"/>
+      <c r="I5" s="410" t="s">
         <v>246</v>
       </c>
-      <c r="J5" s="415"/>
-      <c r="K5" s="415"/>
-      <c r="L5" s="415"/>
-      <c r="M5" s="415"/>
+      <c r="J5" s="410"/>
+      <c r="K5" s="410"/>
+      <c r="L5" s="410"/>
+      <c r="M5" s="410"/>
     </row>
     <row r="6" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="58" t="s">
@@ -19607,88 +19759,88 @@
       <c r="M28" s="170"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="394" t="s">
+      <c r="D29" s="345" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="396"/>
-      <c r="F29" s="420">
+      <c r="E29" s="347"/>
+      <c r="F29" s="421">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="421"/>
+      <c r="G29" s="422"/>
       <c r="I29" s="170"/>
-      <c r="J29" s="394" t="s">
+      <c r="J29" s="345" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="396"/>
-      <c r="L29" s="420">
+      <c r="K29" s="347"/>
+      <c r="L29" s="421">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="421"/>
+      <c r="M29" s="422"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="354" t="s">
+      <c r="D30" s="371" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="315"/>
-      <c r="F30" s="411">
+      <c r="E30" s="319"/>
+      <c r="F30" s="413">
         <f>F27</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="412"/>
+      <c r="G30" s="414"/>
       <c r="I30" s="170"/>
-      <c r="J30" s="354" t="s">
+      <c r="J30" s="371" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="315"/>
-      <c r="L30" s="411">
+      <c r="K30" s="319"/>
+      <c r="L30" s="413">
         <f>L27</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="412"/>
+      <c r="M30" s="414"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="354" t="s">
+      <c r="D31" s="371" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="315"/>
-      <c r="F31" s="416">
+      <c r="E31" s="319"/>
+      <c r="F31" s="415">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="417"/>
+      <c r="G31" s="416"/>
       <c r="I31" s="170"/>
-      <c r="J31" s="354" t="s">
+      <c r="J31" s="371" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="315"/>
-      <c r="L31" s="416">
+      <c r="K31" s="319"/>
+      <c r="L31" s="415">
         <f>Pemasukkan!L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="417"/>
+      <c r="M31" s="416"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="355" t="s">
+      <c r="D32" s="404" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="356"/>
-      <c r="F32" s="422">
+      <c r="E32" s="405"/>
+      <c r="F32" s="419">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="423"/>
+      <c r="G32" s="420"/>
       <c r="I32" s="170"/>
-      <c r="J32" s="355" t="s">
+      <c r="J32" s="404" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="356"/>
-      <c r="L32" s="422">
+      <c r="K32" s="405"/>
+      <c r="L32" s="419">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="423"/>
+      <c r="M32" s="420"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19880,14 +20032,6 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
     <mergeCell ref="C2:K3"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
@@ -19899,6 +20043,14 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -19924,28 +20076,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="426" t="s">
+      <c r="C2" s="427" t="s">
         <v>230</v>
       </c>
-      <c r="D2" s="427"/>
-      <c r="E2" s="427"/>
-      <c r="F2" s="427"/>
-      <c r="G2" s="427"/>
-      <c r="H2" s="427"/>
-      <c r="I2" s="427"/>
-      <c r="J2" s="427"/>
-      <c r="K2" s="427"/>
+      <c r="D2" s="428"/>
+      <c r="E2" s="428"/>
+      <c r="F2" s="428"/>
+      <c r="G2" s="428"/>
+      <c r="H2" s="428"/>
+      <c r="I2" s="428"/>
+      <c r="J2" s="428"/>
+      <c r="K2" s="428"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="427"/>
-      <c r="D3" s="427"/>
-      <c r="E3" s="427"/>
-      <c r="F3" s="427"/>
-      <c r="G3" s="427"/>
-      <c r="H3" s="427"/>
-      <c r="I3" s="427"/>
-      <c r="J3" s="427"/>
-      <c r="K3" s="427"/>
+      <c r="C3" s="428"/>
+      <c r="D3" s="428"/>
+      <c r="E3" s="428"/>
+      <c r="F3" s="428"/>
+      <c r="G3" s="428"/>
+      <c r="H3" s="428"/>
+      <c r="I3" s="428"/>
+      <c r="J3" s="428"/>
+      <c r="K3" s="428"/>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="139"/>
@@ -20303,10 +20455,10 @@
     </row>
     <row r="29" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="139"/>
-      <c r="D29" s="428"/>
-      <c r="E29" s="428"/>
-      <c r="F29" s="429"/>
-      <c r="G29" s="429"/>
+      <c r="D29" s="429"/>
+      <c r="E29" s="429"/>
+      <c r="F29" s="430"/>
+      <c r="G29" s="430"/>
       <c r="H29" s="139"/>
       <c r="I29" s="139"/>
       <c r="J29" s="139"/>
@@ -20314,15 +20466,15 @@
     </row>
     <row r="30" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="24"/>
-      <c r="D30" s="430" t="s">
+      <c r="D30" s="431" t="s">
         <v>229</v>
       </c>
-      <c r="E30" s="431"/>
-      <c r="F30" s="432">
+      <c r="E30" s="432"/>
+      <c r="F30" s="433">
         <f>F27</f>
         <v>226000</v>
       </c>
-      <c r="G30" s="433"/>
+      <c r="G30" s="434"/>
       <c r="H30" s="139"/>
       <c r="I30" s="139"/>
       <c r="J30" s="139"/>
@@ -20337,10 +20489,10 @@
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="139"/>
-      <c r="D32" s="424"/>
-      <c r="E32" s="424"/>
-      <c r="F32" s="425"/>
-      <c r="G32" s="424"/>
+      <c r="D32" s="425"/>
+      <c r="E32" s="425"/>
+      <c r="F32" s="426"/>
+      <c r="G32" s="425"/>
       <c r="H32" s="139"/>
       <c r="I32" s="139"/>
       <c r="J32" s="139"/>
@@ -20377,17 +20529,17 @@
     <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="434" t="s">
+      <c r="C4" s="435" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="435"/>
+      <c r="D4" s="436"/>
       <c r="E4" s="27"/>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
-      <c r="H4" s="434" t="s">
+      <c r="H4" s="435" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="435"/>
+      <c r="I4" s="436"/>
       <c r="J4" s="35"/>
       <c r="K4" s="27"/>
     </row>
@@ -20514,17 +20666,17 @@
     <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26"/>
-      <c r="C17" s="434" t="s">
+      <c r="C17" s="435" t="s">
         <v>144</v>
       </c>
-      <c r="D17" s="435"/>
+      <c r="D17" s="436"/>
       <c r="E17" s="27"/>
       <c r="F17" s="26"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="434" t="s">
+      <c r="H17" s="435" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="435"/>
+      <c r="I17" s="436"/>
       <c r="J17" s="35"/>
       <c r="K17" s="27"/>
     </row>

</xml_diff>

<commit_message>
Modal Perkap Trf ke Angga
sejumlah 200.000
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="400">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -1217,6 +1217,12 @@
   </si>
   <si>
     <t>Muhammad Duta AC Permana</t>
+  </si>
+  <si>
+    <t>17 Februari 2020</t>
+  </si>
+  <si>
+    <t>Modal Perkap(trf angga)</t>
   </si>
 </sst>
 </file>
@@ -3075,20 +3081,47 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="26" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="26" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3104,39 +3137,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3144,36 +3175,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3223,193 +3247,220 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3418,31 +3469,16 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3451,18 +3487,6 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3513,24 +3537,6 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="26" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="26" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4734,126 +4740,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="290" t="s">
+      <c r="A1" s="302" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="291"/>
-      <c r="C1" s="291"/>
-      <c r="D1" s="291"/>
-      <c r="E1" s="291"/>
-      <c r="F1" s="291"/>
-      <c r="G1" s="291"/>
-      <c r="H1" s="291"/>
-      <c r="I1" s="291"/>
-      <c r="J1" s="291"/>
-      <c r="K1" s="291"/>
-      <c r="L1" s="291"/>
-      <c r="M1" s="291"/>
-      <c r="N1" s="291"/>
-      <c r="O1" s="291"/>
-      <c r="P1" s="291"/>
-      <c r="Q1" s="291"/>
-      <c r="R1" s="291"/>
+      <c r="B1" s="303"/>
+      <c r="C1" s="303"/>
+      <c r="D1" s="303"/>
+      <c r="E1" s="303"/>
+      <c r="F1" s="303"/>
+      <c r="G1" s="303"/>
+      <c r="H1" s="303"/>
+      <c r="I1" s="303"/>
+      <c r="J1" s="303"/>
+      <c r="K1" s="303"/>
+      <c r="L1" s="303"/>
+      <c r="M1" s="303"/>
+      <c r="N1" s="303"/>
+      <c r="O1" s="303"/>
+      <c r="P1" s="303"/>
+      <c r="Q1" s="303"/>
+      <c r="R1" s="303"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="292"/>
-      <c r="B2" s="293"/>
-      <c r="C2" s="293"/>
-      <c r="D2" s="293"/>
-      <c r="E2" s="293"/>
-      <c r="F2" s="293"/>
-      <c r="G2" s="293"/>
-      <c r="H2" s="293"/>
-      <c r="I2" s="293"/>
-      <c r="J2" s="293"/>
-      <c r="K2" s="293"/>
-      <c r="L2" s="293"/>
-      <c r="M2" s="293"/>
-      <c r="N2" s="293"/>
-      <c r="O2" s="293"/>
-      <c r="P2" s="293"/>
-      <c r="Q2" s="293"/>
-      <c r="R2" s="293"/>
+      <c r="A2" s="304"/>
+      <c r="B2" s="305"/>
+      <c r="C2" s="305"/>
+      <c r="D2" s="305"/>
+      <c r="E2" s="305"/>
+      <c r="F2" s="305"/>
+      <c r="G2" s="305"/>
+      <c r="H2" s="305"/>
+      <c r="I2" s="305"/>
+      <c r="J2" s="305"/>
+      <c r="K2" s="305"/>
+      <c r="L2" s="305"/>
+      <c r="M2" s="305"/>
+      <c r="N2" s="305"/>
+      <c r="O2" s="305"/>
+      <c r="P2" s="305"/>
+      <c r="Q2" s="305"/>
+      <c r="R2" s="305"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="292"/>
-      <c r="B3" s="293"/>
-      <c r="C3" s="293"/>
-      <c r="D3" s="293"/>
-      <c r="E3" s="293"/>
-      <c r="F3" s="293"/>
-      <c r="G3" s="293"/>
-      <c r="H3" s="293"/>
-      <c r="I3" s="293"/>
-      <c r="J3" s="293"/>
-      <c r="K3" s="293"/>
-      <c r="L3" s="293"/>
-      <c r="M3" s="293"/>
-      <c r="N3" s="293"/>
-      <c r="O3" s="293"/>
-      <c r="P3" s="293"/>
-      <c r="Q3" s="293"/>
-      <c r="R3" s="293"/>
+      <c r="A3" s="304"/>
+      <c r="B3" s="305"/>
+      <c r="C3" s="305"/>
+      <c r="D3" s="305"/>
+      <c r="E3" s="305"/>
+      <c r="F3" s="305"/>
+      <c r="G3" s="305"/>
+      <c r="H3" s="305"/>
+      <c r="I3" s="305"/>
+      <c r="J3" s="305"/>
+      <c r="K3" s="305"/>
+      <c r="L3" s="305"/>
+      <c r="M3" s="305"/>
+      <c r="N3" s="305"/>
+      <c r="O3" s="305"/>
+      <c r="P3" s="305"/>
+      <c r="Q3" s="305"/>
+      <c r="R3" s="305"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="292"/>
-      <c r="B4" s="293"/>
-      <c r="C4" s="293"/>
-      <c r="D4" s="293"/>
-      <c r="E4" s="293"/>
-      <c r="F4" s="293"/>
-      <c r="G4" s="293"/>
-      <c r="H4" s="293"/>
-      <c r="I4" s="293"/>
-      <c r="J4" s="293"/>
-      <c r="K4" s="293"/>
-      <c r="L4" s="293"/>
-      <c r="M4" s="293"/>
-      <c r="N4" s="293"/>
-      <c r="O4" s="293"/>
-      <c r="P4" s="293"/>
-      <c r="Q4" s="293"/>
-      <c r="R4" s="293"/>
+      <c r="A4" s="304"/>
+      <c r="B4" s="305"/>
+      <c r="C4" s="305"/>
+      <c r="D4" s="305"/>
+      <c r="E4" s="305"/>
+      <c r="F4" s="305"/>
+      <c r="G4" s="305"/>
+      <c r="H4" s="305"/>
+      <c r="I4" s="305"/>
+      <c r="J4" s="305"/>
+      <c r="K4" s="305"/>
+      <c r="L4" s="305"/>
+      <c r="M4" s="305"/>
+      <c r="N4" s="305"/>
+      <c r="O4" s="305"/>
+      <c r="P4" s="305"/>
+      <c r="Q4" s="305"/>
+      <c r="R4" s="305"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="292"/>
-      <c r="B5" s="293"/>
-      <c r="C5" s="293"/>
-      <c r="D5" s="293"/>
-      <c r="E5" s="293"/>
-      <c r="F5" s="293"/>
-      <c r="G5" s="293"/>
-      <c r="H5" s="293"/>
-      <c r="I5" s="293"/>
-      <c r="J5" s="293"/>
-      <c r="K5" s="293"/>
-      <c r="L5" s="293"/>
-      <c r="M5" s="293"/>
-      <c r="N5" s="293"/>
-      <c r="O5" s="293"/>
-      <c r="P5" s="293"/>
-      <c r="Q5" s="293"/>
-      <c r="R5" s="293"/>
+      <c r="A5" s="304"/>
+      <c r="B5" s="305"/>
+      <c r="C5" s="305"/>
+      <c r="D5" s="305"/>
+      <c r="E5" s="305"/>
+      <c r="F5" s="305"/>
+      <c r="G5" s="305"/>
+      <c r="H5" s="305"/>
+      <c r="I5" s="305"/>
+      <c r="J5" s="305"/>
+      <c r="K5" s="305"/>
+      <c r="L5" s="305"/>
+      <c r="M5" s="305"/>
+      <c r="N5" s="305"/>
+      <c r="O5" s="305"/>
+      <c r="P5" s="305"/>
+      <c r="Q5" s="305"/>
+      <c r="R5" s="305"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="292"/>
-      <c r="B6" s="293"/>
-      <c r="C6" s="293"/>
-      <c r="D6" s="293"/>
-      <c r="E6" s="293"/>
-      <c r="F6" s="293"/>
-      <c r="G6" s="293"/>
-      <c r="H6" s="293"/>
-      <c r="I6" s="293"/>
-      <c r="J6" s="293"/>
-      <c r="K6" s="293"/>
-      <c r="L6" s="293"/>
-      <c r="M6" s="293"/>
-      <c r="N6" s="293"/>
-      <c r="O6" s="293"/>
-      <c r="P6" s="293"/>
-      <c r="Q6" s="293"/>
-      <c r="R6" s="293"/>
+      <c r="A6" s="304"/>
+      <c r="B6" s="305"/>
+      <c r="C6" s="305"/>
+      <c r="D6" s="305"/>
+      <c r="E6" s="305"/>
+      <c r="F6" s="305"/>
+      <c r="G6" s="305"/>
+      <c r="H6" s="305"/>
+      <c r="I6" s="305"/>
+      <c r="J6" s="305"/>
+      <c r="K6" s="305"/>
+      <c r="L6" s="305"/>
+      <c r="M6" s="305"/>
+      <c r="N6" s="305"/>
+      <c r="O6" s="305"/>
+      <c r="P6" s="305"/>
+      <c r="Q6" s="305"/>
+      <c r="R6" s="305"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
@@ -7960,58 +7966,58 @@
     <row r="77" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J79" s="298" t="s">
+      <c r="J79" s="307" t="s">
         <v>65</v>
       </c>
-      <c r="K79" s="299"/>
-      <c r="L79" s="299"/>
-      <c r="M79" s="299"/>
-      <c r="N79" s="300"/>
-      <c r="P79" s="306" t="s">
+      <c r="K79" s="308"/>
+      <c r="L79" s="308"/>
+      <c r="M79" s="308"/>
+      <c r="N79" s="309"/>
+      <c r="P79" s="315" t="s">
         <v>66</v>
       </c>
-      <c r="Q79" s="299"/>
-      <c r="R79" s="299"/>
-      <c r="S79" s="300"/>
+      <c r="Q79" s="308"/>
+      <c r="R79" s="308"/>
+      <c r="S79" s="309"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J80" s="301" t="s">
+      <c r="J80" s="310" t="s">
         <v>67</v>
       </c>
-      <c r="K80" s="293"/>
-      <c r="L80" s="293"/>
-      <c r="M80" s="293"/>
-      <c r="N80" s="302"/>
-      <c r="P80" s="301" t="s">
+      <c r="K80" s="305"/>
+      <c r="L80" s="305"/>
+      <c r="M80" s="305"/>
+      <c r="N80" s="311"/>
+      <c r="P80" s="310" t="s">
         <v>68</v>
       </c>
-      <c r="Q80" s="293"/>
-      <c r="R80" s="293"/>
-      <c r="S80" s="302"/>
+      <c r="Q80" s="305"/>
+      <c r="R80" s="305"/>
+      <c r="S80" s="311"/>
     </row>
     <row r="81" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J81" s="303"/>
-      <c r="K81" s="304"/>
-      <c r="L81" s="304"/>
-      <c r="M81" s="304"/>
-      <c r="N81" s="305"/>
-      <c r="P81" s="303"/>
-      <c r="Q81" s="304"/>
-      <c r="R81" s="304"/>
-      <c r="S81" s="305"/>
+      <c r="J81" s="312"/>
+      <c r="K81" s="313"/>
+      <c r="L81" s="313"/>
+      <c r="M81" s="313"/>
+      <c r="N81" s="314"/>
+      <c r="P81" s="312"/>
+      <c r="Q81" s="313"/>
+      <c r="R81" s="313"/>
+      <c r="S81" s="314"/>
     </row>
     <row r="82" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="296" t="s">
+      <c r="J82" s="306" t="s">
         <v>19</v>
       </c>
       <c r="K82" s="297"/>
-      <c r="L82" s="295"/>
-      <c r="M82" s="296" t="s">
+      <c r="L82" s="298"/>
+      <c r="M82" s="306" t="s">
         <v>69</v>
       </c>
-      <c r="N82" s="295"/>
-      <c r="P82" s="296"/>
-      <c r="Q82" s="295"/>
+      <c r="N82" s="298"/>
+      <c r="P82" s="306"/>
+      <c r="Q82" s="298"/>
       <c r="R82" s="3" t="s">
         <v>19</v>
       </c>
@@ -8020,38 +8026,38 @@
       </c>
     </row>
     <row r="83" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J83" s="307" t="s">
+      <c r="J83" s="296" t="s">
         <v>70</v>
       </c>
       <c r="K83" s="297"/>
-      <c r="L83" s="295"/>
-      <c r="M83" s="308">
+      <c r="L83" s="298"/>
+      <c r="M83" s="299">
         <v>7350000</v>
       </c>
-      <c r="N83" s="295"/>
-      <c r="P83" s="294" t="s">
+      <c r="N83" s="298"/>
+      <c r="P83" s="300" t="s">
         <v>71</v>
       </c>
-      <c r="Q83" s="295"/>
+      <c r="Q83" s="298"/>
       <c r="R83" s="4"/>
       <c r="S83" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="84" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="307" t="s">
+      <c r="J84" s="296" t="s">
         <v>72</v>
       </c>
       <c r="K84" s="297"/>
-      <c r="L84" s="295"/>
-      <c r="M84" s="309">
+      <c r="L84" s="298"/>
+      <c r="M84" s="301">
         <v>1100000</v>
       </c>
-      <c r="N84" s="295"/>
-      <c r="P84" s="294" t="s">
+      <c r="N84" s="298"/>
+      <c r="P84" s="300" t="s">
         <v>73</v>
       </c>
-      <c r="Q84" s="295"/>
+      <c r="Q84" s="298"/>
       <c r="R84" s="6" t="s">
         <v>74</v>
       </c>
@@ -8060,39 +8066,39 @@
       </c>
     </row>
     <row r="85" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="307" t="s">
+      <c r="J85" s="296" t="s">
         <v>75</v>
       </c>
       <c r="K85" s="297"/>
-      <c r="L85" s="295"/>
-      <c r="M85" s="308">
+      <c r="L85" s="298"/>
+      <c r="M85" s="299">
         <f>M83+M84</f>
         <v>8450000</v>
       </c>
-      <c r="N85" s="295"/>
-      <c r="P85" s="294" t="s">
+      <c r="N85" s="298"/>
+      <c r="P85" s="300" t="s">
         <v>76</v>
       </c>
-      <c r="Q85" s="295"/>
+      <c r="Q85" s="298"/>
       <c r="R85" s="4"/>
       <c r="S85" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="307" t="s">
+      <c r="J86" s="296" t="s">
         <v>77</v>
       </c>
       <c r="K86" s="297"/>
-      <c r="L86" s="295"/>
-      <c r="M86" s="308">
+      <c r="L86" s="298"/>
+      <c r="M86" s="299">
         <v>8411850</v>
       </c>
-      <c r="N86" s="295"/>
-      <c r="P86" s="294" t="s">
+      <c r="N86" s="298"/>
+      <c r="P86" s="300" t="s">
         <v>78</v>
       </c>
-      <c r="Q86" s="295"/>
+      <c r="Q86" s="298"/>
       <c r="R86" s="4"/>
       <c r="S86" s="5">
         <f>S83-S84+S85</f>
@@ -8100,20 +8106,20 @@
       </c>
     </row>
     <row r="87" spans="10:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="307" t="s">
+      <c r="J87" s="296" t="s">
         <v>79</v>
       </c>
       <c r="K87" s="297"/>
-      <c r="L87" s="295"/>
-      <c r="M87" s="308">
+      <c r="L87" s="298"/>
+      <c r="M87" s="299">
         <f>M85-M86</f>
         <v>38150</v>
       </c>
-      <c r="N87" s="295"/>
-      <c r="P87" s="294" t="s">
+      <c r="N87" s="298"/>
+      <c r="P87" s="300" t="s">
         <v>80</v>
       </c>
-      <c r="Q87" s="295"/>
+      <c r="Q87" s="298"/>
       <c r="R87" s="4"/>
       <c r="S87" s="5">
         <f>M87+S86</f>
@@ -8301,17 +8307,6 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="P86:Q86"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="M84:N84"/>
     <mergeCell ref="A1:R6"/>
     <mergeCell ref="P84:Q84"/>
     <mergeCell ref="J82:L82"/>
@@ -8324,6 +8319,17 @@
     <mergeCell ref="P83:Q83"/>
     <mergeCell ref="P82:Q82"/>
     <mergeCell ref="P80:S81"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="P86:Q86"/>
   </mergeCells>
   <conditionalFormatting sqref="T10:T69">
     <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
@@ -8370,28 +8376,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="441" t="s">
+      <c r="B2" s="447" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="442"/>
-      <c r="D2" s="442"/>
-      <c r="E2" s="442"/>
-      <c r="F2" s="442"/>
-      <c r="G2" s="442"/>
-      <c r="H2" s="442"/>
-      <c r="I2" s="442"/>
-      <c r="J2" s="442"/>
+      <c r="C2" s="448"/>
+      <c r="D2" s="448"/>
+      <c r="E2" s="448"/>
+      <c r="F2" s="448"/>
+      <c r="G2" s="448"/>
+      <c r="H2" s="448"/>
+      <c r="I2" s="448"/>
+      <c r="J2" s="448"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="442"/>
-      <c r="C3" s="442"/>
-      <c r="D3" s="442"/>
-      <c r="E3" s="442"/>
-      <c r="F3" s="442"/>
-      <c r="G3" s="442"/>
-      <c r="H3" s="442"/>
-      <c r="I3" s="442"/>
-      <c r="J3" s="442"/>
+      <c r="B3" s="448"/>
+      <c r="C3" s="448"/>
+      <c r="D3" s="448"/>
+      <c r="E3" s="448"/>
+      <c r="F3" s="448"/>
+      <c r="G3" s="448"/>
+      <c r="H3" s="448"/>
+      <c r="I3" s="448"/>
+      <c r="J3" s="448"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -8412,10 +8418,10 @@
       <c r="G6" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="H6" s="367" t="s">
+      <c r="H6" s="363" t="s">
         <v>280</v>
       </c>
-      <c r="I6" s="320"/>
+      <c r="I6" s="329"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -8437,11 +8443,11 @@
       <c r="G7" s="193">
         <v>205000</v>
       </c>
-      <c r="H7" s="443">
+      <c r="H7" s="449">
         <f>F7-G7</f>
         <v>380000</v>
       </c>
-      <c r="I7" s="320"/>
+      <c r="I7" s="329"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="194"/>
@@ -8450,8 +8456,8 @@
       <c r="E8" s="195"/>
       <c r="F8" s="195"/>
       <c r="G8" s="195"/>
-      <c r="H8" s="440"/>
-      <c r="I8" s="440"/>
+      <c r="H8" s="446"/>
+      <c r="I8" s="446"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="194"/>
@@ -8462,11 +8468,11 @@
       <c r="G9" s="196" t="s">
         <v>281</v>
       </c>
-      <c r="H9" s="444">
+      <c r="H9" s="450">
         <f>H7</f>
         <v>380000</v>
       </c>
-      <c r="I9" s="347"/>
+      <c r="I9" s="353"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="194"/>
@@ -8475,8 +8481,8 @@
       <c r="E10" s="195"/>
       <c r="F10" s="195"/>
       <c r="G10" s="195"/>
-      <c r="H10" s="440"/>
-      <c r="I10" s="440"/>
+      <c r="H10" s="446"/>
+      <c r="I10" s="446"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="194"/>
@@ -8485,8 +8491,8 @@
       <c r="E11" s="195"/>
       <c r="F11" s="195"/>
       <c r="G11" s="195"/>
-      <c r="H11" s="440"/>
-      <c r="I11" s="440"/>
+      <c r="H11" s="446"/>
+      <c r="I11" s="446"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="194"/>
@@ -8495,8 +8501,8 @@
       <c r="E12" s="195"/>
       <c r="F12" s="195"/>
       <c r="G12" s="195"/>
-      <c r="H12" s="440"/>
-      <c r="I12" s="440"/>
+      <c r="H12" s="446"/>
+      <c r="I12" s="446"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="194"/>
@@ -8505,8 +8511,8 @@
       <c r="E13" s="195"/>
       <c r="F13" s="195"/>
       <c r="G13" s="195"/>
-      <c r="H13" s="440"/>
-      <c r="I13" s="440"/>
+      <c r="H13" s="446"/>
+      <c r="I13" s="446"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="194"/>
@@ -8515,8 +8521,8 @@
       <c r="E14" s="195"/>
       <c r="F14" s="195"/>
       <c r="G14" s="195"/>
-      <c r="H14" s="440"/>
-      <c r="I14" s="440"/>
+      <c r="H14" s="446"/>
+      <c r="I14" s="446"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="194"/>
@@ -8525,8 +8531,8 @@
       <c r="E15" s="195"/>
       <c r="F15" s="195"/>
       <c r="G15" s="195"/>
-      <c r="H15" s="440"/>
-      <c r="I15" s="440"/>
+      <c r="H15" s="446"/>
+      <c r="I15" s="446"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="194"/>
@@ -8535,8 +8541,8 @@
       <c r="E16" s="195"/>
       <c r="F16" s="195"/>
       <c r="G16" s="195"/>
-      <c r="H16" s="440"/>
-      <c r="I16" s="440"/>
+      <c r="H16" s="446"/>
+      <c r="I16" s="446"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="194"/>
@@ -8545,11 +8551,16 @@
       <c r="E17" s="195"/>
       <c r="F17" s="195"/>
       <c r="G17" s="195"/>
-      <c r="H17" s="440"/>
-      <c r="I17" s="440"/>
+      <c r="H17" s="446"/>
+      <c r="I17" s="446"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="H6:I6"/>
@@ -8558,11 +8569,6 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8616,46 +8622,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="330" t="s">
+      <c r="C2" s="324" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="291"/>
-      <c r="E2" s="291"/>
-      <c r="F2" s="291"/>
-      <c r="G2" s="291"/>
-      <c r="H2" s="291"/>
-      <c r="I2" s="291"/>
-      <c r="J2" s="291"/>
-      <c r="K2" s="291"/>
-      <c r="L2" s="291"/>
-      <c r="M2" s="291"/>
-      <c r="N2" s="291"/>
-      <c r="O2" s="291"/>
-      <c r="P2" s="292"/>
-      <c r="Q2" s="292"/>
-      <c r="R2" s="292"/>
-      <c r="S2" s="291"/>
-      <c r="T2" s="291"/>
+      <c r="D2" s="303"/>
+      <c r="E2" s="303"/>
+      <c r="F2" s="303"/>
+      <c r="G2" s="303"/>
+      <c r="H2" s="303"/>
+      <c r="I2" s="303"/>
+      <c r="J2" s="303"/>
+      <c r="K2" s="303"/>
+      <c r="L2" s="303"/>
+      <c r="M2" s="303"/>
+      <c r="N2" s="303"/>
+      <c r="O2" s="303"/>
+      <c r="P2" s="304"/>
+      <c r="Q2" s="304"/>
+      <c r="R2" s="304"/>
+      <c r="S2" s="303"/>
+      <c r="T2" s="303"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="292"/>
-      <c r="D3" s="293"/>
-      <c r="E3" s="293"/>
-      <c r="F3" s="293"/>
-      <c r="G3" s="293"/>
-      <c r="H3" s="293"/>
-      <c r="I3" s="293"/>
-      <c r="J3" s="293"/>
-      <c r="K3" s="293"/>
-      <c r="L3" s="293"/>
-      <c r="M3" s="293"/>
-      <c r="N3" s="293"/>
-      <c r="O3" s="293"/>
-      <c r="P3" s="293"/>
-      <c r="Q3" s="293"/>
-      <c r="R3" s="293"/>
-      <c r="S3" s="293"/>
-      <c r="T3" s="293"/>
+      <c r="C3" s="304"/>
+      <c r="D3" s="305"/>
+      <c r="E3" s="305"/>
+      <c r="F3" s="305"/>
+      <c r="G3" s="305"/>
+      <c r="H3" s="305"/>
+      <c r="I3" s="305"/>
+      <c r="J3" s="305"/>
+      <c r="K3" s="305"/>
+      <c r="L3" s="305"/>
+      <c r="M3" s="305"/>
+      <c r="N3" s="305"/>
+      <c r="O3" s="305"/>
+      <c r="P3" s="305"/>
+      <c r="Q3" s="305"/>
+      <c r="R3" s="305"/>
+      <c r="S3" s="305"/>
+      <c r="T3" s="305"/>
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8742,7 +8748,7 @@
       <c r="V5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X5" s="322" t="s">
+      <c r="X5" s="330" t="s">
         <v>84</v>
       </c>
       <c r="Y5" s="297"/>
@@ -8760,7 +8766,7 @@
       <c r="AK5" s="297"/>
       <c r="AL5" s="297"/>
       <c r="AM5" s="297"/>
-      <c r="AN5" s="295"/>
+      <c r="AN5" s="298"/>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -8835,29 +8841,29 @@
       <c r="V6" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X6" s="331" t="s">
+      <c r="X6" s="325" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="331" t="s">
+      <c r="Y6" s="325" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="320" t="s">
+      <c r="Z6" s="329" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="321"/>
-      <c r="AB6" s="321"/>
-      <c r="AC6" s="321"/>
-      <c r="AD6" s="321"/>
-      <c r="AE6" s="321"/>
-      <c r="AF6" s="321"/>
-      <c r="AG6" s="321"/>
-      <c r="AH6" s="321"/>
-      <c r="AI6" s="321"/>
-      <c r="AJ6" s="321"/>
-      <c r="AK6" s="321"/>
-      <c r="AL6" s="321"/>
-      <c r="AM6" s="321"/>
-      <c r="AN6" s="321"/>
+      <c r="AA6" s="326"/>
+      <c r="AB6" s="326"/>
+      <c r="AC6" s="326"/>
+      <c r="AD6" s="326"/>
+      <c r="AE6" s="326"/>
+      <c r="AF6" s="326"/>
+      <c r="AG6" s="326"/>
+      <c r="AH6" s="326"/>
+      <c r="AI6" s="326"/>
+      <c r="AJ6" s="326"/>
+      <c r="AK6" s="326"/>
+      <c r="AL6" s="326"/>
+      <c r="AM6" s="326"/>
+      <c r="AN6" s="326"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -8932,27 +8938,27 @@
       <c r="V7" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="X7" s="321"/>
-      <c r="Y7" s="321"/>
-      <c r="Z7" s="320" t="s">
+      <c r="X7" s="326"/>
+      <c r="Y7" s="326"/>
+      <c r="Z7" s="329" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="321"/>
-      <c r="AB7" s="321"/>
-      <c r="AC7" s="321"/>
-      <c r="AD7" s="320" t="s">
+      <c r="AA7" s="326"/>
+      <c r="AB7" s="326"/>
+      <c r="AC7" s="326"/>
+      <c r="AD7" s="329" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="321"/>
-      <c r="AF7" s="321"/>
-      <c r="AG7" s="321"/>
-      <c r="AH7" s="321"/>
-      <c r="AI7" s="321"/>
-      <c r="AJ7" s="321"/>
-      <c r="AK7" s="321"/>
-      <c r="AL7" s="321"/>
-      <c r="AM7" s="321"/>
-      <c r="AN7" s="321"/>
+      <c r="AE7" s="326"/>
+      <c r="AF7" s="326"/>
+      <c r="AG7" s="326"/>
+      <c r="AH7" s="326"/>
+      <c r="AI7" s="326"/>
+      <c r="AJ7" s="326"/>
+      <c r="AK7" s="326"/>
+      <c r="AL7" s="326"/>
+      <c r="AM7" s="326"/>
+      <c r="AN7" s="326"/>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -9002,8 +9008,8 @@
         <v>NO</v>
       </c>
       <c r="V8" s="13"/>
-      <c r="X8" s="321"/>
-      <c r="Y8" s="321"/>
+      <c r="X8" s="326"/>
+      <c r="Y8" s="326"/>
       <c r="Z8" s="151" t="s">
         <v>19</v>
       </c>
@@ -13614,10 +13620,10 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
-      <c r="AA49" s="318" t="s">
+      <c r="AA49" s="327" t="s">
         <v>142</v>
       </c>
-      <c r="AB49" s="319"/>
+      <c r="AB49" s="328"/>
       <c r="AC49" s="16">
         <f>SUM(AC9:AC21)</f>
         <v>20000</v>
@@ -13695,12 +13701,12 @@
       <c r="AE50" s="21"/>
       <c r="AF50" s="21"/>
       <c r="AG50" s="21"/>
-      <c r="AI50" s="314" t="s">
+      <c r="AI50" s="334" t="s">
         <v>170</v>
       </c>
-      <c r="AJ50" s="315"/>
-      <c r="AK50" s="315"/>
-      <c r="AL50" s="316"/>
+      <c r="AJ50" s="335"/>
+      <c r="AK50" s="335"/>
+      <c r="AL50" s="336"/>
       <c r="AM50" s="40">
         <v>3077000</v>
       </c>
@@ -13771,12 +13777,12 @@
       <c r="AF51" s="21"/>
       <c r="AG51" s="21"/>
       <c r="AH51" s="21"/>
-      <c r="AI51" s="311" t="s">
+      <c r="AI51" s="331" t="s">
         <v>176</v>
       </c>
-      <c r="AJ51" s="312"/>
-      <c r="AK51" s="312"/>
-      <c r="AL51" s="313"/>
+      <c r="AJ51" s="332"/>
+      <c r="AK51" s="332"/>
+      <c r="AL51" s="333"/>
       <c r="AM51" s="41">
         <v>2550000</v>
       </c>
@@ -14042,14 +14048,14 @@
         <v>NO</v>
       </c>
       <c r="V55" s="2"/>
-      <c r="AC55" s="317"/>
-      <c r="AD55" s="317"/>
-      <c r="AI55" s="314" t="s">
+      <c r="AC55" s="337"/>
+      <c r="AD55" s="337"/>
+      <c r="AI55" s="334" t="s">
         <v>174</v>
       </c>
-      <c r="AJ55" s="315"/>
-      <c r="AK55" s="315"/>
-      <c r="AL55" s="316"/>
+      <c r="AJ55" s="335"/>
+      <c r="AK55" s="335"/>
+      <c r="AL55" s="336"/>
       <c r="AM55" s="38">
         <f>AM54</f>
         <v>2627000</v>
@@ -14128,12 +14134,12 @@
         <v>OK</v>
       </c>
       <c r="V56" s="2"/>
-      <c r="AI56" s="310" t="s">
+      <c r="AI56" s="316" t="s">
         <v>168</v>
       </c>
-      <c r="AJ56" s="310"/>
-      <c r="AK56" s="310"/>
-      <c r="AL56" s="310"/>
+      <c r="AJ56" s="316"/>
+      <c r="AK56" s="316"/>
+      <c r="AL56" s="316"/>
       <c r="AM56" s="52">
         <f>AM50-AM55</f>
         <v>450000</v>
@@ -14382,32 +14388,32 @@
     <row r="67" spans="3:19" s="256" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="323" t="s">
+      <c r="C69" s="317" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="324"/>
-      <c r="E69" s="324"/>
-      <c r="F69" s="324"/>
-      <c r="G69" s="325"/>
-      <c r="I69" s="329" t="s">
+      <c r="D69" s="318"/>
+      <c r="E69" s="318"/>
+      <c r="F69" s="318"/>
+      <c r="G69" s="319"/>
+      <c r="I69" s="323" t="s">
         <v>178</v>
       </c>
-      <c r="J69" s="329"/>
-      <c r="K69" s="329"/>
-      <c r="L69" s="329"/>
-      <c r="M69" s="329"/>
+      <c r="J69" s="323"/>
+      <c r="K69" s="323"/>
+      <c r="L69" s="323"/>
+      <c r="M69" s="323"/>
     </row>
     <row r="70" spans="3:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="326"/>
-      <c r="D70" s="327"/>
-      <c r="E70" s="327"/>
-      <c r="F70" s="327"/>
-      <c r="G70" s="328"/>
-      <c r="I70" s="329"/>
-      <c r="J70" s="329"/>
-      <c r="K70" s="329"/>
-      <c r="L70" s="329"/>
-      <c r="M70" s="329"/>
+      <c r="C70" s="320"/>
+      <c r="D70" s="321"/>
+      <c r="E70" s="321"/>
+      <c r="F70" s="321"/>
+      <c r="G70" s="322"/>
+      <c r="I70" s="323"/>
+      <c r="J70" s="323"/>
+      <c r="K70" s="323"/>
+      <c r="L70" s="323"/>
+      <c r="M70" s="323"/>
     </row>
     <row r="71" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="3:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14428,10 +14434,10 @@
       <c r="M76" s="55"/>
       <c r="N76" s="55"/>
       <c r="O76" s="55"/>
-      <c r="P76" s="310" t="s">
+      <c r="P76" s="316" t="s">
         <v>214</v>
       </c>
-      <c r="Q76" s="310"/>
+      <c r="Q76" s="316"/>
       <c r="R76" s="55"/>
       <c r="S76" s="55"/>
     </row>
@@ -14898,22 +14904,22 @@
     <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AI56:AL56"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AI50:AL50"/>
+    <mergeCell ref="AI55:AL55"/>
+    <mergeCell ref="AC55:AD55"/>
+    <mergeCell ref="AA49:AB49"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="AD7:AN7"/>
+    <mergeCell ref="X5:AN5"/>
+    <mergeCell ref="Z6:AN6"/>
     <mergeCell ref="P76:Q76"/>
     <mergeCell ref="C69:G70"/>
     <mergeCell ref="I69:M70"/>
     <mergeCell ref="C2:T3"/>
     <mergeCell ref="Y6:Y8"/>
     <mergeCell ref="X6:X8"/>
-    <mergeCell ref="AA49:AB49"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="AD7:AN7"/>
-    <mergeCell ref="X5:AN5"/>
-    <mergeCell ref="Z6:AN6"/>
-    <mergeCell ref="AI56:AL56"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AI50:AL50"/>
-    <mergeCell ref="AI55:AL55"/>
-    <mergeCell ref="AC55:AD55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:V61">
     <cfRule type="expression" dxfId="20" priority="8">
@@ -15003,86 +15009,86 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="332" t="s">
+      <c r="A2" s="338" t="s">
         <v>300</v>
       </c>
-      <c r="B2" s="332"/>
-      <c r="C2" s="332"/>
-      <c r="D2" s="332"/>
-      <c r="E2" s="332"/>
-      <c r="F2" s="332"/>
-      <c r="G2" s="332"/>
-      <c r="H2" s="332"/>
-      <c r="I2" s="332"/>
-      <c r="J2" s="332"/>
-      <c r="K2" s="332"/>
-      <c r="L2" s="332"/>
+      <c r="B2" s="338"/>
+      <c r="C2" s="338"/>
+      <c r="D2" s="338"/>
+      <c r="E2" s="338"/>
+      <c r="F2" s="338"/>
+      <c r="G2" s="338"/>
+      <c r="H2" s="338"/>
+      <c r="I2" s="338"/>
+      <c r="J2" s="338"/>
+      <c r="K2" s="338"/>
+      <c r="L2" s="338"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="332"/>
-      <c r="B3" s="332"/>
-      <c r="C3" s="332"/>
-      <c r="D3" s="332"/>
-      <c r="E3" s="332"/>
-      <c r="F3" s="332"/>
-      <c r="G3" s="332"/>
-      <c r="H3" s="332"/>
-      <c r="I3" s="332"/>
-      <c r="J3" s="332"/>
-      <c r="K3" s="332"/>
-      <c r="L3" s="332"/>
+      <c r="A3" s="338"/>
+      <c r="B3" s="338"/>
+      <c r="C3" s="338"/>
+      <c r="D3" s="338"/>
+      <c r="E3" s="338"/>
+      <c r="F3" s="338"/>
+      <c r="G3" s="338"/>
+      <c r="H3" s="338"/>
+      <c r="I3" s="338"/>
+      <c r="J3" s="338"/>
+      <c r="K3" s="338"/>
+      <c r="L3" s="338"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="329" t="s">
+      <c r="A5" s="323" t="s">
         <v>303</v>
       </c>
-      <c r="B5" s="329"/>
-      <c r="C5" s="329"/>
-      <c r="D5" s="329"/>
-      <c r="E5" s="329"/>
-      <c r="F5" s="329"/>
-      <c r="G5" s="329"/>
-      <c r="H5" s="329"/>
-      <c r="I5" s="329"/>
-      <c r="J5" s="329"/>
-      <c r="K5" s="329"/>
-      <c r="M5" s="329" t="s">
+      <c r="B5" s="323"/>
+      <c r="C5" s="323"/>
+      <c r="D5" s="323"/>
+      <c r="E5" s="323"/>
+      <c r="F5" s="323"/>
+      <c r="G5" s="323"/>
+      <c r="H5" s="323"/>
+      <c r="I5" s="323"/>
+      <c r="J5" s="323"/>
+      <c r="K5" s="323"/>
+      <c r="M5" s="323" t="s">
         <v>324</v>
       </c>
-      <c r="N5" s="329"/>
-      <c r="O5" s="329"/>
-      <c r="P5" s="329"/>
-      <c r="Q5" s="329"/>
-      <c r="R5" s="329"/>
-      <c r="S5" s="329"/>
-      <c r="T5" s="329"/>
-      <c r="U5" s="329"/>
-      <c r="V5" s="329"/>
-      <c r="W5" s="329"/>
+      <c r="N5" s="323"/>
+      <c r="O5" s="323"/>
+      <c r="P5" s="323"/>
+      <c r="Q5" s="323"/>
+      <c r="R5" s="323"/>
+      <c r="S5" s="323"/>
+      <c r="T5" s="323"/>
+      <c r="U5" s="323"/>
+      <c r="V5" s="323"/>
+      <c r="W5" s="323"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="329"/>
-      <c r="B6" s="329"/>
-      <c r="C6" s="329"/>
-      <c r="D6" s="329"/>
-      <c r="E6" s="329"/>
-      <c r="F6" s="329"/>
-      <c r="G6" s="329"/>
-      <c r="H6" s="329"/>
-      <c r="I6" s="329"/>
-      <c r="J6" s="329"/>
-      <c r="K6" s="329"/>
-      <c r="M6" s="329"/>
-      <c r="N6" s="329"/>
-      <c r="O6" s="329"/>
-      <c r="P6" s="329"/>
-      <c r="Q6" s="329"/>
-      <c r="R6" s="329"/>
-      <c r="S6" s="329"/>
-      <c r="T6" s="329"/>
-      <c r="U6" s="329"/>
-      <c r="V6" s="329"/>
-      <c r="W6" s="329"/>
+      <c r="A6" s="323"/>
+      <c r="B6" s="323"/>
+      <c r="C6" s="323"/>
+      <c r="D6" s="323"/>
+      <c r="E6" s="323"/>
+      <c r="F6" s="323"/>
+      <c r="G6" s="323"/>
+      <c r="H6" s="323"/>
+      <c r="I6" s="323"/>
+      <c r="J6" s="323"/>
+      <c r="K6" s="323"/>
+      <c r="M6" s="323"/>
+      <c r="N6" s="323"/>
+      <c r="O6" s="323"/>
+      <c r="P6" s="323"/>
+      <c r="Q6" s="323"/>
+      <c r="R6" s="323"/>
+      <c r="S6" s="323"/>
+      <c r="T6" s="323"/>
+      <c r="U6" s="323"/>
+      <c r="V6" s="323"/>
+      <c r="W6" s="323"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M7" s="249"/>
@@ -15992,27 +15998,27 @@
       <c r="W34" s="249"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B35" s="337" t="s">
+      <c r="B35" s="343" t="s">
         <v>312</v>
       </c>
-      <c r="C35" s="338"/>
-      <c r="D35" s="339"/>
-      <c r="E35" s="333">
+      <c r="C35" s="344"/>
+      <c r="D35" s="345"/>
+      <c r="E35" s="339">
         <f>E34-F34</f>
         <v>2610871.1799999997</v>
       </c>
-      <c r="F35" s="334"/>
+      <c r="F35" s="340"/>
       <c r="M35" s="249"/>
-      <c r="N35" s="337" t="s">
+      <c r="N35" s="343" t="s">
         <v>312</v>
       </c>
-      <c r="O35" s="338"/>
-      <c r="P35" s="339"/>
-      <c r="Q35" s="333">
+      <c r="O35" s="344"/>
+      <c r="P35" s="345"/>
+      <c r="Q35" s="339">
         <f>Q34-R34</f>
         <v>1506144.27</v>
       </c>
-      <c r="R35" s="334"/>
+      <c r="R35" s="340"/>
       <c r="S35" s="249"/>
       <c r="T35" s="249"/>
       <c r="U35" s="249"/>
@@ -16020,17 +16026,17 @@
       <c r="W35" s="249"/>
     </row>
     <row r="36" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="340"/>
-      <c r="C36" s="341"/>
-      <c r="D36" s="342"/>
-      <c r="E36" s="335"/>
-      <c r="F36" s="336"/>
+      <c r="B36" s="346"/>
+      <c r="C36" s="347"/>
+      <c r="D36" s="348"/>
+      <c r="E36" s="341"/>
+      <c r="F36" s="342"/>
       <c r="M36" s="249"/>
-      <c r="N36" s="340"/>
-      <c r="O36" s="341"/>
-      <c r="P36" s="342"/>
-      <c r="Q36" s="335"/>
-      <c r="R36" s="336"/>
+      <c r="N36" s="346"/>
+      <c r="O36" s="347"/>
+      <c r="P36" s="348"/>
+      <c r="Q36" s="341"/>
+      <c r="R36" s="342"/>
       <c r="S36" s="249"/>
       <c r="T36" s="249"/>
       <c r="U36" s="249"/>
@@ -16056,8 +16062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:X57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="K4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16097,21 +16103,21 @@
       <c r="G3" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="I3" s="329" t="s">
+      <c r="I3" s="323" t="s">
         <v>366</v>
       </c>
-      <c r="J3" s="329"/>
-      <c r="K3" s="329"/>
-      <c r="L3" s="329"/>
-      <c r="M3" s="329"/>
-      <c r="N3" s="329"/>
-      <c r="O3" s="329"/>
-      <c r="P3" s="329"/>
-      <c r="Q3" s="329"/>
-      <c r="R3" s="329"/>
-      <c r="S3" s="329"/>
-      <c r="T3" s="329"/>
-      <c r="U3" s="329"/>
+      <c r="J3" s="323"/>
+      <c r="K3" s="323"/>
+      <c r="L3" s="323"/>
+      <c r="M3" s="323"/>
+      <c r="N3" s="323"/>
+      <c r="O3" s="323"/>
+      <c r="P3" s="323"/>
+      <c r="Q3" s="323"/>
+      <c r="R3" s="323"/>
+      <c r="S3" s="323"/>
+      <c r="T3" s="323"/>
+      <c r="U3" s="323"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="57">
@@ -16133,19 +16139,19 @@
         <f>IF(ISNUMBER(SEARCH("SENIOR DISKON",D4)),100000,IF(ISNUMBER(SEARCH("SENIOR",D4)),150000,IF(ISNUMBER(SEARCH("MABA",D4)),125000,0)))</f>
         <v>125000</v>
       </c>
-      <c r="I4" s="329"/>
-      <c r="J4" s="329"/>
-      <c r="K4" s="329"/>
-      <c r="L4" s="329"/>
-      <c r="M4" s="329"/>
-      <c r="N4" s="329"/>
-      <c r="O4" s="329"/>
-      <c r="P4" s="329"/>
-      <c r="Q4" s="329"/>
-      <c r="R4" s="329"/>
-      <c r="S4" s="329"/>
-      <c r="T4" s="329"/>
-      <c r="U4" s="329"/>
+      <c r="I4" s="323"/>
+      <c r="J4" s="323"/>
+      <c r="K4" s="323"/>
+      <c r="L4" s="323"/>
+      <c r="M4" s="323"/>
+      <c r="N4" s="323"/>
+      <c r="O4" s="323"/>
+      <c r="P4" s="323"/>
+      <c r="Q4" s="323"/>
+      <c r="R4" s="323"/>
+      <c r="S4" s="323"/>
+      <c r="T4" s="323"/>
+      <c r="U4" s="323"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B5" s="57">
@@ -16172,7 +16178,7 @@
       <c r="K5" s="214"/>
       <c r="L5" s="203"/>
       <c r="M5" s="203"/>
-      <c r="N5" s="445"/>
+      <c r="N5" s="290"/>
       <c r="O5" s="277"/>
       <c r="P5" s="215"/>
       <c r="Q5" s="277"/>
@@ -16224,15 +16230,15 @@
         <v>65</v>
       </c>
       <c r="Q6" s="277"/>
-      <c r="R6" s="343" t="s">
+      <c r="R6" s="349" t="s">
         <v>368</v>
       </c>
-      <c r="S6" s="344"/>
-      <c r="T6" s="344"/>
-      <c r="U6" s="344"/>
-      <c r="V6" s="344"/>
-      <c r="W6" s="344"/>
-      <c r="X6" s="344"/>
+      <c r="S6" s="350"/>
+      <c r="T6" s="350"/>
+      <c r="U6" s="350"/>
+      <c r="V6" s="350"/>
+      <c r="W6" s="350"/>
+      <c r="X6" s="350"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="57">
@@ -16276,13 +16282,13 @@
         <v>0</v>
       </c>
       <c r="Q7" s="277"/>
-      <c r="R7" s="344"/>
-      <c r="S7" s="344"/>
-      <c r="T7" s="344"/>
-      <c r="U7" s="344"/>
-      <c r="V7" s="344"/>
-      <c r="W7" s="344"/>
-      <c r="X7" s="344"/>
+      <c r="R7" s="350"/>
+      <c r="S7" s="350"/>
+      <c r="T7" s="350"/>
+      <c r="U7" s="350"/>
+      <c r="V7" s="350"/>
+      <c r="W7" s="350"/>
+      <c r="X7" s="350"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B8" s="57">
@@ -16326,13 +16332,13 @@
         <v>500000</v>
       </c>
       <c r="Q8" s="277"/>
-      <c r="R8" s="344"/>
-      <c r="S8" s="344"/>
-      <c r="T8" s="344"/>
-      <c r="U8" s="344"/>
-      <c r="V8" s="344"/>
-      <c r="W8" s="344"/>
-      <c r="X8" s="344"/>
+      <c r="R8" s="350"/>
+      <c r="S8" s="350"/>
+      <c r="T8" s="350"/>
+      <c r="U8" s="350"/>
+      <c r="V8" s="350"/>
+      <c r="W8" s="350"/>
+      <c r="X8" s="350"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B9" s="57">
@@ -16367,7 +16373,7 @@
       <c r="M9" s="289">
         <v>1</v>
       </c>
-      <c r="N9" s="446"/>
+      <c r="N9" s="291"/>
       <c r="O9" s="210">
         <f>G57</f>
         <v>5650000</v>
@@ -16377,13 +16383,13 @@
         <v>0</v>
       </c>
       <c r="Q9" s="277"/>
-      <c r="R9" s="344"/>
-      <c r="S9" s="344"/>
-      <c r="T9" s="344"/>
-      <c r="U9" s="344"/>
-      <c r="V9" s="344"/>
-      <c r="W9" s="344"/>
-      <c r="X9" s="344"/>
+      <c r="R9" s="350"/>
+      <c r="S9" s="350"/>
+      <c r="T9" s="350"/>
+      <c r="U9" s="350"/>
+      <c r="V9" s="350"/>
+      <c r="W9" s="350"/>
+      <c r="X9" s="350"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B10" s="57">
@@ -16418,7 +16424,7 @@
       <c r="M10" s="66">
         <v>1</v>
       </c>
-      <c r="N10" s="447">
+      <c r="N10" s="292">
         <v>1500</v>
       </c>
       <c r="O10" s="210"/>
@@ -16427,13 +16433,13 @@
         <v>1500</v>
       </c>
       <c r="Q10" s="277"/>
-      <c r="R10" s="344"/>
-      <c r="S10" s="344"/>
-      <c r="T10" s="344"/>
-      <c r="U10" s="344"/>
-      <c r="V10" s="344"/>
-      <c r="W10" s="344"/>
-      <c r="X10" s="344"/>
+      <c r="R10" s="350"/>
+      <c r="S10" s="350"/>
+      <c r="T10" s="350"/>
+      <c r="U10" s="350"/>
+      <c r="V10" s="350"/>
+      <c r="W10" s="350"/>
+      <c r="X10" s="350"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B11" s="57">
@@ -16468,7 +16474,7 @@
       <c r="M11" s="66">
         <v>1</v>
       </c>
-      <c r="N11" s="447">
+      <c r="N11" s="292">
         <v>25500</v>
       </c>
       <c r="O11" s="252"/>
@@ -16477,13 +16483,13 @@
         <v>25500</v>
       </c>
       <c r="Q11" s="277"/>
-      <c r="R11" s="344"/>
-      <c r="S11" s="344"/>
-      <c r="T11" s="344"/>
-      <c r="U11" s="344"/>
-      <c r="V11" s="344"/>
-      <c r="W11" s="344"/>
-      <c r="X11" s="344"/>
+      <c r="R11" s="350"/>
+      <c r="S11" s="350"/>
+      <c r="T11" s="350"/>
+      <c r="U11" s="350"/>
+      <c r="V11" s="350"/>
+      <c r="W11" s="350"/>
+      <c r="X11" s="350"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" s="57">
@@ -16527,13 +16533,13 @@
         <v>13000</v>
       </c>
       <c r="Q12" s="277"/>
-      <c r="R12" s="344"/>
-      <c r="S12" s="344"/>
-      <c r="T12" s="344"/>
-      <c r="U12" s="344"/>
-      <c r="V12" s="344"/>
-      <c r="W12" s="344"/>
-      <c r="X12" s="344"/>
+      <c r="R12" s="350"/>
+      <c r="S12" s="350"/>
+      <c r="T12" s="350"/>
+      <c r="U12" s="350"/>
+      <c r="V12" s="350"/>
+      <c r="W12" s="350"/>
+      <c r="X12" s="350"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B13" s="57">
@@ -16568,7 +16574,7 @@
       <c r="M13" s="289">
         <v>3</v>
       </c>
-      <c r="N13" s="446">
+      <c r="N13" s="291">
         <v>750</v>
       </c>
       <c r="O13" s="210"/>
@@ -16653,14 +16659,22 @@
       <c r="J15" s="1">
         <v>9</v>
       </c>
-      <c r="K15" s="216"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="64"/>
+      <c r="K15" s="216" t="s">
+        <v>398</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1</v>
+      </c>
+      <c r="N15" s="64">
+        <v>200000</v>
+      </c>
       <c r="O15" s="210"/>
       <c r="P15" s="211">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>200000</v>
       </c>
       <c r="Q15" s="277"/>
       <c r="R15" s="253"/>
@@ -16697,7 +16711,7 @@
       <c r="K16" s="216"/>
       <c r="L16" s="278"/>
       <c r="M16" s="289"/>
-      <c r="N16" s="446"/>
+      <c r="N16" s="291"/>
       <c r="O16" s="211"/>
       <c r="P16" s="211">
         <f t="shared" si="1"/>
@@ -16738,7 +16752,7 @@
       <c r="K17" s="216"/>
       <c r="L17" s="278"/>
       <c r="M17" s="289"/>
-      <c r="N17" s="446"/>
+      <c r="N17" s="291"/>
       <c r="O17" s="211"/>
       <c r="P17" s="211">
         <f t="shared" si="1"/>
@@ -16779,7 +16793,7 @@
       <c r="K18" s="216"/>
       <c r="L18" s="278"/>
       <c r="M18" s="289"/>
-      <c r="N18" s="446"/>
+      <c r="N18" s="291"/>
       <c r="O18" s="210"/>
       <c r="P18" s="211">
         <f t="shared" si="1"/>
@@ -16818,7 +16832,7 @@
       <c r="K19" s="216"/>
       <c r="L19" s="278"/>
       <c r="M19" s="289"/>
-      <c r="N19" s="446"/>
+      <c r="N19" s="291"/>
       <c r="O19" s="211"/>
       <c r="P19" s="211">
         <f t="shared" si="1"/>
@@ -16857,7 +16871,7 @@
       <c r="K20" s="216"/>
       <c r="L20" s="278"/>
       <c r="M20" s="289"/>
-      <c r="N20" s="446"/>
+      <c r="N20" s="291"/>
       <c r="O20" s="211"/>
       <c r="P20" s="211">
         <f t="shared" si="1"/>
@@ -16935,7 +16949,7 @@
       <c r="K22" s="216"/>
       <c r="L22" s="278"/>
       <c r="M22" s="289"/>
-      <c r="N22" s="446"/>
+      <c r="N22" s="291"/>
       <c r="O22" s="211"/>
       <c r="P22" s="211">
         <f t="shared" si="1"/>
@@ -16974,7 +16988,7 @@
       <c r="K23" s="216"/>
       <c r="L23" s="278"/>
       <c r="M23" s="289"/>
-      <c r="N23" s="446"/>
+      <c r="N23" s="291"/>
       <c r="O23" s="210"/>
       <c r="P23" s="211">
         <f t="shared" si="1"/>
@@ -17091,7 +17105,7 @@
       <c r="K26" s="275"/>
       <c r="L26" s="278"/>
       <c r="M26" s="289"/>
-      <c r="N26" s="446"/>
+      <c r="N26" s="291"/>
       <c r="O26" s="210"/>
       <c r="P26" s="211">
         <f t="shared" si="1"/>
@@ -17290,7 +17304,7 @@
         <v>299</v>
       </c>
       <c r="M31" s="289"/>
-      <c r="N31" s="446"/>
+      <c r="N31" s="291"/>
       <c r="O31" s="56"/>
       <c r="P31" s="211">
         <f t="shared" si="1"/>
@@ -17329,14 +17343,14 @@
       </c>
       <c r="L32" s="222"/>
       <c r="M32" s="222"/>
-      <c r="N32" s="448"/>
+      <c r="N32" s="293"/>
       <c r="O32" s="223">
         <f>SUM(O7:O31)</f>
         <v>7650000</v>
       </c>
       <c r="P32" s="224">
         <f>SUM(P7:P31)</f>
-        <v>632250</v>
+        <v>832250</v>
       </c>
       <c r="Q32" s="277"/>
       <c r="R32" s="277"/>
@@ -17365,18 +17379,18 @@
         <v>100000</v>
       </c>
       <c r="I33" s="277"/>
-      <c r="J33" s="337" t="s">
+      <c r="J33" s="343" t="s">
         <v>365</v>
       </c>
-      <c r="K33" s="338"/>
-      <c r="L33" s="339"/>
+      <c r="K33" s="344"/>
+      <c r="L33" s="345"/>
       <c r="M33" s="287"/>
-      <c r="N33" s="449"/>
-      <c r="O33" s="333">
+      <c r="N33" s="294"/>
+      <c r="O33" s="339">
         <f>O32-P32</f>
-        <v>7017750</v>
-      </c>
-      <c r="P33" s="334"/>
+        <v>6817750</v>
+      </c>
+      <c r="P33" s="340"/>
       <c r="Q33" s="277"/>
       <c r="R33" s="277"/>
       <c r="S33" s="277"/>
@@ -17404,13 +17418,13 @@
         <v>150000</v>
       </c>
       <c r="I34" s="277"/>
-      <c r="J34" s="340"/>
-      <c r="K34" s="341"/>
-      <c r="L34" s="342"/>
+      <c r="J34" s="346"/>
+      <c r="K34" s="347"/>
+      <c r="L34" s="348"/>
       <c r="M34" s="288"/>
-      <c r="N34" s="450"/>
-      <c r="O34" s="335"/>
-      <c r="P34" s="336"/>
+      <c r="N34" s="295"/>
+      <c r="O34" s="341"/>
+      <c r="P34" s="342"/>
       <c r="Q34" s="277"/>
       <c r="R34" s="277"/>
       <c r="S34" s="277"/>
@@ -17842,13 +17856,13 @@
       </c>
     </row>
     <row r="57" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="345" t="s">
+      <c r="B57" s="351" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="346"/>
-      <c r="D57" s="346"/>
-      <c r="E57" s="346"/>
-      <c r="F57" s="347"/>
+      <c r="C57" s="352"/>
+      <c r="D57" s="352"/>
+      <c r="E57" s="352"/>
+      <c r="F57" s="353"/>
       <c r="G57" s="282">
         <f>SUM(G4:G56)</f>
         <v>5650000</v>
@@ -17932,17 +17946,17 @@
       <c r="A2" s="172"/>
       <c r="B2" s="173"/>
       <c r="C2" s="173"/>
-      <c r="D2" s="348" t="s">
+      <c r="D2" s="411" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="348"/>
-      <c r="F2" s="348"/>
-      <c r="G2" s="348"/>
-      <c r="H2" s="348"/>
-      <c r="I2" s="348"/>
-      <c r="J2" s="348"/>
-      <c r="K2" s="348"/>
-      <c r="L2" s="348"/>
+      <c r="E2" s="411"/>
+      <c r="F2" s="411"/>
+      <c r="G2" s="411"/>
+      <c r="H2" s="411"/>
+      <c r="I2" s="411"/>
+      <c r="J2" s="411"/>
+      <c r="K2" s="411"/>
+      <c r="L2" s="411"/>
       <c r="M2" s="174"/>
       <c r="N2" s="24"/>
     </row>
@@ -17960,205 +17974,205 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="176"/>
-      <c r="U3" s="398" t="s">
+      <c r="U3" s="354" t="s">
         <v>195</v>
       </c>
-      <c r="V3" s="399"/>
-      <c r="W3" s="400" t="s">
+      <c r="V3" s="355"/>
+      <c r="W3" s="356" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="399"/>
-      <c r="Y3" s="399"/>
-      <c r="Z3" s="399"/>
-      <c r="AA3" s="399"/>
-      <c r="AB3" s="399"/>
-      <c r="AC3" s="399"/>
-      <c r="AD3" s="401"/>
+      <c r="X3" s="355"/>
+      <c r="Y3" s="355"/>
+      <c r="Z3" s="355"/>
+      <c r="AA3" s="355"/>
+      <c r="AB3" s="355"/>
+      <c r="AC3" s="355"/>
+      <c r="AD3" s="357"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="175"/>
-      <c r="B4" s="363" t="s">
+      <c r="B4" s="415" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="364"/>
-      <c r="D4" s="364"/>
-      <c r="E4" s="364"/>
-      <c r="F4" s="364"/>
+      <c r="C4" s="416"/>
+      <c r="D4" s="416"/>
+      <c r="E4" s="416"/>
+      <c r="F4" s="416"/>
       <c r="G4" s="70">
         <v>1004200</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="367" t="s">
+      <c r="I4" s="363" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="320"/>
-      <c r="K4" s="320"/>
-      <c r="L4" s="320"/>
+      <c r="J4" s="329"/>
+      <c r="K4" s="329"/>
+      <c r="L4" s="329"/>
       <c r="M4" s="176"/>
-      <c r="U4" s="410" t="s">
+      <c r="U4" s="375" t="s">
         <v>196</v>
       </c>
-      <c r="V4" s="320"/>
-      <c r="W4" s="367" t="s">
+      <c r="V4" s="329"/>
+      <c r="W4" s="363" t="s">
         <v>198</v>
       </c>
-      <c r="X4" s="320"/>
-      <c r="Y4" s="320"/>
-      <c r="Z4" s="320"/>
-      <c r="AA4" s="320"/>
-      <c r="AB4" s="320"/>
-      <c r="AC4" s="320"/>
-      <c r="AD4" s="387"/>
+      <c r="X4" s="329"/>
+      <c r="Y4" s="329"/>
+      <c r="Z4" s="329"/>
+      <c r="AA4" s="329"/>
+      <c r="AB4" s="329"/>
+      <c r="AC4" s="329"/>
+      <c r="AD4" s="358"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="175"/>
-      <c r="B5" s="358" t="s">
+      <c r="B5" s="380" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="320"/>
-      <c r="D5" s="320"/>
-      <c r="E5" s="320"/>
-      <c r="F5" s="320"/>
+      <c r="C5" s="329"/>
+      <c r="D5" s="329"/>
+      <c r="E5" s="329"/>
+      <c r="F5" s="329"/>
       <c r="G5" s="152">
         <v>568329.18000000005</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="356" t="s">
+      <c r="I5" s="382" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="357"/>
-      <c r="K5" s="368">
+      <c r="J5" s="403"/>
+      <c r="K5" s="405">
         <f>G7</f>
         <v>2332529.1800000002</v>
       </c>
-      <c r="L5" s="369"/>
+      <c r="L5" s="406"/>
       <c r="M5" s="176"/>
-      <c r="U5" s="394" t="s">
+      <c r="U5" s="376" t="s">
         <v>231</v>
       </c>
-      <c r="V5" s="395"/>
-      <c r="W5" s="356" t="s">
+      <c r="V5" s="377"/>
+      <c r="W5" s="382" t="s">
         <v>232</v>
       </c>
-      <c r="X5" s="381"/>
-      <c r="Y5" s="381"/>
-      <c r="Z5" s="381"/>
-      <c r="AA5" s="381"/>
-      <c r="AB5" s="381"/>
-      <c r="AC5" s="381"/>
-      <c r="AD5" s="382"/>
+      <c r="X5" s="383"/>
+      <c r="Y5" s="383"/>
+      <c r="Z5" s="383"/>
+      <c r="AA5" s="383"/>
+      <c r="AB5" s="383"/>
+      <c r="AC5" s="383"/>
+      <c r="AD5" s="384"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="175"/>
-      <c r="B6" s="350" t="s">
+      <c r="B6" s="373" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="351"/>
-      <c r="D6" s="351"/>
-      <c r="E6" s="351"/>
-      <c r="F6" s="351"/>
+      <c r="C6" s="374"/>
+      <c r="D6" s="374"/>
+      <c r="E6" s="374"/>
+      <c r="F6" s="374"/>
       <c r="G6" s="152">
         <v>760000</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="354" t="s">
+      <c r="I6" s="404" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="355"/>
-      <c r="K6" s="370">
+      <c r="J6" s="399"/>
+      <c r="K6" s="407">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="L6" s="371"/>
+      <c r="L6" s="408"/>
       <c r="M6" s="176"/>
-      <c r="U6" s="396"/>
-      <c r="V6" s="397"/>
-      <c r="W6" s="383" t="s">
+      <c r="U6" s="378"/>
+      <c r="V6" s="379"/>
+      <c r="W6" s="364" t="s">
         <v>233</v>
       </c>
-      <c r="X6" s="384"/>
-      <c r="Y6" s="384"/>
-      <c r="Z6" s="384"/>
-      <c r="AA6" s="384"/>
-      <c r="AB6" s="384"/>
-      <c r="AC6" s="384"/>
-      <c r="AD6" s="385"/>
+      <c r="X6" s="365"/>
+      <c r="Y6" s="365"/>
+      <c r="Z6" s="365"/>
+      <c r="AA6" s="365"/>
+      <c r="AB6" s="365"/>
+      <c r="AC6" s="365"/>
+      <c r="AD6" s="366"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="175"/>
-      <c r="B7" s="361" t="s">
+      <c r="B7" s="385" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="362"/>
-      <c r="D7" s="362"/>
-      <c r="E7" s="362"/>
-      <c r="F7" s="355"/>
+      <c r="C7" s="386"/>
+      <c r="D7" s="386"/>
+      <c r="E7" s="386"/>
+      <c r="F7" s="399"/>
       <c r="G7" s="152">
         <f>SUM(G4:G6)</f>
         <v>2332529.1800000002</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="354" t="s">
+      <c r="I7" s="404" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="355"/>
-      <c r="K7" s="365">
+      <c r="J7" s="399"/>
+      <c r="K7" s="409">
         <f>Pemasukkan!F31</f>
         <v>222000</v>
       </c>
-      <c r="L7" s="366"/>
+      <c r="L7" s="410"/>
       <c r="M7" s="176"/>
-      <c r="U7" s="402"/>
-      <c r="V7" s="403"/>
-      <c r="W7" s="367" t="s">
+      <c r="U7" s="361"/>
+      <c r="V7" s="362"/>
+      <c r="W7" s="363" t="s">
         <v>234</v>
       </c>
-      <c r="X7" s="320"/>
-      <c r="Y7" s="320"/>
-      <c r="Z7" s="320"/>
-      <c r="AA7" s="320"/>
-      <c r="AB7" s="320"/>
-      <c r="AC7" s="320"/>
-      <c r="AD7" s="387"/>
+      <c r="X7" s="329"/>
+      <c r="Y7" s="329"/>
+      <c r="Z7" s="329"/>
+      <c r="AA7" s="329"/>
+      <c r="AB7" s="329"/>
+      <c r="AC7" s="329"/>
+      <c r="AD7" s="358"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="175"/>
-      <c r="B8" s="359" t="s">
+      <c r="B8" s="413" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
+      <c r="C8" s="414"/>
+      <c r="D8" s="414"/>
+      <c r="E8" s="414"/>
+      <c r="F8" s="414"/>
       <c r="G8" s="153">
         <f>K8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="356" t="s">
+      <c r="I8" s="382" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="357"/>
-      <c r="K8" s="352">
+      <c r="J8" s="403"/>
+      <c r="K8" s="394">
         <f>(K5-K6)+K7</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="L8" s="353"/>
+      <c r="L8" s="395"/>
       <c r="M8" s="176"/>
-      <c r="U8" s="406" t="s">
+      <c r="U8" s="369" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="407"/>
-      <c r="W8" s="383" t="s">
+      <c r="V8" s="370"/>
+      <c r="W8" s="364" t="s">
         <v>199</v>
       </c>
-      <c r="X8" s="384"/>
-      <c r="Y8" s="384"/>
-      <c r="Z8" s="384"/>
-      <c r="AA8" s="384"/>
-      <c r="AB8" s="384"/>
-      <c r="AC8" s="384"/>
-      <c r="AD8" s="385"/>
+      <c r="X8" s="365"/>
+      <c r="Y8" s="365"/>
+      <c r="Z8" s="365"/>
+      <c r="AA8" s="365"/>
+      <c r="AB8" s="365"/>
+      <c r="AC8" s="365"/>
+      <c r="AD8" s="366"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="175"/>
@@ -18174,28 +18188,28 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="176"/>
-      <c r="U9" s="408"/>
-      <c r="V9" s="409"/>
-      <c r="W9" s="383" t="s">
+      <c r="U9" s="371"/>
+      <c r="V9" s="372"/>
+      <c r="W9" s="364" t="s">
         <v>237</v>
       </c>
-      <c r="X9" s="384"/>
-      <c r="Y9" s="384"/>
-      <c r="Z9" s="384"/>
-      <c r="AA9" s="384"/>
-      <c r="AB9" s="384"/>
-      <c r="AC9" s="384"/>
-      <c r="AD9" s="385"/>
+      <c r="X9" s="365"/>
+      <c r="Y9" s="365"/>
+      <c r="Z9" s="365"/>
+      <c r="AA9" s="365"/>
+      <c r="AB9" s="365"/>
+      <c r="AC9" s="365"/>
+      <c r="AD9" s="366"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="175"/>
-      <c r="B10" s="320" t="s">
+      <c r="B10" s="329" t="s">
         <v>253</v>
       </c>
-      <c r="C10" s="320"/>
-      <c r="D10" s="320"/>
-      <c r="E10" s="320"/>
-      <c r="F10" s="320"/>
+      <c r="C10" s="329"/>
+      <c r="D10" s="329"/>
+      <c r="E10" s="329"/>
+      <c r="F10" s="329"/>
       <c r="G10" s="56">
         <f>G5</f>
         <v>568329.18000000005</v>
@@ -18206,30 +18220,30 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="176"/>
-      <c r="U10" s="350" t="s">
+      <c r="U10" s="373" t="s">
         <v>243</v>
       </c>
-      <c r="V10" s="351"/>
-      <c r="W10" s="320" t="s">
+      <c r="V10" s="374"/>
+      <c r="W10" s="329" t="s">
         <v>257</v>
       </c>
-      <c r="X10" s="320"/>
-      <c r="Y10" s="320"/>
-      <c r="Z10" s="320"/>
-      <c r="AA10" s="320"/>
-      <c r="AB10" s="320"/>
-      <c r="AC10" s="320"/>
-      <c r="AD10" s="387"/>
+      <c r="X10" s="329"/>
+      <c r="Y10" s="329"/>
+      <c r="Z10" s="329"/>
+      <c r="AA10" s="329"/>
+      <c r="AB10" s="329"/>
+      <c r="AC10" s="329"/>
+      <c r="AD10" s="358"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="175"/>
-      <c r="B11" s="320" t="s">
+      <c r="B11" s="329" t="s">
         <v>254</v>
       </c>
-      <c r="C11" s="320"/>
-      <c r="D11" s="320"/>
-      <c r="E11" s="320"/>
-      <c r="F11" s="320"/>
+      <c r="C11" s="329"/>
+      <c r="D11" s="329"/>
+      <c r="E11" s="329"/>
+      <c r="F11" s="329"/>
       <c r="G11" s="56">
         <v>1089400</v>
       </c>
@@ -18239,30 +18253,30 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="176"/>
-      <c r="U11" s="350" t="s">
+      <c r="U11" s="373" t="s">
         <v>256</v>
       </c>
-      <c r="V11" s="351"/>
-      <c r="W11" s="404" t="s">
+      <c r="V11" s="374"/>
+      <c r="W11" s="367" t="s">
         <v>258</v>
       </c>
-      <c r="X11" s="404"/>
-      <c r="Y11" s="404"/>
-      <c r="Z11" s="404"/>
-      <c r="AA11" s="404"/>
-      <c r="AB11" s="404"/>
-      <c r="AC11" s="404"/>
-      <c r="AD11" s="405"/>
+      <c r="X11" s="367"/>
+      <c r="Y11" s="367"/>
+      <c r="Z11" s="367"/>
+      <c r="AA11" s="367"/>
+      <c r="AB11" s="367"/>
+      <c r="AC11" s="367"/>
+      <c r="AD11" s="368"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="175"/>
-      <c r="B12" s="349" t="s">
+      <c r="B12" s="412" t="s">
         <v>255</v>
       </c>
-      <c r="C12" s="349"/>
-      <c r="D12" s="349"/>
-      <c r="E12" s="349"/>
-      <c r="F12" s="349"/>
+      <c r="C12" s="412"/>
+      <c r="D12" s="412"/>
+      <c r="E12" s="412"/>
+      <c r="F12" s="412"/>
       <c r="G12" s="180">
         <f>SUM(G10:G11)</f>
         <v>1657729.1800000002</v>
@@ -18273,16 +18287,16 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="176"/>
-      <c r="U12" s="350"/>
-      <c r="V12" s="351"/>
-      <c r="W12" s="320"/>
-      <c r="X12" s="320"/>
-      <c r="Y12" s="320"/>
-      <c r="Z12" s="320"/>
-      <c r="AA12" s="320"/>
-      <c r="AB12" s="320"/>
-      <c r="AC12" s="320"/>
-      <c r="AD12" s="387"/>
+      <c r="U12" s="373"/>
+      <c r="V12" s="374"/>
+      <c r="W12" s="329"/>
+      <c r="X12" s="329"/>
+      <c r="Y12" s="329"/>
+      <c r="Z12" s="329"/>
+      <c r="AA12" s="329"/>
+      <c r="AB12" s="329"/>
+      <c r="AC12" s="329"/>
+      <c r="AD12" s="358"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="177"/>
@@ -18298,45 +18312,45 @@
       <c r="K13" s="178"/>
       <c r="L13" s="178"/>
       <c r="M13" s="179"/>
-      <c r="U13" s="350"/>
-      <c r="V13" s="351"/>
-      <c r="W13" s="320"/>
-      <c r="X13" s="320"/>
-      <c r="Y13" s="320"/>
-      <c r="Z13" s="320"/>
-      <c r="AA13" s="320"/>
-      <c r="AB13" s="320"/>
-      <c r="AC13" s="320"/>
-      <c r="AD13" s="387"/>
+      <c r="U13" s="373"/>
+      <c r="V13" s="374"/>
+      <c r="W13" s="329"/>
+      <c r="X13" s="329"/>
+      <c r="Y13" s="329"/>
+      <c r="Z13" s="329"/>
+      <c r="AA13" s="329"/>
+      <c r="AB13" s="329"/>
+      <c r="AC13" s="329"/>
+      <c r="AD13" s="358"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U14" s="388"/>
       <c r="V14" s="389"/>
-      <c r="W14" s="379"/>
-      <c r="X14" s="379"/>
-      <c r="Y14" s="379"/>
-      <c r="Z14" s="379"/>
-      <c r="AA14" s="379"/>
-      <c r="AB14" s="379"/>
-      <c r="AC14" s="379"/>
-      <c r="AD14" s="380"/>
+      <c r="W14" s="359"/>
+      <c r="X14" s="359"/>
+      <c r="Y14" s="359"/>
+      <c r="Z14" s="359"/>
+      <c r="AA14" s="359"/>
+      <c r="AB14" s="359"/>
+      <c r="AC14" s="359"/>
+      <c r="AD14" s="360"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="172"/>
       <c r="B18" s="173"/>
       <c r="C18" s="173"/>
-      <c r="D18" s="348" t="s">
+      <c r="D18" s="411" t="s">
         <v>249</v>
       </c>
-      <c r="E18" s="348"/>
-      <c r="F18" s="348"/>
-      <c r="G18" s="348"/>
-      <c r="H18" s="348"/>
-      <c r="I18" s="348"/>
-      <c r="J18" s="348"/>
-      <c r="K18" s="348"/>
-      <c r="L18" s="348"/>
+      <c r="E18" s="411"/>
+      <c r="F18" s="411"/>
+      <c r="G18" s="411"/>
+      <c r="H18" s="411"/>
+      <c r="I18" s="411"/>
+      <c r="J18" s="411"/>
+      <c r="K18" s="411"/>
+      <c r="L18" s="411"/>
       <c r="M18" s="174"/>
       <c r="O18" s="390" t="s">
         <v>250</v>
@@ -18349,13 +18363,13 @@
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="175"/>
       <c r="M19" s="176"/>
-      <c r="O19" s="358" t="s">
+      <c r="O19" s="380" t="s">
         <v>251</v>
       </c>
-      <c r="P19" s="320"/>
-      <c r="Q19" s="320"/>
-      <c r="R19" s="320"/>
-      <c r="S19" s="387"/>
+      <c r="P19" s="329"/>
+      <c r="Q19" s="329"/>
+      <c r="R19" s="329"/>
+      <c r="S19" s="358"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="175"/>
@@ -18366,119 +18380,119 @@
       <c r="F20" s="200"/>
       <c r="G20" s="68"/>
       <c r="H20" s="24"/>
-      <c r="I20" s="367" t="s">
+      <c r="I20" s="363" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="320"/>
-      <c r="K20" s="320"/>
-      <c r="L20" s="320"/>
+      <c r="J20" s="329"/>
+      <c r="K20" s="329"/>
+      <c r="L20" s="329"/>
       <c r="M20" s="176"/>
-      <c r="O20" s="358" t="s">
+      <c r="O20" s="380" t="s">
         <v>252</v>
       </c>
-      <c r="P20" s="320"/>
-      <c r="Q20" s="320"/>
-      <c r="R20" s="320"/>
-      <c r="S20" s="387"/>
+      <c r="P20" s="329"/>
+      <c r="Q20" s="329"/>
+      <c r="R20" s="329"/>
+      <c r="S20" s="358"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="175"/>
-      <c r="B21" s="372" t="s">
+      <c r="B21" s="396" t="s">
         <v>296</v>
       </c>
-      <c r="C21" s="373"/>
-      <c r="D21" s="373"/>
-      <c r="E21" s="373"/>
-      <c r="F21" s="374"/>
+      <c r="C21" s="397"/>
+      <c r="D21" s="397"/>
+      <c r="E21" s="397"/>
+      <c r="F21" s="398"/>
       <c r="G21" s="70">
         <f>G12</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H21" s="24"/>
-      <c r="I21" s="356" t="s">
+      <c r="I21" s="382" t="s">
         <v>72</v>
       </c>
-      <c r="J21" s="357"/>
-      <c r="K21" s="368">
+      <c r="J21" s="403"/>
+      <c r="K21" s="405">
         <f>G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="L21" s="369"/>
+      <c r="L21" s="406"/>
       <c r="M21" s="176"/>
       <c r="N21" s="170"/>
       <c r="O21" s="393" t="s">
         <v>259</v>
       </c>
-      <c r="P21" s="381"/>
-      <c r="Q21" s="381"/>
-      <c r="R21" s="381"/>
-      <c r="S21" s="382"/>
+      <c r="P21" s="383"/>
+      <c r="Q21" s="383"/>
+      <c r="R21" s="383"/>
+      <c r="S21" s="384"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="175"/>
-      <c r="B22" s="361" t="s">
+      <c r="B22" s="385" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="362"/>
-      <c r="D22" s="362"/>
-      <c r="E22" s="362"/>
-      <c r="F22" s="355"/>
+      <c r="C22" s="386"/>
+      <c r="D22" s="386"/>
+      <c r="E22" s="386"/>
+      <c r="F22" s="399"/>
       <c r="G22" s="152">
         <f>G21</f>
         <v>1657729.1800000002</v>
       </c>
       <c r="H22" s="24"/>
-      <c r="I22" s="354" t="s">
+      <c r="I22" s="404" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="355"/>
-      <c r="K22" s="370">
+      <c r="J22" s="399"/>
+      <c r="K22" s="407">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="L22" s="371"/>
+      <c r="L22" s="408"/>
       <c r="M22" s="176"/>
       <c r="N22" s="170"/>
-      <c r="O22" s="361" t="s">
+      <c r="O22" s="385" t="s">
         <v>260</v>
       </c>
-      <c r="P22" s="362"/>
-      <c r="Q22" s="362"/>
-      <c r="R22" s="362"/>
-      <c r="S22" s="386"/>
+      <c r="P22" s="386"/>
+      <c r="Q22" s="386"/>
+      <c r="R22" s="386"/>
+      <c r="S22" s="387"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="175"/>
-      <c r="B23" s="375" t="s">
+      <c r="B23" s="400" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="376"/>
-      <c r="D23" s="376"/>
-      <c r="E23" s="376"/>
-      <c r="F23" s="377"/>
+      <c r="C23" s="401"/>
+      <c r="D23" s="401"/>
+      <c r="E23" s="401"/>
+      <c r="F23" s="402"/>
       <c r="G23" s="153">
         <f>K24</f>
         <v>1568729.1800000002</v>
       </c>
       <c r="H23" s="24"/>
-      <c r="I23" s="354" t="s">
+      <c r="I23" s="404" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="355"/>
-      <c r="K23" s="365">
+      <c r="J23" s="399"/>
+      <c r="K23" s="409">
         <f>Pemasukkan!L31</f>
         <v>690000</v>
       </c>
-      <c r="L23" s="366"/>
+      <c r="L23" s="410"/>
       <c r="M23" s="176"/>
       <c r="N23" s="170"/>
-      <c r="O23" s="361" t="s">
+      <c r="O23" s="385" t="s">
         <v>261</v>
       </c>
-      <c r="P23" s="362"/>
-      <c r="Q23" s="362"/>
-      <c r="R23" s="362"/>
-      <c r="S23" s="386"/>
+      <c r="P23" s="386"/>
+      <c r="Q23" s="386"/>
+      <c r="R23" s="386"/>
+      <c r="S23" s="387"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="175"/>
@@ -18489,24 +18503,24 @@
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="356" t="s">
+      <c r="I24" s="382" t="s">
         <v>191</v>
       </c>
-      <c r="J24" s="357"/>
-      <c r="K24" s="352">
+      <c r="J24" s="403"/>
+      <c r="K24" s="394">
         <f>(K21-K22)+K23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="L24" s="353"/>
+      <c r="L24" s="395"/>
       <c r="M24" s="176"/>
       <c r="N24" s="170"/>
-      <c r="O24" s="361" t="s">
+      <c r="O24" s="385" t="s">
         <v>262</v>
       </c>
-      <c r="P24" s="362"/>
-      <c r="Q24" s="362"/>
-      <c r="R24" s="362"/>
-      <c r="S24" s="386"/>
+      <c r="P24" s="386"/>
+      <c r="Q24" s="386"/>
+      <c r="R24" s="386"/>
+      <c r="S24" s="387"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="175"/>
@@ -18523,13 +18537,13 @@
       <c r="L25" s="24"/>
       <c r="M25" s="176"/>
       <c r="N25" s="170"/>
-      <c r="O25" s="358" t="s">
+      <c r="O25" s="380" t="s">
         <v>267</v>
       </c>
-      <c r="P25" s="320"/>
-      <c r="Q25" s="320"/>
-      <c r="R25" s="320"/>
-      <c r="S25" s="387"/>
+      <c r="P25" s="329"/>
+      <c r="Q25" s="329"/>
+      <c r="R25" s="329"/>
+      <c r="S25" s="358"/>
     </row>
     <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="175"/>
@@ -18546,11 +18560,11 @@
       <c r="L26" s="24"/>
       <c r="M26" s="176"/>
       <c r="N26" s="170"/>
-      <c r="O26" s="378"/>
-      <c r="P26" s="379"/>
-      <c r="Q26" s="379"/>
-      <c r="R26" s="379"/>
-      <c r="S26" s="380"/>
+      <c r="O26" s="381"/>
+      <c r="P26" s="359"/>
+      <c r="Q26" s="359"/>
+      <c r="R26" s="359"/>
+      <c r="S26" s="360"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="177"/>
@@ -18585,6 +18599,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="D18:L18"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="O26:S26"/>
+    <mergeCell ref="W5:AD5"/>
+    <mergeCell ref="W6:AD6"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="O19:S19"/>
+    <mergeCell ref="O20:S20"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="O18:S18"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O23:S23"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="W4:AD4"/>
+    <mergeCell ref="W8:AD8"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="O25:S25"/>
     <mergeCell ref="U3:V3"/>
     <mergeCell ref="W3:AD3"/>
     <mergeCell ref="W12:AD12"/>
@@ -18601,53 +18662,6 @@
     <mergeCell ref="U12:V12"/>
     <mergeCell ref="U13:V13"/>
     <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:AD4"/>
-    <mergeCell ref="W8:AD8"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="O25:S25"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="W5:AD5"/>
-    <mergeCell ref="W6:AD6"/>
-    <mergeCell ref="O24:S24"/>
-    <mergeCell ref="O19:S19"/>
-    <mergeCell ref="O20:S20"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="O18:S18"/>
-    <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O23:S23"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="D18:L18"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -18681,28 +18695,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="411" t="s">
+      <c r="C2" s="426" t="s">
         <v>186</v>
       </c>
-      <c r="D2" s="412"/>
-      <c r="E2" s="412"/>
-      <c r="F2" s="412"/>
-      <c r="G2" s="412"/>
-      <c r="H2" s="412"/>
-      <c r="I2" s="412"/>
-      <c r="J2" s="412"/>
-      <c r="K2" s="412"/>
+      <c r="D2" s="427"/>
+      <c r="E2" s="427"/>
+      <c r="F2" s="427"/>
+      <c r="G2" s="427"/>
+      <c r="H2" s="427"/>
+      <c r="I2" s="427"/>
+      <c r="J2" s="427"/>
+      <c r="K2" s="427"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="412"/>
-      <c r="D3" s="412"/>
-      <c r="E3" s="412"/>
-      <c r="F3" s="412"/>
-      <c r="G3" s="412"/>
-      <c r="H3" s="412"/>
-      <c r="I3" s="412"/>
-      <c r="J3" s="412"/>
-      <c r="K3" s="412"/>
+      <c r="C3" s="427"/>
+      <c r="D3" s="427"/>
+      <c r="E3" s="427"/>
+      <c r="F3" s="427"/>
+      <c r="G3" s="427"/>
+      <c r="H3" s="427"/>
+      <c r="I3" s="427"/>
+      <c r="J3" s="427"/>
+      <c r="K3" s="427"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="419" t="s">
@@ -19158,83 +19172,83 @@
       <c r="M28" s="170"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="363" t="s">
+      <c r="D29" s="415" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="364"/>
-      <c r="F29" s="413">
+      <c r="E29" s="416"/>
+      <c r="F29" s="420">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="414"/>
+      <c r="G29" s="421"/>
       <c r="I29" s="170"/>
-      <c r="J29" s="363" t="s">
+      <c r="J29" s="415" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="364"/>
-      <c r="L29" s="413">
+      <c r="K29" s="416"/>
+      <c r="L29" s="420">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="414"/>
+      <c r="M29" s="421"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="410" t="s">
+      <c r="D30" s="375" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="320"/>
-      <c r="F30" s="415">
+      <c r="E30" s="329"/>
+      <c r="F30" s="422">
         <f>Pengeluaran!F30</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="416"/>
+      <c r="G30" s="423"/>
       <c r="I30" s="170"/>
-      <c r="J30" s="410" t="s">
+      <c r="J30" s="375" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="320"/>
-      <c r="L30" s="415">
+      <c r="K30" s="329"/>
+      <c r="L30" s="422">
         <f>Pengeluaran!L30</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="416"/>
+      <c r="M30" s="423"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="358" t="s">
+      <c r="D31" s="380" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="320"/>
-      <c r="F31" s="420">
+      <c r="E31" s="329"/>
+      <c r="F31" s="424">
         <f>F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="421"/>
+      <c r="G31" s="425"/>
       <c r="I31" s="170"/>
-      <c r="J31" s="358" t="s">
+      <c r="J31" s="380" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="320"/>
-      <c r="L31" s="420">
+      <c r="K31" s="329"/>
+      <c r="L31" s="424">
         <f>L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="421"/>
+      <c r="M31" s="425"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="359" t="s">
+      <c r="D32" s="413" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="360"/>
+      <c r="E32" s="414"/>
       <c r="F32" s="417">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
       <c r="G32" s="418"/>
       <c r="I32" s="170"/>
-      <c r="J32" s="359" t="s">
+      <c r="J32" s="413" t="s">
         <v>190</v>
       </c>
-      <c r="K32" s="360"/>
+      <c r="K32" s="414"/>
       <c r="L32" s="417">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
@@ -19431,6 +19445,12 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C2:K3"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="J29:K29"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="I5:M5"/>
@@ -19444,12 +19464,6 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J32:K32"/>
-    <mergeCell ref="C2:K3"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -19482,28 +19496,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="422" t="s">
+      <c r="C2" s="432" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="423"/>
-      <c r="E2" s="423"/>
-      <c r="F2" s="423"/>
-      <c r="G2" s="423"/>
-      <c r="H2" s="423"/>
-      <c r="I2" s="423"/>
-      <c r="J2" s="423"/>
-      <c r="K2" s="423"/>
+      <c r="D2" s="433"/>
+      <c r="E2" s="433"/>
+      <c r="F2" s="433"/>
+      <c r="G2" s="433"/>
+      <c r="H2" s="433"/>
+      <c r="I2" s="433"/>
+      <c r="J2" s="433"/>
+      <c r="K2" s="433"/>
     </row>
     <row r="3" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="423"/>
-      <c r="D3" s="423"/>
-      <c r="E3" s="423"/>
-      <c r="F3" s="423"/>
-      <c r="G3" s="423"/>
-      <c r="H3" s="423"/>
-      <c r="I3" s="423"/>
-      <c r="J3" s="423"/>
-      <c r="K3" s="423"/>
+      <c r="C3" s="433"/>
+      <c r="D3" s="433"/>
+      <c r="E3" s="433"/>
+      <c r="F3" s="433"/>
+      <c r="G3" s="433"/>
+      <c r="H3" s="433"/>
+      <c r="I3" s="433"/>
+      <c r="J3" s="433"/>
+      <c r="K3" s="433"/>
     </row>
     <row r="5" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="419" t="s">
@@ -20003,88 +20017,88 @@
       <c r="M28" s="170"/>
     </row>
     <row r="29" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="398" t="s">
+      <c r="D29" s="354" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="400"/>
-      <c r="F29" s="424">
+      <c r="E29" s="356"/>
+      <c r="F29" s="430">
         <f>'Hitung Pemasukan Pengeluaran'!G6</f>
         <v>760000</v>
       </c>
-      <c r="G29" s="425"/>
+      <c r="G29" s="431"/>
       <c r="I29" s="170"/>
-      <c r="J29" s="398" t="s">
+      <c r="J29" s="354" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="400"/>
-      <c r="L29" s="424">
+      <c r="K29" s="356"/>
+      <c r="L29" s="430">
         <f>'Hitung Pemasukan Pengeluaran'!G22</f>
         <v>1657729.1800000002</v>
       </c>
-      <c r="M29" s="425"/>
+      <c r="M29" s="431"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="358" t="s">
+      <c r="D30" s="380" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="320"/>
-      <c r="F30" s="415">
+      <c r="E30" s="329"/>
+      <c r="F30" s="422">
         <f>F27</f>
         <v>903300</v>
       </c>
-      <c r="G30" s="416"/>
+      <c r="G30" s="423"/>
       <c r="I30" s="170"/>
-      <c r="J30" s="358" t="s">
+      <c r="J30" s="380" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="320"/>
-      <c r="L30" s="415">
+      <c r="K30" s="329"/>
+      <c r="L30" s="422">
         <f>L27</f>
         <v>779000</v>
       </c>
-      <c r="M30" s="416"/>
+      <c r="M30" s="423"/>
     </row>
     <row r="31" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="358" t="s">
+      <c r="D31" s="380" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="320"/>
-      <c r="F31" s="420">
+      <c r="E31" s="329"/>
+      <c r="F31" s="424">
         <f>Pemasukkan!F27</f>
         <v>222000</v>
       </c>
-      <c r="G31" s="421"/>
+      <c r="G31" s="425"/>
       <c r="I31" s="170"/>
-      <c r="J31" s="358" t="s">
+      <c r="J31" s="380" t="s">
         <v>98</v>
       </c>
-      <c r="K31" s="320"/>
-      <c r="L31" s="420">
+      <c r="K31" s="329"/>
+      <c r="L31" s="424">
         <f>Pemasukkan!L27</f>
         <v>690000</v>
       </c>
-      <c r="M31" s="421"/>
+      <c r="M31" s="425"/>
     </row>
     <row r="32" spans="3:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="359" t="s">
+      <c r="D32" s="413" t="s">
         <v>191</v>
       </c>
-      <c r="E32" s="360"/>
-      <c r="F32" s="426">
+      <c r="E32" s="414"/>
+      <c r="F32" s="428">
         <f>'Hitung Pemasukan Pengeluaran'!G8</f>
         <v>1651229.1800000002</v>
       </c>
-      <c r="G32" s="427"/>
+      <c r="G32" s="429"/>
       <c r="I32" s="170"/>
-      <c r="J32" s="359" t="s">
+      <c r="J32" s="413" t="s">
         <v>191</v>
       </c>
-      <c r="K32" s="360"/>
-      <c r="L32" s="426">
+      <c r="K32" s="414"/>
+      <c r="L32" s="428">
         <f>'Hitung Pemasukan Pengeluaran'!G23</f>
         <v>1568729.1800000002</v>
       </c>
-      <c r="M32" s="427"/>
+      <c r="M32" s="429"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20276,14 +20290,6 @@
     <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:M31"/>
     <mergeCell ref="C2:K3"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
@@ -20295,6 +20301,14 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:M31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -20320,28 +20334,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="430" t="s">
+      <c r="C2" s="436" t="s">
         <v>230</v>
       </c>
-      <c r="D2" s="431"/>
-      <c r="E2" s="431"/>
-      <c r="F2" s="431"/>
-      <c r="G2" s="431"/>
-      <c r="H2" s="431"/>
-      <c r="I2" s="431"/>
-      <c r="J2" s="431"/>
-      <c r="K2" s="431"/>
+      <c r="D2" s="437"/>
+      <c r="E2" s="437"/>
+      <c r="F2" s="437"/>
+      <c r="G2" s="437"/>
+      <c r="H2" s="437"/>
+      <c r="I2" s="437"/>
+      <c r="J2" s="437"/>
+      <c r="K2" s="437"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="431"/>
-      <c r="D3" s="431"/>
-      <c r="E3" s="431"/>
-      <c r="F3" s="431"/>
-      <c r="G3" s="431"/>
-      <c r="H3" s="431"/>
-      <c r="I3" s="431"/>
-      <c r="J3" s="431"/>
-      <c r="K3" s="431"/>
+      <c r="C3" s="437"/>
+      <c r="D3" s="437"/>
+      <c r="E3" s="437"/>
+      <c r="F3" s="437"/>
+      <c r="G3" s="437"/>
+      <c r="H3" s="437"/>
+      <c r="I3" s="437"/>
+      <c r="J3" s="437"/>
+      <c r="K3" s="437"/>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="139"/>
@@ -20699,10 +20713,10 @@
     </row>
     <row r="29" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="139"/>
-      <c r="D29" s="432"/>
-      <c r="E29" s="432"/>
-      <c r="F29" s="433"/>
-      <c r="G29" s="433"/>
+      <c r="D29" s="438"/>
+      <c r="E29" s="438"/>
+      <c r="F29" s="439"/>
+      <c r="G29" s="439"/>
       <c r="H29" s="139"/>
       <c r="I29" s="139"/>
       <c r="J29" s="139"/>
@@ -20710,15 +20724,15 @@
     </row>
     <row r="30" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="24"/>
-      <c r="D30" s="434" t="s">
+      <c r="D30" s="440" t="s">
         <v>229</v>
       </c>
-      <c r="E30" s="435"/>
-      <c r="F30" s="436">
+      <c r="E30" s="441"/>
+      <c r="F30" s="442">
         <f>F27</f>
         <v>226000</v>
       </c>
-      <c r="G30" s="437"/>
+      <c r="G30" s="443"/>
       <c r="H30" s="139"/>
       <c r="I30" s="139"/>
       <c r="J30" s="139"/>
@@ -20733,10 +20747,10 @@
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="139"/>
-      <c r="D32" s="428"/>
-      <c r="E32" s="428"/>
-      <c r="F32" s="429"/>
-      <c r="G32" s="428"/>
+      <c r="D32" s="434"/>
+      <c r="E32" s="434"/>
+      <c r="F32" s="435"/>
+      <c r="G32" s="434"/>
       <c r="H32" s="139"/>
       <c r="I32" s="139"/>
       <c r="J32" s="139"/>
@@ -20773,17 +20787,17 @@
     <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="438" t="s">
+      <c r="C4" s="444" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="439"/>
+      <c r="D4" s="445"/>
       <c r="E4" s="27"/>
       <c r="F4" s="33"/>
       <c r="G4" s="34"/>
-      <c r="H4" s="438" t="s">
+      <c r="H4" s="444" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="439"/>
+      <c r="I4" s="445"/>
       <c r="J4" s="35"/>
       <c r="K4" s="27"/>
     </row>
@@ -20910,17 +20924,17 @@
     <row r="16" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26"/>
-      <c r="C17" s="438" t="s">
+      <c r="C17" s="444" t="s">
         <v>144</v>
       </c>
-      <c r="D17" s="439"/>
+      <c r="D17" s="445"/>
       <c r="E17" s="27"/>
       <c r="F17" s="26"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="438" t="s">
+      <c r="H17" s="444" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="439"/>
+      <c r="I17" s="445"/>
       <c r="J17" s="35"/>
       <c r="K17" s="27"/>
     </row>

</xml_diff>

<commit_message>
Koreksi dan Pengeluaran Makrab 19
Koreksi :
- Detail nota pembelian Gelang Marshall

Pengeluaran :
-Modal untuk print intel dll (adit)
</commit_message>
<xml_diff>
--- a/GAS/KAS GAS.xlsx
+++ b/GAS/KAS GAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-630" yWindow="570" windowWidth="19815" windowHeight="7365" tabRatio="761" activeTab="2"/>
+    <workbookView xWindow="-630" yWindow="570" windowWidth="19815" windowHeight="7365" tabRatio="761" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2018(NOT UPDATED)" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="Patch OH" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="406">
   <si>
     <t>LAPORAN KEUANGAN KAS GAS</t>
   </si>
@@ -1225,9 +1226,6 @@
     <t>18 Februari 2020</t>
   </si>
   <si>
-    <t>Gelang Marshall</t>
-  </si>
-  <si>
     <t>Yusuf KAS(trf)</t>
   </si>
   <si>
@@ -1235,6 +1233,15 @@
   </si>
   <si>
     <t>Antoni KAS(trf)</t>
+  </si>
+  <si>
+    <t>Biaya Admin Gelang Marshall</t>
+  </si>
+  <si>
+    <t>Modal Print (Adit)</t>
+  </si>
+  <si>
+    <t>Gelang Marshall(Tokped)</t>
   </si>
 </sst>
 </file>
@@ -3111,20 +3118,29 @@
     <xf numFmtId="167" fontId="4" fillId="26" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3140,39 +3156,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3180,36 +3194,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFo